<commit_message>
almoust solved some improvements in filtres at 16/07/2022
</commit_message>
<xml_diff>
--- a/src/Tyres.xlsx
+++ b/src/Tyres.xlsx
@@ -2,22 +2,24 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
-  <workbookProtection/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="0" yWindow="0" windowWidth="23190" windowHeight="9285" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
     <sheet name="Holidays 2019" sheetId="1" state="visible" r:id="rId1"/>
     <sheet name="Sheet" sheetId="2" state="visible" r:id="rId2"/>
   </sheets>
   <definedNames/>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="0" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="0"/>
+  <numFmts count="2">
+    <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd"/>
+    <numFmt numFmtId="165" formatCode="yyyy-mm-dd"/>
+  </numFmts>
   <fonts count="1">
     <font>
       <name val="Calibri"/>
@@ -47,11 +49,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
+    <cellStyle name="Обычный" xfId="0" builtinId="0"/>
   </cellStyles>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
@@ -414,317 +418,1302 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C18"/>
+  <dimension ref="A1:J36"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G4" sqref="A4:G18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15" outlineLevelCol="0"/>
+  <cols>
+    <col width="12.7109375" customWidth="1" min="1" max="1"/>
+    <col width="14.5703125" customWidth="1" min="2" max="2"/>
+    <col width="20.5703125" customWidth="1" min="3" max="3"/>
+    <col width="12.28515625" customWidth="1" min="5" max="5"/>
+    <col width="19.85546875" customWidth="1" min="6" max="6"/>
+    <col width="22.140625" customWidth="1" min="7" max="7"/>
+    <col width="18" customWidth="1" min="8" max="8"/>
+  </cols>
   <sheetData>
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>315/80R22.5</t>
+          <t>BEL-158M</t>
         </is>
       </c>
       <c r="B1" t="inlineStr">
         <is>
-          <t>BEL-158M</t>
+          <t>315/80R22.5</t>
         </is>
       </c>
       <c r="C1" t="inlineStr">
         <is>
-          <t>Ср Гр выт</t>
+          <t>сер груз камневыт</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>Tyre Size</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>Model</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
+        <is>
+          <t>Param</t>
+        </is>
+      </c>
+      <c r="H1" t="inlineStr">
+        <is>
+          <t>Sales value</t>
+        </is>
+      </c>
+      <c r="I1" s="1" t="inlineStr">
+        <is>
+          <t>Date_of_sales</t>
+        </is>
+      </c>
+      <c r="J1" t="inlineStr">
+        <is>
+          <t>Contragent</t>
         </is>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>315/80R22.5</t>
+          <t>BEL-158M</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
+          <t>315/80R22.5</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>груз камневыт трп</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>315/80R22.5</t>
+        </is>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
           <t>BEL-158M</t>
         </is>
       </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>Тр Гр выт</t>
+      <c r="G2" t="inlineStr">
+        <is>
+          <t>груз, камневыт, трп</t>
+        </is>
+      </c>
+      <c r="H2" t="n">
+        <v>259</v>
+      </c>
+      <c r="I2" s="1" t="n">
+        <v>44789</v>
+      </c>
+      <c r="J2" t="inlineStr">
+        <is>
+          <t>none</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>315/80R22.5</t>
+          <t>BEL-278</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
+          <t>315/80R22.5</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>сер груз</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>315/80R22.5</t>
+        </is>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
           <t>BEL-278</t>
         </is>
       </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>Сер Груз</t>
+      <c r="G3" t="inlineStr">
+        <is>
+          <t>сер, груз</t>
+        </is>
+      </c>
+      <c r="H3" t="n">
+        <v>259</v>
+      </c>
+      <c r="I3" s="1" t="n">
+        <v>44789</v>
+      </c>
+      <c r="J3" t="inlineStr">
+        <is>
+          <t>none</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>315/80R22.5</t>
+          <t>BEL-278</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
+          <t>315/80R22.5</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>груз трп</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>315/80R22.5</t>
+        </is>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
           <t>BEL-278</t>
         </is>
       </c>
-      <c r="C4" t="inlineStr">
-        <is>
-          <t>Трп Груз</t>
+      <c r="G4" t="inlineStr">
+        <is>
+          <t>груз, трп</t>
+        </is>
+      </c>
+      <c r="H4" t="n">
+        <v>259</v>
+      </c>
+      <c r="I4" s="1" t="n">
+        <v>44789</v>
+      </c>
+      <c r="J4" t="inlineStr">
+        <is>
+          <t>none</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>315/80R22.5</t>
+          <t>BEL-268</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
+          <t>315/80R22.5</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>сер груз</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>315/80R22.5</t>
+        </is>
+      </c>
+      <c r="F5" t="inlineStr">
+        <is>
           <t>BEL-268</t>
         </is>
       </c>
-      <c r="C5" t="inlineStr">
-        <is>
-          <t>Сер Груз</t>
+      <c r="G5" t="inlineStr">
+        <is>
+          <t>сер, груз</t>
+        </is>
+      </c>
+      <c r="H5" t="n">
+        <v>259</v>
+      </c>
+      <c r="I5" s="1" t="n">
+        <v>44789</v>
+      </c>
+      <c r="J5" t="inlineStr">
+        <is>
+          <t>none</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>315/80R22.5</t>
+          <t>BEL-268</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
+          <t>315/80R22.5</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>груз трп</t>
+        </is>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>315/80R22.5</t>
+        </is>
+      </c>
+      <c r="F6" t="inlineStr">
+        <is>
           <t>BEL-268</t>
         </is>
       </c>
-      <c r="C6" t="inlineStr">
-        <is>
-          <t>Трп Груз</t>
+      <c r="G6" t="inlineStr">
+        <is>
+          <t>груз, трп</t>
+        </is>
+      </c>
+      <c r="H6" t="n">
+        <v>259</v>
+      </c>
+      <c r="I6" s="1" t="n">
+        <v>44789</v>
+      </c>
+      <c r="J6" t="inlineStr">
+        <is>
+          <t>none</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>315/80R22.5</t>
+          <t>BEL-398</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
+          <t>315/80R22.5</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>сер груз</t>
+        </is>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>315/80R22.5</t>
+        </is>
+      </c>
+      <c r="F7" t="inlineStr">
+        <is>
           <t>BEL-398</t>
         </is>
       </c>
-      <c r="C7" t="inlineStr">
-        <is>
-          <t>Сер Груз</t>
+      <c r="G7" t="inlineStr">
+        <is>
+          <t>сер, груз</t>
+        </is>
+      </c>
+      <c r="H7" t="n">
+        <v>259</v>
+      </c>
+      <c r="I7" s="1" t="n">
+        <v>44789</v>
+      </c>
+      <c r="J7" t="inlineStr">
+        <is>
+          <t>none</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>315/80R22.5</t>
+          <t>BEL-326</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
+          <t>315/80R22.5</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>сер груз</t>
+        </is>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>315/80R22.5</t>
+        </is>
+      </c>
+      <c r="F8" t="inlineStr">
+        <is>
           <t>BEL-326</t>
         </is>
       </c>
-      <c r="C8" t="inlineStr">
-        <is>
-          <t>Сер Груз</t>
+      <c r="G8" t="inlineStr">
+        <is>
+          <t>сер, груз</t>
+        </is>
+      </c>
+      <c r="H8" t="n">
+        <v>259</v>
+      </c>
+      <c r="I8" s="1" t="n">
+        <v>44789</v>
+      </c>
+      <c r="J8" t="inlineStr">
+        <is>
+          <t>none</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>315/80R22.5</t>
+          <t>BEL-326</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
+          <t>315/80R22.5</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>груз трп</t>
+        </is>
+      </c>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>315/80R22.5</t>
+        </is>
+      </c>
+      <c r="F9" t="inlineStr">
+        <is>
           <t>BEL-326</t>
         </is>
       </c>
-      <c r="C9" t="inlineStr">
-        <is>
-          <t>Трп Груз</t>
+      <c r="G9" t="inlineStr">
+        <is>
+          <t>груз, трп</t>
+        </is>
+      </c>
+      <c r="H9" t="n">
+        <v>259</v>
+      </c>
+      <c r="I9" s="1" t="n">
+        <v>44789</v>
+      </c>
+      <c r="J9" t="inlineStr">
+        <is>
+          <t>none</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>315/80R22.5</t>
+          <t>BEL-498</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
+          <t>315/80R22.5</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>156L сер груз</t>
+        </is>
+      </c>
+      <c r="E10" t="inlineStr">
+        <is>
+          <t>315/80R22.5</t>
+        </is>
+      </c>
+      <c r="F10" t="inlineStr">
+        <is>
           <t>BEL-498</t>
         </is>
       </c>
-      <c r="C10" t="inlineStr">
-        <is>
-          <t>Сер Гр 156L</t>
+      <c r="G10" t="inlineStr">
+        <is>
+          <t>156L, сер, груз</t>
+        </is>
+      </c>
+      <c r="H10" t="n">
+        <v>259</v>
+      </c>
+      <c r="I10" s="1" t="n">
+        <v>44789</v>
+      </c>
+      <c r="J10" t="inlineStr">
+        <is>
+          <t>none</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>315/80R22.5</t>
+          <t>BEL-518</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
+          <t>315/80R22.5</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>сер груз</t>
+        </is>
+      </c>
+      <c r="E11" t="inlineStr">
+        <is>
+          <t>315/80R22.5</t>
+        </is>
+      </c>
+      <c r="F11" t="inlineStr">
+        <is>
           <t>BEL-518</t>
         </is>
       </c>
-      <c r="C11" t="inlineStr">
-        <is>
-          <t>Сер Груз</t>
+      <c r="G11" t="inlineStr">
+        <is>
+          <t>сер, груз</t>
+        </is>
+      </c>
+      <c r="H11" t="n">
+        <v>259</v>
+      </c>
+      <c r="I11" s="1" t="n">
+        <v>44789</v>
+      </c>
+      <c r="J11" t="inlineStr">
+        <is>
+          <t>none</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>12.00R20</t>
+          <t>ИД-304М</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
+          <t>12.00R20</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>16 сер груз</t>
+        </is>
+      </c>
+      <c r="E12" t="inlineStr">
+        <is>
+          <t>12.00R20</t>
+        </is>
+      </c>
+      <c r="F12" t="inlineStr">
+        <is>
           <t>ИД-304М</t>
         </is>
       </c>
-      <c r="C12" t="inlineStr">
-        <is>
-          <t>Сер Груз 16</t>
+      <c r="G12" t="inlineStr">
+        <is>
+          <t>16, сер, груз</t>
+        </is>
+      </c>
+      <c r="H12" t="n">
+        <v>259</v>
+      </c>
+      <c r="I12" s="1" t="n">
+        <v>44789</v>
+      </c>
+      <c r="J12" t="inlineStr">
+        <is>
+          <t>none</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>12.00R20</t>
+          <t>ИД-304М</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
+          <t>12.00R20</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>18 сер груз</t>
+        </is>
+      </c>
+      <c r="E13" t="inlineStr">
+        <is>
+          <t>12.00R20</t>
+        </is>
+      </c>
+      <c r="F13" t="inlineStr">
+        <is>
           <t>ИД-304М</t>
         </is>
       </c>
-      <c r="C13" t="inlineStr">
-        <is>
-          <t>Сер Груз 18</t>
+      <c r="G13" t="inlineStr">
+        <is>
+          <t>18, сер, груз</t>
+        </is>
+      </c>
+      <c r="H13" t="n">
+        <v>259</v>
+      </c>
+      <c r="I13" s="1" t="n">
+        <v>44789</v>
+      </c>
+      <c r="J13" t="inlineStr">
+        <is>
+          <t>none</t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>12.00R20</t>
+          <t>ИД-304М</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
+          <t>12.00R20</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>16 груз трп</t>
+        </is>
+      </c>
+      <c r="E14" t="inlineStr">
+        <is>
+          <t>12.00R20</t>
+        </is>
+      </c>
+      <c r="F14" t="inlineStr">
+        <is>
           <t>ИД-304М</t>
         </is>
       </c>
-      <c r="C14" t="inlineStr">
-        <is>
-          <t>Трп Груз 16</t>
+      <c r="G14" t="inlineStr">
+        <is>
+          <t>16, груз, трп</t>
+        </is>
+      </c>
+      <c r="H14" t="n">
+        <v>259</v>
+      </c>
+      <c r="I14" s="1" t="n">
+        <v>44789</v>
+      </c>
+      <c r="J14" t="inlineStr">
+        <is>
+          <t>none</t>
         </is>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>12.00R20</t>
+          <t>ИД-304М</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
+          <t>12.00R20</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>18 груз трп</t>
+        </is>
+      </c>
+      <c r="E15" t="inlineStr">
+        <is>
+          <t>12.00R20</t>
+        </is>
+      </c>
+      <c r="F15" t="inlineStr">
+        <is>
           <t>ИД-304М</t>
         </is>
       </c>
-      <c r="C15" t="inlineStr">
-        <is>
-          <t>Трп Груз 18</t>
+      <c r="G15" t="inlineStr">
+        <is>
+          <t>18, груз, трп</t>
+        </is>
+      </c>
+      <c r="H15" t="n">
+        <v>259</v>
+      </c>
+      <c r="I15" s="1" t="n">
+        <v>44789</v>
+      </c>
+      <c r="J15" t="inlineStr">
+        <is>
+          <t>none</t>
         </is>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>12.00R20</t>
+          <t>БИ-368М</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
         <is>
+          <t>12.00R20</t>
+        </is>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>18 сер груз</t>
+        </is>
+      </c>
+      <c r="E16" t="inlineStr">
+        <is>
+          <t>12.00R20</t>
+        </is>
+      </c>
+      <c r="F16" t="inlineStr">
+        <is>
           <t>БИ-368М</t>
         </is>
       </c>
-      <c r="C16" t="inlineStr">
-        <is>
-          <t>Сер Груз 18</t>
+      <c r="G16" t="inlineStr">
+        <is>
+          <t>18, сер, груз</t>
+        </is>
+      </c>
+      <c r="H16" t="n">
+        <v>259</v>
+      </c>
+      <c r="I16" s="1" t="n">
+        <v>44789</v>
+      </c>
+      <c r="J16" t="inlineStr">
+        <is>
+          <t>none</t>
         </is>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>12.00R20</t>
+          <t>БИ-368М</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
         <is>
+          <t>12.00R20</t>
+        </is>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>18 сер груз</t>
+        </is>
+      </c>
+      <c r="E17" t="inlineStr">
+        <is>
+          <t>12.00R20</t>
+        </is>
+      </c>
+      <c r="F17" t="inlineStr">
+        <is>
           <t>БИ-368М</t>
         </is>
       </c>
-      <c r="C17" t="inlineStr">
-        <is>
-          <t>Сер Груз 18</t>
+      <c r="G17" t="inlineStr">
+        <is>
+          <t>18, сер, груз</t>
+        </is>
+      </c>
+      <c r="H17" t="n">
+        <v>259</v>
+      </c>
+      <c r="I17" s="1" t="n">
+        <v>44789</v>
+      </c>
+      <c r="J17" t="inlineStr">
+        <is>
+          <t>none</t>
         </is>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>12.00R20</t>
+          <t>БИ-368М</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
         <is>
+          <t>12.00R20</t>
+        </is>
+      </c>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>18 груз трп</t>
+        </is>
+      </c>
+      <c r="E18" t="inlineStr">
+        <is>
+          <t>12.00R20</t>
+        </is>
+      </c>
+      <c r="F18" t="inlineStr">
+        <is>
           <t>БИ-368М</t>
         </is>
       </c>
-      <c r="C18" t="inlineStr">
-        <is>
-          <t>Трп Груз 18</t>
+      <c r="G18" t="inlineStr">
+        <is>
+          <t>18, груз, трп</t>
+        </is>
+      </c>
+      <c r="H18" t="n">
+        <v>259</v>
+      </c>
+      <c r="I18" s="1" t="n">
+        <v>44789</v>
+      </c>
+      <c r="J18" t="inlineStr">
+        <is>
+          <t>none</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="E19" t="inlineStr">
+        <is>
+          <t>315/80R22.5</t>
+        </is>
+      </c>
+      <c r="F19" t="inlineStr">
+        <is>
+          <t>BEL-158M</t>
+        </is>
+      </c>
+      <c r="G19" t="inlineStr">
+        <is>
+          <t>сер, груз, камневыт</t>
+        </is>
+      </c>
+      <c r="H19" t="n">
+        <v>11</v>
+      </c>
+      <c r="I19" s="2" t="n">
+        <v>44789</v>
+      </c>
+      <c r="J19" t="inlineStr">
+        <is>
+          <t>none</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="E20" t="inlineStr">
+        <is>
+          <t>315/80R22.5</t>
+        </is>
+      </c>
+      <c r="F20" t="inlineStr">
+        <is>
+          <t>BEL-158M</t>
+        </is>
+      </c>
+      <c r="G20" t="inlineStr">
+        <is>
+          <t>груз, камневыт, трп</t>
+        </is>
+      </c>
+      <c r="H20" t="n">
+        <v>11</v>
+      </c>
+      <c r="I20" s="2" t="n">
+        <v>44789</v>
+      </c>
+      <c r="J20" t="inlineStr">
+        <is>
+          <t>none</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="E21" t="inlineStr">
+        <is>
+          <t>315/80R22.5</t>
+        </is>
+      </c>
+      <c r="F21" t="inlineStr">
+        <is>
+          <t>BEL-278</t>
+        </is>
+      </c>
+      <c r="G21" t="inlineStr">
+        <is>
+          <t>сер, груз</t>
+        </is>
+      </c>
+      <c r="H21" t="n">
+        <v>11</v>
+      </c>
+      <c r="I21" s="2" t="n">
+        <v>44789</v>
+      </c>
+      <c r="J21" t="inlineStr">
+        <is>
+          <t>none</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="E22" t="inlineStr">
+        <is>
+          <t>315/80R22.5</t>
+        </is>
+      </c>
+      <c r="F22" t="inlineStr">
+        <is>
+          <t>BEL-278</t>
+        </is>
+      </c>
+      <c r="G22" t="inlineStr">
+        <is>
+          <t>груз, трп</t>
+        </is>
+      </c>
+      <c r="H22" t="n">
+        <v>11</v>
+      </c>
+      <c r="I22" s="2" t="n">
+        <v>44789</v>
+      </c>
+      <c r="J22" t="inlineStr">
+        <is>
+          <t>none</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="E23" t="inlineStr">
+        <is>
+          <t>315/80R22.5</t>
+        </is>
+      </c>
+      <c r="F23" t="inlineStr">
+        <is>
+          <t>BEL-268</t>
+        </is>
+      </c>
+      <c r="G23" t="inlineStr">
+        <is>
+          <t>сер, груз</t>
+        </is>
+      </c>
+      <c r="H23" t="n">
+        <v>11</v>
+      </c>
+      <c r="I23" s="2" t="n">
+        <v>44789</v>
+      </c>
+      <c r="J23" t="inlineStr">
+        <is>
+          <t>none</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="E24" t="inlineStr">
+        <is>
+          <t>315/80R22.5</t>
+        </is>
+      </c>
+      <c r="F24" t="inlineStr">
+        <is>
+          <t>BEL-268</t>
+        </is>
+      </c>
+      <c r="G24" t="inlineStr">
+        <is>
+          <t>груз, трп</t>
+        </is>
+      </c>
+      <c r="H24" t="n">
+        <v>11</v>
+      </c>
+      <c r="I24" s="2" t="n">
+        <v>44789</v>
+      </c>
+      <c r="J24" t="inlineStr">
+        <is>
+          <t>none</t>
+        </is>
+      </c>
+    </row>
+    <row r="25">
+      <c r="E25" t="inlineStr">
+        <is>
+          <t>315/80R22.5</t>
+        </is>
+      </c>
+      <c r="F25" t="inlineStr">
+        <is>
+          <t>BEL-398</t>
+        </is>
+      </c>
+      <c r="G25" t="inlineStr">
+        <is>
+          <t>сер, груз</t>
+        </is>
+      </c>
+      <c r="H25" t="n">
+        <v>11</v>
+      </c>
+      <c r="I25" s="2" t="n">
+        <v>44789</v>
+      </c>
+      <c r="J25" t="inlineStr">
+        <is>
+          <t>none</t>
+        </is>
+      </c>
+    </row>
+    <row r="26">
+      <c r="E26" t="inlineStr">
+        <is>
+          <t>315/80R22.5</t>
+        </is>
+      </c>
+      <c r="F26" t="inlineStr">
+        <is>
+          <t>BEL-326</t>
+        </is>
+      </c>
+      <c r="G26" t="inlineStr">
+        <is>
+          <t>сер, груз</t>
+        </is>
+      </c>
+      <c r="H26" t="n">
+        <v>11</v>
+      </c>
+      <c r="I26" s="2" t="n">
+        <v>44789</v>
+      </c>
+      <c r="J26" t="inlineStr">
+        <is>
+          <t>none</t>
+        </is>
+      </c>
+    </row>
+    <row r="27">
+      <c r="E27" t="inlineStr">
+        <is>
+          <t>315/80R22.5</t>
+        </is>
+      </c>
+      <c r="F27" t="inlineStr">
+        <is>
+          <t>BEL-326</t>
+        </is>
+      </c>
+      <c r="G27" t="inlineStr">
+        <is>
+          <t>груз, трп</t>
+        </is>
+      </c>
+      <c r="H27" t="n">
+        <v>11</v>
+      </c>
+      <c r="I27" s="2" t="n">
+        <v>44789</v>
+      </c>
+      <c r="J27" t="inlineStr">
+        <is>
+          <t>none</t>
+        </is>
+      </c>
+    </row>
+    <row r="28">
+      <c r="E28" t="inlineStr">
+        <is>
+          <t>315/80R22.5</t>
+        </is>
+      </c>
+      <c r="F28" t="inlineStr">
+        <is>
+          <t>BEL-498</t>
+        </is>
+      </c>
+      <c r="G28" t="inlineStr">
+        <is>
+          <t>156L, сер, груз</t>
+        </is>
+      </c>
+      <c r="H28" t="n">
+        <v>11</v>
+      </c>
+      <c r="I28" s="2" t="n">
+        <v>44789</v>
+      </c>
+      <c r="J28" t="inlineStr">
+        <is>
+          <t>none</t>
+        </is>
+      </c>
+    </row>
+    <row r="29">
+      <c r="E29" t="inlineStr">
+        <is>
+          <t>315/80R22.5</t>
+        </is>
+      </c>
+      <c r="F29" t="inlineStr">
+        <is>
+          <t>BEL-518</t>
+        </is>
+      </c>
+      <c r="G29" t="inlineStr">
+        <is>
+          <t>сер, груз</t>
+        </is>
+      </c>
+      <c r="H29" t="n">
+        <v>11</v>
+      </c>
+      <c r="I29" s="2" t="n">
+        <v>44789</v>
+      </c>
+      <c r="J29" t="inlineStr">
+        <is>
+          <t>none</t>
+        </is>
+      </c>
+    </row>
+    <row r="30">
+      <c r="E30" t="inlineStr">
+        <is>
+          <t>12.00R20</t>
+        </is>
+      </c>
+      <c r="F30" t="inlineStr">
+        <is>
+          <t>ИД-304М</t>
+        </is>
+      </c>
+      <c r="G30" t="inlineStr">
+        <is>
+          <t>16, сер, груз</t>
+        </is>
+      </c>
+      <c r="H30" t="n">
+        <v>11</v>
+      </c>
+      <c r="I30" s="2" t="n">
+        <v>44789</v>
+      </c>
+      <c r="J30" t="inlineStr">
+        <is>
+          <t>none</t>
+        </is>
+      </c>
+    </row>
+    <row r="31">
+      <c r="E31" t="inlineStr">
+        <is>
+          <t>12.00R20</t>
+        </is>
+      </c>
+      <c r="F31" t="inlineStr">
+        <is>
+          <t>ИД-304М</t>
+        </is>
+      </c>
+      <c r="G31" t="inlineStr">
+        <is>
+          <t>18, сер, груз</t>
+        </is>
+      </c>
+      <c r="H31" t="n">
+        <v>11</v>
+      </c>
+      <c r="I31" s="2" t="n">
+        <v>44789</v>
+      </c>
+      <c r="J31" t="inlineStr">
+        <is>
+          <t>none</t>
+        </is>
+      </c>
+    </row>
+    <row r="32">
+      <c r="E32" t="inlineStr">
+        <is>
+          <t>12.00R20</t>
+        </is>
+      </c>
+      <c r="F32" t="inlineStr">
+        <is>
+          <t>ИД-304М</t>
+        </is>
+      </c>
+      <c r="G32" t="inlineStr">
+        <is>
+          <t>16, груз, трп</t>
+        </is>
+      </c>
+      <c r="H32" t="n">
+        <v>11</v>
+      </c>
+      <c r="I32" s="2" t="n">
+        <v>44789</v>
+      </c>
+      <c r="J32" t="inlineStr">
+        <is>
+          <t>none</t>
+        </is>
+      </c>
+    </row>
+    <row r="33">
+      <c r="E33" t="inlineStr">
+        <is>
+          <t>12.00R20</t>
+        </is>
+      </c>
+      <c r="F33" t="inlineStr">
+        <is>
+          <t>ИД-304М</t>
+        </is>
+      </c>
+      <c r="G33" t="inlineStr">
+        <is>
+          <t>18, груз, трп</t>
+        </is>
+      </c>
+      <c r="H33" t="n">
+        <v>11</v>
+      </c>
+      <c r="I33" s="2" t="n">
+        <v>44789</v>
+      </c>
+      <c r="J33" t="inlineStr">
+        <is>
+          <t>none</t>
+        </is>
+      </c>
+    </row>
+    <row r="34">
+      <c r="E34" t="inlineStr">
+        <is>
+          <t>12.00R20</t>
+        </is>
+      </c>
+      <c r="F34" t="inlineStr">
+        <is>
+          <t>БИ-368М</t>
+        </is>
+      </c>
+      <c r="G34" t="inlineStr">
+        <is>
+          <t>18, сер, груз</t>
+        </is>
+      </c>
+      <c r="H34" t="n">
+        <v>11</v>
+      </c>
+      <c r="I34" s="2" t="n">
+        <v>44789</v>
+      </c>
+      <c r="J34" t="inlineStr">
+        <is>
+          <t>none</t>
+        </is>
+      </c>
+    </row>
+    <row r="35">
+      <c r="E35" t="inlineStr">
+        <is>
+          <t>12.00R20</t>
+        </is>
+      </c>
+      <c r="F35" t="inlineStr">
+        <is>
+          <t>БИ-368М</t>
+        </is>
+      </c>
+      <c r="G35" t="inlineStr">
+        <is>
+          <t>18, сер, груз</t>
+        </is>
+      </c>
+      <c r="H35" t="n">
+        <v>11</v>
+      </c>
+      <c r="I35" s="2" t="n">
+        <v>44789</v>
+      </c>
+      <c r="J35" t="inlineStr">
+        <is>
+          <t>none</t>
+        </is>
+      </c>
+    </row>
+    <row r="36">
+      <c r="E36" t="inlineStr">
+        <is>
+          <t>12.00R20</t>
+        </is>
+      </c>
+      <c r="F36" t="inlineStr">
+        <is>
+          <t>БИ-368М</t>
+        </is>
+      </c>
+      <c r="G36" t="inlineStr">
+        <is>
+          <t>18, груз, трп</t>
+        </is>
+      </c>
+      <c r="H36" t="n">
+        <v>11</v>
+      </c>
+      <c r="I36" s="2" t="n">
+        <v>44789</v>
+      </c>
+      <c r="J36" t="inlineStr">
+        <is>
+          <t>none</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
abc table periods at 30/08/2022
</commit_message>
<xml_diff>
--- a/src/Tyres.xlsx
+++ b/src/Tyres.xlsx
@@ -17,7 +17,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="0"/>
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="yyyy-mm-dd"/>
+  </numFmts>
   <fonts count="1">
     <font>
       <name val="Calibri"/>
@@ -47,8 +49,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
@@ -414,7 +417,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C18"/>
+  <dimension ref="A1:J55"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -438,6 +441,36 @@
           <t>сер груз камневыт</t>
         </is>
       </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>Tyre Size</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>Model</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
+        <is>
+          <t>Param</t>
+        </is>
+      </c>
+      <c r="H1" t="inlineStr">
+        <is>
+          <t>Sales value</t>
+        </is>
+      </c>
+      <c r="I1" t="inlineStr">
+        <is>
+          <t>Date_of_sales</t>
+        </is>
+      </c>
+      <c r="J1" t="inlineStr">
+        <is>
+          <t>Contragent</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
@@ -455,6 +488,32 @@
           <t>груз камневыт трп</t>
         </is>
       </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>315/80R22.5</t>
+        </is>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>BEL-158M</t>
+        </is>
+      </c>
+      <c r="G2" t="inlineStr">
+        <is>
+          <t>сер, груз, камневыт</t>
+        </is>
+      </c>
+      <c r="H2" t="n">
+        <v>3</v>
+      </c>
+      <c r="I2" s="1" t="n">
+        <v>44737</v>
+      </c>
+      <c r="J2" t="inlineStr">
+        <is>
+          <t>БНХ Польска</t>
+        </is>
+      </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -472,6 +531,32 @@
           <t>сер груз</t>
         </is>
       </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>315/80R22.5</t>
+        </is>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>BEL-158M</t>
+        </is>
+      </c>
+      <c r="G3" t="inlineStr">
+        <is>
+          <t>груз, камневыт, трп</t>
+        </is>
+      </c>
+      <c r="H3" t="n">
+        <v>3</v>
+      </c>
+      <c r="I3" s="1" t="n">
+        <v>44737</v>
+      </c>
+      <c r="J3" t="inlineStr">
+        <is>
+          <t>БНХ Польска</t>
+        </is>
+      </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
@@ -489,6 +574,32 @@
           <t>груз трп</t>
         </is>
       </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>315/80R22.5</t>
+        </is>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>BEL-278</t>
+        </is>
+      </c>
+      <c r="G4" t="inlineStr">
+        <is>
+          <t>сер, груз</t>
+        </is>
+      </c>
+      <c r="H4" t="n">
+        <v>3</v>
+      </c>
+      <c r="I4" s="1" t="n">
+        <v>44737</v>
+      </c>
+      <c r="J4" t="inlineStr">
+        <is>
+          <t>БНХ Польска</t>
+        </is>
+      </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
@@ -506,6 +617,32 @@
           <t>сер груз</t>
         </is>
       </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>315/80R22.5</t>
+        </is>
+      </c>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>BEL-278</t>
+        </is>
+      </c>
+      <c r="G5" t="inlineStr">
+        <is>
+          <t>груз, трп</t>
+        </is>
+      </c>
+      <c r="H5" t="n">
+        <v>3</v>
+      </c>
+      <c r="I5" s="1" t="n">
+        <v>44737</v>
+      </c>
+      <c r="J5" t="inlineStr">
+        <is>
+          <t>БНХ Польска</t>
+        </is>
+      </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
@@ -523,6 +660,32 @@
           <t>груз трп</t>
         </is>
       </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>315/80R22.5</t>
+        </is>
+      </c>
+      <c r="F6" t="inlineStr">
+        <is>
+          <t>BEL-268</t>
+        </is>
+      </c>
+      <c r="G6" t="inlineStr">
+        <is>
+          <t>сер, груз</t>
+        </is>
+      </c>
+      <c r="H6" t="n">
+        <v>3</v>
+      </c>
+      <c r="I6" s="1" t="n">
+        <v>44737</v>
+      </c>
+      <c r="J6" t="inlineStr">
+        <is>
+          <t>БНХ Польска</t>
+        </is>
+      </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
@@ -540,6 +703,32 @@
           <t>сер груз</t>
         </is>
       </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>315/80R22.5</t>
+        </is>
+      </c>
+      <c r="F7" t="inlineStr">
+        <is>
+          <t>BEL-268</t>
+        </is>
+      </c>
+      <c r="G7" t="inlineStr">
+        <is>
+          <t>груз, трп</t>
+        </is>
+      </c>
+      <c r="H7" t="n">
+        <v>3</v>
+      </c>
+      <c r="I7" s="1" t="n">
+        <v>44737</v>
+      </c>
+      <c r="J7" t="inlineStr">
+        <is>
+          <t>БНХ Польска</t>
+        </is>
+      </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
@@ -557,6 +746,32 @@
           <t>сер груз</t>
         </is>
       </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>315/80R22.5</t>
+        </is>
+      </c>
+      <c r="F8" t="inlineStr">
+        <is>
+          <t>BEL-398</t>
+        </is>
+      </c>
+      <c r="G8" t="inlineStr">
+        <is>
+          <t>сер, груз</t>
+        </is>
+      </c>
+      <c r="H8" t="n">
+        <v>3</v>
+      </c>
+      <c r="I8" s="1" t="n">
+        <v>44737</v>
+      </c>
+      <c r="J8" t="inlineStr">
+        <is>
+          <t>БНХ Польска</t>
+        </is>
+      </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
@@ -574,6 +789,32 @@
           <t>груз трп</t>
         </is>
       </c>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>315/80R22.5</t>
+        </is>
+      </c>
+      <c r="F9" t="inlineStr">
+        <is>
+          <t>BEL-326</t>
+        </is>
+      </c>
+      <c r="G9" t="inlineStr">
+        <is>
+          <t>сер, груз</t>
+        </is>
+      </c>
+      <c r="H9" t="n">
+        <v>3</v>
+      </c>
+      <c r="I9" s="1" t="n">
+        <v>44737</v>
+      </c>
+      <c r="J9" t="inlineStr">
+        <is>
+          <t>БНХ Польска</t>
+        </is>
+      </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
@@ -591,6 +832,32 @@
           <t>156L сер груз</t>
         </is>
       </c>
+      <c r="E10" t="inlineStr">
+        <is>
+          <t>315/80R22.5</t>
+        </is>
+      </c>
+      <c r="F10" t="inlineStr">
+        <is>
+          <t>BEL-326</t>
+        </is>
+      </c>
+      <c r="G10" t="inlineStr">
+        <is>
+          <t>груз, трп</t>
+        </is>
+      </c>
+      <c r="H10" t="n">
+        <v>3</v>
+      </c>
+      <c r="I10" s="1" t="n">
+        <v>44737</v>
+      </c>
+      <c r="J10" t="inlineStr">
+        <is>
+          <t>БНХ Польска</t>
+        </is>
+      </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
@@ -608,6 +875,32 @@
           <t>сер груз</t>
         </is>
       </c>
+      <c r="E11" t="inlineStr">
+        <is>
+          <t>315/80R22.5</t>
+        </is>
+      </c>
+      <c r="F11" t="inlineStr">
+        <is>
+          <t>BEL-498</t>
+        </is>
+      </c>
+      <c r="G11" t="inlineStr">
+        <is>
+          <t>156L, сер, груз</t>
+        </is>
+      </c>
+      <c r="H11" t="n">
+        <v>3</v>
+      </c>
+      <c r="I11" s="1" t="n">
+        <v>44737</v>
+      </c>
+      <c r="J11" t="inlineStr">
+        <is>
+          <t>БНХ Польска</t>
+        </is>
+      </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
@@ -625,6 +918,32 @@
           <t>16 сер груз</t>
         </is>
       </c>
+      <c r="E12" t="inlineStr">
+        <is>
+          <t>315/80R22.5</t>
+        </is>
+      </c>
+      <c r="F12" t="inlineStr">
+        <is>
+          <t>BEL-518</t>
+        </is>
+      </c>
+      <c r="G12" t="inlineStr">
+        <is>
+          <t>сер, груз</t>
+        </is>
+      </c>
+      <c r="H12" t="n">
+        <v>3</v>
+      </c>
+      <c r="I12" s="1" t="n">
+        <v>44737</v>
+      </c>
+      <c r="J12" t="inlineStr">
+        <is>
+          <t>БНХ Польска</t>
+        </is>
+      </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
@@ -642,6 +961,32 @@
           <t>18 сер груз</t>
         </is>
       </c>
+      <c r="E13" t="inlineStr">
+        <is>
+          <t>12.00R20</t>
+        </is>
+      </c>
+      <c r="F13" t="inlineStr">
+        <is>
+          <t>ИД-304М</t>
+        </is>
+      </c>
+      <c r="G13" t="inlineStr">
+        <is>
+          <t>16, сер, груз</t>
+        </is>
+      </c>
+      <c r="H13" t="n">
+        <v>3</v>
+      </c>
+      <c r="I13" s="1" t="n">
+        <v>44737</v>
+      </c>
+      <c r="J13" t="inlineStr">
+        <is>
+          <t>БНХ Польска</t>
+        </is>
+      </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
@@ -659,6 +1004,32 @@
           <t>16 груз трп</t>
         </is>
       </c>
+      <c r="E14" t="inlineStr">
+        <is>
+          <t>12.00R20</t>
+        </is>
+      </c>
+      <c r="F14" t="inlineStr">
+        <is>
+          <t>ИД-304М</t>
+        </is>
+      </c>
+      <c r="G14" t="inlineStr">
+        <is>
+          <t>18, сер, груз</t>
+        </is>
+      </c>
+      <c r="H14" t="n">
+        <v>3</v>
+      </c>
+      <c r="I14" s="1" t="n">
+        <v>44737</v>
+      </c>
+      <c r="J14" t="inlineStr">
+        <is>
+          <t>БНХ Польска</t>
+        </is>
+      </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
@@ -676,6 +1047,32 @@
           <t>18 груз трп</t>
         </is>
       </c>
+      <c r="E15" t="inlineStr">
+        <is>
+          <t>12.00R20</t>
+        </is>
+      </c>
+      <c r="F15" t="inlineStr">
+        <is>
+          <t>ИД-304М</t>
+        </is>
+      </c>
+      <c r="G15" t="inlineStr">
+        <is>
+          <t>16, груз, трп</t>
+        </is>
+      </c>
+      <c r="H15" t="n">
+        <v>3</v>
+      </c>
+      <c r="I15" s="1" t="n">
+        <v>44737</v>
+      </c>
+      <c r="J15" t="inlineStr">
+        <is>
+          <t>БНХ Польска</t>
+        </is>
+      </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
@@ -693,6 +1090,32 @@
           <t>18 сер груз</t>
         </is>
       </c>
+      <c r="E16" t="inlineStr">
+        <is>
+          <t>12.00R20</t>
+        </is>
+      </c>
+      <c r="F16" t="inlineStr">
+        <is>
+          <t>ИД-304М</t>
+        </is>
+      </c>
+      <c r="G16" t="inlineStr">
+        <is>
+          <t>18, груз, трп</t>
+        </is>
+      </c>
+      <c r="H16" t="n">
+        <v>3</v>
+      </c>
+      <c r="I16" s="1" t="n">
+        <v>44737</v>
+      </c>
+      <c r="J16" t="inlineStr">
+        <is>
+          <t>БНХ Польска</t>
+        </is>
+      </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
@@ -710,6 +1133,32 @@
           <t>18 сер груз</t>
         </is>
       </c>
+      <c r="E17" t="inlineStr">
+        <is>
+          <t>12.00R20</t>
+        </is>
+      </c>
+      <c r="F17" t="inlineStr">
+        <is>
+          <t>БИ-368М</t>
+        </is>
+      </c>
+      <c r="G17" t="inlineStr">
+        <is>
+          <t>18, сер, груз</t>
+        </is>
+      </c>
+      <c r="H17" t="n">
+        <v>3</v>
+      </c>
+      <c r="I17" s="1" t="n">
+        <v>44737</v>
+      </c>
+      <c r="J17" t="inlineStr">
+        <is>
+          <t>БНХ Польска</t>
+        </is>
+      </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
@@ -725,6 +1174,1068 @@
       <c r="C18" t="inlineStr">
         <is>
           <t>18 груз трп</t>
+        </is>
+      </c>
+      <c r="E18" t="inlineStr">
+        <is>
+          <t>12.00R20</t>
+        </is>
+      </c>
+      <c r="F18" t="inlineStr">
+        <is>
+          <t>БИ-368М</t>
+        </is>
+      </c>
+      <c r="G18" t="inlineStr">
+        <is>
+          <t>18, сер, груз</t>
+        </is>
+      </c>
+      <c r="H18" t="n">
+        <v>4</v>
+      </c>
+      <c r="I18" s="1" t="n">
+        <v>44737</v>
+      </c>
+      <c r="J18" t="inlineStr">
+        <is>
+          <t>БНХ Польска</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="E19" t="inlineStr">
+        <is>
+          <t>12.00R20</t>
+        </is>
+      </c>
+      <c r="F19" t="inlineStr">
+        <is>
+          <t>БИ-368М</t>
+        </is>
+      </c>
+      <c r="G19" t="inlineStr">
+        <is>
+          <t>18, груз, трп</t>
+        </is>
+      </c>
+      <c r="H19" t="n">
+        <v>3</v>
+      </c>
+      <c r="I19" s="1" t="n">
+        <v>44737</v>
+      </c>
+      <c r="J19" t="inlineStr">
+        <is>
+          <t>БНХ Польска</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="E20" t="inlineStr">
+        <is>
+          <t>315/80R22.5</t>
+        </is>
+      </c>
+      <c r="F20" t="inlineStr">
+        <is>
+          <t>BEL-158M</t>
+        </is>
+      </c>
+      <c r="G20" t="inlineStr">
+        <is>
+          <t>сер, груз, камневыт</t>
+        </is>
+      </c>
+      <c r="H20" t="n">
+        <v>3</v>
+      </c>
+      <c r="I20" s="1" t="n">
+        <v>44767</v>
+      </c>
+      <c r="J20" t="inlineStr">
+        <is>
+          <t>БНХ Польска</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="E21" t="inlineStr">
+        <is>
+          <t>315/80R22.5</t>
+        </is>
+      </c>
+      <c r="F21" t="inlineStr">
+        <is>
+          <t>BEL-158M</t>
+        </is>
+      </c>
+      <c r="G21" t="inlineStr">
+        <is>
+          <t>груз, камневыт, трп</t>
+        </is>
+      </c>
+      <c r="H21" t="n">
+        <v>3</v>
+      </c>
+      <c r="I21" s="1" t="n">
+        <v>44767</v>
+      </c>
+      <c r="J21" t="inlineStr">
+        <is>
+          <t>БНХ Польска</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="E22" t="inlineStr">
+        <is>
+          <t>315/80R22.5</t>
+        </is>
+      </c>
+      <c r="F22" t="inlineStr">
+        <is>
+          <t>BEL-278</t>
+        </is>
+      </c>
+      <c r="G22" t="inlineStr">
+        <is>
+          <t>сер, груз</t>
+        </is>
+      </c>
+      <c r="H22" t="n">
+        <v>3</v>
+      </c>
+      <c r="I22" s="1" t="n">
+        <v>44767</v>
+      </c>
+      <c r="J22" t="inlineStr">
+        <is>
+          <t>БНХ Польска</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="E23" t="inlineStr">
+        <is>
+          <t>315/80R22.5</t>
+        </is>
+      </c>
+      <c r="F23" t="inlineStr">
+        <is>
+          <t>BEL-278</t>
+        </is>
+      </c>
+      <c r="G23" t="inlineStr">
+        <is>
+          <t>груз, трп</t>
+        </is>
+      </c>
+      <c r="H23" t="n">
+        <v>3</v>
+      </c>
+      <c r="I23" s="1" t="n">
+        <v>44767</v>
+      </c>
+      <c r="J23" t="inlineStr">
+        <is>
+          <t>БНХ Польска</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="E24" t="inlineStr">
+        <is>
+          <t>315/80R22.5</t>
+        </is>
+      </c>
+      <c r="F24" t="inlineStr">
+        <is>
+          <t>BEL-268</t>
+        </is>
+      </c>
+      <c r="G24" t="inlineStr">
+        <is>
+          <t>сер, груз</t>
+        </is>
+      </c>
+      <c r="H24" t="n">
+        <v>3</v>
+      </c>
+      <c r="I24" s="1" t="n">
+        <v>44767</v>
+      </c>
+      <c r="J24" t="inlineStr">
+        <is>
+          <t>БНХ Польска</t>
+        </is>
+      </c>
+    </row>
+    <row r="25">
+      <c r="E25" t="inlineStr">
+        <is>
+          <t>315/80R22.5</t>
+        </is>
+      </c>
+      <c r="F25" t="inlineStr">
+        <is>
+          <t>BEL-268</t>
+        </is>
+      </c>
+      <c r="G25" t="inlineStr">
+        <is>
+          <t>груз, трп</t>
+        </is>
+      </c>
+      <c r="H25" t="n">
+        <v>3</v>
+      </c>
+      <c r="I25" s="1" t="n">
+        <v>44767</v>
+      </c>
+      <c r="J25" t="inlineStr">
+        <is>
+          <t>БНХ Польска</t>
+        </is>
+      </c>
+    </row>
+    <row r="26">
+      <c r="E26" t="inlineStr">
+        <is>
+          <t>315/80R22.5</t>
+        </is>
+      </c>
+      <c r="F26" t="inlineStr">
+        <is>
+          <t>BEL-398</t>
+        </is>
+      </c>
+      <c r="G26" t="inlineStr">
+        <is>
+          <t>сер, груз</t>
+        </is>
+      </c>
+      <c r="H26" t="n">
+        <v>3</v>
+      </c>
+      <c r="I26" s="1" t="n">
+        <v>44767</v>
+      </c>
+      <c r="J26" t="inlineStr">
+        <is>
+          <t>БНХ Польска</t>
+        </is>
+      </c>
+    </row>
+    <row r="27">
+      <c r="E27" t="inlineStr">
+        <is>
+          <t>315/80R22.5</t>
+        </is>
+      </c>
+      <c r="F27" t="inlineStr">
+        <is>
+          <t>BEL-326</t>
+        </is>
+      </c>
+      <c r="G27" t="inlineStr">
+        <is>
+          <t>сер, груз</t>
+        </is>
+      </c>
+      <c r="H27" t="n">
+        <v>3</v>
+      </c>
+      <c r="I27" s="1" t="n">
+        <v>44767</v>
+      </c>
+      <c r="J27" t="inlineStr">
+        <is>
+          <t>БНХ Польска</t>
+        </is>
+      </c>
+    </row>
+    <row r="28">
+      <c r="E28" t="inlineStr">
+        <is>
+          <t>315/80R22.5</t>
+        </is>
+      </c>
+      <c r="F28" t="inlineStr">
+        <is>
+          <t>BEL-326</t>
+        </is>
+      </c>
+      <c r="G28" t="inlineStr">
+        <is>
+          <t>груз, трп</t>
+        </is>
+      </c>
+      <c r="H28" t="n">
+        <v>3</v>
+      </c>
+      <c r="I28" s="1" t="n">
+        <v>44767</v>
+      </c>
+      <c r="J28" t="inlineStr">
+        <is>
+          <t>БНХ Польска</t>
+        </is>
+      </c>
+    </row>
+    <row r="29">
+      <c r="E29" t="inlineStr">
+        <is>
+          <t>315/80R22.5</t>
+        </is>
+      </c>
+      <c r="F29" t="inlineStr">
+        <is>
+          <t>BEL-498</t>
+        </is>
+      </c>
+      <c r="G29" t="inlineStr">
+        <is>
+          <t>156L, сер, груз</t>
+        </is>
+      </c>
+      <c r="H29" t="n">
+        <v>3</v>
+      </c>
+      <c r="I29" s="1" t="n">
+        <v>44767</v>
+      </c>
+      <c r="J29" t="inlineStr">
+        <is>
+          <t>БНХ Польска</t>
+        </is>
+      </c>
+    </row>
+    <row r="30">
+      <c r="E30" t="inlineStr">
+        <is>
+          <t>315/80R22.5</t>
+        </is>
+      </c>
+      <c r="F30" t="inlineStr">
+        <is>
+          <t>BEL-518</t>
+        </is>
+      </c>
+      <c r="G30" t="inlineStr">
+        <is>
+          <t>сер, груз</t>
+        </is>
+      </c>
+      <c r="H30" t="n">
+        <v>3</v>
+      </c>
+      <c r="I30" s="1" t="n">
+        <v>44767</v>
+      </c>
+      <c r="J30" t="inlineStr">
+        <is>
+          <t>БНХ Польска</t>
+        </is>
+      </c>
+    </row>
+    <row r="31">
+      <c r="E31" t="inlineStr">
+        <is>
+          <t>12.00R20</t>
+        </is>
+      </c>
+      <c r="F31" t="inlineStr">
+        <is>
+          <t>ИД-304М</t>
+        </is>
+      </c>
+      <c r="G31" t="inlineStr">
+        <is>
+          <t>16, сер, груз</t>
+        </is>
+      </c>
+      <c r="H31" t="n">
+        <v>3</v>
+      </c>
+      <c r="I31" s="1" t="n">
+        <v>44767</v>
+      </c>
+      <c r="J31" t="inlineStr">
+        <is>
+          <t>БНХ Польска</t>
+        </is>
+      </c>
+    </row>
+    <row r="32">
+      <c r="E32" t="inlineStr">
+        <is>
+          <t>12.00R20</t>
+        </is>
+      </c>
+      <c r="F32" t="inlineStr">
+        <is>
+          <t>ИД-304М</t>
+        </is>
+      </c>
+      <c r="G32" t="inlineStr">
+        <is>
+          <t>18, сер, груз</t>
+        </is>
+      </c>
+      <c r="H32" t="n">
+        <v>3</v>
+      </c>
+      <c r="I32" s="1" t="n">
+        <v>44767</v>
+      </c>
+      <c r="J32" t="inlineStr">
+        <is>
+          <t>БНХ Польска</t>
+        </is>
+      </c>
+    </row>
+    <row r="33">
+      <c r="E33" t="inlineStr">
+        <is>
+          <t>12.00R20</t>
+        </is>
+      </c>
+      <c r="F33" t="inlineStr">
+        <is>
+          <t>ИД-304М</t>
+        </is>
+      </c>
+      <c r="G33" t="inlineStr">
+        <is>
+          <t>16, груз, трп</t>
+        </is>
+      </c>
+      <c r="H33" t="n">
+        <v>3</v>
+      </c>
+      <c r="I33" s="1" t="n">
+        <v>44767</v>
+      </c>
+      <c r="J33" t="inlineStr">
+        <is>
+          <t>БНХ Польска</t>
+        </is>
+      </c>
+    </row>
+    <row r="34">
+      <c r="E34" t="inlineStr">
+        <is>
+          <t>12.00R20</t>
+        </is>
+      </c>
+      <c r="F34" t="inlineStr">
+        <is>
+          <t>ИД-304М</t>
+        </is>
+      </c>
+      <c r="G34" t="inlineStr">
+        <is>
+          <t>18, груз, трп</t>
+        </is>
+      </c>
+      <c r="H34" t="n">
+        <v>3</v>
+      </c>
+      <c r="I34" s="1" t="n">
+        <v>44767</v>
+      </c>
+      <c r="J34" t="inlineStr">
+        <is>
+          <t>БНХ Польска</t>
+        </is>
+      </c>
+    </row>
+    <row r="35">
+      <c r="E35" t="inlineStr">
+        <is>
+          <t>12.00R20</t>
+        </is>
+      </c>
+      <c r="F35" t="inlineStr">
+        <is>
+          <t>БИ-368М</t>
+        </is>
+      </c>
+      <c r="G35" t="inlineStr">
+        <is>
+          <t>18, сер, груз</t>
+        </is>
+      </c>
+      <c r="H35" t="n">
+        <v>3</v>
+      </c>
+      <c r="I35" s="1" t="n">
+        <v>44767</v>
+      </c>
+      <c r="J35" t="inlineStr">
+        <is>
+          <t>БНХ Польска</t>
+        </is>
+      </c>
+    </row>
+    <row r="36">
+      <c r="E36" t="inlineStr">
+        <is>
+          <t>12.00R20</t>
+        </is>
+      </c>
+      <c r="F36" t="inlineStr">
+        <is>
+          <t>БИ-368М</t>
+        </is>
+      </c>
+      <c r="G36" t="inlineStr">
+        <is>
+          <t>18, сер, груз</t>
+        </is>
+      </c>
+      <c r="H36" t="n">
+        <v>4</v>
+      </c>
+      <c r="I36" s="1" t="n">
+        <v>44767</v>
+      </c>
+      <c r="J36" t="inlineStr">
+        <is>
+          <t>БНХ Польска</t>
+        </is>
+      </c>
+    </row>
+    <row r="37">
+      <c r="E37" t="inlineStr">
+        <is>
+          <t>12.00R20</t>
+        </is>
+      </c>
+      <c r="F37" t="inlineStr">
+        <is>
+          <t>БИ-368М</t>
+        </is>
+      </c>
+      <c r="G37" t="inlineStr">
+        <is>
+          <t>18, груз, трп</t>
+        </is>
+      </c>
+      <c r="H37" t="n">
+        <v>3</v>
+      </c>
+      <c r="I37" s="1" t="n">
+        <v>44767</v>
+      </c>
+      <c r="J37" t="inlineStr">
+        <is>
+          <t>БНХ Польска</t>
+        </is>
+      </c>
+    </row>
+    <row r="38">
+      <c r="E38" t="inlineStr">
+        <is>
+          <t>315/80R22.5</t>
+        </is>
+      </c>
+      <c r="F38" t="inlineStr">
+        <is>
+          <t>BEL-158M</t>
+        </is>
+      </c>
+      <c r="G38" t="inlineStr">
+        <is>
+          <t>сер, груз, камневыт</t>
+        </is>
+      </c>
+      <c r="H38" t="n">
+        <v>3</v>
+      </c>
+      <c r="I38" s="1" t="n">
+        <v>44737</v>
+      </c>
+      <c r="J38" t="inlineStr">
+        <is>
+          <t>БНХ Польска</t>
+        </is>
+      </c>
+    </row>
+    <row r="39">
+      <c r="E39" t="inlineStr">
+        <is>
+          <t>315/80R22.5</t>
+        </is>
+      </c>
+      <c r="F39" t="inlineStr">
+        <is>
+          <t>BEL-158M</t>
+        </is>
+      </c>
+      <c r="G39" t="inlineStr">
+        <is>
+          <t>груз, камневыт, трп</t>
+        </is>
+      </c>
+      <c r="H39" t="n">
+        <v>3</v>
+      </c>
+      <c r="I39" s="1" t="n">
+        <v>44737</v>
+      </c>
+      <c r="J39" t="inlineStr">
+        <is>
+          <t>БНХ Польска</t>
+        </is>
+      </c>
+    </row>
+    <row r="40">
+      <c r="E40" t="inlineStr">
+        <is>
+          <t>315/80R22.5</t>
+        </is>
+      </c>
+      <c r="F40" t="inlineStr">
+        <is>
+          <t>BEL-278</t>
+        </is>
+      </c>
+      <c r="G40" t="inlineStr">
+        <is>
+          <t>сер, груз</t>
+        </is>
+      </c>
+      <c r="H40" t="n">
+        <v>3</v>
+      </c>
+      <c r="I40" s="1" t="n">
+        <v>44737</v>
+      </c>
+      <c r="J40" t="inlineStr">
+        <is>
+          <t>БНХ Польска</t>
+        </is>
+      </c>
+    </row>
+    <row r="41">
+      <c r="E41" t="inlineStr">
+        <is>
+          <t>315/80R22.5</t>
+        </is>
+      </c>
+      <c r="F41" t="inlineStr">
+        <is>
+          <t>BEL-278</t>
+        </is>
+      </c>
+      <c r="G41" t="inlineStr">
+        <is>
+          <t>груз, трп</t>
+        </is>
+      </c>
+      <c r="H41" t="n">
+        <v>3</v>
+      </c>
+      <c r="I41" s="1" t="n">
+        <v>44737</v>
+      </c>
+      <c r="J41" t="inlineStr">
+        <is>
+          <t>БНХ Польска</t>
+        </is>
+      </c>
+    </row>
+    <row r="42">
+      <c r="E42" t="inlineStr">
+        <is>
+          <t>315/80R22.5</t>
+        </is>
+      </c>
+      <c r="F42" t="inlineStr">
+        <is>
+          <t>BEL-268</t>
+        </is>
+      </c>
+      <c r="G42" t="inlineStr">
+        <is>
+          <t>сер, груз</t>
+        </is>
+      </c>
+      <c r="H42" t="n">
+        <v>3</v>
+      </c>
+      <c r="I42" s="1" t="n">
+        <v>44737</v>
+      </c>
+      <c r="J42" t="inlineStr">
+        <is>
+          <t>БНХ Польска</t>
+        </is>
+      </c>
+    </row>
+    <row r="43">
+      <c r="E43" t="inlineStr">
+        <is>
+          <t>315/80R22.5</t>
+        </is>
+      </c>
+      <c r="F43" t="inlineStr">
+        <is>
+          <t>BEL-268</t>
+        </is>
+      </c>
+      <c r="G43" t="inlineStr">
+        <is>
+          <t>груз, трп</t>
+        </is>
+      </c>
+      <c r="H43" t="n">
+        <v>3</v>
+      </c>
+      <c r="I43" s="1" t="n">
+        <v>44737</v>
+      </c>
+      <c r="J43" t="inlineStr">
+        <is>
+          <t>БНХ Польска</t>
+        </is>
+      </c>
+    </row>
+    <row r="44">
+      <c r="E44" t="inlineStr">
+        <is>
+          <t>315/80R22.5</t>
+        </is>
+      </c>
+      <c r="F44" t="inlineStr">
+        <is>
+          <t>BEL-398</t>
+        </is>
+      </c>
+      <c r="G44" t="inlineStr">
+        <is>
+          <t>сер, груз</t>
+        </is>
+      </c>
+      <c r="H44" t="n">
+        <v>3</v>
+      </c>
+      <c r="I44" s="1" t="n">
+        <v>44737</v>
+      </c>
+      <c r="J44" t="inlineStr">
+        <is>
+          <t>БНХ Польска</t>
+        </is>
+      </c>
+    </row>
+    <row r="45">
+      <c r="E45" t="inlineStr">
+        <is>
+          <t>315/80R22.5</t>
+        </is>
+      </c>
+      <c r="F45" t="inlineStr">
+        <is>
+          <t>BEL-326</t>
+        </is>
+      </c>
+      <c r="G45" t="inlineStr">
+        <is>
+          <t>сер, груз</t>
+        </is>
+      </c>
+      <c r="H45" t="n">
+        <v>3</v>
+      </c>
+      <c r="I45" s="1" t="n">
+        <v>44737</v>
+      </c>
+      <c r="J45" t="inlineStr">
+        <is>
+          <t>БНХ Польска</t>
+        </is>
+      </c>
+    </row>
+    <row r="46">
+      <c r="E46" t="inlineStr">
+        <is>
+          <t>315/80R22.5</t>
+        </is>
+      </c>
+      <c r="F46" t="inlineStr">
+        <is>
+          <t>BEL-326</t>
+        </is>
+      </c>
+      <c r="G46" t="inlineStr">
+        <is>
+          <t>груз, трп</t>
+        </is>
+      </c>
+      <c r="H46" t="n">
+        <v>3</v>
+      </c>
+      <c r="I46" s="1" t="n">
+        <v>44737</v>
+      </c>
+      <c r="J46" t="inlineStr">
+        <is>
+          <t>БНХ Польска</t>
+        </is>
+      </c>
+    </row>
+    <row r="47">
+      <c r="E47" t="inlineStr">
+        <is>
+          <t>315/80R22.5</t>
+        </is>
+      </c>
+      <c r="F47" t="inlineStr">
+        <is>
+          <t>BEL-498</t>
+        </is>
+      </c>
+      <c r="G47" t="inlineStr">
+        <is>
+          <t>156L, сер, груз</t>
+        </is>
+      </c>
+      <c r="H47" t="n">
+        <v>3</v>
+      </c>
+      <c r="I47" s="1" t="n">
+        <v>44737</v>
+      </c>
+      <c r="J47" t="inlineStr">
+        <is>
+          <t>БНХ Польска</t>
+        </is>
+      </c>
+    </row>
+    <row r="48">
+      <c r="E48" t="inlineStr">
+        <is>
+          <t>315/80R22.5</t>
+        </is>
+      </c>
+      <c r="F48" t="inlineStr">
+        <is>
+          <t>BEL-518</t>
+        </is>
+      </c>
+      <c r="G48" t="inlineStr">
+        <is>
+          <t>сер, груз</t>
+        </is>
+      </c>
+      <c r="H48" t="n">
+        <v>3</v>
+      </c>
+      <c r="I48" s="1" t="n">
+        <v>44737</v>
+      </c>
+      <c r="J48" t="inlineStr">
+        <is>
+          <t>БНХ Польска</t>
+        </is>
+      </c>
+    </row>
+    <row r="49">
+      <c r="E49" t="inlineStr">
+        <is>
+          <t>12.00R20</t>
+        </is>
+      </c>
+      <c r="F49" t="inlineStr">
+        <is>
+          <t>ИД-304М</t>
+        </is>
+      </c>
+      <c r="G49" t="inlineStr">
+        <is>
+          <t>16, сер, груз</t>
+        </is>
+      </c>
+      <c r="H49" t="n">
+        <v>3</v>
+      </c>
+      <c r="I49" s="1" t="n">
+        <v>44737</v>
+      </c>
+      <c r="J49" t="inlineStr">
+        <is>
+          <t>БНХ Польска</t>
+        </is>
+      </c>
+    </row>
+    <row r="50">
+      <c r="E50" t="inlineStr">
+        <is>
+          <t>12.00R20</t>
+        </is>
+      </c>
+      <c r="F50" t="inlineStr">
+        <is>
+          <t>ИД-304М</t>
+        </is>
+      </c>
+      <c r="G50" t="inlineStr">
+        <is>
+          <t>18, сер, груз</t>
+        </is>
+      </c>
+      <c r="H50" t="n">
+        <v>3</v>
+      </c>
+      <c r="I50" s="1" t="n">
+        <v>44737</v>
+      </c>
+      <c r="J50" t="inlineStr">
+        <is>
+          <t>БНХ Польска</t>
+        </is>
+      </c>
+    </row>
+    <row r="51">
+      <c r="E51" t="inlineStr">
+        <is>
+          <t>12.00R20</t>
+        </is>
+      </c>
+      <c r="F51" t="inlineStr">
+        <is>
+          <t>ИД-304М</t>
+        </is>
+      </c>
+      <c r="G51" t="inlineStr">
+        <is>
+          <t>16, груз, трп</t>
+        </is>
+      </c>
+      <c r="H51" t="n">
+        <v>3</v>
+      </c>
+      <c r="I51" s="1" t="n">
+        <v>44737</v>
+      </c>
+      <c r="J51" t="inlineStr">
+        <is>
+          <t>БНХ Польска</t>
+        </is>
+      </c>
+    </row>
+    <row r="52">
+      <c r="E52" t="inlineStr">
+        <is>
+          <t>12.00R20</t>
+        </is>
+      </c>
+      <c r="F52" t="inlineStr">
+        <is>
+          <t>ИД-304М</t>
+        </is>
+      </c>
+      <c r="G52" t="inlineStr">
+        <is>
+          <t>18, груз, трп</t>
+        </is>
+      </c>
+      <c r="H52" t="n">
+        <v>3</v>
+      </c>
+      <c r="I52" s="1" t="n">
+        <v>44737</v>
+      </c>
+      <c r="J52" t="inlineStr">
+        <is>
+          <t>БНХ Польска</t>
+        </is>
+      </c>
+    </row>
+    <row r="53">
+      <c r="E53" t="inlineStr">
+        <is>
+          <t>12.00R20</t>
+        </is>
+      </c>
+      <c r="F53" t="inlineStr">
+        <is>
+          <t>БИ-368М</t>
+        </is>
+      </c>
+      <c r="G53" t="inlineStr">
+        <is>
+          <t>18, сер, груз</t>
+        </is>
+      </c>
+      <c r="H53" t="n">
+        <v>3</v>
+      </c>
+      <c r="I53" s="1" t="n">
+        <v>44737</v>
+      </c>
+      <c r="J53" t="inlineStr">
+        <is>
+          <t>БНХ Польска</t>
+        </is>
+      </c>
+    </row>
+    <row r="54">
+      <c r="E54" t="inlineStr">
+        <is>
+          <t>12.00R20</t>
+        </is>
+      </c>
+      <c r="F54" t="inlineStr">
+        <is>
+          <t>БИ-368М</t>
+        </is>
+      </c>
+      <c r="G54" t="inlineStr">
+        <is>
+          <t>18, сер, груз</t>
+        </is>
+      </c>
+      <c r="H54" t="n">
+        <v>4</v>
+      </c>
+      <c r="I54" s="1" t="n">
+        <v>44737</v>
+      </c>
+      <c r="J54" t="inlineStr">
+        <is>
+          <t>БНХ Польска</t>
+        </is>
+      </c>
+    </row>
+    <row r="55">
+      <c r="E55" t="inlineStr">
+        <is>
+          <t>12.00R20</t>
+        </is>
+      </c>
+      <c r="F55" t="inlineStr">
+        <is>
+          <t>БИ-368М</t>
+        </is>
+      </c>
+      <c r="G55" t="inlineStr">
+        <is>
+          <t>18, груз, трп</t>
+        </is>
+      </c>
+      <c r="H55" t="n">
+        <v>3</v>
+      </c>
+      <c r="I55" s="1" t="n">
+        <v>44737</v>
+      </c>
+      <c r="J55" t="inlineStr">
+        <is>
+          <t>БНХ Польска</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
home GROUPS new at 05/09/2022
</commit_message>
<xml_diff>
--- a/src/Tyres.xlsx
+++ b/src/Tyres.xlsx
@@ -17,7 +17,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="0"/>
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="yyyy-mm-dd"/>
+  </numFmts>
   <fonts count="1">
     <font>
       <name val="Calibri"/>
@@ -47,8 +49,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
@@ -414,7 +417,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C18"/>
+  <dimension ref="A1:J39"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -435,7 +438,37 @@
       </c>
       <c r="C1" t="inlineStr">
         <is>
-          <t>сер груз камневыт</t>
+          <t>груз камневыт сер</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>Tyre Size</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>Model</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
+        <is>
+          <t>Param</t>
+        </is>
+      </c>
+      <c r="H1" t="inlineStr">
+        <is>
+          <t>Sales value</t>
+        </is>
+      </c>
+      <c r="I1" t="inlineStr">
+        <is>
+          <t>Date_of_sales</t>
+        </is>
+      </c>
+      <c r="J1" t="inlineStr">
+        <is>
+          <t>Contragent</t>
         </is>
       </c>
     </row>
@@ -455,6 +488,32 @@
           <t>груз трп камневыт</t>
         </is>
       </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>315/80R22.5</t>
+        </is>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>BEL-158M</t>
+        </is>
+      </c>
+      <c r="G2" t="inlineStr">
+        <is>
+          <t>груз, камневыт, сер</t>
+        </is>
+      </c>
+      <c r="H2" t="n">
+        <v>12</v>
+      </c>
+      <c r="I2" s="1" t="n">
+        <v>44689</v>
+      </c>
+      <c r="J2" t="inlineStr">
+        <is>
+          <t>БНХ РОС</t>
+        </is>
+      </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -469,7 +528,33 @@
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>сер груз</t>
+          <t>груз сер</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>315/80R22.5</t>
+        </is>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>BEL-158M</t>
+        </is>
+      </c>
+      <c r="G3" t="inlineStr">
+        <is>
+          <t>груз, трп, камневыт</t>
+        </is>
+      </c>
+      <c r="H3" t="n">
+        <v>12</v>
+      </c>
+      <c r="I3" s="1" t="n">
+        <v>44689</v>
+      </c>
+      <c r="J3" t="inlineStr">
+        <is>
+          <t>БНХ РОС</t>
         </is>
       </c>
     </row>
@@ -489,6 +574,32 @@
           <t>груз трп</t>
         </is>
       </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>315/80R22.5</t>
+        </is>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>BEL-278</t>
+        </is>
+      </c>
+      <c r="G4" t="inlineStr">
+        <is>
+          <t>груз, сер</t>
+        </is>
+      </c>
+      <c r="H4" t="n">
+        <v>12</v>
+      </c>
+      <c r="I4" s="1" t="n">
+        <v>44689</v>
+      </c>
+      <c r="J4" t="inlineStr">
+        <is>
+          <t>БНХ РОС</t>
+        </is>
+      </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
@@ -503,7 +614,33 @@
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>сер груз</t>
+          <t>груз сер</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>315/80R22.5</t>
+        </is>
+      </c>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>BEL-278</t>
+        </is>
+      </c>
+      <c r="G5" t="inlineStr">
+        <is>
+          <t>груз, трп</t>
+        </is>
+      </c>
+      <c r="H5" t="n">
+        <v>12</v>
+      </c>
+      <c r="I5" s="1" t="n">
+        <v>44689</v>
+      </c>
+      <c r="J5" t="inlineStr">
+        <is>
+          <t>БНХ РОС</t>
         </is>
       </c>
     </row>
@@ -523,6 +660,32 @@
           <t>груз трп</t>
         </is>
       </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>315/80R22.5</t>
+        </is>
+      </c>
+      <c r="F6" t="inlineStr">
+        <is>
+          <t>BEL-268</t>
+        </is>
+      </c>
+      <c r="G6" t="inlineStr">
+        <is>
+          <t>груз, сер</t>
+        </is>
+      </c>
+      <c r="H6" t="n">
+        <v>12</v>
+      </c>
+      <c r="I6" s="1" t="n">
+        <v>44689</v>
+      </c>
+      <c r="J6" t="inlineStr">
+        <is>
+          <t>БНХ РОС</t>
+        </is>
+      </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
@@ -537,7 +700,33 @@
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>сер груз</t>
+          <t>груз сер</t>
+        </is>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>315/80R22.5</t>
+        </is>
+      </c>
+      <c r="F7" t="inlineStr">
+        <is>
+          <t>BEL-268</t>
+        </is>
+      </c>
+      <c r="G7" t="inlineStr">
+        <is>
+          <t>груз, трп</t>
+        </is>
+      </c>
+      <c r="H7" t="n">
+        <v>12</v>
+      </c>
+      <c r="I7" s="1" t="n">
+        <v>44689</v>
+      </c>
+      <c r="J7" t="inlineStr">
+        <is>
+          <t>БНХ РОС</t>
         </is>
       </c>
     </row>
@@ -554,7 +743,33 @@
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>сер груз</t>
+          <t>груз сер</t>
+        </is>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>315/80R22.5</t>
+        </is>
+      </c>
+      <c r="F8" t="inlineStr">
+        <is>
+          <t>BEL-398</t>
+        </is>
+      </c>
+      <c r="G8" t="inlineStr">
+        <is>
+          <t>груз, сер</t>
+        </is>
+      </c>
+      <c r="H8" t="n">
+        <v>12</v>
+      </c>
+      <c r="I8" s="1" t="n">
+        <v>44689</v>
+      </c>
+      <c r="J8" t="inlineStr">
+        <is>
+          <t>БНХ РОС</t>
         </is>
       </c>
     </row>
@@ -574,6 +789,32 @@
           <t>груз трп</t>
         </is>
       </c>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>315/80R22.5</t>
+        </is>
+      </c>
+      <c r="F9" t="inlineStr">
+        <is>
+          <t>BEL-326</t>
+        </is>
+      </c>
+      <c r="G9" t="inlineStr">
+        <is>
+          <t>груз, сер</t>
+        </is>
+      </c>
+      <c r="H9" t="n">
+        <v>12</v>
+      </c>
+      <c r="I9" s="1" t="n">
+        <v>44689</v>
+      </c>
+      <c r="J9" t="inlineStr">
+        <is>
+          <t>БНХ РОС</t>
+        </is>
+      </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
@@ -588,7 +829,33 @@
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>156L сер груз</t>
+          <t>156L груз сер</t>
+        </is>
+      </c>
+      <c r="E10" t="inlineStr">
+        <is>
+          <t>315/80R22.5</t>
+        </is>
+      </c>
+      <c r="F10" t="inlineStr">
+        <is>
+          <t>BEL-326</t>
+        </is>
+      </c>
+      <c r="G10" t="inlineStr">
+        <is>
+          <t>груз, трп</t>
+        </is>
+      </c>
+      <c r="H10" t="n">
+        <v>12</v>
+      </c>
+      <c r="I10" s="1" t="n">
+        <v>44689</v>
+      </c>
+      <c r="J10" t="inlineStr">
+        <is>
+          <t>БНХ РОС</t>
         </is>
       </c>
     </row>
@@ -605,7 +872,33 @@
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>сер груз</t>
+          <t>груз сер</t>
+        </is>
+      </c>
+      <c r="E11" t="inlineStr">
+        <is>
+          <t>315/80R22.5</t>
+        </is>
+      </c>
+      <c r="F11" t="inlineStr">
+        <is>
+          <t>BEL-498</t>
+        </is>
+      </c>
+      <c r="G11" t="inlineStr">
+        <is>
+          <t>156L, груз, сер</t>
+        </is>
+      </c>
+      <c r="H11" t="n">
+        <v>12</v>
+      </c>
+      <c r="I11" s="1" t="n">
+        <v>44689</v>
+      </c>
+      <c r="J11" t="inlineStr">
+        <is>
+          <t>БНХ РОС</t>
         </is>
       </c>
     </row>
@@ -622,7 +915,33 @@
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>16 сер груз</t>
+          <t>16 груз сер</t>
+        </is>
+      </c>
+      <c r="E12" t="inlineStr">
+        <is>
+          <t>315/80R22.5</t>
+        </is>
+      </c>
+      <c r="F12" t="inlineStr">
+        <is>
+          <t>BEL-518</t>
+        </is>
+      </c>
+      <c r="G12" t="inlineStr">
+        <is>
+          <t>груз, сер</t>
+        </is>
+      </c>
+      <c r="H12" t="n">
+        <v>12</v>
+      </c>
+      <c r="I12" s="1" t="n">
+        <v>44689</v>
+      </c>
+      <c r="J12" t="inlineStr">
+        <is>
+          <t>БНХ РОС</t>
         </is>
       </c>
     </row>
@@ -639,7 +958,33 @@
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>18 сер груз</t>
+          <t>18 груз сер</t>
+        </is>
+      </c>
+      <c r="E13" t="inlineStr">
+        <is>
+          <t>12.00R20</t>
+        </is>
+      </c>
+      <c r="F13" t="inlineStr">
+        <is>
+          <t>ИД-304М</t>
+        </is>
+      </c>
+      <c r="G13" t="inlineStr">
+        <is>
+          <t>16, груз, сер</t>
+        </is>
+      </c>
+      <c r="H13" t="n">
+        <v>12</v>
+      </c>
+      <c r="I13" s="1" t="n">
+        <v>44689</v>
+      </c>
+      <c r="J13" t="inlineStr">
+        <is>
+          <t>БНХ РОС</t>
         </is>
       </c>
     </row>
@@ -659,6 +1004,32 @@
           <t>16 груз трп</t>
         </is>
       </c>
+      <c r="E14" t="inlineStr">
+        <is>
+          <t>12.00R20</t>
+        </is>
+      </c>
+      <c r="F14" t="inlineStr">
+        <is>
+          <t>ИД-304М</t>
+        </is>
+      </c>
+      <c r="G14" t="inlineStr">
+        <is>
+          <t>18, груз, сер</t>
+        </is>
+      </c>
+      <c r="H14" t="n">
+        <v>12</v>
+      </c>
+      <c r="I14" s="1" t="n">
+        <v>44689</v>
+      </c>
+      <c r="J14" t="inlineStr">
+        <is>
+          <t>БНХ РОС</t>
+        </is>
+      </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
@@ -676,6 +1047,32 @@
           <t>18 груз трп</t>
         </is>
       </c>
+      <c r="E15" t="inlineStr">
+        <is>
+          <t>12.00R20</t>
+        </is>
+      </c>
+      <c r="F15" t="inlineStr">
+        <is>
+          <t>ИД-304М</t>
+        </is>
+      </c>
+      <c r="G15" t="inlineStr">
+        <is>
+          <t>16, груз, трп</t>
+        </is>
+      </c>
+      <c r="H15" t="n">
+        <v>12</v>
+      </c>
+      <c r="I15" s="1" t="n">
+        <v>44689</v>
+      </c>
+      <c r="J15" t="inlineStr">
+        <is>
+          <t>БНХ РОС</t>
+        </is>
+      </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
@@ -690,7 +1087,33 @@
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>18 сер груз</t>
+          <t>18 груз сер</t>
+        </is>
+      </c>
+      <c r="E16" t="inlineStr">
+        <is>
+          <t>12.00R20</t>
+        </is>
+      </c>
+      <c r="F16" t="inlineStr">
+        <is>
+          <t>ИД-304М</t>
+        </is>
+      </c>
+      <c r="G16" t="inlineStr">
+        <is>
+          <t>18, груз, трп</t>
+        </is>
+      </c>
+      <c r="H16" t="n">
+        <v>12</v>
+      </c>
+      <c r="I16" s="1" t="n">
+        <v>44689</v>
+      </c>
+      <c r="J16" t="inlineStr">
+        <is>
+          <t>БНХ РОС</t>
         </is>
       </c>
     </row>
@@ -707,7 +1130,33 @@
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>18 сер груз</t>
+          <t>18 груз сер</t>
+        </is>
+      </c>
+      <c r="E17" t="inlineStr">
+        <is>
+          <t>12.00R20</t>
+        </is>
+      </c>
+      <c r="F17" t="inlineStr">
+        <is>
+          <t>БИ-368М</t>
+        </is>
+      </c>
+      <c r="G17" t="inlineStr">
+        <is>
+          <t>18, груз, сер</t>
+        </is>
+      </c>
+      <c r="H17" t="n">
+        <v>12</v>
+      </c>
+      <c r="I17" s="1" t="n">
+        <v>44689</v>
+      </c>
+      <c r="J17" t="inlineStr">
+        <is>
+          <t>БНХ РОС</t>
         </is>
       </c>
     </row>
@@ -725,6 +1174,635 @@
       <c r="C18" t="inlineStr">
         <is>
           <t>18 груз трп</t>
+        </is>
+      </c>
+      <c r="E18" t="inlineStr">
+        <is>
+          <t>12.00R20</t>
+        </is>
+      </c>
+      <c r="F18" t="inlineStr">
+        <is>
+          <t>БИ-368М</t>
+        </is>
+      </c>
+      <c r="G18" t="inlineStr">
+        <is>
+          <t>18, груз, сер</t>
+        </is>
+      </c>
+      <c r="H18" t="n">
+        <v>12</v>
+      </c>
+      <c r="I18" s="1" t="n">
+        <v>44689</v>
+      </c>
+      <c r="J18" t="inlineStr">
+        <is>
+          <t>БНХ РОС</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>BEL-337</t>
+        </is>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>195/65R15</t>
+        </is>
+      </c>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>б/к легк сер</t>
+        </is>
+      </c>
+      <c r="E19" t="inlineStr">
+        <is>
+          <t>12.00R20</t>
+        </is>
+      </c>
+      <c r="F19" t="inlineStr">
+        <is>
+          <t>БИ-368М</t>
+        </is>
+      </c>
+      <c r="G19" t="inlineStr">
+        <is>
+          <t>18, груз, трп</t>
+        </is>
+      </c>
+      <c r="H19" t="n">
+        <v>12</v>
+      </c>
+      <c r="I19" s="1" t="n">
+        <v>44689</v>
+      </c>
+      <c r="J19" t="inlineStr">
+        <is>
+          <t>БНХ РОС</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="E20" t="inlineStr">
+        <is>
+          <t>195/65R15</t>
+        </is>
+      </c>
+      <c r="F20" t="inlineStr">
+        <is>
+          <t>BEL-337</t>
+        </is>
+      </c>
+      <c r="G20" t="inlineStr">
+        <is>
+          <t>б/к, легк, сер</t>
+        </is>
+      </c>
+      <c r="H20" t="n">
+        <v>12</v>
+      </c>
+      <c r="I20" s="1" t="n">
+        <v>44689</v>
+      </c>
+      <c r="J20" t="inlineStr">
+        <is>
+          <t>БНХ РОС</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="E21" t="inlineStr">
+        <is>
+          <t>315/80R22.5</t>
+        </is>
+      </c>
+      <c r="F21" t="inlineStr">
+        <is>
+          <t>BEL-158M</t>
+        </is>
+      </c>
+      <c r="G21" t="inlineStr">
+        <is>
+          <t>груз, камневыт, сер</t>
+        </is>
+      </c>
+      <c r="H21" t="n">
+        <v>20</v>
+      </c>
+      <c r="I21" s="1" t="n">
+        <v>44628</v>
+      </c>
+      <c r="J21" t="inlineStr">
+        <is>
+          <t>БНХ Укр</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="E22" t="inlineStr">
+        <is>
+          <t>315/80R22.5</t>
+        </is>
+      </c>
+      <c r="F22" t="inlineStr">
+        <is>
+          <t>BEL-158M</t>
+        </is>
+      </c>
+      <c r="G22" t="inlineStr">
+        <is>
+          <t>груз, трп, камневыт</t>
+        </is>
+      </c>
+      <c r="H22" t="n">
+        <v>20</v>
+      </c>
+      <c r="I22" s="1" t="n">
+        <v>44628</v>
+      </c>
+      <c r="J22" t="inlineStr">
+        <is>
+          <t>БНХ Укр</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="E23" t="inlineStr">
+        <is>
+          <t>315/80R22.5</t>
+        </is>
+      </c>
+      <c r="F23" t="inlineStr">
+        <is>
+          <t>BEL-278</t>
+        </is>
+      </c>
+      <c r="G23" t="inlineStr">
+        <is>
+          <t>груз, сер</t>
+        </is>
+      </c>
+      <c r="H23" t="n">
+        <v>20</v>
+      </c>
+      <c r="I23" s="1" t="n">
+        <v>44628</v>
+      </c>
+      <c r="J23" t="inlineStr">
+        <is>
+          <t>БНХ Укр</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="E24" t="inlineStr">
+        <is>
+          <t>315/80R22.5</t>
+        </is>
+      </c>
+      <c r="F24" t="inlineStr">
+        <is>
+          <t>BEL-278</t>
+        </is>
+      </c>
+      <c r="G24" t="inlineStr">
+        <is>
+          <t>груз, трп</t>
+        </is>
+      </c>
+      <c r="H24" t="n">
+        <v>20</v>
+      </c>
+      <c r="I24" s="1" t="n">
+        <v>44628</v>
+      </c>
+      <c r="J24" t="inlineStr">
+        <is>
+          <t>БНХ Укр</t>
+        </is>
+      </c>
+    </row>
+    <row r="25">
+      <c r="E25" t="inlineStr">
+        <is>
+          <t>315/80R22.5</t>
+        </is>
+      </c>
+      <c r="F25" t="inlineStr">
+        <is>
+          <t>BEL-268</t>
+        </is>
+      </c>
+      <c r="G25" t="inlineStr">
+        <is>
+          <t>груз, сер</t>
+        </is>
+      </c>
+      <c r="H25" t="n">
+        <v>20</v>
+      </c>
+      <c r="I25" s="1" t="n">
+        <v>44628</v>
+      </c>
+      <c r="J25" t="inlineStr">
+        <is>
+          <t>БНХ Укр</t>
+        </is>
+      </c>
+    </row>
+    <row r="26">
+      <c r="E26" t="inlineStr">
+        <is>
+          <t>315/80R22.5</t>
+        </is>
+      </c>
+      <c r="F26" t="inlineStr">
+        <is>
+          <t>BEL-268</t>
+        </is>
+      </c>
+      <c r="G26" t="inlineStr">
+        <is>
+          <t>груз, трп</t>
+        </is>
+      </c>
+      <c r="H26" t="n">
+        <v>20</v>
+      </c>
+      <c r="I26" s="1" t="n">
+        <v>44628</v>
+      </c>
+      <c r="J26" t="inlineStr">
+        <is>
+          <t>БНХ Укр</t>
+        </is>
+      </c>
+    </row>
+    <row r="27">
+      <c r="E27" t="inlineStr">
+        <is>
+          <t>315/80R22.5</t>
+        </is>
+      </c>
+      <c r="F27" t="inlineStr">
+        <is>
+          <t>BEL-398</t>
+        </is>
+      </c>
+      <c r="G27" t="inlineStr">
+        <is>
+          <t>груз, сер</t>
+        </is>
+      </c>
+      <c r="H27" t="n">
+        <v>20</v>
+      </c>
+      <c r="I27" s="1" t="n">
+        <v>44628</v>
+      </c>
+      <c r="J27" t="inlineStr">
+        <is>
+          <t>БНХ Укр</t>
+        </is>
+      </c>
+    </row>
+    <row r="28">
+      <c r="E28" t="inlineStr">
+        <is>
+          <t>315/80R22.5</t>
+        </is>
+      </c>
+      <c r="F28" t="inlineStr">
+        <is>
+          <t>BEL-326</t>
+        </is>
+      </c>
+      <c r="G28" t="inlineStr">
+        <is>
+          <t>груз, сер</t>
+        </is>
+      </c>
+      <c r="H28" t="n">
+        <v>20</v>
+      </c>
+      <c r="I28" s="1" t="n">
+        <v>44628</v>
+      </c>
+      <c r="J28" t="inlineStr">
+        <is>
+          <t>БНХ Укр</t>
+        </is>
+      </c>
+    </row>
+    <row r="29">
+      <c r="E29" t="inlineStr">
+        <is>
+          <t>315/80R22.5</t>
+        </is>
+      </c>
+      <c r="F29" t="inlineStr">
+        <is>
+          <t>BEL-326</t>
+        </is>
+      </c>
+      <c r="G29" t="inlineStr">
+        <is>
+          <t>груз, трп</t>
+        </is>
+      </c>
+      <c r="H29" t="n">
+        <v>20</v>
+      </c>
+      <c r="I29" s="1" t="n">
+        <v>44628</v>
+      </c>
+      <c r="J29" t="inlineStr">
+        <is>
+          <t>БНХ Укр</t>
+        </is>
+      </c>
+    </row>
+    <row r="30">
+      <c r="E30" t="inlineStr">
+        <is>
+          <t>315/80R22.5</t>
+        </is>
+      </c>
+      <c r="F30" t="inlineStr">
+        <is>
+          <t>BEL-498</t>
+        </is>
+      </c>
+      <c r="G30" t="inlineStr">
+        <is>
+          <t>156L, груз, сер</t>
+        </is>
+      </c>
+      <c r="H30" t="n">
+        <v>20</v>
+      </c>
+      <c r="I30" s="1" t="n">
+        <v>44628</v>
+      </c>
+      <c r="J30" t="inlineStr">
+        <is>
+          <t>БНХ Укр</t>
+        </is>
+      </c>
+    </row>
+    <row r="31">
+      <c r="E31" t="inlineStr">
+        <is>
+          <t>315/80R22.5</t>
+        </is>
+      </c>
+      <c r="F31" t="inlineStr">
+        <is>
+          <t>BEL-518</t>
+        </is>
+      </c>
+      <c r="G31" t="inlineStr">
+        <is>
+          <t>груз, сер</t>
+        </is>
+      </c>
+      <c r="H31" t="n">
+        <v>20</v>
+      </c>
+      <c r="I31" s="1" t="n">
+        <v>44628</v>
+      </c>
+      <c r="J31" t="inlineStr">
+        <is>
+          <t>БНХ Укр</t>
+        </is>
+      </c>
+    </row>
+    <row r="32">
+      <c r="E32" t="inlineStr">
+        <is>
+          <t>12.00R20</t>
+        </is>
+      </c>
+      <c r="F32" t="inlineStr">
+        <is>
+          <t>ИД-304М</t>
+        </is>
+      </c>
+      <c r="G32" t="inlineStr">
+        <is>
+          <t>16, груз, сер</t>
+        </is>
+      </c>
+      <c r="H32" t="n">
+        <v>20</v>
+      </c>
+      <c r="I32" s="1" t="n">
+        <v>44628</v>
+      </c>
+      <c r="J32" t="inlineStr">
+        <is>
+          <t>БНХ Укр</t>
+        </is>
+      </c>
+    </row>
+    <row r="33">
+      <c r="E33" t="inlineStr">
+        <is>
+          <t>12.00R20</t>
+        </is>
+      </c>
+      <c r="F33" t="inlineStr">
+        <is>
+          <t>ИД-304М</t>
+        </is>
+      </c>
+      <c r="G33" t="inlineStr">
+        <is>
+          <t>18, груз, сер</t>
+        </is>
+      </c>
+      <c r="H33" t="n">
+        <v>20</v>
+      </c>
+      <c r="I33" s="1" t="n">
+        <v>44628</v>
+      </c>
+      <c r="J33" t="inlineStr">
+        <is>
+          <t>БНХ Укр</t>
+        </is>
+      </c>
+    </row>
+    <row r="34">
+      <c r="E34" t="inlineStr">
+        <is>
+          <t>12.00R20</t>
+        </is>
+      </c>
+      <c r="F34" t="inlineStr">
+        <is>
+          <t>ИД-304М</t>
+        </is>
+      </c>
+      <c r="G34" t="inlineStr">
+        <is>
+          <t>16, груз, трп</t>
+        </is>
+      </c>
+      <c r="H34" t="n">
+        <v>20</v>
+      </c>
+      <c r="I34" s="1" t="n">
+        <v>44628</v>
+      </c>
+      <c r="J34" t="inlineStr">
+        <is>
+          <t>БНХ Укр</t>
+        </is>
+      </c>
+    </row>
+    <row r="35">
+      <c r="E35" t="inlineStr">
+        <is>
+          <t>12.00R20</t>
+        </is>
+      </c>
+      <c r="F35" t="inlineStr">
+        <is>
+          <t>ИД-304М</t>
+        </is>
+      </c>
+      <c r="G35" t="inlineStr">
+        <is>
+          <t>18, груз, трп</t>
+        </is>
+      </c>
+      <c r="H35" t="n">
+        <v>20</v>
+      </c>
+      <c r="I35" s="1" t="n">
+        <v>44628</v>
+      </c>
+      <c r="J35" t="inlineStr">
+        <is>
+          <t>БНХ Укр</t>
+        </is>
+      </c>
+    </row>
+    <row r="36">
+      <c r="E36" t="inlineStr">
+        <is>
+          <t>12.00R20</t>
+        </is>
+      </c>
+      <c r="F36" t="inlineStr">
+        <is>
+          <t>БИ-368М</t>
+        </is>
+      </c>
+      <c r="G36" t="inlineStr">
+        <is>
+          <t>18, груз, сер</t>
+        </is>
+      </c>
+      <c r="H36" t="n">
+        <v>20</v>
+      </c>
+      <c r="I36" s="1" t="n">
+        <v>44628</v>
+      </c>
+      <c r="J36" t="inlineStr">
+        <is>
+          <t>БНХ Укр</t>
+        </is>
+      </c>
+    </row>
+    <row r="37">
+      <c r="E37" t="inlineStr">
+        <is>
+          <t>12.00R20</t>
+        </is>
+      </c>
+      <c r="F37" t="inlineStr">
+        <is>
+          <t>БИ-368М</t>
+        </is>
+      </c>
+      <c r="G37" t="inlineStr">
+        <is>
+          <t>18, груз, сер</t>
+        </is>
+      </c>
+      <c r="H37" t="n">
+        <v>20</v>
+      </c>
+      <c r="I37" s="1" t="n">
+        <v>44628</v>
+      </c>
+      <c r="J37" t="inlineStr">
+        <is>
+          <t>БНХ Укр</t>
+        </is>
+      </c>
+    </row>
+    <row r="38">
+      <c r="E38" t="inlineStr">
+        <is>
+          <t>12.00R20</t>
+        </is>
+      </c>
+      <c r="F38" t="inlineStr">
+        <is>
+          <t>БИ-368М</t>
+        </is>
+      </c>
+      <c r="G38" t="inlineStr">
+        <is>
+          <t>18, груз, трп</t>
+        </is>
+      </c>
+      <c r="H38" t="n">
+        <v>20</v>
+      </c>
+      <c r="I38" s="1" t="n">
+        <v>44628</v>
+      </c>
+      <c r="J38" t="inlineStr">
+        <is>
+          <t>БНХ Укр</t>
+        </is>
+      </c>
+    </row>
+    <row r="39">
+      <c r="E39" t="inlineStr">
+        <is>
+          <t>195/65R15</t>
+        </is>
+      </c>
+      <c r="F39" t="inlineStr">
+        <is>
+          <t>BEL-337</t>
+        </is>
+      </c>
+      <c r="G39" t="inlineStr">
+        <is>
+          <t>б/к, легк, сер</t>
+        </is>
+      </c>
+      <c r="H39" t="n">
+        <v>20</v>
+      </c>
+      <c r="I39" s="1" t="n">
+        <v>44628</v>
+      </c>
+      <c r="J39" t="inlineStr">
+        <is>
+          <t>БНХ Укр</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
SALES ver 0.8  at 08/09/2022
</commit_message>
<xml_diff>
--- a/src/Tyres.xlsx
+++ b/src/Tyres.xlsx
@@ -417,7 +417,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J39"/>
+  <dimension ref="A1:J134"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1803,6 +1803,2666 @@
       <c r="J39" t="inlineStr">
         <is>
           <t>БНХ Укр</t>
+        </is>
+      </c>
+    </row>
+    <row r="40">
+      <c r="E40" t="inlineStr">
+        <is>
+          <t>315/80R22.5</t>
+        </is>
+      </c>
+      <c r="F40" t="inlineStr">
+        <is>
+          <t>BEL-158M</t>
+        </is>
+      </c>
+      <c r="G40" t="inlineStr">
+        <is>
+          <t>груз, камневыт, сер</t>
+        </is>
+      </c>
+      <c r="H40" t="n">
+        <v>78</v>
+      </c>
+      <c r="I40" s="1" t="n">
+        <v>44628</v>
+      </c>
+      <c r="J40" t="inlineStr">
+        <is>
+          <t>БНХ Польска</t>
+        </is>
+      </c>
+    </row>
+    <row r="41">
+      <c r="E41" t="inlineStr">
+        <is>
+          <t>315/80R22.5</t>
+        </is>
+      </c>
+      <c r="F41" t="inlineStr">
+        <is>
+          <t>BEL-158M</t>
+        </is>
+      </c>
+      <c r="G41" t="inlineStr">
+        <is>
+          <t>груз, трп, камневыт</t>
+        </is>
+      </c>
+      <c r="H41" t="n">
+        <v>78</v>
+      </c>
+      <c r="I41" s="1" t="n">
+        <v>44628</v>
+      </c>
+      <c r="J41" t="inlineStr">
+        <is>
+          <t>БНХ Польска</t>
+        </is>
+      </c>
+    </row>
+    <row r="42">
+      <c r="E42" t="inlineStr">
+        <is>
+          <t>315/80R22.5</t>
+        </is>
+      </c>
+      <c r="F42" t="inlineStr">
+        <is>
+          <t>BEL-278</t>
+        </is>
+      </c>
+      <c r="G42" t="inlineStr">
+        <is>
+          <t>груз, сер</t>
+        </is>
+      </c>
+      <c r="H42" t="n">
+        <v>78</v>
+      </c>
+      <c r="I42" s="1" t="n">
+        <v>44628</v>
+      </c>
+      <c r="J42" t="inlineStr">
+        <is>
+          <t>БНХ Польска</t>
+        </is>
+      </c>
+    </row>
+    <row r="43">
+      <c r="E43" t="inlineStr">
+        <is>
+          <t>315/80R22.5</t>
+        </is>
+      </c>
+      <c r="F43" t="inlineStr">
+        <is>
+          <t>BEL-278</t>
+        </is>
+      </c>
+      <c r="G43" t="inlineStr">
+        <is>
+          <t>груз, трп</t>
+        </is>
+      </c>
+      <c r="H43" t="n">
+        <v>78</v>
+      </c>
+      <c r="I43" s="1" t="n">
+        <v>44628</v>
+      </c>
+      <c r="J43" t="inlineStr">
+        <is>
+          <t>БНХ Польска</t>
+        </is>
+      </c>
+    </row>
+    <row r="44">
+      <c r="E44" t="inlineStr">
+        <is>
+          <t>315/80R22.5</t>
+        </is>
+      </c>
+      <c r="F44" t="inlineStr">
+        <is>
+          <t>BEL-268</t>
+        </is>
+      </c>
+      <c r="G44" t="inlineStr">
+        <is>
+          <t>груз, сер</t>
+        </is>
+      </c>
+      <c r="H44" t="n">
+        <v>78</v>
+      </c>
+      <c r="I44" s="1" t="n">
+        <v>44628</v>
+      </c>
+      <c r="J44" t="inlineStr">
+        <is>
+          <t>БНХ Польска</t>
+        </is>
+      </c>
+    </row>
+    <row r="45">
+      <c r="E45" t="inlineStr">
+        <is>
+          <t>315/80R22.5</t>
+        </is>
+      </c>
+      <c r="F45" t="inlineStr">
+        <is>
+          <t>BEL-268</t>
+        </is>
+      </c>
+      <c r="G45" t="inlineStr">
+        <is>
+          <t>груз, трп</t>
+        </is>
+      </c>
+      <c r="H45" t="n">
+        <v>78</v>
+      </c>
+      <c r="I45" s="1" t="n">
+        <v>44628</v>
+      </c>
+      <c r="J45" t="inlineStr">
+        <is>
+          <t>БНХ Польска</t>
+        </is>
+      </c>
+    </row>
+    <row r="46">
+      <c r="E46" t="inlineStr">
+        <is>
+          <t>315/80R22.5</t>
+        </is>
+      </c>
+      <c r="F46" t="inlineStr">
+        <is>
+          <t>BEL-398</t>
+        </is>
+      </c>
+      <c r="G46" t="inlineStr">
+        <is>
+          <t>груз, сер</t>
+        </is>
+      </c>
+      <c r="H46" t="n">
+        <v>78</v>
+      </c>
+      <c r="I46" s="1" t="n">
+        <v>44628</v>
+      </c>
+      <c r="J46" t="inlineStr">
+        <is>
+          <t>БНХ Польска</t>
+        </is>
+      </c>
+    </row>
+    <row r="47">
+      <c r="E47" t="inlineStr">
+        <is>
+          <t>315/80R22.5</t>
+        </is>
+      </c>
+      <c r="F47" t="inlineStr">
+        <is>
+          <t>BEL-326</t>
+        </is>
+      </c>
+      <c r="G47" t="inlineStr">
+        <is>
+          <t>груз, сер</t>
+        </is>
+      </c>
+      <c r="H47" t="n">
+        <v>78</v>
+      </c>
+      <c r="I47" s="1" t="n">
+        <v>44628</v>
+      </c>
+      <c r="J47" t="inlineStr">
+        <is>
+          <t>БНХ Польска</t>
+        </is>
+      </c>
+    </row>
+    <row r="48">
+      <c r="E48" t="inlineStr">
+        <is>
+          <t>315/80R22.5</t>
+        </is>
+      </c>
+      <c r="F48" t="inlineStr">
+        <is>
+          <t>BEL-326</t>
+        </is>
+      </c>
+      <c r="G48" t="inlineStr">
+        <is>
+          <t>груз, трп</t>
+        </is>
+      </c>
+      <c r="H48" t="n">
+        <v>78</v>
+      </c>
+      <c r="I48" s="1" t="n">
+        <v>44628</v>
+      </c>
+      <c r="J48" t="inlineStr">
+        <is>
+          <t>БНХ Польска</t>
+        </is>
+      </c>
+    </row>
+    <row r="49">
+      <c r="E49" t="inlineStr">
+        <is>
+          <t>315/80R22.5</t>
+        </is>
+      </c>
+      <c r="F49" t="inlineStr">
+        <is>
+          <t>BEL-498</t>
+        </is>
+      </c>
+      <c r="G49" t="inlineStr">
+        <is>
+          <t>156L, груз, сер</t>
+        </is>
+      </c>
+      <c r="H49" t="n">
+        <v>78</v>
+      </c>
+      <c r="I49" s="1" t="n">
+        <v>44628</v>
+      </c>
+      <c r="J49" t="inlineStr">
+        <is>
+          <t>БНХ Польска</t>
+        </is>
+      </c>
+    </row>
+    <row r="50">
+      <c r="E50" t="inlineStr">
+        <is>
+          <t>315/80R22.5</t>
+        </is>
+      </c>
+      <c r="F50" t="inlineStr">
+        <is>
+          <t>BEL-518</t>
+        </is>
+      </c>
+      <c r="G50" t="inlineStr">
+        <is>
+          <t>груз, сер</t>
+        </is>
+      </c>
+      <c r="H50" t="n">
+        <v>78</v>
+      </c>
+      <c r="I50" s="1" t="n">
+        <v>44628</v>
+      </c>
+      <c r="J50" t="inlineStr">
+        <is>
+          <t>БНХ Польска</t>
+        </is>
+      </c>
+    </row>
+    <row r="51">
+      <c r="E51" t="inlineStr">
+        <is>
+          <t>12.00R20</t>
+        </is>
+      </c>
+      <c r="F51" t="inlineStr">
+        <is>
+          <t>ИД-304М</t>
+        </is>
+      </c>
+      <c r="G51" t="inlineStr">
+        <is>
+          <t>16, груз, сер</t>
+        </is>
+      </c>
+      <c r="H51" t="n">
+        <v>78</v>
+      </c>
+      <c r="I51" s="1" t="n">
+        <v>44628</v>
+      </c>
+      <c r="J51" t="inlineStr">
+        <is>
+          <t>БНХ Польска</t>
+        </is>
+      </c>
+    </row>
+    <row r="52">
+      <c r="E52" t="inlineStr">
+        <is>
+          <t>12.00R20</t>
+        </is>
+      </c>
+      <c r="F52" t="inlineStr">
+        <is>
+          <t>ИД-304М</t>
+        </is>
+      </c>
+      <c r="G52" t="inlineStr">
+        <is>
+          <t>18, груз, сер</t>
+        </is>
+      </c>
+      <c r="H52" t="n">
+        <v>78</v>
+      </c>
+      <c r="I52" s="1" t="n">
+        <v>44628</v>
+      </c>
+      <c r="J52" t="inlineStr">
+        <is>
+          <t>БНХ Польска</t>
+        </is>
+      </c>
+    </row>
+    <row r="53">
+      <c r="E53" t="inlineStr">
+        <is>
+          <t>12.00R20</t>
+        </is>
+      </c>
+      <c r="F53" t="inlineStr">
+        <is>
+          <t>ИД-304М</t>
+        </is>
+      </c>
+      <c r="G53" t="inlineStr">
+        <is>
+          <t>16, груз, трп</t>
+        </is>
+      </c>
+      <c r="H53" t="n">
+        <v>78</v>
+      </c>
+      <c r="I53" s="1" t="n">
+        <v>44628</v>
+      </c>
+      <c r="J53" t="inlineStr">
+        <is>
+          <t>БНХ Польска</t>
+        </is>
+      </c>
+    </row>
+    <row r="54">
+      <c r="E54" t="inlineStr">
+        <is>
+          <t>12.00R20</t>
+        </is>
+      </c>
+      <c r="F54" t="inlineStr">
+        <is>
+          <t>ИД-304М</t>
+        </is>
+      </c>
+      <c r="G54" t="inlineStr">
+        <is>
+          <t>18, груз, трп</t>
+        </is>
+      </c>
+      <c r="H54" t="n">
+        <v>78</v>
+      </c>
+      <c r="I54" s="1" t="n">
+        <v>44628</v>
+      </c>
+      <c r="J54" t="inlineStr">
+        <is>
+          <t>БНХ Польска</t>
+        </is>
+      </c>
+    </row>
+    <row r="55">
+      <c r="E55" t="inlineStr">
+        <is>
+          <t>12.00R20</t>
+        </is>
+      </c>
+      <c r="F55" t="inlineStr">
+        <is>
+          <t>БИ-368М</t>
+        </is>
+      </c>
+      <c r="G55" t="inlineStr">
+        <is>
+          <t>18, груз, сер</t>
+        </is>
+      </c>
+      <c r="H55" t="n">
+        <v>78</v>
+      </c>
+      <c r="I55" s="1" t="n">
+        <v>44628</v>
+      </c>
+      <c r="J55" t="inlineStr">
+        <is>
+          <t>БНХ Польска</t>
+        </is>
+      </c>
+    </row>
+    <row r="56">
+      <c r="E56" t="inlineStr">
+        <is>
+          <t>12.00R20</t>
+        </is>
+      </c>
+      <c r="F56" t="inlineStr">
+        <is>
+          <t>БИ-368М</t>
+        </is>
+      </c>
+      <c r="G56" t="inlineStr">
+        <is>
+          <t>18, груз, сер</t>
+        </is>
+      </c>
+      <c r="H56" t="n">
+        <v>78</v>
+      </c>
+      <c r="I56" s="1" t="n">
+        <v>44628</v>
+      </c>
+      <c r="J56" t="inlineStr">
+        <is>
+          <t>БНХ Польска</t>
+        </is>
+      </c>
+    </row>
+    <row r="57">
+      <c r="E57" t="inlineStr">
+        <is>
+          <t>12.00R20</t>
+        </is>
+      </c>
+      <c r="F57" t="inlineStr">
+        <is>
+          <t>БИ-368М</t>
+        </is>
+      </c>
+      <c r="G57" t="inlineStr">
+        <is>
+          <t>18, груз, трп</t>
+        </is>
+      </c>
+      <c r="H57" t="n">
+        <v>78</v>
+      </c>
+      <c r="I57" s="1" t="n">
+        <v>44628</v>
+      </c>
+      <c r="J57" t="inlineStr">
+        <is>
+          <t>БНХ Польска</t>
+        </is>
+      </c>
+    </row>
+    <row r="58">
+      <c r="E58" t="inlineStr">
+        <is>
+          <t>195/65R15</t>
+        </is>
+      </c>
+      <c r="F58" t="inlineStr">
+        <is>
+          <t>BEL-337</t>
+        </is>
+      </c>
+      <c r="G58" t="inlineStr">
+        <is>
+          <t>б/к, легк, сер</t>
+        </is>
+      </c>
+      <c r="H58" t="n">
+        <v>78</v>
+      </c>
+      <c r="I58" s="1" t="n">
+        <v>44628</v>
+      </c>
+      <c r="J58" t="inlineStr">
+        <is>
+          <t>БНХ Польска</t>
+        </is>
+      </c>
+    </row>
+    <row r="59">
+      <c r="E59" t="inlineStr">
+        <is>
+          <t>315/80R22.5</t>
+        </is>
+      </c>
+      <c r="F59" t="inlineStr">
+        <is>
+          <t>BEL-158M</t>
+        </is>
+      </c>
+      <c r="G59" t="inlineStr">
+        <is>
+          <t>груз, камневыт, сер</t>
+        </is>
+      </c>
+      <c r="H59" t="n">
+        <v>8</v>
+      </c>
+      <c r="I59" s="1" t="n">
+        <v>44824</v>
+      </c>
+      <c r="J59" t="inlineStr">
+        <is>
+          <t>БНХ Польска</t>
+        </is>
+      </c>
+    </row>
+    <row r="60">
+      <c r="E60" t="inlineStr">
+        <is>
+          <t>315/80R22.5</t>
+        </is>
+      </c>
+      <c r="F60" t="inlineStr">
+        <is>
+          <t>BEL-158M</t>
+        </is>
+      </c>
+      <c r="G60" t="inlineStr">
+        <is>
+          <t>груз, трп, камневыт</t>
+        </is>
+      </c>
+      <c r="H60" t="n">
+        <v>8</v>
+      </c>
+      <c r="I60" s="1" t="n">
+        <v>44824</v>
+      </c>
+      <c r="J60" t="inlineStr">
+        <is>
+          <t>БНХ Польска</t>
+        </is>
+      </c>
+    </row>
+    <row r="61">
+      <c r="E61" t="inlineStr">
+        <is>
+          <t>315/80R22.5</t>
+        </is>
+      </c>
+      <c r="F61" t="inlineStr">
+        <is>
+          <t>BEL-278</t>
+        </is>
+      </c>
+      <c r="G61" t="inlineStr">
+        <is>
+          <t>груз, сер</t>
+        </is>
+      </c>
+      <c r="H61" t="n">
+        <v>8</v>
+      </c>
+      <c r="I61" s="1" t="n">
+        <v>44824</v>
+      </c>
+      <c r="J61" t="inlineStr">
+        <is>
+          <t>БНХ Польска</t>
+        </is>
+      </c>
+    </row>
+    <row r="62">
+      <c r="E62" t="inlineStr">
+        <is>
+          <t>315/80R22.5</t>
+        </is>
+      </c>
+      <c r="F62" t="inlineStr">
+        <is>
+          <t>BEL-278</t>
+        </is>
+      </c>
+      <c r="G62" t="inlineStr">
+        <is>
+          <t>груз, трп</t>
+        </is>
+      </c>
+      <c r="H62" t="n">
+        <v>8</v>
+      </c>
+      <c r="I62" s="1" t="n">
+        <v>44824</v>
+      </c>
+      <c r="J62" t="inlineStr">
+        <is>
+          <t>БНХ Польска</t>
+        </is>
+      </c>
+    </row>
+    <row r="63">
+      <c r="E63" t="inlineStr">
+        <is>
+          <t>315/80R22.5</t>
+        </is>
+      </c>
+      <c r="F63" t="inlineStr">
+        <is>
+          <t>BEL-268</t>
+        </is>
+      </c>
+      <c r="G63" t="inlineStr">
+        <is>
+          <t>груз, сер</t>
+        </is>
+      </c>
+      <c r="H63" t="n">
+        <v>8</v>
+      </c>
+      <c r="I63" s="1" t="n">
+        <v>44824</v>
+      </c>
+      <c r="J63" t="inlineStr">
+        <is>
+          <t>БНХ Польска</t>
+        </is>
+      </c>
+    </row>
+    <row r="64">
+      <c r="E64" t="inlineStr">
+        <is>
+          <t>315/80R22.5</t>
+        </is>
+      </c>
+      <c r="F64" t="inlineStr">
+        <is>
+          <t>BEL-268</t>
+        </is>
+      </c>
+      <c r="G64" t="inlineStr">
+        <is>
+          <t>груз, трп</t>
+        </is>
+      </c>
+      <c r="H64" t="n">
+        <v>8</v>
+      </c>
+      <c r="I64" s="1" t="n">
+        <v>44824</v>
+      </c>
+      <c r="J64" t="inlineStr">
+        <is>
+          <t>БНХ Польска</t>
+        </is>
+      </c>
+    </row>
+    <row r="65">
+      <c r="E65" t="inlineStr">
+        <is>
+          <t>315/80R22.5</t>
+        </is>
+      </c>
+      <c r="F65" t="inlineStr">
+        <is>
+          <t>BEL-398</t>
+        </is>
+      </c>
+      <c r="G65" t="inlineStr">
+        <is>
+          <t>груз, сер</t>
+        </is>
+      </c>
+      <c r="H65" t="n">
+        <v>8</v>
+      </c>
+      <c r="I65" s="1" t="n">
+        <v>44824</v>
+      </c>
+      <c r="J65" t="inlineStr">
+        <is>
+          <t>БНХ Польска</t>
+        </is>
+      </c>
+    </row>
+    <row r="66">
+      <c r="E66" t="inlineStr">
+        <is>
+          <t>315/80R22.5</t>
+        </is>
+      </c>
+      <c r="F66" t="inlineStr">
+        <is>
+          <t>BEL-326</t>
+        </is>
+      </c>
+      <c r="G66" t="inlineStr">
+        <is>
+          <t>груз, сер</t>
+        </is>
+      </c>
+      <c r="H66" t="n">
+        <v>8</v>
+      </c>
+      <c r="I66" s="1" t="n">
+        <v>44824</v>
+      </c>
+      <c r="J66" t="inlineStr">
+        <is>
+          <t>БНХ Польска</t>
+        </is>
+      </c>
+    </row>
+    <row r="67">
+      <c r="E67" t="inlineStr">
+        <is>
+          <t>315/80R22.5</t>
+        </is>
+      </c>
+      <c r="F67" t="inlineStr">
+        <is>
+          <t>BEL-326</t>
+        </is>
+      </c>
+      <c r="G67" t="inlineStr">
+        <is>
+          <t>груз, трп</t>
+        </is>
+      </c>
+      <c r="H67" t="n">
+        <v>8</v>
+      </c>
+      <c r="I67" s="1" t="n">
+        <v>44824</v>
+      </c>
+      <c r="J67" t="inlineStr">
+        <is>
+          <t>БНХ Польска</t>
+        </is>
+      </c>
+    </row>
+    <row r="68">
+      <c r="E68" t="inlineStr">
+        <is>
+          <t>315/80R22.5</t>
+        </is>
+      </c>
+      <c r="F68" t="inlineStr">
+        <is>
+          <t>BEL-498</t>
+        </is>
+      </c>
+      <c r="G68" t="inlineStr">
+        <is>
+          <t>156L, груз, сер</t>
+        </is>
+      </c>
+      <c r="H68" t="n">
+        <v>8</v>
+      </c>
+      <c r="I68" s="1" t="n">
+        <v>44824</v>
+      </c>
+      <c r="J68" t="inlineStr">
+        <is>
+          <t>БНХ Польска</t>
+        </is>
+      </c>
+    </row>
+    <row r="69">
+      <c r="E69" t="inlineStr">
+        <is>
+          <t>315/80R22.5</t>
+        </is>
+      </c>
+      <c r="F69" t="inlineStr">
+        <is>
+          <t>BEL-518</t>
+        </is>
+      </c>
+      <c r="G69" t="inlineStr">
+        <is>
+          <t>груз, сер</t>
+        </is>
+      </c>
+      <c r="H69" t="n">
+        <v>8</v>
+      </c>
+      <c r="I69" s="1" t="n">
+        <v>44824</v>
+      </c>
+      <c r="J69" t="inlineStr">
+        <is>
+          <t>БНХ Польска</t>
+        </is>
+      </c>
+    </row>
+    <row r="70">
+      <c r="E70" t="inlineStr">
+        <is>
+          <t>12.00R20</t>
+        </is>
+      </c>
+      <c r="F70" t="inlineStr">
+        <is>
+          <t>ИД-304М</t>
+        </is>
+      </c>
+      <c r="G70" t="inlineStr">
+        <is>
+          <t>16, груз, сер</t>
+        </is>
+      </c>
+      <c r="H70" t="n">
+        <v>8</v>
+      </c>
+      <c r="I70" s="1" t="n">
+        <v>44824</v>
+      </c>
+      <c r="J70" t="inlineStr">
+        <is>
+          <t>БНХ Польска</t>
+        </is>
+      </c>
+    </row>
+    <row r="71">
+      <c r="E71" t="inlineStr">
+        <is>
+          <t>12.00R20</t>
+        </is>
+      </c>
+      <c r="F71" t="inlineStr">
+        <is>
+          <t>ИД-304М</t>
+        </is>
+      </c>
+      <c r="G71" t="inlineStr">
+        <is>
+          <t>18, груз, сер</t>
+        </is>
+      </c>
+      <c r="H71" t="n">
+        <v>8</v>
+      </c>
+      <c r="I71" s="1" t="n">
+        <v>44824</v>
+      </c>
+      <c r="J71" t="inlineStr">
+        <is>
+          <t>БНХ Польска</t>
+        </is>
+      </c>
+    </row>
+    <row r="72">
+      <c r="E72" t="inlineStr">
+        <is>
+          <t>12.00R20</t>
+        </is>
+      </c>
+      <c r="F72" t="inlineStr">
+        <is>
+          <t>ИД-304М</t>
+        </is>
+      </c>
+      <c r="G72" t="inlineStr">
+        <is>
+          <t>16, груз, трп</t>
+        </is>
+      </c>
+      <c r="H72" t="n">
+        <v>8</v>
+      </c>
+      <c r="I72" s="1" t="n">
+        <v>44824</v>
+      </c>
+      <c r="J72" t="inlineStr">
+        <is>
+          <t>БНХ Польска</t>
+        </is>
+      </c>
+    </row>
+    <row r="73">
+      <c r="E73" t="inlineStr">
+        <is>
+          <t>12.00R20</t>
+        </is>
+      </c>
+      <c r="F73" t="inlineStr">
+        <is>
+          <t>ИД-304М</t>
+        </is>
+      </c>
+      <c r="G73" t="inlineStr">
+        <is>
+          <t>18, груз, трп</t>
+        </is>
+      </c>
+      <c r="H73" t="n">
+        <v>8</v>
+      </c>
+      <c r="I73" s="1" t="n">
+        <v>44824</v>
+      </c>
+      <c r="J73" t="inlineStr">
+        <is>
+          <t>БНХ Польска</t>
+        </is>
+      </c>
+    </row>
+    <row r="74">
+      <c r="E74" t="inlineStr">
+        <is>
+          <t>12.00R20</t>
+        </is>
+      </c>
+      <c r="F74" t="inlineStr">
+        <is>
+          <t>БИ-368М</t>
+        </is>
+      </c>
+      <c r="G74" t="inlineStr">
+        <is>
+          <t>18, груз, сер</t>
+        </is>
+      </c>
+      <c r="H74" t="n">
+        <v>8</v>
+      </c>
+      <c r="I74" s="1" t="n">
+        <v>44824</v>
+      </c>
+      <c r="J74" t="inlineStr">
+        <is>
+          <t>БНХ Польска</t>
+        </is>
+      </c>
+    </row>
+    <row r="75">
+      <c r="E75" t="inlineStr">
+        <is>
+          <t>12.00R20</t>
+        </is>
+      </c>
+      <c r="F75" t="inlineStr">
+        <is>
+          <t>БИ-368М</t>
+        </is>
+      </c>
+      <c r="G75" t="inlineStr">
+        <is>
+          <t>18, груз, сер</t>
+        </is>
+      </c>
+      <c r="H75" t="n">
+        <v>8</v>
+      </c>
+      <c r="I75" s="1" t="n">
+        <v>44824</v>
+      </c>
+      <c r="J75" t="inlineStr">
+        <is>
+          <t>БНХ Польска</t>
+        </is>
+      </c>
+    </row>
+    <row r="76">
+      <c r="E76" t="inlineStr">
+        <is>
+          <t>12.00R20</t>
+        </is>
+      </c>
+      <c r="F76" t="inlineStr">
+        <is>
+          <t>БИ-368М</t>
+        </is>
+      </c>
+      <c r="G76" t="inlineStr">
+        <is>
+          <t>18, груз, трп</t>
+        </is>
+      </c>
+      <c r="H76" t="n">
+        <v>8</v>
+      </c>
+      <c r="I76" s="1" t="n">
+        <v>44824</v>
+      </c>
+      <c r="J76" t="inlineStr">
+        <is>
+          <t>БНХ Польска</t>
+        </is>
+      </c>
+    </row>
+    <row r="77">
+      <c r="E77" t="inlineStr">
+        <is>
+          <t>195/65R15</t>
+        </is>
+      </c>
+      <c r="F77" t="inlineStr">
+        <is>
+          <t>BEL-337</t>
+        </is>
+      </c>
+      <c r="G77" t="inlineStr">
+        <is>
+          <t>б/к, легк, сер</t>
+        </is>
+      </c>
+      <c r="H77" t="n">
+        <v>8</v>
+      </c>
+      <c r="I77" s="1" t="n">
+        <v>44824</v>
+      </c>
+      <c r="J77" t="inlineStr">
+        <is>
+          <t>БНХ Польска</t>
+        </is>
+      </c>
+    </row>
+    <row r="78">
+      <c r="E78" t="inlineStr">
+        <is>
+          <t>315/80R22.5</t>
+        </is>
+      </c>
+      <c r="F78" t="inlineStr">
+        <is>
+          <t>BEL-158M</t>
+        </is>
+      </c>
+      <c r="G78" t="inlineStr">
+        <is>
+          <t>груз, камневыт, сер</t>
+        </is>
+      </c>
+      <c r="H78" t="n">
+        <v>8</v>
+      </c>
+      <c r="I78" s="1" t="n">
+        <v>44800</v>
+      </c>
+      <c r="J78" t="inlineStr">
+        <is>
+          <t>БНХ Польска</t>
+        </is>
+      </c>
+    </row>
+    <row r="79">
+      <c r="E79" t="inlineStr">
+        <is>
+          <t>315/80R22.5</t>
+        </is>
+      </c>
+      <c r="F79" t="inlineStr">
+        <is>
+          <t>BEL-158M</t>
+        </is>
+      </c>
+      <c r="G79" t="inlineStr">
+        <is>
+          <t>груз, трп, камневыт</t>
+        </is>
+      </c>
+      <c r="H79" t="n">
+        <v>8</v>
+      </c>
+      <c r="I79" s="1" t="n">
+        <v>44800</v>
+      </c>
+      <c r="J79" t="inlineStr">
+        <is>
+          <t>БНХ Польска</t>
+        </is>
+      </c>
+    </row>
+    <row r="80">
+      <c r="E80" t="inlineStr">
+        <is>
+          <t>315/80R22.5</t>
+        </is>
+      </c>
+      <c r="F80" t="inlineStr">
+        <is>
+          <t>BEL-278</t>
+        </is>
+      </c>
+      <c r="G80" t="inlineStr">
+        <is>
+          <t>груз, сер</t>
+        </is>
+      </c>
+      <c r="H80" t="n">
+        <v>8</v>
+      </c>
+      <c r="I80" s="1" t="n">
+        <v>44800</v>
+      </c>
+      <c r="J80" t="inlineStr">
+        <is>
+          <t>БНХ Польска</t>
+        </is>
+      </c>
+    </row>
+    <row r="81">
+      <c r="E81" t="inlineStr">
+        <is>
+          <t>315/80R22.5</t>
+        </is>
+      </c>
+      <c r="F81" t="inlineStr">
+        <is>
+          <t>BEL-278</t>
+        </is>
+      </c>
+      <c r="G81" t="inlineStr">
+        <is>
+          <t>груз, трп</t>
+        </is>
+      </c>
+      <c r="H81" t="n">
+        <v>8</v>
+      </c>
+      <c r="I81" s="1" t="n">
+        <v>44800</v>
+      </c>
+      <c r="J81" t="inlineStr">
+        <is>
+          <t>БНХ Польска</t>
+        </is>
+      </c>
+    </row>
+    <row r="82">
+      <c r="E82" t="inlineStr">
+        <is>
+          <t>315/80R22.5</t>
+        </is>
+      </c>
+      <c r="F82" t="inlineStr">
+        <is>
+          <t>BEL-268</t>
+        </is>
+      </c>
+      <c r="G82" t="inlineStr">
+        <is>
+          <t>груз, сер</t>
+        </is>
+      </c>
+      <c r="H82" t="n">
+        <v>8</v>
+      </c>
+      <c r="I82" s="1" t="n">
+        <v>44800</v>
+      </c>
+      <c r="J82" t="inlineStr">
+        <is>
+          <t>БНХ Польска</t>
+        </is>
+      </c>
+    </row>
+    <row r="83">
+      <c r="E83" t="inlineStr">
+        <is>
+          <t>315/80R22.5</t>
+        </is>
+      </c>
+      <c r="F83" t="inlineStr">
+        <is>
+          <t>BEL-268</t>
+        </is>
+      </c>
+      <c r="G83" t="inlineStr">
+        <is>
+          <t>груз, трп</t>
+        </is>
+      </c>
+      <c r="H83" t="n">
+        <v>8</v>
+      </c>
+      <c r="I83" s="1" t="n">
+        <v>44800</v>
+      </c>
+      <c r="J83" t="inlineStr">
+        <is>
+          <t>БНХ Польска</t>
+        </is>
+      </c>
+    </row>
+    <row r="84">
+      <c r="E84" t="inlineStr">
+        <is>
+          <t>315/80R22.5</t>
+        </is>
+      </c>
+      <c r="F84" t="inlineStr">
+        <is>
+          <t>BEL-398</t>
+        </is>
+      </c>
+      <c r="G84" t="inlineStr">
+        <is>
+          <t>груз, сер</t>
+        </is>
+      </c>
+      <c r="H84" t="n">
+        <v>8</v>
+      </c>
+      <c r="I84" s="1" t="n">
+        <v>44800</v>
+      </c>
+      <c r="J84" t="inlineStr">
+        <is>
+          <t>БНХ Польска</t>
+        </is>
+      </c>
+    </row>
+    <row r="85">
+      <c r="E85" t="inlineStr">
+        <is>
+          <t>315/80R22.5</t>
+        </is>
+      </c>
+      <c r="F85" t="inlineStr">
+        <is>
+          <t>BEL-326</t>
+        </is>
+      </c>
+      <c r="G85" t="inlineStr">
+        <is>
+          <t>груз, сер</t>
+        </is>
+      </c>
+      <c r="H85" t="n">
+        <v>8</v>
+      </c>
+      <c r="I85" s="1" t="n">
+        <v>44800</v>
+      </c>
+      <c r="J85" t="inlineStr">
+        <is>
+          <t>БНХ Польска</t>
+        </is>
+      </c>
+    </row>
+    <row r="86">
+      <c r="E86" t="inlineStr">
+        <is>
+          <t>315/80R22.5</t>
+        </is>
+      </c>
+      <c r="F86" t="inlineStr">
+        <is>
+          <t>BEL-326</t>
+        </is>
+      </c>
+      <c r="G86" t="inlineStr">
+        <is>
+          <t>груз, трп</t>
+        </is>
+      </c>
+      <c r="H86" t="n">
+        <v>8</v>
+      </c>
+      <c r="I86" s="1" t="n">
+        <v>44800</v>
+      </c>
+      <c r="J86" t="inlineStr">
+        <is>
+          <t>БНХ Польска</t>
+        </is>
+      </c>
+    </row>
+    <row r="87">
+      <c r="E87" t="inlineStr">
+        <is>
+          <t>315/80R22.5</t>
+        </is>
+      </c>
+      <c r="F87" t="inlineStr">
+        <is>
+          <t>BEL-498</t>
+        </is>
+      </c>
+      <c r="G87" t="inlineStr">
+        <is>
+          <t>156L, груз, сер</t>
+        </is>
+      </c>
+      <c r="H87" t="n">
+        <v>8</v>
+      </c>
+      <c r="I87" s="1" t="n">
+        <v>44800</v>
+      </c>
+      <c r="J87" t="inlineStr">
+        <is>
+          <t>БНХ Польска</t>
+        </is>
+      </c>
+    </row>
+    <row r="88">
+      <c r="E88" t="inlineStr">
+        <is>
+          <t>315/80R22.5</t>
+        </is>
+      </c>
+      <c r="F88" t="inlineStr">
+        <is>
+          <t>BEL-518</t>
+        </is>
+      </c>
+      <c r="G88" t="inlineStr">
+        <is>
+          <t>груз, сер</t>
+        </is>
+      </c>
+      <c r="H88" t="n">
+        <v>8</v>
+      </c>
+      <c r="I88" s="1" t="n">
+        <v>44800</v>
+      </c>
+      <c r="J88" t="inlineStr">
+        <is>
+          <t>БНХ Польска</t>
+        </is>
+      </c>
+    </row>
+    <row r="89">
+      <c r="E89" t="inlineStr">
+        <is>
+          <t>12.00R20</t>
+        </is>
+      </c>
+      <c r="F89" t="inlineStr">
+        <is>
+          <t>ИД-304М</t>
+        </is>
+      </c>
+      <c r="G89" t="inlineStr">
+        <is>
+          <t>16, груз, сер</t>
+        </is>
+      </c>
+      <c r="H89" t="n">
+        <v>8</v>
+      </c>
+      <c r="I89" s="1" t="n">
+        <v>44800</v>
+      </c>
+      <c r="J89" t="inlineStr">
+        <is>
+          <t>БНХ Польска</t>
+        </is>
+      </c>
+    </row>
+    <row r="90">
+      <c r="E90" t="inlineStr">
+        <is>
+          <t>12.00R20</t>
+        </is>
+      </c>
+      <c r="F90" t="inlineStr">
+        <is>
+          <t>ИД-304М</t>
+        </is>
+      </c>
+      <c r="G90" t="inlineStr">
+        <is>
+          <t>18, груз, сер</t>
+        </is>
+      </c>
+      <c r="H90" t="n">
+        <v>8</v>
+      </c>
+      <c r="I90" s="1" t="n">
+        <v>44800</v>
+      </c>
+      <c r="J90" t="inlineStr">
+        <is>
+          <t>БНХ Польска</t>
+        </is>
+      </c>
+    </row>
+    <row r="91">
+      <c r="E91" t="inlineStr">
+        <is>
+          <t>12.00R20</t>
+        </is>
+      </c>
+      <c r="F91" t="inlineStr">
+        <is>
+          <t>ИД-304М</t>
+        </is>
+      </c>
+      <c r="G91" t="inlineStr">
+        <is>
+          <t>16, груз, трп</t>
+        </is>
+      </c>
+      <c r="H91" t="n">
+        <v>8</v>
+      </c>
+      <c r="I91" s="1" t="n">
+        <v>44800</v>
+      </c>
+      <c r="J91" t="inlineStr">
+        <is>
+          <t>БНХ Польска</t>
+        </is>
+      </c>
+    </row>
+    <row r="92">
+      <c r="E92" t="inlineStr">
+        <is>
+          <t>12.00R20</t>
+        </is>
+      </c>
+      <c r="F92" t="inlineStr">
+        <is>
+          <t>ИД-304М</t>
+        </is>
+      </c>
+      <c r="G92" t="inlineStr">
+        <is>
+          <t>18, груз, трп</t>
+        </is>
+      </c>
+      <c r="H92" t="n">
+        <v>8</v>
+      </c>
+      <c r="I92" s="1" t="n">
+        <v>44800</v>
+      </c>
+      <c r="J92" t="inlineStr">
+        <is>
+          <t>БНХ Польска</t>
+        </is>
+      </c>
+    </row>
+    <row r="93">
+      <c r="E93" t="inlineStr">
+        <is>
+          <t>12.00R20</t>
+        </is>
+      </c>
+      <c r="F93" t="inlineStr">
+        <is>
+          <t>БИ-368М</t>
+        </is>
+      </c>
+      <c r="G93" t="inlineStr">
+        <is>
+          <t>18, груз, сер</t>
+        </is>
+      </c>
+      <c r="H93" t="n">
+        <v>8</v>
+      </c>
+      <c r="I93" s="1" t="n">
+        <v>44800</v>
+      </c>
+      <c r="J93" t="inlineStr">
+        <is>
+          <t>БНХ Польска</t>
+        </is>
+      </c>
+    </row>
+    <row r="94">
+      <c r="E94" t="inlineStr">
+        <is>
+          <t>12.00R20</t>
+        </is>
+      </c>
+      <c r="F94" t="inlineStr">
+        <is>
+          <t>БИ-368М</t>
+        </is>
+      </c>
+      <c r="G94" t="inlineStr">
+        <is>
+          <t>18, груз, сер</t>
+        </is>
+      </c>
+      <c r="H94" t="n">
+        <v>8</v>
+      </c>
+      <c r="I94" s="1" t="n">
+        <v>44800</v>
+      </c>
+      <c r="J94" t="inlineStr">
+        <is>
+          <t>БНХ Польска</t>
+        </is>
+      </c>
+    </row>
+    <row r="95">
+      <c r="E95" t="inlineStr">
+        <is>
+          <t>12.00R20</t>
+        </is>
+      </c>
+      <c r="F95" t="inlineStr">
+        <is>
+          <t>БИ-368М</t>
+        </is>
+      </c>
+      <c r="G95" t="inlineStr">
+        <is>
+          <t>18, груз, трп</t>
+        </is>
+      </c>
+      <c r="H95" t="n">
+        <v>8</v>
+      </c>
+      <c r="I95" s="1" t="n">
+        <v>44800</v>
+      </c>
+      <c r="J95" t="inlineStr">
+        <is>
+          <t>БНХ Польска</t>
+        </is>
+      </c>
+    </row>
+    <row r="96">
+      <c r="E96" t="inlineStr">
+        <is>
+          <t>195/65R15</t>
+        </is>
+      </c>
+      <c r="F96" t="inlineStr">
+        <is>
+          <t>BEL-337</t>
+        </is>
+      </c>
+      <c r="G96" t="inlineStr">
+        <is>
+          <t>б/к, легк, сер</t>
+        </is>
+      </c>
+      <c r="H96" t="n">
+        <v>8</v>
+      </c>
+      <c r="I96" s="1" t="n">
+        <v>44800</v>
+      </c>
+      <c r="J96" t="inlineStr">
+        <is>
+          <t>БНХ Польска</t>
+        </is>
+      </c>
+    </row>
+    <row r="97">
+      <c r="E97" t="inlineStr">
+        <is>
+          <t>315/80R22.5</t>
+        </is>
+      </c>
+      <c r="F97" t="inlineStr">
+        <is>
+          <t>BEL-158M</t>
+        </is>
+      </c>
+      <c r="G97" t="inlineStr">
+        <is>
+          <t>груз, камневыт, сер</t>
+        </is>
+      </c>
+      <c r="H97" t="n">
+        <v>3</v>
+      </c>
+      <c r="I97" s="1" t="n">
+        <v>44824</v>
+      </c>
+      <c r="J97" t="inlineStr">
+        <is>
+          <t>БНХ Укр</t>
+        </is>
+      </c>
+    </row>
+    <row r="98">
+      <c r="E98" t="inlineStr">
+        <is>
+          <t>315/80R22.5</t>
+        </is>
+      </c>
+      <c r="F98" t="inlineStr">
+        <is>
+          <t>BEL-158M</t>
+        </is>
+      </c>
+      <c r="G98" t="inlineStr">
+        <is>
+          <t>груз, трп, камневыт</t>
+        </is>
+      </c>
+      <c r="H98" t="n">
+        <v>3</v>
+      </c>
+      <c r="I98" s="1" t="n">
+        <v>44824</v>
+      </c>
+      <c r="J98" t="inlineStr">
+        <is>
+          <t>БНХ Укр</t>
+        </is>
+      </c>
+    </row>
+    <row r="99">
+      <c r="E99" t="inlineStr">
+        <is>
+          <t>315/80R22.5</t>
+        </is>
+      </c>
+      <c r="F99" t="inlineStr">
+        <is>
+          <t>BEL-278</t>
+        </is>
+      </c>
+      <c r="G99" t="inlineStr">
+        <is>
+          <t>груз, сер</t>
+        </is>
+      </c>
+      <c r="H99" t="n">
+        <v>3</v>
+      </c>
+      <c r="I99" s="1" t="n">
+        <v>44824</v>
+      </c>
+      <c r="J99" t="inlineStr">
+        <is>
+          <t>БНХ Укр</t>
+        </is>
+      </c>
+    </row>
+    <row r="100">
+      <c r="E100" t="inlineStr">
+        <is>
+          <t>315/80R22.5</t>
+        </is>
+      </c>
+      <c r="F100" t="inlineStr">
+        <is>
+          <t>BEL-278</t>
+        </is>
+      </c>
+      <c r="G100" t="inlineStr">
+        <is>
+          <t>груз, трп</t>
+        </is>
+      </c>
+      <c r="H100" t="n">
+        <v>3</v>
+      </c>
+      <c r="I100" s="1" t="n">
+        <v>44824</v>
+      </c>
+      <c r="J100" t="inlineStr">
+        <is>
+          <t>БНХ Укр</t>
+        </is>
+      </c>
+    </row>
+    <row r="101">
+      <c r="E101" t="inlineStr">
+        <is>
+          <t>315/80R22.5</t>
+        </is>
+      </c>
+      <c r="F101" t="inlineStr">
+        <is>
+          <t>BEL-268</t>
+        </is>
+      </c>
+      <c r="G101" t="inlineStr">
+        <is>
+          <t>груз, сер</t>
+        </is>
+      </c>
+      <c r="H101" t="n">
+        <v>3</v>
+      </c>
+      <c r="I101" s="1" t="n">
+        <v>44824</v>
+      </c>
+      <c r="J101" t="inlineStr">
+        <is>
+          <t>БНХ Укр</t>
+        </is>
+      </c>
+    </row>
+    <row r="102">
+      <c r="E102" t="inlineStr">
+        <is>
+          <t>315/80R22.5</t>
+        </is>
+      </c>
+      <c r="F102" t="inlineStr">
+        <is>
+          <t>BEL-268</t>
+        </is>
+      </c>
+      <c r="G102" t="inlineStr">
+        <is>
+          <t>груз, трп</t>
+        </is>
+      </c>
+      <c r="H102" t="n">
+        <v>3</v>
+      </c>
+      <c r="I102" s="1" t="n">
+        <v>44824</v>
+      </c>
+      <c r="J102" t="inlineStr">
+        <is>
+          <t>БНХ Укр</t>
+        </is>
+      </c>
+    </row>
+    <row r="103">
+      <c r="E103" t="inlineStr">
+        <is>
+          <t>315/80R22.5</t>
+        </is>
+      </c>
+      <c r="F103" t="inlineStr">
+        <is>
+          <t>BEL-398</t>
+        </is>
+      </c>
+      <c r="G103" t="inlineStr">
+        <is>
+          <t>груз, сер</t>
+        </is>
+      </c>
+      <c r="H103" t="n">
+        <v>3</v>
+      </c>
+      <c r="I103" s="1" t="n">
+        <v>44824</v>
+      </c>
+      <c r="J103" t="inlineStr">
+        <is>
+          <t>БНХ Укр</t>
+        </is>
+      </c>
+    </row>
+    <row r="104">
+      <c r="E104" t="inlineStr">
+        <is>
+          <t>315/80R22.5</t>
+        </is>
+      </c>
+      <c r="F104" t="inlineStr">
+        <is>
+          <t>BEL-326</t>
+        </is>
+      </c>
+      <c r="G104" t="inlineStr">
+        <is>
+          <t>груз, сер</t>
+        </is>
+      </c>
+      <c r="H104" t="n">
+        <v>3</v>
+      </c>
+      <c r="I104" s="1" t="n">
+        <v>44824</v>
+      </c>
+      <c r="J104" t="inlineStr">
+        <is>
+          <t>БНХ Укр</t>
+        </is>
+      </c>
+    </row>
+    <row r="105">
+      <c r="E105" t="inlineStr">
+        <is>
+          <t>315/80R22.5</t>
+        </is>
+      </c>
+      <c r="F105" t="inlineStr">
+        <is>
+          <t>BEL-326</t>
+        </is>
+      </c>
+      <c r="G105" t="inlineStr">
+        <is>
+          <t>груз, трп</t>
+        </is>
+      </c>
+      <c r="H105" t="n">
+        <v>3</v>
+      </c>
+      <c r="I105" s="1" t="n">
+        <v>44824</v>
+      </c>
+      <c r="J105" t="inlineStr">
+        <is>
+          <t>БНХ Укр</t>
+        </is>
+      </c>
+    </row>
+    <row r="106">
+      <c r="E106" t="inlineStr">
+        <is>
+          <t>315/80R22.5</t>
+        </is>
+      </c>
+      <c r="F106" t="inlineStr">
+        <is>
+          <t>BEL-498</t>
+        </is>
+      </c>
+      <c r="G106" t="inlineStr">
+        <is>
+          <t>156L, груз, сер</t>
+        </is>
+      </c>
+      <c r="H106" t="n">
+        <v>3</v>
+      </c>
+      <c r="I106" s="1" t="n">
+        <v>44824</v>
+      </c>
+      <c r="J106" t="inlineStr">
+        <is>
+          <t>БНХ Укр</t>
+        </is>
+      </c>
+    </row>
+    <row r="107">
+      <c r="E107" t="inlineStr">
+        <is>
+          <t>315/80R22.5</t>
+        </is>
+      </c>
+      <c r="F107" t="inlineStr">
+        <is>
+          <t>BEL-518</t>
+        </is>
+      </c>
+      <c r="G107" t="inlineStr">
+        <is>
+          <t>груз, сер</t>
+        </is>
+      </c>
+      <c r="H107" t="n">
+        <v>3</v>
+      </c>
+      <c r="I107" s="1" t="n">
+        <v>44824</v>
+      </c>
+      <c r="J107" t="inlineStr">
+        <is>
+          <t>БНХ Укр</t>
+        </is>
+      </c>
+    </row>
+    <row r="108">
+      <c r="E108" t="inlineStr">
+        <is>
+          <t>12.00R20</t>
+        </is>
+      </c>
+      <c r="F108" t="inlineStr">
+        <is>
+          <t>ИД-304М</t>
+        </is>
+      </c>
+      <c r="G108" t="inlineStr">
+        <is>
+          <t>16, груз, сер</t>
+        </is>
+      </c>
+      <c r="H108" t="n">
+        <v>3</v>
+      </c>
+      <c r="I108" s="1" t="n">
+        <v>44824</v>
+      </c>
+      <c r="J108" t="inlineStr">
+        <is>
+          <t>БНХ Укр</t>
+        </is>
+      </c>
+    </row>
+    <row r="109">
+      <c r="E109" t="inlineStr">
+        <is>
+          <t>12.00R20</t>
+        </is>
+      </c>
+      <c r="F109" t="inlineStr">
+        <is>
+          <t>ИД-304М</t>
+        </is>
+      </c>
+      <c r="G109" t="inlineStr">
+        <is>
+          <t>18, груз, сер</t>
+        </is>
+      </c>
+      <c r="H109" t="n">
+        <v>3</v>
+      </c>
+      <c r="I109" s="1" t="n">
+        <v>44824</v>
+      </c>
+      <c r="J109" t="inlineStr">
+        <is>
+          <t>БНХ Укр</t>
+        </is>
+      </c>
+    </row>
+    <row r="110">
+      <c r="E110" t="inlineStr">
+        <is>
+          <t>12.00R20</t>
+        </is>
+      </c>
+      <c r="F110" t="inlineStr">
+        <is>
+          <t>ИД-304М</t>
+        </is>
+      </c>
+      <c r="G110" t="inlineStr">
+        <is>
+          <t>16, груз, трп</t>
+        </is>
+      </c>
+      <c r="H110" t="n">
+        <v>3</v>
+      </c>
+      <c r="I110" s="1" t="n">
+        <v>44824</v>
+      </c>
+      <c r="J110" t="inlineStr">
+        <is>
+          <t>БНХ Укр</t>
+        </is>
+      </c>
+    </row>
+    <row r="111">
+      <c r="E111" t="inlineStr">
+        <is>
+          <t>12.00R20</t>
+        </is>
+      </c>
+      <c r="F111" t="inlineStr">
+        <is>
+          <t>ИД-304М</t>
+        </is>
+      </c>
+      <c r="G111" t="inlineStr">
+        <is>
+          <t>18, груз, трп</t>
+        </is>
+      </c>
+      <c r="H111" t="n">
+        <v>3</v>
+      </c>
+      <c r="I111" s="1" t="n">
+        <v>44824</v>
+      </c>
+      <c r="J111" t="inlineStr">
+        <is>
+          <t>БНХ Укр</t>
+        </is>
+      </c>
+    </row>
+    <row r="112">
+      <c r="E112" t="inlineStr">
+        <is>
+          <t>12.00R20</t>
+        </is>
+      </c>
+      <c r="F112" t="inlineStr">
+        <is>
+          <t>БИ-368М</t>
+        </is>
+      </c>
+      <c r="G112" t="inlineStr">
+        <is>
+          <t>18, груз, сер</t>
+        </is>
+      </c>
+      <c r="H112" t="n">
+        <v>3</v>
+      </c>
+      <c r="I112" s="1" t="n">
+        <v>44824</v>
+      </c>
+      <c r="J112" t="inlineStr">
+        <is>
+          <t>БНХ Укр</t>
+        </is>
+      </c>
+    </row>
+    <row r="113">
+      <c r="E113" t="inlineStr">
+        <is>
+          <t>12.00R20</t>
+        </is>
+      </c>
+      <c r="F113" t="inlineStr">
+        <is>
+          <t>БИ-368М</t>
+        </is>
+      </c>
+      <c r="G113" t="inlineStr">
+        <is>
+          <t>18, груз, сер</t>
+        </is>
+      </c>
+      <c r="H113" t="n">
+        <v>3</v>
+      </c>
+      <c r="I113" s="1" t="n">
+        <v>44824</v>
+      </c>
+      <c r="J113" t="inlineStr">
+        <is>
+          <t>БНХ Укр</t>
+        </is>
+      </c>
+    </row>
+    <row r="114">
+      <c r="E114" t="inlineStr">
+        <is>
+          <t>12.00R20</t>
+        </is>
+      </c>
+      <c r="F114" t="inlineStr">
+        <is>
+          <t>БИ-368М</t>
+        </is>
+      </c>
+      <c r="G114" t="inlineStr">
+        <is>
+          <t>18, груз, трп</t>
+        </is>
+      </c>
+      <c r="H114" t="n">
+        <v>3</v>
+      </c>
+      <c r="I114" s="1" t="n">
+        <v>44824</v>
+      </c>
+      <c r="J114" t="inlineStr">
+        <is>
+          <t>БНХ Укр</t>
+        </is>
+      </c>
+    </row>
+    <row r="115">
+      <c r="E115" t="inlineStr">
+        <is>
+          <t>195/65R15</t>
+        </is>
+      </c>
+      <c r="F115" t="inlineStr">
+        <is>
+          <t>BEL-337</t>
+        </is>
+      </c>
+      <c r="G115" t="inlineStr">
+        <is>
+          <t>б/к, легк, сер</t>
+        </is>
+      </c>
+      <c r="H115" t="n">
+        <v>3</v>
+      </c>
+      <c r="I115" s="1" t="n">
+        <v>44824</v>
+      </c>
+      <c r="J115" t="inlineStr">
+        <is>
+          <t>БНХ Укр</t>
+        </is>
+      </c>
+    </row>
+    <row r="116">
+      <c r="E116" t="inlineStr">
+        <is>
+          <t>315/80R22.5</t>
+        </is>
+      </c>
+      <c r="F116" t="inlineStr">
+        <is>
+          <t>BEL-158M</t>
+        </is>
+      </c>
+      <c r="G116" t="inlineStr">
+        <is>
+          <t>груз, камневыт, сер</t>
+        </is>
+      </c>
+      <c r="H116" t="n">
+        <v>4</v>
+      </c>
+      <c r="I116" s="1" t="n">
+        <v>44824</v>
+      </c>
+      <c r="J116" t="inlineStr">
+        <is>
+          <t xml:space="preserve">	БНХ РОС</t>
+        </is>
+      </c>
+    </row>
+    <row r="117">
+      <c r="E117" t="inlineStr">
+        <is>
+          <t>315/80R22.5</t>
+        </is>
+      </c>
+      <c r="F117" t="inlineStr">
+        <is>
+          <t>BEL-158M</t>
+        </is>
+      </c>
+      <c r="G117" t="inlineStr">
+        <is>
+          <t>груз, трп, камневыт</t>
+        </is>
+      </c>
+      <c r="H117" t="n">
+        <v>4</v>
+      </c>
+      <c r="I117" s="1" t="n">
+        <v>44824</v>
+      </c>
+      <c r="J117" t="inlineStr">
+        <is>
+          <t xml:space="preserve">	БНХ РОС</t>
+        </is>
+      </c>
+    </row>
+    <row r="118">
+      <c r="E118" t="inlineStr">
+        <is>
+          <t>315/80R22.5</t>
+        </is>
+      </c>
+      <c r="F118" t="inlineStr">
+        <is>
+          <t>BEL-278</t>
+        </is>
+      </c>
+      <c r="G118" t="inlineStr">
+        <is>
+          <t>груз, сер</t>
+        </is>
+      </c>
+      <c r="H118" t="n">
+        <v>4</v>
+      </c>
+      <c r="I118" s="1" t="n">
+        <v>44824</v>
+      </c>
+      <c r="J118" t="inlineStr">
+        <is>
+          <t xml:space="preserve">	БНХ РОС</t>
+        </is>
+      </c>
+    </row>
+    <row r="119">
+      <c r="E119" t="inlineStr">
+        <is>
+          <t>315/80R22.5</t>
+        </is>
+      </c>
+      <c r="F119" t="inlineStr">
+        <is>
+          <t>BEL-278</t>
+        </is>
+      </c>
+      <c r="G119" t="inlineStr">
+        <is>
+          <t>груз, трп</t>
+        </is>
+      </c>
+      <c r="H119" t="n">
+        <v>4</v>
+      </c>
+      <c r="I119" s="1" t="n">
+        <v>44824</v>
+      </c>
+      <c r="J119" t="inlineStr">
+        <is>
+          <t xml:space="preserve">	БНХ РОС</t>
+        </is>
+      </c>
+    </row>
+    <row r="120">
+      <c r="E120" t="inlineStr">
+        <is>
+          <t>315/80R22.5</t>
+        </is>
+      </c>
+      <c r="F120" t="inlineStr">
+        <is>
+          <t>BEL-268</t>
+        </is>
+      </c>
+      <c r="G120" t="inlineStr">
+        <is>
+          <t>груз, сер</t>
+        </is>
+      </c>
+      <c r="H120" t="n">
+        <v>4</v>
+      </c>
+      <c r="I120" s="1" t="n">
+        <v>44824</v>
+      </c>
+      <c r="J120" t="inlineStr">
+        <is>
+          <t xml:space="preserve">	БНХ РОС</t>
+        </is>
+      </c>
+    </row>
+    <row r="121">
+      <c r="E121" t="inlineStr">
+        <is>
+          <t>315/80R22.5</t>
+        </is>
+      </c>
+      <c r="F121" t="inlineStr">
+        <is>
+          <t>BEL-268</t>
+        </is>
+      </c>
+      <c r="G121" t="inlineStr">
+        <is>
+          <t>груз, трп</t>
+        </is>
+      </c>
+      <c r="H121" t="n">
+        <v>4</v>
+      </c>
+      <c r="I121" s="1" t="n">
+        <v>44824</v>
+      </c>
+      <c r="J121" t="inlineStr">
+        <is>
+          <t xml:space="preserve">	БНХ РОС</t>
+        </is>
+      </c>
+    </row>
+    <row r="122">
+      <c r="E122" t="inlineStr">
+        <is>
+          <t>315/80R22.5</t>
+        </is>
+      </c>
+      <c r="F122" t="inlineStr">
+        <is>
+          <t>BEL-398</t>
+        </is>
+      </c>
+      <c r="G122" t="inlineStr">
+        <is>
+          <t>груз, сер</t>
+        </is>
+      </c>
+      <c r="H122" t="n">
+        <v>4</v>
+      </c>
+      <c r="I122" s="1" t="n">
+        <v>44824</v>
+      </c>
+      <c r="J122" t="inlineStr">
+        <is>
+          <t xml:space="preserve">	БНХ РОС</t>
+        </is>
+      </c>
+    </row>
+    <row r="123">
+      <c r="E123" t="inlineStr">
+        <is>
+          <t>315/80R22.5</t>
+        </is>
+      </c>
+      <c r="F123" t="inlineStr">
+        <is>
+          <t>BEL-326</t>
+        </is>
+      </c>
+      <c r="G123" t="inlineStr">
+        <is>
+          <t>груз, сер</t>
+        </is>
+      </c>
+      <c r="H123" t="n">
+        <v>4</v>
+      </c>
+      <c r="I123" s="1" t="n">
+        <v>44824</v>
+      </c>
+      <c r="J123" t="inlineStr">
+        <is>
+          <t xml:space="preserve">	БНХ РОС</t>
+        </is>
+      </c>
+    </row>
+    <row r="124">
+      <c r="E124" t="inlineStr">
+        <is>
+          <t>315/80R22.5</t>
+        </is>
+      </c>
+      <c r="F124" t="inlineStr">
+        <is>
+          <t>BEL-326</t>
+        </is>
+      </c>
+      <c r="G124" t="inlineStr">
+        <is>
+          <t>груз, трп</t>
+        </is>
+      </c>
+      <c r="H124" t="n">
+        <v>4</v>
+      </c>
+      <c r="I124" s="1" t="n">
+        <v>44824</v>
+      </c>
+      <c r="J124" t="inlineStr">
+        <is>
+          <t xml:space="preserve">	БНХ РОС</t>
+        </is>
+      </c>
+    </row>
+    <row r="125">
+      <c r="E125" t="inlineStr">
+        <is>
+          <t>315/80R22.5</t>
+        </is>
+      </c>
+      <c r="F125" t="inlineStr">
+        <is>
+          <t>BEL-498</t>
+        </is>
+      </c>
+      <c r="G125" t="inlineStr">
+        <is>
+          <t>156L, груз, сер</t>
+        </is>
+      </c>
+      <c r="H125" t="n">
+        <v>4</v>
+      </c>
+      <c r="I125" s="1" t="n">
+        <v>44824</v>
+      </c>
+      <c r="J125" t="inlineStr">
+        <is>
+          <t xml:space="preserve">	БНХ РОС</t>
+        </is>
+      </c>
+    </row>
+    <row r="126">
+      <c r="E126" t="inlineStr">
+        <is>
+          <t>315/80R22.5</t>
+        </is>
+      </c>
+      <c r="F126" t="inlineStr">
+        <is>
+          <t>BEL-518</t>
+        </is>
+      </c>
+      <c r="G126" t="inlineStr">
+        <is>
+          <t>груз, сер</t>
+        </is>
+      </c>
+      <c r="H126" t="n">
+        <v>4</v>
+      </c>
+      <c r="I126" s="1" t="n">
+        <v>44824</v>
+      </c>
+      <c r="J126" t="inlineStr">
+        <is>
+          <t xml:space="preserve">	БНХ РОС</t>
+        </is>
+      </c>
+    </row>
+    <row r="127">
+      <c r="E127" t="inlineStr">
+        <is>
+          <t>12.00R20</t>
+        </is>
+      </c>
+      <c r="F127" t="inlineStr">
+        <is>
+          <t>ИД-304М</t>
+        </is>
+      </c>
+      <c r="G127" t="inlineStr">
+        <is>
+          <t>16, груз, сер</t>
+        </is>
+      </c>
+      <c r="H127" t="n">
+        <v>4</v>
+      </c>
+      <c r="I127" s="1" t="n">
+        <v>44824</v>
+      </c>
+      <c r="J127" t="inlineStr">
+        <is>
+          <t xml:space="preserve">	БНХ РОС</t>
+        </is>
+      </c>
+    </row>
+    <row r="128">
+      <c r="E128" t="inlineStr">
+        <is>
+          <t>12.00R20</t>
+        </is>
+      </c>
+      <c r="F128" t="inlineStr">
+        <is>
+          <t>ИД-304М</t>
+        </is>
+      </c>
+      <c r="G128" t="inlineStr">
+        <is>
+          <t>18, груз, сер</t>
+        </is>
+      </c>
+      <c r="H128" t="n">
+        <v>4</v>
+      </c>
+      <c r="I128" s="1" t="n">
+        <v>44824</v>
+      </c>
+      <c r="J128" t="inlineStr">
+        <is>
+          <t xml:space="preserve">	БНХ РОС</t>
+        </is>
+      </c>
+    </row>
+    <row r="129">
+      <c r="E129" t="inlineStr">
+        <is>
+          <t>12.00R20</t>
+        </is>
+      </c>
+      <c r="F129" t="inlineStr">
+        <is>
+          <t>ИД-304М</t>
+        </is>
+      </c>
+      <c r="G129" t="inlineStr">
+        <is>
+          <t>16, груз, трп</t>
+        </is>
+      </c>
+      <c r="H129" t="n">
+        <v>4</v>
+      </c>
+      <c r="I129" s="1" t="n">
+        <v>44824</v>
+      </c>
+      <c r="J129" t="inlineStr">
+        <is>
+          <t xml:space="preserve">	БНХ РОС</t>
+        </is>
+      </c>
+    </row>
+    <row r="130">
+      <c r="E130" t="inlineStr">
+        <is>
+          <t>12.00R20</t>
+        </is>
+      </c>
+      <c r="F130" t="inlineStr">
+        <is>
+          <t>ИД-304М</t>
+        </is>
+      </c>
+      <c r="G130" t="inlineStr">
+        <is>
+          <t>18, груз, трп</t>
+        </is>
+      </c>
+      <c r="H130" t="n">
+        <v>4</v>
+      </c>
+      <c r="I130" s="1" t="n">
+        <v>44824</v>
+      </c>
+      <c r="J130" t="inlineStr">
+        <is>
+          <t xml:space="preserve">	БНХ РОС</t>
+        </is>
+      </c>
+    </row>
+    <row r="131">
+      <c r="E131" t="inlineStr">
+        <is>
+          <t>12.00R20</t>
+        </is>
+      </c>
+      <c r="F131" t="inlineStr">
+        <is>
+          <t>БИ-368М</t>
+        </is>
+      </c>
+      <c r="G131" t="inlineStr">
+        <is>
+          <t>18, груз, сер</t>
+        </is>
+      </c>
+      <c r="H131" t="n">
+        <v>4</v>
+      </c>
+      <c r="I131" s="1" t="n">
+        <v>44824</v>
+      </c>
+      <c r="J131" t="inlineStr">
+        <is>
+          <t xml:space="preserve">	БНХ РОС</t>
+        </is>
+      </c>
+    </row>
+    <row r="132">
+      <c r="E132" t="inlineStr">
+        <is>
+          <t>12.00R20</t>
+        </is>
+      </c>
+      <c r="F132" t="inlineStr">
+        <is>
+          <t>БИ-368М</t>
+        </is>
+      </c>
+      <c r="G132" t="inlineStr">
+        <is>
+          <t>18, груз, сер</t>
+        </is>
+      </c>
+      <c r="H132" t="n">
+        <v>4</v>
+      </c>
+      <c r="I132" s="1" t="n">
+        <v>44824</v>
+      </c>
+      <c r="J132" t="inlineStr">
+        <is>
+          <t xml:space="preserve">	БНХ РОС</t>
+        </is>
+      </c>
+    </row>
+    <row r="133">
+      <c r="E133" t="inlineStr">
+        <is>
+          <t>12.00R20</t>
+        </is>
+      </c>
+      <c r="F133" t="inlineStr">
+        <is>
+          <t>БИ-368М</t>
+        </is>
+      </c>
+      <c r="G133" t="inlineStr">
+        <is>
+          <t>18, груз, трп</t>
+        </is>
+      </c>
+      <c r="H133" t="n">
+        <v>4</v>
+      </c>
+      <c r="I133" s="1" t="n">
+        <v>44824</v>
+      </c>
+      <c r="J133" t="inlineStr">
+        <is>
+          <t xml:space="preserve">	БНХ РОС</t>
+        </is>
+      </c>
+    </row>
+    <row r="134">
+      <c r="E134" t="inlineStr">
+        <is>
+          <t>195/65R15</t>
+        </is>
+      </c>
+      <c r="F134" t="inlineStr">
+        <is>
+          <t>BEL-337</t>
+        </is>
+      </c>
+      <c r="G134" t="inlineStr">
+        <is>
+          <t>б/к, легк, сер</t>
+        </is>
+      </c>
+      <c r="H134" t="n">
+        <v>4</v>
+      </c>
+      <c r="I134" s="1" t="n">
+        <v>44824</v>
+      </c>
+      <c r="J134" t="inlineStr">
+        <is>
+          <t xml:space="preserve">	БНХ РОС</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
SALES fixed  at 09/09/2022
</commit_message>
<xml_diff>
--- a/src/Tyres.xlsx
+++ b/src/Tyres.xlsx
@@ -417,7 +417,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J96"/>
+  <dimension ref="A1:J115"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -438,7 +438,7 @@
       </c>
       <c r="C1" t="inlineStr">
         <is>
-          <t>груз камневыт сер</t>
+          <t>камневыт груз сер</t>
         </is>
       </c>
       <c r="E1" t="inlineStr">
@@ -485,7 +485,7 @@
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>груз трп камневыт</t>
+          <t>камневыт груз трп</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
@@ -500,18 +500,18 @@
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>груз, камневыт, сер</t>
+          <t>камневыт, груз, сер</t>
         </is>
       </c>
       <c r="H2" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="I2" s="1" t="n">
-        <v>44824</v>
+        <v>44805</v>
       </c>
       <c r="J2" t="inlineStr">
         <is>
-          <t>БНХ РОС</t>
+          <t>БНХ УКР</t>
         </is>
       </c>
     </row>
@@ -543,18 +543,18 @@
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>груз, трп, камневыт</t>
+          <t>камневыт, груз, трп</t>
         </is>
       </c>
       <c r="H3" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="I3" s="1" t="n">
-        <v>44824</v>
+        <v>44805</v>
       </c>
       <c r="J3" t="inlineStr">
         <is>
-          <t>БНХ РОС</t>
+          <t>БНХ УКР</t>
         </is>
       </c>
     </row>
@@ -590,14 +590,14 @@
         </is>
       </c>
       <c r="H4" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="I4" s="1" t="n">
-        <v>44824</v>
+        <v>44805</v>
       </c>
       <c r="J4" t="inlineStr">
         <is>
-          <t>БНХ РОС</t>
+          <t>БНХ УКР</t>
         </is>
       </c>
     </row>
@@ -633,14 +633,14 @@
         </is>
       </c>
       <c r="H5" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="I5" s="1" t="n">
-        <v>44824</v>
+        <v>44805</v>
       </c>
       <c r="J5" t="inlineStr">
         <is>
-          <t>БНХ РОС</t>
+          <t>БНХ УКР</t>
         </is>
       </c>
     </row>
@@ -676,14 +676,14 @@
         </is>
       </c>
       <c r="H6" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="I6" s="1" t="n">
-        <v>44824</v>
+        <v>44805</v>
       </c>
       <c r="J6" t="inlineStr">
         <is>
-          <t>БНХ РОС</t>
+          <t>БНХ УКР</t>
         </is>
       </c>
     </row>
@@ -719,14 +719,14 @@
         </is>
       </c>
       <c r="H7" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="I7" s="1" t="n">
-        <v>44824</v>
+        <v>44805</v>
       </c>
       <c r="J7" t="inlineStr">
         <is>
-          <t>БНХ РОС</t>
+          <t>БНХ УКР</t>
         </is>
       </c>
     </row>
@@ -762,14 +762,14 @@
         </is>
       </c>
       <c r="H8" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="I8" s="1" t="n">
-        <v>44824</v>
+        <v>44805</v>
       </c>
       <c r="J8" t="inlineStr">
         <is>
-          <t>БНХ РОС</t>
+          <t>БНХ УКР</t>
         </is>
       </c>
     </row>
@@ -805,14 +805,14 @@
         </is>
       </c>
       <c r="H9" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="I9" s="1" t="n">
-        <v>44824</v>
+        <v>44805</v>
       </c>
       <c r="J9" t="inlineStr">
         <is>
-          <t>БНХ РОС</t>
+          <t>БНХ УКР</t>
         </is>
       </c>
     </row>
@@ -848,14 +848,14 @@
         </is>
       </c>
       <c r="H10" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="I10" s="1" t="n">
-        <v>44824</v>
+        <v>44805</v>
       </c>
       <c r="J10" t="inlineStr">
         <is>
-          <t>БНХ РОС</t>
+          <t>БНХ УКР</t>
         </is>
       </c>
     </row>
@@ -891,14 +891,14 @@
         </is>
       </c>
       <c r="H11" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="I11" s="1" t="n">
-        <v>44824</v>
+        <v>44805</v>
       </c>
       <c r="J11" t="inlineStr">
         <is>
-          <t>БНХ РОС</t>
+          <t>БНХ УКР</t>
         </is>
       </c>
     </row>
@@ -934,14 +934,14 @@
         </is>
       </c>
       <c r="H12" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="I12" s="1" t="n">
-        <v>44824</v>
+        <v>44805</v>
       </c>
       <c r="J12" t="inlineStr">
         <is>
-          <t>БНХ РОС</t>
+          <t>БНХ УКР</t>
         </is>
       </c>
     </row>
@@ -977,14 +977,14 @@
         </is>
       </c>
       <c r="H13" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="I13" s="1" t="n">
-        <v>44824</v>
+        <v>44805</v>
       </c>
       <c r="J13" t="inlineStr">
         <is>
-          <t>БНХ РОС</t>
+          <t>БНХ УКР</t>
         </is>
       </c>
     </row>
@@ -1020,14 +1020,14 @@
         </is>
       </c>
       <c r="H14" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="I14" s="1" t="n">
-        <v>44824</v>
+        <v>44805</v>
       </c>
       <c r="J14" t="inlineStr">
         <is>
-          <t>БНХ РОС</t>
+          <t>БНХ УКР</t>
         </is>
       </c>
     </row>
@@ -1063,14 +1063,14 @@
         </is>
       </c>
       <c r="H15" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="I15" s="1" t="n">
-        <v>44824</v>
+        <v>44805</v>
       </c>
       <c r="J15" t="inlineStr">
         <is>
-          <t>БНХ РОС</t>
+          <t>БНХ УКР</t>
         </is>
       </c>
     </row>
@@ -1106,14 +1106,14 @@
         </is>
       </c>
       <c r="H16" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="I16" s="1" t="n">
-        <v>44824</v>
+        <v>44805</v>
       </c>
       <c r="J16" t="inlineStr">
         <is>
-          <t>БНХ РОС</t>
+          <t>БНХ УКР</t>
         </is>
       </c>
     </row>
@@ -1149,14 +1149,14 @@
         </is>
       </c>
       <c r="H17" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="I17" s="1" t="n">
-        <v>44824</v>
+        <v>44805</v>
       </c>
       <c r="J17" t="inlineStr">
         <is>
-          <t>БНХ РОС</t>
+          <t>БНХ УКР</t>
         </is>
       </c>
     </row>
@@ -1192,14 +1192,14 @@
         </is>
       </c>
       <c r="H18" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="I18" s="1" t="n">
-        <v>44824</v>
+        <v>44805</v>
       </c>
       <c r="J18" t="inlineStr">
         <is>
-          <t>БНХ РОС</t>
+          <t>БНХ УКР</t>
         </is>
       </c>
     </row>
@@ -1235,14 +1235,14 @@
         </is>
       </c>
       <c r="H19" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="I19" s="1" t="n">
-        <v>44824</v>
+        <v>44805</v>
       </c>
       <c r="J19" t="inlineStr">
         <is>
-          <t>БНХ РОС</t>
+          <t>БНХ УКР</t>
         </is>
       </c>
     </row>
@@ -1263,14 +1263,14 @@
         </is>
       </c>
       <c r="H20" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="I20" s="1" t="n">
-        <v>44824</v>
+        <v>44805</v>
       </c>
       <c r="J20" t="inlineStr">
         <is>
-          <t>БНХ РОС</t>
+          <t>БНХ УКР</t>
         </is>
       </c>
     </row>
@@ -1287,14 +1287,14 @@
       </c>
       <c r="G21" t="inlineStr">
         <is>
-          <t>груз, камневыт, сер</t>
+          <t>камневыт, груз, сер</t>
         </is>
       </c>
       <c r="H21" t="n">
         <v>3</v>
       </c>
       <c r="I21" s="1" t="n">
-        <v>44824</v>
+        <v>44806</v>
       </c>
       <c r="J21" t="inlineStr">
         <is>
@@ -1315,14 +1315,14 @@
       </c>
       <c r="G22" t="inlineStr">
         <is>
-          <t>груз, трп, камневыт</t>
+          <t>камневыт, груз, трп</t>
         </is>
       </c>
       <c r="H22" t="n">
         <v>3</v>
       </c>
       <c r="I22" s="1" t="n">
-        <v>44824</v>
+        <v>44806</v>
       </c>
       <c r="J22" t="inlineStr">
         <is>
@@ -1350,7 +1350,7 @@
         <v>3</v>
       </c>
       <c r="I23" s="1" t="n">
-        <v>44824</v>
+        <v>44806</v>
       </c>
       <c r="J23" t="inlineStr">
         <is>
@@ -1378,7 +1378,7 @@
         <v>3</v>
       </c>
       <c r="I24" s="1" t="n">
-        <v>44824</v>
+        <v>44806</v>
       </c>
       <c r="J24" t="inlineStr">
         <is>
@@ -1406,7 +1406,7 @@
         <v>3</v>
       </c>
       <c r="I25" s="1" t="n">
-        <v>44824</v>
+        <v>44806</v>
       </c>
       <c r="J25" t="inlineStr">
         <is>
@@ -1434,7 +1434,7 @@
         <v>3</v>
       </c>
       <c r="I26" s="1" t="n">
-        <v>44824</v>
+        <v>44806</v>
       </c>
       <c r="J26" t="inlineStr">
         <is>
@@ -1462,7 +1462,7 @@
         <v>3</v>
       </c>
       <c r="I27" s="1" t="n">
-        <v>44824</v>
+        <v>44806</v>
       </c>
       <c r="J27" t="inlineStr">
         <is>
@@ -1490,7 +1490,7 @@
         <v>3</v>
       </c>
       <c r="I28" s="1" t="n">
-        <v>44824</v>
+        <v>44806</v>
       </c>
       <c r="J28" t="inlineStr">
         <is>
@@ -1518,7 +1518,7 @@
         <v>3</v>
       </c>
       <c r="I29" s="1" t="n">
-        <v>44824</v>
+        <v>44806</v>
       </c>
       <c r="J29" t="inlineStr">
         <is>
@@ -1546,7 +1546,7 @@
         <v>3</v>
       </c>
       <c r="I30" s="1" t="n">
-        <v>44824</v>
+        <v>44806</v>
       </c>
       <c r="J30" t="inlineStr">
         <is>
@@ -1574,7 +1574,7 @@
         <v>3</v>
       </c>
       <c r="I31" s="1" t="n">
-        <v>44824</v>
+        <v>44806</v>
       </c>
       <c r="J31" t="inlineStr">
         <is>
@@ -1602,7 +1602,7 @@
         <v>3</v>
       </c>
       <c r="I32" s="1" t="n">
-        <v>44824</v>
+        <v>44806</v>
       </c>
       <c r="J32" t="inlineStr">
         <is>
@@ -1630,7 +1630,7 @@
         <v>3</v>
       </c>
       <c r="I33" s="1" t="n">
-        <v>44824</v>
+        <v>44806</v>
       </c>
       <c r="J33" t="inlineStr">
         <is>
@@ -1658,7 +1658,7 @@
         <v>3</v>
       </c>
       <c r="I34" s="1" t="n">
-        <v>44824</v>
+        <v>44806</v>
       </c>
       <c r="J34" t="inlineStr">
         <is>
@@ -1686,7 +1686,7 @@
         <v>3</v>
       </c>
       <c r="I35" s="1" t="n">
-        <v>44824</v>
+        <v>44806</v>
       </c>
       <c r="J35" t="inlineStr">
         <is>
@@ -1714,7 +1714,7 @@
         <v>3</v>
       </c>
       <c r="I36" s="1" t="n">
-        <v>44824</v>
+        <v>44806</v>
       </c>
       <c r="J36" t="inlineStr">
         <is>
@@ -1742,7 +1742,7 @@
         <v>3</v>
       </c>
       <c r="I37" s="1" t="n">
-        <v>44824</v>
+        <v>44806</v>
       </c>
       <c r="J37" t="inlineStr">
         <is>
@@ -1770,7 +1770,7 @@
         <v>3</v>
       </c>
       <c r="I38" s="1" t="n">
-        <v>44824</v>
+        <v>44806</v>
       </c>
       <c r="J38" t="inlineStr">
         <is>
@@ -1798,7 +1798,7 @@
         <v>3</v>
       </c>
       <c r="I39" s="1" t="n">
-        <v>44824</v>
+        <v>44806</v>
       </c>
       <c r="J39" t="inlineStr">
         <is>
@@ -1819,18 +1819,18 @@
       </c>
       <c r="G40" t="inlineStr">
         <is>
-          <t>груз, камневыт, сер</t>
+          <t>камневыт, груз, сер</t>
         </is>
       </c>
       <c r="H40" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="I40" s="1" t="n">
-        <v>44824</v>
+        <v>44807</v>
       </c>
       <c r="J40" t="inlineStr">
         <is>
-          <t>БНХ Польска</t>
+          <t>БНХ УКР</t>
         </is>
       </c>
     </row>
@@ -1847,18 +1847,18 @@
       </c>
       <c r="G41" t="inlineStr">
         <is>
-          <t>груз, трп, камневыт</t>
+          <t>камневыт, груз, трп</t>
         </is>
       </c>
       <c r="H41" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="I41" s="1" t="n">
-        <v>44824</v>
+        <v>44807</v>
       </c>
       <c r="J41" t="inlineStr">
         <is>
-          <t>БНХ Польска</t>
+          <t>БНХ УКР</t>
         </is>
       </c>
     </row>
@@ -1879,14 +1879,14 @@
         </is>
       </c>
       <c r="H42" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="I42" s="1" t="n">
-        <v>44824</v>
+        <v>44807</v>
       </c>
       <c r="J42" t="inlineStr">
         <is>
-          <t>БНХ Польска</t>
+          <t>БНХ УКР</t>
         </is>
       </c>
     </row>
@@ -1907,14 +1907,14 @@
         </is>
       </c>
       <c r="H43" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="I43" s="1" t="n">
-        <v>44824</v>
+        <v>44807</v>
       </c>
       <c r="J43" t="inlineStr">
         <is>
-          <t>БНХ Польска</t>
+          <t>БНХ УКР</t>
         </is>
       </c>
     </row>
@@ -1935,14 +1935,14 @@
         </is>
       </c>
       <c r="H44" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="I44" s="1" t="n">
-        <v>44824</v>
+        <v>44807</v>
       </c>
       <c r="J44" t="inlineStr">
         <is>
-          <t>БНХ Польска</t>
+          <t>БНХ УКР</t>
         </is>
       </c>
     </row>
@@ -1963,14 +1963,14 @@
         </is>
       </c>
       <c r="H45" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="I45" s="1" t="n">
-        <v>44824</v>
+        <v>44807</v>
       </c>
       <c r="J45" t="inlineStr">
         <is>
-          <t>БНХ Польска</t>
+          <t>БНХ УКР</t>
         </is>
       </c>
     </row>
@@ -1991,14 +1991,14 @@
         </is>
       </c>
       <c r="H46" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="I46" s="1" t="n">
-        <v>44824</v>
+        <v>44807</v>
       </c>
       <c r="J46" t="inlineStr">
         <is>
-          <t>БНХ Польска</t>
+          <t>БНХ УКР</t>
         </is>
       </c>
     </row>
@@ -2019,14 +2019,14 @@
         </is>
       </c>
       <c r="H47" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="I47" s="1" t="n">
-        <v>44824</v>
+        <v>44807</v>
       </c>
       <c r="J47" t="inlineStr">
         <is>
-          <t>БНХ Польска</t>
+          <t>БНХ УКР</t>
         </is>
       </c>
     </row>
@@ -2047,14 +2047,14 @@
         </is>
       </c>
       <c r="H48" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="I48" s="1" t="n">
-        <v>44824</v>
+        <v>44807</v>
       </c>
       <c r="J48" t="inlineStr">
         <is>
-          <t>БНХ Польска</t>
+          <t>БНХ УКР</t>
         </is>
       </c>
     </row>
@@ -2075,14 +2075,14 @@
         </is>
       </c>
       <c r="H49" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="I49" s="1" t="n">
-        <v>44824</v>
+        <v>44807</v>
       </c>
       <c r="J49" t="inlineStr">
         <is>
-          <t>БНХ Польска</t>
+          <t>БНХ УКР</t>
         </is>
       </c>
     </row>
@@ -2103,14 +2103,14 @@
         </is>
       </c>
       <c r="H50" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="I50" s="1" t="n">
-        <v>44824</v>
+        <v>44807</v>
       </c>
       <c r="J50" t="inlineStr">
         <is>
-          <t>БНХ Польска</t>
+          <t>БНХ УКР</t>
         </is>
       </c>
     </row>
@@ -2131,14 +2131,14 @@
         </is>
       </c>
       <c r="H51" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="I51" s="1" t="n">
-        <v>44824</v>
+        <v>44807</v>
       </c>
       <c r="J51" t="inlineStr">
         <is>
-          <t>БНХ Польска</t>
+          <t>БНХ УКР</t>
         </is>
       </c>
     </row>
@@ -2159,14 +2159,14 @@
         </is>
       </c>
       <c r="H52" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="I52" s="1" t="n">
-        <v>44824</v>
+        <v>44807</v>
       </c>
       <c r="J52" t="inlineStr">
         <is>
-          <t>БНХ Польска</t>
+          <t>БНХ УКР</t>
         </is>
       </c>
     </row>
@@ -2187,14 +2187,14 @@
         </is>
       </c>
       <c r="H53" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="I53" s="1" t="n">
-        <v>44824</v>
+        <v>44807</v>
       </c>
       <c r="J53" t="inlineStr">
         <is>
-          <t>БНХ Польска</t>
+          <t>БНХ УКР</t>
         </is>
       </c>
     </row>
@@ -2215,14 +2215,14 @@
         </is>
       </c>
       <c r="H54" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="I54" s="1" t="n">
-        <v>44824</v>
+        <v>44807</v>
       </c>
       <c r="J54" t="inlineStr">
         <is>
-          <t>БНХ Польска</t>
+          <t>БНХ УКР</t>
         </is>
       </c>
     </row>
@@ -2243,14 +2243,14 @@
         </is>
       </c>
       <c r="H55" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="I55" s="1" t="n">
-        <v>44824</v>
+        <v>44807</v>
       </c>
       <c r="J55" t="inlineStr">
         <is>
-          <t>БНХ Польска</t>
+          <t>БНХ УКР</t>
         </is>
       </c>
     </row>
@@ -2271,14 +2271,14 @@
         </is>
       </c>
       <c r="H56" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="I56" s="1" t="n">
-        <v>44824</v>
+        <v>44807</v>
       </c>
       <c r="J56" t="inlineStr">
         <is>
-          <t>БНХ Польска</t>
+          <t>БНХ УКР</t>
         </is>
       </c>
     </row>
@@ -2299,14 +2299,14 @@
         </is>
       </c>
       <c r="H57" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="I57" s="1" t="n">
-        <v>44824</v>
+        <v>44807</v>
       </c>
       <c r="J57" t="inlineStr">
         <is>
-          <t>БНХ Польска</t>
+          <t>БНХ УКР</t>
         </is>
       </c>
     </row>
@@ -2327,14 +2327,14 @@
         </is>
       </c>
       <c r="H58" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="I58" s="1" t="n">
-        <v>44824</v>
+        <v>44807</v>
       </c>
       <c r="J58" t="inlineStr">
         <is>
-          <t>БНХ Польска</t>
+          <t>БНХ УКР</t>
         </is>
       </c>
     </row>
@@ -2351,18 +2351,18 @@
       </c>
       <c r="G59" t="inlineStr">
         <is>
-          <t>груз, камневыт, сер</t>
+          <t>камневыт, груз, сер</t>
         </is>
       </c>
       <c r="H59" t="n">
         <v>6</v>
       </c>
       <c r="I59" s="1" t="n">
-        <v>44769</v>
+        <v>44807</v>
       </c>
       <c r="J59" t="inlineStr">
         <is>
-          <t>БНХ Польска</t>
+          <t>БНХ РОС</t>
         </is>
       </c>
     </row>
@@ -2379,18 +2379,18 @@
       </c>
       <c r="G60" t="inlineStr">
         <is>
-          <t>груз, трп, камневыт</t>
+          <t>камневыт, груз, трп</t>
         </is>
       </c>
       <c r="H60" t="n">
         <v>6</v>
       </c>
       <c r="I60" s="1" t="n">
-        <v>44769</v>
+        <v>44807</v>
       </c>
       <c r="J60" t="inlineStr">
         <is>
-          <t>БНХ Польска</t>
+          <t>БНХ РОС</t>
         </is>
       </c>
     </row>
@@ -2414,11 +2414,11 @@
         <v>6</v>
       </c>
       <c r="I61" s="1" t="n">
-        <v>44769</v>
+        <v>44807</v>
       </c>
       <c r="J61" t="inlineStr">
         <is>
-          <t>БНХ Польска</t>
+          <t>БНХ РОС</t>
         </is>
       </c>
     </row>
@@ -2442,11 +2442,11 @@
         <v>6</v>
       </c>
       <c r="I62" s="1" t="n">
-        <v>44769</v>
+        <v>44807</v>
       </c>
       <c r="J62" t="inlineStr">
         <is>
-          <t>БНХ Польска</t>
+          <t>БНХ РОС</t>
         </is>
       </c>
     </row>
@@ -2470,11 +2470,11 @@
         <v>6</v>
       </c>
       <c r="I63" s="1" t="n">
-        <v>44769</v>
+        <v>44807</v>
       </c>
       <c r="J63" t="inlineStr">
         <is>
-          <t>БНХ Польска</t>
+          <t>БНХ РОС</t>
         </is>
       </c>
     </row>
@@ -2498,11 +2498,11 @@
         <v>6</v>
       </c>
       <c r="I64" s="1" t="n">
-        <v>44769</v>
+        <v>44807</v>
       </c>
       <c r="J64" t="inlineStr">
         <is>
-          <t>БНХ Польска</t>
+          <t>БНХ РОС</t>
         </is>
       </c>
     </row>
@@ -2526,11 +2526,11 @@
         <v>6</v>
       </c>
       <c r="I65" s="1" t="n">
-        <v>44769</v>
+        <v>44807</v>
       </c>
       <c r="J65" t="inlineStr">
         <is>
-          <t>БНХ Польска</t>
+          <t>БНХ РОС</t>
         </is>
       </c>
     </row>
@@ -2554,11 +2554,11 @@
         <v>6</v>
       </c>
       <c r="I66" s="1" t="n">
-        <v>44769</v>
+        <v>44807</v>
       </c>
       <c r="J66" t="inlineStr">
         <is>
-          <t>БНХ Польска</t>
+          <t>БНХ РОС</t>
         </is>
       </c>
     </row>
@@ -2582,11 +2582,11 @@
         <v>6</v>
       </c>
       <c r="I67" s="1" t="n">
-        <v>44769</v>
+        <v>44807</v>
       </c>
       <c r="J67" t="inlineStr">
         <is>
-          <t>БНХ Польска</t>
+          <t>БНХ РОС</t>
         </is>
       </c>
     </row>
@@ -2610,11 +2610,11 @@
         <v>6</v>
       </c>
       <c r="I68" s="1" t="n">
-        <v>44769</v>
+        <v>44807</v>
       </c>
       <c r="J68" t="inlineStr">
         <is>
-          <t>БНХ Польска</t>
+          <t>БНХ РОС</t>
         </is>
       </c>
     </row>
@@ -2638,11 +2638,11 @@
         <v>6</v>
       </c>
       <c r="I69" s="1" t="n">
-        <v>44769</v>
+        <v>44807</v>
       </c>
       <c r="J69" t="inlineStr">
         <is>
-          <t>БНХ Польска</t>
+          <t>БНХ РОС</t>
         </is>
       </c>
     </row>
@@ -2666,11 +2666,11 @@
         <v>6</v>
       </c>
       <c r="I70" s="1" t="n">
-        <v>44769</v>
+        <v>44807</v>
       </c>
       <c r="J70" t="inlineStr">
         <is>
-          <t>БНХ Польска</t>
+          <t>БНХ РОС</t>
         </is>
       </c>
     </row>
@@ -2694,11 +2694,11 @@
         <v>6</v>
       </c>
       <c r="I71" s="1" t="n">
-        <v>44769</v>
+        <v>44807</v>
       </c>
       <c r="J71" t="inlineStr">
         <is>
-          <t>БНХ Польска</t>
+          <t>БНХ РОС</t>
         </is>
       </c>
     </row>
@@ -2722,11 +2722,11 @@
         <v>6</v>
       </c>
       <c r="I72" s="1" t="n">
-        <v>44769</v>
+        <v>44807</v>
       </c>
       <c r="J72" t="inlineStr">
         <is>
-          <t>БНХ Польска</t>
+          <t>БНХ РОС</t>
         </is>
       </c>
     </row>
@@ -2750,11 +2750,11 @@
         <v>6</v>
       </c>
       <c r="I73" s="1" t="n">
-        <v>44769</v>
+        <v>44807</v>
       </c>
       <c r="J73" t="inlineStr">
         <is>
-          <t>БНХ Польска</t>
+          <t>БНХ РОС</t>
         </is>
       </c>
     </row>
@@ -2778,11 +2778,11 @@
         <v>6</v>
       </c>
       <c r="I74" s="1" t="n">
-        <v>44769</v>
+        <v>44807</v>
       </c>
       <c r="J74" t="inlineStr">
         <is>
-          <t>БНХ Польска</t>
+          <t>БНХ РОС</t>
         </is>
       </c>
     </row>
@@ -2806,11 +2806,11 @@
         <v>6</v>
       </c>
       <c r="I75" s="1" t="n">
-        <v>44769</v>
+        <v>44807</v>
       </c>
       <c r="J75" t="inlineStr">
         <is>
-          <t>БНХ Польска</t>
+          <t>БНХ РОС</t>
         </is>
       </c>
     </row>
@@ -2834,11 +2834,11 @@
         <v>6</v>
       </c>
       <c r="I76" s="1" t="n">
-        <v>44769</v>
+        <v>44807</v>
       </c>
       <c r="J76" t="inlineStr">
         <is>
-          <t>БНХ Польска</t>
+          <t>БНХ РОС</t>
         </is>
       </c>
     </row>
@@ -2862,11 +2862,11 @@
         <v>6</v>
       </c>
       <c r="I77" s="1" t="n">
-        <v>44769</v>
+        <v>44807</v>
       </c>
       <c r="J77" t="inlineStr">
         <is>
-          <t>БНХ Польска</t>
+          <t>БНХ РОС</t>
         </is>
       </c>
     </row>
@@ -2883,18 +2883,18 @@
       </c>
       <c r="G78" t="inlineStr">
         <is>
-          <t>груз, камневыт, сер</t>
+          <t>камневыт, груз, сер</t>
         </is>
       </c>
       <c r="H78" t="n">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="I78" s="1" t="n">
-        <v>44696</v>
+        <v>44807</v>
       </c>
       <c r="J78" t="inlineStr">
         <is>
-          <t>БНХ Польска</t>
+          <t>БНХ ПОЛЬСКА</t>
         </is>
       </c>
     </row>
@@ -2911,18 +2911,18 @@
       </c>
       <c r="G79" t="inlineStr">
         <is>
-          <t>груз, трп, камневыт</t>
+          <t>камневыт, груз, трп</t>
         </is>
       </c>
       <c r="H79" t="n">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="I79" s="1" t="n">
-        <v>44696</v>
+        <v>44807</v>
       </c>
       <c r="J79" t="inlineStr">
         <is>
-          <t>БНХ Польска</t>
+          <t>БНХ ПОЛЬСКА</t>
         </is>
       </c>
     </row>
@@ -2943,14 +2943,14 @@
         </is>
       </c>
       <c r="H80" t="n">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="I80" s="1" t="n">
-        <v>44696</v>
+        <v>44807</v>
       </c>
       <c r="J80" t="inlineStr">
         <is>
-          <t>БНХ Польска</t>
+          <t>БНХ ПОЛЬСКА</t>
         </is>
       </c>
     </row>
@@ -2971,14 +2971,14 @@
         </is>
       </c>
       <c r="H81" t="n">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="I81" s="1" t="n">
-        <v>44696</v>
+        <v>44807</v>
       </c>
       <c r="J81" t="inlineStr">
         <is>
-          <t>БНХ Польска</t>
+          <t>БНХ ПОЛЬСКА</t>
         </is>
       </c>
     </row>
@@ -2999,14 +2999,14 @@
         </is>
       </c>
       <c r="H82" t="n">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="I82" s="1" t="n">
-        <v>44696</v>
+        <v>44807</v>
       </c>
       <c r="J82" t="inlineStr">
         <is>
-          <t>БНХ Польска</t>
+          <t>БНХ ПОЛЬСКА</t>
         </is>
       </c>
     </row>
@@ -3027,14 +3027,14 @@
         </is>
       </c>
       <c r="H83" t="n">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="I83" s="1" t="n">
-        <v>44696</v>
+        <v>44807</v>
       </c>
       <c r="J83" t="inlineStr">
         <is>
-          <t>БНХ Польска</t>
+          <t>БНХ ПОЛЬСКА</t>
         </is>
       </c>
     </row>
@@ -3055,14 +3055,14 @@
         </is>
       </c>
       <c r="H84" t="n">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="I84" s="1" t="n">
-        <v>44696</v>
+        <v>44807</v>
       </c>
       <c r="J84" t="inlineStr">
         <is>
-          <t>БНХ Польска</t>
+          <t>БНХ ПОЛЬСКА</t>
         </is>
       </c>
     </row>
@@ -3083,14 +3083,14 @@
         </is>
       </c>
       <c r="H85" t="n">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="I85" s="1" t="n">
-        <v>44696</v>
+        <v>44807</v>
       </c>
       <c r="J85" t="inlineStr">
         <is>
-          <t>БНХ Польска</t>
+          <t>БНХ ПОЛЬСКА</t>
         </is>
       </c>
     </row>
@@ -3111,14 +3111,14 @@
         </is>
       </c>
       <c r="H86" t="n">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="I86" s="1" t="n">
-        <v>44696</v>
+        <v>44807</v>
       </c>
       <c r="J86" t="inlineStr">
         <is>
-          <t>БНХ Польска</t>
+          <t>БНХ ПОЛЬСКА</t>
         </is>
       </c>
     </row>
@@ -3139,14 +3139,14 @@
         </is>
       </c>
       <c r="H87" t="n">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="I87" s="1" t="n">
-        <v>44696</v>
+        <v>44807</v>
       </c>
       <c r="J87" t="inlineStr">
         <is>
-          <t>БНХ Польска</t>
+          <t>БНХ ПОЛЬСКА</t>
         </is>
       </c>
     </row>
@@ -3167,14 +3167,14 @@
         </is>
       </c>
       <c r="H88" t="n">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="I88" s="1" t="n">
-        <v>44696</v>
+        <v>44807</v>
       </c>
       <c r="J88" t="inlineStr">
         <is>
-          <t>БНХ Польска</t>
+          <t>БНХ ПОЛЬСКА</t>
         </is>
       </c>
     </row>
@@ -3195,14 +3195,14 @@
         </is>
       </c>
       <c r="H89" t="n">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="I89" s="1" t="n">
-        <v>44696</v>
+        <v>44807</v>
       </c>
       <c r="J89" t="inlineStr">
         <is>
-          <t>БНХ Польска</t>
+          <t>БНХ ПОЛЬСКА</t>
         </is>
       </c>
     </row>
@@ -3223,14 +3223,14 @@
         </is>
       </c>
       <c r="H90" t="n">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="I90" s="1" t="n">
-        <v>44696</v>
+        <v>44807</v>
       </c>
       <c r="J90" t="inlineStr">
         <is>
-          <t>БНХ Польска</t>
+          <t>БНХ ПОЛЬСКА</t>
         </is>
       </c>
     </row>
@@ -3251,14 +3251,14 @@
         </is>
       </c>
       <c r="H91" t="n">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="I91" s="1" t="n">
-        <v>44696</v>
+        <v>44807</v>
       </c>
       <c r="J91" t="inlineStr">
         <is>
-          <t>БНХ Польска</t>
+          <t>БНХ ПОЛЬСКА</t>
         </is>
       </c>
     </row>
@@ -3279,14 +3279,14 @@
         </is>
       </c>
       <c r="H92" t="n">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="I92" s="1" t="n">
-        <v>44696</v>
+        <v>44807</v>
       </c>
       <c r="J92" t="inlineStr">
         <is>
-          <t>БНХ Польска</t>
+          <t>БНХ ПОЛЬСКА</t>
         </is>
       </c>
     </row>
@@ -3307,14 +3307,14 @@
         </is>
       </c>
       <c r="H93" t="n">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="I93" s="1" t="n">
-        <v>44696</v>
+        <v>44807</v>
       </c>
       <c r="J93" t="inlineStr">
         <is>
-          <t>БНХ Польска</t>
+          <t>БНХ ПОЛЬСКА</t>
         </is>
       </c>
     </row>
@@ -3335,14 +3335,14 @@
         </is>
       </c>
       <c r="H94" t="n">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="I94" s="1" t="n">
-        <v>44696</v>
+        <v>44807</v>
       </c>
       <c r="J94" t="inlineStr">
         <is>
-          <t>БНХ Польска</t>
+          <t>БНХ ПОЛЬСКА</t>
         </is>
       </c>
     </row>
@@ -3363,14 +3363,14 @@
         </is>
       </c>
       <c r="H95" t="n">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="I95" s="1" t="n">
-        <v>44696</v>
+        <v>44807</v>
       </c>
       <c r="J95" t="inlineStr">
         <is>
-          <t>БНХ Польска</t>
+          <t>БНХ ПОЛЬСКА</t>
         </is>
       </c>
     </row>
@@ -3391,14 +3391,546 @@
         </is>
       </c>
       <c r="H96" t="n">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="I96" s="1" t="n">
-        <v>44696</v>
+        <v>44807</v>
       </c>
       <c r="J96" t="inlineStr">
         <is>
-          <t>БНХ Польска</t>
+          <t>БНХ ПОЛЬСКА</t>
+        </is>
+      </c>
+    </row>
+    <row r="97">
+      <c r="E97" t="inlineStr">
+        <is>
+          <t>315/80R22.5</t>
+        </is>
+      </c>
+      <c r="F97" t="inlineStr">
+        <is>
+          <t>BEL-158M</t>
+        </is>
+      </c>
+      <c r="G97" t="inlineStr">
+        <is>
+          <t>камневыт, груз, сер</t>
+        </is>
+      </c>
+      <c r="H97" t="n">
+        <v>8</v>
+      </c>
+      <c r="I97" s="1" t="n">
+        <v>44745</v>
+      </c>
+      <c r="J97" t="inlineStr">
+        <is>
+          <t>БНХ ПОЛЬСКА</t>
+        </is>
+      </c>
+    </row>
+    <row r="98">
+      <c r="E98" t="inlineStr">
+        <is>
+          <t>315/80R22.5</t>
+        </is>
+      </c>
+      <c r="F98" t="inlineStr">
+        <is>
+          <t>BEL-158M</t>
+        </is>
+      </c>
+      <c r="G98" t="inlineStr">
+        <is>
+          <t>камневыт, груз, трп</t>
+        </is>
+      </c>
+      <c r="H98" t="n">
+        <v>8</v>
+      </c>
+      <c r="I98" s="1" t="n">
+        <v>44745</v>
+      </c>
+      <c r="J98" t="inlineStr">
+        <is>
+          <t>БНХ ПОЛЬСКА</t>
+        </is>
+      </c>
+    </row>
+    <row r="99">
+      <c r="E99" t="inlineStr">
+        <is>
+          <t>315/80R22.5</t>
+        </is>
+      </c>
+      <c r="F99" t="inlineStr">
+        <is>
+          <t>BEL-278</t>
+        </is>
+      </c>
+      <c r="G99" t="inlineStr">
+        <is>
+          <t>груз, сер</t>
+        </is>
+      </c>
+      <c r="H99" t="n">
+        <v>8</v>
+      </c>
+      <c r="I99" s="1" t="n">
+        <v>44745</v>
+      </c>
+      <c r="J99" t="inlineStr">
+        <is>
+          <t>БНХ ПОЛЬСКА</t>
+        </is>
+      </c>
+    </row>
+    <row r="100">
+      <c r="E100" t="inlineStr">
+        <is>
+          <t>315/80R22.5</t>
+        </is>
+      </c>
+      <c r="F100" t="inlineStr">
+        <is>
+          <t>BEL-278</t>
+        </is>
+      </c>
+      <c r="G100" t="inlineStr">
+        <is>
+          <t>груз, трп</t>
+        </is>
+      </c>
+      <c r="H100" t="n">
+        <v>8</v>
+      </c>
+      <c r="I100" s="1" t="n">
+        <v>44745</v>
+      </c>
+      <c r="J100" t="inlineStr">
+        <is>
+          <t>БНХ ПОЛЬСКА</t>
+        </is>
+      </c>
+    </row>
+    <row r="101">
+      <c r="E101" t="inlineStr">
+        <is>
+          <t>315/80R22.5</t>
+        </is>
+      </c>
+      <c r="F101" t="inlineStr">
+        <is>
+          <t>BEL-268</t>
+        </is>
+      </c>
+      <c r="G101" t="inlineStr">
+        <is>
+          <t>груз, сер</t>
+        </is>
+      </c>
+      <c r="H101" t="n">
+        <v>8</v>
+      </c>
+      <c r="I101" s="1" t="n">
+        <v>44745</v>
+      </c>
+      <c r="J101" t="inlineStr">
+        <is>
+          <t>БНХ ПОЛЬСКА</t>
+        </is>
+      </c>
+    </row>
+    <row r="102">
+      <c r="E102" t="inlineStr">
+        <is>
+          <t>315/80R22.5</t>
+        </is>
+      </c>
+      <c r="F102" t="inlineStr">
+        <is>
+          <t>BEL-268</t>
+        </is>
+      </c>
+      <c r="G102" t="inlineStr">
+        <is>
+          <t>груз, трп</t>
+        </is>
+      </c>
+      <c r="H102" t="n">
+        <v>8</v>
+      </c>
+      <c r="I102" s="1" t="n">
+        <v>44745</v>
+      </c>
+      <c r="J102" t="inlineStr">
+        <is>
+          <t>БНХ ПОЛЬСКА</t>
+        </is>
+      </c>
+    </row>
+    <row r="103">
+      <c r="E103" t="inlineStr">
+        <is>
+          <t>315/80R22.5</t>
+        </is>
+      </c>
+      <c r="F103" t="inlineStr">
+        <is>
+          <t>BEL-398</t>
+        </is>
+      </c>
+      <c r="G103" t="inlineStr">
+        <is>
+          <t>груз, сер</t>
+        </is>
+      </c>
+      <c r="H103" t="n">
+        <v>8</v>
+      </c>
+      <c r="I103" s="1" t="n">
+        <v>44745</v>
+      </c>
+      <c r="J103" t="inlineStr">
+        <is>
+          <t>БНХ ПОЛЬСКА</t>
+        </is>
+      </c>
+    </row>
+    <row r="104">
+      <c r="E104" t="inlineStr">
+        <is>
+          <t>315/80R22.5</t>
+        </is>
+      </c>
+      <c r="F104" t="inlineStr">
+        <is>
+          <t>BEL-326</t>
+        </is>
+      </c>
+      <c r="G104" t="inlineStr">
+        <is>
+          <t>груз, сер</t>
+        </is>
+      </c>
+      <c r="H104" t="n">
+        <v>8</v>
+      </c>
+      <c r="I104" s="1" t="n">
+        <v>44745</v>
+      </c>
+      <c r="J104" t="inlineStr">
+        <is>
+          <t>БНХ ПОЛЬСКА</t>
+        </is>
+      </c>
+    </row>
+    <row r="105">
+      <c r="E105" t="inlineStr">
+        <is>
+          <t>315/80R22.5</t>
+        </is>
+      </c>
+      <c r="F105" t="inlineStr">
+        <is>
+          <t>BEL-326</t>
+        </is>
+      </c>
+      <c r="G105" t="inlineStr">
+        <is>
+          <t>груз, трп</t>
+        </is>
+      </c>
+      <c r="H105" t="n">
+        <v>8</v>
+      </c>
+      <c r="I105" s="1" t="n">
+        <v>44745</v>
+      </c>
+      <c r="J105" t="inlineStr">
+        <is>
+          <t>БНХ ПОЛЬСКА</t>
+        </is>
+      </c>
+    </row>
+    <row r="106">
+      <c r="E106" t="inlineStr">
+        <is>
+          <t>315/80R22.5</t>
+        </is>
+      </c>
+      <c r="F106" t="inlineStr">
+        <is>
+          <t>BEL-498</t>
+        </is>
+      </c>
+      <c r="G106" t="inlineStr">
+        <is>
+          <t>156L, груз, сер</t>
+        </is>
+      </c>
+      <c r="H106" t="n">
+        <v>8</v>
+      </c>
+      <c r="I106" s="1" t="n">
+        <v>44745</v>
+      </c>
+      <c r="J106" t="inlineStr">
+        <is>
+          <t>БНХ ПОЛЬСКА</t>
+        </is>
+      </c>
+    </row>
+    <row r="107">
+      <c r="E107" t="inlineStr">
+        <is>
+          <t>315/80R22.5</t>
+        </is>
+      </c>
+      <c r="F107" t="inlineStr">
+        <is>
+          <t>BEL-518</t>
+        </is>
+      </c>
+      <c r="G107" t="inlineStr">
+        <is>
+          <t>груз, сер</t>
+        </is>
+      </c>
+      <c r="H107" t="n">
+        <v>8</v>
+      </c>
+      <c r="I107" s="1" t="n">
+        <v>44745</v>
+      </c>
+      <c r="J107" t="inlineStr">
+        <is>
+          <t>БНХ ПОЛЬСКА</t>
+        </is>
+      </c>
+    </row>
+    <row r="108">
+      <c r="E108" t="inlineStr">
+        <is>
+          <t>12.00R20</t>
+        </is>
+      </c>
+      <c r="F108" t="inlineStr">
+        <is>
+          <t>ИД-304М</t>
+        </is>
+      </c>
+      <c r="G108" t="inlineStr">
+        <is>
+          <t>16, груз, сер</t>
+        </is>
+      </c>
+      <c r="H108" t="n">
+        <v>8</v>
+      </c>
+      <c r="I108" s="1" t="n">
+        <v>44745</v>
+      </c>
+      <c r="J108" t="inlineStr">
+        <is>
+          <t>БНХ ПОЛЬСКА</t>
+        </is>
+      </c>
+    </row>
+    <row r="109">
+      <c r="E109" t="inlineStr">
+        <is>
+          <t>12.00R20</t>
+        </is>
+      </c>
+      <c r="F109" t="inlineStr">
+        <is>
+          <t>ИД-304М</t>
+        </is>
+      </c>
+      <c r="G109" t="inlineStr">
+        <is>
+          <t>18, груз, сер</t>
+        </is>
+      </c>
+      <c r="H109" t="n">
+        <v>8</v>
+      </c>
+      <c r="I109" s="1" t="n">
+        <v>44745</v>
+      </c>
+      <c r="J109" t="inlineStr">
+        <is>
+          <t>БНХ ПОЛЬСКА</t>
+        </is>
+      </c>
+    </row>
+    <row r="110">
+      <c r="E110" t="inlineStr">
+        <is>
+          <t>12.00R20</t>
+        </is>
+      </c>
+      <c r="F110" t="inlineStr">
+        <is>
+          <t>ИД-304М</t>
+        </is>
+      </c>
+      <c r="G110" t="inlineStr">
+        <is>
+          <t>16, груз, трп</t>
+        </is>
+      </c>
+      <c r="H110" t="n">
+        <v>8</v>
+      </c>
+      <c r="I110" s="1" t="n">
+        <v>44745</v>
+      </c>
+      <c r="J110" t="inlineStr">
+        <is>
+          <t>БНХ ПОЛЬСКА</t>
+        </is>
+      </c>
+    </row>
+    <row r="111">
+      <c r="E111" t="inlineStr">
+        <is>
+          <t>12.00R20</t>
+        </is>
+      </c>
+      <c r="F111" t="inlineStr">
+        <is>
+          <t>ИД-304М</t>
+        </is>
+      </c>
+      <c r="G111" t="inlineStr">
+        <is>
+          <t>18, груз, трп</t>
+        </is>
+      </c>
+      <c r="H111" t="n">
+        <v>8</v>
+      </c>
+      <c r="I111" s="1" t="n">
+        <v>44745</v>
+      </c>
+      <c r="J111" t="inlineStr">
+        <is>
+          <t>БНХ ПОЛЬСКА</t>
+        </is>
+      </c>
+    </row>
+    <row r="112">
+      <c r="E112" t="inlineStr">
+        <is>
+          <t>12.00R20</t>
+        </is>
+      </c>
+      <c r="F112" t="inlineStr">
+        <is>
+          <t>БИ-368М</t>
+        </is>
+      </c>
+      <c r="G112" t="inlineStr">
+        <is>
+          <t>18, груз, сер</t>
+        </is>
+      </c>
+      <c r="H112" t="n">
+        <v>8</v>
+      </c>
+      <c r="I112" s="1" t="n">
+        <v>44745</v>
+      </c>
+      <c r="J112" t="inlineStr">
+        <is>
+          <t>БНХ ПОЛЬСКА</t>
+        </is>
+      </c>
+    </row>
+    <row r="113">
+      <c r="E113" t="inlineStr">
+        <is>
+          <t>12.00R20</t>
+        </is>
+      </c>
+      <c r="F113" t="inlineStr">
+        <is>
+          <t>БИ-368М</t>
+        </is>
+      </c>
+      <c r="G113" t="inlineStr">
+        <is>
+          <t>18, груз, сер</t>
+        </is>
+      </c>
+      <c r="H113" t="n">
+        <v>8</v>
+      </c>
+      <c r="I113" s="1" t="n">
+        <v>44745</v>
+      </c>
+      <c r="J113" t="inlineStr">
+        <is>
+          <t>БНХ ПОЛЬСКА</t>
+        </is>
+      </c>
+    </row>
+    <row r="114">
+      <c r="E114" t="inlineStr">
+        <is>
+          <t>12.00R20</t>
+        </is>
+      </c>
+      <c r="F114" t="inlineStr">
+        <is>
+          <t>БИ-368М</t>
+        </is>
+      </c>
+      <c r="G114" t="inlineStr">
+        <is>
+          <t>18, груз, трп</t>
+        </is>
+      </c>
+      <c r="H114" t="n">
+        <v>8</v>
+      </c>
+      <c r="I114" s="1" t="n">
+        <v>44745</v>
+      </c>
+      <c r="J114" t="inlineStr">
+        <is>
+          <t>БНХ ПОЛЬСКА</t>
+        </is>
+      </c>
+    </row>
+    <row r="115">
+      <c r="E115" t="inlineStr">
+        <is>
+          <t>195/65R15</t>
+        </is>
+      </c>
+      <c r="F115" t="inlineStr">
+        <is>
+          <t>BEL-337</t>
+        </is>
+      </c>
+      <c r="G115" t="inlineStr">
+        <is>
+          <t>б/к, легк, сер</t>
+        </is>
+      </c>
+      <c r="H115" t="n">
+        <v>8</v>
+      </c>
+      <c r="I115" s="1" t="n">
+        <v>44745</v>
+      </c>
+      <c r="J115" t="inlineStr">
+        <is>
+          <t>БНХ ПОЛЬСКА</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
SALES fixed + grops filter  at 09/09/2022
</commit_message>
<xml_diff>
--- a/src/Tyres.xlsx
+++ b/src/Tyres.xlsx
@@ -417,7 +417,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J115"/>
+  <dimension ref="A1:J134"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -3929,6 +3929,538 @@
         <v>44745</v>
       </c>
       <c r="J115" t="inlineStr">
+        <is>
+          <t>БНХ ПОЛЬСКА</t>
+        </is>
+      </c>
+    </row>
+    <row r="116">
+      <c r="E116" t="inlineStr">
+        <is>
+          <t>315/80R22.5</t>
+        </is>
+      </c>
+      <c r="F116" t="inlineStr">
+        <is>
+          <t>BEL-158M</t>
+        </is>
+      </c>
+      <c r="G116" t="inlineStr">
+        <is>
+          <t>камневыт, груз, сер</t>
+        </is>
+      </c>
+      <c r="H116" t="n">
+        <v>201</v>
+      </c>
+      <c r="I116" s="1" t="n">
+        <v>44701</v>
+      </c>
+      <c r="J116" t="inlineStr">
+        <is>
+          <t>БНХ ПОЛЬСКА</t>
+        </is>
+      </c>
+    </row>
+    <row r="117">
+      <c r="E117" t="inlineStr">
+        <is>
+          <t>315/80R22.5</t>
+        </is>
+      </c>
+      <c r="F117" t="inlineStr">
+        <is>
+          <t>BEL-158M</t>
+        </is>
+      </c>
+      <c r="G117" t="inlineStr">
+        <is>
+          <t>камневыт, груз, трп</t>
+        </is>
+      </c>
+      <c r="H117" t="n">
+        <v>201</v>
+      </c>
+      <c r="I117" s="1" t="n">
+        <v>44701</v>
+      </c>
+      <c r="J117" t="inlineStr">
+        <is>
+          <t>БНХ ПОЛЬСКА</t>
+        </is>
+      </c>
+    </row>
+    <row r="118">
+      <c r="E118" t="inlineStr">
+        <is>
+          <t>315/80R22.5</t>
+        </is>
+      </c>
+      <c r="F118" t="inlineStr">
+        <is>
+          <t>BEL-278</t>
+        </is>
+      </c>
+      <c r="G118" t="inlineStr">
+        <is>
+          <t>груз, сер</t>
+        </is>
+      </c>
+      <c r="H118" t="n">
+        <v>201</v>
+      </c>
+      <c r="I118" s="1" t="n">
+        <v>44701</v>
+      </c>
+      <c r="J118" t="inlineStr">
+        <is>
+          <t>БНХ ПОЛЬСКА</t>
+        </is>
+      </c>
+    </row>
+    <row r="119">
+      <c r="E119" t="inlineStr">
+        <is>
+          <t>315/80R22.5</t>
+        </is>
+      </c>
+      <c r="F119" t="inlineStr">
+        <is>
+          <t>BEL-278</t>
+        </is>
+      </c>
+      <c r="G119" t="inlineStr">
+        <is>
+          <t>груз, трп</t>
+        </is>
+      </c>
+      <c r="H119" t="n">
+        <v>201</v>
+      </c>
+      <c r="I119" s="1" t="n">
+        <v>44701</v>
+      </c>
+      <c r="J119" t="inlineStr">
+        <is>
+          <t>БНХ ПОЛЬСКА</t>
+        </is>
+      </c>
+    </row>
+    <row r="120">
+      <c r="E120" t="inlineStr">
+        <is>
+          <t>315/80R22.5</t>
+        </is>
+      </c>
+      <c r="F120" t="inlineStr">
+        <is>
+          <t>BEL-268</t>
+        </is>
+      </c>
+      <c r="G120" t="inlineStr">
+        <is>
+          <t>груз, сер</t>
+        </is>
+      </c>
+      <c r="H120" t="n">
+        <v>201</v>
+      </c>
+      <c r="I120" s="1" t="n">
+        <v>44701</v>
+      </c>
+      <c r="J120" t="inlineStr">
+        <is>
+          <t>БНХ ПОЛЬСКА</t>
+        </is>
+      </c>
+    </row>
+    <row r="121">
+      <c r="E121" t="inlineStr">
+        <is>
+          <t>315/80R22.5</t>
+        </is>
+      </c>
+      <c r="F121" t="inlineStr">
+        <is>
+          <t>BEL-268</t>
+        </is>
+      </c>
+      <c r="G121" t="inlineStr">
+        <is>
+          <t>груз, трп</t>
+        </is>
+      </c>
+      <c r="H121" t="n">
+        <v>201</v>
+      </c>
+      <c r="I121" s="1" t="n">
+        <v>44701</v>
+      </c>
+      <c r="J121" t="inlineStr">
+        <is>
+          <t>БНХ ПОЛЬСКА</t>
+        </is>
+      </c>
+    </row>
+    <row r="122">
+      <c r="E122" t="inlineStr">
+        <is>
+          <t>315/80R22.5</t>
+        </is>
+      </c>
+      <c r="F122" t="inlineStr">
+        <is>
+          <t>BEL-398</t>
+        </is>
+      </c>
+      <c r="G122" t="inlineStr">
+        <is>
+          <t>груз, сер</t>
+        </is>
+      </c>
+      <c r="H122" t="n">
+        <v>201</v>
+      </c>
+      <c r="I122" s="1" t="n">
+        <v>44701</v>
+      </c>
+      <c r="J122" t="inlineStr">
+        <is>
+          <t>БНХ ПОЛЬСКА</t>
+        </is>
+      </c>
+    </row>
+    <row r="123">
+      <c r="E123" t="inlineStr">
+        <is>
+          <t>315/80R22.5</t>
+        </is>
+      </c>
+      <c r="F123" t="inlineStr">
+        <is>
+          <t>BEL-326</t>
+        </is>
+      </c>
+      <c r="G123" t="inlineStr">
+        <is>
+          <t>груз, сер</t>
+        </is>
+      </c>
+      <c r="H123" t="n">
+        <v>201</v>
+      </c>
+      <c r="I123" s="1" t="n">
+        <v>44701</v>
+      </c>
+      <c r="J123" t="inlineStr">
+        <is>
+          <t>БНХ ПОЛЬСКА</t>
+        </is>
+      </c>
+    </row>
+    <row r="124">
+      <c r="E124" t="inlineStr">
+        <is>
+          <t>315/80R22.5</t>
+        </is>
+      </c>
+      <c r="F124" t="inlineStr">
+        <is>
+          <t>BEL-326</t>
+        </is>
+      </c>
+      <c r="G124" t="inlineStr">
+        <is>
+          <t>груз, трп</t>
+        </is>
+      </c>
+      <c r="H124" t="n">
+        <v>201</v>
+      </c>
+      <c r="I124" s="1" t="n">
+        <v>44701</v>
+      </c>
+      <c r="J124" t="inlineStr">
+        <is>
+          <t>БНХ ПОЛЬСКА</t>
+        </is>
+      </c>
+    </row>
+    <row r="125">
+      <c r="E125" t="inlineStr">
+        <is>
+          <t>315/80R22.5</t>
+        </is>
+      </c>
+      <c r="F125" t="inlineStr">
+        <is>
+          <t>BEL-498</t>
+        </is>
+      </c>
+      <c r="G125" t="inlineStr">
+        <is>
+          <t>156L, груз, сер</t>
+        </is>
+      </c>
+      <c r="H125" t="n">
+        <v>201</v>
+      </c>
+      <c r="I125" s="1" t="n">
+        <v>44701</v>
+      </c>
+      <c r="J125" t="inlineStr">
+        <is>
+          <t>БНХ ПОЛЬСКА</t>
+        </is>
+      </c>
+    </row>
+    <row r="126">
+      <c r="E126" t="inlineStr">
+        <is>
+          <t>315/80R22.5</t>
+        </is>
+      </c>
+      <c r="F126" t="inlineStr">
+        <is>
+          <t>BEL-518</t>
+        </is>
+      </c>
+      <c r="G126" t="inlineStr">
+        <is>
+          <t>груз, сер</t>
+        </is>
+      </c>
+      <c r="H126" t="n">
+        <v>201</v>
+      </c>
+      <c r="I126" s="1" t="n">
+        <v>44701</v>
+      </c>
+      <c r="J126" t="inlineStr">
+        <is>
+          <t>БНХ ПОЛЬСКА</t>
+        </is>
+      </c>
+    </row>
+    <row r="127">
+      <c r="E127" t="inlineStr">
+        <is>
+          <t>12.00R20</t>
+        </is>
+      </c>
+      <c r="F127" t="inlineStr">
+        <is>
+          <t>ИД-304М</t>
+        </is>
+      </c>
+      <c r="G127" t="inlineStr">
+        <is>
+          <t>16, груз, сер</t>
+        </is>
+      </c>
+      <c r="H127" t="n">
+        <v>201</v>
+      </c>
+      <c r="I127" s="1" t="n">
+        <v>44701</v>
+      </c>
+      <c r="J127" t="inlineStr">
+        <is>
+          <t>БНХ ПОЛЬСКА</t>
+        </is>
+      </c>
+    </row>
+    <row r="128">
+      <c r="E128" t="inlineStr">
+        <is>
+          <t>12.00R20</t>
+        </is>
+      </c>
+      <c r="F128" t="inlineStr">
+        <is>
+          <t>ИД-304М</t>
+        </is>
+      </c>
+      <c r="G128" t="inlineStr">
+        <is>
+          <t>18, груз, сер</t>
+        </is>
+      </c>
+      <c r="H128" t="n">
+        <v>201</v>
+      </c>
+      <c r="I128" s="1" t="n">
+        <v>44701</v>
+      </c>
+      <c r="J128" t="inlineStr">
+        <is>
+          <t>БНХ ПОЛЬСКА</t>
+        </is>
+      </c>
+    </row>
+    <row r="129">
+      <c r="E129" t="inlineStr">
+        <is>
+          <t>12.00R20</t>
+        </is>
+      </c>
+      <c r="F129" t="inlineStr">
+        <is>
+          <t>ИД-304М</t>
+        </is>
+      </c>
+      <c r="G129" t="inlineStr">
+        <is>
+          <t>16, груз, трп</t>
+        </is>
+      </c>
+      <c r="H129" t="n">
+        <v>201</v>
+      </c>
+      <c r="I129" s="1" t="n">
+        <v>44701</v>
+      </c>
+      <c r="J129" t="inlineStr">
+        <is>
+          <t>БНХ ПОЛЬСКА</t>
+        </is>
+      </c>
+    </row>
+    <row r="130">
+      <c r="E130" t="inlineStr">
+        <is>
+          <t>12.00R20</t>
+        </is>
+      </c>
+      <c r="F130" t="inlineStr">
+        <is>
+          <t>ИД-304М</t>
+        </is>
+      </c>
+      <c r="G130" t="inlineStr">
+        <is>
+          <t>18, груз, трп</t>
+        </is>
+      </c>
+      <c r="H130" t="n">
+        <v>201</v>
+      </c>
+      <c r="I130" s="1" t="n">
+        <v>44701</v>
+      </c>
+      <c r="J130" t="inlineStr">
+        <is>
+          <t>БНХ ПОЛЬСКА</t>
+        </is>
+      </c>
+    </row>
+    <row r="131">
+      <c r="E131" t="inlineStr">
+        <is>
+          <t>12.00R20</t>
+        </is>
+      </c>
+      <c r="F131" t="inlineStr">
+        <is>
+          <t>БИ-368М</t>
+        </is>
+      </c>
+      <c r="G131" t="inlineStr">
+        <is>
+          <t>18, груз, сер</t>
+        </is>
+      </c>
+      <c r="H131" t="n">
+        <v>201</v>
+      </c>
+      <c r="I131" s="1" t="n">
+        <v>44701</v>
+      </c>
+      <c r="J131" t="inlineStr">
+        <is>
+          <t>БНХ ПОЛЬСКА</t>
+        </is>
+      </c>
+    </row>
+    <row r="132">
+      <c r="E132" t="inlineStr">
+        <is>
+          <t>12.00R20</t>
+        </is>
+      </c>
+      <c r="F132" t="inlineStr">
+        <is>
+          <t>БИ-368М</t>
+        </is>
+      </c>
+      <c r="G132" t="inlineStr">
+        <is>
+          <t>18, груз, сер</t>
+        </is>
+      </c>
+      <c r="H132" t="n">
+        <v>201</v>
+      </c>
+      <c r="I132" s="1" t="n">
+        <v>44701</v>
+      </c>
+      <c r="J132" t="inlineStr">
+        <is>
+          <t>БНХ ПОЛЬСКА</t>
+        </is>
+      </c>
+    </row>
+    <row r="133">
+      <c r="E133" t="inlineStr">
+        <is>
+          <t>12.00R20</t>
+        </is>
+      </c>
+      <c r="F133" t="inlineStr">
+        <is>
+          <t>БИ-368М</t>
+        </is>
+      </c>
+      <c r="G133" t="inlineStr">
+        <is>
+          <t>18, груз, трп</t>
+        </is>
+      </c>
+      <c r="H133" t="n">
+        <v>201</v>
+      </c>
+      <c r="I133" s="1" t="n">
+        <v>44701</v>
+      </c>
+      <c r="J133" t="inlineStr">
+        <is>
+          <t>БНХ ПОЛЬСКА</t>
+        </is>
+      </c>
+    </row>
+    <row r="134">
+      <c r="E134" t="inlineStr">
+        <is>
+          <t>195/65R15</t>
+        </is>
+      </c>
+      <c r="F134" t="inlineStr">
+        <is>
+          <t>BEL-337</t>
+        </is>
+      </c>
+      <c r="G134" t="inlineStr">
+        <is>
+          <t>б/к, легк, сер</t>
+        </is>
+      </c>
+      <c r="H134" t="n">
+        <v>201</v>
+      </c>
+      <c r="I134" s="1" t="n">
+        <v>44701</v>
+      </c>
+      <c r="J134" t="inlineStr">
         <is>
           <t>БНХ ПОЛЬСКА</t>
         </is>

</xml_diff>

<commit_message>
ABC_XYZ fixed with time filter at 10/10/2022
</commit_message>
<xml_diff>
--- a/src/Tyres.xlsx
+++ b/src/Tyres.xlsx
@@ -417,7 +417,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J134"/>
+  <dimension ref="A1:J153"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -4461,6 +4461,538 @@
         <v>44701</v>
       </c>
       <c r="J134" t="inlineStr">
+        <is>
+          <t>БНХ ПОЛЬСКА</t>
+        </is>
+      </c>
+    </row>
+    <row r="135">
+      <c r="E135" t="inlineStr">
+        <is>
+          <t>315/80R22.5</t>
+        </is>
+      </c>
+      <c r="F135" t="inlineStr">
+        <is>
+          <t>BEL-158M</t>
+        </is>
+      </c>
+      <c r="G135" t="inlineStr">
+        <is>
+          <t>камневыт, груз, сер</t>
+        </is>
+      </c>
+      <c r="H135" t="n">
+        <v>113</v>
+      </c>
+      <c r="I135" s="1" t="n">
+        <v>44671</v>
+      </c>
+      <c r="J135" t="inlineStr">
+        <is>
+          <t>БНХ ПОЛЬСКА</t>
+        </is>
+      </c>
+    </row>
+    <row r="136">
+      <c r="E136" t="inlineStr">
+        <is>
+          <t>315/80R22.5</t>
+        </is>
+      </c>
+      <c r="F136" t="inlineStr">
+        <is>
+          <t>BEL-158M</t>
+        </is>
+      </c>
+      <c r="G136" t="inlineStr">
+        <is>
+          <t>камневыт, груз, трп</t>
+        </is>
+      </c>
+      <c r="H136" t="n">
+        <v>113</v>
+      </c>
+      <c r="I136" s="1" t="n">
+        <v>44671</v>
+      </c>
+      <c r="J136" t="inlineStr">
+        <is>
+          <t>БНХ ПОЛЬСКА</t>
+        </is>
+      </c>
+    </row>
+    <row r="137">
+      <c r="E137" t="inlineStr">
+        <is>
+          <t>315/80R22.5</t>
+        </is>
+      </c>
+      <c r="F137" t="inlineStr">
+        <is>
+          <t>BEL-278</t>
+        </is>
+      </c>
+      <c r="G137" t="inlineStr">
+        <is>
+          <t>груз, сер</t>
+        </is>
+      </c>
+      <c r="H137" t="n">
+        <v>113</v>
+      </c>
+      <c r="I137" s="1" t="n">
+        <v>44671</v>
+      </c>
+      <c r="J137" t="inlineStr">
+        <is>
+          <t>БНХ ПОЛЬСКА</t>
+        </is>
+      </c>
+    </row>
+    <row r="138">
+      <c r="E138" t="inlineStr">
+        <is>
+          <t>315/80R22.5</t>
+        </is>
+      </c>
+      <c r="F138" t="inlineStr">
+        <is>
+          <t>BEL-278</t>
+        </is>
+      </c>
+      <c r="G138" t="inlineStr">
+        <is>
+          <t>груз, трп</t>
+        </is>
+      </c>
+      <c r="H138" t="n">
+        <v>113</v>
+      </c>
+      <c r="I138" s="1" t="n">
+        <v>44671</v>
+      </c>
+      <c r="J138" t="inlineStr">
+        <is>
+          <t>БНХ ПОЛЬСКА</t>
+        </is>
+      </c>
+    </row>
+    <row r="139">
+      <c r="E139" t="inlineStr">
+        <is>
+          <t>315/80R22.5</t>
+        </is>
+      </c>
+      <c r="F139" t="inlineStr">
+        <is>
+          <t>BEL-268</t>
+        </is>
+      </c>
+      <c r="G139" t="inlineStr">
+        <is>
+          <t>груз, сер</t>
+        </is>
+      </c>
+      <c r="H139" t="n">
+        <v>113</v>
+      </c>
+      <c r="I139" s="1" t="n">
+        <v>44671</v>
+      </c>
+      <c r="J139" t="inlineStr">
+        <is>
+          <t>БНХ ПОЛЬСКА</t>
+        </is>
+      </c>
+    </row>
+    <row r="140">
+      <c r="E140" t="inlineStr">
+        <is>
+          <t>315/80R22.5</t>
+        </is>
+      </c>
+      <c r="F140" t="inlineStr">
+        <is>
+          <t>BEL-268</t>
+        </is>
+      </c>
+      <c r="G140" t="inlineStr">
+        <is>
+          <t>груз, трп</t>
+        </is>
+      </c>
+      <c r="H140" t="n">
+        <v>113</v>
+      </c>
+      <c r="I140" s="1" t="n">
+        <v>44671</v>
+      </c>
+      <c r="J140" t="inlineStr">
+        <is>
+          <t>БНХ ПОЛЬСКА</t>
+        </is>
+      </c>
+    </row>
+    <row r="141">
+      <c r="E141" t="inlineStr">
+        <is>
+          <t>315/80R22.5</t>
+        </is>
+      </c>
+      <c r="F141" t="inlineStr">
+        <is>
+          <t>BEL-398</t>
+        </is>
+      </c>
+      <c r="G141" t="inlineStr">
+        <is>
+          <t>груз, сер</t>
+        </is>
+      </c>
+      <c r="H141" t="n">
+        <v>113</v>
+      </c>
+      <c r="I141" s="1" t="n">
+        <v>44671</v>
+      </c>
+      <c r="J141" t="inlineStr">
+        <is>
+          <t>БНХ ПОЛЬСКА</t>
+        </is>
+      </c>
+    </row>
+    <row r="142">
+      <c r="E142" t="inlineStr">
+        <is>
+          <t>315/80R22.5</t>
+        </is>
+      </c>
+      <c r="F142" t="inlineStr">
+        <is>
+          <t>BEL-326</t>
+        </is>
+      </c>
+      <c r="G142" t="inlineStr">
+        <is>
+          <t>груз, сер</t>
+        </is>
+      </c>
+      <c r="H142" t="n">
+        <v>113</v>
+      </c>
+      <c r="I142" s="1" t="n">
+        <v>44671</v>
+      </c>
+      <c r="J142" t="inlineStr">
+        <is>
+          <t>БНХ ПОЛЬСКА</t>
+        </is>
+      </c>
+    </row>
+    <row r="143">
+      <c r="E143" t="inlineStr">
+        <is>
+          <t>315/80R22.5</t>
+        </is>
+      </c>
+      <c r="F143" t="inlineStr">
+        <is>
+          <t>BEL-326</t>
+        </is>
+      </c>
+      <c r="G143" t="inlineStr">
+        <is>
+          <t>груз, трп</t>
+        </is>
+      </c>
+      <c r="H143" t="n">
+        <v>113</v>
+      </c>
+      <c r="I143" s="1" t="n">
+        <v>44671</v>
+      </c>
+      <c r="J143" t="inlineStr">
+        <is>
+          <t>БНХ ПОЛЬСКА</t>
+        </is>
+      </c>
+    </row>
+    <row r="144">
+      <c r="E144" t="inlineStr">
+        <is>
+          <t>315/80R22.5</t>
+        </is>
+      </c>
+      <c r="F144" t="inlineStr">
+        <is>
+          <t>BEL-498</t>
+        </is>
+      </c>
+      <c r="G144" t="inlineStr">
+        <is>
+          <t>156L, груз, сер</t>
+        </is>
+      </c>
+      <c r="H144" t="n">
+        <v>113</v>
+      </c>
+      <c r="I144" s="1" t="n">
+        <v>44671</v>
+      </c>
+      <c r="J144" t="inlineStr">
+        <is>
+          <t>БНХ ПОЛЬСКА</t>
+        </is>
+      </c>
+    </row>
+    <row r="145">
+      <c r="E145" t="inlineStr">
+        <is>
+          <t>315/80R22.5</t>
+        </is>
+      </c>
+      <c r="F145" t="inlineStr">
+        <is>
+          <t>BEL-518</t>
+        </is>
+      </c>
+      <c r="G145" t="inlineStr">
+        <is>
+          <t>груз, сер</t>
+        </is>
+      </c>
+      <c r="H145" t="n">
+        <v>113</v>
+      </c>
+      <c r="I145" s="1" t="n">
+        <v>44671</v>
+      </c>
+      <c r="J145" t="inlineStr">
+        <is>
+          <t>БНХ ПОЛЬСКА</t>
+        </is>
+      </c>
+    </row>
+    <row r="146">
+      <c r="E146" t="inlineStr">
+        <is>
+          <t>12.00R20</t>
+        </is>
+      </c>
+      <c r="F146" t="inlineStr">
+        <is>
+          <t>ИД-304М</t>
+        </is>
+      </c>
+      <c r="G146" t="inlineStr">
+        <is>
+          <t>16, груз, сер</t>
+        </is>
+      </c>
+      <c r="H146" t="n">
+        <v>113</v>
+      </c>
+      <c r="I146" s="1" t="n">
+        <v>44671</v>
+      </c>
+      <c r="J146" t="inlineStr">
+        <is>
+          <t>БНХ ПОЛЬСКА</t>
+        </is>
+      </c>
+    </row>
+    <row r="147">
+      <c r="E147" t="inlineStr">
+        <is>
+          <t>12.00R20</t>
+        </is>
+      </c>
+      <c r="F147" t="inlineStr">
+        <is>
+          <t>ИД-304М</t>
+        </is>
+      </c>
+      <c r="G147" t="inlineStr">
+        <is>
+          <t>18, груз, сер</t>
+        </is>
+      </c>
+      <c r="H147" t="n">
+        <v>113</v>
+      </c>
+      <c r="I147" s="1" t="n">
+        <v>44671</v>
+      </c>
+      <c r="J147" t="inlineStr">
+        <is>
+          <t>БНХ ПОЛЬСКА</t>
+        </is>
+      </c>
+    </row>
+    <row r="148">
+      <c r="E148" t="inlineStr">
+        <is>
+          <t>12.00R20</t>
+        </is>
+      </c>
+      <c r="F148" t="inlineStr">
+        <is>
+          <t>ИД-304М</t>
+        </is>
+      </c>
+      <c r="G148" t="inlineStr">
+        <is>
+          <t>16, груз, трп</t>
+        </is>
+      </c>
+      <c r="H148" t="n">
+        <v>113</v>
+      </c>
+      <c r="I148" s="1" t="n">
+        <v>44671</v>
+      </c>
+      <c r="J148" t="inlineStr">
+        <is>
+          <t>БНХ ПОЛЬСКА</t>
+        </is>
+      </c>
+    </row>
+    <row r="149">
+      <c r="E149" t="inlineStr">
+        <is>
+          <t>12.00R20</t>
+        </is>
+      </c>
+      <c r="F149" t="inlineStr">
+        <is>
+          <t>ИД-304М</t>
+        </is>
+      </c>
+      <c r="G149" t="inlineStr">
+        <is>
+          <t>18, груз, трп</t>
+        </is>
+      </c>
+      <c r="H149" t="n">
+        <v>113</v>
+      </c>
+      <c r="I149" s="1" t="n">
+        <v>44671</v>
+      </c>
+      <c r="J149" t="inlineStr">
+        <is>
+          <t>БНХ ПОЛЬСКА</t>
+        </is>
+      </c>
+    </row>
+    <row r="150">
+      <c r="E150" t="inlineStr">
+        <is>
+          <t>12.00R20</t>
+        </is>
+      </c>
+      <c r="F150" t="inlineStr">
+        <is>
+          <t>БИ-368М</t>
+        </is>
+      </c>
+      <c r="G150" t="inlineStr">
+        <is>
+          <t>18, груз, сер</t>
+        </is>
+      </c>
+      <c r="H150" t="n">
+        <v>113</v>
+      </c>
+      <c r="I150" s="1" t="n">
+        <v>44671</v>
+      </c>
+      <c r="J150" t="inlineStr">
+        <is>
+          <t>БНХ ПОЛЬСКА</t>
+        </is>
+      </c>
+    </row>
+    <row r="151">
+      <c r="E151" t="inlineStr">
+        <is>
+          <t>12.00R20</t>
+        </is>
+      </c>
+      <c r="F151" t="inlineStr">
+        <is>
+          <t>БИ-368М</t>
+        </is>
+      </c>
+      <c r="G151" t="inlineStr">
+        <is>
+          <t>18, груз, сер</t>
+        </is>
+      </c>
+      <c r="H151" t="n">
+        <v>113</v>
+      </c>
+      <c r="I151" s="1" t="n">
+        <v>44671</v>
+      </c>
+      <c r="J151" t="inlineStr">
+        <is>
+          <t>БНХ ПОЛЬСКА</t>
+        </is>
+      </c>
+    </row>
+    <row r="152">
+      <c r="E152" t="inlineStr">
+        <is>
+          <t>12.00R20</t>
+        </is>
+      </c>
+      <c r="F152" t="inlineStr">
+        <is>
+          <t>БИ-368М</t>
+        </is>
+      </c>
+      <c r="G152" t="inlineStr">
+        <is>
+          <t>18, груз, трп</t>
+        </is>
+      </c>
+      <c r="H152" t="n">
+        <v>113</v>
+      </c>
+      <c r="I152" s="1" t="n">
+        <v>44671</v>
+      </c>
+      <c r="J152" t="inlineStr">
+        <is>
+          <t>БНХ ПОЛЬСКА</t>
+        </is>
+      </c>
+    </row>
+    <row r="153">
+      <c r="E153" t="inlineStr">
+        <is>
+          <t>195/65R15</t>
+        </is>
+      </c>
+      <c r="F153" t="inlineStr">
+        <is>
+          <t>BEL-337</t>
+        </is>
+      </c>
+      <c r="G153" t="inlineStr">
+        <is>
+          <t>б/к, легк, сер</t>
+        </is>
+      </c>
+      <c r="H153" t="n">
+        <v>113</v>
+      </c>
+      <c r="I153" s="1" t="n">
+        <v>44671</v>
+      </c>
+      <c r="J153" t="inlineStr">
         <is>
           <t>БНХ ПОЛЬСКА</t>
         </is>

</xml_diff>

<commit_message>
ABC_XYZ improved by value ercentage at 15/09/2022
</commit_message>
<xml_diff>
--- a/src/Tyres.xlsx
+++ b/src/Tyres.xlsx
@@ -417,7 +417,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J77"/>
+  <dimension ref="A1:J40"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -438,7 +438,7 @@
       </c>
       <c r="C1" t="inlineStr">
         <is>
-          <t>сер груз камневыт</t>
+          <t>камневыт груз сер</t>
         </is>
       </c>
       <c r="E1" t="inlineStr">
@@ -485,7 +485,7 @@
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>груз камневыт трп</t>
+          <t>камневыт груз трп</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
@@ -500,18 +500,18 @@
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>сер, груз, камневыт</t>
+          <t>камневыт, груз, сер</t>
         </is>
       </c>
       <c r="H2" t="n">
-        <v>16</v>
+        <v>259</v>
       </c>
       <c r="I2" s="1" t="n">
-        <v>44819</v>
+        <v>44826</v>
       </c>
       <c r="J2" t="inlineStr">
         <is>
-          <t>БНХ УКР</t>
+          <t>БНХ РОС</t>
         </is>
       </c>
     </row>
@@ -528,7 +528,7 @@
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>сер груз</t>
+          <t>груз сер</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
@@ -543,18 +543,18 @@
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>груз, камневыт, трп</t>
+          <t>камневыт, груз, трп</t>
         </is>
       </c>
       <c r="H3" t="n">
-        <v>16</v>
+        <v>265</v>
       </c>
       <c r="I3" s="1" t="n">
-        <v>44819</v>
+        <v>44826</v>
       </c>
       <c r="J3" t="inlineStr">
         <is>
-          <t>БНХ УКР</t>
+          <t>БНХ РОС</t>
         </is>
       </c>
     </row>
@@ -586,18 +586,18 @@
       </c>
       <c r="G4" t="inlineStr">
         <is>
-          <t>сер, груз</t>
+          <t>груз, сер</t>
         </is>
       </c>
       <c r="H4" t="n">
-        <v>16</v>
+        <v>281</v>
       </c>
       <c r="I4" s="1" t="n">
-        <v>44819</v>
+        <v>44826</v>
       </c>
       <c r="J4" t="inlineStr">
         <is>
-          <t>БНХ УКР</t>
+          <t>БНХ РОС</t>
         </is>
       </c>
     </row>
@@ -614,7 +614,7 @@
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>сер груз</t>
+          <t>груз сер</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
@@ -633,14 +633,14 @@
         </is>
       </c>
       <c r="H5" t="n">
-        <v>16</v>
+        <v>287</v>
       </c>
       <c r="I5" s="1" t="n">
-        <v>44819</v>
+        <v>44826</v>
       </c>
       <c r="J5" t="inlineStr">
         <is>
-          <t>БНХ УКР</t>
+          <t>БНХ РОС</t>
         </is>
       </c>
     </row>
@@ -672,18 +672,18 @@
       </c>
       <c r="G6" t="inlineStr">
         <is>
-          <t>сер, груз</t>
+          <t>груз, сер</t>
         </is>
       </c>
       <c r="H6" t="n">
-        <v>16</v>
+        <v>283</v>
       </c>
       <c r="I6" s="1" t="n">
-        <v>44819</v>
+        <v>44826</v>
       </c>
       <c r="J6" t="inlineStr">
         <is>
-          <t>БНХ УКР</t>
+          <t>БНХ РОС</t>
         </is>
       </c>
     </row>
@@ -700,7 +700,7 @@
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>сер груз</t>
+          <t>груз сер</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
@@ -719,14 +719,14 @@
         </is>
       </c>
       <c r="H7" t="n">
-        <v>16</v>
+        <v>287</v>
       </c>
       <c r="I7" s="1" t="n">
-        <v>44819</v>
+        <v>44826</v>
       </c>
       <c r="J7" t="inlineStr">
         <is>
-          <t>БНХ УКР</t>
+          <t>БНХ РОС</t>
         </is>
       </c>
     </row>
@@ -743,7 +743,7 @@
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>сер груз</t>
+          <t>груз сер</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
@@ -758,18 +758,18 @@
       </c>
       <c r="G8" t="inlineStr">
         <is>
-          <t>сер, груз</t>
+          <t>груз, сер</t>
         </is>
       </c>
       <c r="H8" t="n">
-        <v>16</v>
+        <v>265</v>
       </c>
       <c r="I8" s="1" t="n">
-        <v>44819</v>
+        <v>44826</v>
       </c>
       <c r="J8" t="inlineStr">
         <is>
-          <t>БНХ УКР</t>
+          <t>БНХ РОС</t>
         </is>
       </c>
     </row>
@@ -801,18 +801,18 @@
       </c>
       <c r="G9" t="inlineStr">
         <is>
-          <t>сер, груз</t>
+          <t>груз, сер</t>
         </is>
       </c>
       <c r="H9" t="n">
-        <v>16</v>
+        <v>269</v>
       </c>
       <c r="I9" s="1" t="n">
-        <v>44819</v>
+        <v>44826</v>
       </c>
       <c r="J9" t="inlineStr">
         <is>
-          <t>БНХ УКР</t>
+          <t>БНХ РОС</t>
         </is>
       </c>
     </row>
@@ -829,7 +829,7 @@
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>156L сер груз</t>
+          <t>156L груз сер</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
@@ -848,14 +848,14 @@
         </is>
       </c>
       <c r="H10" t="n">
-        <v>16</v>
+        <v>273</v>
       </c>
       <c r="I10" s="1" t="n">
-        <v>44819</v>
+        <v>44826</v>
       </c>
       <c r="J10" t="inlineStr">
         <is>
-          <t>БНХ УКР</t>
+          <t>БНХ РОС</t>
         </is>
       </c>
     </row>
@@ -872,7 +872,7 @@
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>сер груз</t>
+          <t>груз сер</t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
@@ -887,18 +887,18 @@
       </c>
       <c r="G11" t="inlineStr">
         <is>
-          <t>156L, сер, груз</t>
+          <t>156L, груз, сер</t>
         </is>
       </c>
       <c r="H11" t="n">
-        <v>16</v>
+        <v>247</v>
       </c>
       <c r="I11" s="1" t="n">
-        <v>44819</v>
+        <v>44826</v>
       </c>
       <c r="J11" t="inlineStr">
         <is>
-          <t>БНХ УКР</t>
+          <t>БНХ РОС</t>
         </is>
       </c>
     </row>
@@ -915,7 +915,7 @@
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>16 сер груз</t>
+          <t>16 груз сер</t>
         </is>
       </c>
       <c r="E12" t="inlineStr">
@@ -930,18 +930,18 @@
       </c>
       <c r="G12" t="inlineStr">
         <is>
-          <t>сер, груз</t>
+          <t>груз, сер</t>
         </is>
       </c>
       <c r="H12" t="n">
-        <v>16</v>
+        <v>255</v>
       </c>
       <c r="I12" s="1" t="n">
-        <v>44819</v>
+        <v>44826</v>
       </c>
       <c r="J12" t="inlineStr">
         <is>
-          <t>БНХ УКР</t>
+          <t>БНХ РОС</t>
         </is>
       </c>
     </row>
@@ -958,7 +958,7 @@
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>18 сер груз</t>
+          <t>18 груз сер</t>
         </is>
       </c>
       <c r="E13" t="inlineStr">
@@ -973,18 +973,18 @@
       </c>
       <c r="G13" t="inlineStr">
         <is>
-          <t>16, сер, груз</t>
+          <t>16, груз, сер</t>
         </is>
       </c>
       <c r="H13" t="n">
-        <v>16</v>
+        <v>279</v>
       </c>
       <c r="I13" s="1" t="n">
-        <v>44819</v>
+        <v>44826</v>
       </c>
       <c r="J13" t="inlineStr">
         <is>
-          <t>БНХ УКР</t>
+          <t>БНХ РОС</t>
         </is>
       </c>
     </row>
@@ -1016,18 +1016,18 @@
       </c>
       <c r="G14" t="inlineStr">
         <is>
-          <t>18, сер, груз</t>
+          <t>18, груз, сер</t>
         </is>
       </c>
       <c r="H14" t="n">
-        <v>16</v>
+        <v>285</v>
       </c>
       <c r="I14" s="1" t="n">
-        <v>44819</v>
+        <v>44826</v>
       </c>
       <c r="J14" t="inlineStr">
         <is>
-          <t>БНХ УКР</t>
+          <t>БНХ РОС</t>
         </is>
       </c>
     </row>
@@ -1063,14 +1063,14 @@
         </is>
       </c>
       <c r="H15" t="n">
-        <v>16</v>
+        <v>290</v>
       </c>
       <c r="I15" s="1" t="n">
-        <v>44819</v>
+        <v>44826</v>
       </c>
       <c r="J15" t="inlineStr">
         <is>
-          <t>БНХ УКР</t>
+          <t>БНХ РОС</t>
         </is>
       </c>
     </row>
@@ -1087,7 +1087,7 @@
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>18 сер груз</t>
+          <t>18 груз сер</t>
         </is>
       </c>
       <c r="E16" t="inlineStr">
@@ -1106,14 +1106,14 @@
         </is>
       </c>
       <c r="H16" t="n">
-        <v>16</v>
+        <v>296</v>
       </c>
       <c r="I16" s="1" t="n">
-        <v>44819</v>
+        <v>44826</v>
       </c>
       <c r="J16" t="inlineStr">
         <is>
-          <t>БНХ УКР</t>
+          <t>БНХ РОС</t>
         </is>
       </c>
     </row>
@@ -1130,7 +1130,7 @@
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>18 сер груз</t>
+          <t>18 груз сер</t>
         </is>
       </c>
       <c r="E17" t="inlineStr">
@@ -1145,18 +1145,18 @@
       </c>
       <c r="G17" t="inlineStr">
         <is>
-          <t>18, сер, груз</t>
+          <t>18, груз, сер</t>
         </is>
       </c>
       <c r="H17" t="n">
-        <v>16</v>
+        <v>283</v>
       </c>
       <c r="I17" s="1" t="n">
-        <v>44819</v>
+        <v>44826</v>
       </c>
       <c r="J17" t="inlineStr">
         <is>
-          <t>БНХ УКР</t>
+          <t>БНХ РОС</t>
         </is>
       </c>
     </row>
@@ -1188,18 +1188,18 @@
       </c>
       <c r="G18" t="inlineStr">
         <is>
-          <t>18, сер, груз</t>
+          <t>18, груз, сер</t>
         </is>
       </c>
       <c r="H18" t="n">
-        <v>16</v>
+        <v>283</v>
       </c>
       <c r="I18" s="1" t="n">
-        <v>44819</v>
+        <v>44826</v>
       </c>
       <c r="J18" t="inlineStr">
         <is>
-          <t>БНХ УКР</t>
+          <t>БНХ РОС</t>
         </is>
       </c>
     </row>
@@ -1216,7 +1216,7 @@
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>сер легк б/к</t>
+          <t>б/к сер легк</t>
         </is>
       </c>
       <c r="E19" t="inlineStr">
@@ -1235,14 +1235,14 @@
         </is>
       </c>
       <c r="H19" t="n">
-        <v>16</v>
+        <v>291</v>
       </c>
       <c r="I19" s="1" t="n">
-        <v>44819</v>
+        <v>44826</v>
       </c>
       <c r="J19" t="inlineStr">
         <is>
-          <t>БНХ УКР</t>
+          <t>БНХ РОС</t>
         </is>
       </c>
     </row>
@@ -1259,18 +1259,18 @@
       </c>
       <c r="G20" t="inlineStr">
         <is>
-          <t>сер, легк, б/к</t>
+          <t>б/к, сер, легк</t>
         </is>
       </c>
       <c r="H20" t="n">
-        <v>16</v>
+        <v>291</v>
       </c>
       <c r="I20" s="1" t="n">
-        <v>44819</v>
+        <v>44826</v>
       </c>
       <c r="J20" t="inlineStr">
         <is>
-          <t>БНХ УКР</t>
+          <t>БНХ РОС</t>
         </is>
       </c>
     </row>
@@ -1282,23 +1282,23 @@
       </c>
       <c r="F21" t="inlineStr">
         <is>
-          <t>BEL-158M</t>
+          <t>BEL-326</t>
         </is>
       </c>
       <c r="G21" t="inlineStr">
         <is>
-          <t>сер, груз, камневыт</t>
+          <t>груз, трп</t>
         </is>
       </c>
       <c r="H21" t="n">
-        <v>20</v>
+        <v>27</v>
       </c>
       <c r="I21" s="1" t="n">
-        <v>44819</v>
+        <v>44826</v>
       </c>
       <c r="J21" t="inlineStr">
         <is>
-          <t>БНХ ПОЛЬСКА</t>
+          <t>БНХ РОС</t>
         </is>
       </c>
     </row>
@@ -1315,18 +1315,18 @@
       </c>
       <c r="G22" t="inlineStr">
         <is>
-          <t>груз, камневыт, трп</t>
+          <t>камневыт, груз, сер</t>
         </is>
       </c>
       <c r="H22" t="n">
-        <v>20</v>
+        <v>259</v>
       </c>
       <c r="I22" s="1" t="n">
-        <v>44819</v>
+        <v>44849</v>
       </c>
       <c r="J22" t="inlineStr">
         <is>
-          <t>БНХ ПОЛЬСКА</t>
+          <t>БНХ РОС</t>
         </is>
       </c>
     </row>
@@ -1338,23 +1338,23 @@
       </c>
       <c r="F23" t="inlineStr">
         <is>
-          <t>BEL-278</t>
+          <t>BEL-158M</t>
         </is>
       </c>
       <c r="G23" t="inlineStr">
         <is>
-          <t>сер, груз</t>
+          <t>камневыт, груз, трп</t>
         </is>
       </c>
       <c r="H23" t="n">
-        <v>20</v>
+        <v>265</v>
       </c>
       <c r="I23" s="1" t="n">
-        <v>44819</v>
+        <v>44849</v>
       </c>
       <c r="J23" t="inlineStr">
         <is>
-          <t>БНХ ПОЛЬСКА</t>
+          <t>БНХ РОС</t>
         </is>
       </c>
     </row>
@@ -1371,18 +1371,18 @@
       </c>
       <c r="G24" t="inlineStr">
         <is>
-          <t>груз, трп</t>
+          <t>груз, сер</t>
         </is>
       </c>
       <c r="H24" t="n">
-        <v>20</v>
+        <v>281</v>
       </c>
       <c r="I24" s="1" t="n">
-        <v>44819</v>
+        <v>44849</v>
       </c>
       <c r="J24" t="inlineStr">
         <is>
-          <t>БНХ ПОЛЬСКА</t>
+          <t>БНХ РОС</t>
         </is>
       </c>
     </row>
@@ -1394,23 +1394,23 @@
       </c>
       <c r="F25" t="inlineStr">
         <is>
-          <t>BEL-268</t>
+          <t>BEL-278</t>
         </is>
       </c>
       <c r="G25" t="inlineStr">
         <is>
-          <t>сер, груз</t>
+          <t>груз, трп</t>
         </is>
       </c>
       <c r="H25" t="n">
-        <v>20</v>
+        <v>287</v>
       </c>
       <c r="I25" s="1" t="n">
-        <v>44819</v>
+        <v>44849</v>
       </c>
       <c r="J25" t="inlineStr">
         <is>
-          <t>БНХ ПОЛЬСКА</t>
+          <t>БНХ РОС</t>
         </is>
       </c>
     </row>
@@ -1427,18 +1427,18 @@
       </c>
       <c r="G26" t="inlineStr">
         <is>
-          <t>груз, трп</t>
+          <t>груз, сер</t>
         </is>
       </c>
       <c r="H26" t="n">
-        <v>20</v>
+        <v>283</v>
       </c>
       <c r="I26" s="1" t="n">
-        <v>44819</v>
+        <v>44849</v>
       </c>
       <c r="J26" t="inlineStr">
         <is>
-          <t>БНХ ПОЛЬСКА</t>
+          <t>БНХ РОС</t>
         </is>
       </c>
     </row>
@@ -1450,23 +1450,23 @@
       </c>
       <c r="F27" t="inlineStr">
         <is>
-          <t>BEL-398</t>
+          <t>BEL-268</t>
         </is>
       </c>
       <c r="G27" t="inlineStr">
         <is>
-          <t>сер, груз</t>
+          <t>груз, трп</t>
         </is>
       </c>
       <c r="H27" t="n">
-        <v>20</v>
+        <v>287</v>
       </c>
       <c r="I27" s="1" t="n">
-        <v>44819</v>
+        <v>44849</v>
       </c>
       <c r="J27" t="inlineStr">
         <is>
-          <t>БНХ ПОЛЬСКА</t>
+          <t>БНХ РОС</t>
         </is>
       </c>
     </row>
@@ -1478,23 +1478,23 @@
       </c>
       <c r="F28" t="inlineStr">
         <is>
-          <t>BEL-326</t>
+          <t>BEL-398</t>
         </is>
       </c>
       <c r="G28" t="inlineStr">
         <is>
-          <t>сер, груз</t>
+          <t>груз, сер</t>
         </is>
       </c>
       <c r="H28" t="n">
-        <v>20</v>
+        <v>265</v>
       </c>
       <c r="I28" s="1" t="n">
-        <v>44819</v>
+        <v>44849</v>
       </c>
       <c r="J28" t="inlineStr">
         <is>
-          <t>БНХ ПОЛЬСКА</t>
+          <t>БНХ РОС</t>
         </is>
       </c>
     </row>
@@ -1511,18 +1511,18 @@
       </c>
       <c r="G29" t="inlineStr">
         <is>
-          <t>груз, трп</t>
+          <t>груз, сер</t>
         </is>
       </c>
       <c r="H29" t="n">
-        <v>20</v>
+        <v>269</v>
       </c>
       <c r="I29" s="1" t="n">
-        <v>44819</v>
+        <v>44849</v>
       </c>
       <c r="J29" t="inlineStr">
         <is>
-          <t>БНХ ПОЛЬСКА</t>
+          <t>БНХ РОС</t>
         </is>
       </c>
     </row>
@@ -1534,23 +1534,23 @@
       </c>
       <c r="F30" t="inlineStr">
         <is>
-          <t>BEL-498</t>
+          <t>BEL-326</t>
         </is>
       </c>
       <c r="G30" t="inlineStr">
         <is>
-          <t>156L, сер, груз</t>
+          <t>груз, трп</t>
         </is>
       </c>
       <c r="H30" t="n">
-        <v>20</v>
+        <v>27</v>
       </c>
       <c r="I30" s="1" t="n">
-        <v>44819</v>
+        <v>44849</v>
       </c>
       <c r="J30" t="inlineStr">
         <is>
-          <t>БНХ ПОЛЬСКА</t>
+          <t>БНХ РОС</t>
         </is>
       </c>
     </row>
@@ -1562,51 +1562,51 @@
       </c>
       <c r="F31" t="inlineStr">
         <is>
-          <t>BEL-518</t>
+          <t>BEL-498</t>
         </is>
       </c>
       <c r="G31" t="inlineStr">
         <is>
-          <t>сер, груз</t>
+          <t>156L, груз, сер</t>
         </is>
       </c>
       <c r="H31" t="n">
-        <v>20</v>
+        <v>247</v>
       </c>
       <c r="I31" s="1" t="n">
-        <v>44819</v>
+        <v>44849</v>
       </c>
       <c r="J31" t="inlineStr">
         <is>
-          <t>БНХ ПОЛЬСКА</t>
+          <t>БНХ РОС</t>
         </is>
       </c>
     </row>
     <row r="32">
       <c r="E32" t="inlineStr">
         <is>
-          <t>12.00R20</t>
+          <t>315/80R22.5</t>
         </is>
       </c>
       <c r="F32" t="inlineStr">
         <is>
-          <t>ИД-304М</t>
+          <t>BEL-518</t>
         </is>
       </c>
       <c r="G32" t="inlineStr">
         <is>
-          <t>16, сер, груз</t>
+          <t>груз, сер</t>
         </is>
       </c>
       <c r="H32" t="n">
-        <v>20</v>
+        <v>255</v>
       </c>
       <c r="I32" s="1" t="n">
-        <v>44819</v>
+        <v>44849</v>
       </c>
       <c r="J32" t="inlineStr">
         <is>
-          <t>БНХ ПОЛЬСКА</t>
+          <t>БНХ РОС</t>
         </is>
       </c>
     </row>
@@ -1623,18 +1623,18 @@
       </c>
       <c r="G33" t="inlineStr">
         <is>
-          <t>18, сер, груз</t>
+          <t>16, груз, сер</t>
         </is>
       </c>
       <c r="H33" t="n">
-        <v>20</v>
+        <v>279</v>
       </c>
       <c r="I33" s="1" t="n">
-        <v>44819</v>
+        <v>44849</v>
       </c>
       <c r="J33" t="inlineStr">
         <is>
-          <t>БНХ ПОЛЬСКА</t>
+          <t>БНХ РОС</t>
         </is>
       </c>
     </row>
@@ -1651,18 +1651,18 @@
       </c>
       <c r="G34" t="inlineStr">
         <is>
-          <t>16, груз, трп</t>
+          <t>18, груз, сер</t>
         </is>
       </c>
       <c r="H34" t="n">
-        <v>20</v>
+        <v>285</v>
       </c>
       <c r="I34" s="1" t="n">
-        <v>44819</v>
+        <v>44849</v>
       </c>
       <c r="J34" t="inlineStr">
         <is>
-          <t>БНХ ПОЛЬСКА</t>
+          <t>БНХ РОС</t>
         </is>
       </c>
     </row>
@@ -1679,18 +1679,18 @@
       </c>
       <c r="G35" t="inlineStr">
         <is>
-          <t>18, груз, трп</t>
+          <t>16, груз, трп</t>
         </is>
       </c>
       <c r="H35" t="n">
-        <v>20</v>
+        <v>290</v>
       </c>
       <c r="I35" s="1" t="n">
-        <v>44819</v>
+        <v>44849</v>
       </c>
       <c r="J35" t="inlineStr">
         <is>
-          <t>БНХ ПОЛЬСКА</t>
+          <t>БНХ РОС</t>
         </is>
       </c>
     </row>
@@ -1702,23 +1702,23 @@
       </c>
       <c r="F36" t="inlineStr">
         <is>
-          <t>БИ-368М</t>
+          <t>ИД-304М</t>
         </is>
       </c>
       <c r="G36" t="inlineStr">
         <is>
-          <t>18, сер, груз</t>
+          <t>18, груз, трп</t>
         </is>
       </c>
       <c r="H36" t="n">
-        <v>20</v>
+        <v>296</v>
       </c>
       <c r="I36" s="1" t="n">
-        <v>44819</v>
+        <v>44849</v>
       </c>
       <c r="J36" t="inlineStr">
         <is>
-          <t>БНХ ПОЛЬСКА</t>
+          <t>БНХ РОС</t>
         </is>
       </c>
     </row>
@@ -1735,18 +1735,18 @@
       </c>
       <c r="G37" t="inlineStr">
         <is>
-          <t>18, сер, груз</t>
+          <t>18, груз, сер</t>
         </is>
       </c>
       <c r="H37" t="n">
-        <v>20</v>
+        <v>283</v>
       </c>
       <c r="I37" s="1" t="n">
-        <v>44819</v>
+        <v>44849</v>
       </c>
       <c r="J37" t="inlineStr">
         <is>
-          <t>БНХ ПОЛЬСКА</t>
+          <t>БНХ РОС</t>
         </is>
       </c>
     </row>
@@ -1763,1108 +1763,72 @@
       </c>
       <c r="G38" t="inlineStr">
         <is>
-          <t>18, груз, трп</t>
+          <t>18, груз, сер</t>
         </is>
       </c>
       <c r="H38" t="n">
-        <v>20</v>
+        <v>283</v>
       </c>
       <c r="I38" s="1" t="n">
-        <v>44819</v>
+        <v>44849</v>
       </c>
       <c r="J38" t="inlineStr">
         <is>
-          <t>БНХ ПОЛЬСКА</t>
+          <t>БНХ РОС</t>
         </is>
       </c>
     </row>
     <row r="39">
       <c r="E39" t="inlineStr">
         <is>
-          <t>195/65R15</t>
+          <t>12.00R20</t>
         </is>
       </c>
       <c r="F39" t="inlineStr">
         <is>
-          <t>BEL-337</t>
+          <t>БИ-368М</t>
         </is>
       </c>
       <c r="G39" t="inlineStr">
         <is>
-          <t>сер, легк, б/к</t>
+          <t>18, груз, трп</t>
         </is>
       </c>
       <c r="H39" t="n">
-        <v>20</v>
+        <v>291</v>
       </c>
       <c r="I39" s="1" t="n">
-        <v>44819</v>
+        <v>44849</v>
       </c>
       <c r="J39" t="inlineStr">
         <is>
-          <t>БНХ ПОЛЬСКА</t>
+          <t>БНХ РОС</t>
         </is>
       </c>
     </row>
     <row r="40">
       <c r="E40" t="inlineStr">
         <is>
-          <t>315/80R22.5</t>
+          <t>195/65R15</t>
         </is>
       </c>
       <c r="F40" t="inlineStr">
         <is>
-          <t>BEL-158M</t>
+          <t>BEL-337</t>
         </is>
       </c>
       <c r="G40" t="inlineStr">
         <is>
-          <t>сер, груз, камневыт</t>
+          <t>б/к, сер, легк</t>
         </is>
       </c>
       <c r="H40" t="n">
-        <v>9</v>
+        <v>291</v>
       </c>
       <c r="I40" s="1" t="n">
-        <v>44822</v>
+        <v>44849</v>
       </c>
       <c r="J40" t="inlineStr">
-        <is>
-          <t>БНХ ПОЛЬСКА</t>
-        </is>
-      </c>
-    </row>
-    <row r="41">
-      <c r="E41" t="inlineStr">
-        <is>
-          <t>315/80R22.5</t>
-        </is>
-      </c>
-      <c r="F41" t="inlineStr">
-        <is>
-          <t>BEL-158M</t>
-        </is>
-      </c>
-      <c r="G41" t="inlineStr">
-        <is>
-          <t>груз, камневыт, трп</t>
-        </is>
-      </c>
-      <c r="H41" t="n">
-        <v>9</v>
-      </c>
-      <c r="I41" s="1" t="n">
-        <v>44822</v>
-      </c>
-      <c r="J41" t="inlineStr">
-        <is>
-          <t>БНХ ПОЛЬСКА</t>
-        </is>
-      </c>
-    </row>
-    <row r="42">
-      <c r="E42" t="inlineStr">
-        <is>
-          <t>315/80R22.5</t>
-        </is>
-      </c>
-      <c r="F42" t="inlineStr">
-        <is>
-          <t>BEL-278</t>
-        </is>
-      </c>
-      <c r="G42" t="inlineStr">
-        <is>
-          <t>сер, груз</t>
-        </is>
-      </c>
-      <c r="H42" t="n">
-        <v>9</v>
-      </c>
-      <c r="I42" s="1" t="n">
-        <v>44822</v>
-      </c>
-      <c r="J42" t="inlineStr">
-        <is>
-          <t>БНХ ПОЛЬСКА</t>
-        </is>
-      </c>
-    </row>
-    <row r="43">
-      <c r="E43" t="inlineStr">
-        <is>
-          <t>315/80R22.5</t>
-        </is>
-      </c>
-      <c r="F43" t="inlineStr">
-        <is>
-          <t>BEL-278</t>
-        </is>
-      </c>
-      <c r="G43" t="inlineStr">
-        <is>
-          <t>груз, трп</t>
-        </is>
-      </c>
-      <c r="H43" t="n">
-        <v>9</v>
-      </c>
-      <c r="I43" s="1" t="n">
-        <v>44822</v>
-      </c>
-      <c r="J43" t="inlineStr">
-        <is>
-          <t>БНХ ПОЛЬСКА</t>
-        </is>
-      </c>
-    </row>
-    <row r="44">
-      <c r="E44" t="inlineStr">
-        <is>
-          <t>315/80R22.5</t>
-        </is>
-      </c>
-      <c r="F44" t="inlineStr">
-        <is>
-          <t>BEL-268</t>
-        </is>
-      </c>
-      <c r="G44" t="inlineStr">
-        <is>
-          <t>сер, груз</t>
-        </is>
-      </c>
-      <c r="H44" t="n">
-        <v>9</v>
-      </c>
-      <c r="I44" s="1" t="n">
-        <v>44822</v>
-      </c>
-      <c r="J44" t="inlineStr">
-        <is>
-          <t>БНХ ПОЛЬСКА</t>
-        </is>
-      </c>
-    </row>
-    <row r="45">
-      <c r="E45" t="inlineStr">
-        <is>
-          <t>315/80R22.5</t>
-        </is>
-      </c>
-      <c r="F45" t="inlineStr">
-        <is>
-          <t>BEL-268</t>
-        </is>
-      </c>
-      <c r="G45" t="inlineStr">
-        <is>
-          <t>груз, трп</t>
-        </is>
-      </c>
-      <c r="H45" t="n">
-        <v>9</v>
-      </c>
-      <c r="I45" s="1" t="n">
-        <v>44822</v>
-      </c>
-      <c r="J45" t="inlineStr">
-        <is>
-          <t>БНХ ПОЛЬСКА</t>
-        </is>
-      </c>
-    </row>
-    <row r="46">
-      <c r="E46" t="inlineStr">
-        <is>
-          <t>315/80R22.5</t>
-        </is>
-      </c>
-      <c r="F46" t="inlineStr">
-        <is>
-          <t>BEL-398</t>
-        </is>
-      </c>
-      <c r="G46" t="inlineStr">
-        <is>
-          <t>сер, груз</t>
-        </is>
-      </c>
-      <c r="H46" t="n">
-        <v>9</v>
-      </c>
-      <c r="I46" s="1" t="n">
-        <v>44822</v>
-      </c>
-      <c r="J46" t="inlineStr">
-        <is>
-          <t>БНХ ПОЛЬСКА</t>
-        </is>
-      </c>
-    </row>
-    <row r="47">
-      <c r="E47" t="inlineStr">
-        <is>
-          <t>315/80R22.5</t>
-        </is>
-      </c>
-      <c r="F47" t="inlineStr">
-        <is>
-          <t>BEL-326</t>
-        </is>
-      </c>
-      <c r="G47" t="inlineStr">
-        <is>
-          <t>сер, груз</t>
-        </is>
-      </c>
-      <c r="H47" t="n">
-        <v>9</v>
-      </c>
-      <c r="I47" s="1" t="n">
-        <v>44822</v>
-      </c>
-      <c r="J47" t="inlineStr">
-        <is>
-          <t>БНХ ПОЛЬСКА</t>
-        </is>
-      </c>
-    </row>
-    <row r="48">
-      <c r="E48" t="inlineStr">
-        <is>
-          <t>315/80R22.5</t>
-        </is>
-      </c>
-      <c r="F48" t="inlineStr">
-        <is>
-          <t>BEL-326</t>
-        </is>
-      </c>
-      <c r="G48" t="inlineStr">
-        <is>
-          <t>груз, трп</t>
-        </is>
-      </c>
-      <c r="H48" t="n">
-        <v>9</v>
-      </c>
-      <c r="I48" s="1" t="n">
-        <v>44822</v>
-      </c>
-      <c r="J48" t="inlineStr">
-        <is>
-          <t>БНХ ПОЛЬСКА</t>
-        </is>
-      </c>
-    </row>
-    <row r="49">
-      <c r="E49" t="inlineStr">
-        <is>
-          <t>315/80R22.5</t>
-        </is>
-      </c>
-      <c r="F49" t="inlineStr">
-        <is>
-          <t>BEL-498</t>
-        </is>
-      </c>
-      <c r="G49" t="inlineStr">
-        <is>
-          <t>156L, сер, груз</t>
-        </is>
-      </c>
-      <c r="H49" t="n">
-        <v>9</v>
-      </c>
-      <c r="I49" s="1" t="n">
-        <v>44822</v>
-      </c>
-      <c r="J49" t="inlineStr">
-        <is>
-          <t>БНХ ПОЛЬСКА</t>
-        </is>
-      </c>
-    </row>
-    <row r="50">
-      <c r="E50" t="inlineStr">
-        <is>
-          <t>315/80R22.5</t>
-        </is>
-      </c>
-      <c r="F50" t="inlineStr">
-        <is>
-          <t>BEL-518</t>
-        </is>
-      </c>
-      <c r="G50" t="inlineStr">
-        <is>
-          <t>сер, груз</t>
-        </is>
-      </c>
-      <c r="H50" t="n">
-        <v>9</v>
-      </c>
-      <c r="I50" s="1" t="n">
-        <v>44822</v>
-      </c>
-      <c r="J50" t="inlineStr">
-        <is>
-          <t>БНХ ПОЛЬСКА</t>
-        </is>
-      </c>
-    </row>
-    <row r="51">
-      <c r="E51" t="inlineStr">
-        <is>
-          <t>12.00R20</t>
-        </is>
-      </c>
-      <c r="F51" t="inlineStr">
-        <is>
-          <t>ИД-304М</t>
-        </is>
-      </c>
-      <c r="G51" t="inlineStr">
-        <is>
-          <t>16, сер, груз</t>
-        </is>
-      </c>
-      <c r="H51" t="n">
-        <v>9</v>
-      </c>
-      <c r="I51" s="1" t="n">
-        <v>44822</v>
-      </c>
-      <c r="J51" t="inlineStr">
-        <is>
-          <t>БНХ ПОЛЬСКА</t>
-        </is>
-      </c>
-    </row>
-    <row r="52">
-      <c r="E52" t="inlineStr">
-        <is>
-          <t>12.00R20</t>
-        </is>
-      </c>
-      <c r="F52" t="inlineStr">
-        <is>
-          <t>ИД-304М</t>
-        </is>
-      </c>
-      <c r="G52" t="inlineStr">
-        <is>
-          <t>18, сер, груз</t>
-        </is>
-      </c>
-      <c r="H52" t="n">
-        <v>9</v>
-      </c>
-      <c r="I52" s="1" t="n">
-        <v>44822</v>
-      </c>
-      <c r="J52" t="inlineStr">
-        <is>
-          <t>БНХ ПОЛЬСКА</t>
-        </is>
-      </c>
-    </row>
-    <row r="53">
-      <c r="E53" t="inlineStr">
-        <is>
-          <t>12.00R20</t>
-        </is>
-      </c>
-      <c r="F53" t="inlineStr">
-        <is>
-          <t>ИД-304М</t>
-        </is>
-      </c>
-      <c r="G53" t="inlineStr">
-        <is>
-          <t>16, груз, трп</t>
-        </is>
-      </c>
-      <c r="H53" t="n">
-        <v>9</v>
-      </c>
-      <c r="I53" s="1" t="n">
-        <v>44822</v>
-      </c>
-      <c r="J53" t="inlineStr">
-        <is>
-          <t>БНХ ПОЛЬСКА</t>
-        </is>
-      </c>
-    </row>
-    <row r="54">
-      <c r="E54" t="inlineStr">
-        <is>
-          <t>12.00R20</t>
-        </is>
-      </c>
-      <c r="F54" t="inlineStr">
-        <is>
-          <t>ИД-304М</t>
-        </is>
-      </c>
-      <c r="G54" t="inlineStr">
-        <is>
-          <t>18, груз, трп</t>
-        </is>
-      </c>
-      <c r="H54" t="n">
-        <v>9</v>
-      </c>
-      <c r="I54" s="1" t="n">
-        <v>44822</v>
-      </c>
-      <c r="J54" t="inlineStr">
-        <is>
-          <t>БНХ ПОЛЬСКА</t>
-        </is>
-      </c>
-    </row>
-    <row r="55">
-      <c r="E55" t="inlineStr">
-        <is>
-          <t>12.00R20</t>
-        </is>
-      </c>
-      <c r="F55" t="inlineStr">
-        <is>
-          <t>БИ-368М</t>
-        </is>
-      </c>
-      <c r="G55" t="inlineStr">
-        <is>
-          <t>18, сер, груз</t>
-        </is>
-      </c>
-      <c r="H55" t="n">
-        <v>9</v>
-      </c>
-      <c r="I55" s="1" t="n">
-        <v>44822</v>
-      </c>
-      <c r="J55" t="inlineStr">
-        <is>
-          <t>БНХ ПОЛЬСКА</t>
-        </is>
-      </c>
-    </row>
-    <row r="56">
-      <c r="E56" t="inlineStr">
-        <is>
-          <t>12.00R20</t>
-        </is>
-      </c>
-      <c r="F56" t="inlineStr">
-        <is>
-          <t>БИ-368М</t>
-        </is>
-      </c>
-      <c r="G56" t="inlineStr">
-        <is>
-          <t>18, сер, груз</t>
-        </is>
-      </c>
-      <c r="H56" t="n">
-        <v>9</v>
-      </c>
-      <c r="I56" s="1" t="n">
-        <v>44822</v>
-      </c>
-      <c r="J56" t="inlineStr">
-        <is>
-          <t>БНХ ПОЛЬСКА</t>
-        </is>
-      </c>
-    </row>
-    <row r="57">
-      <c r="E57" t="inlineStr">
-        <is>
-          <t>12.00R20</t>
-        </is>
-      </c>
-      <c r="F57" t="inlineStr">
-        <is>
-          <t>БИ-368М</t>
-        </is>
-      </c>
-      <c r="G57" t="inlineStr">
-        <is>
-          <t>18, груз, трп</t>
-        </is>
-      </c>
-      <c r="H57" t="n">
-        <v>9</v>
-      </c>
-      <c r="I57" s="1" t="n">
-        <v>44822</v>
-      </c>
-      <c r="J57" t="inlineStr">
-        <is>
-          <t>БНХ ПОЛЬСКА</t>
-        </is>
-      </c>
-    </row>
-    <row r="58">
-      <c r="E58" t="inlineStr">
-        <is>
-          <t>195/65R15</t>
-        </is>
-      </c>
-      <c r="F58" t="inlineStr">
-        <is>
-          <t>BEL-337</t>
-        </is>
-      </c>
-      <c r="G58" t="inlineStr">
-        <is>
-          <t>сер, легк, б/к</t>
-        </is>
-      </c>
-      <c r="H58" t="n">
-        <v>9</v>
-      </c>
-      <c r="I58" s="1" t="n">
-        <v>44822</v>
-      </c>
-      <c r="J58" t="inlineStr">
-        <is>
-          <t>БНХ ПОЛЬСКА</t>
-        </is>
-      </c>
-    </row>
-    <row r="59">
-      <c r="E59" t="inlineStr">
-        <is>
-          <t>315/80R22.5</t>
-        </is>
-      </c>
-      <c r="F59" t="inlineStr">
-        <is>
-          <t>BEL-158M</t>
-        </is>
-      </c>
-      <c r="G59" t="inlineStr">
-        <is>
-          <t>сер, груз, камневыт</t>
-        </is>
-      </c>
-      <c r="H59" t="n">
-        <v>78</v>
-      </c>
-      <c r="I59" s="1" t="n">
-        <v>44826</v>
-      </c>
-      <c r="J59" t="inlineStr">
-        <is>
-          <t>БНХ РОС</t>
-        </is>
-      </c>
-    </row>
-    <row r="60">
-      <c r="E60" t="inlineStr">
-        <is>
-          <t>315/80R22.5</t>
-        </is>
-      </c>
-      <c r="F60" t="inlineStr">
-        <is>
-          <t>BEL-158M</t>
-        </is>
-      </c>
-      <c r="G60" t="inlineStr">
-        <is>
-          <t>груз, камневыт, трп</t>
-        </is>
-      </c>
-      <c r="H60" t="n">
-        <v>78</v>
-      </c>
-      <c r="I60" s="1" t="n">
-        <v>44826</v>
-      </c>
-      <c r="J60" t="inlineStr">
-        <is>
-          <t>БНХ РОС</t>
-        </is>
-      </c>
-    </row>
-    <row r="61">
-      <c r="E61" t="inlineStr">
-        <is>
-          <t>315/80R22.5</t>
-        </is>
-      </c>
-      <c r="F61" t="inlineStr">
-        <is>
-          <t>BEL-278</t>
-        </is>
-      </c>
-      <c r="G61" t="inlineStr">
-        <is>
-          <t>сер, груз</t>
-        </is>
-      </c>
-      <c r="H61" t="n">
-        <v>78</v>
-      </c>
-      <c r="I61" s="1" t="n">
-        <v>44826</v>
-      </c>
-      <c r="J61" t="inlineStr">
-        <is>
-          <t>БНХ РОС</t>
-        </is>
-      </c>
-    </row>
-    <row r="62">
-      <c r="E62" t="inlineStr">
-        <is>
-          <t>315/80R22.5</t>
-        </is>
-      </c>
-      <c r="F62" t="inlineStr">
-        <is>
-          <t>BEL-278</t>
-        </is>
-      </c>
-      <c r="G62" t="inlineStr">
-        <is>
-          <t>груз, трп</t>
-        </is>
-      </c>
-      <c r="H62" t="n">
-        <v>78</v>
-      </c>
-      <c r="I62" s="1" t="n">
-        <v>44826</v>
-      </c>
-      <c r="J62" t="inlineStr">
-        <is>
-          <t>БНХ РОС</t>
-        </is>
-      </c>
-    </row>
-    <row r="63">
-      <c r="E63" t="inlineStr">
-        <is>
-          <t>315/80R22.5</t>
-        </is>
-      </c>
-      <c r="F63" t="inlineStr">
-        <is>
-          <t>BEL-268</t>
-        </is>
-      </c>
-      <c r="G63" t="inlineStr">
-        <is>
-          <t>сер, груз</t>
-        </is>
-      </c>
-      <c r="H63" t="n">
-        <v>78</v>
-      </c>
-      <c r="I63" s="1" t="n">
-        <v>44826</v>
-      </c>
-      <c r="J63" t="inlineStr">
-        <is>
-          <t>БНХ РОС</t>
-        </is>
-      </c>
-    </row>
-    <row r="64">
-      <c r="E64" t="inlineStr">
-        <is>
-          <t>315/80R22.5</t>
-        </is>
-      </c>
-      <c r="F64" t="inlineStr">
-        <is>
-          <t>BEL-268</t>
-        </is>
-      </c>
-      <c r="G64" t="inlineStr">
-        <is>
-          <t>груз, трп</t>
-        </is>
-      </c>
-      <c r="H64" t="n">
-        <v>78</v>
-      </c>
-      <c r="I64" s="1" t="n">
-        <v>44826</v>
-      </c>
-      <c r="J64" t="inlineStr">
-        <is>
-          <t>БНХ РОС</t>
-        </is>
-      </c>
-    </row>
-    <row r="65">
-      <c r="E65" t="inlineStr">
-        <is>
-          <t>315/80R22.5</t>
-        </is>
-      </c>
-      <c r="F65" t="inlineStr">
-        <is>
-          <t>BEL-398</t>
-        </is>
-      </c>
-      <c r="G65" t="inlineStr">
-        <is>
-          <t>сер, груз</t>
-        </is>
-      </c>
-      <c r="H65" t="n">
-        <v>78</v>
-      </c>
-      <c r="I65" s="1" t="n">
-        <v>44826</v>
-      </c>
-      <c r="J65" t="inlineStr">
-        <is>
-          <t>БНХ РОС</t>
-        </is>
-      </c>
-    </row>
-    <row r="66">
-      <c r="E66" t="inlineStr">
-        <is>
-          <t>315/80R22.5</t>
-        </is>
-      </c>
-      <c r="F66" t="inlineStr">
-        <is>
-          <t>BEL-326</t>
-        </is>
-      </c>
-      <c r="G66" t="inlineStr">
-        <is>
-          <t>сер, груз</t>
-        </is>
-      </c>
-      <c r="H66" t="n">
-        <v>78</v>
-      </c>
-      <c r="I66" s="1" t="n">
-        <v>44826</v>
-      </c>
-      <c r="J66" t="inlineStr">
-        <is>
-          <t>БНХ РОС</t>
-        </is>
-      </c>
-    </row>
-    <row r="67">
-      <c r="E67" t="inlineStr">
-        <is>
-          <t>315/80R22.5</t>
-        </is>
-      </c>
-      <c r="F67" t="inlineStr">
-        <is>
-          <t>BEL-326</t>
-        </is>
-      </c>
-      <c r="G67" t="inlineStr">
-        <is>
-          <t>груз, трп</t>
-        </is>
-      </c>
-      <c r="H67" t="n">
-        <v>78</v>
-      </c>
-      <c r="I67" s="1" t="n">
-        <v>44826</v>
-      </c>
-      <c r="J67" t="inlineStr">
-        <is>
-          <t>БНХ РОС</t>
-        </is>
-      </c>
-    </row>
-    <row r="68">
-      <c r="E68" t="inlineStr">
-        <is>
-          <t>315/80R22.5</t>
-        </is>
-      </c>
-      <c r="F68" t="inlineStr">
-        <is>
-          <t>BEL-498</t>
-        </is>
-      </c>
-      <c r="G68" t="inlineStr">
-        <is>
-          <t>156L, сер, груз</t>
-        </is>
-      </c>
-      <c r="H68" t="n">
-        <v>78</v>
-      </c>
-      <c r="I68" s="1" t="n">
-        <v>44826</v>
-      </c>
-      <c r="J68" t="inlineStr">
-        <is>
-          <t>БНХ РОС</t>
-        </is>
-      </c>
-    </row>
-    <row r="69">
-      <c r="E69" t="inlineStr">
-        <is>
-          <t>315/80R22.5</t>
-        </is>
-      </c>
-      <c r="F69" t="inlineStr">
-        <is>
-          <t>BEL-518</t>
-        </is>
-      </c>
-      <c r="G69" t="inlineStr">
-        <is>
-          <t>сер, груз</t>
-        </is>
-      </c>
-      <c r="H69" t="n">
-        <v>78</v>
-      </c>
-      <c r="I69" s="1" t="n">
-        <v>44826</v>
-      </c>
-      <c r="J69" t="inlineStr">
-        <is>
-          <t>БНХ РОС</t>
-        </is>
-      </c>
-    </row>
-    <row r="70">
-      <c r="E70" t="inlineStr">
-        <is>
-          <t>12.00R20</t>
-        </is>
-      </c>
-      <c r="F70" t="inlineStr">
-        <is>
-          <t>ИД-304М</t>
-        </is>
-      </c>
-      <c r="G70" t="inlineStr">
-        <is>
-          <t>16, сер, груз</t>
-        </is>
-      </c>
-      <c r="H70" t="n">
-        <v>78</v>
-      </c>
-      <c r="I70" s="1" t="n">
-        <v>44826</v>
-      </c>
-      <c r="J70" t="inlineStr">
-        <is>
-          <t>БНХ РОС</t>
-        </is>
-      </c>
-    </row>
-    <row r="71">
-      <c r="E71" t="inlineStr">
-        <is>
-          <t>12.00R20</t>
-        </is>
-      </c>
-      <c r="F71" t="inlineStr">
-        <is>
-          <t>ИД-304М</t>
-        </is>
-      </c>
-      <c r="G71" t="inlineStr">
-        <is>
-          <t>18, сер, груз</t>
-        </is>
-      </c>
-      <c r="H71" t="n">
-        <v>78</v>
-      </c>
-      <c r="I71" s="1" t="n">
-        <v>44826</v>
-      </c>
-      <c r="J71" t="inlineStr">
-        <is>
-          <t>БНХ РОС</t>
-        </is>
-      </c>
-    </row>
-    <row r="72">
-      <c r="E72" t="inlineStr">
-        <is>
-          <t>12.00R20</t>
-        </is>
-      </c>
-      <c r="F72" t="inlineStr">
-        <is>
-          <t>ИД-304М</t>
-        </is>
-      </c>
-      <c r="G72" t="inlineStr">
-        <is>
-          <t>16, груз, трп</t>
-        </is>
-      </c>
-      <c r="H72" t="n">
-        <v>78</v>
-      </c>
-      <c r="I72" s="1" t="n">
-        <v>44826</v>
-      </c>
-      <c r="J72" t="inlineStr">
-        <is>
-          <t>БНХ РОС</t>
-        </is>
-      </c>
-    </row>
-    <row r="73">
-      <c r="E73" t="inlineStr">
-        <is>
-          <t>12.00R20</t>
-        </is>
-      </c>
-      <c r="F73" t="inlineStr">
-        <is>
-          <t>ИД-304М</t>
-        </is>
-      </c>
-      <c r="G73" t="inlineStr">
-        <is>
-          <t>18, груз, трп</t>
-        </is>
-      </c>
-      <c r="H73" t="n">
-        <v>78</v>
-      </c>
-      <c r="I73" s="1" t="n">
-        <v>44826</v>
-      </c>
-      <c r="J73" t="inlineStr">
-        <is>
-          <t>БНХ РОС</t>
-        </is>
-      </c>
-    </row>
-    <row r="74">
-      <c r="E74" t="inlineStr">
-        <is>
-          <t>12.00R20</t>
-        </is>
-      </c>
-      <c r="F74" t="inlineStr">
-        <is>
-          <t>БИ-368М</t>
-        </is>
-      </c>
-      <c r="G74" t="inlineStr">
-        <is>
-          <t>18, сер, груз</t>
-        </is>
-      </c>
-      <c r="H74" t="n">
-        <v>78</v>
-      </c>
-      <c r="I74" s="1" t="n">
-        <v>44826</v>
-      </c>
-      <c r="J74" t="inlineStr">
-        <is>
-          <t>БНХ РОС</t>
-        </is>
-      </c>
-    </row>
-    <row r="75">
-      <c r="E75" t="inlineStr">
-        <is>
-          <t>12.00R20</t>
-        </is>
-      </c>
-      <c r="F75" t="inlineStr">
-        <is>
-          <t>БИ-368М</t>
-        </is>
-      </c>
-      <c r="G75" t="inlineStr">
-        <is>
-          <t>18, сер, груз</t>
-        </is>
-      </c>
-      <c r="H75" t="n">
-        <v>78</v>
-      </c>
-      <c r="I75" s="1" t="n">
-        <v>44826</v>
-      </c>
-      <c r="J75" t="inlineStr">
-        <is>
-          <t>БНХ РОС</t>
-        </is>
-      </c>
-    </row>
-    <row r="76">
-      <c r="E76" t="inlineStr">
-        <is>
-          <t>12.00R20</t>
-        </is>
-      </c>
-      <c r="F76" t="inlineStr">
-        <is>
-          <t>БИ-368М</t>
-        </is>
-      </c>
-      <c r="G76" t="inlineStr">
-        <is>
-          <t>18, груз, трп</t>
-        </is>
-      </c>
-      <c r="H76" t="n">
-        <v>78</v>
-      </c>
-      <c r="I76" s="1" t="n">
-        <v>44826</v>
-      </c>
-      <c r="J76" t="inlineStr">
-        <is>
-          <t>БНХ РОС</t>
-        </is>
-      </c>
-    </row>
-    <row r="77">
-      <c r="E77" t="inlineStr">
-        <is>
-          <t>195/65R15</t>
-        </is>
-      </c>
-      <c r="F77" t="inlineStr">
-        <is>
-          <t>BEL-337</t>
-        </is>
-      </c>
-      <c r="G77" t="inlineStr">
-        <is>
-          <t>сер, легк, б/к</t>
-        </is>
-      </c>
-      <c r="H77" t="n">
-        <v>78</v>
-      </c>
-      <c r="I77" s="1" t="n">
-        <v>44826</v>
-      </c>
-      <c r="J77" t="inlineStr">
         <is>
           <t>БНХ РОС</t>
         </is>

</xml_diff>

<commit_message>
SALES  improved contagents 0.8 at 15/10/2022
</commit_message>
<xml_diff>
--- a/src/Tyres.xlsx
+++ b/src/Tyres.xlsx
@@ -417,7 +417,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J40"/>
+  <dimension ref="A1:J56"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -507,11 +507,11 @@
         <v>259</v>
       </c>
       <c r="I2" s="1" t="n">
-        <v>44826</v>
+        <v>44814</v>
       </c>
       <c r="J2" t="inlineStr">
         <is>
-          <t>БНХ РОС</t>
+          <t>HHHDFD</t>
         </is>
       </c>
     </row>
@@ -547,14 +547,14 @@
         </is>
       </c>
       <c r="H3" t="n">
-        <v>265</v>
+        <v>285</v>
       </c>
       <c r="I3" s="1" t="n">
-        <v>44826</v>
+        <v>44814</v>
       </c>
       <c r="J3" t="inlineStr">
         <is>
-          <t>БНХ РОС</t>
+          <t>HHHDFD</t>
         </is>
       </c>
     </row>
@@ -593,11 +593,11 @@
         <v>281</v>
       </c>
       <c r="I4" s="1" t="n">
-        <v>44826</v>
+        <v>44814</v>
       </c>
       <c r="J4" t="inlineStr">
         <is>
-          <t>БНХ РОС</t>
+          <t>HHHDFD</t>
         </is>
       </c>
     </row>
@@ -636,11 +636,11 @@
         <v>287</v>
       </c>
       <c r="I5" s="1" t="n">
-        <v>44826</v>
+        <v>44814</v>
       </c>
       <c r="J5" t="inlineStr">
         <is>
-          <t>БНХ РОС</t>
+          <t>HHHDFD</t>
         </is>
       </c>
     </row>
@@ -679,7 +679,7 @@
         <v>283</v>
       </c>
       <c r="I6" s="1" t="n">
-        <v>44826</v>
+        <v>44814</v>
       </c>
       <c r="J6" t="inlineStr">
         <is>
@@ -722,11 +722,11 @@
         <v>287</v>
       </c>
       <c r="I7" s="1" t="n">
-        <v>44826</v>
+        <v>44814</v>
       </c>
       <c r="J7" t="inlineStr">
         <is>
-          <t>БНХ РОС</t>
+          <t>HHHDFD</t>
         </is>
       </c>
     </row>
@@ -765,11 +765,11 @@
         <v>265</v>
       </c>
       <c r="I8" s="1" t="n">
-        <v>44826</v>
+        <v>44814</v>
       </c>
       <c r="J8" t="inlineStr">
         <is>
-          <t>БНХ РОС</t>
+          <t>нет данных</t>
         </is>
       </c>
     </row>
@@ -808,11 +808,11 @@
         <v>269</v>
       </c>
       <c r="I9" s="1" t="n">
-        <v>44826</v>
+        <v>44814</v>
       </c>
       <c r="J9" t="inlineStr">
         <is>
-          <t>БНХ РОС</t>
+          <t>нет данных</t>
         </is>
       </c>
     </row>
@@ -848,14 +848,14 @@
         </is>
       </c>
       <c r="H10" t="n">
-        <v>273</v>
+        <v>27</v>
       </c>
       <c r="I10" s="1" t="n">
-        <v>44826</v>
+        <v>44814</v>
       </c>
       <c r="J10" t="inlineStr">
         <is>
-          <t>БНХ РОС</t>
+          <t>HHHDFD</t>
         </is>
       </c>
     </row>
@@ -894,11 +894,11 @@
         <v>247</v>
       </c>
       <c r="I11" s="1" t="n">
-        <v>44826</v>
+        <v>44814</v>
       </c>
       <c r="J11" t="inlineStr">
         <is>
-          <t>БНХ РОС</t>
+          <t>нет данных</t>
         </is>
       </c>
     </row>
@@ -937,11 +937,11 @@
         <v>255</v>
       </c>
       <c r="I12" s="1" t="n">
-        <v>44826</v>
+        <v>44814</v>
       </c>
       <c r="J12" t="inlineStr">
         <is>
-          <t>БНХ РОС</t>
+          <t>HHHDFD</t>
         </is>
       </c>
     </row>
@@ -977,14 +977,14 @@
         </is>
       </c>
       <c r="H13" t="n">
-        <v>279</v>
+        <v>1555</v>
       </c>
       <c r="I13" s="1" t="n">
-        <v>44826</v>
+        <v>44814</v>
       </c>
       <c r="J13" t="inlineStr">
         <is>
-          <t>БНХ РОС</t>
+          <t>нет данных</t>
         </is>
       </c>
     </row>
@@ -1023,11 +1023,11 @@
         <v>285</v>
       </c>
       <c r="I14" s="1" t="n">
-        <v>44826</v>
+        <v>44814</v>
       </c>
       <c r="J14" t="inlineStr">
         <is>
-          <t>БНХ РОС</t>
+          <t>HHHDFD</t>
         </is>
       </c>
     </row>
@@ -1066,11 +1066,11 @@
         <v>290</v>
       </c>
       <c r="I15" s="1" t="n">
-        <v>44826</v>
+        <v>44814</v>
       </c>
       <c r="J15" t="inlineStr">
         <is>
-          <t>БНХ РОС</t>
+          <t>HHHDFD</t>
         </is>
       </c>
     </row>
@@ -1109,11 +1109,11 @@
         <v>296</v>
       </c>
       <c r="I16" s="1" t="n">
-        <v>44826</v>
+        <v>44814</v>
       </c>
       <c r="J16" t="inlineStr">
         <is>
-          <t>БНХ РОС</t>
+          <t>HHHDFD</t>
         </is>
       </c>
     </row>
@@ -1149,14 +1149,14 @@
         </is>
       </c>
       <c r="H17" t="n">
-        <v>283</v>
+        <v>4565</v>
       </c>
       <c r="I17" s="1" t="n">
-        <v>44826</v>
+        <v>44814</v>
       </c>
       <c r="J17" t="inlineStr">
         <is>
-          <t>БНХ РОС</t>
+          <t>нет данных</t>
         </is>
       </c>
     </row>
@@ -1192,14 +1192,14 @@
         </is>
       </c>
       <c r="H18" t="n">
-        <v>283</v>
+        <v>4565</v>
       </c>
       <c r="I18" s="1" t="n">
-        <v>44826</v>
+        <v>44814</v>
       </c>
       <c r="J18" t="inlineStr">
         <is>
-          <t>БНХ РОС</t>
+          <t>нет данных</t>
         </is>
       </c>
     </row>
@@ -1231,102 +1231,102 @@
       </c>
       <c r="G19" t="inlineStr">
         <is>
-          <t>18, груз, трп</t>
+          <t>18, груз, сер</t>
         </is>
       </c>
       <c r="H19" t="n">
-        <v>291</v>
+        <v>283</v>
       </c>
       <c r="I19" s="1" t="n">
-        <v>44826</v>
+        <v>44814</v>
       </c>
       <c r="J19" t="inlineStr">
         <is>
-          <t>БНХ РОС</t>
+          <t>нет данных</t>
         </is>
       </c>
     </row>
     <row r="20">
       <c r="E20" t="inlineStr">
         <is>
-          <t>195/65R15</t>
+          <t>12.00R20</t>
         </is>
       </c>
       <c r="F20" t="inlineStr">
         <is>
-          <t>BEL-337</t>
+          <t>БИ-368М</t>
         </is>
       </c>
       <c r="G20" t="inlineStr">
         <is>
-          <t>б/к, сер, легк</t>
+          <t>18, груз, сер</t>
         </is>
       </c>
       <c r="H20" t="n">
-        <v>291</v>
+        <v>283</v>
       </c>
       <c r="I20" s="1" t="n">
-        <v>44826</v>
+        <v>44814</v>
       </c>
       <c r="J20" t="inlineStr">
         <is>
-          <t>БНХ РОС</t>
+          <t>нет данных</t>
         </is>
       </c>
     </row>
     <row r="21">
       <c r="E21" t="inlineStr">
         <is>
-          <t>315/80R22.5</t>
+          <t>12.00R20</t>
         </is>
       </c>
       <c r="F21" t="inlineStr">
         <is>
-          <t>BEL-326</t>
+          <t>БИ-368М</t>
         </is>
       </c>
       <c r="G21" t="inlineStr">
         <is>
-          <t>груз, трп</t>
+          <t>18, груз, трп</t>
         </is>
       </c>
       <c r="H21" t="n">
-        <v>27</v>
+        <v>291</v>
       </c>
       <c r="I21" s="1" t="n">
-        <v>44826</v>
+        <v>44814</v>
       </c>
       <c r="J21" t="inlineStr">
         <is>
-          <t>БНХ РОС</t>
+          <t>HHHDFD</t>
         </is>
       </c>
     </row>
     <row r="22">
       <c r="E22" t="inlineStr">
         <is>
-          <t>315/80R22.5</t>
+          <t>195/65R15</t>
         </is>
       </c>
       <c r="F22" t="inlineStr">
         <is>
-          <t>BEL-158M</t>
+          <t>BEL-337</t>
         </is>
       </c>
       <c r="G22" t="inlineStr">
         <is>
-          <t>камневыт, груз, сер</t>
+          <t>б/к, сер, легк</t>
         </is>
       </c>
       <c r="H22" t="n">
-        <v>259</v>
+        <v>291</v>
       </c>
       <c r="I22" s="1" t="n">
-        <v>44849</v>
+        <v>44814</v>
       </c>
       <c r="J22" t="inlineStr">
         <is>
-          <t>БНХ РОС</t>
+          <t>HHHDFD</t>
         </is>
       </c>
     </row>
@@ -1343,14 +1343,14 @@
       </c>
       <c r="G23" t="inlineStr">
         <is>
-          <t>камневыт, груз, трп</t>
+          <t>камневыт, груз, сер</t>
         </is>
       </c>
       <c r="H23" t="n">
-        <v>265</v>
+        <v>259</v>
       </c>
       <c r="I23" s="1" t="n">
-        <v>44849</v>
+        <v>44752</v>
       </c>
       <c r="J23" t="inlineStr">
         <is>
@@ -1366,19 +1366,19 @@
       </c>
       <c r="F24" t="inlineStr">
         <is>
-          <t>BEL-278</t>
+          <t>BEL-158M</t>
         </is>
       </c>
       <c r="G24" t="inlineStr">
         <is>
-          <t>груз, сер</t>
+          <t>камневыт, груз, трп</t>
         </is>
       </c>
       <c r="H24" t="n">
-        <v>281</v>
+        <v>285</v>
       </c>
       <c r="I24" s="1" t="n">
-        <v>44849</v>
+        <v>44752</v>
       </c>
       <c r="J24" t="inlineStr">
         <is>
@@ -1399,14 +1399,14 @@
       </c>
       <c r="G25" t="inlineStr">
         <is>
-          <t>груз, трп</t>
+          <t>груз, сер</t>
         </is>
       </c>
       <c r="H25" t="n">
-        <v>287</v>
+        <v>281</v>
       </c>
       <c r="I25" s="1" t="n">
-        <v>44849</v>
+        <v>44752</v>
       </c>
       <c r="J25" t="inlineStr">
         <is>
@@ -1422,19 +1422,19 @@
       </c>
       <c r="F26" t="inlineStr">
         <is>
-          <t>BEL-268</t>
+          <t>BEL-278</t>
         </is>
       </c>
       <c r="G26" t="inlineStr">
         <is>
-          <t>груз, сер</t>
+          <t>груз, трп</t>
         </is>
       </c>
       <c r="H26" t="n">
-        <v>283</v>
+        <v>287</v>
       </c>
       <c r="I26" s="1" t="n">
-        <v>44849</v>
+        <v>44752</v>
       </c>
       <c r="J26" t="inlineStr">
         <is>
@@ -1455,14 +1455,14 @@
       </c>
       <c r="G27" t="inlineStr">
         <is>
-          <t>груз, трп</t>
+          <t>груз, сер</t>
         </is>
       </c>
       <c r="H27" t="n">
-        <v>287</v>
+        <v>283</v>
       </c>
       <c r="I27" s="1" t="n">
-        <v>44849</v>
+        <v>44752</v>
       </c>
       <c r="J27" t="inlineStr">
         <is>
@@ -1478,19 +1478,19 @@
       </c>
       <c r="F28" t="inlineStr">
         <is>
-          <t>BEL-398</t>
+          <t>BEL-268</t>
         </is>
       </c>
       <c r="G28" t="inlineStr">
         <is>
-          <t>груз, сер</t>
+          <t>груз, трп</t>
         </is>
       </c>
       <c r="H28" t="n">
-        <v>265</v>
+        <v>287</v>
       </c>
       <c r="I28" s="1" t="n">
-        <v>44849</v>
+        <v>44752</v>
       </c>
       <c r="J28" t="inlineStr">
         <is>
@@ -1506,7 +1506,7 @@
       </c>
       <c r="F29" t="inlineStr">
         <is>
-          <t>BEL-326</t>
+          <t>BEL-398</t>
         </is>
       </c>
       <c r="G29" t="inlineStr">
@@ -1515,14 +1515,14 @@
         </is>
       </c>
       <c r="H29" t="n">
-        <v>269</v>
+        <v>265</v>
       </c>
       <c r="I29" s="1" t="n">
-        <v>44849</v>
+        <v>44752</v>
       </c>
       <c r="J29" t="inlineStr">
         <is>
-          <t>БНХ РОС</t>
+          <t>нет данных</t>
         </is>
       </c>
     </row>
@@ -1539,18 +1539,18 @@
       </c>
       <c r="G30" t="inlineStr">
         <is>
-          <t>груз, трп</t>
+          <t>груз, сер</t>
         </is>
       </c>
       <c r="H30" t="n">
-        <v>27</v>
+        <v>269</v>
       </c>
       <c r="I30" s="1" t="n">
-        <v>44849</v>
+        <v>44752</v>
       </c>
       <c r="J30" t="inlineStr">
         <is>
-          <t>БНХ РОС</t>
+          <t>нет данных</t>
         </is>
       </c>
     </row>
@@ -1562,19 +1562,19 @@
       </c>
       <c r="F31" t="inlineStr">
         <is>
-          <t>BEL-498</t>
+          <t>BEL-326</t>
         </is>
       </c>
       <c r="G31" t="inlineStr">
         <is>
-          <t>156L, груз, сер</t>
+          <t>груз, трп</t>
         </is>
       </c>
       <c r="H31" t="n">
-        <v>247</v>
+        <v>27</v>
       </c>
       <c r="I31" s="1" t="n">
-        <v>44849</v>
+        <v>44752</v>
       </c>
       <c r="J31" t="inlineStr">
         <is>
@@ -1590,47 +1590,47 @@
       </c>
       <c r="F32" t="inlineStr">
         <is>
-          <t>BEL-518</t>
+          <t>BEL-498</t>
         </is>
       </c>
       <c r="G32" t="inlineStr">
         <is>
-          <t>груз, сер</t>
+          <t>156L, груз, сер</t>
         </is>
       </c>
       <c r="H32" t="n">
-        <v>255</v>
+        <v>247</v>
       </c>
       <c r="I32" s="1" t="n">
-        <v>44849</v>
+        <v>44752</v>
       </c>
       <c r="J32" t="inlineStr">
         <is>
-          <t>БНХ РОС</t>
+          <t>нет данных</t>
         </is>
       </c>
     </row>
     <row r="33">
       <c r="E33" t="inlineStr">
         <is>
-          <t>12.00R20</t>
+          <t>315/80R22.5</t>
         </is>
       </c>
       <c r="F33" t="inlineStr">
         <is>
-          <t>ИД-304М</t>
+          <t>BEL-518</t>
         </is>
       </c>
       <c r="G33" t="inlineStr">
         <is>
-          <t>16, груз, сер</t>
+          <t>груз, сер</t>
         </is>
       </c>
       <c r="H33" t="n">
-        <v>279</v>
+        <v>255</v>
       </c>
       <c r="I33" s="1" t="n">
-        <v>44849</v>
+        <v>44752</v>
       </c>
       <c r="J33" t="inlineStr">
         <is>
@@ -1651,18 +1651,18 @@
       </c>
       <c r="G34" t="inlineStr">
         <is>
-          <t>18, груз, сер</t>
+          <t>16, груз, сер</t>
         </is>
       </c>
       <c r="H34" t="n">
-        <v>285</v>
+        <v>1555</v>
       </c>
       <c r="I34" s="1" t="n">
-        <v>44849</v>
+        <v>44752</v>
       </c>
       <c r="J34" t="inlineStr">
         <is>
-          <t>БНХ РОС</t>
+          <t>нет данных</t>
         </is>
       </c>
     </row>
@@ -1679,14 +1679,14 @@
       </c>
       <c r="G35" t="inlineStr">
         <is>
-          <t>16, груз, трп</t>
+          <t>18, груз, сер</t>
         </is>
       </c>
       <c r="H35" t="n">
-        <v>290</v>
+        <v>285</v>
       </c>
       <c r="I35" s="1" t="n">
-        <v>44849</v>
+        <v>44752</v>
       </c>
       <c r="J35" t="inlineStr">
         <is>
@@ -1707,14 +1707,14 @@
       </c>
       <c r="G36" t="inlineStr">
         <is>
-          <t>18, груз, трп</t>
+          <t>16, груз, трп</t>
         </is>
       </c>
       <c r="H36" t="n">
-        <v>296</v>
+        <v>290</v>
       </c>
       <c r="I36" s="1" t="n">
-        <v>44849</v>
+        <v>44752</v>
       </c>
       <c r="J36" t="inlineStr">
         <is>
@@ -1730,19 +1730,19 @@
       </c>
       <c r="F37" t="inlineStr">
         <is>
-          <t>БИ-368М</t>
+          <t>ИД-304М</t>
         </is>
       </c>
       <c r="G37" t="inlineStr">
         <is>
-          <t>18, груз, сер</t>
+          <t>18, груз, трп</t>
         </is>
       </c>
       <c r="H37" t="n">
-        <v>283</v>
+        <v>296</v>
       </c>
       <c r="I37" s="1" t="n">
-        <v>44849</v>
+        <v>44752</v>
       </c>
       <c r="J37" t="inlineStr">
         <is>
@@ -1767,14 +1767,14 @@
         </is>
       </c>
       <c r="H38" t="n">
-        <v>283</v>
+        <v>4565</v>
       </c>
       <c r="I38" s="1" t="n">
-        <v>44849</v>
+        <v>44752</v>
       </c>
       <c r="J38" t="inlineStr">
         <is>
-          <t>БНХ РОС</t>
+          <t>нет данных</t>
         </is>
       </c>
     </row>
@@ -1791,46 +1791,494 @@
       </c>
       <c r="G39" t="inlineStr">
         <is>
-          <t>18, груз, трп</t>
+          <t>18, груз, сер</t>
         </is>
       </c>
       <c r="H39" t="n">
-        <v>291</v>
+        <v>4565</v>
       </c>
       <c r="I39" s="1" t="n">
-        <v>44849</v>
+        <v>44752</v>
       </c>
       <c r="J39" t="inlineStr">
         <is>
-          <t>БНХ РОС</t>
+          <t>нет данных</t>
         </is>
       </c>
     </row>
     <row r="40">
       <c r="E40" t="inlineStr">
         <is>
+          <t>12.00R20</t>
+        </is>
+      </c>
+      <c r="F40" t="inlineStr">
+        <is>
+          <t>БИ-368М</t>
+        </is>
+      </c>
+      <c r="G40" t="inlineStr">
+        <is>
+          <t>18, груз, сер</t>
+        </is>
+      </c>
+      <c r="H40" t="n">
+        <v>283</v>
+      </c>
+      <c r="I40" s="1" t="n">
+        <v>44752</v>
+      </c>
+      <c r="J40" t="inlineStr">
+        <is>
+          <t>нет данных</t>
+        </is>
+      </c>
+    </row>
+    <row r="41">
+      <c r="E41" t="inlineStr">
+        <is>
+          <t>12.00R20</t>
+        </is>
+      </c>
+      <c r="F41" t="inlineStr">
+        <is>
+          <t>БИ-368М</t>
+        </is>
+      </c>
+      <c r="G41" t="inlineStr">
+        <is>
+          <t>18, груз, сер</t>
+        </is>
+      </c>
+      <c r="H41" t="n">
+        <v>283</v>
+      </c>
+      <c r="I41" s="1" t="n">
+        <v>44752</v>
+      </c>
+      <c r="J41" t="inlineStr">
+        <is>
+          <t>нет данных</t>
+        </is>
+      </c>
+    </row>
+    <row r="42">
+      <c r="E42" t="inlineStr">
+        <is>
+          <t>12.00R20</t>
+        </is>
+      </c>
+      <c r="F42" t="inlineStr">
+        <is>
+          <t>БИ-368М</t>
+        </is>
+      </c>
+      <c r="G42" t="inlineStr">
+        <is>
+          <t>18, груз, трп</t>
+        </is>
+      </c>
+      <c r="H42" t="n">
+        <v>291</v>
+      </c>
+      <c r="I42" s="1" t="n">
+        <v>44752</v>
+      </c>
+      <c r="J42" t="inlineStr">
+        <is>
+          <t>HHHDFD</t>
+        </is>
+      </c>
+    </row>
+    <row r="43">
+      <c r="E43" t="inlineStr">
+        <is>
           <t>195/65R15</t>
         </is>
       </c>
-      <c r="F40" t="inlineStr">
+      <c r="F43" t="inlineStr">
         <is>
           <t>BEL-337</t>
         </is>
       </c>
-      <c r="G40" t="inlineStr">
+      <c r="G43" t="inlineStr">
         <is>
           <t>б/к, сер, легк</t>
         </is>
       </c>
-      <c r="H40" t="n">
+      <c r="H43" t="n">
         <v>291</v>
       </c>
-      <c r="I40" s="1" t="n">
-        <v>44849</v>
-      </c>
-      <c r="J40" t="inlineStr">
-        <is>
-          <t>БНХ РОС</t>
+      <c r="I43" s="1" t="n">
+        <v>44752</v>
+      </c>
+      <c r="J43" t="inlineStr">
+        <is>
+          <t>HHHDFD</t>
+        </is>
+      </c>
+    </row>
+    <row r="44">
+      <c r="E44" t="inlineStr">
+        <is>
+          <t>315/80R22.5</t>
+        </is>
+      </c>
+      <c r="F44" t="inlineStr">
+        <is>
+          <t>BEL-158M</t>
+        </is>
+      </c>
+      <c r="G44" t="inlineStr">
+        <is>
+          <t>камневыт, груз, сер</t>
+        </is>
+      </c>
+      <c r="H44" t="n">
+        <v>259</v>
+      </c>
+      <c r="I44" s="1" t="n">
+        <v>44752</v>
+      </c>
+      <c r="J44" t="inlineStr">
+        <is>
+          <t>HHHDFD</t>
+        </is>
+      </c>
+    </row>
+    <row r="45">
+      <c r="E45" t="inlineStr">
+        <is>
+          <t>315/80R22.5</t>
+        </is>
+      </c>
+      <c r="F45" t="inlineStr">
+        <is>
+          <t>BEL-158M</t>
+        </is>
+      </c>
+      <c r="G45" t="inlineStr">
+        <is>
+          <t>камневыт, груз, трп</t>
+        </is>
+      </c>
+      <c r="H45" t="n">
+        <v>285</v>
+      </c>
+      <c r="I45" s="1" t="n">
+        <v>44752</v>
+      </c>
+      <c r="J45" t="inlineStr">
+        <is>
+          <t>HHHDFD</t>
+        </is>
+      </c>
+    </row>
+    <row r="46">
+      <c r="E46" t="inlineStr">
+        <is>
+          <t>315/80R22.5</t>
+        </is>
+      </c>
+      <c r="F46" t="inlineStr">
+        <is>
+          <t>BEL-278</t>
+        </is>
+      </c>
+      <c r="G46" t="inlineStr">
+        <is>
+          <t>груз, сер</t>
+        </is>
+      </c>
+      <c r="H46" t="n">
+        <v>281</v>
+      </c>
+      <c r="I46" s="1" t="n">
+        <v>44752</v>
+      </c>
+      <c r="J46" t="inlineStr">
+        <is>
+          <t>HHHDFD</t>
+        </is>
+      </c>
+    </row>
+    <row r="47">
+      <c r="E47" t="inlineStr">
+        <is>
+          <t>315/80R22.5</t>
+        </is>
+      </c>
+      <c r="F47" t="inlineStr">
+        <is>
+          <t>BEL-278</t>
+        </is>
+      </c>
+      <c r="G47" t="inlineStr">
+        <is>
+          <t>груз, трп</t>
+        </is>
+      </c>
+      <c r="H47" t="n">
+        <v>287</v>
+      </c>
+      <c r="I47" s="1" t="n">
+        <v>44752</v>
+      </c>
+      <c r="J47" t="inlineStr">
+        <is>
+          <t>HHHDFD</t>
+        </is>
+      </c>
+    </row>
+    <row r="48">
+      <c r="E48" t="inlineStr">
+        <is>
+          <t>315/80R22.5</t>
+        </is>
+      </c>
+      <c r="F48" t="inlineStr">
+        <is>
+          <t>BEL-268</t>
+        </is>
+      </c>
+      <c r="G48" t="inlineStr">
+        <is>
+          <t>груз, сер</t>
+        </is>
+      </c>
+      <c r="H48" t="n">
+        <v>283</v>
+      </c>
+      <c r="I48" s="1" t="n">
+        <v>44752</v>
+      </c>
+      <c r="J48" t="inlineStr">
+        <is>
+          <t>HHHDFD</t>
+        </is>
+      </c>
+    </row>
+    <row r="49">
+      <c r="E49" t="inlineStr">
+        <is>
+          <t>315/80R22.5</t>
+        </is>
+      </c>
+      <c r="F49" t="inlineStr">
+        <is>
+          <t>BEL-268</t>
+        </is>
+      </c>
+      <c r="G49" t="inlineStr">
+        <is>
+          <t>груз, трп</t>
+        </is>
+      </c>
+      <c r="H49" t="n">
+        <v>287</v>
+      </c>
+      <c r="I49" s="1" t="n">
+        <v>44752</v>
+      </c>
+      <c r="J49" t="inlineStr">
+        <is>
+          <t>HHHDFD</t>
+        </is>
+      </c>
+    </row>
+    <row r="50">
+      <c r="E50" t="inlineStr">
+        <is>
+          <t>315/80R22.5</t>
+        </is>
+      </c>
+      <c r="F50" t="inlineStr">
+        <is>
+          <t>BEL-326</t>
+        </is>
+      </c>
+      <c r="G50" t="inlineStr">
+        <is>
+          <t>груз, трп</t>
+        </is>
+      </c>
+      <c r="H50" t="n">
+        <v>27</v>
+      </c>
+      <c r="I50" s="1" t="n">
+        <v>44752</v>
+      </c>
+      <c r="J50" t="inlineStr">
+        <is>
+          <t>HHHDFD</t>
+        </is>
+      </c>
+    </row>
+    <row r="51">
+      <c r="E51" t="inlineStr">
+        <is>
+          <t>315/80R22.5</t>
+        </is>
+      </c>
+      <c r="F51" t="inlineStr">
+        <is>
+          <t>BEL-518</t>
+        </is>
+      </c>
+      <c r="G51" t="inlineStr">
+        <is>
+          <t>груз, сер</t>
+        </is>
+      </c>
+      <c r="H51" t="n">
+        <v>255</v>
+      </c>
+      <c r="I51" s="1" t="n">
+        <v>44752</v>
+      </c>
+      <c r="J51" t="inlineStr">
+        <is>
+          <t>HHHDFD</t>
+        </is>
+      </c>
+    </row>
+    <row r="52">
+      <c r="E52" t="inlineStr">
+        <is>
+          <t>12.00R20</t>
+        </is>
+      </c>
+      <c r="F52" t="inlineStr">
+        <is>
+          <t>ИД-304М</t>
+        </is>
+      </c>
+      <c r="G52" t="inlineStr">
+        <is>
+          <t>18, груз, сер</t>
+        </is>
+      </c>
+      <c r="H52" t="n">
+        <v>285</v>
+      </c>
+      <c r="I52" s="1" t="n">
+        <v>44752</v>
+      </c>
+      <c r="J52" t="inlineStr">
+        <is>
+          <t>HHHDFD</t>
+        </is>
+      </c>
+    </row>
+    <row r="53">
+      <c r="E53" t="inlineStr">
+        <is>
+          <t>12.00R20</t>
+        </is>
+      </c>
+      <c r="F53" t="inlineStr">
+        <is>
+          <t>ИД-304М</t>
+        </is>
+      </c>
+      <c r="G53" t="inlineStr">
+        <is>
+          <t>16, груз, трп</t>
+        </is>
+      </c>
+      <c r="H53" t="n">
+        <v>290</v>
+      </c>
+      <c r="I53" s="1" t="n">
+        <v>44752</v>
+      </c>
+      <c r="J53" t="inlineStr">
+        <is>
+          <t>БНХ УКР</t>
+        </is>
+      </c>
+    </row>
+    <row r="54">
+      <c r="E54" t="inlineStr">
+        <is>
+          <t>12.00R20</t>
+        </is>
+      </c>
+      <c r="F54" t="inlineStr">
+        <is>
+          <t>ИД-304М</t>
+        </is>
+      </c>
+      <c r="G54" t="inlineStr">
+        <is>
+          <t>18, груз, трп</t>
+        </is>
+      </c>
+      <c r="H54" t="n">
+        <v>296</v>
+      </c>
+      <c r="I54" s="1" t="n">
+        <v>44752</v>
+      </c>
+      <c r="J54" t="inlineStr">
+        <is>
+          <t>БНХ УКР</t>
+        </is>
+      </c>
+    </row>
+    <row r="55">
+      <c r="E55" t="inlineStr">
+        <is>
+          <t>12.00R20</t>
+        </is>
+      </c>
+      <c r="F55" t="inlineStr">
+        <is>
+          <t>БИ-368М</t>
+        </is>
+      </c>
+      <c r="G55" t="inlineStr">
+        <is>
+          <t>18, груз, трп</t>
+        </is>
+      </c>
+      <c r="H55" t="n">
+        <v>291</v>
+      </c>
+      <c r="I55" s="1" t="n">
+        <v>44752</v>
+      </c>
+      <c r="J55" t="inlineStr">
+        <is>
+          <t>БНХ УКР</t>
+        </is>
+      </c>
+    </row>
+    <row r="56">
+      <c r="E56" t="inlineStr">
+        <is>
+          <t>195/65R15</t>
+        </is>
+      </c>
+      <c r="F56" t="inlineStr">
+        <is>
+          <t>BEL-337</t>
+        </is>
+      </c>
+      <c r="G56" t="inlineStr">
+        <is>
+          <t>б/к, сер, легк</t>
+        </is>
+      </c>
+      <c r="H56" t="n">
+        <v>291</v>
+      </c>
+      <c r="I56" s="1" t="n">
+        <v>44752</v>
+      </c>
+      <c r="J56" t="inlineStr">
+        <is>
+          <t>БНХ УКР</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
prices Onliner done 06/12/2022
</commit_message>
<xml_diff>
--- a/src/Tyres.xlsx
+++ b/src/Tyres.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Holidays 2019" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet name="Sheet" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Holidays 2019" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet" sheetId="2" state="visible" r:id="rId2"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -417,7 +417,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J44"/>
+  <dimension ref="A1:J146"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -428,17 +428,17 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>BEL-158M</t>
+          <t>ФБел-283</t>
         </is>
       </c>
       <c r="B1" t="inlineStr">
         <is>
-          <t>315/80R22.5</t>
+          <t>35/65-33</t>
         </is>
       </c>
       <c r="C1" t="inlineStr">
         <is>
-          <t>камневыт сер груз</t>
+          <t>42 груз сер</t>
         </is>
       </c>
       <c r="E1" t="inlineStr">
@@ -475,36 +475,36 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>BEL-158M</t>
+          <t>Бел-122</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>315/80R22.5</t>
+          <t>24.00R35</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>камневыт трп груз</t>
+          <t>груз сер LS-2 Type</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>315/80R22.5</t>
+          <t>205/60R16</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>BEL-158M</t>
+          <t>BEL-277</t>
         </is>
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>камневыт, сер, груз</t>
+          <t>б/к, сер, легк</t>
         </is>
       </c>
       <c r="H2" t="n">
-        <v>259</v>
+        <v>281</v>
       </c>
       <c r="I2" s="1" t="n">
         <v>44752</v>
@@ -518,254 +518,254 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>BEL-278</t>
+          <t>Бел-122</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>315/80R22.5</t>
+          <t>24.00R35</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>сер груз</t>
+          <t>груз сер Type H</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>315/80R22.5</t>
+          <t>35/65-33</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>BEL-158M</t>
+          <t>ФБел-283</t>
         </is>
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>камневыт, трп, груз</t>
+          <t>42, груз, сер</t>
         </is>
       </c>
       <c r="H3" t="n">
-        <v>285</v>
+        <v>2</v>
       </c>
       <c r="I3" s="1" t="n">
-        <v>44752</v>
+        <v>44893</v>
       </c>
       <c r="J3" t="inlineStr">
         <is>
-          <t>HHHDFD</t>
+          <t>нет данных</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>BEL-278</t>
+          <t>Бел-122</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>315/80R22.5</t>
+          <t>24.00R35</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>трп груз</t>
+          <t>груз сер Type C</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>315/80R22.5</t>
+          <t>24.00R35</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>BEL-278</t>
+          <t>Бел-122</t>
         </is>
       </c>
       <c r="G4" t="inlineStr">
         <is>
-          <t>сер, груз</t>
+          <t>груз, сер, LS-2, Type</t>
         </is>
       </c>
       <c r="H4" t="n">
-        <v>281</v>
+        <v>2</v>
       </c>
       <c r="I4" s="1" t="n">
-        <v>44752</v>
+        <v>44893</v>
       </c>
       <c r="J4" t="inlineStr">
         <is>
-          <t>HHHDFD</t>
+          <t>нет данных</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>BEL-268</t>
+          <t>Бел-202</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>315/80R22.5</t>
+          <t>24.00R35</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>сер груз</t>
+          <t>210B сер LS-2 Type</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>315/80R22.5</t>
+          <t>24.00R35</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>BEL-278</t>
+          <t>Бел-122</t>
         </is>
       </c>
       <c r="G5" t="inlineStr">
         <is>
-          <t>трп, груз</t>
+          <t>груз, сер, Type, H</t>
         </is>
       </c>
       <c r="H5" t="n">
-        <v>287</v>
+        <v>2</v>
       </c>
       <c r="I5" s="1" t="n">
-        <v>44752</v>
+        <v>44893</v>
       </c>
       <c r="J5" t="inlineStr">
         <is>
-          <t>HHHDFD</t>
+          <t>нет данных</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>BEL-268</t>
+          <t>Бел-202</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>315/80R22.5</t>
+          <t>24.00R35</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>трп груз</t>
+          <t>210B сер Type H</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>315/80R22.5</t>
+          <t>24.00R35</t>
         </is>
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>BEL-268</t>
+          <t>Бел-122</t>
         </is>
       </c>
       <c r="G6" t="inlineStr">
         <is>
-          <t>сер, груз</t>
+          <t>груз, сер, Type, C</t>
         </is>
       </c>
       <c r="H6" t="n">
-        <v>283</v>
+        <v>2</v>
       </c>
       <c r="I6" s="1" t="n">
-        <v>44752</v>
+        <v>44893</v>
       </c>
       <c r="J6" t="inlineStr">
         <is>
-          <t>HHHDFD</t>
+          <t>нет данных</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>BEL-398</t>
+          <t>Бел-202</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>315/80R22.5</t>
+          <t>24.00R35</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>сер груз</t>
+          <t>210B сер Type C</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>315/80R22.5</t>
+          <t>24.00R35</t>
         </is>
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>BEL-268</t>
+          <t>Бел-202</t>
         </is>
       </c>
       <c r="G7" t="inlineStr">
         <is>
-          <t>трп, груз</t>
+          <t>210B, сер, LS-2, Type</t>
         </is>
       </c>
       <c r="H7" t="n">
-        <v>287</v>
+        <v>2</v>
       </c>
       <c r="I7" s="1" t="n">
-        <v>44752</v>
+        <v>44893</v>
       </c>
       <c r="J7" t="inlineStr">
         <is>
-          <t>HHHDFD</t>
+          <t>нет данных</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>BEL-326</t>
+          <t>Бел-212</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>315/80R22.5</t>
+          <t>24.00R35</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>сер груз</t>
+          <t>груз сер LS-2 Type</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>315/80R22.5</t>
+          <t>24.00R35</t>
         </is>
       </c>
       <c r="F8" t="inlineStr">
         <is>
-          <t>BEL-398</t>
+          <t>Бел-202</t>
         </is>
       </c>
       <c r="G8" t="inlineStr">
         <is>
-          <t>сер, груз</t>
+          <t>210B, сер, Type, H</t>
         </is>
       </c>
       <c r="H8" t="n">
-        <v>265</v>
+        <v>2</v>
       </c>
       <c r="I8" s="1" t="n">
-        <v>44752</v>
+        <v>44893</v>
       </c>
       <c r="J8" t="inlineStr">
         <is>
@@ -776,39 +776,39 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>BEL-326</t>
+          <t>Бел-212</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>315/80R22.5</t>
+          <t>24.00R35</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>трп груз</t>
+          <t>груз сер Type H</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>315/80R22.5</t>
+          <t>24.00R35</t>
         </is>
       </c>
       <c r="F9" t="inlineStr">
         <is>
-          <t>BEL-326</t>
+          <t>Бел-202</t>
         </is>
       </c>
       <c r="G9" t="inlineStr">
         <is>
-          <t>сер, груз</t>
+          <t>210B, сер, Type, C</t>
         </is>
       </c>
       <c r="H9" t="n">
-        <v>269</v>
+        <v>2</v>
       </c>
       <c r="I9" s="1" t="n">
-        <v>44752</v>
+        <v>44893</v>
       </c>
       <c r="J9" t="inlineStr">
         <is>
@@ -819,82 +819,82 @@
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>BEL-498</t>
+          <t>Бел-212</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>315/80R22.5</t>
+          <t>24.00R35</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>156L сер груз</t>
+          <t>груз сер Type C</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>315/80R22.5</t>
+          <t>24.00R35</t>
         </is>
       </c>
       <c r="F10" t="inlineStr">
         <is>
-          <t>BEL-326</t>
+          <t>Бел-212</t>
         </is>
       </c>
       <c r="G10" t="inlineStr">
         <is>
-          <t>трп, груз</t>
+          <t>груз, сер, LS-2, Type</t>
         </is>
       </c>
       <c r="H10" t="n">
-        <v>27</v>
+        <v>2</v>
       </c>
       <c r="I10" s="1" t="n">
-        <v>44752</v>
+        <v>44893</v>
       </c>
       <c r="J10" t="inlineStr">
         <is>
-          <t>HHHDFD</t>
+          <t>нет данных</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>BEL-518</t>
+          <t>Бел-200</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>315/80R22.5</t>
+          <t>21.00R35</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>сер груз</t>
+          <t>202B сер LS-2 Type</t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>315/80R22.5</t>
+          <t>24.00R35</t>
         </is>
       </c>
       <c r="F11" t="inlineStr">
         <is>
-          <t>BEL-498</t>
+          <t>Бел-212</t>
         </is>
       </c>
       <c r="G11" t="inlineStr">
         <is>
-          <t>156L, сер, груз</t>
+          <t>груз, сер, Type, H</t>
         </is>
       </c>
       <c r="H11" t="n">
-        <v>247</v>
+        <v>2</v>
       </c>
       <c r="I11" s="1" t="n">
-        <v>44752</v>
+        <v>44893</v>
       </c>
       <c r="J11" t="inlineStr">
         <is>
@@ -905,82 +905,82 @@
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>ИД-304М</t>
+          <t>Бел-200</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>12.00R20</t>
+          <t>21.00R35</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>16 сер груз</t>
+          <t>202B сер Type H</t>
         </is>
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>315/80R22.5</t>
+          <t>24.00R35</t>
         </is>
       </c>
       <c r="F12" t="inlineStr">
         <is>
-          <t>BEL-518</t>
+          <t>Бел-212</t>
         </is>
       </c>
       <c r="G12" t="inlineStr">
         <is>
-          <t>сер, груз</t>
+          <t>груз, сер, Type, C</t>
         </is>
       </c>
       <c r="H12" t="n">
-        <v>255</v>
+        <v>2</v>
       </c>
       <c r="I12" s="1" t="n">
-        <v>44752</v>
+        <v>44893</v>
       </c>
       <c r="J12" t="inlineStr">
         <is>
-          <t>HHHDFD</t>
+          <t>нет данных</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>ИД-304М</t>
+          <t>Бел-200</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>12.00R20</t>
+          <t>21.00R35</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>18 сер груз</t>
+          <t>202B сер Type C</t>
         </is>
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>12.00R20</t>
+          <t>21.00R35</t>
         </is>
       </c>
       <c r="F13" t="inlineStr">
         <is>
-          <t>ИД-304М</t>
+          <t>Бел-200</t>
         </is>
       </c>
       <c r="G13" t="inlineStr">
         <is>
-          <t>16, сер, груз</t>
+          <t>202B, сер, LS-2, Type</t>
         </is>
       </c>
       <c r="H13" t="n">
-        <v>1555</v>
+        <v>2</v>
       </c>
       <c r="I13" s="1" t="n">
-        <v>44752</v>
+        <v>44893</v>
       </c>
       <c r="J13" t="inlineStr">
         <is>
@@ -991,168 +991,168 @@
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>ИД-304М</t>
+          <t>Бел-210</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>12.00R20</t>
+          <t>21.00R35</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>16 трп груз</t>
+          <t>202B сер LS-2 Type</t>
         </is>
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>12.00R20</t>
+          <t>21.00R35</t>
         </is>
       </c>
       <c r="F14" t="inlineStr">
         <is>
-          <t>ИД-304М</t>
+          <t>Бел-200</t>
         </is>
       </c>
       <c r="G14" t="inlineStr">
         <is>
-          <t>18, сер, груз</t>
+          <t>202B, сер, Type, H</t>
         </is>
       </c>
       <c r="H14" t="n">
-        <v>285</v>
+        <v>2</v>
       </c>
       <c r="I14" s="1" t="n">
-        <v>44752</v>
+        <v>44893</v>
       </c>
       <c r="J14" t="inlineStr">
         <is>
-          <t>HHHDFD</t>
+          <t>нет данных</t>
         </is>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>ИД-304М</t>
+          <t>Бел-210</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>12.00R20</t>
+          <t>21.00R35</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>18 трп груз</t>
+          <t>202B сер Type H</t>
         </is>
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t>12.00R20</t>
+          <t>21.00R35</t>
         </is>
       </c>
       <c r="F15" t="inlineStr">
         <is>
-          <t>ИД-304М</t>
+          <t>Бел-200</t>
         </is>
       </c>
       <c r="G15" t="inlineStr">
         <is>
-          <t>16, трп, груз</t>
+          <t>202B, сер, Type, C</t>
         </is>
       </c>
       <c r="H15" t="n">
-        <v>290</v>
+        <v>2</v>
       </c>
       <c r="I15" s="1" t="n">
-        <v>44752</v>
+        <v>44893</v>
       </c>
       <c r="J15" t="inlineStr">
         <is>
-          <t>БНХ УКР</t>
+          <t>нет данных</t>
         </is>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>БИ-368М</t>
+          <t>Бел-210</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>12.00R20</t>
+          <t>21.00R35</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>18 сер груз</t>
+          <t>202B сер Type C</t>
         </is>
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>12.00R20</t>
+          <t>21.00R35</t>
         </is>
       </c>
       <c r="F16" t="inlineStr">
         <is>
-          <t>ИД-304М</t>
+          <t>Бел-210</t>
         </is>
       </c>
       <c r="G16" t="inlineStr">
         <is>
-          <t>18, трп, груз</t>
+          <t>202B, сер, LS-2, Type</t>
         </is>
       </c>
       <c r="H16" t="n">
-        <v>296</v>
+        <v>2</v>
       </c>
       <c r="I16" s="1" t="n">
-        <v>44752</v>
+        <v>44893</v>
       </c>
       <c r="J16" t="inlineStr">
         <is>
-          <t>БНХ УКР</t>
+          <t>нет данных</t>
         </is>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>БИ-368М</t>
+          <t>BEL-248</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>12.00R20</t>
+          <t>14.00R20</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>18 сер груз</t>
+          <t>груз сер</t>
         </is>
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>12.00R20</t>
+          <t>21.00R35</t>
         </is>
       </c>
       <c r="F17" t="inlineStr">
         <is>
-          <t>БИ-368М</t>
+          <t>Бел-210</t>
         </is>
       </c>
       <c r="G17" t="inlineStr">
         <is>
-          <t>18, сер, груз</t>
+          <t>202B, сер, Type, H</t>
         </is>
       </c>
       <c r="H17" t="n">
-        <v>4565</v>
+        <v>2</v>
       </c>
       <c r="I17" s="1" t="n">
-        <v>44752</v>
+        <v>44893</v>
       </c>
       <c r="J17" t="inlineStr">
         <is>
@@ -1163,39 +1163,39 @@
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>БИ-368М</t>
+          <t>BEL-248</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>12.00R20</t>
+          <t>14.00R20</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>18 трп груз</t>
+          <t>б/к груз сер</t>
         </is>
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t>12.00R20</t>
+          <t>21.00R35</t>
         </is>
       </c>
       <c r="F18" t="inlineStr">
         <is>
-          <t>БИ-368М</t>
+          <t>Бел-210</t>
         </is>
       </c>
       <c r="G18" t="inlineStr">
         <is>
-          <t>18, сер, груз</t>
+          <t>202B, сер, Type, C</t>
         </is>
       </c>
       <c r="H18" t="n">
-        <v>4565</v>
+        <v>2</v>
       </c>
       <c r="I18" s="1" t="n">
-        <v>44752</v>
+        <v>44893</v>
       </c>
       <c r="J18" t="inlineStr">
         <is>
@@ -1206,151 +1206,211 @@
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>BEL-337</t>
+          <t>BEL-248</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>195/65R15</t>
+          <t>14.00R20</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>легк б/к сер</t>
+          <t>груз сер</t>
         </is>
       </c>
       <c r="E19" t="inlineStr">
         <is>
+          <t>14.00R20</t>
+        </is>
+      </c>
+      <c r="F19" t="inlineStr">
+        <is>
+          <t>BEL-248</t>
+        </is>
+      </c>
+      <c r="G19" t="inlineStr">
+        <is>
+          <t>груз, сер</t>
+        </is>
+      </c>
+      <c r="H19" t="n">
+        <v>2</v>
+      </c>
+      <c r="I19" s="1" t="n">
+        <v>44893</v>
+      </c>
+      <c r="J19" t="inlineStr">
+        <is>
+          <t>нет данных</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>BEL-248</t>
+        </is>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>14.00R20</t>
+        </is>
+      </c>
+      <c r="C20" t="inlineStr">
+        <is>
+          <t>груз сер</t>
+        </is>
+      </c>
+      <c r="E20" t="inlineStr">
+        <is>
+          <t>14.00R20</t>
+        </is>
+      </c>
+      <c r="F20" t="inlineStr">
+        <is>
+          <t>BEL-248</t>
+        </is>
+      </c>
+      <c r="G20" t="inlineStr">
+        <is>
+          <t>груз, сер</t>
+        </is>
+      </c>
+      <c r="H20" t="n">
+        <v>2</v>
+      </c>
+      <c r="I20" s="1" t="n">
+        <v>44893</v>
+      </c>
+      <c r="J20" t="inlineStr">
+        <is>
+          <t>нет данных</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>BEL-288</t>
+        </is>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
           <t>12.00R20</t>
         </is>
       </c>
-      <c r="F19" t="inlineStr">
-        <is>
-          <t>БИ-368М</t>
-        </is>
-      </c>
-      <c r="G19" t="inlineStr">
-        <is>
-          <t>18, сер, груз</t>
-        </is>
-      </c>
-      <c r="H19" t="n">
-        <v>283</v>
-      </c>
-      <c r="I19" s="1" t="n">
-        <v>44752</v>
-      </c>
-      <c r="J19" t="inlineStr">
-        <is>
-          <t>нет данных</t>
-        </is>
-      </c>
-    </row>
-    <row r="20">
-      <c r="E20" t="inlineStr">
+      <c r="C21" t="inlineStr">
+        <is>
+          <t>груз сер</t>
+        </is>
+      </c>
+      <c r="E21" t="inlineStr">
+        <is>
+          <t>14.00R20</t>
+        </is>
+      </c>
+      <c r="F21" t="inlineStr">
+        <is>
+          <t>BEL-248</t>
+        </is>
+      </c>
+      <c r="G21" t="inlineStr">
+        <is>
+          <t>б/к, груз, сер</t>
+        </is>
+      </c>
+      <c r="H21" t="n">
+        <v>2</v>
+      </c>
+      <c r="I21" s="1" t="n">
+        <v>44893</v>
+      </c>
+      <c r="J21" t="inlineStr">
+        <is>
+          <t>нет данных</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>Бел-95</t>
+        </is>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>16.00R20</t>
+        </is>
+      </c>
+      <c r="C22" t="inlineStr">
+        <is>
+          <t>173G б/к груз сер</t>
+        </is>
+      </c>
+      <c r="E22" t="inlineStr">
+        <is>
+          <t>14.00R20</t>
+        </is>
+      </c>
+      <c r="F22" t="inlineStr">
+        <is>
+          <t>BEL-248</t>
+        </is>
+      </c>
+      <c r="G22" t="inlineStr">
+        <is>
+          <t>груз, сер</t>
+        </is>
+      </c>
+      <c r="H22" t="n">
+        <v>2</v>
+      </c>
+      <c r="I22" s="1" t="n">
+        <v>44893</v>
+      </c>
+      <c r="J22" t="inlineStr">
+        <is>
+          <t>нет данных</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>Бел-95</t>
+        </is>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>16.00R20</t>
+        </is>
+      </c>
+      <c r="C23" t="inlineStr">
+        <is>
+          <t>173G груз сер</t>
+        </is>
+      </c>
+      <c r="E23" t="inlineStr">
         <is>
           <t>12.00R20</t>
         </is>
       </c>
-      <c r="F20" t="inlineStr">
-        <is>
-          <t>БИ-368М</t>
-        </is>
-      </c>
-      <c r="G20" t="inlineStr">
-        <is>
-          <t>18, сер, груз</t>
-        </is>
-      </c>
-      <c r="H20" t="n">
-        <v>283</v>
-      </c>
-      <c r="I20" s="1" t="n">
-        <v>44752</v>
-      </c>
-      <c r="J20" t="inlineStr">
-        <is>
-          <t>нет данных</t>
-        </is>
-      </c>
-    </row>
-    <row r="21">
-      <c r="E21" t="inlineStr">
-        <is>
-          <t>12.00R20</t>
-        </is>
-      </c>
-      <c r="F21" t="inlineStr">
-        <is>
-          <t>БИ-368М</t>
-        </is>
-      </c>
-      <c r="G21" t="inlineStr">
-        <is>
-          <t>18, трп, груз</t>
-        </is>
-      </c>
-      <c r="H21" t="n">
-        <v>291</v>
-      </c>
-      <c r="I21" s="1" t="n">
-        <v>44752</v>
-      </c>
-      <c r="J21" t="inlineStr">
-        <is>
-          <t>БНХ УКР</t>
-        </is>
-      </c>
-    </row>
-    <row r="22">
-      <c r="E22" t="inlineStr">
-        <is>
-          <t>195/65R15</t>
-        </is>
-      </c>
-      <c r="F22" t="inlineStr">
-        <is>
-          <t>BEL-337</t>
-        </is>
-      </c>
-      <c r="G22" t="inlineStr">
-        <is>
-          <t>легк, б/к, сер</t>
-        </is>
-      </c>
-      <c r="H22" t="n">
-        <v>291</v>
-      </c>
-      <c r="I22" s="1" t="n">
-        <v>44752</v>
-      </c>
-      <c r="J22" t="inlineStr">
-        <is>
-          <t>БНХ УКР</t>
-        </is>
-      </c>
-    </row>
-    <row r="23">
-      <c r="E23" t="inlineStr">
-        <is>
-          <t>315/80R22.5</t>
-        </is>
-      </c>
       <c r="F23" t="inlineStr">
         <is>
-          <t>BEL-158M</t>
+          <t>BEL-288</t>
         </is>
       </c>
       <c r="G23" t="inlineStr">
         <is>
-          <t>камневыт, сер, груз</t>
+          <t>груз, сер</t>
         </is>
       </c>
       <c r="H23" t="n">
         <v>2</v>
       </c>
       <c r="I23" s="1" t="n">
-        <v>44863</v>
+        <v>44893</v>
       </c>
       <c r="J23" t="inlineStr">
         <is>
@@ -1359,26 +1419,41 @@
       </c>
     </row>
     <row r="24">
+      <c r="A24" t="inlineStr">
+        <is>
+          <t>Бел-95</t>
+        </is>
+      </c>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>16.00R20</t>
+        </is>
+      </c>
+      <c r="C24" t="inlineStr">
+        <is>
+          <t>173G груз сер</t>
+        </is>
+      </c>
       <c r="E24" t="inlineStr">
         <is>
-          <t>315/80R22.5</t>
+          <t>16.00R20</t>
         </is>
       </c>
       <c r="F24" t="inlineStr">
         <is>
-          <t>BEL-278</t>
+          <t>Бел-95</t>
         </is>
       </c>
       <c r="G24" t="inlineStr">
         <is>
-          <t>сер, груз</t>
+          <t>173G, б/к, груз, сер</t>
         </is>
       </c>
       <c r="H24" t="n">
         <v>2</v>
       </c>
       <c r="I24" s="1" t="n">
-        <v>44863</v>
+        <v>44893</v>
       </c>
       <c r="J24" t="inlineStr">
         <is>
@@ -1387,26 +1462,41 @@
       </c>
     </row>
     <row r="25">
+      <c r="A25" t="inlineStr">
+        <is>
+          <t>Бел-95</t>
+        </is>
+      </c>
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>16.00R20</t>
+        </is>
+      </c>
+      <c r="C25" t="inlineStr">
+        <is>
+          <t>173G груз сер</t>
+        </is>
+      </c>
       <c r="E25" t="inlineStr">
         <is>
-          <t>315/80R22.5</t>
+          <t>16.00R20</t>
         </is>
       </c>
       <c r="F25" t="inlineStr">
         <is>
-          <t>BEL-268</t>
+          <t>Бел-95</t>
         </is>
       </c>
       <c r="G25" t="inlineStr">
         <is>
-          <t>сер, груз</t>
+          <t>173G, груз, сер</t>
         </is>
       </c>
       <c r="H25" t="n">
         <v>2</v>
       </c>
       <c r="I25" s="1" t="n">
-        <v>44863</v>
+        <v>44893</v>
       </c>
       <c r="J25" t="inlineStr">
         <is>
@@ -1415,26 +1505,41 @@
       </c>
     </row>
     <row r="26">
+      <c r="A26" t="inlineStr">
+        <is>
+          <t>Бел-95</t>
+        </is>
+      </c>
+      <c r="B26" t="inlineStr">
+        <is>
+          <t>16.00R20</t>
+        </is>
+      </c>
+      <c r="C26" t="inlineStr">
+        <is>
+          <t>173G груз сер</t>
+        </is>
+      </c>
       <c r="E26" t="inlineStr">
         <is>
-          <t>315/80R22.5</t>
+          <t>16.00R20</t>
         </is>
       </c>
       <c r="F26" t="inlineStr">
         <is>
-          <t>BEL-398</t>
+          <t>Бел-95</t>
         </is>
       </c>
       <c r="G26" t="inlineStr">
         <is>
-          <t>сер, груз</t>
+          <t>173G, груз, сер</t>
         </is>
       </c>
       <c r="H26" t="n">
         <v>2</v>
       </c>
       <c r="I26" s="1" t="n">
-        <v>44863</v>
+        <v>44893</v>
       </c>
       <c r="J26" t="inlineStr">
         <is>
@@ -1443,26 +1548,41 @@
       </c>
     </row>
     <row r="27">
+      <c r="A27" t="inlineStr">
+        <is>
+          <t>Бел-95</t>
+        </is>
+      </c>
+      <c r="B27" t="inlineStr">
+        <is>
+          <t>16.00R20</t>
+        </is>
+      </c>
+      <c r="C27" t="inlineStr">
+        <is>
+          <t>173G груз сер</t>
+        </is>
+      </c>
       <c r="E27" t="inlineStr">
         <is>
-          <t>315/80R22.5</t>
+          <t>16.00R20</t>
         </is>
       </c>
       <c r="F27" t="inlineStr">
         <is>
-          <t>BEL-326</t>
+          <t>Бел-95</t>
         </is>
       </c>
       <c r="G27" t="inlineStr">
         <is>
-          <t>сер, груз</t>
+          <t>173G, груз, сер</t>
         </is>
       </c>
       <c r="H27" t="n">
         <v>2</v>
       </c>
       <c r="I27" s="1" t="n">
-        <v>44863</v>
+        <v>44893</v>
       </c>
       <c r="J27" t="inlineStr">
         <is>
@@ -1471,26 +1591,41 @@
       </c>
     </row>
     <row r="28">
+      <c r="A28" t="inlineStr">
+        <is>
+          <t>Бел-95</t>
+        </is>
+      </c>
+      <c r="B28" t="inlineStr">
+        <is>
+          <t>16.00R20</t>
+        </is>
+      </c>
+      <c r="C28" t="inlineStr">
+        <is>
+          <t>173G сер</t>
+        </is>
+      </c>
       <c r="E28" t="inlineStr">
         <is>
-          <t>315/80R22.5</t>
+          <t>16.00R20</t>
         </is>
       </c>
       <c r="F28" t="inlineStr">
         <is>
-          <t>BEL-498</t>
+          <t>Бел-95</t>
         </is>
       </c>
       <c r="G28" t="inlineStr">
         <is>
-          <t>156L, сер, груз</t>
+          <t>173G, груз, сер</t>
         </is>
       </c>
       <c r="H28" t="n">
         <v>2</v>
       </c>
       <c r="I28" s="1" t="n">
-        <v>44863</v>
+        <v>44893</v>
       </c>
       <c r="J28" t="inlineStr">
         <is>
@@ -1499,26 +1634,41 @@
       </c>
     </row>
     <row r="29">
+      <c r="A29" t="inlineStr">
+        <is>
+          <t>BEL-405</t>
+        </is>
+      </c>
+      <c r="B29" t="inlineStr">
+        <is>
+          <t>395/85R20</t>
+        </is>
+      </c>
+      <c r="C29" t="inlineStr">
+        <is>
+          <t>168J груз сер</t>
+        </is>
+      </c>
       <c r="E29" t="inlineStr">
         <is>
-          <t>12.00R20</t>
+          <t>16.00R20</t>
         </is>
       </c>
       <c r="F29" t="inlineStr">
         <is>
-          <t>ИД-304М</t>
+          <t>Бел-95</t>
         </is>
       </c>
       <c r="G29" t="inlineStr">
         <is>
-          <t>16, сер, груз</t>
+          <t>173G, груз, сер</t>
         </is>
       </c>
       <c r="H29" t="n">
         <v>2</v>
       </c>
       <c r="I29" s="1" t="n">
-        <v>44863</v>
+        <v>44893</v>
       </c>
       <c r="J29" t="inlineStr">
         <is>
@@ -1527,26 +1677,41 @@
       </c>
     </row>
     <row r="30">
+      <c r="A30" t="inlineStr">
+        <is>
+          <t>Бел-145</t>
+        </is>
+      </c>
+      <c r="B30" t="inlineStr">
+        <is>
+          <t>445/65R22.5</t>
+        </is>
+      </c>
+      <c r="C30" t="inlineStr">
+        <is>
+          <t>б/к груз сер</t>
+        </is>
+      </c>
       <c r="E30" t="inlineStr">
         <is>
-          <t>12.00R20</t>
+          <t>16.00R20</t>
         </is>
       </c>
       <c r="F30" t="inlineStr">
         <is>
-          <t>ИД-304М</t>
+          <t>Бел-95</t>
         </is>
       </c>
       <c r="G30" t="inlineStr">
         <is>
-          <t>18, сер, груз</t>
+          <t>173G, сер</t>
         </is>
       </c>
       <c r="H30" t="n">
         <v>2</v>
       </c>
       <c r="I30" s="1" t="n">
-        <v>44863</v>
+        <v>44893</v>
       </c>
       <c r="J30" t="inlineStr">
         <is>
@@ -1555,26 +1720,41 @@
       </c>
     </row>
     <row r="31">
+      <c r="A31" t="inlineStr">
+        <is>
+          <t>Бел-230</t>
+        </is>
+      </c>
+      <c r="B31" t="inlineStr">
+        <is>
+          <t>355/65-15</t>
+        </is>
+      </c>
+      <c r="C31" t="inlineStr">
+        <is>
+          <t>сер</t>
+        </is>
+      </c>
       <c r="E31" t="inlineStr">
         <is>
-          <t>12.00R20</t>
+          <t>395/85R20</t>
         </is>
       </c>
       <c r="F31" t="inlineStr">
         <is>
-          <t>БИ-368М</t>
+          <t>BEL-405</t>
         </is>
       </c>
       <c r="G31" t="inlineStr">
         <is>
-          <t>18, сер, груз</t>
+          <t>168J, груз, сер</t>
         </is>
       </c>
       <c r="H31" t="n">
         <v>2</v>
       </c>
       <c r="I31" s="1" t="n">
-        <v>44863</v>
+        <v>44893</v>
       </c>
       <c r="J31" t="inlineStr">
         <is>
@@ -1583,26 +1763,41 @@
       </c>
     </row>
     <row r="32">
+      <c r="A32" t="inlineStr">
+        <is>
+          <t>Бел-230М</t>
+        </is>
+      </c>
+      <c r="B32" t="inlineStr">
+        <is>
+          <t>355/65-15</t>
+        </is>
+      </c>
+      <c r="C32" t="inlineStr">
+        <is>
+          <t>сер</t>
+        </is>
+      </c>
       <c r="E32" t="inlineStr">
         <is>
-          <t>12.00R20</t>
+          <t>445/65R22.5</t>
         </is>
       </c>
       <c r="F32" t="inlineStr">
         <is>
-          <t>БИ-368М</t>
+          <t>Бел-145</t>
         </is>
       </c>
       <c r="G32" t="inlineStr">
         <is>
-          <t>18, сер, груз</t>
+          <t>б/к, груз, сер</t>
         </is>
       </c>
       <c r="H32" t="n">
         <v>2</v>
       </c>
       <c r="I32" s="1" t="n">
-        <v>44863</v>
+        <v>44893</v>
       </c>
       <c r="J32" t="inlineStr">
         <is>
@@ -1611,26 +1806,41 @@
       </c>
     </row>
     <row r="33">
+      <c r="A33" t="inlineStr">
+        <is>
+          <t>BEL-262</t>
+        </is>
+      </c>
+      <c r="B33" t="inlineStr">
+        <is>
+          <t>205/55R16</t>
+        </is>
+      </c>
+      <c r="C33" t="inlineStr">
+        <is>
+          <t>б/к сер легк</t>
+        </is>
+      </c>
       <c r="E33" t="inlineStr">
         <is>
-          <t>195/65R15</t>
+          <t>355/65-15</t>
         </is>
       </c>
       <c r="F33" t="inlineStr">
         <is>
-          <t>BEL-337</t>
+          <t>Бел-230</t>
         </is>
       </c>
       <c r="G33" t="inlineStr">
         <is>
-          <t>легк, б/к, сер</t>
+          <t>сер</t>
         </is>
       </c>
       <c r="H33" t="n">
         <v>2</v>
       </c>
       <c r="I33" s="1" t="n">
-        <v>44863</v>
+        <v>44893</v>
       </c>
       <c r="J33" t="inlineStr">
         <is>
@@ -1639,26 +1849,41 @@
       </c>
     </row>
     <row r="34">
+      <c r="A34" t="inlineStr">
+        <is>
+          <t>BEL-317</t>
+        </is>
+      </c>
+      <c r="B34" t="inlineStr">
+        <is>
+          <t>205/55R16</t>
+        </is>
+      </c>
+      <c r="C34" t="inlineStr">
+        <is>
+          <t>б/к сер легк</t>
+        </is>
+      </c>
       <c r="E34" t="inlineStr">
         <is>
-          <t>315/80R22.5</t>
+          <t>355/65-15</t>
         </is>
       </c>
       <c r="F34" t="inlineStr">
         <is>
-          <t>BEL-158M</t>
+          <t>Бел-230М</t>
         </is>
       </c>
       <c r="G34" t="inlineStr">
         <is>
-          <t>камневыт, сер, груз</t>
+          <t>сер</t>
         </is>
       </c>
       <c r="H34" t="n">
         <v>2</v>
       </c>
       <c r="I34" s="1" t="n">
-        <v>44864</v>
+        <v>44893</v>
       </c>
       <c r="J34" t="inlineStr">
         <is>
@@ -1667,26 +1892,41 @@
       </c>
     </row>
     <row r="35">
+      <c r="A35" t="inlineStr">
+        <is>
+          <t>BEL-317S</t>
+        </is>
+      </c>
+      <c r="B35" t="inlineStr">
+        <is>
+          <t>205/55R16</t>
+        </is>
+      </c>
+      <c r="C35" t="inlineStr">
+        <is>
+          <t>сер ошип</t>
+        </is>
+      </c>
       <c r="E35" t="inlineStr">
         <is>
-          <t>315/80R22.5</t>
+          <t>205/55R16</t>
         </is>
       </c>
       <c r="F35" t="inlineStr">
         <is>
-          <t>BEL-278</t>
+          <t>BEL-262</t>
         </is>
       </c>
       <c r="G35" t="inlineStr">
         <is>
-          <t>сер, груз</t>
+          <t>б/к, сер, легк</t>
         </is>
       </c>
       <c r="H35" t="n">
         <v>2</v>
       </c>
       <c r="I35" s="1" t="n">
-        <v>44864</v>
+        <v>44893</v>
       </c>
       <c r="J35" t="inlineStr">
         <is>
@@ -1695,26 +1935,41 @@
       </c>
     </row>
     <row r="36">
+      <c r="A36" t="inlineStr">
+        <is>
+          <t>BEL-277</t>
+        </is>
+      </c>
+      <c r="B36" t="inlineStr">
+        <is>
+          <t>205/60R16</t>
+        </is>
+      </c>
+      <c r="C36" t="inlineStr">
+        <is>
+          <t>б/к сер легк</t>
+        </is>
+      </c>
       <c r="E36" t="inlineStr">
         <is>
-          <t>315/80R22.5</t>
+          <t>205/55R16</t>
         </is>
       </c>
       <c r="F36" t="inlineStr">
         <is>
-          <t>BEL-268</t>
+          <t>BEL-317</t>
         </is>
       </c>
       <c r="G36" t="inlineStr">
         <is>
-          <t>сер, груз</t>
+          <t>б/к, сер, легк</t>
         </is>
       </c>
       <c r="H36" t="n">
         <v>2</v>
       </c>
       <c r="I36" s="1" t="n">
-        <v>44864</v>
+        <v>44893</v>
       </c>
       <c r="J36" t="inlineStr">
         <is>
@@ -1725,24 +1980,24 @@
     <row r="37">
       <c r="E37" t="inlineStr">
         <is>
-          <t>315/80R22.5</t>
+          <t>205/55R16</t>
         </is>
       </c>
       <c r="F37" t="inlineStr">
         <is>
-          <t>BEL-398</t>
+          <t>BEL-317S</t>
         </is>
       </c>
       <c r="G37" t="inlineStr">
         <is>
-          <t>сер, груз</t>
+          <t>сер, ошип</t>
         </is>
       </c>
       <c r="H37" t="n">
         <v>2</v>
       </c>
       <c r="I37" s="1" t="n">
-        <v>44864</v>
+        <v>44893</v>
       </c>
       <c r="J37" t="inlineStr">
         <is>
@@ -1753,24 +2008,24 @@
     <row r="38">
       <c r="E38" t="inlineStr">
         <is>
-          <t>315/80R22.5</t>
+          <t>205/60R16</t>
         </is>
       </c>
       <c r="F38" t="inlineStr">
         <is>
-          <t>BEL-326</t>
+          <t>BEL-277</t>
         </is>
       </c>
       <c r="G38" t="inlineStr">
         <is>
-          <t>сер, груз</t>
+          <t>б/к, сер, легк</t>
         </is>
       </c>
       <c r="H38" t="n">
         <v>2</v>
       </c>
       <c r="I38" s="1" t="n">
-        <v>44864</v>
+        <v>44893</v>
       </c>
       <c r="J38" t="inlineStr">
         <is>
@@ -1781,24 +2036,24 @@
     <row r="39">
       <c r="E39" t="inlineStr">
         <is>
-          <t>315/80R22.5</t>
+          <t>35/65-33</t>
         </is>
       </c>
       <c r="F39" t="inlineStr">
         <is>
-          <t>BEL-498</t>
+          <t>ФБел-283</t>
         </is>
       </c>
       <c r="G39" t="inlineStr">
         <is>
-          <t>156L, сер, груз</t>
+          <t>42, груз, сер</t>
         </is>
       </c>
       <c r="H39" t="n">
         <v>2</v>
       </c>
       <c r="I39" s="1" t="n">
-        <v>44864</v>
+        <v>44894</v>
       </c>
       <c r="J39" t="inlineStr">
         <is>
@@ -1809,24 +2064,24 @@
     <row r="40">
       <c r="E40" t="inlineStr">
         <is>
-          <t>12.00R20</t>
+          <t>24.00R35</t>
         </is>
       </c>
       <c r="F40" t="inlineStr">
         <is>
-          <t>ИД-304М</t>
+          <t>Бел-122</t>
         </is>
       </c>
       <c r="G40" t="inlineStr">
         <is>
-          <t>16, сер, груз</t>
+          <t>груз, сер, LS-2, Type</t>
         </is>
       </c>
       <c r="H40" t="n">
         <v>2</v>
       </c>
       <c r="I40" s="1" t="n">
-        <v>44864</v>
+        <v>44894</v>
       </c>
       <c r="J40" t="inlineStr">
         <is>
@@ -1837,24 +2092,24 @@
     <row r="41">
       <c r="E41" t="inlineStr">
         <is>
-          <t>12.00R20</t>
+          <t>24.00R35</t>
         </is>
       </c>
       <c r="F41" t="inlineStr">
         <is>
-          <t>ИД-304М</t>
+          <t>Бел-122</t>
         </is>
       </c>
       <c r="G41" t="inlineStr">
         <is>
-          <t>18, сер, груз</t>
+          <t>груз, сер, Type, H</t>
         </is>
       </c>
       <c r="H41" t="n">
         <v>2</v>
       </c>
       <c r="I41" s="1" t="n">
-        <v>44864</v>
+        <v>44894</v>
       </c>
       <c r="J41" t="inlineStr">
         <is>
@@ -1865,24 +2120,24 @@
     <row r="42">
       <c r="E42" t="inlineStr">
         <is>
-          <t>12.00R20</t>
+          <t>24.00R35</t>
         </is>
       </c>
       <c r="F42" t="inlineStr">
         <is>
-          <t>БИ-368М</t>
+          <t>Бел-122</t>
         </is>
       </c>
       <c r="G42" t="inlineStr">
         <is>
-          <t>18, сер, груз</t>
+          <t>груз, сер, Type, C</t>
         </is>
       </c>
       <c r="H42" t="n">
         <v>2</v>
       </c>
       <c r="I42" s="1" t="n">
-        <v>44864</v>
+        <v>44894</v>
       </c>
       <c r="J42" t="inlineStr">
         <is>
@@ -1893,24 +2148,24 @@
     <row r="43">
       <c r="E43" t="inlineStr">
         <is>
-          <t>12.00R20</t>
+          <t>24.00R35</t>
         </is>
       </c>
       <c r="F43" t="inlineStr">
         <is>
-          <t>БИ-368М</t>
+          <t>Бел-202</t>
         </is>
       </c>
       <c r="G43" t="inlineStr">
         <is>
-          <t>18, сер, груз</t>
+          <t>210B, сер, LS-2, Type</t>
         </is>
       </c>
       <c r="H43" t="n">
         <v>2</v>
       </c>
       <c r="I43" s="1" t="n">
-        <v>44864</v>
+        <v>44894</v>
       </c>
       <c r="J43" t="inlineStr">
         <is>
@@ -1921,26 +2176,2882 @@
     <row r="44">
       <c r="E44" t="inlineStr">
         <is>
-          <t>195/65R15</t>
+          <t>24.00R35</t>
         </is>
       </c>
       <c r="F44" t="inlineStr">
         <is>
-          <t>BEL-337</t>
+          <t>Бел-202</t>
         </is>
       </c>
       <c r="G44" t="inlineStr">
         <is>
-          <t>легк, б/к, сер</t>
+          <t>210B, сер, Type, H</t>
         </is>
       </c>
       <c r="H44" t="n">
         <v>2</v>
       </c>
       <c r="I44" s="1" t="n">
-        <v>44864</v>
+        <v>44894</v>
       </c>
       <c r="J44" t="inlineStr">
+        <is>
+          <t>нет данных</t>
+        </is>
+      </c>
+    </row>
+    <row r="45">
+      <c r="E45" t="inlineStr">
+        <is>
+          <t>24.00R35</t>
+        </is>
+      </c>
+      <c r="F45" t="inlineStr">
+        <is>
+          <t>Бел-202</t>
+        </is>
+      </c>
+      <c r="G45" t="inlineStr">
+        <is>
+          <t>210B, сер, Type, C</t>
+        </is>
+      </c>
+      <c r="H45" t="n">
+        <v>2</v>
+      </c>
+      <c r="I45" s="1" t="n">
+        <v>44894</v>
+      </c>
+      <c r="J45" t="inlineStr">
+        <is>
+          <t>нет данных</t>
+        </is>
+      </c>
+    </row>
+    <row r="46">
+      <c r="E46" t="inlineStr">
+        <is>
+          <t>24.00R35</t>
+        </is>
+      </c>
+      <c r="F46" t="inlineStr">
+        <is>
+          <t>Бел-212</t>
+        </is>
+      </c>
+      <c r="G46" t="inlineStr">
+        <is>
+          <t>груз, сер, LS-2, Type</t>
+        </is>
+      </c>
+      <c r="H46" t="n">
+        <v>2</v>
+      </c>
+      <c r="I46" s="1" t="n">
+        <v>44894</v>
+      </c>
+      <c r="J46" t="inlineStr">
+        <is>
+          <t>нет данных</t>
+        </is>
+      </c>
+    </row>
+    <row r="47">
+      <c r="E47" t="inlineStr">
+        <is>
+          <t>24.00R35</t>
+        </is>
+      </c>
+      <c r="F47" t="inlineStr">
+        <is>
+          <t>Бел-212</t>
+        </is>
+      </c>
+      <c r="G47" t="inlineStr">
+        <is>
+          <t>груз, сер, Type, H</t>
+        </is>
+      </c>
+      <c r="H47" t="n">
+        <v>2</v>
+      </c>
+      <c r="I47" s="1" t="n">
+        <v>44894</v>
+      </c>
+      <c r="J47" t="inlineStr">
+        <is>
+          <t>нет данных</t>
+        </is>
+      </c>
+    </row>
+    <row r="48">
+      <c r="E48" t="inlineStr">
+        <is>
+          <t>24.00R35</t>
+        </is>
+      </c>
+      <c r="F48" t="inlineStr">
+        <is>
+          <t>Бел-212</t>
+        </is>
+      </c>
+      <c r="G48" t="inlineStr">
+        <is>
+          <t>груз, сер, Type, C</t>
+        </is>
+      </c>
+      <c r="H48" t="n">
+        <v>2</v>
+      </c>
+      <c r="I48" s="1" t="n">
+        <v>44894</v>
+      </c>
+      <c r="J48" t="inlineStr">
+        <is>
+          <t>нет данных</t>
+        </is>
+      </c>
+    </row>
+    <row r="49">
+      <c r="E49" t="inlineStr">
+        <is>
+          <t>21.00R35</t>
+        </is>
+      </c>
+      <c r="F49" t="inlineStr">
+        <is>
+          <t>Бел-200</t>
+        </is>
+      </c>
+      <c r="G49" t="inlineStr">
+        <is>
+          <t>202B, сер, LS-2, Type</t>
+        </is>
+      </c>
+      <c r="H49" t="n">
+        <v>2</v>
+      </c>
+      <c r="I49" s="1" t="n">
+        <v>44894</v>
+      </c>
+      <c r="J49" t="inlineStr">
+        <is>
+          <t>нет данных</t>
+        </is>
+      </c>
+    </row>
+    <row r="50">
+      <c r="E50" t="inlineStr">
+        <is>
+          <t>21.00R35</t>
+        </is>
+      </c>
+      <c r="F50" t="inlineStr">
+        <is>
+          <t>Бел-200</t>
+        </is>
+      </c>
+      <c r="G50" t="inlineStr">
+        <is>
+          <t>202B, сер, Type, H</t>
+        </is>
+      </c>
+      <c r="H50" t="n">
+        <v>2</v>
+      </c>
+      <c r="I50" s="1" t="n">
+        <v>44894</v>
+      </c>
+      <c r="J50" t="inlineStr">
+        <is>
+          <t>нет данных</t>
+        </is>
+      </c>
+    </row>
+    <row r="51">
+      <c r="E51" t="inlineStr">
+        <is>
+          <t>21.00R35</t>
+        </is>
+      </c>
+      <c r="F51" t="inlineStr">
+        <is>
+          <t>Бел-200</t>
+        </is>
+      </c>
+      <c r="G51" t="inlineStr">
+        <is>
+          <t>202B, сер, Type, C</t>
+        </is>
+      </c>
+      <c r="H51" t="n">
+        <v>2</v>
+      </c>
+      <c r="I51" s="1" t="n">
+        <v>44894</v>
+      </c>
+      <c r="J51" t="inlineStr">
+        <is>
+          <t>нет данных</t>
+        </is>
+      </c>
+    </row>
+    <row r="52">
+      <c r="E52" t="inlineStr">
+        <is>
+          <t>21.00R35</t>
+        </is>
+      </c>
+      <c r="F52" t="inlineStr">
+        <is>
+          <t>Бел-210</t>
+        </is>
+      </c>
+      <c r="G52" t="inlineStr">
+        <is>
+          <t>202B, сер, LS-2, Type</t>
+        </is>
+      </c>
+      <c r="H52" t="n">
+        <v>2</v>
+      </c>
+      <c r="I52" s="1" t="n">
+        <v>44894</v>
+      </c>
+      <c r="J52" t="inlineStr">
+        <is>
+          <t>нет данных</t>
+        </is>
+      </c>
+    </row>
+    <row r="53">
+      <c r="E53" t="inlineStr">
+        <is>
+          <t>21.00R35</t>
+        </is>
+      </c>
+      <c r="F53" t="inlineStr">
+        <is>
+          <t>Бел-210</t>
+        </is>
+      </c>
+      <c r="G53" t="inlineStr">
+        <is>
+          <t>202B, сер, Type, H</t>
+        </is>
+      </c>
+      <c r="H53" t="n">
+        <v>2</v>
+      </c>
+      <c r="I53" s="1" t="n">
+        <v>44894</v>
+      </c>
+      <c r="J53" t="inlineStr">
+        <is>
+          <t>нет данных</t>
+        </is>
+      </c>
+    </row>
+    <row r="54">
+      <c r="E54" t="inlineStr">
+        <is>
+          <t>21.00R35</t>
+        </is>
+      </c>
+      <c r="F54" t="inlineStr">
+        <is>
+          <t>Бел-210</t>
+        </is>
+      </c>
+      <c r="G54" t="inlineStr">
+        <is>
+          <t>202B, сер, Type, C</t>
+        </is>
+      </c>
+      <c r="H54" t="n">
+        <v>2</v>
+      </c>
+      <c r="I54" s="1" t="n">
+        <v>44894</v>
+      </c>
+      <c r="J54" t="inlineStr">
+        <is>
+          <t>нет данных</t>
+        </is>
+      </c>
+    </row>
+    <row r="55">
+      <c r="E55" t="inlineStr">
+        <is>
+          <t>14.00R20</t>
+        </is>
+      </c>
+      <c r="F55" t="inlineStr">
+        <is>
+          <t>BEL-248</t>
+        </is>
+      </c>
+      <c r="G55" t="inlineStr">
+        <is>
+          <t>груз, сер</t>
+        </is>
+      </c>
+      <c r="H55" t="n">
+        <v>2</v>
+      </c>
+      <c r="I55" s="1" t="n">
+        <v>44894</v>
+      </c>
+      <c r="J55" t="inlineStr">
+        <is>
+          <t>нет данных</t>
+        </is>
+      </c>
+    </row>
+    <row r="56">
+      <c r="E56" t="inlineStr">
+        <is>
+          <t>14.00R20</t>
+        </is>
+      </c>
+      <c r="F56" t="inlineStr">
+        <is>
+          <t>BEL-248</t>
+        </is>
+      </c>
+      <c r="G56" t="inlineStr">
+        <is>
+          <t>груз, сер</t>
+        </is>
+      </c>
+      <c r="H56" t="n">
+        <v>2</v>
+      </c>
+      <c r="I56" s="1" t="n">
+        <v>44894</v>
+      </c>
+      <c r="J56" t="inlineStr">
+        <is>
+          <t>нет данных</t>
+        </is>
+      </c>
+    </row>
+    <row r="57">
+      <c r="E57" t="inlineStr">
+        <is>
+          <t>14.00R20</t>
+        </is>
+      </c>
+      <c r="F57" t="inlineStr">
+        <is>
+          <t>BEL-248</t>
+        </is>
+      </c>
+      <c r="G57" t="inlineStr">
+        <is>
+          <t>б/к, груз, сер</t>
+        </is>
+      </c>
+      <c r="H57" t="n">
+        <v>2</v>
+      </c>
+      <c r="I57" s="1" t="n">
+        <v>44894</v>
+      </c>
+      <c r="J57" t="inlineStr">
+        <is>
+          <t>нет данных</t>
+        </is>
+      </c>
+    </row>
+    <row r="58">
+      <c r="E58" t="inlineStr">
+        <is>
+          <t>14.00R20</t>
+        </is>
+      </c>
+      <c r="F58" t="inlineStr">
+        <is>
+          <t>BEL-248</t>
+        </is>
+      </c>
+      <c r="G58" t="inlineStr">
+        <is>
+          <t>груз, сер</t>
+        </is>
+      </c>
+      <c r="H58" t="n">
+        <v>2</v>
+      </c>
+      <c r="I58" s="1" t="n">
+        <v>44894</v>
+      </c>
+      <c r="J58" t="inlineStr">
+        <is>
+          <t>нет данных</t>
+        </is>
+      </c>
+    </row>
+    <row r="59">
+      <c r="E59" t="inlineStr">
+        <is>
+          <t>12.00R20</t>
+        </is>
+      </c>
+      <c r="F59" t="inlineStr">
+        <is>
+          <t>BEL-288</t>
+        </is>
+      </c>
+      <c r="G59" t="inlineStr">
+        <is>
+          <t>груз, сер</t>
+        </is>
+      </c>
+      <c r="H59" t="n">
+        <v>2</v>
+      </c>
+      <c r="I59" s="1" t="n">
+        <v>44894</v>
+      </c>
+      <c r="J59" t="inlineStr">
+        <is>
+          <t>нет данных</t>
+        </is>
+      </c>
+    </row>
+    <row r="60">
+      <c r="E60" t="inlineStr">
+        <is>
+          <t>16.00R20</t>
+        </is>
+      </c>
+      <c r="F60" t="inlineStr">
+        <is>
+          <t>Бел-95</t>
+        </is>
+      </c>
+      <c r="G60" t="inlineStr">
+        <is>
+          <t>173G, б/к, груз, сер</t>
+        </is>
+      </c>
+      <c r="H60" t="n">
+        <v>2</v>
+      </c>
+      <c r="I60" s="1" t="n">
+        <v>44894</v>
+      </c>
+      <c r="J60" t="inlineStr">
+        <is>
+          <t>нет данных</t>
+        </is>
+      </c>
+    </row>
+    <row r="61">
+      <c r="E61" t="inlineStr">
+        <is>
+          <t>16.00R20</t>
+        </is>
+      </c>
+      <c r="F61" t="inlineStr">
+        <is>
+          <t>Бел-95</t>
+        </is>
+      </c>
+      <c r="G61" t="inlineStr">
+        <is>
+          <t>173G, груз, сер</t>
+        </is>
+      </c>
+      <c r="H61" t="n">
+        <v>2</v>
+      </c>
+      <c r="I61" s="1" t="n">
+        <v>44894</v>
+      </c>
+      <c r="J61" t="inlineStr">
+        <is>
+          <t>нет данных</t>
+        </is>
+      </c>
+    </row>
+    <row r="62">
+      <c r="E62" t="inlineStr">
+        <is>
+          <t>16.00R20</t>
+        </is>
+      </c>
+      <c r="F62" t="inlineStr">
+        <is>
+          <t>Бел-95</t>
+        </is>
+      </c>
+      <c r="G62" t="inlineStr">
+        <is>
+          <t>173G, груз, сер</t>
+        </is>
+      </c>
+      <c r="H62" t="n">
+        <v>2</v>
+      </c>
+      <c r="I62" s="1" t="n">
+        <v>44894</v>
+      </c>
+      <c r="J62" t="inlineStr">
+        <is>
+          <t>нет данных</t>
+        </is>
+      </c>
+    </row>
+    <row r="63">
+      <c r="E63" t="inlineStr">
+        <is>
+          <t>16.00R20</t>
+        </is>
+      </c>
+      <c r="F63" t="inlineStr">
+        <is>
+          <t>Бел-95</t>
+        </is>
+      </c>
+      <c r="G63" t="inlineStr">
+        <is>
+          <t>173G, груз, сер</t>
+        </is>
+      </c>
+      <c r="H63" t="n">
+        <v>2</v>
+      </c>
+      <c r="I63" s="1" t="n">
+        <v>44894</v>
+      </c>
+      <c r="J63" t="inlineStr">
+        <is>
+          <t>нет данных</t>
+        </is>
+      </c>
+    </row>
+    <row r="64">
+      <c r="E64" t="inlineStr">
+        <is>
+          <t>16.00R20</t>
+        </is>
+      </c>
+      <c r="F64" t="inlineStr">
+        <is>
+          <t>Бел-95</t>
+        </is>
+      </c>
+      <c r="G64" t="inlineStr">
+        <is>
+          <t>173G, груз, сер</t>
+        </is>
+      </c>
+      <c r="H64" t="n">
+        <v>2</v>
+      </c>
+      <c r="I64" s="1" t="n">
+        <v>44894</v>
+      </c>
+      <c r="J64" t="inlineStr">
+        <is>
+          <t>нет данных</t>
+        </is>
+      </c>
+    </row>
+    <row r="65">
+      <c r="E65" t="inlineStr">
+        <is>
+          <t>16.00R20</t>
+        </is>
+      </c>
+      <c r="F65" t="inlineStr">
+        <is>
+          <t>Бел-95</t>
+        </is>
+      </c>
+      <c r="G65" t="inlineStr">
+        <is>
+          <t>173G, груз, сер</t>
+        </is>
+      </c>
+      <c r="H65" t="n">
+        <v>2</v>
+      </c>
+      <c r="I65" s="1" t="n">
+        <v>44894</v>
+      </c>
+      <c r="J65" t="inlineStr">
+        <is>
+          <t>нет данных</t>
+        </is>
+      </c>
+    </row>
+    <row r="66">
+      <c r="E66" t="inlineStr">
+        <is>
+          <t>16.00R20</t>
+        </is>
+      </c>
+      <c r="F66" t="inlineStr">
+        <is>
+          <t>Бел-95</t>
+        </is>
+      </c>
+      <c r="G66" t="inlineStr">
+        <is>
+          <t>173G, сер</t>
+        </is>
+      </c>
+      <c r="H66" t="n">
+        <v>2</v>
+      </c>
+      <c r="I66" s="1" t="n">
+        <v>44894</v>
+      </c>
+      <c r="J66" t="inlineStr">
+        <is>
+          <t>нет данных</t>
+        </is>
+      </c>
+    </row>
+    <row r="67">
+      <c r="E67" t="inlineStr">
+        <is>
+          <t>395/85R20</t>
+        </is>
+      </c>
+      <c r="F67" t="inlineStr">
+        <is>
+          <t>BEL-405</t>
+        </is>
+      </c>
+      <c r="G67" t="inlineStr">
+        <is>
+          <t>168J, груз, сер</t>
+        </is>
+      </c>
+      <c r="H67" t="n">
+        <v>2</v>
+      </c>
+      <c r="I67" s="1" t="n">
+        <v>44894</v>
+      </c>
+      <c r="J67" t="inlineStr">
+        <is>
+          <t>нет данных</t>
+        </is>
+      </c>
+    </row>
+    <row r="68">
+      <c r="E68" t="inlineStr">
+        <is>
+          <t>445/65R22.5</t>
+        </is>
+      </c>
+      <c r="F68" t="inlineStr">
+        <is>
+          <t>Бел-145</t>
+        </is>
+      </c>
+      <c r="G68" t="inlineStr">
+        <is>
+          <t>б/к, груз, сер</t>
+        </is>
+      </c>
+      <c r="H68" t="n">
+        <v>2</v>
+      </c>
+      <c r="I68" s="1" t="n">
+        <v>44894</v>
+      </c>
+      <c r="J68" t="inlineStr">
+        <is>
+          <t>нет данных</t>
+        </is>
+      </c>
+    </row>
+    <row r="69">
+      <c r="E69" t="inlineStr">
+        <is>
+          <t>355/65-15</t>
+        </is>
+      </c>
+      <c r="F69" t="inlineStr">
+        <is>
+          <t>Бел-230</t>
+        </is>
+      </c>
+      <c r="G69" t="inlineStr">
+        <is>
+          <t>сер</t>
+        </is>
+      </c>
+      <c r="H69" t="n">
+        <v>2</v>
+      </c>
+      <c r="I69" s="1" t="n">
+        <v>44894</v>
+      </c>
+      <c r="J69" t="inlineStr">
+        <is>
+          <t>нет данных</t>
+        </is>
+      </c>
+    </row>
+    <row r="70">
+      <c r="E70" t="inlineStr">
+        <is>
+          <t>355/65-15</t>
+        </is>
+      </c>
+      <c r="F70" t="inlineStr">
+        <is>
+          <t>Бел-230М</t>
+        </is>
+      </c>
+      <c r="G70" t="inlineStr">
+        <is>
+          <t>сер</t>
+        </is>
+      </c>
+      <c r="H70" t="n">
+        <v>2</v>
+      </c>
+      <c r="I70" s="1" t="n">
+        <v>44894</v>
+      </c>
+      <c r="J70" t="inlineStr">
+        <is>
+          <t>нет данных</t>
+        </is>
+      </c>
+    </row>
+    <row r="71">
+      <c r="E71" t="inlineStr">
+        <is>
+          <t>205/55R16</t>
+        </is>
+      </c>
+      <c r="F71" t="inlineStr">
+        <is>
+          <t>BEL-262</t>
+        </is>
+      </c>
+      <c r="G71" t="inlineStr">
+        <is>
+          <t>б/к, сер, легк</t>
+        </is>
+      </c>
+      <c r="H71" t="n">
+        <v>2</v>
+      </c>
+      <c r="I71" s="1" t="n">
+        <v>44894</v>
+      </c>
+      <c r="J71" t="inlineStr">
+        <is>
+          <t>нет данных</t>
+        </is>
+      </c>
+    </row>
+    <row r="72">
+      <c r="E72" t="inlineStr">
+        <is>
+          <t>205/55R16</t>
+        </is>
+      </c>
+      <c r="F72" t="inlineStr">
+        <is>
+          <t>BEL-317</t>
+        </is>
+      </c>
+      <c r="G72" t="inlineStr">
+        <is>
+          <t>б/к, сер, легк</t>
+        </is>
+      </c>
+      <c r="H72" t="n">
+        <v>2</v>
+      </c>
+      <c r="I72" s="1" t="n">
+        <v>44894</v>
+      </c>
+      <c r="J72" t="inlineStr">
+        <is>
+          <t>нет данных</t>
+        </is>
+      </c>
+    </row>
+    <row r="73">
+      <c r="E73" t="inlineStr">
+        <is>
+          <t>205/55R16</t>
+        </is>
+      </c>
+      <c r="F73" t="inlineStr">
+        <is>
+          <t>BEL-317S</t>
+        </is>
+      </c>
+      <c r="G73" t="inlineStr">
+        <is>
+          <t>сер, ошип</t>
+        </is>
+      </c>
+      <c r="H73" t="n">
+        <v>2</v>
+      </c>
+      <c r="I73" s="1" t="n">
+        <v>44894</v>
+      </c>
+      <c r="J73" t="inlineStr">
+        <is>
+          <t>нет данных</t>
+        </is>
+      </c>
+    </row>
+    <row r="74">
+      <c r="E74" t="inlineStr">
+        <is>
+          <t>205/60R16</t>
+        </is>
+      </c>
+      <c r="F74" t="inlineStr">
+        <is>
+          <t>BEL-277</t>
+        </is>
+      </c>
+      <c r="G74" t="inlineStr">
+        <is>
+          <t>б/к, сер, легк</t>
+        </is>
+      </c>
+      <c r="H74" t="n">
+        <v>2</v>
+      </c>
+      <c r="I74" s="1" t="n">
+        <v>44894</v>
+      </c>
+      <c r="J74" t="inlineStr">
+        <is>
+          <t>нет данных</t>
+        </is>
+      </c>
+    </row>
+    <row r="75">
+      <c r="E75" t="inlineStr">
+        <is>
+          <t>35/65-33</t>
+        </is>
+      </c>
+      <c r="F75" t="inlineStr">
+        <is>
+          <t>ФБел-283</t>
+        </is>
+      </c>
+      <c r="G75" t="inlineStr">
+        <is>
+          <t>42, груз, сер</t>
+        </is>
+      </c>
+      <c r="H75" t="n">
+        <v>2</v>
+      </c>
+      <c r="I75" s="1" t="n">
+        <v>44899</v>
+      </c>
+      <c r="J75" t="inlineStr">
+        <is>
+          <t>нет данных</t>
+        </is>
+      </c>
+    </row>
+    <row r="76">
+      <c r="E76" t="inlineStr">
+        <is>
+          <t>24.00R35</t>
+        </is>
+      </c>
+      <c r="F76" t="inlineStr">
+        <is>
+          <t>Бел-122</t>
+        </is>
+      </c>
+      <c r="G76" t="inlineStr">
+        <is>
+          <t>груз, сер, LS-2, Type</t>
+        </is>
+      </c>
+      <c r="H76" t="n">
+        <v>2</v>
+      </c>
+      <c r="I76" s="1" t="n">
+        <v>44899</v>
+      </c>
+      <c r="J76" t="inlineStr">
+        <is>
+          <t>нет данных</t>
+        </is>
+      </c>
+    </row>
+    <row r="77">
+      <c r="E77" t="inlineStr">
+        <is>
+          <t>24.00R35</t>
+        </is>
+      </c>
+      <c r="F77" t="inlineStr">
+        <is>
+          <t>Бел-122</t>
+        </is>
+      </c>
+      <c r="G77" t="inlineStr">
+        <is>
+          <t>груз, сер, Type, H</t>
+        </is>
+      </c>
+      <c r="H77" t="n">
+        <v>2</v>
+      </c>
+      <c r="I77" s="1" t="n">
+        <v>44899</v>
+      </c>
+      <c r="J77" t="inlineStr">
+        <is>
+          <t>нет данных</t>
+        </is>
+      </c>
+    </row>
+    <row r="78">
+      <c r="E78" t="inlineStr">
+        <is>
+          <t>24.00R35</t>
+        </is>
+      </c>
+      <c r="F78" t="inlineStr">
+        <is>
+          <t>Бел-122</t>
+        </is>
+      </c>
+      <c r="G78" t="inlineStr">
+        <is>
+          <t>груз, сер, Type, C</t>
+        </is>
+      </c>
+      <c r="H78" t="n">
+        <v>2</v>
+      </c>
+      <c r="I78" s="1" t="n">
+        <v>44899</v>
+      </c>
+      <c r="J78" t="inlineStr">
+        <is>
+          <t>нет данных</t>
+        </is>
+      </c>
+    </row>
+    <row r="79">
+      <c r="E79" t="inlineStr">
+        <is>
+          <t>24.00R35</t>
+        </is>
+      </c>
+      <c r="F79" t="inlineStr">
+        <is>
+          <t>Бел-202</t>
+        </is>
+      </c>
+      <c r="G79" t="inlineStr">
+        <is>
+          <t>210B, сер, LS-2, Type</t>
+        </is>
+      </c>
+      <c r="H79" t="n">
+        <v>2</v>
+      </c>
+      <c r="I79" s="1" t="n">
+        <v>44899</v>
+      </c>
+      <c r="J79" t="inlineStr">
+        <is>
+          <t>нет данных</t>
+        </is>
+      </c>
+    </row>
+    <row r="80">
+      <c r="E80" t="inlineStr">
+        <is>
+          <t>24.00R35</t>
+        </is>
+      </c>
+      <c r="F80" t="inlineStr">
+        <is>
+          <t>Бел-202</t>
+        </is>
+      </c>
+      <c r="G80" t="inlineStr">
+        <is>
+          <t>210B, сер, Type, H</t>
+        </is>
+      </c>
+      <c r="H80" t="n">
+        <v>2</v>
+      </c>
+      <c r="I80" s="1" t="n">
+        <v>44899</v>
+      </c>
+      <c r="J80" t="inlineStr">
+        <is>
+          <t>нет данных</t>
+        </is>
+      </c>
+    </row>
+    <row r="81">
+      <c r="E81" t="inlineStr">
+        <is>
+          <t>24.00R35</t>
+        </is>
+      </c>
+      <c r="F81" t="inlineStr">
+        <is>
+          <t>Бел-202</t>
+        </is>
+      </c>
+      <c r="G81" t="inlineStr">
+        <is>
+          <t>210B, сер, Type, C</t>
+        </is>
+      </c>
+      <c r="H81" t="n">
+        <v>2</v>
+      </c>
+      <c r="I81" s="1" t="n">
+        <v>44899</v>
+      </c>
+      <c r="J81" t="inlineStr">
+        <is>
+          <t>нет данных</t>
+        </is>
+      </c>
+    </row>
+    <row r="82">
+      <c r="E82" t="inlineStr">
+        <is>
+          <t>24.00R35</t>
+        </is>
+      </c>
+      <c r="F82" t="inlineStr">
+        <is>
+          <t>Бел-212</t>
+        </is>
+      </c>
+      <c r="G82" t="inlineStr">
+        <is>
+          <t>груз, сер, LS-2, Type</t>
+        </is>
+      </c>
+      <c r="H82" t="n">
+        <v>2</v>
+      </c>
+      <c r="I82" s="1" t="n">
+        <v>44899</v>
+      </c>
+      <c r="J82" t="inlineStr">
+        <is>
+          <t>нет данных</t>
+        </is>
+      </c>
+    </row>
+    <row r="83">
+      <c r="E83" t="inlineStr">
+        <is>
+          <t>24.00R35</t>
+        </is>
+      </c>
+      <c r="F83" t="inlineStr">
+        <is>
+          <t>Бел-212</t>
+        </is>
+      </c>
+      <c r="G83" t="inlineStr">
+        <is>
+          <t>груз, сер, Type, H</t>
+        </is>
+      </c>
+      <c r="H83" t="n">
+        <v>2</v>
+      </c>
+      <c r="I83" s="1" t="n">
+        <v>44899</v>
+      </c>
+      <c r="J83" t="inlineStr">
+        <is>
+          <t>нет данных</t>
+        </is>
+      </c>
+    </row>
+    <row r="84">
+      <c r="E84" t="inlineStr">
+        <is>
+          <t>24.00R35</t>
+        </is>
+      </c>
+      <c r="F84" t="inlineStr">
+        <is>
+          <t>Бел-212</t>
+        </is>
+      </c>
+      <c r="G84" t="inlineStr">
+        <is>
+          <t>груз, сер, Type, C</t>
+        </is>
+      </c>
+      <c r="H84" t="n">
+        <v>2</v>
+      </c>
+      <c r="I84" s="1" t="n">
+        <v>44899</v>
+      </c>
+      <c r="J84" t="inlineStr">
+        <is>
+          <t>нет данных</t>
+        </is>
+      </c>
+    </row>
+    <row r="85">
+      <c r="E85" t="inlineStr">
+        <is>
+          <t>21.00R35</t>
+        </is>
+      </c>
+      <c r="F85" t="inlineStr">
+        <is>
+          <t>Бел-200</t>
+        </is>
+      </c>
+      <c r="G85" t="inlineStr">
+        <is>
+          <t>202B, сер, LS-2, Type</t>
+        </is>
+      </c>
+      <c r="H85" t="n">
+        <v>2</v>
+      </c>
+      <c r="I85" s="1" t="n">
+        <v>44899</v>
+      </c>
+      <c r="J85" t="inlineStr">
+        <is>
+          <t>нет данных</t>
+        </is>
+      </c>
+    </row>
+    <row r="86">
+      <c r="E86" t="inlineStr">
+        <is>
+          <t>21.00R35</t>
+        </is>
+      </c>
+      <c r="F86" t="inlineStr">
+        <is>
+          <t>Бел-200</t>
+        </is>
+      </c>
+      <c r="G86" t="inlineStr">
+        <is>
+          <t>202B, сер, Type, H</t>
+        </is>
+      </c>
+      <c r="H86" t="n">
+        <v>2</v>
+      </c>
+      <c r="I86" s="1" t="n">
+        <v>44899</v>
+      </c>
+      <c r="J86" t="inlineStr">
+        <is>
+          <t>нет данных</t>
+        </is>
+      </c>
+    </row>
+    <row r="87">
+      <c r="E87" t="inlineStr">
+        <is>
+          <t>21.00R35</t>
+        </is>
+      </c>
+      <c r="F87" t="inlineStr">
+        <is>
+          <t>Бел-200</t>
+        </is>
+      </c>
+      <c r="G87" t="inlineStr">
+        <is>
+          <t>202B, сер, Type, C</t>
+        </is>
+      </c>
+      <c r="H87" t="n">
+        <v>2</v>
+      </c>
+      <c r="I87" s="1" t="n">
+        <v>44899</v>
+      </c>
+      <c r="J87" t="inlineStr">
+        <is>
+          <t>нет данных</t>
+        </is>
+      </c>
+    </row>
+    <row r="88">
+      <c r="E88" t="inlineStr">
+        <is>
+          <t>21.00R35</t>
+        </is>
+      </c>
+      <c r="F88" t="inlineStr">
+        <is>
+          <t>Бел-210</t>
+        </is>
+      </c>
+      <c r="G88" t="inlineStr">
+        <is>
+          <t>202B, сер, LS-2, Type</t>
+        </is>
+      </c>
+      <c r="H88" t="n">
+        <v>2</v>
+      </c>
+      <c r="I88" s="1" t="n">
+        <v>44899</v>
+      </c>
+      <c r="J88" t="inlineStr">
+        <is>
+          <t>нет данных</t>
+        </is>
+      </c>
+    </row>
+    <row r="89">
+      <c r="E89" t="inlineStr">
+        <is>
+          <t>21.00R35</t>
+        </is>
+      </c>
+      <c r="F89" t="inlineStr">
+        <is>
+          <t>Бел-210</t>
+        </is>
+      </c>
+      <c r="G89" t="inlineStr">
+        <is>
+          <t>202B, сер, Type, H</t>
+        </is>
+      </c>
+      <c r="H89" t="n">
+        <v>2</v>
+      </c>
+      <c r="I89" s="1" t="n">
+        <v>44899</v>
+      </c>
+      <c r="J89" t="inlineStr">
+        <is>
+          <t>нет данных</t>
+        </is>
+      </c>
+    </row>
+    <row r="90">
+      <c r="E90" t="inlineStr">
+        <is>
+          <t>21.00R35</t>
+        </is>
+      </c>
+      <c r="F90" t="inlineStr">
+        <is>
+          <t>Бел-210</t>
+        </is>
+      </c>
+      <c r="G90" t="inlineStr">
+        <is>
+          <t>202B, сер, Type, C</t>
+        </is>
+      </c>
+      <c r="H90" t="n">
+        <v>2</v>
+      </c>
+      <c r="I90" s="1" t="n">
+        <v>44899</v>
+      </c>
+      <c r="J90" t="inlineStr">
+        <is>
+          <t>нет данных</t>
+        </is>
+      </c>
+    </row>
+    <row r="91">
+      <c r="E91" t="inlineStr">
+        <is>
+          <t>14.00R20</t>
+        </is>
+      </c>
+      <c r="F91" t="inlineStr">
+        <is>
+          <t>BEL-248</t>
+        </is>
+      </c>
+      <c r="G91" t="inlineStr">
+        <is>
+          <t>груз, сер</t>
+        </is>
+      </c>
+      <c r="H91" t="n">
+        <v>2</v>
+      </c>
+      <c r="I91" s="1" t="n">
+        <v>44899</v>
+      </c>
+      <c r="J91" t="inlineStr">
+        <is>
+          <t>нет данных</t>
+        </is>
+      </c>
+    </row>
+    <row r="92">
+      <c r="E92" t="inlineStr">
+        <is>
+          <t>14.00R20</t>
+        </is>
+      </c>
+      <c r="F92" t="inlineStr">
+        <is>
+          <t>BEL-248</t>
+        </is>
+      </c>
+      <c r="G92" t="inlineStr">
+        <is>
+          <t>груз, сер</t>
+        </is>
+      </c>
+      <c r="H92" t="n">
+        <v>2</v>
+      </c>
+      <c r="I92" s="1" t="n">
+        <v>44899</v>
+      </c>
+      <c r="J92" t="inlineStr">
+        <is>
+          <t>нет данных</t>
+        </is>
+      </c>
+    </row>
+    <row r="93">
+      <c r="E93" t="inlineStr">
+        <is>
+          <t>14.00R20</t>
+        </is>
+      </c>
+      <c r="F93" t="inlineStr">
+        <is>
+          <t>BEL-248</t>
+        </is>
+      </c>
+      <c r="G93" t="inlineStr">
+        <is>
+          <t>б/к, груз, сер</t>
+        </is>
+      </c>
+      <c r="H93" t="n">
+        <v>2</v>
+      </c>
+      <c r="I93" s="1" t="n">
+        <v>44899</v>
+      </c>
+      <c r="J93" t="inlineStr">
+        <is>
+          <t>нет данных</t>
+        </is>
+      </c>
+    </row>
+    <row r="94">
+      <c r="E94" t="inlineStr">
+        <is>
+          <t>14.00R20</t>
+        </is>
+      </c>
+      <c r="F94" t="inlineStr">
+        <is>
+          <t>BEL-248</t>
+        </is>
+      </c>
+      <c r="G94" t="inlineStr">
+        <is>
+          <t>груз, сер</t>
+        </is>
+      </c>
+      <c r="H94" t="n">
+        <v>2</v>
+      </c>
+      <c r="I94" s="1" t="n">
+        <v>44899</v>
+      </c>
+      <c r="J94" t="inlineStr">
+        <is>
+          <t>нет данных</t>
+        </is>
+      </c>
+    </row>
+    <row r="95">
+      <c r="E95" t="inlineStr">
+        <is>
+          <t>12.00R20</t>
+        </is>
+      </c>
+      <c r="F95" t="inlineStr">
+        <is>
+          <t>BEL-288</t>
+        </is>
+      </c>
+      <c r="G95" t="inlineStr">
+        <is>
+          <t>груз, сер</t>
+        </is>
+      </c>
+      <c r="H95" t="n">
+        <v>2</v>
+      </c>
+      <c r="I95" s="1" t="n">
+        <v>44899</v>
+      </c>
+      <c r="J95" t="inlineStr">
+        <is>
+          <t>нет данных</t>
+        </is>
+      </c>
+    </row>
+    <row r="96">
+      <c r="E96" t="inlineStr">
+        <is>
+          <t>16.00R20</t>
+        </is>
+      </c>
+      <c r="F96" t="inlineStr">
+        <is>
+          <t>Бел-95</t>
+        </is>
+      </c>
+      <c r="G96" t="inlineStr">
+        <is>
+          <t>173G, б/к, груз, сер</t>
+        </is>
+      </c>
+      <c r="H96" t="n">
+        <v>2</v>
+      </c>
+      <c r="I96" s="1" t="n">
+        <v>44899</v>
+      </c>
+      <c r="J96" t="inlineStr">
+        <is>
+          <t>нет данных</t>
+        </is>
+      </c>
+    </row>
+    <row r="97">
+      <c r="E97" t="inlineStr">
+        <is>
+          <t>16.00R20</t>
+        </is>
+      </c>
+      <c r="F97" t="inlineStr">
+        <is>
+          <t>Бел-95</t>
+        </is>
+      </c>
+      <c r="G97" t="inlineStr">
+        <is>
+          <t>173G, груз, сер</t>
+        </is>
+      </c>
+      <c r="H97" t="n">
+        <v>2</v>
+      </c>
+      <c r="I97" s="1" t="n">
+        <v>44899</v>
+      </c>
+      <c r="J97" t="inlineStr">
+        <is>
+          <t>нет данных</t>
+        </is>
+      </c>
+    </row>
+    <row r="98">
+      <c r="E98" t="inlineStr">
+        <is>
+          <t>16.00R20</t>
+        </is>
+      </c>
+      <c r="F98" t="inlineStr">
+        <is>
+          <t>Бел-95</t>
+        </is>
+      </c>
+      <c r="G98" t="inlineStr">
+        <is>
+          <t>173G, груз, сер</t>
+        </is>
+      </c>
+      <c r="H98" t="n">
+        <v>2</v>
+      </c>
+      <c r="I98" s="1" t="n">
+        <v>44899</v>
+      </c>
+      <c r="J98" t="inlineStr">
+        <is>
+          <t>нет данных</t>
+        </is>
+      </c>
+    </row>
+    <row r="99">
+      <c r="E99" t="inlineStr">
+        <is>
+          <t>16.00R20</t>
+        </is>
+      </c>
+      <c r="F99" t="inlineStr">
+        <is>
+          <t>Бел-95</t>
+        </is>
+      </c>
+      <c r="G99" t="inlineStr">
+        <is>
+          <t>173G, груз, сер</t>
+        </is>
+      </c>
+      <c r="H99" t="n">
+        <v>2</v>
+      </c>
+      <c r="I99" s="1" t="n">
+        <v>44899</v>
+      </c>
+      <c r="J99" t="inlineStr">
+        <is>
+          <t>нет данных</t>
+        </is>
+      </c>
+    </row>
+    <row r="100">
+      <c r="E100" t="inlineStr">
+        <is>
+          <t>16.00R20</t>
+        </is>
+      </c>
+      <c r="F100" t="inlineStr">
+        <is>
+          <t>Бел-95</t>
+        </is>
+      </c>
+      <c r="G100" t="inlineStr">
+        <is>
+          <t>173G, груз, сер</t>
+        </is>
+      </c>
+      <c r="H100" t="n">
+        <v>2</v>
+      </c>
+      <c r="I100" s="1" t="n">
+        <v>44899</v>
+      </c>
+      <c r="J100" t="inlineStr">
+        <is>
+          <t>нет данных</t>
+        </is>
+      </c>
+    </row>
+    <row r="101">
+      <c r="E101" t="inlineStr">
+        <is>
+          <t>16.00R20</t>
+        </is>
+      </c>
+      <c r="F101" t="inlineStr">
+        <is>
+          <t>Бел-95</t>
+        </is>
+      </c>
+      <c r="G101" t="inlineStr">
+        <is>
+          <t>173G, груз, сер</t>
+        </is>
+      </c>
+      <c r="H101" t="n">
+        <v>2</v>
+      </c>
+      <c r="I101" s="1" t="n">
+        <v>44899</v>
+      </c>
+      <c r="J101" t="inlineStr">
+        <is>
+          <t>нет данных</t>
+        </is>
+      </c>
+    </row>
+    <row r="102">
+      <c r="E102" t="inlineStr">
+        <is>
+          <t>16.00R20</t>
+        </is>
+      </c>
+      <c r="F102" t="inlineStr">
+        <is>
+          <t>Бел-95</t>
+        </is>
+      </c>
+      <c r="G102" t="inlineStr">
+        <is>
+          <t>173G, сер</t>
+        </is>
+      </c>
+      <c r="H102" t="n">
+        <v>2</v>
+      </c>
+      <c r="I102" s="1" t="n">
+        <v>44899</v>
+      </c>
+      <c r="J102" t="inlineStr">
+        <is>
+          <t>нет данных</t>
+        </is>
+      </c>
+    </row>
+    <row r="103">
+      <c r="E103" t="inlineStr">
+        <is>
+          <t>395/85R20</t>
+        </is>
+      </c>
+      <c r="F103" t="inlineStr">
+        <is>
+          <t>BEL-405</t>
+        </is>
+      </c>
+      <c r="G103" t="inlineStr">
+        <is>
+          <t>168J, груз, сер</t>
+        </is>
+      </c>
+      <c r="H103" t="n">
+        <v>2</v>
+      </c>
+      <c r="I103" s="1" t="n">
+        <v>44899</v>
+      </c>
+      <c r="J103" t="inlineStr">
+        <is>
+          <t>нет данных</t>
+        </is>
+      </c>
+    </row>
+    <row r="104">
+      <c r="E104" t="inlineStr">
+        <is>
+          <t>445/65R22.5</t>
+        </is>
+      </c>
+      <c r="F104" t="inlineStr">
+        <is>
+          <t>Бел-145</t>
+        </is>
+      </c>
+      <c r="G104" t="inlineStr">
+        <is>
+          <t>б/к, груз, сер</t>
+        </is>
+      </c>
+      <c r="H104" t="n">
+        <v>2</v>
+      </c>
+      <c r="I104" s="1" t="n">
+        <v>44899</v>
+      </c>
+      <c r="J104" t="inlineStr">
+        <is>
+          <t>нет данных</t>
+        </is>
+      </c>
+    </row>
+    <row r="105">
+      <c r="E105" t="inlineStr">
+        <is>
+          <t>355/65-15</t>
+        </is>
+      </c>
+      <c r="F105" t="inlineStr">
+        <is>
+          <t>Бел-230</t>
+        </is>
+      </c>
+      <c r="G105" t="inlineStr">
+        <is>
+          <t>сер</t>
+        </is>
+      </c>
+      <c r="H105" t="n">
+        <v>2</v>
+      </c>
+      <c r="I105" s="1" t="n">
+        <v>44899</v>
+      </c>
+      <c r="J105" t="inlineStr">
+        <is>
+          <t>нет данных</t>
+        </is>
+      </c>
+    </row>
+    <row r="106">
+      <c r="E106" t="inlineStr">
+        <is>
+          <t>355/65-15</t>
+        </is>
+      </c>
+      <c r="F106" t="inlineStr">
+        <is>
+          <t>Бел-230М</t>
+        </is>
+      </c>
+      <c r="G106" t="inlineStr">
+        <is>
+          <t>сер</t>
+        </is>
+      </c>
+      <c r="H106" t="n">
+        <v>2</v>
+      </c>
+      <c r="I106" s="1" t="n">
+        <v>44899</v>
+      </c>
+      <c r="J106" t="inlineStr">
+        <is>
+          <t>нет данных</t>
+        </is>
+      </c>
+    </row>
+    <row r="107">
+      <c r="E107" t="inlineStr">
+        <is>
+          <t>205/55R16</t>
+        </is>
+      </c>
+      <c r="F107" t="inlineStr">
+        <is>
+          <t>BEL-262</t>
+        </is>
+      </c>
+      <c r="G107" t="inlineStr">
+        <is>
+          <t>б/к, сер, легк</t>
+        </is>
+      </c>
+      <c r="H107" t="n">
+        <v>2</v>
+      </c>
+      <c r="I107" s="1" t="n">
+        <v>44899</v>
+      </c>
+      <c r="J107" t="inlineStr">
+        <is>
+          <t>нет данных</t>
+        </is>
+      </c>
+    </row>
+    <row r="108">
+      <c r="E108" t="inlineStr">
+        <is>
+          <t>205/55R16</t>
+        </is>
+      </c>
+      <c r="F108" t="inlineStr">
+        <is>
+          <t>BEL-317</t>
+        </is>
+      </c>
+      <c r="G108" t="inlineStr">
+        <is>
+          <t>б/к, сер, легк</t>
+        </is>
+      </c>
+      <c r="H108" t="n">
+        <v>2</v>
+      </c>
+      <c r="I108" s="1" t="n">
+        <v>44899</v>
+      </c>
+      <c r="J108" t="inlineStr">
+        <is>
+          <t>нет данных</t>
+        </is>
+      </c>
+    </row>
+    <row r="109">
+      <c r="E109" t="inlineStr">
+        <is>
+          <t>205/55R16</t>
+        </is>
+      </c>
+      <c r="F109" t="inlineStr">
+        <is>
+          <t>BEL-317S</t>
+        </is>
+      </c>
+      <c r="G109" t="inlineStr">
+        <is>
+          <t>сер, ошип</t>
+        </is>
+      </c>
+      <c r="H109" t="n">
+        <v>2</v>
+      </c>
+      <c r="I109" s="1" t="n">
+        <v>44899</v>
+      </c>
+      <c r="J109" t="inlineStr">
+        <is>
+          <t>нет данных</t>
+        </is>
+      </c>
+    </row>
+    <row r="110">
+      <c r="E110" t="inlineStr">
+        <is>
+          <t>205/60R16</t>
+        </is>
+      </c>
+      <c r="F110" t="inlineStr">
+        <is>
+          <t>BEL-277</t>
+        </is>
+      </c>
+      <c r="G110" t="inlineStr">
+        <is>
+          <t>б/к, сер, легк</t>
+        </is>
+      </c>
+      <c r="H110" t="n">
+        <v>2</v>
+      </c>
+      <c r="I110" s="1" t="n">
+        <v>44899</v>
+      </c>
+      <c r="J110" t="inlineStr">
+        <is>
+          <t>нет данных</t>
+        </is>
+      </c>
+    </row>
+    <row r="111">
+      <c r="E111" t="inlineStr">
+        <is>
+          <t>35/65-33</t>
+        </is>
+      </c>
+      <c r="F111" t="inlineStr">
+        <is>
+          <t>ФБел-283</t>
+        </is>
+      </c>
+      <c r="G111" t="inlineStr">
+        <is>
+          <t>42, груз, сер</t>
+        </is>
+      </c>
+      <c r="H111" t="n">
+        <v>2</v>
+      </c>
+      <c r="I111" s="1" t="n">
+        <v>44900</v>
+      </c>
+      <c r="J111" t="inlineStr">
+        <is>
+          <t>нет данных</t>
+        </is>
+      </c>
+    </row>
+    <row r="112">
+      <c r="E112" t="inlineStr">
+        <is>
+          <t>24.00R35</t>
+        </is>
+      </c>
+      <c r="F112" t="inlineStr">
+        <is>
+          <t>Бел-122</t>
+        </is>
+      </c>
+      <c r="G112" t="inlineStr">
+        <is>
+          <t>груз, сер, LS-2, Type</t>
+        </is>
+      </c>
+      <c r="H112" t="n">
+        <v>2</v>
+      </c>
+      <c r="I112" s="1" t="n">
+        <v>44900</v>
+      </c>
+      <c r="J112" t="inlineStr">
+        <is>
+          <t>нет данных</t>
+        </is>
+      </c>
+    </row>
+    <row r="113">
+      <c r="E113" t="inlineStr">
+        <is>
+          <t>24.00R35</t>
+        </is>
+      </c>
+      <c r="F113" t="inlineStr">
+        <is>
+          <t>Бел-122</t>
+        </is>
+      </c>
+      <c r="G113" t="inlineStr">
+        <is>
+          <t>груз, сер, Type, H</t>
+        </is>
+      </c>
+      <c r="H113" t="n">
+        <v>2</v>
+      </c>
+      <c r="I113" s="1" t="n">
+        <v>44900</v>
+      </c>
+      <c r="J113" t="inlineStr">
+        <is>
+          <t>нет данных</t>
+        </is>
+      </c>
+    </row>
+    <row r="114">
+      <c r="E114" t="inlineStr">
+        <is>
+          <t>24.00R35</t>
+        </is>
+      </c>
+      <c r="F114" t="inlineStr">
+        <is>
+          <t>Бел-122</t>
+        </is>
+      </c>
+      <c r="G114" t="inlineStr">
+        <is>
+          <t>груз, сер, Type, C</t>
+        </is>
+      </c>
+      <c r="H114" t="n">
+        <v>2</v>
+      </c>
+      <c r="I114" s="1" t="n">
+        <v>44900</v>
+      </c>
+      <c r="J114" t="inlineStr">
+        <is>
+          <t>нет данных</t>
+        </is>
+      </c>
+    </row>
+    <row r="115">
+      <c r="E115" t="inlineStr">
+        <is>
+          <t>24.00R35</t>
+        </is>
+      </c>
+      <c r="F115" t="inlineStr">
+        <is>
+          <t>Бел-202</t>
+        </is>
+      </c>
+      <c r="G115" t="inlineStr">
+        <is>
+          <t>210B, сер, LS-2, Type</t>
+        </is>
+      </c>
+      <c r="H115" t="n">
+        <v>2</v>
+      </c>
+      <c r="I115" s="1" t="n">
+        <v>44900</v>
+      </c>
+      <c r="J115" t="inlineStr">
+        <is>
+          <t>нет данных</t>
+        </is>
+      </c>
+    </row>
+    <row r="116">
+      <c r="E116" t="inlineStr">
+        <is>
+          <t>24.00R35</t>
+        </is>
+      </c>
+      <c r="F116" t="inlineStr">
+        <is>
+          <t>Бел-202</t>
+        </is>
+      </c>
+      <c r="G116" t="inlineStr">
+        <is>
+          <t>210B, сер, Type, H</t>
+        </is>
+      </c>
+      <c r="H116" t="n">
+        <v>2</v>
+      </c>
+      <c r="I116" s="1" t="n">
+        <v>44900</v>
+      </c>
+      <c r="J116" t="inlineStr">
+        <is>
+          <t>нет данных</t>
+        </is>
+      </c>
+    </row>
+    <row r="117">
+      <c r="E117" t="inlineStr">
+        <is>
+          <t>24.00R35</t>
+        </is>
+      </c>
+      <c r="F117" t="inlineStr">
+        <is>
+          <t>Бел-202</t>
+        </is>
+      </c>
+      <c r="G117" t="inlineStr">
+        <is>
+          <t>210B, сер, Type, C</t>
+        </is>
+      </c>
+      <c r="H117" t="n">
+        <v>2</v>
+      </c>
+      <c r="I117" s="1" t="n">
+        <v>44900</v>
+      </c>
+      <c r="J117" t="inlineStr">
+        <is>
+          <t>нет данных</t>
+        </is>
+      </c>
+    </row>
+    <row r="118">
+      <c r="E118" t="inlineStr">
+        <is>
+          <t>24.00R35</t>
+        </is>
+      </c>
+      <c r="F118" t="inlineStr">
+        <is>
+          <t>Бел-212</t>
+        </is>
+      </c>
+      <c r="G118" t="inlineStr">
+        <is>
+          <t>груз, сер, LS-2, Type</t>
+        </is>
+      </c>
+      <c r="H118" t="n">
+        <v>2</v>
+      </c>
+      <c r="I118" s="1" t="n">
+        <v>44900</v>
+      </c>
+      <c r="J118" t="inlineStr">
+        <is>
+          <t>нет данных</t>
+        </is>
+      </c>
+    </row>
+    <row r="119">
+      <c r="E119" t="inlineStr">
+        <is>
+          <t>24.00R35</t>
+        </is>
+      </c>
+      <c r="F119" t="inlineStr">
+        <is>
+          <t>Бел-212</t>
+        </is>
+      </c>
+      <c r="G119" t="inlineStr">
+        <is>
+          <t>груз, сер, Type, H</t>
+        </is>
+      </c>
+      <c r="H119" t="n">
+        <v>2</v>
+      </c>
+      <c r="I119" s="1" t="n">
+        <v>44900</v>
+      </c>
+      <c r="J119" t="inlineStr">
+        <is>
+          <t>нет данных</t>
+        </is>
+      </c>
+    </row>
+    <row r="120">
+      <c r="E120" t="inlineStr">
+        <is>
+          <t>24.00R35</t>
+        </is>
+      </c>
+      <c r="F120" t="inlineStr">
+        <is>
+          <t>Бел-212</t>
+        </is>
+      </c>
+      <c r="G120" t="inlineStr">
+        <is>
+          <t>груз, сер, Type, C</t>
+        </is>
+      </c>
+      <c r="H120" t="n">
+        <v>2</v>
+      </c>
+      <c r="I120" s="1" t="n">
+        <v>44900</v>
+      </c>
+      <c r="J120" t="inlineStr">
+        <is>
+          <t>нет данных</t>
+        </is>
+      </c>
+    </row>
+    <row r="121">
+      <c r="E121" t="inlineStr">
+        <is>
+          <t>21.00R35</t>
+        </is>
+      </c>
+      <c r="F121" t="inlineStr">
+        <is>
+          <t>Бел-200</t>
+        </is>
+      </c>
+      <c r="G121" t="inlineStr">
+        <is>
+          <t>202B, сер, LS-2, Type</t>
+        </is>
+      </c>
+      <c r="H121" t="n">
+        <v>2</v>
+      </c>
+      <c r="I121" s="1" t="n">
+        <v>44900</v>
+      </c>
+      <c r="J121" t="inlineStr">
+        <is>
+          <t>нет данных</t>
+        </is>
+      </c>
+    </row>
+    <row r="122">
+      <c r="E122" t="inlineStr">
+        <is>
+          <t>21.00R35</t>
+        </is>
+      </c>
+      <c r="F122" t="inlineStr">
+        <is>
+          <t>Бел-200</t>
+        </is>
+      </c>
+      <c r="G122" t="inlineStr">
+        <is>
+          <t>202B, сер, Type, H</t>
+        </is>
+      </c>
+      <c r="H122" t="n">
+        <v>2</v>
+      </c>
+      <c r="I122" s="1" t="n">
+        <v>44900</v>
+      </c>
+      <c r="J122" t="inlineStr">
+        <is>
+          <t>нет данных</t>
+        </is>
+      </c>
+    </row>
+    <row r="123">
+      <c r="E123" t="inlineStr">
+        <is>
+          <t>21.00R35</t>
+        </is>
+      </c>
+      <c r="F123" t="inlineStr">
+        <is>
+          <t>Бел-200</t>
+        </is>
+      </c>
+      <c r="G123" t="inlineStr">
+        <is>
+          <t>202B, сер, Type, C</t>
+        </is>
+      </c>
+      <c r="H123" t="n">
+        <v>2</v>
+      </c>
+      <c r="I123" s="1" t="n">
+        <v>44900</v>
+      </c>
+      <c r="J123" t="inlineStr">
+        <is>
+          <t>нет данных</t>
+        </is>
+      </c>
+    </row>
+    <row r="124">
+      <c r="E124" t="inlineStr">
+        <is>
+          <t>21.00R35</t>
+        </is>
+      </c>
+      <c r="F124" t="inlineStr">
+        <is>
+          <t>Бел-210</t>
+        </is>
+      </c>
+      <c r="G124" t="inlineStr">
+        <is>
+          <t>202B, сер, LS-2, Type</t>
+        </is>
+      </c>
+      <c r="H124" t="n">
+        <v>2</v>
+      </c>
+      <c r="I124" s="1" t="n">
+        <v>44900</v>
+      </c>
+      <c r="J124" t="inlineStr">
+        <is>
+          <t>нет данных</t>
+        </is>
+      </c>
+    </row>
+    <row r="125">
+      <c r="E125" t="inlineStr">
+        <is>
+          <t>21.00R35</t>
+        </is>
+      </c>
+      <c r="F125" t="inlineStr">
+        <is>
+          <t>Бел-210</t>
+        </is>
+      </c>
+      <c r="G125" t="inlineStr">
+        <is>
+          <t>202B, сер, Type, H</t>
+        </is>
+      </c>
+      <c r="H125" t="n">
+        <v>2</v>
+      </c>
+      <c r="I125" s="1" t="n">
+        <v>44900</v>
+      </c>
+      <c r="J125" t="inlineStr">
+        <is>
+          <t>нет данных</t>
+        </is>
+      </c>
+    </row>
+    <row r="126">
+      <c r="E126" t="inlineStr">
+        <is>
+          <t>21.00R35</t>
+        </is>
+      </c>
+      <c r="F126" t="inlineStr">
+        <is>
+          <t>Бел-210</t>
+        </is>
+      </c>
+      <c r="G126" t="inlineStr">
+        <is>
+          <t>202B, сер, Type, C</t>
+        </is>
+      </c>
+      <c r="H126" t="n">
+        <v>2</v>
+      </c>
+      <c r="I126" s="1" t="n">
+        <v>44900</v>
+      </c>
+      <c r="J126" t="inlineStr">
+        <is>
+          <t>нет данных</t>
+        </is>
+      </c>
+    </row>
+    <row r="127">
+      <c r="E127" t="inlineStr">
+        <is>
+          <t>14.00R20</t>
+        </is>
+      </c>
+      <c r="F127" t="inlineStr">
+        <is>
+          <t>BEL-248</t>
+        </is>
+      </c>
+      <c r="G127" t="inlineStr">
+        <is>
+          <t>груз, сер</t>
+        </is>
+      </c>
+      <c r="H127" t="n">
+        <v>2</v>
+      </c>
+      <c r="I127" s="1" t="n">
+        <v>44900</v>
+      </c>
+      <c r="J127" t="inlineStr">
+        <is>
+          <t>нет данных</t>
+        </is>
+      </c>
+    </row>
+    <row r="128">
+      <c r="E128" t="inlineStr">
+        <is>
+          <t>14.00R20</t>
+        </is>
+      </c>
+      <c r="F128" t="inlineStr">
+        <is>
+          <t>BEL-248</t>
+        </is>
+      </c>
+      <c r="G128" t="inlineStr">
+        <is>
+          <t>груз, сер</t>
+        </is>
+      </c>
+      <c r="H128" t="n">
+        <v>2</v>
+      </c>
+      <c r="I128" s="1" t="n">
+        <v>44900</v>
+      </c>
+      <c r="J128" t="inlineStr">
+        <is>
+          <t>нет данных</t>
+        </is>
+      </c>
+    </row>
+    <row r="129">
+      <c r="E129" t="inlineStr">
+        <is>
+          <t>14.00R20</t>
+        </is>
+      </c>
+      <c r="F129" t="inlineStr">
+        <is>
+          <t>BEL-248</t>
+        </is>
+      </c>
+      <c r="G129" t="inlineStr">
+        <is>
+          <t>б/к, груз, сер</t>
+        </is>
+      </c>
+      <c r="H129" t="n">
+        <v>2</v>
+      </c>
+      <c r="I129" s="1" t="n">
+        <v>44900</v>
+      </c>
+      <c r="J129" t="inlineStr">
+        <is>
+          <t>нет данных</t>
+        </is>
+      </c>
+    </row>
+    <row r="130">
+      <c r="E130" t="inlineStr">
+        <is>
+          <t>14.00R20</t>
+        </is>
+      </c>
+      <c r="F130" t="inlineStr">
+        <is>
+          <t>BEL-248</t>
+        </is>
+      </c>
+      <c r="G130" t="inlineStr">
+        <is>
+          <t>груз, сер</t>
+        </is>
+      </c>
+      <c r="H130" t="n">
+        <v>2</v>
+      </c>
+      <c r="I130" s="1" t="n">
+        <v>44900</v>
+      </c>
+      <c r="J130" t="inlineStr">
+        <is>
+          <t>нет данных</t>
+        </is>
+      </c>
+    </row>
+    <row r="131">
+      <c r="E131" t="inlineStr">
+        <is>
+          <t>12.00R20</t>
+        </is>
+      </c>
+      <c r="F131" t="inlineStr">
+        <is>
+          <t>BEL-288</t>
+        </is>
+      </c>
+      <c r="G131" t="inlineStr">
+        <is>
+          <t>груз, сер</t>
+        </is>
+      </c>
+      <c r="H131" t="n">
+        <v>2</v>
+      </c>
+      <c r="I131" s="1" t="n">
+        <v>44900</v>
+      </c>
+      <c r="J131" t="inlineStr">
+        <is>
+          <t>нет данных</t>
+        </is>
+      </c>
+    </row>
+    <row r="132">
+      <c r="E132" t="inlineStr">
+        <is>
+          <t>16.00R20</t>
+        </is>
+      </c>
+      <c r="F132" t="inlineStr">
+        <is>
+          <t>Бел-95</t>
+        </is>
+      </c>
+      <c r="G132" t="inlineStr">
+        <is>
+          <t>173G, б/к, груз, сер</t>
+        </is>
+      </c>
+      <c r="H132" t="n">
+        <v>2</v>
+      </c>
+      <c r="I132" s="1" t="n">
+        <v>44900</v>
+      </c>
+      <c r="J132" t="inlineStr">
+        <is>
+          <t>нет данных</t>
+        </is>
+      </c>
+    </row>
+    <row r="133">
+      <c r="E133" t="inlineStr">
+        <is>
+          <t>16.00R20</t>
+        </is>
+      </c>
+      <c r="F133" t="inlineStr">
+        <is>
+          <t>Бел-95</t>
+        </is>
+      </c>
+      <c r="G133" t="inlineStr">
+        <is>
+          <t>173G, груз, сер</t>
+        </is>
+      </c>
+      <c r="H133" t="n">
+        <v>2</v>
+      </c>
+      <c r="I133" s="1" t="n">
+        <v>44900</v>
+      </c>
+      <c r="J133" t="inlineStr">
+        <is>
+          <t>нет данных</t>
+        </is>
+      </c>
+    </row>
+    <row r="134">
+      <c r="E134" t="inlineStr">
+        <is>
+          <t>16.00R20</t>
+        </is>
+      </c>
+      <c r="F134" t="inlineStr">
+        <is>
+          <t>Бел-95</t>
+        </is>
+      </c>
+      <c r="G134" t="inlineStr">
+        <is>
+          <t>173G, груз, сер</t>
+        </is>
+      </c>
+      <c r="H134" t="n">
+        <v>2</v>
+      </c>
+      <c r="I134" s="1" t="n">
+        <v>44900</v>
+      </c>
+      <c r="J134" t="inlineStr">
+        <is>
+          <t>нет данных</t>
+        </is>
+      </c>
+    </row>
+    <row r="135">
+      <c r="E135" t="inlineStr">
+        <is>
+          <t>16.00R20</t>
+        </is>
+      </c>
+      <c r="F135" t="inlineStr">
+        <is>
+          <t>Бел-95</t>
+        </is>
+      </c>
+      <c r="G135" t="inlineStr">
+        <is>
+          <t>173G, груз, сер</t>
+        </is>
+      </c>
+      <c r="H135" t="n">
+        <v>2</v>
+      </c>
+      <c r="I135" s="1" t="n">
+        <v>44900</v>
+      </c>
+      <c r="J135" t="inlineStr">
+        <is>
+          <t>нет данных</t>
+        </is>
+      </c>
+    </row>
+    <row r="136">
+      <c r="E136" t="inlineStr">
+        <is>
+          <t>16.00R20</t>
+        </is>
+      </c>
+      <c r="F136" t="inlineStr">
+        <is>
+          <t>Бел-95</t>
+        </is>
+      </c>
+      <c r="G136" t="inlineStr">
+        <is>
+          <t>173G, груз, сер</t>
+        </is>
+      </c>
+      <c r="H136" t="n">
+        <v>2</v>
+      </c>
+      <c r="I136" s="1" t="n">
+        <v>44900</v>
+      </c>
+      <c r="J136" t="inlineStr">
+        <is>
+          <t>нет данных</t>
+        </is>
+      </c>
+    </row>
+    <row r="137">
+      <c r="E137" t="inlineStr">
+        <is>
+          <t>16.00R20</t>
+        </is>
+      </c>
+      <c r="F137" t="inlineStr">
+        <is>
+          <t>Бел-95</t>
+        </is>
+      </c>
+      <c r="G137" t="inlineStr">
+        <is>
+          <t>173G, груз, сер</t>
+        </is>
+      </c>
+      <c r="H137" t="n">
+        <v>2</v>
+      </c>
+      <c r="I137" s="1" t="n">
+        <v>44900</v>
+      </c>
+      <c r="J137" t="inlineStr">
+        <is>
+          <t>нет данных</t>
+        </is>
+      </c>
+    </row>
+    <row r="138">
+      <c r="E138" t="inlineStr">
+        <is>
+          <t>16.00R20</t>
+        </is>
+      </c>
+      <c r="F138" t="inlineStr">
+        <is>
+          <t>Бел-95</t>
+        </is>
+      </c>
+      <c r="G138" t="inlineStr">
+        <is>
+          <t>173G, сер</t>
+        </is>
+      </c>
+      <c r="H138" t="n">
+        <v>2</v>
+      </c>
+      <c r="I138" s="1" t="n">
+        <v>44900</v>
+      </c>
+      <c r="J138" t="inlineStr">
+        <is>
+          <t>нет данных</t>
+        </is>
+      </c>
+    </row>
+    <row r="139">
+      <c r="E139" t="inlineStr">
+        <is>
+          <t>395/85R20</t>
+        </is>
+      </c>
+      <c r="F139" t="inlineStr">
+        <is>
+          <t>BEL-405</t>
+        </is>
+      </c>
+      <c r="G139" t="inlineStr">
+        <is>
+          <t>168J, груз, сер</t>
+        </is>
+      </c>
+      <c r="H139" t="n">
+        <v>2</v>
+      </c>
+      <c r="I139" s="1" t="n">
+        <v>44900</v>
+      </c>
+      <c r="J139" t="inlineStr">
+        <is>
+          <t>нет данных</t>
+        </is>
+      </c>
+    </row>
+    <row r="140">
+      <c r="E140" t="inlineStr">
+        <is>
+          <t>445/65R22.5</t>
+        </is>
+      </c>
+      <c r="F140" t="inlineStr">
+        <is>
+          <t>Бел-145</t>
+        </is>
+      </c>
+      <c r="G140" t="inlineStr">
+        <is>
+          <t>б/к, груз, сер</t>
+        </is>
+      </c>
+      <c r="H140" t="n">
+        <v>2</v>
+      </c>
+      <c r="I140" s="1" t="n">
+        <v>44900</v>
+      </c>
+      <c r="J140" t="inlineStr">
+        <is>
+          <t>нет данных</t>
+        </is>
+      </c>
+    </row>
+    <row r="141">
+      <c r="E141" t="inlineStr">
+        <is>
+          <t>355/65-15</t>
+        </is>
+      </c>
+      <c r="F141" t="inlineStr">
+        <is>
+          <t>Бел-230</t>
+        </is>
+      </c>
+      <c r="G141" t="inlineStr">
+        <is>
+          <t>сер</t>
+        </is>
+      </c>
+      <c r="H141" t="n">
+        <v>2</v>
+      </c>
+      <c r="I141" s="1" t="n">
+        <v>44900</v>
+      </c>
+      <c r="J141" t="inlineStr">
+        <is>
+          <t>нет данных</t>
+        </is>
+      </c>
+    </row>
+    <row r="142">
+      <c r="E142" t="inlineStr">
+        <is>
+          <t>355/65-15</t>
+        </is>
+      </c>
+      <c r="F142" t="inlineStr">
+        <is>
+          <t>Бел-230М</t>
+        </is>
+      </c>
+      <c r="G142" t="inlineStr">
+        <is>
+          <t>сер</t>
+        </is>
+      </c>
+      <c r="H142" t="n">
+        <v>2</v>
+      </c>
+      <c r="I142" s="1" t="n">
+        <v>44900</v>
+      </c>
+      <c r="J142" t="inlineStr">
+        <is>
+          <t>нет данных</t>
+        </is>
+      </c>
+    </row>
+    <row r="143">
+      <c r="E143" t="inlineStr">
+        <is>
+          <t>205/55R16</t>
+        </is>
+      </c>
+      <c r="F143" t="inlineStr">
+        <is>
+          <t>BEL-262</t>
+        </is>
+      </c>
+      <c r="G143" t="inlineStr">
+        <is>
+          <t>б/к, сер, легк</t>
+        </is>
+      </c>
+      <c r="H143" t="n">
+        <v>2</v>
+      </c>
+      <c r="I143" s="1" t="n">
+        <v>44900</v>
+      </c>
+      <c r="J143" t="inlineStr">
+        <is>
+          <t>нет данных</t>
+        </is>
+      </c>
+    </row>
+    <row r="144">
+      <c r="E144" t="inlineStr">
+        <is>
+          <t>205/55R16</t>
+        </is>
+      </c>
+      <c r="F144" t="inlineStr">
+        <is>
+          <t>BEL-317</t>
+        </is>
+      </c>
+      <c r="G144" t="inlineStr">
+        <is>
+          <t>б/к, сер, легк</t>
+        </is>
+      </c>
+      <c r="H144" t="n">
+        <v>2</v>
+      </c>
+      <c r="I144" s="1" t="n">
+        <v>44900</v>
+      </c>
+      <c r="J144" t="inlineStr">
+        <is>
+          <t>нет данных</t>
+        </is>
+      </c>
+    </row>
+    <row r="145">
+      <c r="E145" t="inlineStr">
+        <is>
+          <t>205/55R16</t>
+        </is>
+      </c>
+      <c r="F145" t="inlineStr">
+        <is>
+          <t>BEL-317S</t>
+        </is>
+      </c>
+      <c r="G145" t="inlineStr">
+        <is>
+          <t>сер, ошип</t>
+        </is>
+      </c>
+      <c r="H145" t="n">
+        <v>2</v>
+      </c>
+      <c r="I145" s="1" t="n">
+        <v>44900</v>
+      </c>
+      <c r="J145" t="inlineStr">
+        <is>
+          <t>нет данных</t>
+        </is>
+      </c>
+    </row>
+    <row r="146">
+      <c r="E146" t="inlineStr">
+        <is>
+          <t>205/60R16</t>
+        </is>
+      </c>
+      <c r="F146" t="inlineStr">
+        <is>
+          <t>BEL-277</t>
+        </is>
+      </c>
+      <c r="G146" t="inlineStr">
+        <is>
+          <t>б/к, сер, легк</t>
+        </is>
+      </c>
+      <c r="H146" t="n">
+        <v>2</v>
+      </c>
+      <c r="I146" s="1" t="n">
+        <v>44900</v>
+      </c>
+      <c r="J146" t="inlineStr">
         <is>
           <t>нет данных</t>
         </is>

</xml_diff>

<commit_message>
prices Onliner done 13/12/2022
</commit_message>
<xml_diff>
--- a/src/Tyres.xlsx
+++ b/src/Tyres.xlsx
@@ -417,7 +417,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J146"/>
+  <dimension ref="A1:J218"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -5052,6 +5052,2022 @@
         <v>44900</v>
       </c>
       <c r="J146" t="inlineStr">
+        <is>
+          <t>нет данных</t>
+        </is>
+      </c>
+    </row>
+    <row r="147">
+      <c r="E147" t="inlineStr">
+        <is>
+          <t>35/65-33</t>
+        </is>
+      </c>
+      <c r="F147" t="inlineStr">
+        <is>
+          <t>ФБел-283</t>
+        </is>
+      </c>
+      <c r="G147" t="inlineStr">
+        <is>
+          <t>42, груз, сер</t>
+        </is>
+      </c>
+      <c r="H147" t="n">
+        <v>2</v>
+      </c>
+      <c r="I147" s="1" t="n">
+        <v>44902</v>
+      </c>
+      <c r="J147" t="inlineStr">
+        <is>
+          <t>нет данных</t>
+        </is>
+      </c>
+    </row>
+    <row r="148">
+      <c r="E148" t="inlineStr">
+        <is>
+          <t>24.00R35</t>
+        </is>
+      </c>
+      <c r="F148" t="inlineStr">
+        <is>
+          <t>Бел-122</t>
+        </is>
+      </c>
+      <c r="G148" t="inlineStr">
+        <is>
+          <t>груз, сер, LS-2, Type</t>
+        </is>
+      </c>
+      <c r="H148" t="n">
+        <v>2</v>
+      </c>
+      <c r="I148" s="1" t="n">
+        <v>44902</v>
+      </c>
+      <c r="J148" t="inlineStr">
+        <is>
+          <t>нет данных</t>
+        </is>
+      </c>
+    </row>
+    <row r="149">
+      <c r="E149" t="inlineStr">
+        <is>
+          <t>24.00R35</t>
+        </is>
+      </c>
+      <c r="F149" t="inlineStr">
+        <is>
+          <t>Бел-122</t>
+        </is>
+      </c>
+      <c r="G149" t="inlineStr">
+        <is>
+          <t>груз, сер, Type, H</t>
+        </is>
+      </c>
+      <c r="H149" t="n">
+        <v>2</v>
+      </c>
+      <c r="I149" s="1" t="n">
+        <v>44902</v>
+      </c>
+      <c r="J149" t="inlineStr">
+        <is>
+          <t>нет данных</t>
+        </is>
+      </c>
+    </row>
+    <row r="150">
+      <c r="E150" t="inlineStr">
+        <is>
+          <t>24.00R35</t>
+        </is>
+      </c>
+      <c r="F150" t="inlineStr">
+        <is>
+          <t>Бел-122</t>
+        </is>
+      </c>
+      <c r="G150" t="inlineStr">
+        <is>
+          <t>груз, сер, Type, C</t>
+        </is>
+      </c>
+      <c r="H150" t="n">
+        <v>2</v>
+      </c>
+      <c r="I150" s="1" t="n">
+        <v>44902</v>
+      </c>
+      <c r="J150" t="inlineStr">
+        <is>
+          <t>нет данных</t>
+        </is>
+      </c>
+    </row>
+    <row r="151">
+      <c r="E151" t="inlineStr">
+        <is>
+          <t>24.00R35</t>
+        </is>
+      </c>
+      <c r="F151" t="inlineStr">
+        <is>
+          <t>Бел-202</t>
+        </is>
+      </c>
+      <c r="G151" t="inlineStr">
+        <is>
+          <t>210B, сер, LS-2, Type</t>
+        </is>
+      </c>
+      <c r="H151" t="n">
+        <v>2</v>
+      </c>
+      <c r="I151" s="1" t="n">
+        <v>44902</v>
+      </c>
+      <c r="J151" t="inlineStr">
+        <is>
+          <t>нет данных</t>
+        </is>
+      </c>
+    </row>
+    <row r="152">
+      <c r="E152" t="inlineStr">
+        <is>
+          <t>24.00R35</t>
+        </is>
+      </c>
+      <c r="F152" t="inlineStr">
+        <is>
+          <t>Бел-202</t>
+        </is>
+      </c>
+      <c r="G152" t="inlineStr">
+        <is>
+          <t>210B, сер, Type, H</t>
+        </is>
+      </c>
+      <c r="H152" t="n">
+        <v>2</v>
+      </c>
+      <c r="I152" s="1" t="n">
+        <v>44902</v>
+      </c>
+      <c r="J152" t="inlineStr">
+        <is>
+          <t>нет данных</t>
+        </is>
+      </c>
+    </row>
+    <row r="153">
+      <c r="E153" t="inlineStr">
+        <is>
+          <t>24.00R35</t>
+        </is>
+      </c>
+      <c r="F153" t="inlineStr">
+        <is>
+          <t>Бел-202</t>
+        </is>
+      </c>
+      <c r="G153" t="inlineStr">
+        <is>
+          <t>210B, сер, Type, C</t>
+        </is>
+      </c>
+      <c r="H153" t="n">
+        <v>2</v>
+      </c>
+      <c r="I153" s="1" t="n">
+        <v>44902</v>
+      </c>
+      <c r="J153" t="inlineStr">
+        <is>
+          <t>нет данных</t>
+        </is>
+      </c>
+    </row>
+    <row r="154">
+      <c r="E154" t="inlineStr">
+        <is>
+          <t>24.00R35</t>
+        </is>
+      </c>
+      <c r="F154" t="inlineStr">
+        <is>
+          <t>Бел-212</t>
+        </is>
+      </c>
+      <c r="G154" t="inlineStr">
+        <is>
+          <t>груз, сер, LS-2, Type</t>
+        </is>
+      </c>
+      <c r="H154" t="n">
+        <v>2</v>
+      </c>
+      <c r="I154" s="1" t="n">
+        <v>44902</v>
+      </c>
+      <c r="J154" t="inlineStr">
+        <is>
+          <t>нет данных</t>
+        </is>
+      </c>
+    </row>
+    <row r="155">
+      <c r="E155" t="inlineStr">
+        <is>
+          <t>24.00R35</t>
+        </is>
+      </c>
+      <c r="F155" t="inlineStr">
+        <is>
+          <t>Бел-212</t>
+        </is>
+      </c>
+      <c r="G155" t="inlineStr">
+        <is>
+          <t>груз, сер, Type, H</t>
+        </is>
+      </c>
+      <c r="H155" t="n">
+        <v>2</v>
+      </c>
+      <c r="I155" s="1" t="n">
+        <v>44902</v>
+      </c>
+      <c r="J155" t="inlineStr">
+        <is>
+          <t>нет данных</t>
+        </is>
+      </c>
+    </row>
+    <row r="156">
+      <c r="E156" t="inlineStr">
+        <is>
+          <t>24.00R35</t>
+        </is>
+      </c>
+      <c r="F156" t="inlineStr">
+        <is>
+          <t>Бел-212</t>
+        </is>
+      </c>
+      <c r="G156" t="inlineStr">
+        <is>
+          <t>груз, сер, Type, C</t>
+        </is>
+      </c>
+      <c r="H156" t="n">
+        <v>2</v>
+      </c>
+      <c r="I156" s="1" t="n">
+        <v>44902</v>
+      </c>
+      <c r="J156" t="inlineStr">
+        <is>
+          <t>нет данных</t>
+        </is>
+      </c>
+    </row>
+    <row r="157">
+      <c r="E157" t="inlineStr">
+        <is>
+          <t>21.00R35</t>
+        </is>
+      </c>
+      <c r="F157" t="inlineStr">
+        <is>
+          <t>Бел-200</t>
+        </is>
+      </c>
+      <c r="G157" t="inlineStr">
+        <is>
+          <t>202B, сер, LS-2, Type</t>
+        </is>
+      </c>
+      <c r="H157" t="n">
+        <v>2</v>
+      </c>
+      <c r="I157" s="1" t="n">
+        <v>44902</v>
+      </c>
+      <c r="J157" t="inlineStr">
+        <is>
+          <t>нет данных</t>
+        </is>
+      </c>
+    </row>
+    <row r="158">
+      <c r="E158" t="inlineStr">
+        <is>
+          <t>21.00R35</t>
+        </is>
+      </c>
+      <c r="F158" t="inlineStr">
+        <is>
+          <t>Бел-200</t>
+        </is>
+      </c>
+      <c r="G158" t="inlineStr">
+        <is>
+          <t>202B, сер, Type, H</t>
+        </is>
+      </c>
+      <c r="H158" t="n">
+        <v>2</v>
+      </c>
+      <c r="I158" s="1" t="n">
+        <v>44902</v>
+      </c>
+      <c r="J158" t="inlineStr">
+        <is>
+          <t>нет данных</t>
+        </is>
+      </c>
+    </row>
+    <row r="159">
+      <c r="E159" t="inlineStr">
+        <is>
+          <t>21.00R35</t>
+        </is>
+      </c>
+      <c r="F159" t="inlineStr">
+        <is>
+          <t>Бел-200</t>
+        </is>
+      </c>
+      <c r="G159" t="inlineStr">
+        <is>
+          <t>202B, сер, Type, C</t>
+        </is>
+      </c>
+      <c r="H159" t="n">
+        <v>2</v>
+      </c>
+      <c r="I159" s="1" t="n">
+        <v>44902</v>
+      </c>
+      <c r="J159" t="inlineStr">
+        <is>
+          <t>нет данных</t>
+        </is>
+      </c>
+    </row>
+    <row r="160">
+      <c r="E160" t="inlineStr">
+        <is>
+          <t>21.00R35</t>
+        </is>
+      </c>
+      <c r="F160" t="inlineStr">
+        <is>
+          <t>Бел-210</t>
+        </is>
+      </c>
+      <c r="G160" t="inlineStr">
+        <is>
+          <t>202B, сер, LS-2, Type</t>
+        </is>
+      </c>
+      <c r="H160" t="n">
+        <v>2</v>
+      </c>
+      <c r="I160" s="1" t="n">
+        <v>44902</v>
+      </c>
+      <c r="J160" t="inlineStr">
+        <is>
+          <t>нет данных</t>
+        </is>
+      </c>
+    </row>
+    <row r="161">
+      <c r="E161" t="inlineStr">
+        <is>
+          <t>21.00R35</t>
+        </is>
+      </c>
+      <c r="F161" t="inlineStr">
+        <is>
+          <t>Бел-210</t>
+        </is>
+      </c>
+      <c r="G161" t="inlineStr">
+        <is>
+          <t>202B, сер, Type, H</t>
+        </is>
+      </c>
+      <c r="H161" t="n">
+        <v>2</v>
+      </c>
+      <c r="I161" s="1" t="n">
+        <v>44902</v>
+      </c>
+      <c r="J161" t="inlineStr">
+        <is>
+          <t>нет данных</t>
+        </is>
+      </c>
+    </row>
+    <row r="162">
+      <c r="E162" t="inlineStr">
+        <is>
+          <t>21.00R35</t>
+        </is>
+      </c>
+      <c r="F162" t="inlineStr">
+        <is>
+          <t>Бел-210</t>
+        </is>
+      </c>
+      <c r="G162" t="inlineStr">
+        <is>
+          <t>202B, сер, Type, C</t>
+        </is>
+      </c>
+      <c r="H162" t="n">
+        <v>2</v>
+      </c>
+      <c r="I162" s="1" t="n">
+        <v>44902</v>
+      </c>
+      <c r="J162" t="inlineStr">
+        <is>
+          <t>нет данных</t>
+        </is>
+      </c>
+    </row>
+    <row r="163">
+      <c r="E163" t="inlineStr">
+        <is>
+          <t>14.00R20</t>
+        </is>
+      </c>
+      <c r="F163" t="inlineStr">
+        <is>
+          <t>BEL-248</t>
+        </is>
+      </c>
+      <c r="G163" t="inlineStr">
+        <is>
+          <t>груз, сер</t>
+        </is>
+      </c>
+      <c r="H163" t="n">
+        <v>2</v>
+      </c>
+      <c r="I163" s="1" t="n">
+        <v>44902</v>
+      </c>
+      <c r="J163" t="inlineStr">
+        <is>
+          <t>нет данных</t>
+        </is>
+      </c>
+    </row>
+    <row r="164">
+      <c r="E164" t="inlineStr">
+        <is>
+          <t>14.00R20</t>
+        </is>
+      </c>
+      <c r="F164" t="inlineStr">
+        <is>
+          <t>BEL-248</t>
+        </is>
+      </c>
+      <c r="G164" t="inlineStr">
+        <is>
+          <t>груз, сер</t>
+        </is>
+      </c>
+      <c r="H164" t="n">
+        <v>2</v>
+      </c>
+      <c r="I164" s="1" t="n">
+        <v>44902</v>
+      </c>
+      <c r="J164" t="inlineStr">
+        <is>
+          <t>нет данных</t>
+        </is>
+      </c>
+    </row>
+    <row r="165">
+      <c r="E165" t="inlineStr">
+        <is>
+          <t>14.00R20</t>
+        </is>
+      </c>
+      <c r="F165" t="inlineStr">
+        <is>
+          <t>BEL-248</t>
+        </is>
+      </c>
+      <c r="G165" t="inlineStr">
+        <is>
+          <t>б/к, груз, сер</t>
+        </is>
+      </c>
+      <c r="H165" t="n">
+        <v>2</v>
+      </c>
+      <c r="I165" s="1" t="n">
+        <v>44902</v>
+      </c>
+      <c r="J165" t="inlineStr">
+        <is>
+          <t>нет данных</t>
+        </is>
+      </c>
+    </row>
+    <row r="166">
+      <c r="E166" t="inlineStr">
+        <is>
+          <t>14.00R20</t>
+        </is>
+      </c>
+      <c r="F166" t="inlineStr">
+        <is>
+          <t>BEL-248</t>
+        </is>
+      </c>
+      <c r="G166" t="inlineStr">
+        <is>
+          <t>груз, сер</t>
+        </is>
+      </c>
+      <c r="H166" t="n">
+        <v>2</v>
+      </c>
+      <c r="I166" s="1" t="n">
+        <v>44902</v>
+      </c>
+      <c r="J166" t="inlineStr">
+        <is>
+          <t>нет данных</t>
+        </is>
+      </c>
+    </row>
+    <row r="167">
+      <c r="E167" t="inlineStr">
+        <is>
+          <t>12.00R20</t>
+        </is>
+      </c>
+      <c r="F167" t="inlineStr">
+        <is>
+          <t>BEL-288</t>
+        </is>
+      </c>
+      <c r="G167" t="inlineStr">
+        <is>
+          <t>груз, сер</t>
+        </is>
+      </c>
+      <c r="H167" t="n">
+        <v>2</v>
+      </c>
+      <c r="I167" s="1" t="n">
+        <v>44902</v>
+      </c>
+      <c r="J167" t="inlineStr">
+        <is>
+          <t>нет данных</t>
+        </is>
+      </c>
+    </row>
+    <row r="168">
+      <c r="E168" t="inlineStr">
+        <is>
+          <t>16.00R20</t>
+        </is>
+      </c>
+      <c r="F168" t="inlineStr">
+        <is>
+          <t>Бел-95</t>
+        </is>
+      </c>
+      <c r="G168" t="inlineStr">
+        <is>
+          <t>173G, б/к, груз, сер</t>
+        </is>
+      </c>
+      <c r="H168" t="n">
+        <v>2</v>
+      </c>
+      <c r="I168" s="1" t="n">
+        <v>44902</v>
+      </c>
+      <c r="J168" t="inlineStr">
+        <is>
+          <t>нет данных</t>
+        </is>
+      </c>
+    </row>
+    <row r="169">
+      <c r="E169" t="inlineStr">
+        <is>
+          <t>16.00R20</t>
+        </is>
+      </c>
+      <c r="F169" t="inlineStr">
+        <is>
+          <t>Бел-95</t>
+        </is>
+      </c>
+      <c r="G169" t="inlineStr">
+        <is>
+          <t>173G, груз, сер</t>
+        </is>
+      </c>
+      <c r="H169" t="n">
+        <v>2</v>
+      </c>
+      <c r="I169" s="1" t="n">
+        <v>44902</v>
+      </c>
+      <c r="J169" t="inlineStr">
+        <is>
+          <t>нет данных</t>
+        </is>
+      </c>
+    </row>
+    <row r="170">
+      <c r="E170" t="inlineStr">
+        <is>
+          <t>16.00R20</t>
+        </is>
+      </c>
+      <c r="F170" t="inlineStr">
+        <is>
+          <t>Бел-95</t>
+        </is>
+      </c>
+      <c r="G170" t="inlineStr">
+        <is>
+          <t>173G, груз, сер</t>
+        </is>
+      </c>
+      <c r="H170" t="n">
+        <v>2</v>
+      </c>
+      <c r="I170" s="1" t="n">
+        <v>44902</v>
+      </c>
+      <c r="J170" t="inlineStr">
+        <is>
+          <t>нет данных</t>
+        </is>
+      </c>
+    </row>
+    <row r="171">
+      <c r="E171" t="inlineStr">
+        <is>
+          <t>16.00R20</t>
+        </is>
+      </c>
+      <c r="F171" t="inlineStr">
+        <is>
+          <t>Бел-95</t>
+        </is>
+      </c>
+      <c r="G171" t="inlineStr">
+        <is>
+          <t>173G, груз, сер</t>
+        </is>
+      </c>
+      <c r="H171" t="n">
+        <v>2</v>
+      </c>
+      <c r="I171" s="1" t="n">
+        <v>44902</v>
+      </c>
+      <c r="J171" t="inlineStr">
+        <is>
+          <t>нет данных</t>
+        </is>
+      </c>
+    </row>
+    <row r="172">
+      <c r="E172" t="inlineStr">
+        <is>
+          <t>16.00R20</t>
+        </is>
+      </c>
+      <c r="F172" t="inlineStr">
+        <is>
+          <t>Бел-95</t>
+        </is>
+      </c>
+      <c r="G172" t="inlineStr">
+        <is>
+          <t>173G, груз, сер</t>
+        </is>
+      </c>
+      <c r="H172" t="n">
+        <v>2</v>
+      </c>
+      <c r="I172" s="1" t="n">
+        <v>44902</v>
+      </c>
+      <c r="J172" t="inlineStr">
+        <is>
+          <t>нет данных</t>
+        </is>
+      </c>
+    </row>
+    <row r="173">
+      <c r="E173" t="inlineStr">
+        <is>
+          <t>16.00R20</t>
+        </is>
+      </c>
+      <c r="F173" t="inlineStr">
+        <is>
+          <t>Бел-95</t>
+        </is>
+      </c>
+      <c r="G173" t="inlineStr">
+        <is>
+          <t>173G, груз, сер</t>
+        </is>
+      </c>
+      <c r="H173" t="n">
+        <v>2</v>
+      </c>
+      <c r="I173" s="1" t="n">
+        <v>44902</v>
+      </c>
+      <c r="J173" t="inlineStr">
+        <is>
+          <t>нет данных</t>
+        </is>
+      </c>
+    </row>
+    <row r="174">
+      <c r="E174" t="inlineStr">
+        <is>
+          <t>16.00R20</t>
+        </is>
+      </c>
+      <c r="F174" t="inlineStr">
+        <is>
+          <t>Бел-95</t>
+        </is>
+      </c>
+      <c r="G174" t="inlineStr">
+        <is>
+          <t>173G, сер</t>
+        </is>
+      </c>
+      <c r="H174" t="n">
+        <v>2</v>
+      </c>
+      <c r="I174" s="1" t="n">
+        <v>44902</v>
+      </c>
+      <c r="J174" t="inlineStr">
+        <is>
+          <t>нет данных</t>
+        </is>
+      </c>
+    </row>
+    <row r="175">
+      <c r="E175" t="inlineStr">
+        <is>
+          <t>395/85R20</t>
+        </is>
+      </c>
+      <c r="F175" t="inlineStr">
+        <is>
+          <t>BEL-405</t>
+        </is>
+      </c>
+      <c r="G175" t="inlineStr">
+        <is>
+          <t>168J, груз, сер</t>
+        </is>
+      </c>
+      <c r="H175" t="n">
+        <v>2</v>
+      </c>
+      <c r="I175" s="1" t="n">
+        <v>44902</v>
+      </c>
+      <c r="J175" t="inlineStr">
+        <is>
+          <t>нет данных</t>
+        </is>
+      </c>
+    </row>
+    <row r="176">
+      <c r="E176" t="inlineStr">
+        <is>
+          <t>445/65R22.5</t>
+        </is>
+      </c>
+      <c r="F176" t="inlineStr">
+        <is>
+          <t>Бел-145</t>
+        </is>
+      </c>
+      <c r="G176" t="inlineStr">
+        <is>
+          <t>б/к, груз, сер</t>
+        </is>
+      </c>
+      <c r="H176" t="n">
+        <v>2</v>
+      </c>
+      <c r="I176" s="1" t="n">
+        <v>44902</v>
+      </c>
+      <c r="J176" t="inlineStr">
+        <is>
+          <t>нет данных</t>
+        </is>
+      </c>
+    </row>
+    <row r="177">
+      <c r="E177" t="inlineStr">
+        <is>
+          <t>355/65-15</t>
+        </is>
+      </c>
+      <c r="F177" t="inlineStr">
+        <is>
+          <t>Бел-230</t>
+        </is>
+      </c>
+      <c r="G177" t="inlineStr">
+        <is>
+          <t>сер</t>
+        </is>
+      </c>
+      <c r="H177" t="n">
+        <v>2</v>
+      </c>
+      <c r="I177" s="1" t="n">
+        <v>44902</v>
+      </c>
+      <c r="J177" t="inlineStr">
+        <is>
+          <t>нет данных</t>
+        </is>
+      </c>
+    </row>
+    <row r="178">
+      <c r="E178" t="inlineStr">
+        <is>
+          <t>355/65-15</t>
+        </is>
+      </c>
+      <c r="F178" t="inlineStr">
+        <is>
+          <t>Бел-230М</t>
+        </is>
+      </c>
+      <c r="G178" t="inlineStr">
+        <is>
+          <t>сер</t>
+        </is>
+      </c>
+      <c r="H178" t="n">
+        <v>2</v>
+      </c>
+      <c r="I178" s="1" t="n">
+        <v>44902</v>
+      </c>
+      <c r="J178" t="inlineStr">
+        <is>
+          <t>нет данных</t>
+        </is>
+      </c>
+    </row>
+    <row r="179">
+      <c r="E179" t="inlineStr">
+        <is>
+          <t>205/55R16</t>
+        </is>
+      </c>
+      <c r="F179" t="inlineStr">
+        <is>
+          <t>BEL-262</t>
+        </is>
+      </c>
+      <c r="G179" t="inlineStr">
+        <is>
+          <t>б/к, сер, легк</t>
+        </is>
+      </c>
+      <c r="H179" t="n">
+        <v>2</v>
+      </c>
+      <c r="I179" s="1" t="n">
+        <v>44902</v>
+      </c>
+      <c r="J179" t="inlineStr">
+        <is>
+          <t>нет данных</t>
+        </is>
+      </c>
+    </row>
+    <row r="180">
+      <c r="E180" t="inlineStr">
+        <is>
+          <t>205/55R16</t>
+        </is>
+      </c>
+      <c r="F180" t="inlineStr">
+        <is>
+          <t>BEL-317</t>
+        </is>
+      </c>
+      <c r="G180" t="inlineStr">
+        <is>
+          <t>б/к, сер, легк</t>
+        </is>
+      </c>
+      <c r="H180" t="n">
+        <v>2</v>
+      </c>
+      <c r="I180" s="1" t="n">
+        <v>44902</v>
+      </c>
+      <c r="J180" t="inlineStr">
+        <is>
+          <t>нет данных</t>
+        </is>
+      </c>
+    </row>
+    <row r="181">
+      <c r="E181" t="inlineStr">
+        <is>
+          <t>205/55R16</t>
+        </is>
+      </c>
+      <c r="F181" t="inlineStr">
+        <is>
+          <t>BEL-317S</t>
+        </is>
+      </c>
+      <c r="G181" t="inlineStr">
+        <is>
+          <t>сер, ошип</t>
+        </is>
+      </c>
+      <c r="H181" t="n">
+        <v>2</v>
+      </c>
+      <c r="I181" s="1" t="n">
+        <v>44902</v>
+      </c>
+      <c r="J181" t="inlineStr">
+        <is>
+          <t>нет данных</t>
+        </is>
+      </c>
+    </row>
+    <row r="182">
+      <c r="E182" t="inlineStr">
+        <is>
+          <t>205/60R16</t>
+        </is>
+      </c>
+      <c r="F182" t="inlineStr">
+        <is>
+          <t>BEL-277</t>
+        </is>
+      </c>
+      <c r="G182" t="inlineStr">
+        <is>
+          <t>б/к, сер, легк</t>
+        </is>
+      </c>
+      <c r="H182" t="n">
+        <v>2</v>
+      </c>
+      <c r="I182" s="1" t="n">
+        <v>44902</v>
+      </c>
+      <c r="J182" t="inlineStr">
+        <is>
+          <t>нет данных</t>
+        </is>
+      </c>
+    </row>
+    <row r="183">
+      <c r="E183" t="inlineStr">
+        <is>
+          <t>35/65-33</t>
+        </is>
+      </c>
+      <c r="F183" t="inlineStr">
+        <is>
+          <t>ФБел-283</t>
+        </is>
+      </c>
+      <c r="G183" t="inlineStr">
+        <is>
+          <t>42, груз, сер</t>
+        </is>
+      </c>
+      <c r="H183" t="n">
+        <v>2</v>
+      </c>
+      <c r="I183" s="1" t="n">
+        <v>44906</v>
+      </c>
+      <c r="J183" t="inlineStr">
+        <is>
+          <t>нет данных</t>
+        </is>
+      </c>
+    </row>
+    <row r="184">
+      <c r="E184" t="inlineStr">
+        <is>
+          <t>24.00R35</t>
+        </is>
+      </c>
+      <c r="F184" t="inlineStr">
+        <is>
+          <t>Бел-122</t>
+        </is>
+      </c>
+      <c r="G184" t="inlineStr">
+        <is>
+          <t>груз, сер, LS-2, Type</t>
+        </is>
+      </c>
+      <c r="H184" t="n">
+        <v>2</v>
+      </c>
+      <c r="I184" s="1" t="n">
+        <v>44906</v>
+      </c>
+      <c r="J184" t="inlineStr">
+        <is>
+          <t>нет данных</t>
+        </is>
+      </c>
+    </row>
+    <row r="185">
+      <c r="E185" t="inlineStr">
+        <is>
+          <t>24.00R35</t>
+        </is>
+      </c>
+      <c r="F185" t="inlineStr">
+        <is>
+          <t>Бел-122</t>
+        </is>
+      </c>
+      <c r="G185" t="inlineStr">
+        <is>
+          <t>груз, сер, Type, H</t>
+        </is>
+      </c>
+      <c r="H185" t="n">
+        <v>2</v>
+      </c>
+      <c r="I185" s="1" t="n">
+        <v>44906</v>
+      </c>
+      <c r="J185" t="inlineStr">
+        <is>
+          <t>нет данных</t>
+        </is>
+      </c>
+    </row>
+    <row r="186">
+      <c r="E186" t="inlineStr">
+        <is>
+          <t>24.00R35</t>
+        </is>
+      </c>
+      <c r="F186" t="inlineStr">
+        <is>
+          <t>Бел-122</t>
+        </is>
+      </c>
+      <c r="G186" t="inlineStr">
+        <is>
+          <t>груз, сер, Type, C</t>
+        </is>
+      </c>
+      <c r="H186" t="n">
+        <v>2</v>
+      </c>
+      <c r="I186" s="1" t="n">
+        <v>44906</v>
+      </c>
+      <c r="J186" t="inlineStr">
+        <is>
+          <t>нет данных</t>
+        </is>
+      </c>
+    </row>
+    <row r="187">
+      <c r="E187" t="inlineStr">
+        <is>
+          <t>24.00R35</t>
+        </is>
+      </c>
+      <c r="F187" t="inlineStr">
+        <is>
+          <t>Бел-202</t>
+        </is>
+      </c>
+      <c r="G187" t="inlineStr">
+        <is>
+          <t>210B, сер, LS-2, Type</t>
+        </is>
+      </c>
+      <c r="H187" t="n">
+        <v>2</v>
+      </c>
+      <c r="I187" s="1" t="n">
+        <v>44906</v>
+      </c>
+      <c r="J187" t="inlineStr">
+        <is>
+          <t>нет данных</t>
+        </is>
+      </c>
+    </row>
+    <row r="188">
+      <c r="E188" t="inlineStr">
+        <is>
+          <t>24.00R35</t>
+        </is>
+      </c>
+      <c r="F188" t="inlineStr">
+        <is>
+          <t>Бел-202</t>
+        </is>
+      </c>
+      <c r="G188" t="inlineStr">
+        <is>
+          <t>210B, сер, Type, H</t>
+        </is>
+      </c>
+      <c r="H188" t="n">
+        <v>2</v>
+      </c>
+      <c r="I188" s="1" t="n">
+        <v>44906</v>
+      </c>
+      <c r="J188" t="inlineStr">
+        <is>
+          <t>нет данных</t>
+        </is>
+      </c>
+    </row>
+    <row r="189">
+      <c r="E189" t="inlineStr">
+        <is>
+          <t>24.00R35</t>
+        </is>
+      </c>
+      <c r="F189" t="inlineStr">
+        <is>
+          <t>Бел-202</t>
+        </is>
+      </c>
+      <c r="G189" t="inlineStr">
+        <is>
+          <t>210B, сер, Type, C</t>
+        </is>
+      </c>
+      <c r="H189" t="n">
+        <v>2</v>
+      </c>
+      <c r="I189" s="1" t="n">
+        <v>44906</v>
+      </c>
+      <c r="J189" t="inlineStr">
+        <is>
+          <t>нет данных</t>
+        </is>
+      </c>
+    </row>
+    <row r="190">
+      <c r="E190" t="inlineStr">
+        <is>
+          <t>24.00R35</t>
+        </is>
+      </c>
+      <c r="F190" t="inlineStr">
+        <is>
+          <t>Бел-212</t>
+        </is>
+      </c>
+      <c r="G190" t="inlineStr">
+        <is>
+          <t>груз, сер, LS-2, Type</t>
+        </is>
+      </c>
+      <c r="H190" t="n">
+        <v>2</v>
+      </c>
+      <c r="I190" s="1" t="n">
+        <v>44906</v>
+      </c>
+      <c r="J190" t="inlineStr">
+        <is>
+          <t>нет данных</t>
+        </is>
+      </c>
+    </row>
+    <row r="191">
+      <c r="E191" t="inlineStr">
+        <is>
+          <t>24.00R35</t>
+        </is>
+      </c>
+      <c r="F191" t="inlineStr">
+        <is>
+          <t>Бел-212</t>
+        </is>
+      </c>
+      <c r="G191" t="inlineStr">
+        <is>
+          <t>груз, сер, Type, H</t>
+        </is>
+      </c>
+      <c r="H191" t="n">
+        <v>2</v>
+      </c>
+      <c r="I191" s="1" t="n">
+        <v>44906</v>
+      </c>
+      <c r="J191" t="inlineStr">
+        <is>
+          <t>нет данных</t>
+        </is>
+      </c>
+    </row>
+    <row r="192">
+      <c r="E192" t="inlineStr">
+        <is>
+          <t>24.00R35</t>
+        </is>
+      </c>
+      <c r="F192" t="inlineStr">
+        <is>
+          <t>Бел-212</t>
+        </is>
+      </c>
+      <c r="G192" t="inlineStr">
+        <is>
+          <t>груз, сер, Type, C</t>
+        </is>
+      </c>
+      <c r="H192" t="n">
+        <v>2</v>
+      </c>
+      <c r="I192" s="1" t="n">
+        <v>44906</v>
+      </c>
+      <c r="J192" t="inlineStr">
+        <is>
+          <t>нет данных</t>
+        </is>
+      </c>
+    </row>
+    <row r="193">
+      <c r="E193" t="inlineStr">
+        <is>
+          <t>21.00R35</t>
+        </is>
+      </c>
+      <c r="F193" t="inlineStr">
+        <is>
+          <t>Бел-200</t>
+        </is>
+      </c>
+      <c r="G193" t="inlineStr">
+        <is>
+          <t>202B, сер, LS-2, Type</t>
+        </is>
+      </c>
+      <c r="H193" t="n">
+        <v>2</v>
+      </c>
+      <c r="I193" s="1" t="n">
+        <v>44906</v>
+      </c>
+      <c r="J193" t="inlineStr">
+        <is>
+          <t>нет данных</t>
+        </is>
+      </c>
+    </row>
+    <row r="194">
+      <c r="E194" t="inlineStr">
+        <is>
+          <t>21.00R35</t>
+        </is>
+      </c>
+      <c r="F194" t="inlineStr">
+        <is>
+          <t>Бел-200</t>
+        </is>
+      </c>
+      <c r="G194" t="inlineStr">
+        <is>
+          <t>202B, сер, Type, H</t>
+        </is>
+      </c>
+      <c r="H194" t="n">
+        <v>2</v>
+      </c>
+      <c r="I194" s="1" t="n">
+        <v>44906</v>
+      </c>
+      <c r="J194" t="inlineStr">
+        <is>
+          <t>нет данных</t>
+        </is>
+      </c>
+    </row>
+    <row r="195">
+      <c r="E195" t="inlineStr">
+        <is>
+          <t>21.00R35</t>
+        </is>
+      </c>
+      <c r="F195" t="inlineStr">
+        <is>
+          <t>Бел-200</t>
+        </is>
+      </c>
+      <c r="G195" t="inlineStr">
+        <is>
+          <t>202B, сер, Type, C</t>
+        </is>
+      </c>
+      <c r="H195" t="n">
+        <v>2</v>
+      </c>
+      <c r="I195" s="1" t="n">
+        <v>44906</v>
+      </c>
+      <c r="J195" t="inlineStr">
+        <is>
+          <t>нет данных</t>
+        </is>
+      </c>
+    </row>
+    <row r="196">
+      <c r="E196" t="inlineStr">
+        <is>
+          <t>21.00R35</t>
+        </is>
+      </c>
+      <c r="F196" t="inlineStr">
+        <is>
+          <t>Бел-210</t>
+        </is>
+      </c>
+      <c r="G196" t="inlineStr">
+        <is>
+          <t>202B, сер, LS-2, Type</t>
+        </is>
+      </c>
+      <c r="H196" t="n">
+        <v>2</v>
+      </c>
+      <c r="I196" s="1" t="n">
+        <v>44906</v>
+      </c>
+      <c r="J196" t="inlineStr">
+        <is>
+          <t>нет данных</t>
+        </is>
+      </c>
+    </row>
+    <row r="197">
+      <c r="E197" t="inlineStr">
+        <is>
+          <t>21.00R35</t>
+        </is>
+      </c>
+      <c r="F197" t="inlineStr">
+        <is>
+          <t>Бел-210</t>
+        </is>
+      </c>
+      <c r="G197" t="inlineStr">
+        <is>
+          <t>202B, сер, Type, H</t>
+        </is>
+      </c>
+      <c r="H197" t="n">
+        <v>2</v>
+      </c>
+      <c r="I197" s="1" t="n">
+        <v>44906</v>
+      </c>
+      <c r="J197" t="inlineStr">
+        <is>
+          <t>нет данных</t>
+        </is>
+      </c>
+    </row>
+    <row r="198">
+      <c r="E198" t="inlineStr">
+        <is>
+          <t>21.00R35</t>
+        </is>
+      </c>
+      <c r="F198" t="inlineStr">
+        <is>
+          <t>Бел-210</t>
+        </is>
+      </c>
+      <c r="G198" t="inlineStr">
+        <is>
+          <t>202B, сер, Type, C</t>
+        </is>
+      </c>
+      <c r="H198" t="n">
+        <v>2</v>
+      </c>
+      <c r="I198" s="1" t="n">
+        <v>44906</v>
+      </c>
+      <c r="J198" t="inlineStr">
+        <is>
+          <t>нет данных</t>
+        </is>
+      </c>
+    </row>
+    <row r="199">
+      <c r="E199" t="inlineStr">
+        <is>
+          <t>14.00R20</t>
+        </is>
+      </c>
+      <c r="F199" t="inlineStr">
+        <is>
+          <t>BEL-248</t>
+        </is>
+      </c>
+      <c r="G199" t="inlineStr">
+        <is>
+          <t>груз, сер</t>
+        </is>
+      </c>
+      <c r="H199" t="n">
+        <v>2</v>
+      </c>
+      <c r="I199" s="1" t="n">
+        <v>44906</v>
+      </c>
+      <c r="J199" t="inlineStr">
+        <is>
+          <t>нет данных</t>
+        </is>
+      </c>
+    </row>
+    <row r="200">
+      <c r="E200" t="inlineStr">
+        <is>
+          <t>14.00R20</t>
+        </is>
+      </c>
+      <c r="F200" t="inlineStr">
+        <is>
+          <t>BEL-248</t>
+        </is>
+      </c>
+      <c r="G200" t="inlineStr">
+        <is>
+          <t>груз, сер</t>
+        </is>
+      </c>
+      <c r="H200" t="n">
+        <v>2</v>
+      </c>
+      <c r="I200" s="1" t="n">
+        <v>44906</v>
+      </c>
+      <c r="J200" t="inlineStr">
+        <is>
+          <t>нет данных</t>
+        </is>
+      </c>
+    </row>
+    <row r="201">
+      <c r="E201" t="inlineStr">
+        <is>
+          <t>14.00R20</t>
+        </is>
+      </c>
+      <c r="F201" t="inlineStr">
+        <is>
+          <t>BEL-248</t>
+        </is>
+      </c>
+      <c r="G201" t="inlineStr">
+        <is>
+          <t>б/к, груз, сер</t>
+        </is>
+      </c>
+      <c r="H201" t="n">
+        <v>2</v>
+      </c>
+      <c r="I201" s="1" t="n">
+        <v>44906</v>
+      </c>
+      <c r="J201" t="inlineStr">
+        <is>
+          <t>нет данных</t>
+        </is>
+      </c>
+    </row>
+    <row r="202">
+      <c r="E202" t="inlineStr">
+        <is>
+          <t>14.00R20</t>
+        </is>
+      </c>
+      <c r="F202" t="inlineStr">
+        <is>
+          <t>BEL-248</t>
+        </is>
+      </c>
+      <c r="G202" t="inlineStr">
+        <is>
+          <t>груз, сер</t>
+        </is>
+      </c>
+      <c r="H202" t="n">
+        <v>2</v>
+      </c>
+      <c r="I202" s="1" t="n">
+        <v>44906</v>
+      </c>
+      <c r="J202" t="inlineStr">
+        <is>
+          <t>нет данных</t>
+        </is>
+      </c>
+    </row>
+    <row r="203">
+      <c r="E203" t="inlineStr">
+        <is>
+          <t>12.00R20</t>
+        </is>
+      </c>
+      <c r="F203" t="inlineStr">
+        <is>
+          <t>BEL-288</t>
+        </is>
+      </c>
+      <c r="G203" t="inlineStr">
+        <is>
+          <t>груз, сер</t>
+        </is>
+      </c>
+      <c r="H203" t="n">
+        <v>2</v>
+      </c>
+      <c r="I203" s="1" t="n">
+        <v>44906</v>
+      </c>
+      <c r="J203" t="inlineStr">
+        <is>
+          <t>нет данных</t>
+        </is>
+      </c>
+    </row>
+    <row r="204">
+      <c r="E204" t="inlineStr">
+        <is>
+          <t>16.00R20</t>
+        </is>
+      </c>
+      <c r="F204" t="inlineStr">
+        <is>
+          <t>Бел-95</t>
+        </is>
+      </c>
+      <c r="G204" t="inlineStr">
+        <is>
+          <t>173G, б/к, груз, сер</t>
+        </is>
+      </c>
+      <c r="H204" t="n">
+        <v>2</v>
+      </c>
+      <c r="I204" s="1" t="n">
+        <v>44906</v>
+      </c>
+      <c r="J204" t="inlineStr">
+        <is>
+          <t>нет данных</t>
+        </is>
+      </c>
+    </row>
+    <row r="205">
+      <c r="E205" t="inlineStr">
+        <is>
+          <t>16.00R20</t>
+        </is>
+      </c>
+      <c r="F205" t="inlineStr">
+        <is>
+          <t>Бел-95</t>
+        </is>
+      </c>
+      <c r="G205" t="inlineStr">
+        <is>
+          <t>173G, груз, сер</t>
+        </is>
+      </c>
+      <c r="H205" t="n">
+        <v>2</v>
+      </c>
+      <c r="I205" s="1" t="n">
+        <v>44906</v>
+      </c>
+      <c r="J205" t="inlineStr">
+        <is>
+          <t>нет данных</t>
+        </is>
+      </c>
+    </row>
+    <row r="206">
+      <c r="E206" t="inlineStr">
+        <is>
+          <t>16.00R20</t>
+        </is>
+      </c>
+      <c r="F206" t="inlineStr">
+        <is>
+          <t>Бел-95</t>
+        </is>
+      </c>
+      <c r="G206" t="inlineStr">
+        <is>
+          <t>173G, груз, сер</t>
+        </is>
+      </c>
+      <c r="H206" t="n">
+        <v>2</v>
+      </c>
+      <c r="I206" s="1" t="n">
+        <v>44906</v>
+      </c>
+      <c r="J206" t="inlineStr">
+        <is>
+          <t>нет данных</t>
+        </is>
+      </c>
+    </row>
+    <row r="207">
+      <c r="E207" t="inlineStr">
+        <is>
+          <t>16.00R20</t>
+        </is>
+      </c>
+      <c r="F207" t="inlineStr">
+        <is>
+          <t>Бел-95</t>
+        </is>
+      </c>
+      <c r="G207" t="inlineStr">
+        <is>
+          <t>173G, груз, сер</t>
+        </is>
+      </c>
+      <c r="H207" t="n">
+        <v>2</v>
+      </c>
+      <c r="I207" s="1" t="n">
+        <v>44906</v>
+      </c>
+      <c r="J207" t="inlineStr">
+        <is>
+          <t>нет данных</t>
+        </is>
+      </c>
+    </row>
+    <row r="208">
+      <c r="E208" t="inlineStr">
+        <is>
+          <t>16.00R20</t>
+        </is>
+      </c>
+      <c r="F208" t="inlineStr">
+        <is>
+          <t>Бел-95</t>
+        </is>
+      </c>
+      <c r="G208" t="inlineStr">
+        <is>
+          <t>173G, груз, сер</t>
+        </is>
+      </c>
+      <c r="H208" t="n">
+        <v>2</v>
+      </c>
+      <c r="I208" s="1" t="n">
+        <v>44906</v>
+      </c>
+      <c r="J208" t="inlineStr">
+        <is>
+          <t>нет данных</t>
+        </is>
+      </c>
+    </row>
+    <row r="209">
+      <c r="E209" t="inlineStr">
+        <is>
+          <t>16.00R20</t>
+        </is>
+      </c>
+      <c r="F209" t="inlineStr">
+        <is>
+          <t>Бел-95</t>
+        </is>
+      </c>
+      <c r="G209" t="inlineStr">
+        <is>
+          <t>173G, груз, сер</t>
+        </is>
+      </c>
+      <c r="H209" t="n">
+        <v>2</v>
+      </c>
+      <c r="I209" s="1" t="n">
+        <v>44906</v>
+      </c>
+      <c r="J209" t="inlineStr">
+        <is>
+          <t>нет данных</t>
+        </is>
+      </c>
+    </row>
+    <row r="210">
+      <c r="E210" t="inlineStr">
+        <is>
+          <t>16.00R20</t>
+        </is>
+      </c>
+      <c r="F210" t="inlineStr">
+        <is>
+          <t>Бел-95</t>
+        </is>
+      </c>
+      <c r="G210" t="inlineStr">
+        <is>
+          <t>173G, сер</t>
+        </is>
+      </c>
+      <c r="H210" t="n">
+        <v>2</v>
+      </c>
+      <c r="I210" s="1" t="n">
+        <v>44906</v>
+      </c>
+      <c r="J210" t="inlineStr">
+        <is>
+          <t>нет данных</t>
+        </is>
+      </c>
+    </row>
+    <row r="211">
+      <c r="E211" t="inlineStr">
+        <is>
+          <t>395/85R20</t>
+        </is>
+      </c>
+      <c r="F211" t="inlineStr">
+        <is>
+          <t>BEL-405</t>
+        </is>
+      </c>
+      <c r="G211" t="inlineStr">
+        <is>
+          <t>168J, груз, сер</t>
+        </is>
+      </c>
+      <c r="H211" t="n">
+        <v>2</v>
+      </c>
+      <c r="I211" s="1" t="n">
+        <v>44906</v>
+      </c>
+      <c r="J211" t="inlineStr">
+        <is>
+          <t>нет данных</t>
+        </is>
+      </c>
+    </row>
+    <row r="212">
+      <c r="E212" t="inlineStr">
+        <is>
+          <t>445/65R22.5</t>
+        </is>
+      </c>
+      <c r="F212" t="inlineStr">
+        <is>
+          <t>Бел-145</t>
+        </is>
+      </c>
+      <c r="G212" t="inlineStr">
+        <is>
+          <t>б/к, груз, сер</t>
+        </is>
+      </c>
+      <c r="H212" t="n">
+        <v>2</v>
+      </c>
+      <c r="I212" s="1" t="n">
+        <v>44906</v>
+      </c>
+      <c r="J212" t="inlineStr">
+        <is>
+          <t>нет данных</t>
+        </is>
+      </c>
+    </row>
+    <row r="213">
+      <c r="E213" t="inlineStr">
+        <is>
+          <t>355/65-15</t>
+        </is>
+      </c>
+      <c r="F213" t="inlineStr">
+        <is>
+          <t>Бел-230</t>
+        </is>
+      </c>
+      <c r="G213" t="inlineStr">
+        <is>
+          <t>сер</t>
+        </is>
+      </c>
+      <c r="H213" t="n">
+        <v>2</v>
+      </c>
+      <c r="I213" s="1" t="n">
+        <v>44906</v>
+      </c>
+      <c r="J213" t="inlineStr">
+        <is>
+          <t>нет данных</t>
+        </is>
+      </c>
+    </row>
+    <row r="214">
+      <c r="E214" t="inlineStr">
+        <is>
+          <t>355/65-15</t>
+        </is>
+      </c>
+      <c r="F214" t="inlineStr">
+        <is>
+          <t>Бел-230М</t>
+        </is>
+      </c>
+      <c r="G214" t="inlineStr">
+        <is>
+          <t>сер</t>
+        </is>
+      </c>
+      <c r="H214" t="n">
+        <v>2</v>
+      </c>
+      <c r="I214" s="1" t="n">
+        <v>44906</v>
+      </c>
+      <c r="J214" t="inlineStr">
+        <is>
+          <t>нет данных</t>
+        </is>
+      </c>
+    </row>
+    <row r="215">
+      <c r="E215" t="inlineStr">
+        <is>
+          <t>205/55R16</t>
+        </is>
+      </c>
+      <c r="F215" t="inlineStr">
+        <is>
+          <t>BEL-262</t>
+        </is>
+      </c>
+      <c r="G215" t="inlineStr">
+        <is>
+          <t>б/к, сер, легк</t>
+        </is>
+      </c>
+      <c r="H215" t="n">
+        <v>2</v>
+      </c>
+      <c r="I215" s="1" t="n">
+        <v>44906</v>
+      </c>
+      <c r="J215" t="inlineStr">
+        <is>
+          <t>нет данных</t>
+        </is>
+      </c>
+    </row>
+    <row r="216">
+      <c r="E216" t="inlineStr">
+        <is>
+          <t>205/55R16</t>
+        </is>
+      </c>
+      <c r="F216" t="inlineStr">
+        <is>
+          <t>BEL-317</t>
+        </is>
+      </c>
+      <c r="G216" t="inlineStr">
+        <is>
+          <t>б/к, сер, легк</t>
+        </is>
+      </c>
+      <c r="H216" t="n">
+        <v>2</v>
+      </c>
+      <c r="I216" s="1" t="n">
+        <v>44906</v>
+      </c>
+      <c r="J216" t="inlineStr">
+        <is>
+          <t>нет данных</t>
+        </is>
+      </c>
+    </row>
+    <row r="217">
+      <c r="E217" t="inlineStr">
+        <is>
+          <t>205/55R16</t>
+        </is>
+      </c>
+      <c r="F217" t="inlineStr">
+        <is>
+          <t>BEL-317S</t>
+        </is>
+      </c>
+      <c r="G217" t="inlineStr">
+        <is>
+          <t>сер, ошип</t>
+        </is>
+      </c>
+      <c r="H217" t="n">
+        <v>2</v>
+      </c>
+      <c r="I217" s="1" t="n">
+        <v>44906</v>
+      </c>
+      <c r="J217" t="inlineStr">
+        <is>
+          <t>нет данных</t>
+        </is>
+      </c>
+    </row>
+    <row r="218">
+      <c r="E218" t="inlineStr">
+        <is>
+          <t>205/60R16</t>
+        </is>
+      </c>
+      <c r="F218" t="inlineStr">
+        <is>
+          <t>BEL-277</t>
+        </is>
+      </c>
+      <c r="G218" t="inlineStr">
+        <is>
+          <t>б/к, сер, легк</t>
+        </is>
+      </c>
+      <c r="H218" t="n">
+        <v>2</v>
+      </c>
+      <c r="I218" s="1" t="n">
+        <v>44906</v>
+      </c>
+      <c r="J218" t="inlineStr">
         <is>
           <t>нет данных</t>
         </is>

</xml_diff>

<commit_message>
prices Onliner season filter done at 19/12/2022
</commit_message>
<xml_diff>
--- a/src/Tyres.xlsx
+++ b/src/Tyres.xlsx
@@ -417,7 +417,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J277"/>
+  <dimension ref="A1:J300"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -8720,6 +8720,650 @@
         <v>44909</v>
       </c>
       <c r="J277" t="inlineStr">
+        <is>
+          <t>нет данных</t>
+        </is>
+      </c>
+    </row>
+    <row r="278">
+      <c r="E278" t="inlineStr">
+        <is>
+          <t>35/65-33</t>
+        </is>
+      </c>
+      <c r="F278" t="inlineStr">
+        <is>
+          <t>ФБел-283</t>
+        </is>
+      </c>
+      <c r="G278" t="inlineStr">
+        <is>
+          <t>42, груз, сер</t>
+        </is>
+      </c>
+      <c r="H278" t="n">
+        <v>2</v>
+      </c>
+      <c r="I278" s="1" t="n">
+        <v>44910</v>
+      </c>
+      <c r="J278" t="inlineStr">
+        <is>
+          <t>нет данных</t>
+        </is>
+      </c>
+    </row>
+    <row r="279">
+      <c r="E279" t="inlineStr">
+        <is>
+          <t>205/55R16</t>
+        </is>
+      </c>
+      <c r="F279" t="inlineStr">
+        <is>
+          <t>BEL-262</t>
+        </is>
+      </c>
+      <c r="G279" t="inlineStr">
+        <is>
+          <t>б/к, сер, легк</t>
+        </is>
+      </c>
+      <c r="H279" t="n">
+        <v>2</v>
+      </c>
+      <c r="I279" s="1" t="n">
+        <v>44910</v>
+      </c>
+      <c r="J279" t="inlineStr">
+        <is>
+          <t>нет данных</t>
+        </is>
+      </c>
+    </row>
+    <row r="280">
+      <c r="E280" t="inlineStr">
+        <is>
+          <t>205/55R16</t>
+        </is>
+      </c>
+      <c r="F280" t="inlineStr">
+        <is>
+          <t>BEL-317</t>
+        </is>
+      </c>
+      <c r="G280" t="inlineStr">
+        <is>
+          <t>б/к, сер, легк</t>
+        </is>
+      </c>
+      <c r="H280" t="n">
+        <v>2</v>
+      </c>
+      <c r="I280" s="1" t="n">
+        <v>44910</v>
+      </c>
+      <c r="J280" t="inlineStr">
+        <is>
+          <t>нет данных</t>
+        </is>
+      </c>
+    </row>
+    <row r="281">
+      <c r="E281" t="inlineStr">
+        <is>
+          <t>205/55R16</t>
+        </is>
+      </c>
+      <c r="F281" t="inlineStr">
+        <is>
+          <t>BEL-317S</t>
+        </is>
+      </c>
+      <c r="G281" t="inlineStr">
+        <is>
+          <t>сер, ошип</t>
+        </is>
+      </c>
+      <c r="H281" t="n">
+        <v>2</v>
+      </c>
+      <c r="I281" s="1" t="n">
+        <v>44910</v>
+      </c>
+      <c r="J281" t="inlineStr">
+        <is>
+          <t>нет данных</t>
+        </is>
+      </c>
+    </row>
+    <row r="282">
+      <c r="E282" t="inlineStr">
+        <is>
+          <t>24.00R35</t>
+        </is>
+      </c>
+      <c r="F282" t="inlineStr">
+        <is>
+          <t>Бел-122</t>
+        </is>
+      </c>
+      <c r="G282" t="inlineStr">
+        <is>
+          <t>груз, сер, LS-2, Type</t>
+        </is>
+      </c>
+      <c r="H282" t="n">
+        <v>2</v>
+      </c>
+      <c r="I282" s="1" t="n">
+        <v>44910</v>
+      </c>
+      <c r="J282" t="inlineStr">
+        <is>
+          <t>нет данных</t>
+        </is>
+      </c>
+    </row>
+    <row r="283">
+      <c r="E283" t="inlineStr">
+        <is>
+          <t>24.00R35</t>
+        </is>
+      </c>
+      <c r="F283" t="inlineStr">
+        <is>
+          <t>Бел-122</t>
+        </is>
+      </c>
+      <c r="G283" t="inlineStr">
+        <is>
+          <t>груз, сер, Type, H</t>
+        </is>
+      </c>
+      <c r="H283" t="n">
+        <v>2</v>
+      </c>
+      <c r="I283" s="1" t="n">
+        <v>44910</v>
+      </c>
+      <c r="J283" t="inlineStr">
+        <is>
+          <t>нет данных</t>
+        </is>
+      </c>
+    </row>
+    <row r="284">
+      <c r="E284" t="inlineStr">
+        <is>
+          <t>24.00R35</t>
+        </is>
+      </c>
+      <c r="F284" t="inlineStr">
+        <is>
+          <t>Бел-122</t>
+        </is>
+      </c>
+      <c r="G284" t="inlineStr">
+        <is>
+          <t>груз, сер, Type, C</t>
+        </is>
+      </c>
+      <c r="H284" t="n">
+        <v>2</v>
+      </c>
+      <c r="I284" s="1" t="n">
+        <v>44910</v>
+      </c>
+      <c r="J284" t="inlineStr">
+        <is>
+          <t>нет данных</t>
+        </is>
+      </c>
+    </row>
+    <row r="285">
+      <c r="E285" t="inlineStr">
+        <is>
+          <t>24.00R35</t>
+        </is>
+      </c>
+      <c r="F285" t="inlineStr">
+        <is>
+          <t>Бел-202</t>
+        </is>
+      </c>
+      <c r="G285" t="inlineStr">
+        <is>
+          <t>210B, сер, LS-2, Type</t>
+        </is>
+      </c>
+      <c r="H285" t="n">
+        <v>2</v>
+      </c>
+      <c r="I285" s="1" t="n">
+        <v>44910</v>
+      </c>
+      <c r="J285" t="inlineStr">
+        <is>
+          <t>нет данных</t>
+        </is>
+      </c>
+    </row>
+    <row r="286">
+      <c r="E286" t="inlineStr">
+        <is>
+          <t>24.00R35</t>
+        </is>
+      </c>
+      <c r="F286" t="inlineStr">
+        <is>
+          <t>Бел-202</t>
+        </is>
+      </c>
+      <c r="G286" t="inlineStr">
+        <is>
+          <t>210B, сер, Type, H</t>
+        </is>
+      </c>
+      <c r="H286" t="n">
+        <v>2</v>
+      </c>
+      <c r="I286" s="1" t="n">
+        <v>44910</v>
+      </c>
+      <c r="J286" t="inlineStr">
+        <is>
+          <t>нет данных</t>
+        </is>
+      </c>
+    </row>
+    <row r="287">
+      <c r="E287" t="inlineStr">
+        <is>
+          <t>24.00R35</t>
+        </is>
+      </c>
+      <c r="F287" t="inlineStr">
+        <is>
+          <t>Бел-202</t>
+        </is>
+      </c>
+      <c r="G287" t="inlineStr">
+        <is>
+          <t>210B, сер, Type, C</t>
+        </is>
+      </c>
+      <c r="H287" t="n">
+        <v>2</v>
+      </c>
+      <c r="I287" s="1" t="n">
+        <v>44910</v>
+      </c>
+      <c r="J287" t="inlineStr">
+        <is>
+          <t>нет данных</t>
+        </is>
+      </c>
+    </row>
+    <row r="288">
+      <c r="E288" t="inlineStr">
+        <is>
+          <t>24.00R35</t>
+        </is>
+      </c>
+      <c r="F288" t="inlineStr">
+        <is>
+          <t>Бел-212</t>
+        </is>
+      </c>
+      <c r="G288" t="inlineStr">
+        <is>
+          <t>груз, сер, LS-2, Type</t>
+        </is>
+      </c>
+      <c r="H288" t="n">
+        <v>2</v>
+      </c>
+      <c r="I288" s="1" t="n">
+        <v>44910</v>
+      </c>
+      <c r="J288" t="inlineStr">
+        <is>
+          <t>нет данных</t>
+        </is>
+      </c>
+    </row>
+    <row r="289">
+      <c r="E289" t="inlineStr">
+        <is>
+          <t>24.00R35</t>
+        </is>
+      </c>
+      <c r="F289" t="inlineStr">
+        <is>
+          <t>Бел-212</t>
+        </is>
+      </c>
+      <c r="G289" t="inlineStr">
+        <is>
+          <t>груз, сер, Type, H</t>
+        </is>
+      </c>
+      <c r="H289" t="n">
+        <v>2</v>
+      </c>
+      <c r="I289" s="1" t="n">
+        <v>44910</v>
+      </c>
+      <c r="J289" t="inlineStr">
+        <is>
+          <t>нет данных</t>
+        </is>
+      </c>
+    </row>
+    <row r="290">
+      <c r="E290" t="inlineStr">
+        <is>
+          <t>24.00R35</t>
+        </is>
+      </c>
+      <c r="F290" t="inlineStr">
+        <is>
+          <t>Бел-212</t>
+        </is>
+      </c>
+      <c r="G290" t="inlineStr">
+        <is>
+          <t>груз, сер, Type, C</t>
+        </is>
+      </c>
+      <c r="H290" t="n">
+        <v>2</v>
+      </c>
+      <c r="I290" s="1" t="n">
+        <v>44910</v>
+      </c>
+      <c r="J290" t="inlineStr">
+        <is>
+          <t>нет данных</t>
+        </is>
+      </c>
+    </row>
+    <row r="291">
+      <c r="E291" t="inlineStr">
+        <is>
+          <t>21.00R35</t>
+        </is>
+      </c>
+      <c r="F291" t="inlineStr">
+        <is>
+          <t>Бел-200</t>
+        </is>
+      </c>
+      <c r="G291" t="inlineStr">
+        <is>
+          <t>202B, сер, LS-2, Type</t>
+        </is>
+      </c>
+      <c r="H291" t="n">
+        <v>2</v>
+      </c>
+      <c r="I291" s="1" t="n">
+        <v>44910</v>
+      </c>
+      <c r="J291" t="inlineStr">
+        <is>
+          <t>нет данных</t>
+        </is>
+      </c>
+    </row>
+    <row r="292">
+      <c r="E292" t="inlineStr">
+        <is>
+          <t>21.00R35</t>
+        </is>
+      </c>
+      <c r="F292" t="inlineStr">
+        <is>
+          <t>Бел-200</t>
+        </is>
+      </c>
+      <c r="G292" t="inlineStr">
+        <is>
+          <t>202B, сер, Type, H</t>
+        </is>
+      </c>
+      <c r="H292" t="n">
+        <v>2</v>
+      </c>
+      <c r="I292" s="1" t="n">
+        <v>44910</v>
+      </c>
+      <c r="J292" t="inlineStr">
+        <is>
+          <t>нет данных</t>
+        </is>
+      </c>
+    </row>
+    <row r="293">
+      <c r="E293" t="inlineStr">
+        <is>
+          <t>21.00R35</t>
+        </is>
+      </c>
+      <c r="F293" t="inlineStr">
+        <is>
+          <t>Бел-200</t>
+        </is>
+      </c>
+      <c r="G293" t="inlineStr">
+        <is>
+          <t>202B, сер, Type, C</t>
+        </is>
+      </c>
+      <c r="H293" t="n">
+        <v>2</v>
+      </c>
+      <c r="I293" s="1" t="n">
+        <v>44910</v>
+      </c>
+      <c r="J293" t="inlineStr">
+        <is>
+          <t>нет данных</t>
+        </is>
+      </c>
+    </row>
+    <row r="294">
+      <c r="E294" t="inlineStr">
+        <is>
+          <t>21.00R35</t>
+        </is>
+      </c>
+      <c r="F294" t="inlineStr">
+        <is>
+          <t>Бел-210</t>
+        </is>
+      </c>
+      <c r="G294" t="inlineStr">
+        <is>
+          <t>202B, сер, LS-2, Type</t>
+        </is>
+      </c>
+      <c r="H294" t="n">
+        <v>2</v>
+      </c>
+      <c r="I294" s="1" t="n">
+        <v>44910</v>
+      </c>
+      <c r="J294" t="inlineStr">
+        <is>
+          <t>нет данных</t>
+        </is>
+      </c>
+    </row>
+    <row r="295">
+      <c r="E295" t="inlineStr">
+        <is>
+          <t>21.00R35</t>
+        </is>
+      </c>
+      <c r="F295" t="inlineStr">
+        <is>
+          <t>Бел-210</t>
+        </is>
+      </c>
+      <c r="G295" t="inlineStr">
+        <is>
+          <t>202B, сер, Type, H</t>
+        </is>
+      </c>
+      <c r="H295" t="n">
+        <v>2</v>
+      </c>
+      <c r="I295" s="1" t="n">
+        <v>44910</v>
+      </c>
+      <c r="J295" t="inlineStr">
+        <is>
+          <t>нет данных</t>
+        </is>
+      </c>
+    </row>
+    <row r="296">
+      <c r="E296" t="inlineStr">
+        <is>
+          <t>21.00R35</t>
+        </is>
+      </c>
+      <c r="F296" t="inlineStr">
+        <is>
+          <t>Бел-210</t>
+        </is>
+      </c>
+      <c r="G296" t="inlineStr">
+        <is>
+          <t>202B, сер, Type, C</t>
+        </is>
+      </c>
+      <c r="H296" t="n">
+        <v>2</v>
+      </c>
+      <c r="I296" s="1" t="n">
+        <v>44910</v>
+      </c>
+      <c r="J296" t="inlineStr">
+        <is>
+          <t>нет данных</t>
+        </is>
+      </c>
+    </row>
+    <row r="297">
+      <c r="E297" t="inlineStr">
+        <is>
+          <t>14.00R20</t>
+        </is>
+      </c>
+      <c r="F297" t="inlineStr">
+        <is>
+          <t>BEL-248</t>
+        </is>
+      </c>
+      <c r="G297" t="inlineStr">
+        <is>
+          <t>груз, сер</t>
+        </is>
+      </c>
+      <c r="H297" t="n">
+        <v>2</v>
+      </c>
+      <c r="I297" s="1" t="n">
+        <v>44910</v>
+      </c>
+      <c r="J297" t="inlineStr">
+        <is>
+          <t>нет данных</t>
+        </is>
+      </c>
+    </row>
+    <row r="298">
+      <c r="E298" t="inlineStr">
+        <is>
+          <t>14.00R20</t>
+        </is>
+      </c>
+      <c r="F298" t="inlineStr">
+        <is>
+          <t>BEL-248</t>
+        </is>
+      </c>
+      <c r="G298" t="inlineStr">
+        <is>
+          <t>груз, сер</t>
+        </is>
+      </c>
+      <c r="H298" t="n">
+        <v>2</v>
+      </c>
+      <c r="I298" s="1" t="n">
+        <v>44910</v>
+      </c>
+      <c r="J298" t="inlineStr">
+        <is>
+          <t>нет данных</t>
+        </is>
+      </c>
+    </row>
+    <row r="299">
+      <c r="E299" t="inlineStr">
+        <is>
+          <t>14.00R20</t>
+        </is>
+      </c>
+      <c r="F299" t="inlineStr">
+        <is>
+          <t>BEL-248</t>
+        </is>
+      </c>
+      <c r="G299" t="inlineStr">
+        <is>
+          <t>б/к, груз, сер</t>
+        </is>
+      </c>
+      <c r="H299" t="n">
+        <v>2</v>
+      </c>
+      <c r="I299" s="1" t="n">
+        <v>44910</v>
+      </c>
+      <c r="J299" t="inlineStr">
+        <is>
+          <t>нет данных</t>
+        </is>
+      </c>
+    </row>
+    <row r="300">
+      <c r="E300" t="inlineStr">
+        <is>
+          <t>14.00R20</t>
+        </is>
+      </c>
+      <c r="F300" t="inlineStr">
+        <is>
+          <t>BEL-248</t>
+        </is>
+      </c>
+      <c r="G300" t="inlineStr">
+        <is>
+          <t>груз, сер</t>
+        </is>
+      </c>
+      <c r="H300" t="n">
+        <v>2</v>
+      </c>
+      <c r="I300" s="1" t="n">
+        <v>44910</v>
+      </c>
+      <c r="J300" t="inlineStr">
         <is>
           <t>нет данных</t>
         </is>

</xml_diff>

<commit_message>
improved import files CHEMCURIER or OTHER files  done at 16/01/2023
</commit_message>
<xml_diff>
--- a/src/Tyres.xlsx
+++ b/src/Tyres.xlsx
@@ -417,7 +417,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J77"/>
+  <dimension ref="A1:J41"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -485,33 +485,33 @@
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>Type сер LS-2 груз</t>
+          <t>сер груз Type LS-2</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>35/65-33</t>
+          <t>205/60R16</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>ФБел-283</t>
+          <t>BEL-277</t>
         </is>
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>42, сер, груз</t>
+          <t>сер, легк, б/к</t>
         </is>
       </c>
       <c r="H2" t="n">
-        <v>2</v>
+        <v>281</v>
       </c>
       <c r="I2" s="1" t="n">
-        <v>44930</v>
+        <v>44752</v>
       </c>
       <c r="J2" t="inlineStr">
         <is>
-          <t>нет данных</t>
+          <t>HHHDFD</t>
         </is>
       </c>
     </row>
@@ -528,33 +528,33 @@
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>Type H сер груз</t>
+          <t>сер H груз Type</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>24.00R35</t>
+          <t>175/70R13</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>Бел-122</t>
+          <t>Бел-103</t>
         </is>
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>Type, сер, LS-2, груз</t>
+          <t>сер, легк, б/к</t>
         </is>
       </c>
       <c r="H3" t="n">
-        <v>2</v>
+        <v>287</v>
       </c>
       <c r="I3" s="1" t="n">
-        <v>44930</v>
+        <v>44752</v>
       </c>
       <c r="J3" t="inlineStr">
         <is>
-          <t>нет данных</t>
+          <t>HHHDFD</t>
         </is>
       </c>
     </row>
@@ -571,33 +571,33 @@
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>Type сер C груз</t>
+          <t>сер груз Type C</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>24.00R35</t>
+          <t>175/70R13</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>Бел-122</t>
+          <t>Бел-103</t>
         </is>
       </c>
       <c r="G4" t="inlineStr">
         <is>
-          <t>Type, H, сер, груз</t>
+          <t>сер, легк, б/к</t>
         </is>
       </c>
       <c r="H4" t="n">
-        <v>2</v>
+        <v>283</v>
       </c>
       <c r="I4" s="1" t="n">
-        <v>44930</v>
+        <v>44752</v>
       </c>
       <c r="J4" t="inlineStr">
         <is>
-          <t>нет данных</t>
+          <t>HHHDFD</t>
         </is>
       </c>
     </row>
@@ -614,29 +614,29 @@
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>210B Type сер LS-2</t>
+          <t>210B сер Type LS-2</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>24.00R35</t>
+          <t>35/65-33</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>Бел-122</t>
+          <t>ФБел-283</t>
         </is>
       </c>
       <c r="G5" t="inlineStr">
         <is>
-          <t>Type, сер, C, груз</t>
+          <t>42, сер, груз</t>
         </is>
       </c>
       <c r="H5" t="n">
         <v>2</v>
       </c>
       <c r="I5" s="1" t="n">
-        <v>44930</v>
+        <v>44942</v>
       </c>
       <c r="J5" t="inlineStr">
         <is>
@@ -657,7 +657,7 @@
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>210B Type H сер</t>
+          <t>210B сер H Type</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
@@ -667,19 +667,19 @@
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>Бел-202</t>
+          <t>Бел-122</t>
         </is>
       </c>
       <c r="G6" t="inlineStr">
         <is>
-          <t>210B, Type, сер, LS-2</t>
+          <t>сер, груз, Type, LS-2</t>
         </is>
       </c>
       <c r="H6" t="n">
         <v>2</v>
       </c>
       <c r="I6" s="1" t="n">
-        <v>44930</v>
+        <v>44942</v>
       </c>
       <c r="J6" t="inlineStr">
         <is>
@@ -700,7 +700,7 @@
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>210B Type сер C</t>
+          <t>210B сер Type C</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
@@ -710,19 +710,19 @@
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>Бел-202</t>
+          <t>Бел-122</t>
         </is>
       </c>
       <c r="G7" t="inlineStr">
         <is>
-          <t>210B, Type, H, сер</t>
+          <t>сер, H, груз, Type</t>
         </is>
       </c>
       <c r="H7" t="n">
         <v>2</v>
       </c>
       <c r="I7" s="1" t="n">
-        <v>44930</v>
+        <v>44942</v>
       </c>
       <c r="J7" t="inlineStr">
         <is>
@@ -743,7 +743,7 @@
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>Type сер LS-2 груз</t>
+          <t>сер груз Type LS-2</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
@@ -753,19 +753,19 @@
       </c>
       <c r="F8" t="inlineStr">
         <is>
-          <t>Бел-202</t>
+          <t>Бел-122</t>
         </is>
       </c>
       <c r="G8" t="inlineStr">
         <is>
-          <t>210B, Type, сер, C</t>
+          <t>сер, груз, Type, C</t>
         </is>
       </c>
       <c r="H8" t="n">
         <v>2</v>
       </c>
       <c r="I8" s="1" t="n">
-        <v>44930</v>
+        <v>44942</v>
       </c>
       <c r="J8" t="inlineStr">
         <is>
@@ -786,7 +786,7 @@
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>Type H сер груз</t>
+          <t>сер H груз Type</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
@@ -796,19 +796,19 @@
       </c>
       <c r="F9" t="inlineStr">
         <is>
-          <t>Бел-212</t>
+          <t>Бел-202</t>
         </is>
       </c>
       <c r="G9" t="inlineStr">
         <is>
-          <t>Type, сер, LS-2, груз</t>
+          <t>210B, сер, Type, LS-2</t>
         </is>
       </c>
       <c r="H9" t="n">
         <v>2</v>
       </c>
       <c r="I9" s="1" t="n">
-        <v>44930</v>
+        <v>44942</v>
       </c>
       <c r="J9" t="inlineStr">
         <is>
@@ -829,7 +829,7 @@
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>Type сер C груз</t>
+          <t>сер груз Type C</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
@@ -839,19 +839,19 @@
       </c>
       <c r="F10" t="inlineStr">
         <is>
-          <t>Бел-212</t>
+          <t>Бел-202</t>
         </is>
       </c>
       <c r="G10" t="inlineStr">
         <is>
-          <t>Type, H, сер, груз</t>
+          <t>210B, сер, H, Type</t>
         </is>
       </c>
       <c r="H10" t="n">
         <v>2</v>
       </c>
       <c r="I10" s="1" t="n">
-        <v>44930</v>
+        <v>44942</v>
       </c>
       <c r="J10" t="inlineStr">
         <is>
@@ -872,7 +872,7 @@
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>202B Type сер LS-2</t>
+          <t>202B сер Type LS-2</t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
@@ -882,19 +882,19 @@
       </c>
       <c r="F11" t="inlineStr">
         <is>
-          <t>Бел-212</t>
+          <t>Бел-202</t>
         </is>
       </c>
       <c r="G11" t="inlineStr">
         <is>
-          <t>Type, сер, C, груз</t>
+          <t>210B, сер, Type, C</t>
         </is>
       </c>
       <c r="H11" t="n">
         <v>2</v>
       </c>
       <c r="I11" s="1" t="n">
-        <v>44930</v>
+        <v>44942</v>
       </c>
       <c r="J11" t="inlineStr">
         <is>
@@ -915,29 +915,29 @@
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>202B Type H сер</t>
+          <t>202B сер H Type</t>
         </is>
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>21.00R35</t>
+          <t>24.00R35</t>
         </is>
       </c>
       <c r="F12" t="inlineStr">
         <is>
-          <t>Бел-200</t>
+          <t>Бел-212</t>
         </is>
       </c>
       <c r="G12" t="inlineStr">
         <is>
-          <t>202B, Type, сер, LS-2</t>
+          <t>сер, груз, Type, LS-2</t>
         </is>
       </c>
       <c r="H12" t="n">
         <v>2</v>
       </c>
       <c r="I12" s="1" t="n">
-        <v>44930</v>
+        <v>44942</v>
       </c>
       <c r="J12" t="inlineStr">
         <is>
@@ -958,29 +958,29 @@
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>202B Type сер C</t>
+          <t>202B сер Type C</t>
         </is>
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>21.00R35</t>
+          <t>24.00R35</t>
         </is>
       </c>
       <c r="F13" t="inlineStr">
         <is>
-          <t>Бел-200</t>
+          <t>Бел-212</t>
         </is>
       </c>
       <c r="G13" t="inlineStr">
         <is>
-          <t>202B, Type, H, сер</t>
+          <t>сер, H, груз, Type</t>
         </is>
       </c>
       <c r="H13" t="n">
         <v>2</v>
       </c>
       <c r="I13" s="1" t="n">
-        <v>44930</v>
+        <v>44942</v>
       </c>
       <c r="J13" t="inlineStr">
         <is>
@@ -1001,29 +1001,29 @@
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>202B Type сер LS-2</t>
+          <t>202B сер Type LS-2</t>
         </is>
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>21.00R35</t>
+          <t>24.00R35</t>
         </is>
       </c>
       <c r="F14" t="inlineStr">
         <is>
-          <t>Бел-200</t>
+          <t>Бел-212</t>
         </is>
       </c>
       <c r="G14" t="inlineStr">
         <is>
-          <t>202B, Type, сер, C</t>
+          <t>сер, груз, Type, C</t>
         </is>
       </c>
       <c r="H14" t="n">
         <v>2</v>
       </c>
       <c r="I14" s="1" t="n">
-        <v>44930</v>
+        <v>44942</v>
       </c>
       <c r="J14" t="inlineStr">
         <is>
@@ -1044,7 +1044,7 @@
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>202B Type H сер</t>
+          <t>202B сер H Type</t>
         </is>
       </c>
       <c r="E15" t="inlineStr">
@@ -1054,19 +1054,19 @@
       </c>
       <c r="F15" t="inlineStr">
         <is>
-          <t>Бел-210</t>
+          <t>Бел-200</t>
         </is>
       </c>
       <c r="G15" t="inlineStr">
         <is>
-          <t>202B, Type, сер, LS-2</t>
+          <t>202B, сер, Type, LS-2</t>
         </is>
       </c>
       <c r="H15" t="n">
         <v>2</v>
       </c>
       <c r="I15" s="1" t="n">
-        <v>44930</v>
+        <v>44942</v>
       </c>
       <c r="J15" t="inlineStr">
         <is>
@@ -1087,7 +1087,7 @@
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>202B Type сер C</t>
+          <t>202B сер Type C</t>
         </is>
       </c>
       <c r="E16" t="inlineStr">
@@ -1097,19 +1097,19 @@
       </c>
       <c r="F16" t="inlineStr">
         <is>
-          <t>Бел-210</t>
+          <t>Бел-200</t>
         </is>
       </c>
       <c r="G16" t="inlineStr">
         <is>
-          <t>202B, Type, H, сер</t>
+          <t>202B, сер, H, Type</t>
         </is>
       </c>
       <c r="H16" t="n">
         <v>2</v>
       </c>
       <c r="I16" s="1" t="n">
-        <v>44930</v>
+        <v>44942</v>
       </c>
       <c r="J16" t="inlineStr">
         <is>
@@ -1140,19 +1140,19 @@
       </c>
       <c r="F17" t="inlineStr">
         <is>
-          <t>Бел-210</t>
+          <t>Бел-200</t>
         </is>
       </c>
       <c r="G17" t="inlineStr">
         <is>
-          <t>202B, Type, сер, C</t>
+          <t>202B, сер, Type, C</t>
         </is>
       </c>
       <c r="H17" t="n">
         <v>2</v>
       </c>
       <c r="I17" s="1" t="n">
-        <v>44930</v>
+        <v>44942</v>
       </c>
       <c r="J17" t="inlineStr">
         <is>
@@ -1173,29 +1173,29 @@
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>сер б/к груз</t>
+          <t>сер груз б/к</t>
         </is>
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t>14.00R20</t>
+          <t>21.00R35</t>
         </is>
       </c>
       <c r="F18" t="inlineStr">
         <is>
-          <t>BEL-248</t>
+          <t>Бел-210</t>
         </is>
       </c>
       <c r="G18" t="inlineStr">
         <is>
-          <t>сер, груз</t>
+          <t>202B, сер, Type, LS-2</t>
         </is>
       </c>
       <c r="H18" t="n">
         <v>2</v>
       </c>
       <c r="I18" s="1" t="n">
-        <v>44930</v>
+        <v>44942</v>
       </c>
       <c r="J18" t="inlineStr">
         <is>
@@ -1221,24 +1221,24 @@
       </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t>14.00R20</t>
+          <t>21.00R35</t>
         </is>
       </c>
       <c r="F19" t="inlineStr">
         <is>
-          <t>BEL-248</t>
+          <t>Бел-210</t>
         </is>
       </c>
       <c r="G19" t="inlineStr">
         <is>
-          <t>сер, б/к, груз</t>
+          <t>202B, сер, H, Type</t>
         </is>
       </c>
       <c r="H19" t="n">
         <v>2</v>
       </c>
       <c r="I19" s="1" t="n">
-        <v>44930</v>
+        <v>44942</v>
       </c>
       <c r="J19" t="inlineStr">
         <is>
@@ -1264,24 +1264,24 @@
       </c>
       <c r="E20" t="inlineStr">
         <is>
-          <t>14.00R20</t>
+          <t>21.00R35</t>
         </is>
       </c>
       <c r="F20" t="inlineStr">
         <is>
-          <t>BEL-248</t>
+          <t>Бел-210</t>
         </is>
       </c>
       <c r="G20" t="inlineStr">
         <is>
-          <t>сер, груз</t>
+          <t>202B, сер, Type, C</t>
         </is>
       </c>
       <c r="H20" t="n">
         <v>2</v>
       </c>
       <c r="I20" s="1" t="n">
-        <v>44930</v>
+        <v>44942</v>
       </c>
       <c r="J20" t="inlineStr">
         <is>
@@ -1324,7 +1324,7 @@
         <v>2</v>
       </c>
       <c r="I21" s="1" t="n">
-        <v>44930</v>
+        <v>44942</v>
       </c>
       <c r="J21" t="inlineStr">
         <is>
@@ -1345,17 +1345,17 @@
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>173G сер б/к груз</t>
+          <t>173G сер груз б/к</t>
         </is>
       </c>
       <c r="E22" t="inlineStr">
         <is>
-          <t>12.00R20</t>
+          <t>14.00R20</t>
         </is>
       </c>
       <c r="F22" t="inlineStr">
         <is>
-          <t>BEL-288</t>
+          <t>BEL-248</t>
         </is>
       </c>
       <c r="G22" t="inlineStr">
@@ -1367,7 +1367,7 @@
         <v>2</v>
       </c>
       <c r="I22" s="1" t="n">
-        <v>44930</v>
+        <v>44942</v>
       </c>
       <c r="J22" t="inlineStr">
         <is>
@@ -1393,24 +1393,24 @@
       </c>
       <c r="E23" t="inlineStr">
         <is>
-          <t>16.00R20</t>
+          <t>14.00R20</t>
         </is>
       </c>
       <c r="F23" t="inlineStr">
         <is>
-          <t>Бел-95</t>
+          <t>BEL-248</t>
         </is>
       </c>
       <c r="G23" t="inlineStr">
         <is>
-          <t>173G, сер, б/к, груз</t>
+          <t>сер, груз</t>
         </is>
       </c>
       <c r="H23" t="n">
         <v>2</v>
       </c>
       <c r="I23" s="1" t="n">
-        <v>44930</v>
+        <v>44942</v>
       </c>
       <c r="J23" t="inlineStr">
         <is>
@@ -1436,24 +1436,24 @@
       </c>
       <c r="E24" t="inlineStr">
         <is>
-          <t>16.00R20</t>
+          <t>14.00R20</t>
         </is>
       </c>
       <c r="F24" t="inlineStr">
         <is>
-          <t>Бел-95</t>
+          <t>BEL-248</t>
         </is>
       </c>
       <c r="G24" t="inlineStr">
         <is>
-          <t>173G, сер, груз</t>
+          <t>сер, груз, б/к</t>
         </is>
       </c>
       <c r="H24" t="n">
         <v>2</v>
       </c>
       <c r="I24" s="1" t="n">
-        <v>44930</v>
+        <v>44942</v>
       </c>
       <c r="J24" t="inlineStr">
         <is>
@@ -1479,24 +1479,24 @@
       </c>
       <c r="E25" t="inlineStr">
         <is>
-          <t>16.00R20</t>
+          <t>12.00R20</t>
         </is>
       </c>
       <c r="F25" t="inlineStr">
         <is>
-          <t>Бел-95</t>
+          <t>BEL-288</t>
         </is>
       </c>
       <c r="G25" t="inlineStr">
         <is>
-          <t>173G, сер, груз</t>
+          <t>сер, груз</t>
         </is>
       </c>
       <c r="H25" t="n">
         <v>2</v>
       </c>
       <c r="I25" s="1" t="n">
-        <v>44930</v>
+        <v>44942</v>
       </c>
       <c r="J25" t="inlineStr">
         <is>
@@ -1532,14 +1532,14 @@
       </c>
       <c r="G26" t="inlineStr">
         <is>
-          <t>173G, сер, груз</t>
+          <t>173G, сер, груз, б/к</t>
         </is>
       </c>
       <c r="H26" t="n">
         <v>2</v>
       </c>
       <c r="I26" s="1" t="n">
-        <v>44930</v>
+        <v>44942</v>
       </c>
       <c r="J26" t="inlineStr">
         <is>
@@ -1582,7 +1582,7 @@
         <v>2</v>
       </c>
       <c r="I27" s="1" t="n">
-        <v>44930</v>
+        <v>44942</v>
       </c>
       <c r="J27" t="inlineStr">
         <is>
@@ -1625,7 +1625,7 @@
         <v>2</v>
       </c>
       <c r="I28" s="1" t="n">
-        <v>44930</v>
+        <v>44942</v>
       </c>
       <c r="J28" t="inlineStr">
         <is>
@@ -1661,14 +1661,14 @@
       </c>
       <c r="G29" t="inlineStr">
         <is>
-          <t>173G, сер</t>
+          <t>173G, сер, груз</t>
         </is>
       </c>
       <c r="H29" t="n">
         <v>2</v>
       </c>
       <c r="I29" s="1" t="n">
-        <v>44930</v>
+        <v>44942</v>
       </c>
       <c r="J29" t="inlineStr">
         <is>
@@ -1689,29 +1689,29 @@
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>сер б/к груз</t>
+          <t>сер груз б/к</t>
         </is>
       </c>
       <c r="E30" t="inlineStr">
         <is>
-          <t>395/85R20</t>
+          <t>16.00R20</t>
         </is>
       </c>
       <c r="F30" t="inlineStr">
         <is>
-          <t>BEL-405</t>
+          <t>Бел-95</t>
         </is>
       </c>
       <c r="G30" t="inlineStr">
         <is>
-          <t>168J, сер, груз</t>
+          <t>173G, сер, груз</t>
         </is>
       </c>
       <c r="H30" t="n">
         <v>2</v>
       </c>
       <c r="I30" s="1" t="n">
-        <v>44930</v>
+        <v>44942</v>
       </c>
       <c r="J30" t="inlineStr">
         <is>
@@ -1737,24 +1737,24 @@
       </c>
       <c r="E31" t="inlineStr">
         <is>
-          <t>445/65R22.5</t>
+          <t>16.00R20</t>
         </is>
       </c>
       <c r="F31" t="inlineStr">
         <is>
-          <t>Бел-145</t>
+          <t>Бел-95</t>
         </is>
       </c>
       <c r="G31" t="inlineStr">
         <is>
-          <t>сер, б/к, груз</t>
+          <t>173G, сер, груз</t>
         </is>
       </c>
       <c r="H31" t="n">
         <v>2</v>
       </c>
       <c r="I31" s="1" t="n">
-        <v>44930</v>
+        <v>44942</v>
       </c>
       <c r="J31" t="inlineStr">
         <is>
@@ -1780,24 +1780,24 @@
       </c>
       <c r="E32" t="inlineStr">
         <is>
-          <t>355/65-15</t>
+          <t>16.00R20</t>
         </is>
       </c>
       <c r="F32" t="inlineStr">
         <is>
-          <t>Бел-230</t>
+          <t>Бел-95</t>
         </is>
       </c>
       <c r="G32" t="inlineStr">
         <is>
-          <t>сер</t>
+          <t>173G, сер</t>
         </is>
       </c>
       <c r="H32" t="n">
         <v>2</v>
       </c>
       <c r="I32" s="1" t="n">
-        <v>44930</v>
+        <v>44942</v>
       </c>
       <c r="J32" t="inlineStr">
         <is>
@@ -1818,29 +1818,29 @@
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>легк сер б/к</t>
+          <t>сер легк б/к</t>
         </is>
       </c>
       <c r="E33" t="inlineStr">
         <is>
-          <t>355/65-15</t>
+          <t>395/85R20</t>
         </is>
       </c>
       <c r="F33" t="inlineStr">
         <is>
-          <t>Бел-230М</t>
+          <t>BEL-405</t>
         </is>
       </c>
       <c r="G33" t="inlineStr">
         <is>
-          <t>сер</t>
+          <t>168J, сер, груз</t>
         </is>
       </c>
       <c r="H33" t="n">
         <v>2</v>
       </c>
       <c r="I33" s="1" t="n">
-        <v>44930</v>
+        <v>44942</v>
       </c>
       <c r="J33" t="inlineStr">
         <is>
@@ -1861,29 +1861,29 @@
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>легк сер б/к</t>
+          <t>сер легк б/к</t>
         </is>
       </c>
       <c r="E34" t="inlineStr">
         <is>
-          <t>205/55R16</t>
+          <t>445/65R22.5</t>
         </is>
       </c>
       <c r="F34" t="inlineStr">
         <is>
-          <t>BEL-262</t>
+          <t>Бел-145</t>
         </is>
       </c>
       <c r="G34" t="inlineStr">
         <is>
-          <t>легк, сер, б/к</t>
+          <t>сер, груз, б/к</t>
         </is>
       </c>
       <c r="H34" t="n">
         <v>2</v>
       </c>
       <c r="I34" s="1" t="n">
-        <v>44930</v>
+        <v>44942</v>
       </c>
       <c r="J34" t="inlineStr">
         <is>
@@ -1909,24 +1909,24 @@
       </c>
       <c r="E35" t="inlineStr">
         <is>
-          <t>205/55R16</t>
+          <t>355/65-15</t>
         </is>
       </c>
       <c r="F35" t="inlineStr">
         <is>
-          <t>BEL-317</t>
+          <t>Бел-230</t>
         </is>
       </c>
       <c r="G35" t="inlineStr">
         <is>
-          <t>легк, сер, б/к</t>
+          <t>сер</t>
         </is>
       </c>
       <c r="H35" t="n">
         <v>2</v>
       </c>
       <c r="I35" s="1" t="n">
-        <v>44930</v>
+        <v>44942</v>
       </c>
       <c r="J35" t="inlineStr">
         <is>
@@ -1947,29 +1947,29 @@
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>легк сер б/к</t>
+          <t>сер легк б/к</t>
         </is>
       </c>
       <c r="E36" t="inlineStr">
         <is>
-          <t>205/55R16</t>
+          <t>355/65-15</t>
         </is>
       </c>
       <c r="F36" t="inlineStr">
         <is>
-          <t>BEL-317S</t>
+          <t>Бел-230М</t>
         </is>
       </c>
       <c r="G36" t="inlineStr">
         <is>
-          <t>сер, ошип</t>
+          <t>сер</t>
         </is>
       </c>
       <c r="H36" t="n">
         <v>2</v>
       </c>
       <c r="I36" s="1" t="n">
-        <v>44930</v>
+        <v>44942</v>
       </c>
       <c r="J36" t="inlineStr">
         <is>
@@ -1980,713 +1980,155 @@
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t xml:space="preserve"> </t>
+          <t>Бел-103</t>
         </is>
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t xml:space="preserve"> </t>
+          <t>175/70R13</t>
+        </is>
+      </c>
+      <c r="C37" t="inlineStr">
+        <is>
+          <t>сер легк б/к</t>
         </is>
       </c>
       <c r="E37" t="inlineStr">
         <is>
+          <t>205/55R16</t>
+        </is>
+      </c>
+      <c r="F37" t="inlineStr">
+        <is>
+          <t>BEL-262</t>
+        </is>
+      </c>
+      <c r="G37" t="inlineStr">
+        <is>
+          <t>сер, легк, б/к</t>
+        </is>
+      </c>
+      <c r="H37" t="n">
+        <v>2</v>
+      </c>
+      <c r="I37" s="1" t="n">
+        <v>44942</v>
+      </c>
+      <c r="J37" t="inlineStr">
+        <is>
+          <t>нет данных</t>
+        </is>
+      </c>
+    </row>
+    <row r="38">
+      <c r="E38" t="inlineStr">
+        <is>
+          <t>205/55R16</t>
+        </is>
+      </c>
+      <c r="F38" t="inlineStr">
+        <is>
+          <t>BEL-317</t>
+        </is>
+      </c>
+      <c r="G38" t="inlineStr">
+        <is>
+          <t>сер, легк, б/к</t>
+        </is>
+      </c>
+      <c r="H38" t="n">
+        <v>2</v>
+      </c>
+      <c r="I38" s="1" t="n">
+        <v>44942</v>
+      </c>
+      <c r="J38" t="inlineStr">
+        <is>
+          <t>нет данных</t>
+        </is>
+      </c>
+    </row>
+    <row r="39">
+      <c r="E39" t="inlineStr">
+        <is>
+          <t>205/55R16</t>
+        </is>
+      </c>
+      <c r="F39" t="inlineStr">
+        <is>
+          <t>BEL-317S</t>
+        </is>
+      </c>
+      <c r="G39" t="inlineStr">
+        <is>
+          <t>сер, ошип</t>
+        </is>
+      </c>
+      <c r="H39" t="n">
+        <v>2</v>
+      </c>
+      <c r="I39" s="1" t="n">
+        <v>44942</v>
+      </c>
+      <c r="J39" t="inlineStr">
+        <is>
+          <t>нет данных</t>
+        </is>
+      </c>
+    </row>
+    <row r="40">
+      <c r="E40" t="inlineStr">
+        <is>
           <t>205/60R16</t>
         </is>
       </c>
-      <c r="F37" t="inlineStr">
+      <c r="F40" t="inlineStr">
         <is>
           <t>BEL-277</t>
         </is>
       </c>
-      <c r="G37" t="inlineStr">
-        <is>
-          <t>легк, сер, б/к</t>
-        </is>
-      </c>
-      <c r="H37" t="n">
-        <v>2</v>
-      </c>
-      <c r="I37" s="1" t="n">
-        <v>44930</v>
-      </c>
-      <c r="J37" t="inlineStr">
-        <is>
-          <t>нет данных</t>
-        </is>
-      </c>
-    </row>
-    <row r="38">
-      <c r="A38" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> </t>
-        </is>
-      </c>
-      <c r="B38" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> </t>
-        </is>
-      </c>
-    </row>
-    <row r="39">
-      <c r="A39" t="inlineStr">
-        <is>
-          <t>ФБел-283</t>
-        </is>
-      </c>
-      <c r="B39" t="inlineStr">
-        <is>
-          <t>35/65-33</t>
-        </is>
-      </c>
-      <c r="C39" t="inlineStr">
-        <is>
-          <t>42 сер груз</t>
-        </is>
-      </c>
-    </row>
-    <row r="40">
-      <c r="A40" t="inlineStr">
-        <is>
-          <t>Бел-122</t>
-        </is>
-      </c>
-      <c r="B40" t="inlineStr">
-        <is>
-          <t>24.00R35</t>
-        </is>
-      </c>
-      <c r="C40" t="inlineStr">
-        <is>
-          <t>Type сер LS-2 груз</t>
+      <c r="G40" t="inlineStr">
+        <is>
+          <t>сер, легк, б/к</t>
+        </is>
+      </c>
+      <c r="H40" t="n">
+        <v>2</v>
+      </c>
+      <c r="I40" s="1" t="n">
+        <v>44942</v>
+      </c>
+      <c r="J40" t="inlineStr">
+        <is>
+          <t>нет данных</t>
         </is>
       </c>
     </row>
     <row r="41">
-      <c r="A41" t="inlineStr">
-        <is>
-          <t>Бел-122</t>
-        </is>
-      </c>
-      <c r="B41" t="inlineStr">
-        <is>
-          <t>24.00R35</t>
-        </is>
-      </c>
-      <c r="C41" t="inlineStr">
-        <is>
-          <t>Type H сер груз</t>
-        </is>
-      </c>
-    </row>
-    <row r="42">
-      <c r="A42" t="inlineStr">
-        <is>
-          <t>Бел-122</t>
-        </is>
-      </c>
-      <c r="B42" t="inlineStr">
-        <is>
-          <t>24.00R35</t>
-        </is>
-      </c>
-      <c r="C42" t="inlineStr">
-        <is>
-          <t>Type сер C груз</t>
-        </is>
-      </c>
-    </row>
-    <row r="43">
-      <c r="A43" t="inlineStr">
-        <is>
-          <t>Бел-202</t>
-        </is>
-      </c>
-      <c r="B43" t="inlineStr">
-        <is>
-          <t>24.00R35</t>
-        </is>
-      </c>
-      <c r="C43" t="inlineStr">
-        <is>
-          <t>210B Type сер LS-2</t>
-        </is>
-      </c>
-    </row>
-    <row r="44">
-      <c r="A44" t="inlineStr">
-        <is>
-          <t>Бел-202</t>
-        </is>
-      </c>
-      <c r="B44" t="inlineStr">
-        <is>
-          <t>24.00R35</t>
-        </is>
-      </c>
-      <c r="C44" t="inlineStr">
-        <is>
-          <t>210B Type H сер</t>
-        </is>
-      </c>
-    </row>
-    <row r="45">
-      <c r="A45" t="inlineStr">
-        <is>
-          <t>Бел-202</t>
-        </is>
-      </c>
-      <c r="B45" t="inlineStr">
-        <is>
-          <t>24.00R35</t>
-        </is>
-      </c>
-      <c r="C45" t="inlineStr">
-        <is>
-          <t>210B Type сер C</t>
-        </is>
-      </c>
-    </row>
-    <row r="46">
-      <c r="A46" t="inlineStr">
-        <is>
-          <t>Бел-212</t>
-        </is>
-      </c>
-      <c r="B46" t="inlineStr">
-        <is>
-          <t>24.00R35</t>
-        </is>
-      </c>
-      <c r="C46" t="inlineStr">
-        <is>
-          <t>Type сер LS-2 груз</t>
-        </is>
-      </c>
-    </row>
-    <row r="47">
-      <c r="A47" t="inlineStr">
-        <is>
-          <t>Бел-212</t>
-        </is>
-      </c>
-      <c r="B47" t="inlineStr">
-        <is>
-          <t>24.00R35</t>
-        </is>
-      </c>
-      <c r="C47" t="inlineStr">
-        <is>
-          <t>Type H сер груз</t>
-        </is>
-      </c>
-    </row>
-    <row r="48">
-      <c r="A48" t="inlineStr">
-        <is>
-          <t>Бел-212</t>
-        </is>
-      </c>
-      <c r="B48" t="inlineStr">
-        <is>
-          <t>24.00R35</t>
-        </is>
-      </c>
-      <c r="C48" t="inlineStr">
-        <is>
-          <t>Type сер C груз</t>
-        </is>
-      </c>
-    </row>
-    <row r="49">
-      <c r="A49" t="inlineStr">
-        <is>
-          <t>Бел-200</t>
-        </is>
-      </c>
-      <c r="B49" t="inlineStr">
-        <is>
-          <t>21.00R35</t>
-        </is>
-      </c>
-      <c r="C49" t="inlineStr">
-        <is>
-          <t>202B Type сер LS-2</t>
-        </is>
-      </c>
-    </row>
-    <row r="50">
-      <c r="A50" t="inlineStr">
-        <is>
-          <t>Бел-200</t>
-        </is>
-      </c>
-      <c r="B50" t="inlineStr">
-        <is>
-          <t>21.00R35</t>
-        </is>
-      </c>
-      <c r="C50" t="inlineStr">
-        <is>
-          <t>202B Type H сер</t>
-        </is>
-      </c>
-    </row>
-    <row r="51">
-      <c r="A51" t="inlineStr">
-        <is>
-          <t>Бел-200</t>
-        </is>
-      </c>
-      <c r="B51" t="inlineStr">
-        <is>
-          <t>21.00R35</t>
-        </is>
-      </c>
-      <c r="C51" t="inlineStr">
-        <is>
-          <t>202B Type сер C</t>
-        </is>
-      </c>
-    </row>
-    <row r="52">
-      <c r="A52" t="inlineStr">
-        <is>
-          <t>Бел-210</t>
-        </is>
-      </c>
-      <c r="B52" t="inlineStr">
-        <is>
-          <t>21.00R35</t>
-        </is>
-      </c>
-      <c r="C52" t="inlineStr">
-        <is>
-          <t>202B Type сер LS-2</t>
-        </is>
-      </c>
-    </row>
-    <row r="53">
-      <c r="A53" t="inlineStr">
-        <is>
-          <t>Бел-210</t>
-        </is>
-      </c>
-      <c r="B53" t="inlineStr">
-        <is>
-          <t>21.00R35</t>
-        </is>
-      </c>
-      <c r="C53" t="inlineStr">
-        <is>
-          <t>202B Type H сер</t>
-        </is>
-      </c>
-    </row>
-    <row r="54">
-      <c r="A54" t="inlineStr">
-        <is>
-          <t>Бел-210</t>
-        </is>
-      </c>
-      <c r="B54" t="inlineStr">
-        <is>
-          <t>21.00R35</t>
-        </is>
-      </c>
-      <c r="C54" t="inlineStr">
-        <is>
-          <t>202B Type сер C</t>
-        </is>
-      </c>
-    </row>
-    <row r="55">
-      <c r="A55" t="inlineStr">
-        <is>
-          <t>BEL-248</t>
-        </is>
-      </c>
-      <c r="B55" t="inlineStr">
-        <is>
-          <t>14.00R20</t>
-        </is>
-      </c>
-      <c r="C55" t="inlineStr">
-        <is>
-          <t>сер груз</t>
-        </is>
-      </c>
-    </row>
-    <row r="56">
-      <c r="A56" t="inlineStr">
-        <is>
-          <t>BEL-248</t>
-        </is>
-      </c>
-      <c r="B56" t="inlineStr">
-        <is>
-          <t>14.00R20</t>
-        </is>
-      </c>
-      <c r="C56" t="inlineStr">
-        <is>
-          <t>сер б/к груз</t>
-        </is>
-      </c>
-    </row>
-    <row r="57">
-      <c r="A57" t="inlineStr">
-        <is>
-          <t>BEL-248</t>
-        </is>
-      </c>
-      <c r="B57" t="inlineStr">
-        <is>
-          <t>14.00R20</t>
-        </is>
-      </c>
-      <c r="C57" t="inlineStr">
-        <is>
-          <t>сер груз</t>
-        </is>
-      </c>
-    </row>
-    <row r="58">
-      <c r="A58" t="inlineStr">
-        <is>
-          <t>BEL-248</t>
-        </is>
-      </c>
-      <c r="B58" t="inlineStr">
-        <is>
-          <t>14.00R20</t>
-        </is>
-      </c>
-      <c r="C58" t="inlineStr">
-        <is>
-          <t>сер груз</t>
-        </is>
-      </c>
-    </row>
-    <row r="59">
-      <c r="A59" t="inlineStr">
-        <is>
-          <t>BEL-288</t>
-        </is>
-      </c>
-      <c r="B59" t="inlineStr">
-        <is>
-          <t>12.00R20</t>
-        </is>
-      </c>
-      <c r="C59" t="inlineStr">
-        <is>
-          <t>сер груз</t>
-        </is>
-      </c>
-    </row>
-    <row r="60">
-      <c r="A60" t="inlineStr">
-        <is>
-          <t>Бел-95</t>
-        </is>
-      </c>
-      <c r="B60" t="inlineStr">
-        <is>
-          <t>16.00R20</t>
-        </is>
-      </c>
-      <c r="C60" t="inlineStr">
-        <is>
-          <t>173G сер б/к груз</t>
-        </is>
-      </c>
-    </row>
-    <row r="61">
-      <c r="A61" t="inlineStr">
-        <is>
-          <t>Бел-95</t>
-        </is>
-      </c>
-      <c r="B61" t="inlineStr">
-        <is>
-          <t>16.00R20</t>
-        </is>
-      </c>
-      <c r="C61" t="inlineStr">
-        <is>
-          <t>173G сер груз</t>
-        </is>
-      </c>
-    </row>
-    <row r="62">
-      <c r="A62" t="inlineStr">
-        <is>
-          <t>Бел-95</t>
-        </is>
-      </c>
-      <c r="B62" t="inlineStr">
-        <is>
-          <t>16.00R20</t>
-        </is>
-      </c>
-      <c r="C62" t="inlineStr">
-        <is>
-          <t>173G сер груз</t>
-        </is>
-      </c>
-    </row>
-    <row r="63">
-      <c r="A63" t="inlineStr">
-        <is>
-          <t>Бел-95</t>
-        </is>
-      </c>
-      <c r="B63" t="inlineStr">
-        <is>
-          <t>16.00R20</t>
-        </is>
-      </c>
-      <c r="C63" t="inlineStr">
-        <is>
-          <t>173G сер груз</t>
-        </is>
-      </c>
-    </row>
-    <row r="64">
-      <c r="A64" t="inlineStr">
-        <is>
-          <t>Бел-95</t>
-        </is>
-      </c>
-      <c r="B64" t="inlineStr">
-        <is>
-          <t>16.00R20</t>
-        </is>
-      </c>
-      <c r="C64" t="inlineStr">
-        <is>
-          <t>173G сер груз</t>
-        </is>
-      </c>
-    </row>
-    <row r="65">
-      <c r="A65" t="inlineStr">
-        <is>
-          <t>Бел-95</t>
-        </is>
-      </c>
-      <c r="B65" t="inlineStr">
-        <is>
-          <t>16.00R20</t>
-        </is>
-      </c>
-      <c r="C65" t="inlineStr">
-        <is>
-          <t>173G сер груз</t>
-        </is>
-      </c>
-    </row>
-    <row r="66">
-      <c r="A66" t="inlineStr">
-        <is>
-          <t>Бел-95</t>
-        </is>
-      </c>
-      <c r="B66" t="inlineStr">
-        <is>
-          <t>16.00R20</t>
-        </is>
-      </c>
-      <c r="C66" t="inlineStr">
-        <is>
-          <t>173G сер</t>
-        </is>
-      </c>
-    </row>
-    <row r="67">
-      <c r="A67" t="inlineStr">
-        <is>
-          <t>BEL-405</t>
-        </is>
-      </c>
-      <c r="B67" t="inlineStr">
-        <is>
-          <t>395/85R20</t>
-        </is>
-      </c>
-      <c r="C67" t="inlineStr">
-        <is>
-          <t>168J сер груз</t>
-        </is>
-      </c>
-    </row>
-    <row r="68">
-      <c r="A68" t="inlineStr">
-        <is>
-          <t>Бел-145</t>
-        </is>
-      </c>
-      <c r="B68" t="inlineStr">
-        <is>
-          <t>445/65R22.5</t>
-        </is>
-      </c>
-      <c r="C68" t="inlineStr">
-        <is>
-          <t>сер б/к груз</t>
-        </is>
-      </c>
-    </row>
-    <row r="69">
-      <c r="A69" t="inlineStr">
-        <is>
-          <t>Бел-230</t>
-        </is>
-      </c>
-      <c r="B69" t="inlineStr">
-        <is>
-          <t>355/65-15</t>
-        </is>
-      </c>
-      <c r="C69" t="inlineStr">
-        <is>
-          <t>сер</t>
-        </is>
-      </c>
-    </row>
-    <row r="70">
-      <c r="A70" t="inlineStr">
-        <is>
-          <t>Бел-230М</t>
-        </is>
-      </c>
-      <c r="B70" t="inlineStr">
-        <is>
-          <t>355/65-15</t>
-        </is>
-      </c>
-      <c r="C70" t="inlineStr">
-        <is>
-          <t>сер</t>
-        </is>
-      </c>
-    </row>
-    <row r="71">
-      <c r="A71" t="inlineStr">
-        <is>
-          <t>BEL-262</t>
-        </is>
-      </c>
-      <c r="B71" t="inlineStr">
-        <is>
-          <t>205/55R16</t>
-        </is>
-      </c>
-      <c r="C71" t="inlineStr">
-        <is>
-          <t>легк сер б/к</t>
-        </is>
-      </c>
-    </row>
-    <row r="72">
-      <c r="A72" t="inlineStr">
-        <is>
-          <t>BEL-317</t>
-        </is>
-      </c>
-      <c r="B72" t="inlineStr">
-        <is>
-          <t>205/55R16</t>
-        </is>
-      </c>
-      <c r="C72" t="inlineStr">
-        <is>
-          <t>легк сер б/к</t>
-        </is>
-      </c>
-    </row>
-    <row r="73">
-      <c r="A73" t="inlineStr">
-        <is>
-          <t>BEL-317S</t>
-        </is>
-      </c>
-      <c r="B73" t="inlineStr">
-        <is>
-          <t>205/55R16</t>
-        </is>
-      </c>
-      <c r="C73" t="inlineStr">
-        <is>
-          <t>сер ошип</t>
-        </is>
-      </c>
-    </row>
-    <row r="74">
-      <c r="A74" t="inlineStr">
-        <is>
-          <t>BEL-277</t>
-        </is>
-      </c>
-      <c r="B74" t="inlineStr">
-        <is>
-          <t>205/60R16</t>
-        </is>
-      </c>
-      <c r="C74" t="inlineStr">
-        <is>
-          <t>легк сер б/к</t>
-        </is>
-      </c>
-    </row>
-    <row r="75">
-      <c r="A75" t="inlineStr">
+      <c r="E41" t="inlineStr">
+        <is>
+          <t>175/70R13</t>
+        </is>
+      </c>
+      <c r="F41" t="inlineStr">
         <is>
           <t>Бел-103</t>
         </is>
       </c>
-      <c r="B75" t="inlineStr">
-        <is>
-          <t>175/70R13</t>
-        </is>
-      </c>
-      <c r="C75" t="inlineStr">
-        <is>
-          <t>легк сер б/к</t>
-        </is>
-      </c>
-    </row>
-    <row r="76">
-      <c r="A76" t="inlineStr">
-        <is>
-          <t>Бел-100</t>
-        </is>
-      </c>
-      <c r="B76" t="inlineStr">
-        <is>
-          <t>175/70R13</t>
-        </is>
-      </c>
-      <c r="C76" t="inlineStr">
-        <is>
-          <t>легк сер б/к</t>
-        </is>
-      </c>
-    </row>
-    <row r="77">
-      <c r="A77" t="inlineStr">
-        <is>
-          <t>Ф-35-1</t>
-        </is>
-      </c>
-      <c r="B77" t="inlineStr">
-        <is>
-          <t>11.2-20</t>
-        </is>
-      </c>
-      <c r="C77" t="inlineStr">
-        <is>
-          <t>168J сер 8 сх</t>
+      <c r="G41" t="inlineStr">
+        <is>
+          <t>сер, легк, б/к</t>
+        </is>
+      </c>
+      <c r="H41" t="n">
+        <v>2</v>
+      </c>
+      <c r="I41" s="1" t="n">
+        <v>44942</v>
+      </c>
+      <c r="J41" t="inlineStr">
+        <is>
+          <t>нет данных</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
improved import files CHEMCURIER or OTHER files done at 22/01/2023
</commit_message>
<xml_diff>
--- a/src/Tyres.xlsx
+++ b/src/Tyres.xlsx
@@ -417,7 +417,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J41"/>
+  <dimension ref="A1:J32"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -428,17 +428,12 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>ФБел-283</t>
+          <t xml:space="preserve"> </t>
         </is>
       </c>
       <c r="B1" t="inlineStr">
         <is>
-          <t>35/65-33</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>42 сер груз</t>
+          <t xml:space="preserve"> </t>
         </is>
       </c>
       <c r="E1" t="inlineStr">
@@ -475,113 +470,108 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Бел-122</t>
+          <t xml:space="preserve"> </t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>24.00R35</t>
-        </is>
-      </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>сер груз Type LS-2</t>
+          <t xml:space="preserve"> </t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>205/60R16</t>
+          <t>35/65-33</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>BEL-277</t>
+          <t>ФБел-283</t>
         </is>
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>сер, легк, б/к</t>
+          <t>42, груз, сер</t>
         </is>
       </c>
       <c r="H2" t="n">
-        <v>281</v>
+        <v>2</v>
       </c>
       <c r="I2" s="1" t="n">
-        <v>44752</v>
+        <v>44943</v>
       </c>
       <c r="J2" t="inlineStr">
         <is>
-          <t>HHHDFD</t>
+          <t>нет данных</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Бел-122</t>
+          <t>ФБел-283</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>24.00R35</t>
+          <t>35/65-33</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>сер H груз Type</t>
+          <t>42 груз сер</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>175/70R13</t>
+          <t>35/65-33</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>Бел-103</t>
+          <t>ФБел-283</t>
         </is>
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>сер, легк, б/к</t>
+          <t>30, груз, сер</t>
         </is>
       </c>
       <c r="H3" t="n">
-        <v>287</v>
+        <v>2</v>
       </c>
       <c r="I3" s="1" t="n">
-        <v>44752</v>
+        <v>44943</v>
       </c>
       <c r="J3" t="inlineStr">
         <is>
-          <t>HHHDFD</t>
+          <t>нет данных</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Бел-122</t>
+          <t>ФБел-283</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>24.00R35</t>
+          <t>35/65-33</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>сер груз Type C</t>
+          <t>30 груз сер</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>175/70R13</t>
+          <t>205/55R16</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>Бел-103</t>
+          <t>BEL-262</t>
         </is>
       </c>
       <c r="G4" t="inlineStr">
@@ -590,53 +580,53 @@
         </is>
       </c>
       <c r="H4" t="n">
-        <v>283</v>
+        <v>2</v>
       </c>
       <c r="I4" s="1" t="n">
-        <v>44752</v>
+        <v>44943</v>
       </c>
       <c r="J4" t="inlineStr">
         <is>
-          <t>HHHDFD</t>
+          <t>нет данных</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Бел-202</t>
+          <t>BEL-262</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>24.00R35</t>
+          <t>205/55R16</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>210B сер Type LS-2</t>
+          <t>сер легк б/к</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>35/65-33</t>
+          <t>205/55R16</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>ФБел-283</t>
+          <t>BEL-317</t>
         </is>
       </c>
       <c r="G5" t="inlineStr">
         <is>
-          <t>42, сер, груз</t>
+          <t>сер, легк, б/к</t>
         </is>
       </c>
       <c r="H5" t="n">
         <v>2</v>
       </c>
       <c r="I5" s="1" t="n">
-        <v>44942</v>
+        <v>44943</v>
       </c>
       <c r="J5" t="inlineStr">
         <is>
@@ -647,39 +637,39 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>Бел-202</t>
+          <t>BEL-317</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>24.00R35</t>
+          <t>205/55R16</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>210B сер H Type</t>
+          <t>сер легк б/к</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>24.00R35</t>
+          <t>205/55R16</t>
         </is>
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>Бел-122</t>
+          <t>BEL-317S</t>
         </is>
       </c>
       <c r="G6" t="inlineStr">
         <is>
-          <t>сер, груз, Type, LS-2</t>
+          <t>сер, ошип</t>
         </is>
       </c>
       <c r="H6" t="n">
         <v>2</v>
       </c>
       <c r="I6" s="1" t="n">
-        <v>44942</v>
+        <v>44943</v>
       </c>
       <c r="J6" t="inlineStr">
         <is>
@@ -690,24 +680,24 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>Бел-202</t>
+          <t>BEL-317S</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
+          <t>205/55R16</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>сер ошип</t>
+        </is>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
           <t>24.00R35</t>
         </is>
       </c>
-      <c r="C7" t="inlineStr">
-        <is>
-          <t>210B сер Type C</t>
-        </is>
-      </c>
-      <c r="E7" t="inlineStr">
-        <is>
-          <t>24.00R35</t>
-        </is>
-      </c>
       <c r="F7" t="inlineStr">
         <is>
           <t>Бел-122</t>
@@ -715,14 +705,14 @@
       </c>
       <c r="G7" t="inlineStr">
         <is>
-          <t>сер, H, груз, Type</t>
+          <t>груз, сер, LS-2, Type</t>
         </is>
       </c>
       <c r="H7" t="n">
         <v>2</v>
       </c>
       <c r="I7" s="1" t="n">
-        <v>44942</v>
+        <v>44943</v>
       </c>
       <c r="J7" t="inlineStr">
         <is>
@@ -733,7 +723,7 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>Бел-212</t>
+          <t>Бел-122</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
@@ -743,7 +733,7 @@
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>сер груз Type LS-2</t>
+          <t>груз сер LS-2 Type</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
@@ -758,14 +748,14 @@
       </c>
       <c r="G8" t="inlineStr">
         <is>
-          <t>сер, груз, Type, C</t>
+          <t>груз, сер, H, Type</t>
         </is>
       </c>
       <c r="H8" t="n">
         <v>2</v>
       </c>
       <c r="I8" s="1" t="n">
-        <v>44942</v>
+        <v>44943</v>
       </c>
       <c r="J8" t="inlineStr">
         <is>
@@ -776,7 +766,7 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>Бел-212</t>
+          <t>Бел-122</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
@@ -786,7 +776,7 @@
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>сер H груз Type</t>
+          <t>груз сер H Type</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
@@ -796,19 +786,19 @@
       </c>
       <c r="F9" t="inlineStr">
         <is>
-          <t>Бел-202</t>
+          <t>Бел-122</t>
         </is>
       </c>
       <c r="G9" t="inlineStr">
         <is>
-          <t>210B, сер, Type, LS-2</t>
+          <t>груз, сер, C, Type</t>
         </is>
       </c>
       <c r="H9" t="n">
         <v>2</v>
       </c>
       <c r="I9" s="1" t="n">
-        <v>44942</v>
+        <v>44943</v>
       </c>
       <c r="J9" t="inlineStr">
         <is>
@@ -819,7 +809,7 @@
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>Бел-212</t>
+          <t>Бел-122</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
@@ -829,7 +819,7 @@
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>сер груз Type C</t>
+          <t>груз сер C Type</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
@@ -844,14 +834,14 @@
       </c>
       <c r="G10" t="inlineStr">
         <is>
-          <t>210B, сер, H, Type</t>
+          <t>210B, сер, LS-2, Type</t>
         </is>
       </c>
       <c r="H10" t="n">
         <v>2</v>
       </c>
       <c r="I10" s="1" t="n">
-        <v>44942</v>
+        <v>44943</v>
       </c>
       <c r="J10" t="inlineStr">
         <is>
@@ -862,17 +852,17 @@
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>Бел-200</t>
+          <t>Бел-202</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>21.00R35</t>
+          <t>24.00R35</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>202B сер Type LS-2</t>
+          <t>210B сер LS-2 Type</t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
@@ -887,14 +877,14 @@
       </c>
       <c r="G11" t="inlineStr">
         <is>
-          <t>210B, сер, Type, C</t>
+          <t>210B, сер, H, Type</t>
         </is>
       </c>
       <c r="H11" t="n">
         <v>2</v>
       </c>
       <c r="I11" s="1" t="n">
-        <v>44942</v>
+        <v>44943</v>
       </c>
       <c r="J11" t="inlineStr">
         <is>
@@ -905,17 +895,17 @@
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>Бел-200</t>
+          <t>Бел-202</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>21.00R35</t>
+          <t>24.00R35</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>202B сер H Type</t>
+          <t>210B сер H Type</t>
         </is>
       </c>
       <c r="E12" t="inlineStr">
@@ -925,19 +915,19 @@
       </c>
       <c r="F12" t="inlineStr">
         <is>
-          <t>Бел-212</t>
+          <t>Бел-202</t>
         </is>
       </c>
       <c r="G12" t="inlineStr">
         <is>
-          <t>сер, груз, Type, LS-2</t>
+          <t>210B, сер, C, Type</t>
         </is>
       </c>
       <c r="H12" t="n">
         <v>2</v>
       </c>
       <c r="I12" s="1" t="n">
-        <v>44942</v>
+        <v>44943</v>
       </c>
       <c r="J12" t="inlineStr">
         <is>
@@ -948,17 +938,17 @@
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>Бел-200</t>
+          <t>Бел-202</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>21.00R35</t>
+          <t>24.00R35</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>202B сер Type C</t>
+          <t>210B сер C Type</t>
         </is>
       </c>
       <c r="E13" t="inlineStr">
@@ -973,14 +963,14 @@
       </c>
       <c r="G13" t="inlineStr">
         <is>
-          <t>сер, H, груз, Type</t>
+          <t>груз, сер, LS-2, Type</t>
         </is>
       </c>
       <c r="H13" t="n">
         <v>2</v>
       </c>
       <c r="I13" s="1" t="n">
-        <v>44942</v>
+        <v>44943</v>
       </c>
       <c r="J13" t="inlineStr">
         <is>
@@ -991,17 +981,17 @@
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>Бел-210</t>
+          <t>Бел-212</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>21.00R35</t>
+          <t>24.00R35</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>202B сер Type LS-2</t>
+          <t>груз сер LS-2 Type</t>
         </is>
       </c>
       <c r="E14" t="inlineStr">
@@ -1016,14 +1006,14 @@
       </c>
       <c r="G14" t="inlineStr">
         <is>
-          <t>сер, груз, Type, C</t>
+          <t>груз, сер, H, Type</t>
         </is>
       </c>
       <c r="H14" t="n">
         <v>2</v>
       </c>
       <c r="I14" s="1" t="n">
-        <v>44942</v>
+        <v>44943</v>
       </c>
       <c r="J14" t="inlineStr">
         <is>
@@ -1034,39 +1024,39 @@
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>Бел-210</t>
+          <t>Бел-212</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>21.00R35</t>
+          <t>24.00R35</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>202B сер H Type</t>
+          <t>груз сер H Type</t>
         </is>
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t>21.00R35</t>
+          <t>24.00R35</t>
         </is>
       </c>
       <c r="F15" t="inlineStr">
         <is>
-          <t>Бел-200</t>
+          <t>Бел-212</t>
         </is>
       </c>
       <c r="G15" t="inlineStr">
         <is>
-          <t>202B, сер, Type, LS-2</t>
+          <t>груз, сер, C, Type</t>
         </is>
       </c>
       <c r="H15" t="n">
         <v>2</v>
       </c>
       <c r="I15" s="1" t="n">
-        <v>44942</v>
+        <v>44943</v>
       </c>
       <c r="J15" t="inlineStr">
         <is>
@@ -1077,24 +1067,24 @@
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>Бел-210</t>
+          <t>Бел-212</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
         <is>
+          <t>24.00R35</t>
+        </is>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>груз сер C Type</t>
+        </is>
+      </c>
+      <c r="E16" t="inlineStr">
+        <is>
           <t>21.00R35</t>
         </is>
       </c>
-      <c r="C16" t="inlineStr">
-        <is>
-          <t>202B сер Type C</t>
-        </is>
-      </c>
-      <c r="E16" t="inlineStr">
-        <is>
-          <t>21.00R35</t>
-        </is>
-      </c>
       <c r="F16" t="inlineStr">
         <is>
           <t>Бел-200</t>
@@ -1102,14 +1092,14 @@
       </c>
       <c r="G16" t="inlineStr">
         <is>
-          <t>202B, сер, H, Type</t>
+          <t>202B, сер, LS-2, Type</t>
         </is>
       </c>
       <c r="H16" t="n">
         <v>2</v>
       </c>
       <c r="I16" s="1" t="n">
-        <v>44942</v>
+        <v>44943</v>
       </c>
       <c r="J16" t="inlineStr">
         <is>
@@ -1120,17 +1110,17 @@
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>BEL-248</t>
+          <t>Бел-200</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>14.00R20</t>
+          <t>21.00R35</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>сер груз</t>
+          <t>202B сер LS-2 Type</t>
         </is>
       </c>
       <c r="E17" t="inlineStr">
@@ -1145,14 +1135,14 @@
       </c>
       <c r="G17" t="inlineStr">
         <is>
-          <t>202B, сер, Type, C</t>
+          <t>202B, сер, H, Type</t>
         </is>
       </c>
       <c r="H17" t="n">
         <v>2</v>
       </c>
       <c r="I17" s="1" t="n">
-        <v>44942</v>
+        <v>44943</v>
       </c>
       <c r="J17" t="inlineStr">
         <is>
@@ -1163,17 +1153,17 @@
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>BEL-248</t>
+          <t>Бел-200</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>14.00R20</t>
+          <t>21.00R35</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>сер груз б/к</t>
+          <t>202B сер H Type</t>
         </is>
       </c>
       <c r="E18" t="inlineStr">
@@ -1183,19 +1173,19 @@
       </c>
       <c r="F18" t="inlineStr">
         <is>
-          <t>Бел-210</t>
+          <t>Бел-200</t>
         </is>
       </c>
       <c r="G18" t="inlineStr">
         <is>
-          <t>202B, сер, Type, LS-2</t>
+          <t>202B, сер, C, Type</t>
         </is>
       </c>
       <c r="H18" t="n">
         <v>2</v>
       </c>
       <c r="I18" s="1" t="n">
-        <v>44942</v>
+        <v>44943</v>
       </c>
       <c r="J18" t="inlineStr">
         <is>
@@ -1206,17 +1196,17 @@
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>BEL-248</t>
+          <t>Бел-200</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>14.00R20</t>
+          <t>21.00R35</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>сер груз</t>
+          <t>202B сер C Type</t>
         </is>
       </c>
       <c r="E19" t="inlineStr">
@@ -1231,14 +1221,14 @@
       </c>
       <c r="G19" t="inlineStr">
         <is>
-          <t>202B, сер, H, Type</t>
+          <t>202B, сер, LS-2, Type</t>
         </is>
       </c>
       <c r="H19" t="n">
         <v>2</v>
       </c>
       <c r="I19" s="1" t="n">
-        <v>44942</v>
+        <v>44943</v>
       </c>
       <c r="J19" t="inlineStr">
         <is>
@@ -1249,17 +1239,17 @@
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>BEL-248</t>
+          <t>Бел-210</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>14.00R20</t>
+          <t>21.00R35</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>сер груз</t>
+          <t>202B сер LS-2 Type</t>
         </is>
       </c>
       <c r="E20" t="inlineStr">
@@ -1274,14 +1264,14 @@
       </c>
       <c r="G20" t="inlineStr">
         <is>
-          <t>202B, сер, Type, C</t>
+          <t>202B, сер, H, Type</t>
         </is>
       </c>
       <c r="H20" t="n">
         <v>2</v>
       </c>
       <c r="I20" s="1" t="n">
-        <v>44942</v>
+        <v>44943</v>
       </c>
       <c r="J20" t="inlineStr">
         <is>
@@ -1292,39 +1282,39 @@
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>BEL-288</t>
+          <t>Бел-210</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>12.00R20</t>
+          <t>21.00R35</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>сер груз</t>
+          <t>202B сер H Type</t>
         </is>
       </c>
       <c r="E21" t="inlineStr">
         <is>
-          <t>14.00R20</t>
+          <t>21.00R35</t>
         </is>
       </c>
       <c r="F21" t="inlineStr">
         <is>
-          <t>BEL-248</t>
+          <t>Бел-210</t>
         </is>
       </c>
       <c r="G21" t="inlineStr">
         <is>
-          <t>сер, груз</t>
+          <t>202B, сер, C, Type</t>
         </is>
       </c>
       <c r="H21" t="n">
         <v>2</v>
       </c>
       <c r="I21" s="1" t="n">
-        <v>44942</v>
+        <v>44943</v>
       </c>
       <c r="J21" t="inlineStr">
         <is>
@@ -1335,17 +1325,17 @@
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>Бел-95</t>
+          <t>Бел-210</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>16.00R20</t>
+          <t>21.00R35</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>173G сер груз б/к</t>
+          <t>202B сер C Type</t>
         </is>
       </c>
       <c r="E22" t="inlineStr">
@@ -1360,14 +1350,14 @@
       </c>
       <c r="G22" t="inlineStr">
         <is>
-          <t>сер, груз</t>
+          <t>груз, сер, б/к</t>
         </is>
       </c>
       <c r="H22" t="n">
         <v>2</v>
       </c>
       <c r="I22" s="1" t="n">
-        <v>44942</v>
+        <v>44943</v>
       </c>
       <c r="J22" t="inlineStr">
         <is>
@@ -1378,17 +1368,17 @@
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>Бел-95</t>
+          <t>BEL-248</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>16.00R20</t>
+          <t>14.00R20</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>173G сер груз</t>
+          <t>груз сер</t>
         </is>
       </c>
       <c r="E23" t="inlineStr">
@@ -1403,14 +1393,14 @@
       </c>
       <c r="G23" t="inlineStr">
         <is>
-          <t>сер, груз</t>
+          <t>груз, сер</t>
         </is>
       </c>
       <c r="H23" t="n">
         <v>2</v>
       </c>
       <c r="I23" s="1" t="n">
-        <v>44942</v>
+        <v>44943</v>
       </c>
       <c r="J23" t="inlineStr">
         <is>
@@ -1421,17 +1411,17 @@
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>Бел-95</t>
+          <t>BEL-248</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>16.00R20</t>
+          <t>14.00R20</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>173G сер груз</t>
+          <t>груз сер б/к</t>
         </is>
       </c>
       <c r="E24" t="inlineStr">
@@ -1446,14 +1436,14 @@
       </c>
       <c r="G24" t="inlineStr">
         <is>
-          <t>сер, груз, б/к</t>
+          <t>груз, сер</t>
         </is>
       </c>
       <c r="H24" t="n">
         <v>2</v>
       </c>
       <c r="I24" s="1" t="n">
-        <v>44942</v>
+        <v>44943</v>
       </c>
       <c r="J24" t="inlineStr">
         <is>
@@ -1464,39 +1454,39 @@
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>Бел-95</t>
+          <t>BEL-248</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>16.00R20</t>
+          <t>14.00R20</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>173G сер груз</t>
+          <t>груз сер</t>
         </is>
       </c>
       <c r="E25" t="inlineStr">
         <is>
-          <t>12.00R20</t>
+          <t>14.00R20</t>
         </is>
       </c>
       <c r="F25" t="inlineStr">
         <is>
-          <t>BEL-288</t>
+          <t>BEL-248</t>
         </is>
       </c>
       <c r="G25" t="inlineStr">
         <is>
-          <t>сер, груз</t>
+          <t>груз, сер</t>
         </is>
       </c>
       <c r="H25" t="n">
         <v>2</v>
       </c>
       <c r="I25" s="1" t="n">
-        <v>44942</v>
+        <v>44943</v>
       </c>
       <c r="J25" t="inlineStr">
         <is>
@@ -1507,39 +1497,39 @@
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>Бел-95</t>
+          <t>BEL-248</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>16.00R20</t>
+          <t>14.00R20</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>173G сер груз</t>
+          <t>груз сер</t>
         </is>
       </c>
       <c r="E26" t="inlineStr">
         <is>
-          <t>16.00R20</t>
+          <t>175/70R13</t>
         </is>
       </c>
       <c r="F26" t="inlineStr">
         <is>
-          <t>Бел-95</t>
+          <t>Бел-103</t>
         </is>
       </c>
       <c r="G26" t="inlineStr">
         <is>
-          <t>173G, сер, груз, б/к</t>
+          <t>сер, легк, б/к</t>
         </is>
       </c>
       <c r="H26" t="n">
         <v>2</v>
       </c>
       <c r="I26" s="1" t="n">
-        <v>44942</v>
+        <v>44943</v>
       </c>
       <c r="J26" t="inlineStr">
         <is>
@@ -1550,39 +1540,39 @@
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>Бел-95</t>
+          <t>Бел-103</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>16.00R20</t>
+          <t>175/70R13</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>173G сер груз</t>
+          <t>сер легк б/к</t>
         </is>
       </c>
       <c r="E27" t="inlineStr">
         <is>
-          <t>16.00R20</t>
+          <t>175/70R13</t>
         </is>
       </c>
       <c r="F27" t="inlineStr">
         <is>
-          <t>Бел-95</t>
+          <t>Бел-100</t>
         </is>
       </c>
       <c r="G27" t="inlineStr">
         <is>
-          <t>173G, сер, груз</t>
+          <t>сер, легк, б/к</t>
         </is>
       </c>
       <c r="H27" t="n">
         <v>2</v>
       </c>
       <c r="I27" s="1" t="n">
-        <v>44942</v>
+        <v>44943</v>
       </c>
       <c r="J27" t="inlineStr">
         <is>
@@ -1593,39 +1583,39 @@
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>Бел-95</t>
+          <t>Бел-100</t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>16.00R20</t>
+          <t>175/70R13</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>173G сер</t>
+          <t>сер легк б/к</t>
         </is>
       </c>
       <c r="E28" t="inlineStr">
         <is>
-          <t>16.00R20</t>
+          <t>195/65R15</t>
         </is>
       </c>
       <c r="F28" t="inlineStr">
         <is>
-          <t>Бел-95</t>
+          <t>Бел-119</t>
         </is>
       </c>
       <c r="G28" t="inlineStr">
         <is>
-          <t>173G, сер, груз</t>
+          <t>сер, легк</t>
         </is>
       </c>
       <c r="H28" t="n">
         <v>2</v>
       </c>
       <c r="I28" s="1" t="n">
-        <v>44942</v>
+        <v>44943</v>
       </c>
       <c r="J28" t="inlineStr">
         <is>
@@ -1636,39 +1626,39 @@
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>BEL-405</t>
+          <t>Ф-35-1</t>
         </is>
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>395/85R20</t>
+          <t>11.2-20</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>168J сер груз</t>
+          <t>8 сер сх</t>
         </is>
       </c>
       <c r="E29" t="inlineStr">
         <is>
-          <t>16.00R20</t>
+          <t>195/65R15</t>
         </is>
       </c>
       <c r="F29" t="inlineStr">
         <is>
-          <t>Бел-95</t>
+          <t>Бел-119</t>
         </is>
       </c>
       <c r="G29" t="inlineStr">
         <is>
-          <t>173G, сер, груз</t>
+          <t>сер, легк</t>
         </is>
       </c>
       <c r="H29" t="n">
         <v>2</v>
       </c>
       <c r="I29" s="1" t="n">
-        <v>44942</v>
+        <v>44943</v>
       </c>
       <c r="J29" t="inlineStr">
         <is>
@@ -1679,39 +1669,39 @@
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>Бел-145</t>
+          <t>Бел-119</t>
         </is>
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>445/65R22.5</t>
+          <t>195/65R15</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>сер груз б/к</t>
+          <t>сер легк</t>
         </is>
       </c>
       <c r="E30" t="inlineStr">
         <is>
-          <t>16.00R20</t>
+          <t>195/65R15</t>
         </is>
       </c>
       <c r="F30" t="inlineStr">
         <is>
-          <t>Бел-95</t>
+          <t>Бел-119</t>
         </is>
       </c>
       <c r="G30" t="inlineStr">
         <is>
-          <t>173G, сер, груз</t>
+          <t>сер, легк</t>
         </is>
       </c>
       <c r="H30" t="n">
         <v>2</v>
       </c>
       <c r="I30" s="1" t="n">
-        <v>44942</v>
+        <v>44943</v>
       </c>
       <c r="J30" t="inlineStr">
         <is>
@@ -1722,413 +1712,34 @@
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>Бел-230</t>
+          <t>Бел-119</t>
         </is>
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>355/65-15</t>
+          <t>195/65R15</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>сер</t>
-        </is>
-      </c>
-      <c r="E31" t="inlineStr">
-        <is>
-          <t>16.00R20</t>
-        </is>
-      </c>
-      <c r="F31" t="inlineStr">
-        <is>
-          <t>Бел-95</t>
-        </is>
-      </c>
-      <c r="G31" t="inlineStr">
-        <is>
-          <t>173G, сер, груз</t>
-        </is>
-      </c>
-      <c r="H31" t="n">
-        <v>2</v>
-      </c>
-      <c r="I31" s="1" t="n">
-        <v>44942</v>
-      </c>
-      <c r="J31" t="inlineStr">
-        <is>
-          <t>нет данных</t>
+          <t>сер легк</t>
         </is>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>Бел-230М</t>
+          <t>Бел-119</t>
         </is>
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>355/65-15</t>
+          <t>195/65R15</t>
         </is>
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>сер</t>
-        </is>
-      </c>
-      <c r="E32" t="inlineStr">
-        <is>
-          <t>16.00R20</t>
-        </is>
-      </c>
-      <c r="F32" t="inlineStr">
-        <is>
-          <t>Бел-95</t>
-        </is>
-      </c>
-      <c r="G32" t="inlineStr">
-        <is>
-          <t>173G, сер</t>
-        </is>
-      </c>
-      <c r="H32" t="n">
-        <v>2</v>
-      </c>
-      <c r="I32" s="1" t="n">
-        <v>44942</v>
-      </c>
-      <c r="J32" t="inlineStr">
-        <is>
-          <t>нет данных</t>
-        </is>
-      </c>
-    </row>
-    <row r="33">
-      <c r="A33" t="inlineStr">
-        <is>
-          <t>BEL-262</t>
-        </is>
-      </c>
-      <c r="B33" t="inlineStr">
-        <is>
-          <t>205/55R16</t>
-        </is>
-      </c>
-      <c r="C33" t="inlineStr">
-        <is>
-          <t>сер легк б/к</t>
-        </is>
-      </c>
-      <c r="E33" t="inlineStr">
-        <is>
-          <t>395/85R20</t>
-        </is>
-      </c>
-      <c r="F33" t="inlineStr">
-        <is>
-          <t>BEL-405</t>
-        </is>
-      </c>
-      <c r="G33" t="inlineStr">
-        <is>
-          <t>168J, сер, груз</t>
-        </is>
-      </c>
-      <c r="H33" t="n">
-        <v>2</v>
-      </c>
-      <c r="I33" s="1" t="n">
-        <v>44942</v>
-      </c>
-      <c r="J33" t="inlineStr">
-        <is>
-          <t>нет данных</t>
-        </is>
-      </c>
-    </row>
-    <row r="34">
-      <c r="A34" t="inlineStr">
-        <is>
-          <t>BEL-317</t>
-        </is>
-      </c>
-      <c r="B34" t="inlineStr">
-        <is>
-          <t>205/55R16</t>
-        </is>
-      </c>
-      <c r="C34" t="inlineStr">
-        <is>
-          <t>сер легк б/к</t>
-        </is>
-      </c>
-      <c r="E34" t="inlineStr">
-        <is>
-          <t>445/65R22.5</t>
-        </is>
-      </c>
-      <c r="F34" t="inlineStr">
-        <is>
-          <t>Бел-145</t>
-        </is>
-      </c>
-      <c r="G34" t="inlineStr">
-        <is>
-          <t>сер, груз, б/к</t>
-        </is>
-      </c>
-      <c r="H34" t="n">
-        <v>2</v>
-      </c>
-      <c r="I34" s="1" t="n">
-        <v>44942</v>
-      </c>
-      <c r="J34" t="inlineStr">
-        <is>
-          <t>нет данных</t>
-        </is>
-      </c>
-    </row>
-    <row r="35">
-      <c r="A35" t="inlineStr">
-        <is>
-          <t>BEL-317S</t>
-        </is>
-      </c>
-      <c r="B35" t="inlineStr">
-        <is>
-          <t>205/55R16</t>
-        </is>
-      </c>
-      <c r="C35" t="inlineStr">
-        <is>
-          <t>сер ошип</t>
-        </is>
-      </c>
-      <c r="E35" t="inlineStr">
-        <is>
-          <t>355/65-15</t>
-        </is>
-      </c>
-      <c r="F35" t="inlineStr">
-        <is>
-          <t>Бел-230</t>
-        </is>
-      </c>
-      <c r="G35" t="inlineStr">
-        <is>
-          <t>сер</t>
-        </is>
-      </c>
-      <c r="H35" t="n">
-        <v>2</v>
-      </c>
-      <c r="I35" s="1" t="n">
-        <v>44942</v>
-      </c>
-      <c r="J35" t="inlineStr">
-        <is>
-          <t>нет данных</t>
-        </is>
-      </c>
-    </row>
-    <row r="36">
-      <c r="A36" t="inlineStr">
-        <is>
-          <t>BEL-277</t>
-        </is>
-      </c>
-      <c r="B36" t="inlineStr">
-        <is>
-          <t>205/60R16</t>
-        </is>
-      </c>
-      <c r="C36" t="inlineStr">
-        <is>
-          <t>сер легк б/к</t>
-        </is>
-      </c>
-      <c r="E36" t="inlineStr">
-        <is>
-          <t>355/65-15</t>
-        </is>
-      </c>
-      <c r="F36" t="inlineStr">
-        <is>
-          <t>Бел-230М</t>
-        </is>
-      </c>
-      <c r="G36" t="inlineStr">
-        <is>
-          <t>сер</t>
-        </is>
-      </c>
-      <c r="H36" t="n">
-        <v>2</v>
-      </c>
-      <c r="I36" s="1" t="n">
-        <v>44942</v>
-      </c>
-      <c r="J36" t="inlineStr">
-        <is>
-          <t>нет данных</t>
-        </is>
-      </c>
-    </row>
-    <row r="37">
-      <c r="A37" t="inlineStr">
-        <is>
-          <t>Бел-103</t>
-        </is>
-      </c>
-      <c r="B37" t="inlineStr">
-        <is>
-          <t>175/70R13</t>
-        </is>
-      </c>
-      <c r="C37" t="inlineStr">
-        <is>
-          <t>сер легк б/к</t>
-        </is>
-      </c>
-      <c r="E37" t="inlineStr">
-        <is>
-          <t>205/55R16</t>
-        </is>
-      </c>
-      <c r="F37" t="inlineStr">
-        <is>
-          <t>BEL-262</t>
-        </is>
-      </c>
-      <c r="G37" t="inlineStr">
-        <is>
-          <t>сер, легк, б/к</t>
-        </is>
-      </c>
-      <c r="H37" t="n">
-        <v>2</v>
-      </c>
-      <c r="I37" s="1" t="n">
-        <v>44942</v>
-      </c>
-      <c r="J37" t="inlineStr">
-        <is>
-          <t>нет данных</t>
-        </is>
-      </c>
-    </row>
-    <row r="38">
-      <c r="E38" t="inlineStr">
-        <is>
-          <t>205/55R16</t>
-        </is>
-      </c>
-      <c r="F38" t="inlineStr">
-        <is>
-          <t>BEL-317</t>
-        </is>
-      </c>
-      <c r="G38" t="inlineStr">
-        <is>
-          <t>сер, легк, б/к</t>
-        </is>
-      </c>
-      <c r="H38" t="n">
-        <v>2</v>
-      </c>
-      <c r="I38" s="1" t="n">
-        <v>44942</v>
-      </c>
-      <c r="J38" t="inlineStr">
-        <is>
-          <t>нет данных</t>
-        </is>
-      </c>
-    </row>
-    <row r="39">
-      <c r="E39" t="inlineStr">
-        <is>
-          <t>205/55R16</t>
-        </is>
-      </c>
-      <c r="F39" t="inlineStr">
-        <is>
-          <t>BEL-317S</t>
-        </is>
-      </c>
-      <c r="G39" t="inlineStr">
-        <is>
-          <t>сер, ошип</t>
-        </is>
-      </c>
-      <c r="H39" t="n">
-        <v>2</v>
-      </c>
-      <c r="I39" s="1" t="n">
-        <v>44942</v>
-      </c>
-      <c r="J39" t="inlineStr">
-        <is>
-          <t>нет данных</t>
-        </is>
-      </c>
-    </row>
-    <row r="40">
-      <c r="E40" t="inlineStr">
-        <is>
-          <t>205/60R16</t>
-        </is>
-      </c>
-      <c r="F40" t="inlineStr">
-        <is>
-          <t>BEL-277</t>
-        </is>
-      </c>
-      <c r="G40" t="inlineStr">
-        <is>
-          <t>сер, легк, б/к</t>
-        </is>
-      </c>
-      <c r="H40" t="n">
-        <v>2</v>
-      </c>
-      <c r="I40" s="1" t="n">
-        <v>44942</v>
-      </c>
-      <c r="J40" t="inlineStr">
-        <is>
-          <t>нет данных</t>
-        </is>
-      </c>
-    </row>
-    <row r="41">
-      <c r="E41" t="inlineStr">
-        <is>
-          <t>175/70R13</t>
-        </is>
-      </c>
-      <c r="F41" t="inlineStr">
-        <is>
-          <t>Бел-103</t>
-        </is>
-      </c>
-      <c r="G41" t="inlineStr">
-        <is>
-          <t>сер, легк, б/к</t>
-        </is>
-      </c>
-      <c r="H41" t="n">
-        <v>2</v>
-      </c>
-      <c r="I41" s="1" t="n">
-        <v>44942</v>
-      </c>
-      <c r="J41" t="inlineStr">
-        <is>
-          <t>нет данных</t>
+          <t>сер легк</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
improved prices filter switchers  at 05/02/2023
</commit_message>
<xml_diff>
--- a/src/Tyres.xlsx
+++ b/src/Tyres.xlsx
@@ -17,7 +17,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="0"/>
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="yyyy-mm-dd"/>
+  </numFmts>
   <fonts count="1">
     <font>
       <name val="Calibri"/>
@@ -47,8 +49,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
@@ -414,7 +417,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C38"/>
+  <dimension ref="A1:J51"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -438,6 +441,36 @@
           <t>42 сер груз</t>
         </is>
       </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>Tyre Size</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>Model</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
+        <is>
+          <t>Param</t>
+        </is>
+      </c>
+      <c r="H1" t="inlineStr">
+        <is>
+          <t>Sales value</t>
+        </is>
+      </c>
+      <c r="I1" t="inlineStr">
+        <is>
+          <t>Date_of_sales</t>
+        </is>
+      </c>
+      <c r="J1" t="inlineStr">
+        <is>
+          <t>Contragent</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
@@ -455,6 +488,32 @@
           <t>Type сер груз LS-2</t>
         </is>
       </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>35/65-33</t>
+        </is>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>ФБел-283</t>
+        </is>
+      </c>
+      <c r="G2" t="inlineStr">
+        <is>
+          <t>42, сер, груз</t>
+        </is>
+      </c>
+      <c r="H2" t="n">
+        <v>2</v>
+      </c>
+      <c r="I2" s="1" t="n">
+        <v>44949</v>
+      </c>
+      <c r="J2" t="inlineStr">
+        <is>
+          <t>нет данных</t>
+        </is>
+      </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -472,6 +531,32 @@
           <t>H Type сер груз</t>
         </is>
       </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>205/55R16</t>
+        </is>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>BEL-262</t>
+        </is>
+      </c>
+      <c r="G3" t="inlineStr">
+        <is>
+          <t>сер, легк, б/к</t>
+        </is>
+      </c>
+      <c r="H3" t="n">
+        <v>2</v>
+      </c>
+      <c r="I3" s="1" t="n">
+        <v>44949</v>
+      </c>
+      <c r="J3" t="inlineStr">
+        <is>
+          <t>нет данных</t>
+        </is>
+      </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
@@ -489,6 +574,32 @@
           <t>Type сер груз C</t>
         </is>
       </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>205/55R16</t>
+        </is>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>BEL-317</t>
+        </is>
+      </c>
+      <c r="G4" t="inlineStr">
+        <is>
+          <t>сер, легк, б/к</t>
+        </is>
+      </c>
+      <c r="H4" t="n">
+        <v>2</v>
+      </c>
+      <c r="I4" s="1" t="n">
+        <v>44949</v>
+      </c>
+      <c r="J4" t="inlineStr">
+        <is>
+          <t>нет данных</t>
+        </is>
+      </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
@@ -506,6 +617,32 @@
           <t>210B Type сер LS-2</t>
         </is>
       </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>205/55R16</t>
+        </is>
+      </c>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>BEL-317S</t>
+        </is>
+      </c>
+      <c r="G5" t="inlineStr">
+        <is>
+          <t>сер, ошип</t>
+        </is>
+      </c>
+      <c r="H5" t="n">
+        <v>2</v>
+      </c>
+      <c r="I5" s="1" t="n">
+        <v>44949</v>
+      </c>
+      <c r="J5" t="inlineStr">
+        <is>
+          <t>нет данных</t>
+        </is>
+      </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
@@ -523,6 +660,32 @@
           <t>210B H Type сер</t>
         </is>
       </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>24.00R35</t>
+        </is>
+      </c>
+      <c r="F6" t="inlineStr">
+        <is>
+          <t>Бел-122</t>
+        </is>
+      </c>
+      <c r="G6" t="inlineStr">
+        <is>
+          <t>Type, сер, груз, LS-2</t>
+        </is>
+      </c>
+      <c r="H6" t="n">
+        <v>2</v>
+      </c>
+      <c r="I6" s="1" t="n">
+        <v>44949</v>
+      </c>
+      <c r="J6" t="inlineStr">
+        <is>
+          <t>нет данных</t>
+        </is>
+      </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
@@ -540,6 +703,32 @@
           <t>210B Type сер C</t>
         </is>
       </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>24.00R35</t>
+        </is>
+      </c>
+      <c r="F7" t="inlineStr">
+        <is>
+          <t>Бел-122</t>
+        </is>
+      </c>
+      <c r="G7" t="inlineStr">
+        <is>
+          <t>H, Type, сер, груз</t>
+        </is>
+      </c>
+      <c r="H7" t="n">
+        <v>2</v>
+      </c>
+      <c r="I7" s="1" t="n">
+        <v>44949</v>
+      </c>
+      <c r="J7" t="inlineStr">
+        <is>
+          <t>нет данных</t>
+        </is>
+      </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
@@ -557,6 +746,32 @@
           <t>Type сер груз LS-2</t>
         </is>
       </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>24.00R35</t>
+        </is>
+      </c>
+      <c r="F8" t="inlineStr">
+        <is>
+          <t>Бел-122</t>
+        </is>
+      </c>
+      <c r="G8" t="inlineStr">
+        <is>
+          <t>Type, сер, груз, C</t>
+        </is>
+      </c>
+      <c r="H8" t="n">
+        <v>2</v>
+      </c>
+      <c r="I8" s="1" t="n">
+        <v>44949</v>
+      </c>
+      <c r="J8" t="inlineStr">
+        <is>
+          <t>нет данных</t>
+        </is>
+      </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
@@ -574,6 +789,32 @@
           <t>H Type сер груз</t>
         </is>
       </c>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>24.00R35</t>
+        </is>
+      </c>
+      <c r="F9" t="inlineStr">
+        <is>
+          <t>Бел-202</t>
+        </is>
+      </c>
+      <c r="G9" t="inlineStr">
+        <is>
+          <t>210B, Type, сер, LS-2</t>
+        </is>
+      </c>
+      <c r="H9" t="n">
+        <v>2</v>
+      </c>
+      <c r="I9" s="1" t="n">
+        <v>44949</v>
+      </c>
+      <c r="J9" t="inlineStr">
+        <is>
+          <t>нет данных</t>
+        </is>
+      </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
@@ -591,6 +832,32 @@
           <t>Type сер груз C</t>
         </is>
       </c>
+      <c r="E10" t="inlineStr">
+        <is>
+          <t>24.00R35</t>
+        </is>
+      </c>
+      <c r="F10" t="inlineStr">
+        <is>
+          <t>Бел-202</t>
+        </is>
+      </c>
+      <c r="G10" t="inlineStr">
+        <is>
+          <t>210B, H, Type, сер</t>
+        </is>
+      </c>
+      <c r="H10" t="n">
+        <v>2</v>
+      </c>
+      <c r="I10" s="1" t="n">
+        <v>44949</v>
+      </c>
+      <c r="J10" t="inlineStr">
+        <is>
+          <t>нет данных</t>
+        </is>
+      </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
@@ -608,6 +875,32 @@
           <t>202B Type сер LS-2</t>
         </is>
       </c>
+      <c r="E11" t="inlineStr">
+        <is>
+          <t>24.00R35</t>
+        </is>
+      </c>
+      <c r="F11" t="inlineStr">
+        <is>
+          <t>Бел-202</t>
+        </is>
+      </c>
+      <c r="G11" t="inlineStr">
+        <is>
+          <t>210B, Type, сер, C</t>
+        </is>
+      </c>
+      <c r="H11" t="n">
+        <v>2</v>
+      </c>
+      <c r="I11" s="1" t="n">
+        <v>44949</v>
+      </c>
+      <c r="J11" t="inlineStr">
+        <is>
+          <t>нет данных</t>
+        </is>
+      </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
@@ -625,6 +918,32 @@
           <t>202B H Type сер</t>
         </is>
       </c>
+      <c r="E12" t="inlineStr">
+        <is>
+          <t>24.00R35</t>
+        </is>
+      </c>
+      <c r="F12" t="inlineStr">
+        <is>
+          <t>Бел-212</t>
+        </is>
+      </c>
+      <c r="G12" t="inlineStr">
+        <is>
+          <t>Type, сер, груз, LS-2</t>
+        </is>
+      </c>
+      <c r="H12" t="n">
+        <v>2</v>
+      </c>
+      <c r="I12" s="1" t="n">
+        <v>44949</v>
+      </c>
+      <c r="J12" t="inlineStr">
+        <is>
+          <t>нет данных</t>
+        </is>
+      </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
@@ -642,6 +961,32 @@
           <t>202B Type сер C</t>
         </is>
       </c>
+      <c r="E13" t="inlineStr">
+        <is>
+          <t>24.00R35</t>
+        </is>
+      </c>
+      <c r="F13" t="inlineStr">
+        <is>
+          <t>Бел-212</t>
+        </is>
+      </c>
+      <c r="G13" t="inlineStr">
+        <is>
+          <t>H, Type, сер, груз</t>
+        </is>
+      </c>
+      <c r="H13" t="n">
+        <v>2</v>
+      </c>
+      <c r="I13" s="1" t="n">
+        <v>44949</v>
+      </c>
+      <c r="J13" t="inlineStr">
+        <is>
+          <t>нет данных</t>
+        </is>
+      </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
@@ -659,6 +1004,32 @@
           <t>202B Type сер LS-2</t>
         </is>
       </c>
+      <c r="E14" t="inlineStr">
+        <is>
+          <t>24.00R35</t>
+        </is>
+      </c>
+      <c r="F14" t="inlineStr">
+        <is>
+          <t>Бел-212</t>
+        </is>
+      </c>
+      <c r="G14" t="inlineStr">
+        <is>
+          <t>Type, сер, груз, C</t>
+        </is>
+      </c>
+      <c r="H14" t="n">
+        <v>2</v>
+      </c>
+      <c r="I14" s="1" t="n">
+        <v>44949</v>
+      </c>
+      <c r="J14" t="inlineStr">
+        <is>
+          <t>нет данных</t>
+        </is>
+      </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
@@ -676,6 +1047,32 @@
           <t>202B H Type сер</t>
         </is>
       </c>
+      <c r="E15" t="inlineStr">
+        <is>
+          <t>21.00R35</t>
+        </is>
+      </c>
+      <c r="F15" t="inlineStr">
+        <is>
+          <t>Бел-200</t>
+        </is>
+      </c>
+      <c r="G15" t="inlineStr">
+        <is>
+          <t>202B, Type, сер, LS-2</t>
+        </is>
+      </c>
+      <c r="H15" t="n">
+        <v>2</v>
+      </c>
+      <c r="I15" s="1" t="n">
+        <v>44949</v>
+      </c>
+      <c r="J15" t="inlineStr">
+        <is>
+          <t>нет данных</t>
+        </is>
+      </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
@@ -693,6 +1090,32 @@
           <t>202B Type сер C</t>
         </is>
       </c>
+      <c r="E16" t="inlineStr">
+        <is>
+          <t>21.00R35</t>
+        </is>
+      </c>
+      <c r="F16" t="inlineStr">
+        <is>
+          <t>Бел-200</t>
+        </is>
+      </c>
+      <c r="G16" t="inlineStr">
+        <is>
+          <t>202B, H, Type, сер</t>
+        </is>
+      </c>
+      <c r="H16" t="n">
+        <v>2</v>
+      </c>
+      <c r="I16" s="1" t="n">
+        <v>44949</v>
+      </c>
+      <c r="J16" t="inlineStr">
+        <is>
+          <t>нет данных</t>
+        </is>
+      </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
@@ -710,6 +1133,32 @@
           <t>сер груз</t>
         </is>
       </c>
+      <c r="E17" t="inlineStr">
+        <is>
+          <t>21.00R35</t>
+        </is>
+      </c>
+      <c r="F17" t="inlineStr">
+        <is>
+          <t>Бел-200</t>
+        </is>
+      </c>
+      <c r="G17" t="inlineStr">
+        <is>
+          <t>202B, Type, сер, C</t>
+        </is>
+      </c>
+      <c r="H17" t="n">
+        <v>2</v>
+      </c>
+      <c r="I17" s="1" t="n">
+        <v>44949</v>
+      </c>
+      <c r="J17" t="inlineStr">
+        <is>
+          <t>нет данных</t>
+        </is>
+      </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
@@ -727,6 +1176,32 @@
           <t>сер груз б/к</t>
         </is>
       </c>
+      <c r="E18" t="inlineStr">
+        <is>
+          <t>21.00R35</t>
+        </is>
+      </c>
+      <c r="F18" t="inlineStr">
+        <is>
+          <t>Бел-210</t>
+        </is>
+      </c>
+      <c r="G18" t="inlineStr">
+        <is>
+          <t>202B, Type, сер, LS-2</t>
+        </is>
+      </c>
+      <c r="H18" t="n">
+        <v>2</v>
+      </c>
+      <c r="I18" s="1" t="n">
+        <v>44949</v>
+      </c>
+      <c r="J18" t="inlineStr">
+        <is>
+          <t>нет данных</t>
+        </is>
+      </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
@@ -744,6 +1219,32 @@
           <t>сер груз</t>
         </is>
       </c>
+      <c r="E19" t="inlineStr">
+        <is>
+          <t>21.00R35</t>
+        </is>
+      </c>
+      <c r="F19" t="inlineStr">
+        <is>
+          <t>Бел-210</t>
+        </is>
+      </c>
+      <c r="G19" t="inlineStr">
+        <is>
+          <t>202B, H, Type, сер</t>
+        </is>
+      </c>
+      <c r="H19" t="n">
+        <v>2</v>
+      </c>
+      <c r="I19" s="1" t="n">
+        <v>44949</v>
+      </c>
+      <c r="J19" t="inlineStr">
+        <is>
+          <t>нет данных</t>
+        </is>
+      </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
@@ -761,6 +1262,32 @@
           <t>сер груз</t>
         </is>
       </c>
+      <c r="E20" t="inlineStr">
+        <is>
+          <t>21.00R35</t>
+        </is>
+      </c>
+      <c r="F20" t="inlineStr">
+        <is>
+          <t>Бел-210</t>
+        </is>
+      </c>
+      <c r="G20" t="inlineStr">
+        <is>
+          <t>202B, Type, сер, C</t>
+        </is>
+      </c>
+      <c r="H20" t="n">
+        <v>2</v>
+      </c>
+      <c r="I20" s="1" t="n">
+        <v>44949</v>
+      </c>
+      <c r="J20" t="inlineStr">
+        <is>
+          <t>нет данных</t>
+        </is>
+      </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
@@ -778,6 +1305,32 @@
           <t>сер груз</t>
         </is>
       </c>
+      <c r="E21" t="inlineStr">
+        <is>
+          <t>14.00R20</t>
+        </is>
+      </c>
+      <c r="F21" t="inlineStr">
+        <is>
+          <t>BEL-248</t>
+        </is>
+      </c>
+      <c r="G21" t="inlineStr">
+        <is>
+          <t>сер, груз</t>
+        </is>
+      </c>
+      <c r="H21" t="n">
+        <v>2</v>
+      </c>
+      <c r="I21" s="1" t="n">
+        <v>44949</v>
+      </c>
+      <c r="J21" t="inlineStr">
+        <is>
+          <t>нет данных</t>
+        </is>
+      </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
@@ -795,6 +1348,32 @@
           <t>173G сер груз б/к</t>
         </is>
       </c>
+      <c r="E22" t="inlineStr">
+        <is>
+          <t>14.00R20</t>
+        </is>
+      </c>
+      <c r="F22" t="inlineStr">
+        <is>
+          <t>BEL-248</t>
+        </is>
+      </c>
+      <c r="G22" t="inlineStr">
+        <is>
+          <t>сер, груз, б/к</t>
+        </is>
+      </c>
+      <c r="H22" t="n">
+        <v>2</v>
+      </c>
+      <c r="I22" s="1" t="n">
+        <v>44949</v>
+      </c>
+      <c r="J22" t="inlineStr">
+        <is>
+          <t>нет данных</t>
+        </is>
+      </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
@@ -812,6 +1391,32 @@
           <t>173G сер груз</t>
         </is>
       </c>
+      <c r="E23" t="inlineStr">
+        <is>
+          <t>14.00R20</t>
+        </is>
+      </c>
+      <c r="F23" t="inlineStr">
+        <is>
+          <t>BEL-248</t>
+        </is>
+      </c>
+      <c r="G23" t="inlineStr">
+        <is>
+          <t>сер, груз</t>
+        </is>
+      </c>
+      <c r="H23" t="n">
+        <v>2</v>
+      </c>
+      <c r="I23" s="1" t="n">
+        <v>44949</v>
+      </c>
+      <c r="J23" t="inlineStr">
+        <is>
+          <t>нет данных</t>
+        </is>
+      </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
@@ -829,6 +1434,32 @@
           <t>173G сер груз</t>
         </is>
       </c>
+      <c r="E24" t="inlineStr">
+        <is>
+          <t>14.00R20</t>
+        </is>
+      </c>
+      <c r="F24" t="inlineStr">
+        <is>
+          <t>BEL-248</t>
+        </is>
+      </c>
+      <c r="G24" t="inlineStr">
+        <is>
+          <t>сер, груз</t>
+        </is>
+      </c>
+      <c r="H24" t="n">
+        <v>2</v>
+      </c>
+      <c r="I24" s="1" t="n">
+        <v>44949</v>
+      </c>
+      <c r="J24" t="inlineStr">
+        <is>
+          <t>нет данных</t>
+        </is>
+      </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
@@ -846,6 +1477,32 @@
           <t>173G сер груз</t>
         </is>
       </c>
+      <c r="E25" t="inlineStr">
+        <is>
+          <t>175/70R13</t>
+        </is>
+      </c>
+      <c r="F25" t="inlineStr">
+        <is>
+          <t>Бел-103</t>
+        </is>
+      </c>
+      <c r="G25" t="inlineStr">
+        <is>
+          <t>сер, легк, б/к</t>
+        </is>
+      </c>
+      <c r="H25" t="n">
+        <v>2</v>
+      </c>
+      <c r="I25" s="1" t="n">
+        <v>44949</v>
+      </c>
+      <c r="J25" t="inlineStr">
+        <is>
+          <t>нет данных</t>
+        </is>
+      </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
@@ -863,6 +1520,32 @@
           <t>173G сер груз</t>
         </is>
       </c>
+      <c r="E26" t="inlineStr">
+        <is>
+          <t>195/65R15</t>
+        </is>
+      </c>
+      <c r="F26" t="inlineStr">
+        <is>
+          <t>Бел-119</t>
+        </is>
+      </c>
+      <c r="G26" t="inlineStr">
+        <is>
+          <t>сер, легк</t>
+        </is>
+      </c>
+      <c r="H26" t="n">
+        <v>2</v>
+      </c>
+      <c r="I26" s="1" t="n">
+        <v>44949</v>
+      </c>
+      <c r="J26" t="inlineStr">
+        <is>
+          <t>нет данных</t>
+        </is>
+      </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
@@ -880,6 +1563,32 @@
           <t>173G сер груз</t>
         </is>
       </c>
+      <c r="E27" t="inlineStr">
+        <is>
+          <t>35/65-33</t>
+        </is>
+      </c>
+      <c r="F27" t="inlineStr">
+        <is>
+          <t>ФБел-283</t>
+        </is>
+      </c>
+      <c r="G27" t="inlineStr">
+        <is>
+          <t>42, сер, груз</t>
+        </is>
+      </c>
+      <c r="H27" t="n">
+        <v>2</v>
+      </c>
+      <c r="I27" s="1" t="n">
+        <v>44957</v>
+      </c>
+      <c r="J27" t="inlineStr">
+        <is>
+          <t>нет данных</t>
+        </is>
+      </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
@@ -897,6 +1606,32 @@
           <t>173G сер</t>
         </is>
       </c>
+      <c r="E28" t="inlineStr">
+        <is>
+          <t>205/55R16</t>
+        </is>
+      </c>
+      <c r="F28" t="inlineStr">
+        <is>
+          <t>BEL-262</t>
+        </is>
+      </c>
+      <c r="G28" t="inlineStr">
+        <is>
+          <t>сер, легк, б/к</t>
+        </is>
+      </c>
+      <c r="H28" t="n">
+        <v>2</v>
+      </c>
+      <c r="I28" s="1" t="n">
+        <v>44957</v>
+      </c>
+      <c r="J28" t="inlineStr">
+        <is>
+          <t>нет данных</t>
+        </is>
+      </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
@@ -914,6 +1649,32 @@
           <t>168J сер груз</t>
         </is>
       </c>
+      <c r="E29" t="inlineStr">
+        <is>
+          <t>205/55R16</t>
+        </is>
+      </c>
+      <c r="F29" t="inlineStr">
+        <is>
+          <t>BEL-317</t>
+        </is>
+      </c>
+      <c r="G29" t="inlineStr">
+        <is>
+          <t>сер, легк, б/к</t>
+        </is>
+      </c>
+      <c r="H29" t="n">
+        <v>2</v>
+      </c>
+      <c r="I29" s="1" t="n">
+        <v>44957</v>
+      </c>
+      <c r="J29" t="inlineStr">
+        <is>
+          <t>нет данных</t>
+        </is>
+      </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
@@ -931,6 +1692,32 @@
           <t>сер груз б/к</t>
         </is>
       </c>
+      <c r="E30" t="inlineStr">
+        <is>
+          <t>205/55R16</t>
+        </is>
+      </c>
+      <c r="F30" t="inlineStr">
+        <is>
+          <t>BEL-317S</t>
+        </is>
+      </c>
+      <c r="G30" t="inlineStr">
+        <is>
+          <t>сер, ошип</t>
+        </is>
+      </c>
+      <c r="H30" t="n">
+        <v>2</v>
+      </c>
+      <c r="I30" s="1" t="n">
+        <v>44957</v>
+      </c>
+      <c r="J30" t="inlineStr">
+        <is>
+          <t>нет данных</t>
+        </is>
+      </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
@@ -948,6 +1735,32 @@
           <t>сер</t>
         </is>
       </c>
+      <c r="E31" t="inlineStr">
+        <is>
+          <t>24.00R35</t>
+        </is>
+      </c>
+      <c r="F31" t="inlineStr">
+        <is>
+          <t>Бел-122</t>
+        </is>
+      </c>
+      <c r="G31" t="inlineStr">
+        <is>
+          <t>Type, сер, груз, LS-2</t>
+        </is>
+      </c>
+      <c r="H31" t="n">
+        <v>2</v>
+      </c>
+      <c r="I31" s="1" t="n">
+        <v>44957</v>
+      </c>
+      <c r="J31" t="inlineStr">
+        <is>
+          <t>нет данных</t>
+        </is>
+      </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
@@ -965,6 +1778,32 @@
           <t>сер</t>
         </is>
       </c>
+      <c r="E32" t="inlineStr">
+        <is>
+          <t>24.00R35</t>
+        </is>
+      </c>
+      <c r="F32" t="inlineStr">
+        <is>
+          <t>Бел-122</t>
+        </is>
+      </c>
+      <c r="G32" t="inlineStr">
+        <is>
+          <t>H, Type, сер, груз</t>
+        </is>
+      </c>
+      <c r="H32" t="n">
+        <v>2</v>
+      </c>
+      <c r="I32" s="1" t="n">
+        <v>44957</v>
+      </c>
+      <c r="J32" t="inlineStr">
+        <is>
+          <t>нет данных</t>
+        </is>
+      </c>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
@@ -982,6 +1821,32 @@
           <t>сер легк б/к</t>
         </is>
       </c>
+      <c r="E33" t="inlineStr">
+        <is>
+          <t>24.00R35</t>
+        </is>
+      </c>
+      <c r="F33" t="inlineStr">
+        <is>
+          <t>Бел-122</t>
+        </is>
+      </c>
+      <c r="G33" t="inlineStr">
+        <is>
+          <t>Type, сер, груз, C</t>
+        </is>
+      </c>
+      <c r="H33" t="n">
+        <v>2</v>
+      </c>
+      <c r="I33" s="1" t="n">
+        <v>44957</v>
+      </c>
+      <c r="J33" t="inlineStr">
+        <is>
+          <t>нет данных</t>
+        </is>
+      </c>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
@@ -999,6 +1864,32 @@
           <t>сер легк б/к</t>
         </is>
       </c>
+      <c r="E34" t="inlineStr">
+        <is>
+          <t>24.00R35</t>
+        </is>
+      </c>
+      <c r="F34" t="inlineStr">
+        <is>
+          <t>Бел-202</t>
+        </is>
+      </c>
+      <c r="G34" t="inlineStr">
+        <is>
+          <t>210B, Type, сер, LS-2</t>
+        </is>
+      </c>
+      <c r="H34" t="n">
+        <v>2</v>
+      </c>
+      <c r="I34" s="1" t="n">
+        <v>44957</v>
+      </c>
+      <c r="J34" t="inlineStr">
+        <is>
+          <t>нет данных</t>
+        </is>
+      </c>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
@@ -1016,6 +1907,32 @@
           <t>сер ошип</t>
         </is>
       </c>
+      <c r="E35" t="inlineStr">
+        <is>
+          <t>24.00R35</t>
+        </is>
+      </c>
+      <c r="F35" t="inlineStr">
+        <is>
+          <t>Бел-202</t>
+        </is>
+      </c>
+      <c r="G35" t="inlineStr">
+        <is>
+          <t>210B, H, Type, сер</t>
+        </is>
+      </c>
+      <c r="H35" t="n">
+        <v>2</v>
+      </c>
+      <c r="I35" s="1" t="n">
+        <v>44957</v>
+      </c>
+      <c r="J35" t="inlineStr">
+        <is>
+          <t>нет данных</t>
+        </is>
+      </c>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
@@ -1033,6 +1950,32 @@
           <t>сер легк б/к</t>
         </is>
       </c>
+      <c r="E36" t="inlineStr">
+        <is>
+          <t>24.00R35</t>
+        </is>
+      </c>
+      <c r="F36" t="inlineStr">
+        <is>
+          <t>Бел-202</t>
+        </is>
+      </c>
+      <c r="G36" t="inlineStr">
+        <is>
+          <t>210B, Type, сер, C</t>
+        </is>
+      </c>
+      <c r="H36" t="n">
+        <v>2</v>
+      </c>
+      <c r="I36" s="1" t="n">
+        <v>44957</v>
+      </c>
+      <c r="J36" t="inlineStr">
+        <is>
+          <t>нет данных</t>
+        </is>
+      </c>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
@@ -1050,6 +1993,32 @@
           <t>сер легк б/к</t>
         </is>
       </c>
+      <c r="E37" t="inlineStr">
+        <is>
+          <t>24.00R35</t>
+        </is>
+      </c>
+      <c r="F37" t="inlineStr">
+        <is>
+          <t>Бел-212</t>
+        </is>
+      </c>
+      <c r="G37" t="inlineStr">
+        <is>
+          <t>Type, сер, груз, LS-2</t>
+        </is>
+      </c>
+      <c r="H37" t="n">
+        <v>2</v>
+      </c>
+      <c r="I37" s="1" t="n">
+        <v>44957</v>
+      </c>
+      <c r="J37" t="inlineStr">
+        <is>
+          <t>нет данных</t>
+        </is>
+      </c>
     </row>
     <row r="38">
       <c r="A38" t="inlineStr">
@@ -1065,6 +2034,396 @@
       <c r="C38" t="inlineStr">
         <is>
           <t>сер легк</t>
+        </is>
+      </c>
+      <c r="E38" t="inlineStr">
+        <is>
+          <t>24.00R35</t>
+        </is>
+      </c>
+      <c r="F38" t="inlineStr">
+        <is>
+          <t>Бел-212</t>
+        </is>
+      </c>
+      <c r="G38" t="inlineStr">
+        <is>
+          <t>H, Type, сер, груз</t>
+        </is>
+      </c>
+      <c r="H38" t="n">
+        <v>2</v>
+      </c>
+      <c r="I38" s="1" t="n">
+        <v>44957</v>
+      </c>
+      <c r="J38" t="inlineStr">
+        <is>
+          <t>нет данных</t>
+        </is>
+      </c>
+    </row>
+    <row r="39">
+      <c r="E39" t="inlineStr">
+        <is>
+          <t>24.00R35</t>
+        </is>
+      </c>
+      <c r="F39" t="inlineStr">
+        <is>
+          <t>Бел-212</t>
+        </is>
+      </c>
+      <c r="G39" t="inlineStr">
+        <is>
+          <t>Type, сер, груз, C</t>
+        </is>
+      </c>
+      <c r="H39" t="n">
+        <v>2</v>
+      </c>
+      <c r="I39" s="1" t="n">
+        <v>44957</v>
+      </c>
+      <c r="J39" t="inlineStr">
+        <is>
+          <t>нет данных</t>
+        </is>
+      </c>
+    </row>
+    <row r="40">
+      <c r="E40" t="inlineStr">
+        <is>
+          <t>21.00R35</t>
+        </is>
+      </c>
+      <c r="F40" t="inlineStr">
+        <is>
+          <t>Бел-200</t>
+        </is>
+      </c>
+      <c r="G40" t="inlineStr">
+        <is>
+          <t>202B, Type, сер, LS-2</t>
+        </is>
+      </c>
+      <c r="H40" t="n">
+        <v>2</v>
+      </c>
+      <c r="I40" s="1" t="n">
+        <v>44957</v>
+      </c>
+      <c r="J40" t="inlineStr">
+        <is>
+          <t>нет данных</t>
+        </is>
+      </c>
+    </row>
+    <row r="41">
+      <c r="E41" t="inlineStr">
+        <is>
+          <t>21.00R35</t>
+        </is>
+      </c>
+      <c r="F41" t="inlineStr">
+        <is>
+          <t>Бел-200</t>
+        </is>
+      </c>
+      <c r="G41" t="inlineStr">
+        <is>
+          <t>202B, H, Type, сер</t>
+        </is>
+      </c>
+      <c r="H41" t="n">
+        <v>2</v>
+      </c>
+      <c r="I41" s="1" t="n">
+        <v>44957</v>
+      </c>
+      <c r="J41" t="inlineStr">
+        <is>
+          <t>нет данных</t>
+        </is>
+      </c>
+    </row>
+    <row r="42">
+      <c r="E42" t="inlineStr">
+        <is>
+          <t>21.00R35</t>
+        </is>
+      </c>
+      <c r="F42" t="inlineStr">
+        <is>
+          <t>Бел-200</t>
+        </is>
+      </c>
+      <c r="G42" t="inlineStr">
+        <is>
+          <t>202B, Type, сер, C</t>
+        </is>
+      </c>
+      <c r="H42" t="n">
+        <v>2</v>
+      </c>
+      <c r="I42" s="1" t="n">
+        <v>44957</v>
+      </c>
+      <c r="J42" t="inlineStr">
+        <is>
+          <t>нет данных</t>
+        </is>
+      </c>
+    </row>
+    <row r="43">
+      <c r="E43" t="inlineStr">
+        <is>
+          <t>21.00R35</t>
+        </is>
+      </c>
+      <c r="F43" t="inlineStr">
+        <is>
+          <t>Бел-210</t>
+        </is>
+      </c>
+      <c r="G43" t="inlineStr">
+        <is>
+          <t>202B, Type, сер, LS-2</t>
+        </is>
+      </c>
+      <c r="H43" t="n">
+        <v>2</v>
+      </c>
+      <c r="I43" s="1" t="n">
+        <v>44957</v>
+      </c>
+      <c r="J43" t="inlineStr">
+        <is>
+          <t>нет данных</t>
+        </is>
+      </c>
+    </row>
+    <row r="44">
+      <c r="E44" t="inlineStr">
+        <is>
+          <t>21.00R35</t>
+        </is>
+      </c>
+      <c r="F44" t="inlineStr">
+        <is>
+          <t>Бел-210</t>
+        </is>
+      </c>
+      <c r="G44" t="inlineStr">
+        <is>
+          <t>202B, H, Type, сер</t>
+        </is>
+      </c>
+      <c r="H44" t="n">
+        <v>2</v>
+      </c>
+      <c r="I44" s="1" t="n">
+        <v>44957</v>
+      </c>
+      <c r="J44" t="inlineStr">
+        <is>
+          <t>нет данных</t>
+        </is>
+      </c>
+    </row>
+    <row r="45">
+      <c r="E45" t="inlineStr">
+        <is>
+          <t>21.00R35</t>
+        </is>
+      </c>
+      <c r="F45" t="inlineStr">
+        <is>
+          <t>Бел-210</t>
+        </is>
+      </c>
+      <c r="G45" t="inlineStr">
+        <is>
+          <t>202B, Type, сер, C</t>
+        </is>
+      </c>
+      <c r="H45" t="n">
+        <v>2</v>
+      </c>
+      <c r="I45" s="1" t="n">
+        <v>44957</v>
+      </c>
+      <c r="J45" t="inlineStr">
+        <is>
+          <t>нет данных</t>
+        </is>
+      </c>
+    </row>
+    <row r="46">
+      <c r="E46" t="inlineStr">
+        <is>
+          <t>14.00R20</t>
+        </is>
+      </c>
+      <c r="F46" t="inlineStr">
+        <is>
+          <t>BEL-248</t>
+        </is>
+      </c>
+      <c r="G46" t="inlineStr">
+        <is>
+          <t>сер, груз</t>
+        </is>
+      </c>
+      <c r="H46" t="n">
+        <v>2</v>
+      </c>
+      <c r="I46" s="1" t="n">
+        <v>44957</v>
+      </c>
+      <c r="J46" t="inlineStr">
+        <is>
+          <t>нет данных</t>
+        </is>
+      </c>
+    </row>
+    <row r="47">
+      <c r="E47" t="inlineStr">
+        <is>
+          <t>14.00R20</t>
+        </is>
+      </c>
+      <c r="F47" t="inlineStr">
+        <is>
+          <t>BEL-248</t>
+        </is>
+      </c>
+      <c r="G47" t="inlineStr">
+        <is>
+          <t>сер, груз, б/к</t>
+        </is>
+      </c>
+      <c r="H47" t="n">
+        <v>2</v>
+      </c>
+      <c r="I47" s="1" t="n">
+        <v>44957</v>
+      </c>
+      <c r="J47" t="inlineStr">
+        <is>
+          <t>нет данных</t>
+        </is>
+      </c>
+    </row>
+    <row r="48">
+      <c r="E48" t="inlineStr">
+        <is>
+          <t>14.00R20</t>
+        </is>
+      </c>
+      <c r="F48" t="inlineStr">
+        <is>
+          <t>BEL-248</t>
+        </is>
+      </c>
+      <c r="G48" t="inlineStr">
+        <is>
+          <t>сер, груз</t>
+        </is>
+      </c>
+      <c r="H48" t="n">
+        <v>2</v>
+      </c>
+      <c r="I48" s="1" t="n">
+        <v>44957</v>
+      </c>
+      <c r="J48" t="inlineStr">
+        <is>
+          <t>нет данных</t>
+        </is>
+      </c>
+    </row>
+    <row r="49">
+      <c r="E49" t="inlineStr">
+        <is>
+          <t>14.00R20</t>
+        </is>
+      </c>
+      <c r="F49" t="inlineStr">
+        <is>
+          <t>BEL-248</t>
+        </is>
+      </c>
+      <c r="G49" t="inlineStr">
+        <is>
+          <t>сер, груз</t>
+        </is>
+      </c>
+      <c r="H49" t="n">
+        <v>2</v>
+      </c>
+      <c r="I49" s="1" t="n">
+        <v>44957</v>
+      </c>
+      <c r="J49" t="inlineStr">
+        <is>
+          <t>нет данных</t>
+        </is>
+      </c>
+    </row>
+    <row r="50">
+      <c r="E50" t="inlineStr">
+        <is>
+          <t>175/70R13</t>
+        </is>
+      </c>
+      <c r="F50" t="inlineStr">
+        <is>
+          <t>Бел-103</t>
+        </is>
+      </c>
+      <c r="G50" t="inlineStr">
+        <is>
+          <t>сер, легк, б/к</t>
+        </is>
+      </c>
+      <c r="H50" t="n">
+        <v>2</v>
+      </c>
+      <c r="I50" s="1" t="n">
+        <v>44957</v>
+      </c>
+      <c r="J50" t="inlineStr">
+        <is>
+          <t>нет данных</t>
+        </is>
+      </c>
+    </row>
+    <row r="51">
+      <c r="E51" t="inlineStr">
+        <is>
+          <t>195/65R15</t>
+        </is>
+      </c>
+      <c r="F51" t="inlineStr">
+        <is>
+          <t>Бел-119</t>
+        </is>
+      </c>
+      <c r="G51" t="inlineStr">
+        <is>
+          <t>сер, легк</t>
+        </is>
+      </c>
+      <c r="H51" t="n">
+        <v>2</v>
+      </c>
+      <c r="I51" s="1" t="n">
+        <v>44957</v>
+      </c>
+      <c r="J51" t="inlineStr">
+        <is>
+          <t>нет данных</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
improved prices table prices currncy input 15/03/2023
</commit_message>
<xml_diff>
--- a/src/Tyres.xlsx
+++ b/src/Tyres.xlsx
@@ -417,7 +417,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J85"/>
+  <dimension ref="A1:J169"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -3419,6 +3419,2358 @@
         <v>44985</v>
       </c>
       <c r="J85" t="inlineStr">
+        <is>
+          <t>нет данных</t>
+        </is>
+      </c>
+    </row>
+    <row r="86">
+      <c r="E86" t="inlineStr">
+        <is>
+          <t>35/65-33</t>
+        </is>
+      </c>
+      <c r="F86" t="inlineStr">
+        <is>
+          <t>ФБел-283</t>
+        </is>
+      </c>
+      <c r="G86" t="inlineStr">
+        <is>
+          <t>42, сер, груз</t>
+        </is>
+      </c>
+      <c r="H86" t="n">
+        <v>2</v>
+      </c>
+      <c r="I86" s="1" t="n">
+        <v>44991</v>
+      </c>
+      <c r="J86" t="inlineStr">
+        <is>
+          <t>нет данных</t>
+        </is>
+      </c>
+    </row>
+    <row r="87">
+      <c r="E87" t="inlineStr">
+        <is>
+          <t>205/55R16</t>
+        </is>
+      </c>
+      <c r="F87" t="inlineStr">
+        <is>
+          <t>BEL-262</t>
+        </is>
+      </c>
+      <c r="G87" t="inlineStr">
+        <is>
+          <t>б/к, сер, легк</t>
+        </is>
+      </c>
+      <c r="H87" t="n">
+        <v>2</v>
+      </c>
+      <c r="I87" s="1" t="n">
+        <v>44991</v>
+      </c>
+      <c r="J87" t="inlineStr">
+        <is>
+          <t>нет данных</t>
+        </is>
+      </c>
+    </row>
+    <row r="88">
+      <c r="E88" t="inlineStr">
+        <is>
+          <t>205/55R16</t>
+        </is>
+      </c>
+      <c r="F88" t="inlineStr">
+        <is>
+          <t>BEL-317</t>
+        </is>
+      </c>
+      <c r="G88" t="inlineStr">
+        <is>
+          <t>б/к, сер, легк</t>
+        </is>
+      </c>
+      <c r="H88" t="n">
+        <v>2</v>
+      </c>
+      <c r="I88" s="1" t="n">
+        <v>44991</v>
+      </c>
+      <c r="J88" t="inlineStr">
+        <is>
+          <t>нет данных</t>
+        </is>
+      </c>
+    </row>
+    <row r="89">
+      <c r="E89" t="inlineStr">
+        <is>
+          <t>205/55R16</t>
+        </is>
+      </c>
+      <c r="F89" t="inlineStr">
+        <is>
+          <t>BEL-317S</t>
+        </is>
+      </c>
+      <c r="G89" t="inlineStr">
+        <is>
+          <t>сер, ошип</t>
+        </is>
+      </c>
+      <c r="H89" t="n">
+        <v>2</v>
+      </c>
+      <c r="I89" s="1" t="n">
+        <v>44991</v>
+      </c>
+      <c r="J89" t="inlineStr">
+        <is>
+          <t>нет данных</t>
+        </is>
+      </c>
+    </row>
+    <row r="90">
+      <c r="E90" t="inlineStr">
+        <is>
+          <t>24.00R35</t>
+        </is>
+      </c>
+      <c r="F90" t="inlineStr">
+        <is>
+          <t>Бел-122</t>
+        </is>
+      </c>
+      <c r="G90" t="inlineStr">
+        <is>
+          <t>Type, сер, груз, LS-2</t>
+        </is>
+      </c>
+      <c r="H90" t="n">
+        <v>2</v>
+      </c>
+      <c r="I90" s="1" t="n">
+        <v>44991</v>
+      </c>
+      <c r="J90" t="inlineStr">
+        <is>
+          <t>нет данных</t>
+        </is>
+      </c>
+    </row>
+    <row r="91">
+      <c r="E91" t="inlineStr">
+        <is>
+          <t>24.00R35</t>
+        </is>
+      </c>
+      <c r="F91" t="inlineStr">
+        <is>
+          <t>Бел-122</t>
+        </is>
+      </c>
+      <c r="G91" t="inlineStr">
+        <is>
+          <t>Type, сер, груз, H</t>
+        </is>
+      </c>
+      <c r="H91" t="n">
+        <v>2</v>
+      </c>
+      <c r="I91" s="1" t="n">
+        <v>44991</v>
+      </c>
+      <c r="J91" t="inlineStr">
+        <is>
+          <t>нет данных</t>
+        </is>
+      </c>
+    </row>
+    <row r="92">
+      <c r="E92" t="inlineStr">
+        <is>
+          <t>24.00R35</t>
+        </is>
+      </c>
+      <c r="F92" t="inlineStr">
+        <is>
+          <t>Бел-122</t>
+        </is>
+      </c>
+      <c r="G92" t="inlineStr">
+        <is>
+          <t>Type, сер, груз, C</t>
+        </is>
+      </c>
+      <c r="H92" t="n">
+        <v>2</v>
+      </c>
+      <c r="I92" s="1" t="n">
+        <v>44991</v>
+      </c>
+      <c r="J92" t="inlineStr">
+        <is>
+          <t>нет данных</t>
+        </is>
+      </c>
+    </row>
+    <row r="93">
+      <c r="E93" t="inlineStr">
+        <is>
+          <t>24.00R35</t>
+        </is>
+      </c>
+      <c r="F93" t="inlineStr">
+        <is>
+          <t>Бел-202</t>
+        </is>
+      </c>
+      <c r="G93" t="inlineStr">
+        <is>
+          <t>210B, Type, сер, LS-2</t>
+        </is>
+      </c>
+      <c r="H93" t="n">
+        <v>2</v>
+      </c>
+      <c r="I93" s="1" t="n">
+        <v>44991</v>
+      </c>
+      <c r="J93" t="inlineStr">
+        <is>
+          <t>нет данных</t>
+        </is>
+      </c>
+    </row>
+    <row r="94">
+      <c r="E94" t="inlineStr">
+        <is>
+          <t>24.00R35</t>
+        </is>
+      </c>
+      <c r="F94" t="inlineStr">
+        <is>
+          <t>Бел-202</t>
+        </is>
+      </c>
+      <c r="G94" t="inlineStr">
+        <is>
+          <t>210B, Type, сер, H</t>
+        </is>
+      </c>
+      <c r="H94" t="n">
+        <v>2</v>
+      </c>
+      <c r="I94" s="1" t="n">
+        <v>44991</v>
+      </c>
+      <c r="J94" t="inlineStr">
+        <is>
+          <t>нет данных</t>
+        </is>
+      </c>
+    </row>
+    <row r="95">
+      <c r="E95" t="inlineStr">
+        <is>
+          <t>24.00R35</t>
+        </is>
+      </c>
+      <c r="F95" t="inlineStr">
+        <is>
+          <t>Бел-202</t>
+        </is>
+      </c>
+      <c r="G95" t="inlineStr">
+        <is>
+          <t>210B, Type, сер, C</t>
+        </is>
+      </c>
+      <c r="H95" t="n">
+        <v>2</v>
+      </c>
+      <c r="I95" s="1" t="n">
+        <v>44991</v>
+      </c>
+      <c r="J95" t="inlineStr">
+        <is>
+          <t>нет данных</t>
+        </is>
+      </c>
+    </row>
+    <row r="96">
+      <c r="E96" t="inlineStr">
+        <is>
+          <t>24.00R35</t>
+        </is>
+      </c>
+      <c r="F96" t="inlineStr">
+        <is>
+          <t>Бел-212</t>
+        </is>
+      </c>
+      <c r="G96" t="inlineStr">
+        <is>
+          <t>Type, сер, груз, LS-2</t>
+        </is>
+      </c>
+      <c r="H96" t="n">
+        <v>2</v>
+      </c>
+      <c r="I96" s="1" t="n">
+        <v>44991</v>
+      </c>
+      <c r="J96" t="inlineStr">
+        <is>
+          <t>нет данных</t>
+        </is>
+      </c>
+    </row>
+    <row r="97">
+      <c r="E97" t="inlineStr">
+        <is>
+          <t>24.00R35</t>
+        </is>
+      </c>
+      <c r="F97" t="inlineStr">
+        <is>
+          <t>Бел-212</t>
+        </is>
+      </c>
+      <c r="G97" t="inlineStr">
+        <is>
+          <t>Type, сер, груз, H</t>
+        </is>
+      </c>
+      <c r="H97" t="n">
+        <v>2</v>
+      </c>
+      <c r="I97" s="1" t="n">
+        <v>44991</v>
+      </c>
+      <c r="J97" t="inlineStr">
+        <is>
+          <t>нет данных</t>
+        </is>
+      </c>
+    </row>
+    <row r="98">
+      <c r="E98" t="inlineStr">
+        <is>
+          <t>24.00R35</t>
+        </is>
+      </c>
+      <c r="F98" t="inlineStr">
+        <is>
+          <t>Бел-212</t>
+        </is>
+      </c>
+      <c r="G98" t="inlineStr">
+        <is>
+          <t>Type, сер, груз, C</t>
+        </is>
+      </c>
+      <c r="H98" t="n">
+        <v>2</v>
+      </c>
+      <c r="I98" s="1" t="n">
+        <v>44991</v>
+      </c>
+      <c r="J98" t="inlineStr">
+        <is>
+          <t>нет данных</t>
+        </is>
+      </c>
+    </row>
+    <row r="99">
+      <c r="E99" t="inlineStr">
+        <is>
+          <t>21.00R35</t>
+        </is>
+      </c>
+      <c r="F99" t="inlineStr">
+        <is>
+          <t>Бел-200</t>
+        </is>
+      </c>
+      <c r="G99" t="inlineStr">
+        <is>
+          <t>202B, Type, сер, LS-2</t>
+        </is>
+      </c>
+      <c r="H99" t="n">
+        <v>2</v>
+      </c>
+      <c r="I99" s="1" t="n">
+        <v>44991</v>
+      </c>
+      <c r="J99" t="inlineStr">
+        <is>
+          <t>нет данных</t>
+        </is>
+      </c>
+    </row>
+    <row r="100">
+      <c r="E100" t="inlineStr">
+        <is>
+          <t>21.00R35</t>
+        </is>
+      </c>
+      <c r="F100" t="inlineStr">
+        <is>
+          <t>Бел-200</t>
+        </is>
+      </c>
+      <c r="G100" t="inlineStr">
+        <is>
+          <t>202B, Type, сер, H</t>
+        </is>
+      </c>
+      <c r="H100" t="n">
+        <v>2</v>
+      </c>
+      <c r="I100" s="1" t="n">
+        <v>44991</v>
+      </c>
+      <c r="J100" t="inlineStr">
+        <is>
+          <t>нет данных</t>
+        </is>
+      </c>
+    </row>
+    <row r="101">
+      <c r="E101" t="inlineStr">
+        <is>
+          <t>21.00R35</t>
+        </is>
+      </c>
+      <c r="F101" t="inlineStr">
+        <is>
+          <t>Бел-200</t>
+        </is>
+      </c>
+      <c r="G101" t="inlineStr">
+        <is>
+          <t>202B, Type, сер, C</t>
+        </is>
+      </c>
+      <c r="H101" t="n">
+        <v>2</v>
+      </c>
+      <c r="I101" s="1" t="n">
+        <v>44991</v>
+      </c>
+      <c r="J101" t="inlineStr">
+        <is>
+          <t>нет данных</t>
+        </is>
+      </c>
+    </row>
+    <row r="102">
+      <c r="E102" t="inlineStr">
+        <is>
+          <t>21.00R35</t>
+        </is>
+      </c>
+      <c r="F102" t="inlineStr">
+        <is>
+          <t>Бел-210</t>
+        </is>
+      </c>
+      <c r="G102" t="inlineStr">
+        <is>
+          <t>202B, Type, сер, LS-2</t>
+        </is>
+      </c>
+      <c r="H102" t="n">
+        <v>2</v>
+      </c>
+      <c r="I102" s="1" t="n">
+        <v>44991</v>
+      </c>
+      <c r="J102" t="inlineStr">
+        <is>
+          <t>нет данных</t>
+        </is>
+      </c>
+    </row>
+    <row r="103">
+      <c r="E103" t="inlineStr">
+        <is>
+          <t>21.00R35</t>
+        </is>
+      </c>
+      <c r="F103" t="inlineStr">
+        <is>
+          <t>Бел-210</t>
+        </is>
+      </c>
+      <c r="G103" t="inlineStr">
+        <is>
+          <t>202B, Type, сер, H</t>
+        </is>
+      </c>
+      <c r="H103" t="n">
+        <v>2</v>
+      </c>
+      <c r="I103" s="1" t="n">
+        <v>44991</v>
+      </c>
+      <c r="J103" t="inlineStr">
+        <is>
+          <t>нет данных</t>
+        </is>
+      </c>
+    </row>
+    <row r="104">
+      <c r="E104" t="inlineStr">
+        <is>
+          <t>21.00R35</t>
+        </is>
+      </c>
+      <c r="F104" t="inlineStr">
+        <is>
+          <t>Бел-210</t>
+        </is>
+      </c>
+      <c r="G104" t="inlineStr">
+        <is>
+          <t>202B, Type, сер, C</t>
+        </is>
+      </c>
+      <c r="H104" t="n">
+        <v>2</v>
+      </c>
+      <c r="I104" s="1" t="n">
+        <v>44991</v>
+      </c>
+      <c r="J104" t="inlineStr">
+        <is>
+          <t>нет данных</t>
+        </is>
+      </c>
+    </row>
+    <row r="105">
+      <c r="E105" t="inlineStr">
+        <is>
+          <t>14.00R20</t>
+        </is>
+      </c>
+      <c r="F105" t="inlineStr">
+        <is>
+          <t>BEL-248</t>
+        </is>
+      </c>
+      <c r="G105" t="inlineStr">
+        <is>
+          <t>сер, груз</t>
+        </is>
+      </c>
+      <c r="H105" t="n">
+        <v>2</v>
+      </c>
+      <c r="I105" s="1" t="n">
+        <v>44991</v>
+      </c>
+      <c r="J105" t="inlineStr">
+        <is>
+          <t>нет данных</t>
+        </is>
+      </c>
+    </row>
+    <row r="106">
+      <c r="E106" t="inlineStr">
+        <is>
+          <t>14.00R20</t>
+        </is>
+      </c>
+      <c r="F106" t="inlineStr">
+        <is>
+          <t>BEL-248</t>
+        </is>
+      </c>
+      <c r="G106" t="inlineStr">
+        <is>
+          <t>сер, груз</t>
+        </is>
+      </c>
+      <c r="H106" t="n">
+        <v>2</v>
+      </c>
+      <c r="I106" s="1" t="n">
+        <v>44991</v>
+      </c>
+      <c r="J106" t="inlineStr">
+        <is>
+          <t>нет данных</t>
+        </is>
+      </c>
+    </row>
+    <row r="107">
+      <c r="E107" t="inlineStr">
+        <is>
+          <t>14.00R20</t>
+        </is>
+      </c>
+      <c r="F107" t="inlineStr">
+        <is>
+          <t>BEL-248</t>
+        </is>
+      </c>
+      <c r="G107" t="inlineStr">
+        <is>
+          <t>б/к, сер, груз</t>
+        </is>
+      </c>
+      <c r="H107" t="n">
+        <v>2</v>
+      </c>
+      <c r="I107" s="1" t="n">
+        <v>44991</v>
+      </c>
+      <c r="J107" t="inlineStr">
+        <is>
+          <t>нет данных</t>
+        </is>
+      </c>
+    </row>
+    <row r="108">
+      <c r="E108" t="inlineStr">
+        <is>
+          <t>14.00R20</t>
+        </is>
+      </c>
+      <c r="F108" t="inlineStr">
+        <is>
+          <t>BEL-248</t>
+        </is>
+      </c>
+      <c r="G108" t="inlineStr">
+        <is>
+          <t>сер, груз</t>
+        </is>
+      </c>
+      <c r="H108" t="n">
+        <v>2</v>
+      </c>
+      <c r="I108" s="1" t="n">
+        <v>44991</v>
+      </c>
+      <c r="J108" t="inlineStr">
+        <is>
+          <t>нет данных</t>
+        </is>
+      </c>
+    </row>
+    <row r="109">
+      <c r="E109" t="inlineStr">
+        <is>
+          <t>175/70R13</t>
+        </is>
+      </c>
+      <c r="F109" t="inlineStr">
+        <is>
+          <t>Бел-103</t>
+        </is>
+      </c>
+      <c r="G109" t="inlineStr">
+        <is>
+          <t>б/к, сер, легк</t>
+        </is>
+      </c>
+      <c r="H109" t="n">
+        <v>2</v>
+      </c>
+      <c r="I109" s="1" t="n">
+        <v>44991</v>
+      </c>
+      <c r="J109" t="inlineStr">
+        <is>
+          <t>нет данных</t>
+        </is>
+      </c>
+    </row>
+    <row r="110">
+      <c r="E110" t="inlineStr">
+        <is>
+          <t>195/65R15</t>
+        </is>
+      </c>
+      <c r="F110" t="inlineStr">
+        <is>
+          <t>Бел-119</t>
+        </is>
+      </c>
+      <c r="G110" t="inlineStr">
+        <is>
+          <t>сер, легк</t>
+        </is>
+      </c>
+      <c r="H110" t="n">
+        <v>2</v>
+      </c>
+      <c r="I110" s="1" t="n">
+        <v>44991</v>
+      </c>
+      <c r="J110" t="inlineStr">
+        <is>
+          <t>нет данных</t>
+        </is>
+      </c>
+    </row>
+    <row r="111">
+      <c r="E111" t="inlineStr">
+        <is>
+          <t>210/80R16</t>
+        </is>
+      </c>
+      <c r="F111" t="inlineStr">
+        <is>
+          <t>Бел-777</t>
+        </is>
+      </c>
+      <c r="G111" t="inlineStr">
+        <is>
+          <t>сер, легк</t>
+        </is>
+      </c>
+      <c r="H111" t="n">
+        <v>2</v>
+      </c>
+      <c r="I111" s="1" t="n">
+        <v>44991</v>
+      </c>
+      <c r="J111" t="inlineStr">
+        <is>
+          <t>нет данных</t>
+        </is>
+      </c>
+    </row>
+    <row r="112">
+      <c r="E112" t="inlineStr">
+        <is>
+          <t>215/65R16C</t>
+        </is>
+      </c>
+      <c r="F112" t="inlineStr">
+        <is>
+          <t>Бел-1000</t>
+        </is>
+      </c>
+      <c r="G112" t="inlineStr">
+        <is>
+          <t>сер, легк</t>
+        </is>
+      </c>
+      <c r="H112" t="n">
+        <v>2</v>
+      </c>
+      <c r="I112" s="1" t="n">
+        <v>44991</v>
+      </c>
+      <c r="J112" t="inlineStr">
+        <is>
+          <t>нет данных</t>
+        </is>
+      </c>
+    </row>
+    <row r="113">
+      <c r="E113" t="inlineStr">
+        <is>
+          <t>175/65R15</t>
+        </is>
+      </c>
+      <c r="F113" t="inlineStr">
+        <is>
+          <t>Бел-1001</t>
+        </is>
+      </c>
+      <c r="G113" t="inlineStr">
+        <is>
+          <t>сер, легк</t>
+        </is>
+      </c>
+      <c r="H113" t="n">
+        <v>2</v>
+      </c>
+      <c r="I113" s="1" t="n">
+        <v>44991</v>
+      </c>
+      <c r="J113" t="inlineStr">
+        <is>
+          <t>нет данных</t>
+        </is>
+      </c>
+    </row>
+    <row r="114">
+      <c r="E114" t="inlineStr">
+        <is>
+          <t>35/65-33</t>
+        </is>
+      </c>
+      <c r="F114" t="inlineStr">
+        <is>
+          <t>ФБел-283</t>
+        </is>
+      </c>
+      <c r="G114" t="inlineStr">
+        <is>
+          <t>42, сер, груз</t>
+        </is>
+      </c>
+      <c r="H114" t="n">
+        <v>2</v>
+      </c>
+      <c r="I114" s="1" t="n">
+        <v>44992</v>
+      </c>
+      <c r="J114" t="inlineStr">
+        <is>
+          <t>нет данных</t>
+        </is>
+      </c>
+    </row>
+    <row r="115">
+      <c r="E115" t="inlineStr">
+        <is>
+          <t>205/55R16</t>
+        </is>
+      </c>
+      <c r="F115" t="inlineStr">
+        <is>
+          <t>BEL-262</t>
+        </is>
+      </c>
+      <c r="G115" t="inlineStr">
+        <is>
+          <t>б/к, сер, легк</t>
+        </is>
+      </c>
+      <c r="H115" t="n">
+        <v>2</v>
+      </c>
+      <c r="I115" s="1" t="n">
+        <v>44992</v>
+      </c>
+      <c r="J115" t="inlineStr">
+        <is>
+          <t>нет данных</t>
+        </is>
+      </c>
+    </row>
+    <row r="116">
+      <c r="E116" t="inlineStr">
+        <is>
+          <t>205/55R16</t>
+        </is>
+      </c>
+      <c r="F116" t="inlineStr">
+        <is>
+          <t>BEL-317</t>
+        </is>
+      </c>
+      <c r="G116" t="inlineStr">
+        <is>
+          <t>б/к, сер, легк</t>
+        </is>
+      </c>
+      <c r="H116" t="n">
+        <v>2</v>
+      </c>
+      <c r="I116" s="1" t="n">
+        <v>44992</v>
+      </c>
+      <c r="J116" t="inlineStr">
+        <is>
+          <t>нет данных</t>
+        </is>
+      </c>
+    </row>
+    <row r="117">
+      <c r="E117" t="inlineStr">
+        <is>
+          <t>205/55R16</t>
+        </is>
+      </c>
+      <c r="F117" t="inlineStr">
+        <is>
+          <t>BEL-317S</t>
+        </is>
+      </c>
+      <c r="G117" t="inlineStr">
+        <is>
+          <t>сер, ошип</t>
+        </is>
+      </c>
+      <c r="H117" t="n">
+        <v>2</v>
+      </c>
+      <c r="I117" s="1" t="n">
+        <v>44992</v>
+      </c>
+      <c r="J117" t="inlineStr">
+        <is>
+          <t>нет данных</t>
+        </is>
+      </c>
+    </row>
+    <row r="118">
+      <c r="E118" t="inlineStr">
+        <is>
+          <t>24.00R35</t>
+        </is>
+      </c>
+      <c r="F118" t="inlineStr">
+        <is>
+          <t>Бел-122</t>
+        </is>
+      </c>
+      <c r="G118" t="inlineStr">
+        <is>
+          <t>Type, сер, груз, LS-2</t>
+        </is>
+      </c>
+      <c r="H118" t="n">
+        <v>2</v>
+      </c>
+      <c r="I118" s="1" t="n">
+        <v>44992</v>
+      </c>
+      <c r="J118" t="inlineStr">
+        <is>
+          <t>нет данных</t>
+        </is>
+      </c>
+    </row>
+    <row r="119">
+      <c r="E119" t="inlineStr">
+        <is>
+          <t>24.00R35</t>
+        </is>
+      </c>
+      <c r="F119" t="inlineStr">
+        <is>
+          <t>Бел-122</t>
+        </is>
+      </c>
+      <c r="G119" t="inlineStr">
+        <is>
+          <t>Type, сер, груз, H</t>
+        </is>
+      </c>
+      <c r="H119" t="n">
+        <v>2</v>
+      </c>
+      <c r="I119" s="1" t="n">
+        <v>44992</v>
+      </c>
+      <c r="J119" t="inlineStr">
+        <is>
+          <t>нет данных</t>
+        </is>
+      </c>
+    </row>
+    <row r="120">
+      <c r="E120" t="inlineStr">
+        <is>
+          <t>24.00R35</t>
+        </is>
+      </c>
+      <c r="F120" t="inlineStr">
+        <is>
+          <t>Бел-122</t>
+        </is>
+      </c>
+      <c r="G120" t="inlineStr">
+        <is>
+          <t>Type, сер, груз, C</t>
+        </is>
+      </c>
+      <c r="H120" t="n">
+        <v>2</v>
+      </c>
+      <c r="I120" s="1" t="n">
+        <v>44992</v>
+      </c>
+      <c r="J120" t="inlineStr">
+        <is>
+          <t>нет данных</t>
+        </is>
+      </c>
+    </row>
+    <row r="121">
+      <c r="E121" t="inlineStr">
+        <is>
+          <t>24.00R35</t>
+        </is>
+      </c>
+      <c r="F121" t="inlineStr">
+        <is>
+          <t>Бел-202</t>
+        </is>
+      </c>
+      <c r="G121" t="inlineStr">
+        <is>
+          <t>210B, Type, сер, LS-2</t>
+        </is>
+      </c>
+      <c r="H121" t="n">
+        <v>2</v>
+      </c>
+      <c r="I121" s="1" t="n">
+        <v>44992</v>
+      </c>
+      <c r="J121" t="inlineStr">
+        <is>
+          <t>нет данных</t>
+        </is>
+      </c>
+    </row>
+    <row r="122">
+      <c r="E122" t="inlineStr">
+        <is>
+          <t>24.00R35</t>
+        </is>
+      </c>
+      <c r="F122" t="inlineStr">
+        <is>
+          <t>Бел-202</t>
+        </is>
+      </c>
+      <c r="G122" t="inlineStr">
+        <is>
+          <t>210B, Type, сер, H</t>
+        </is>
+      </c>
+      <c r="H122" t="n">
+        <v>2</v>
+      </c>
+      <c r="I122" s="1" t="n">
+        <v>44992</v>
+      </c>
+      <c r="J122" t="inlineStr">
+        <is>
+          <t>нет данных</t>
+        </is>
+      </c>
+    </row>
+    <row r="123">
+      <c r="E123" t="inlineStr">
+        <is>
+          <t>24.00R35</t>
+        </is>
+      </c>
+      <c r="F123" t="inlineStr">
+        <is>
+          <t>Бел-202</t>
+        </is>
+      </c>
+      <c r="G123" t="inlineStr">
+        <is>
+          <t>210B, Type, сер, C</t>
+        </is>
+      </c>
+      <c r="H123" t="n">
+        <v>2</v>
+      </c>
+      <c r="I123" s="1" t="n">
+        <v>44992</v>
+      </c>
+      <c r="J123" t="inlineStr">
+        <is>
+          <t>нет данных</t>
+        </is>
+      </c>
+    </row>
+    <row r="124">
+      <c r="E124" t="inlineStr">
+        <is>
+          <t>24.00R35</t>
+        </is>
+      </c>
+      <c r="F124" t="inlineStr">
+        <is>
+          <t>Бел-212</t>
+        </is>
+      </c>
+      <c r="G124" t="inlineStr">
+        <is>
+          <t>Type, сер, груз, LS-2</t>
+        </is>
+      </c>
+      <c r="H124" t="n">
+        <v>2</v>
+      </c>
+      <c r="I124" s="1" t="n">
+        <v>44992</v>
+      </c>
+      <c r="J124" t="inlineStr">
+        <is>
+          <t>нет данных</t>
+        </is>
+      </c>
+    </row>
+    <row r="125">
+      <c r="E125" t="inlineStr">
+        <is>
+          <t>24.00R35</t>
+        </is>
+      </c>
+      <c r="F125" t="inlineStr">
+        <is>
+          <t>Бел-212</t>
+        </is>
+      </c>
+      <c r="G125" t="inlineStr">
+        <is>
+          <t>Type, сер, груз, H</t>
+        </is>
+      </c>
+      <c r="H125" t="n">
+        <v>2</v>
+      </c>
+      <c r="I125" s="1" t="n">
+        <v>44992</v>
+      </c>
+      <c r="J125" t="inlineStr">
+        <is>
+          <t>нет данных</t>
+        </is>
+      </c>
+    </row>
+    <row r="126">
+      <c r="E126" t="inlineStr">
+        <is>
+          <t>24.00R35</t>
+        </is>
+      </c>
+      <c r="F126" t="inlineStr">
+        <is>
+          <t>Бел-212</t>
+        </is>
+      </c>
+      <c r="G126" t="inlineStr">
+        <is>
+          <t>Type, сер, груз, C</t>
+        </is>
+      </c>
+      <c r="H126" t="n">
+        <v>2</v>
+      </c>
+      <c r="I126" s="1" t="n">
+        <v>44992</v>
+      </c>
+      <c r="J126" t="inlineStr">
+        <is>
+          <t>нет данных</t>
+        </is>
+      </c>
+    </row>
+    <row r="127">
+      <c r="E127" t="inlineStr">
+        <is>
+          <t>21.00R35</t>
+        </is>
+      </c>
+      <c r="F127" t="inlineStr">
+        <is>
+          <t>Бел-200</t>
+        </is>
+      </c>
+      <c r="G127" t="inlineStr">
+        <is>
+          <t>202B, Type, сер, LS-2</t>
+        </is>
+      </c>
+      <c r="H127" t="n">
+        <v>2</v>
+      </c>
+      <c r="I127" s="1" t="n">
+        <v>44992</v>
+      </c>
+      <c r="J127" t="inlineStr">
+        <is>
+          <t>нет данных</t>
+        </is>
+      </c>
+    </row>
+    <row r="128">
+      <c r="E128" t="inlineStr">
+        <is>
+          <t>21.00R35</t>
+        </is>
+      </c>
+      <c r="F128" t="inlineStr">
+        <is>
+          <t>Бел-200</t>
+        </is>
+      </c>
+      <c r="G128" t="inlineStr">
+        <is>
+          <t>202B, Type, сер, H</t>
+        </is>
+      </c>
+      <c r="H128" t="n">
+        <v>2</v>
+      </c>
+      <c r="I128" s="1" t="n">
+        <v>44992</v>
+      </c>
+      <c r="J128" t="inlineStr">
+        <is>
+          <t>нет данных</t>
+        </is>
+      </c>
+    </row>
+    <row r="129">
+      <c r="E129" t="inlineStr">
+        <is>
+          <t>21.00R35</t>
+        </is>
+      </c>
+      <c r="F129" t="inlineStr">
+        <is>
+          <t>Бел-200</t>
+        </is>
+      </c>
+      <c r="G129" t="inlineStr">
+        <is>
+          <t>202B, Type, сер, C</t>
+        </is>
+      </c>
+      <c r="H129" t="n">
+        <v>2</v>
+      </c>
+      <c r="I129" s="1" t="n">
+        <v>44992</v>
+      </c>
+      <c r="J129" t="inlineStr">
+        <is>
+          <t>нет данных</t>
+        </is>
+      </c>
+    </row>
+    <row r="130">
+      <c r="E130" t="inlineStr">
+        <is>
+          <t>21.00R35</t>
+        </is>
+      </c>
+      <c r="F130" t="inlineStr">
+        <is>
+          <t>Бел-210</t>
+        </is>
+      </c>
+      <c r="G130" t="inlineStr">
+        <is>
+          <t>202B, Type, сер, LS-2</t>
+        </is>
+      </c>
+      <c r="H130" t="n">
+        <v>2</v>
+      </c>
+      <c r="I130" s="1" t="n">
+        <v>44992</v>
+      </c>
+      <c r="J130" t="inlineStr">
+        <is>
+          <t>нет данных</t>
+        </is>
+      </c>
+    </row>
+    <row r="131">
+      <c r="E131" t="inlineStr">
+        <is>
+          <t>21.00R35</t>
+        </is>
+      </c>
+      <c r="F131" t="inlineStr">
+        <is>
+          <t>Бел-210</t>
+        </is>
+      </c>
+      <c r="G131" t="inlineStr">
+        <is>
+          <t>202B, Type, сер, H</t>
+        </is>
+      </c>
+      <c r="H131" t="n">
+        <v>2</v>
+      </c>
+      <c r="I131" s="1" t="n">
+        <v>44992</v>
+      </c>
+      <c r="J131" t="inlineStr">
+        <is>
+          <t>нет данных</t>
+        </is>
+      </c>
+    </row>
+    <row r="132">
+      <c r="E132" t="inlineStr">
+        <is>
+          <t>21.00R35</t>
+        </is>
+      </c>
+      <c r="F132" t="inlineStr">
+        <is>
+          <t>Бел-210</t>
+        </is>
+      </c>
+      <c r="G132" t="inlineStr">
+        <is>
+          <t>202B, Type, сер, C</t>
+        </is>
+      </c>
+      <c r="H132" t="n">
+        <v>2</v>
+      </c>
+      <c r="I132" s="1" t="n">
+        <v>44992</v>
+      </c>
+      <c r="J132" t="inlineStr">
+        <is>
+          <t>нет данных</t>
+        </is>
+      </c>
+    </row>
+    <row r="133">
+      <c r="E133" t="inlineStr">
+        <is>
+          <t>14.00R20</t>
+        </is>
+      </c>
+      <c r="F133" t="inlineStr">
+        <is>
+          <t>BEL-248</t>
+        </is>
+      </c>
+      <c r="G133" t="inlineStr">
+        <is>
+          <t>сер, груз</t>
+        </is>
+      </c>
+      <c r="H133" t="n">
+        <v>2</v>
+      </c>
+      <c r="I133" s="1" t="n">
+        <v>44992</v>
+      </c>
+      <c r="J133" t="inlineStr">
+        <is>
+          <t>нет данных</t>
+        </is>
+      </c>
+    </row>
+    <row r="134">
+      <c r="E134" t="inlineStr">
+        <is>
+          <t>14.00R20</t>
+        </is>
+      </c>
+      <c r="F134" t="inlineStr">
+        <is>
+          <t>BEL-248</t>
+        </is>
+      </c>
+      <c r="G134" t="inlineStr">
+        <is>
+          <t>сер, груз</t>
+        </is>
+      </c>
+      <c r="H134" t="n">
+        <v>2</v>
+      </c>
+      <c r="I134" s="1" t="n">
+        <v>44992</v>
+      </c>
+      <c r="J134" t="inlineStr">
+        <is>
+          <t>нет данных</t>
+        </is>
+      </c>
+    </row>
+    <row r="135">
+      <c r="E135" t="inlineStr">
+        <is>
+          <t>14.00R20</t>
+        </is>
+      </c>
+      <c r="F135" t="inlineStr">
+        <is>
+          <t>BEL-248</t>
+        </is>
+      </c>
+      <c r="G135" t="inlineStr">
+        <is>
+          <t>б/к, сер, груз</t>
+        </is>
+      </c>
+      <c r="H135" t="n">
+        <v>2</v>
+      </c>
+      <c r="I135" s="1" t="n">
+        <v>44992</v>
+      </c>
+      <c r="J135" t="inlineStr">
+        <is>
+          <t>нет данных</t>
+        </is>
+      </c>
+    </row>
+    <row r="136">
+      <c r="E136" t="inlineStr">
+        <is>
+          <t>14.00R20</t>
+        </is>
+      </c>
+      <c r="F136" t="inlineStr">
+        <is>
+          <t>BEL-248</t>
+        </is>
+      </c>
+      <c r="G136" t="inlineStr">
+        <is>
+          <t>сер, груз</t>
+        </is>
+      </c>
+      <c r="H136" t="n">
+        <v>2</v>
+      </c>
+      <c r="I136" s="1" t="n">
+        <v>44992</v>
+      </c>
+      <c r="J136" t="inlineStr">
+        <is>
+          <t>нет данных</t>
+        </is>
+      </c>
+    </row>
+    <row r="137">
+      <c r="E137" t="inlineStr">
+        <is>
+          <t>175/70R13</t>
+        </is>
+      </c>
+      <c r="F137" t="inlineStr">
+        <is>
+          <t>Бел-103</t>
+        </is>
+      </c>
+      <c r="G137" t="inlineStr">
+        <is>
+          <t>б/к, сер, легк</t>
+        </is>
+      </c>
+      <c r="H137" t="n">
+        <v>2</v>
+      </c>
+      <c r="I137" s="1" t="n">
+        <v>44992</v>
+      </c>
+      <c r="J137" t="inlineStr">
+        <is>
+          <t>нет данных</t>
+        </is>
+      </c>
+    </row>
+    <row r="138">
+      <c r="E138" t="inlineStr">
+        <is>
+          <t>195/65R15</t>
+        </is>
+      </c>
+      <c r="F138" t="inlineStr">
+        <is>
+          <t>Бел-119</t>
+        </is>
+      </c>
+      <c r="G138" t="inlineStr">
+        <is>
+          <t>сер, легк</t>
+        </is>
+      </c>
+      <c r="H138" t="n">
+        <v>2</v>
+      </c>
+      <c r="I138" s="1" t="n">
+        <v>44992</v>
+      </c>
+      <c r="J138" t="inlineStr">
+        <is>
+          <t>нет данных</t>
+        </is>
+      </c>
+    </row>
+    <row r="139">
+      <c r="E139" t="inlineStr">
+        <is>
+          <t>210/80R16</t>
+        </is>
+      </c>
+      <c r="F139" t="inlineStr">
+        <is>
+          <t>Бел-777</t>
+        </is>
+      </c>
+      <c r="G139" t="inlineStr">
+        <is>
+          <t>сер, легк</t>
+        </is>
+      </c>
+      <c r="H139" t="n">
+        <v>2</v>
+      </c>
+      <c r="I139" s="1" t="n">
+        <v>44992</v>
+      </c>
+      <c r="J139" t="inlineStr">
+        <is>
+          <t>нет данных</t>
+        </is>
+      </c>
+    </row>
+    <row r="140">
+      <c r="E140" t="inlineStr">
+        <is>
+          <t>215/65R16C</t>
+        </is>
+      </c>
+      <c r="F140" t="inlineStr">
+        <is>
+          <t>Бел-1000</t>
+        </is>
+      </c>
+      <c r="G140" t="inlineStr">
+        <is>
+          <t>сер, легк</t>
+        </is>
+      </c>
+      <c r="H140" t="n">
+        <v>2</v>
+      </c>
+      <c r="I140" s="1" t="n">
+        <v>44992</v>
+      </c>
+      <c r="J140" t="inlineStr">
+        <is>
+          <t>нет данных</t>
+        </is>
+      </c>
+    </row>
+    <row r="141">
+      <c r="E141" t="inlineStr">
+        <is>
+          <t>175/65R15</t>
+        </is>
+      </c>
+      <c r="F141" t="inlineStr">
+        <is>
+          <t>Бел-1001</t>
+        </is>
+      </c>
+      <c r="G141" t="inlineStr">
+        <is>
+          <t>сер, легк</t>
+        </is>
+      </c>
+      <c r="H141" t="n">
+        <v>2</v>
+      </c>
+      <c r="I141" s="1" t="n">
+        <v>44992</v>
+      </c>
+      <c r="J141" t="inlineStr">
+        <is>
+          <t>нет данных</t>
+        </is>
+      </c>
+    </row>
+    <row r="142">
+      <c r="E142" t="inlineStr">
+        <is>
+          <t>35/65-33</t>
+        </is>
+      </c>
+      <c r="F142" t="inlineStr">
+        <is>
+          <t>ФБел-283</t>
+        </is>
+      </c>
+      <c r="G142" t="inlineStr">
+        <is>
+          <t>42, сер, груз</t>
+        </is>
+      </c>
+      <c r="H142" t="n">
+        <v>2</v>
+      </c>
+      <c r="I142" s="1" t="n">
+        <v>44997</v>
+      </c>
+      <c r="J142" t="inlineStr">
+        <is>
+          <t>нет данных</t>
+        </is>
+      </c>
+    </row>
+    <row r="143">
+      <c r="E143" t="inlineStr">
+        <is>
+          <t>205/55R16</t>
+        </is>
+      </c>
+      <c r="F143" t="inlineStr">
+        <is>
+          <t>BEL-262</t>
+        </is>
+      </c>
+      <c r="G143" t="inlineStr">
+        <is>
+          <t>б/к, сер, легк</t>
+        </is>
+      </c>
+      <c r="H143" t="n">
+        <v>2</v>
+      </c>
+      <c r="I143" s="1" t="n">
+        <v>44997</v>
+      </c>
+      <c r="J143" t="inlineStr">
+        <is>
+          <t>нет данных</t>
+        </is>
+      </c>
+    </row>
+    <row r="144">
+      <c r="E144" t="inlineStr">
+        <is>
+          <t>205/55R16</t>
+        </is>
+      </c>
+      <c r="F144" t="inlineStr">
+        <is>
+          <t>BEL-317</t>
+        </is>
+      </c>
+      <c r="G144" t="inlineStr">
+        <is>
+          <t>б/к, сер, легк</t>
+        </is>
+      </c>
+      <c r="H144" t="n">
+        <v>2</v>
+      </c>
+      <c r="I144" s="1" t="n">
+        <v>44997</v>
+      </c>
+      <c r="J144" t="inlineStr">
+        <is>
+          <t>нет данных</t>
+        </is>
+      </c>
+    </row>
+    <row r="145">
+      <c r="E145" t="inlineStr">
+        <is>
+          <t>205/55R16</t>
+        </is>
+      </c>
+      <c r="F145" t="inlineStr">
+        <is>
+          <t>BEL-317S</t>
+        </is>
+      </c>
+      <c r="G145" t="inlineStr">
+        <is>
+          <t>сер, ошип</t>
+        </is>
+      </c>
+      <c r="H145" t="n">
+        <v>2</v>
+      </c>
+      <c r="I145" s="1" t="n">
+        <v>44997</v>
+      </c>
+      <c r="J145" t="inlineStr">
+        <is>
+          <t>нет данных</t>
+        </is>
+      </c>
+    </row>
+    <row r="146">
+      <c r="E146" t="inlineStr">
+        <is>
+          <t>24.00R35</t>
+        </is>
+      </c>
+      <c r="F146" t="inlineStr">
+        <is>
+          <t>Бел-122</t>
+        </is>
+      </c>
+      <c r="G146" t="inlineStr">
+        <is>
+          <t>Type, сер, груз, LS-2</t>
+        </is>
+      </c>
+      <c r="H146" t="n">
+        <v>2</v>
+      </c>
+      <c r="I146" s="1" t="n">
+        <v>44997</v>
+      </c>
+      <c r="J146" t="inlineStr">
+        <is>
+          <t>нет данных</t>
+        </is>
+      </c>
+    </row>
+    <row r="147">
+      <c r="E147" t="inlineStr">
+        <is>
+          <t>24.00R35</t>
+        </is>
+      </c>
+      <c r="F147" t="inlineStr">
+        <is>
+          <t>Бел-122</t>
+        </is>
+      </c>
+      <c r="G147" t="inlineStr">
+        <is>
+          <t>Type, сер, груз, H</t>
+        </is>
+      </c>
+      <c r="H147" t="n">
+        <v>2</v>
+      </c>
+      <c r="I147" s="1" t="n">
+        <v>44997</v>
+      </c>
+      <c r="J147" t="inlineStr">
+        <is>
+          <t>нет данных</t>
+        </is>
+      </c>
+    </row>
+    <row r="148">
+      <c r="E148" t="inlineStr">
+        <is>
+          <t>24.00R35</t>
+        </is>
+      </c>
+      <c r="F148" t="inlineStr">
+        <is>
+          <t>Бел-122</t>
+        </is>
+      </c>
+      <c r="G148" t="inlineStr">
+        <is>
+          <t>Type, сер, груз, C</t>
+        </is>
+      </c>
+      <c r="H148" t="n">
+        <v>2</v>
+      </c>
+      <c r="I148" s="1" t="n">
+        <v>44997</v>
+      </c>
+      <c r="J148" t="inlineStr">
+        <is>
+          <t>нет данных</t>
+        </is>
+      </c>
+    </row>
+    <row r="149">
+      <c r="E149" t="inlineStr">
+        <is>
+          <t>24.00R35</t>
+        </is>
+      </c>
+      <c r="F149" t="inlineStr">
+        <is>
+          <t>Бел-202</t>
+        </is>
+      </c>
+      <c r="G149" t="inlineStr">
+        <is>
+          <t>210B, Type, сер, LS-2</t>
+        </is>
+      </c>
+      <c r="H149" t="n">
+        <v>2</v>
+      </c>
+      <c r="I149" s="1" t="n">
+        <v>44997</v>
+      </c>
+      <c r="J149" t="inlineStr">
+        <is>
+          <t>нет данных</t>
+        </is>
+      </c>
+    </row>
+    <row r="150">
+      <c r="E150" t="inlineStr">
+        <is>
+          <t>24.00R35</t>
+        </is>
+      </c>
+      <c r="F150" t="inlineStr">
+        <is>
+          <t>Бел-202</t>
+        </is>
+      </c>
+      <c r="G150" t="inlineStr">
+        <is>
+          <t>210B, Type, сер, H</t>
+        </is>
+      </c>
+      <c r="H150" t="n">
+        <v>2</v>
+      </c>
+      <c r="I150" s="1" t="n">
+        <v>44997</v>
+      </c>
+      <c r="J150" t="inlineStr">
+        <is>
+          <t>нет данных</t>
+        </is>
+      </c>
+    </row>
+    <row r="151">
+      <c r="E151" t="inlineStr">
+        <is>
+          <t>24.00R35</t>
+        </is>
+      </c>
+      <c r="F151" t="inlineStr">
+        <is>
+          <t>Бел-202</t>
+        </is>
+      </c>
+      <c r="G151" t="inlineStr">
+        <is>
+          <t>210B, Type, сер, C</t>
+        </is>
+      </c>
+      <c r="H151" t="n">
+        <v>2</v>
+      </c>
+      <c r="I151" s="1" t="n">
+        <v>44997</v>
+      </c>
+      <c r="J151" t="inlineStr">
+        <is>
+          <t>нет данных</t>
+        </is>
+      </c>
+    </row>
+    <row r="152">
+      <c r="E152" t="inlineStr">
+        <is>
+          <t>24.00R35</t>
+        </is>
+      </c>
+      <c r="F152" t="inlineStr">
+        <is>
+          <t>Бел-212</t>
+        </is>
+      </c>
+      <c r="G152" t="inlineStr">
+        <is>
+          <t>Type, сер, груз, LS-2</t>
+        </is>
+      </c>
+      <c r="H152" t="n">
+        <v>2</v>
+      </c>
+      <c r="I152" s="1" t="n">
+        <v>44997</v>
+      </c>
+      <c r="J152" t="inlineStr">
+        <is>
+          <t>нет данных</t>
+        </is>
+      </c>
+    </row>
+    <row r="153">
+      <c r="E153" t="inlineStr">
+        <is>
+          <t>24.00R35</t>
+        </is>
+      </c>
+      <c r="F153" t="inlineStr">
+        <is>
+          <t>Бел-212</t>
+        </is>
+      </c>
+      <c r="G153" t="inlineStr">
+        <is>
+          <t>Type, сер, груз, H</t>
+        </is>
+      </c>
+      <c r="H153" t="n">
+        <v>2</v>
+      </c>
+      <c r="I153" s="1" t="n">
+        <v>44997</v>
+      </c>
+      <c r="J153" t="inlineStr">
+        <is>
+          <t>нет данных</t>
+        </is>
+      </c>
+    </row>
+    <row r="154">
+      <c r="E154" t="inlineStr">
+        <is>
+          <t>24.00R35</t>
+        </is>
+      </c>
+      <c r="F154" t="inlineStr">
+        <is>
+          <t>Бел-212</t>
+        </is>
+      </c>
+      <c r="G154" t="inlineStr">
+        <is>
+          <t>Type, сер, груз, C</t>
+        </is>
+      </c>
+      <c r="H154" t="n">
+        <v>2</v>
+      </c>
+      <c r="I154" s="1" t="n">
+        <v>44997</v>
+      </c>
+      <c r="J154" t="inlineStr">
+        <is>
+          <t>нет данных</t>
+        </is>
+      </c>
+    </row>
+    <row r="155">
+      <c r="E155" t="inlineStr">
+        <is>
+          <t>21.00R35</t>
+        </is>
+      </c>
+      <c r="F155" t="inlineStr">
+        <is>
+          <t>Бел-200</t>
+        </is>
+      </c>
+      <c r="G155" t="inlineStr">
+        <is>
+          <t>202B, Type, сер, LS-2</t>
+        </is>
+      </c>
+      <c r="H155" t="n">
+        <v>2</v>
+      </c>
+      <c r="I155" s="1" t="n">
+        <v>44997</v>
+      </c>
+      <c r="J155" t="inlineStr">
+        <is>
+          <t>нет данных</t>
+        </is>
+      </c>
+    </row>
+    <row r="156">
+      <c r="E156" t="inlineStr">
+        <is>
+          <t>21.00R35</t>
+        </is>
+      </c>
+      <c r="F156" t="inlineStr">
+        <is>
+          <t>Бел-200</t>
+        </is>
+      </c>
+      <c r="G156" t="inlineStr">
+        <is>
+          <t>202B, Type, сер, H</t>
+        </is>
+      </c>
+      <c r="H156" t="n">
+        <v>2</v>
+      </c>
+      <c r="I156" s="1" t="n">
+        <v>44997</v>
+      </c>
+      <c r="J156" t="inlineStr">
+        <is>
+          <t>нет данных</t>
+        </is>
+      </c>
+    </row>
+    <row r="157">
+      <c r="E157" t="inlineStr">
+        <is>
+          <t>21.00R35</t>
+        </is>
+      </c>
+      <c r="F157" t="inlineStr">
+        <is>
+          <t>Бел-200</t>
+        </is>
+      </c>
+      <c r="G157" t="inlineStr">
+        <is>
+          <t>202B, Type, сер, C</t>
+        </is>
+      </c>
+      <c r="H157" t="n">
+        <v>2</v>
+      </c>
+      <c r="I157" s="1" t="n">
+        <v>44997</v>
+      </c>
+      <c r="J157" t="inlineStr">
+        <is>
+          <t>нет данных</t>
+        </is>
+      </c>
+    </row>
+    <row r="158">
+      <c r="E158" t="inlineStr">
+        <is>
+          <t>21.00R35</t>
+        </is>
+      </c>
+      <c r="F158" t="inlineStr">
+        <is>
+          <t>Бел-210</t>
+        </is>
+      </c>
+      <c r="G158" t="inlineStr">
+        <is>
+          <t>202B, Type, сер, LS-2</t>
+        </is>
+      </c>
+      <c r="H158" t="n">
+        <v>2</v>
+      </c>
+      <c r="I158" s="1" t="n">
+        <v>44997</v>
+      </c>
+      <c r="J158" t="inlineStr">
+        <is>
+          <t>нет данных</t>
+        </is>
+      </c>
+    </row>
+    <row r="159">
+      <c r="E159" t="inlineStr">
+        <is>
+          <t>21.00R35</t>
+        </is>
+      </c>
+      <c r="F159" t="inlineStr">
+        <is>
+          <t>Бел-210</t>
+        </is>
+      </c>
+      <c r="G159" t="inlineStr">
+        <is>
+          <t>202B, Type, сер, H</t>
+        </is>
+      </c>
+      <c r="H159" t="n">
+        <v>2</v>
+      </c>
+      <c r="I159" s="1" t="n">
+        <v>44997</v>
+      </c>
+      <c r="J159" t="inlineStr">
+        <is>
+          <t>нет данных</t>
+        </is>
+      </c>
+    </row>
+    <row r="160">
+      <c r="E160" t="inlineStr">
+        <is>
+          <t>21.00R35</t>
+        </is>
+      </c>
+      <c r="F160" t="inlineStr">
+        <is>
+          <t>Бел-210</t>
+        </is>
+      </c>
+      <c r="G160" t="inlineStr">
+        <is>
+          <t>202B, Type, сер, C</t>
+        </is>
+      </c>
+      <c r="H160" t="n">
+        <v>2</v>
+      </c>
+      <c r="I160" s="1" t="n">
+        <v>44997</v>
+      </c>
+      <c r="J160" t="inlineStr">
+        <is>
+          <t>нет данных</t>
+        </is>
+      </c>
+    </row>
+    <row r="161">
+      <c r="E161" t="inlineStr">
+        <is>
+          <t>14.00R20</t>
+        </is>
+      </c>
+      <c r="F161" t="inlineStr">
+        <is>
+          <t>BEL-248</t>
+        </is>
+      </c>
+      <c r="G161" t="inlineStr">
+        <is>
+          <t>сер, груз</t>
+        </is>
+      </c>
+      <c r="H161" t="n">
+        <v>2</v>
+      </c>
+      <c r="I161" s="1" t="n">
+        <v>44997</v>
+      </c>
+      <c r="J161" t="inlineStr">
+        <is>
+          <t>нет данных</t>
+        </is>
+      </c>
+    </row>
+    <row r="162">
+      <c r="E162" t="inlineStr">
+        <is>
+          <t>14.00R20</t>
+        </is>
+      </c>
+      <c r="F162" t="inlineStr">
+        <is>
+          <t>BEL-248</t>
+        </is>
+      </c>
+      <c r="G162" t="inlineStr">
+        <is>
+          <t>сер, груз</t>
+        </is>
+      </c>
+      <c r="H162" t="n">
+        <v>2</v>
+      </c>
+      <c r="I162" s="1" t="n">
+        <v>44997</v>
+      </c>
+      <c r="J162" t="inlineStr">
+        <is>
+          <t>нет данных</t>
+        </is>
+      </c>
+    </row>
+    <row r="163">
+      <c r="E163" t="inlineStr">
+        <is>
+          <t>14.00R20</t>
+        </is>
+      </c>
+      <c r="F163" t="inlineStr">
+        <is>
+          <t>BEL-248</t>
+        </is>
+      </c>
+      <c r="G163" t="inlineStr">
+        <is>
+          <t>б/к, сер, груз</t>
+        </is>
+      </c>
+      <c r="H163" t="n">
+        <v>2</v>
+      </c>
+      <c r="I163" s="1" t="n">
+        <v>44997</v>
+      </c>
+      <c r="J163" t="inlineStr">
+        <is>
+          <t>нет данных</t>
+        </is>
+      </c>
+    </row>
+    <row r="164">
+      <c r="E164" t="inlineStr">
+        <is>
+          <t>14.00R20</t>
+        </is>
+      </c>
+      <c r="F164" t="inlineStr">
+        <is>
+          <t>BEL-248</t>
+        </is>
+      </c>
+      <c r="G164" t="inlineStr">
+        <is>
+          <t>сер, груз</t>
+        </is>
+      </c>
+      <c r="H164" t="n">
+        <v>2</v>
+      </c>
+      <c r="I164" s="1" t="n">
+        <v>44997</v>
+      </c>
+      <c r="J164" t="inlineStr">
+        <is>
+          <t>нет данных</t>
+        </is>
+      </c>
+    </row>
+    <row r="165">
+      <c r="E165" t="inlineStr">
+        <is>
+          <t>175/70R13</t>
+        </is>
+      </c>
+      <c r="F165" t="inlineStr">
+        <is>
+          <t>Бел-103</t>
+        </is>
+      </c>
+      <c r="G165" t="inlineStr">
+        <is>
+          <t>б/к, сер, легк</t>
+        </is>
+      </c>
+      <c r="H165" t="n">
+        <v>2</v>
+      </c>
+      <c r="I165" s="1" t="n">
+        <v>44997</v>
+      </c>
+      <c r="J165" t="inlineStr">
+        <is>
+          <t>нет данных</t>
+        </is>
+      </c>
+    </row>
+    <row r="166">
+      <c r="E166" t="inlineStr">
+        <is>
+          <t>195/65R15</t>
+        </is>
+      </c>
+      <c r="F166" t="inlineStr">
+        <is>
+          <t>Бел-119</t>
+        </is>
+      </c>
+      <c r="G166" t="inlineStr">
+        <is>
+          <t>сер, легк</t>
+        </is>
+      </c>
+      <c r="H166" t="n">
+        <v>2</v>
+      </c>
+      <c r="I166" s="1" t="n">
+        <v>44997</v>
+      </c>
+      <c r="J166" t="inlineStr">
+        <is>
+          <t>нет данных</t>
+        </is>
+      </c>
+    </row>
+    <row r="167">
+      <c r="E167" t="inlineStr">
+        <is>
+          <t>210/80R16</t>
+        </is>
+      </c>
+      <c r="F167" t="inlineStr">
+        <is>
+          <t>Бел-777</t>
+        </is>
+      </c>
+      <c r="G167" t="inlineStr">
+        <is>
+          <t>сер, легк</t>
+        </is>
+      </c>
+      <c r="H167" t="n">
+        <v>2</v>
+      </c>
+      <c r="I167" s="1" t="n">
+        <v>44997</v>
+      </c>
+      <c r="J167" t="inlineStr">
+        <is>
+          <t>нет данных</t>
+        </is>
+      </c>
+    </row>
+    <row r="168">
+      <c r="E168" t="inlineStr">
+        <is>
+          <t>215/65R16C</t>
+        </is>
+      </c>
+      <c r="F168" t="inlineStr">
+        <is>
+          <t>Бел-1000</t>
+        </is>
+      </c>
+      <c r="G168" t="inlineStr">
+        <is>
+          <t>сер, легк</t>
+        </is>
+      </c>
+      <c r="H168" t="n">
+        <v>2</v>
+      </c>
+      <c r="I168" s="1" t="n">
+        <v>44997</v>
+      </c>
+      <c r="J168" t="inlineStr">
+        <is>
+          <t>нет данных</t>
+        </is>
+      </c>
+    </row>
+    <row r="169">
+      <c r="E169" t="inlineStr">
+        <is>
+          <t>175/65R15</t>
+        </is>
+      </c>
+      <c r="F169" t="inlineStr">
+        <is>
+          <t>Бел-1001</t>
+        </is>
+      </c>
+      <c r="G169" t="inlineStr">
+        <is>
+          <t>сер, легк</t>
+        </is>
+      </c>
+      <c r="H169" t="n">
+        <v>2</v>
+      </c>
+      <c r="I169" s="1" t="n">
+        <v>44997</v>
+      </c>
+      <c r="J169" t="inlineStr">
         <is>
           <t>нет данных</t>
         </is>

</xml_diff>

<commit_message>
Tyre.objects creation update in filemanager view + ComparativeAnalysisTyresModel привязка в РБ 03/07/2023
</commit_message>
<xml_diff>
--- a/src/Tyres.xlsx
+++ b/src/Tyres.xlsx
@@ -417,7 +417,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J41"/>
+  <dimension ref="A1:J22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -428,17 +428,12 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>ФБел-283</t>
+          <t xml:space="preserve"> </t>
         </is>
       </c>
       <c r="B1" t="inlineStr">
         <is>
-          <t>35/65-33</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
-          <t>42 груз сер</t>
+          <t xml:space="preserve"> </t>
         </is>
       </c>
       <c r="E1" t="inlineStr">
@@ -475,17 +470,17 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Бел-122</t>
+          <t>ФБел-283</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>24.00R35</t>
+          <t>35/65-33</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>груз Type сер LS-2</t>
+          <t>42 30 груз сер</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
@@ -500,14 +495,14 @@
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>42, груз, сер</t>
+          <t>42, 30, груз, сер</t>
         </is>
       </c>
       <c r="H2" t="n">
         <v>2</v>
       </c>
       <c r="I2" s="1" t="n">
-        <v>45005</v>
+        <v>45110</v>
       </c>
       <c r="J2" t="inlineStr">
         <is>
@@ -518,17 +513,17 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Бел-122</t>
+          <t>BEL-262</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>24.00R35</t>
+          <t>205/55R16</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>груз H Type сер</t>
+          <t>сер легк б/к</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
@@ -543,14 +538,14 @@
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>б/к, сер, легк</t>
+          <t>сер, легк, б/к</t>
         </is>
       </c>
       <c r="H3" t="n">
         <v>2</v>
       </c>
       <c r="I3" s="1" t="n">
-        <v>45005</v>
+        <v>45110</v>
       </c>
       <c r="J3" t="inlineStr">
         <is>
@@ -561,17 +556,17 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Бел-122</t>
+          <t>BEL-317</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>24.00R35</t>
+          <t>205/55R16</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>груз C Type сер</t>
+          <t>сер легк б/к</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
@@ -586,14 +581,14 @@
       </c>
       <c r="G4" t="inlineStr">
         <is>
-          <t>б/к, сер, легк</t>
+          <t>сер, легк, б/к</t>
         </is>
       </c>
       <c r="H4" t="n">
         <v>2</v>
       </c>
       <c r="I4" s="1" t="n">
-        <v>45005</v>
+        <v>45110</v>
       </c>
       <c r="J4" t="inlineStr">
         <is>
@@ -604,17 +599,17 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Бел-202</t>
+          <t>BEL-317S</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>24.00R35</t>
+          <t>205/55R16</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>210B Type сер LS-2</t>
+          <t>ошип сер</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
@@ -629,14 +624,14 @@
       </c>
       <c r="G5" t="inlineStr">
         <is>
-          <t>сер, ошип</t>
+          <t>ошип, сер</t>
         </is>
       </c>
       <c r="H5" t="n">
         <v>2</v>
       </c>
       <c r="I5" s="1" t="n">
-        <v>45005</v>
+        <v>45110</v>
       </c>
       <c r="J5" t="inlineStr">
         <is>
@@ -647,39 +642,39 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>Бел-202</t>
+          <t>BEL-1001</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>24.00R35</t>
+          <t>235/75R15</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>210B H Type сер</t>
+          <t>сер легк</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>24.00R35</t>
+          <t>235/75R15</t>
         </is>
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>Бел-122</t>
+          <t>BEL-1001</t>
         </is>
       </c>
       <c r="G6" t="inlineStr">
         <is>
-          <t>груз, Type, сер, LS-2</t>
+          <t>сер, легк</t>
         </is>
       </c>
       <c r="H6" t="n">
         <v>2</v>
       </c>
       <c r="I6" s="1" t="n">
-        <v>45005</v>
+        <v>45110</v>
       </c>
       <c r="J6" t="inlineStr">
         <is>
@@ -690,39 +685,39 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>Бел-202</t>
+          <t>BEL-1002</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>24.00R35</t>
+          <t>155/65R13</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>210B C Type сер</t>
+          <t>сер легк</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>24.00R35</t>
+          <t>155/65R13</t>
         </is>
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>Бел-122</t>
+          <t>BEL-1002</t>
         </is>
       </c>
       <c r="G7" t="inlineStr">
         <is>
-          <t>груз, H, Type, сер</t>
+          <t>сер, легк</t>
         </is>
       </c>
       <c r="H7" t="n">
         <v>2</v>
       </c>
       <c r="I7" s="1" t="n">
-        <v>45005</v>
+        <v>45110</v>
       </c>
       <c r="J7" t="inlineStr">
         <is>
@@ -733,39 +728,39 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>Бел-212</t>
+          <t>BEL-1004</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>24.00R35</t>
+          <t>205/55R16</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>груз Type сер LS-2</t>
+          <t>сер легк</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>24.00R35</t>
+          <t>205/55R16</t>
         </is>
       </c>
       <c r="F8" t="inlineStr">
         <is>
-          <t>Бел-122</t>
+          <t>BEL-1004</t>
         </is>
       </c>
       <c r="G8" t="inlineStr">
         <is>
-          <t>груз, C, Type, сер</t>
+          <t>сер, легк</t>
         </is>
       </c>
       <c r="H8" t="n">
         <v>2</v>
       </c>
       <c r="I8" s="1" t="n">
-        <v>45005</v>
+        <v>45110</v>
       </c>
       <c r="J8" t="inlineStr">
         <is>
@@ -776,39 +771,39 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>Бел-212</t>
+          <t>BEL-1005</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>24.00R35</t>
+          <t>225/50R17</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>груз H Type сер</t>
+          <t>сер легк</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>24.00R35</t>
+          <t>225/50R17</t>
         </is>
       </c>
       <c r="F9" t="inlineStr">
         <is>
-          <t>Бел-202</t>
+          <t>BEL-1005</t>
         </is>
       </c>
       <c r="G9" t="inlineStr">
         <is>
-          <t>210B, Type, сер, LS-2</t>
+          <t>сер, легк</t>
         </is>
       </c>
       <c r="H9" t="n">
         <v>2</v>
       </c>
       <c r="I9" s="1" t="n">
-        <v>45005</v>
+        <v>45110</v>
       </c>
       <c r="J9" t="inlineStr">
         <is>
@@ -819,7 +814,7 @@
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>Бел-212</t>
+          <t>Бел-202</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
@@ -829,7 +824,7 @@
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>груз C Type сер</t>
+          <t>210B H Type C сер</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
@@ -844,14 +839,14 @@
       </c>
       <c r="G10" t="inlineStr">
         <is>
-          <t>210B, H, Type, сер</t>
+          <t>210B, H, Type, C, сер</t>
         </is>
       </c>
       <c r="H10" t="n">
         <v>2</v>
       </c>
       <c r="I10" s="1" t="n">
-        <v>45005</v>
+        <v>45110</v>
       </c>
       <c r="J10" t="inlineStr">
         <is>
@@ -862,17 +857,17 @@
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>Бел-200</t>
+          <t>Бел-212</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>21.00R35</t>
+          <t>24.00R35</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>202B Type сер LS-2</t>
+          <t>груз Type LS-2 сер</t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
@@ -882,19 +877,19 @@
       </c>
       <c r="F11" t="inlineStr">
         <is>
-          <t>Бел-202</t>
+          <t>Бел-212</t>
         </is>
       </c>
       <c r="G11" t="inlineStr">
         <is>
-          <t>210B, C, Type, сер</t>
+          <t>груз, Type, LS-2, сер</t>
         </is>
       </c>
       <c r="H11" t="n">
         <v>2</v>
       </c>
       <c r="I11" s="1" t="n">
-        <v>45005</v>
+        <v>45110</v>
       </c>
       <c r="J11" t="inlineStr">
         <is>
@@ -915,29 +910,29 @@
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>202B H Type сер</t>
+          <t>202B Type C сер</t>
         </is>
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>24.00R35</t>
+          <t>21.00R35</t>
         </is>
       </c>
       <c r="F12" t="inlineStr">
         <is>
-          <t>Бел-212</t>
+          <t>Бел-200</t>
         </is>
       </c>
       <c r="G12" t="inlineStr">
         <is>
-          <t>груз, Type, сер, LS-2</t>
+          <t>202B, Type, C, сер</t>
         </is>
       </c>
       <c r="H12" t="n">
         <v>2</v>
       </c>
       <c r="I12" s="1" t="n">
-        <v>45005</v>
+        <v>45110</v>
       </c>
       <c r="J12" t="inlineStr">
         <is>
@@ -948,7 +943,7 @@
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>Бел-200</t>
+          <t>Бел-210</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
@@ -958,29 +953,29 @@
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>202B C Type сер</t>
+          <t>202B H Type LS-2 C сер</t>
         </is>
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>24.00R35</t>
+          <t>21.00R35</t>
         </is>
       </c>
       <c r="F13" t="inlineStr">
         <is>
-          <t>Бел-212</t>
+          <t>Бел-210</t>
         </is>
       </c>
       <c r="G13" t="inlineStr">
         <is>
-          <t>груз, H, Type, сер</t>
+          <t>202B, H, Type, LS-2, C, сер</t>
         </is>
       </c>
       <c r="H13" t="n">
         <v>2</v>
       </c>
       <c r="I13" s="1" t="n">
-        <v>45005</v>
+        <v>45110</v>
       </c>
       <c r="J13" t="inlineStr">
         <is>
@@ -991,39 +986,39 @@
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>Бел-210</t>
+          <t>BEL-248</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>21.00R35</t>
+          <t>14.00R20</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>202B Type сер LS-2</t>
+          <t>груз сер б/к</t>
         </is>
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>24.00R35</t>
+          <t>14.00R20</t>
         </is>
       </c>
       <c r="F14" t="inlineStr">
         <is>
-          <t>Бел-212</t>
+          <t>BEL-248</t>
         </is>
       </c>
       <c r="G14" t="inlineStr">
         <is>
-          <t>груз, C, Type, сер</t>
+          <t>груз, сер, б/к</t>
         </is>
       </c>
       <c r="H14" t="n">
         <v>2</v>
       </c>
       <c r="I14" s="1" t="n">
-        <v>45005</v>
+        <v>45110</v>
       </c>
       <c r="J14" t="inlineStr">
         <is>
@@ -1034,39 +1029,39 @@
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>Бел-210</t>
+          <t>Бел-103</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>21.00R35</t>
+          <t>175/70R13</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>202B H Type сер</t>
+          <t>сер легк б/к</t>
         </is>
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t>21.00R35</t>
+          <t>175/70R13</t>
         </is>
       </c>
       <c r="F15" t="inlineStr">
         <is>
-          <t>Бел-200</t>
+          <t>Бел-103</t>
         </is>
       </c>
       <c r="G15" t="inlineStr">
         <is>
-          <t>202B, Type, сер, LS-2</t>
+          <t>сер, легк, б/к</t>
         </is>
       </c>
       <c r="H15" t="n">
         <v>2</v>
       </c>
       <c r="I15" s="1" t="n">
-        <v>45005</v>
+        <v>45110</v>
       </c>
       <c r="J15" t="inlineStr">
         <is>
@@ -1077,39 +1072,39 @@
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>Бел-210</t>
+          <t>Бел-100</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>21.00R35</t>
+          <t>175/70R13</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>202B C Type сер</t>
+          <t>сер легк б/к</t>
         </is>
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>21.00R35</t>
+          <t>175/70R13</t>
         </is>
       </c>
       <c r="F16" t="inlineStr">
         <is>
-          <t>Бел-200</t>
+          <t>Бел-100</t>
         </is>
       </c>
       <c r="G16" t="inlineStr">
         <is>
-          <t>202B, H, Type, сер</t>
+          <t>сер, легк, б/к</t>
         </is>
       </c>
       <c r="H16" t="n">
         <v>2</v>
       </c>
       <c r="I16" s="1" t="n">
-        <v>45005</v>
+        <v>45110</v>
       </c>
       <c r="J16" t="inlineStr">
         <is>
@@ -1120,39 +1115,39 @@
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>BEL-248</t>
+          <t>Ф-35-1</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>14.00R20</t>
+          <t>11.2-20</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>груз сер</t>
+          <t>8 сх сер</t>
         </is>
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>21.00R35</t>
+          <t>195/65R15</t>
         </is>
       </c>
       <c r="F17" t="inlineStr">
         <is>
-          <t>Бел-200</t>
+          <t>Бел-119</t>
         </is>
       </c>
       <c r="G17" t="inlineStr">
         <is>
-          <t>202B, C, Type, сер</t>
+          <t>сер, легк</t>
         </is>
       </c>
       <c r="H17" t="n">
         <v>2</v>
       </c>
       <c r="I17" s="1" t="n">
-        <v>45005</v>
+        <v>45110</v>
       </c>
       <c r="J17" t="inlineStr">
         <is>
@@ -1163,39 +1158,39 @@
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>BEL-248</t>
+          <t>Бел-119</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>14.00R20</t>
+          <t>195/65R15</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>б/к груз сер</t>
+          <t>сер легк</t>
         </is>
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t>21.00R35</t>
+          <t>210/80R16</t>
         </is>
       </c>
       <c r="F18" t="inlineStr">
         <is>
-          <t>Бел-210</t>
+          <t>Бел-777</t>
         </is>
       </c>
       <c r="G18" t="inlineStr">
         <is>
-          <t>202B, Type, сер, LS-2</t>
+          <t>сер, легк</t>
         </is>
       </c>
       <c r="H18" t="n">
         <v>2</v>
       </c>
       <c r="I18" s="1" t="n">
-        <v>45005</v>
+        <v>45110</v>
       </c>
       <c r="J18" t="inlineStr">
         <is>
@@ -1206,39 +1201,39 @@
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>BEL-248</t>
+          <t>Бел-777</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>14.00R20</t>
+          <t>210/80R16</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>груз сер</t>
+          <t>сер легк</t>
         </is>
       </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t>21.00R35</t>
+          <t>215/65R16C</t>
         </is>
       </c>
       <c r="F19" t="inlineStr">
         <is>
-          <t>Бел-210</t>
+          <t>Бел-1000</t>
         </is>
       </c>
       <c r="G19" t="inlineStr">
         <is>
-          <t>202B, H, Type, сер</t>
+          <t>сер, легк</t>
         </is>
       </c>
       <c r="H19" t="n">
         <v>2</v>
       </c>
       <c r="I19" s="1" t="n">
-        <v>45005</v>
+        <v>45110</v>
       </c>
       <c r="J19" t="inlineStr">
         <is>
@@ -1249,39 +1244,39 @@
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>BEL-248</t>
+          <t>Бел-1000</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>14.00R20</t>
+          <t>215/65R16C</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>груз сер</t>
+          <t>сер легк</t>
         </is>
       </c>
       <c r="E20" t="inlineStr">
         <is>
-          <t>21.00R35</t>
+          <t>205/55R16</t>
         </is>
       </c>
       <c r="F20" t="inlineStr">
         <is>
-          <t>Бел-210</t>
+          <t>Бел-1001</t>
         </is>
       </c>
       <c r="G20" t="inlineStr">
         <is>
-          <t>202B, C, Type, сер</t>
+          <t>сер, легк</t>
         </is>
       </c>
       <c r="H20" t="n">
         <v>2</v>
       </c>
       <c r="I20" s="1" t="n">
-        <v>45005</v>
+        <v>45110</v>
       </c>
       <c r="J20" t="inlineStr">
         <is>
@@ -1292,39 +1287,39 @@
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>BEL-288</t>
+          <t>Бел-1001</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>12.00R20</t>
+          <t>205/55R16</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>груз сер</t>
+          <t>сер легк</t>
         </is>
       </c>
       <c r="E21" t="inlineStr">
         <is>
-          <t>14.00R20</t>
+          <t>225/50R17</t>
         </is>
       </c>
       <c r="F21" t="inlineStr">
         <is>
-          <t>BEL-248</t>
+          <t>Бел-1005</t>
         </is>
       </c>
       <c r="G21" t="inlineStr">
         <is>
-          <t>груз, сер</t>
+          <t>сер, легк</t>
         </is>
       </c>
       <c r="H21" t="n">
         <v>2</v>
       </c>
       <c r="I21" s="1" t="n">
-        <v>45005</v>
+        <v>45110</v>
       </c>
       <c r="J21" t="inlineStr">
         <is>
@@ -1335,546 +1330,15 @@
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>Бел-95</t>
+          <t>Бел-1005</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>16.00R20</t>
+          <t>225/50R17</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
-        <is>
-          <t>173G б/к груз сер</t>
-        </is>
-      </c>
-      <c r="E22" t="inlineStr">
-        <is>
-          <t>14.00R20</t>
-        </is>
-      </c>
-      <c r="F22" t="inlineStr">
-        <is>
-          <t>BEL-248</t>
-        </is>
-      </c>
-      <c r="G22" t="inlineStr">
-        <is>
-          <t>б/к, груз, сер</t>
-        </is>
-      </c>
-      <c r="H22" t="n">
-        <v>2</v>
-      </c>
-      <c r="I22" s="1" t="n">
-        <v>45005</v>
-      </c>
-      <c r="J22" t="inlineStr">
-        <is>
-          <t>нет данных</t>
-        </is>
-      </c>
-    </row>
-    <row r="23">
-      <c r="A23" t="inlineStr">
-        <is>
-          <t>Бел-95</t>
-        </is>
-      </c>
-      <c r="B23" t="inlineStr">
-        <is>
-          <t>16.00R20</t>
-        </is>
-      </c>
-      <c r="C23" t="inlineStr">
-        <is>
-          <t>173G груз сер</t>
-        </is>
-      </c>
-      <c r="E23" t="inlineStr">
-        <is>
-          <t>14.00R20</t>
-        </is>
-      </c>
-      <c r="F23" t="inlineStr">
-        <is>
-          <t>BEL-248</t>
-        </is>
-      </c>
-      <c r="G23" t="inlineStr">
-        <is>
-          <t>груз, сер</t>
-        </is>
-      </c>
-      <c r="H23" t="n">
-        <v>2</v>
-      </c>
-      <c r="I23" s="1" t="n">
-        <v>45005</v>
-      </c>
-      <c r="J23" t="inlineStr">
-        <is>
-          <t>нет данных</t>
-        </is>
-      </c>
-    </row>
-    <row r="24">
-      <c r="A24" t="inlineStr">
-        <is>
-          <t>Бел-95</t>
-        </is>
-      </c>
-      <c r="B24" t="inlineStr">
-        <is>
-          <t>16.00R20</t>
-        </is>
-      </c>
-      <c r="C24" t="inlineStr">
-        <is>
-          <t>173G груз сер</t>
-        </is>
-      </c>
-      <c r="E24" t="inlineStr">
-        <is>
-          <t>14.00R20</t>
-        </is>
-      </c>
-      <c r="F24" t="inlineStr">
-        <is>
-          <t>BEL-248</t>
-        </is>
-      </c>
-      <c r="G24" t="inlineStr">
-        <is>
-          <t>груз, сер</t>
-        </is>
-      </c>
-      <c r="H24" t="n">
-        <v>2</v>
-      </c>
-      <c r="I24" s="1" t="n">
-        <v>45005</v>
-      </c>
-      <c r="J24" t="inlineStr">
-        <is>
-          <t>нет данных</t>
-        </is>
-      </c>
-    </row>
-    <row r="25">
-      <c r="A25" t="inlineStr">
-        <is>
-          <t>Бел-95</t>
-        </is>
-      </c>
-      <c r="B25" t="inlineStr">
-        <is>
-          <t>16.00R20</t>
-        </is>
-      </c>
-      <c r="C25" t="inlineStr">
-        <is>
-          <t>173G груз сер</t>
-        </is>
-      </c>
-      <c r="E25" t="inlineStr">
-        <is>
-          <t>175/70R13</t>
-        </is>
-      </c>
-      <c r="F25" t="inlineStr">
-        <is>
-          <t>Бел-103</t>
-        </is>
-      </c>
-      <c r="G25" t="inlineStr">
-        <is>
-          <t>б/к, сер, легк</t>
-        </is>
-      </c>
-      <c r="H25" t="n">
-        <v>2</v>
-      </c>
-      <c r="I25" s="1" t="n">
-        <v>45005</v>
-      </c>
-      <c r="J25" t="inlineStr">
-        <is>
-          <t>нет данных</t>
-        </is>
-      </c>
-    </row>
-    <row r="26">
-      <c r="A26" t="inlineStr">
-        <is>
-          <t>Бел-95</t>
-        </is>
-      </c>
-      <c r="B26" t="inlineStr">
-        <is>
-          <t>16.00R20</t>
-        </is>
-      </c>
-      <c r="C26" t="inlineStr">
-        <is>
-          <t>173G груз сер</t>
-        </is>
-      </c>
-      <c r="E26" t="inlineStr">
-        <is>
-          <t>195/65R15</t>
-        </is>
-      </c>
-      <c r="F26" t="inlineStr">
-        <is>
-          <t>Бел-119</t>
-        </is>
-      </c>
-      <c r="G26" t="inlineStr">
-        <is>
-          <t>сер, легк</t>
-        </is>
-      </c>
-      <c r="H26" t="n">
-        <v>2</v>
-      </c>
-      <c r="I26" s="1" t="n">
-        <v>45005</v>
-      </c>
-      <c r="J26" t="inlineStr">
-        <is>
-          <t>нет данных</t>
-        </is>
-      </c>
-    </row>
-    <row r="27">
-      <c r="A27" t="inlineStr">
-        <is>
-          <t>Бел-95</t>
-        </is>
-      </c>
-      <c r="B27" t="inlineStr">
-        <is>
-          <t>16.00R20</t>
-        </is>
-      </c>
-      <c r="C27" t="inlineStr">
-        <is>
-          <t>173G груз сер</t>
-        </is>
-      </c>
-      <c r="E27" t="inlineStr">
-        <is>
-          <t>210/80R16</t>
-        </is>
-      </c>
-      <c r="F27" t="inlineStr">
-        <is>
-          <t>Бел-777</t>
-        </is>
-      </c>
-      <c r="G27" t="inlineStr">
-        <is>
-          <t>сер, легк</t>
-        </is>
-      </c>
-      <c r="H27" t="n">
-        <v>2</v>
-      </c>
-      <c r="I27" s="1" t="n">
-        <v>45005</v>
-      </c>
-      <c r="J27" t="inlineStr">
-        <is>
-          <t>нет данных</t>
-        </is>
-      </c>
-    </row>
-    <row r="28">
-      <c r="A28" t="inlineStr">
-        <is>
-          <t>Бел-95</t>
-        </is>
-      </c>
-      <c r="B28" t="inlineStr">
-        <is>
-          <t>16.00R20</t>
-        </is>
-      </c>
-      <c r="C28" t="inlineStr">
-        <is>
-          <t>173G сер</t>
-        </is>
-      </c>
-      <c r="E28" t="inlineStr">
-        <is>
-          <t>215/65R16C</t>
-        </is>
-      </c>
-      <c r="F28" t="inlineStr">
-        <is>
-          <t>Бел-1000</t>
-        </is>
-      </c>
-      <c r="G28" t="inlineStr">
-        <is>
-          <t>сер, легк</t>
-        </is>
-      </c>
-      <c r="H28" t="n">
-        <v>2</v>
-      </c>
-      <c r="I28" s="1" t="n">
-        <v>45005</v>
-      </c>
-      <c r="J28" t="inlineStr">
-        <is>
-          <t>нет данных</t>
-        </is>
-      </c>
-    </row>
-    <row r="29">
-      <c r="A29" t="inlineStr">
-        <is>
-          <t>BEL-405</t>
-        </is>
-      </c>
-      <c r="B29" t="inlineStr">
-        <is>
-          <t>395/85R20</t>
-        </is>
-      </c>
-      <c r="C29" t="inlineStr">
-        <is>
-          <t>168J груз сер</t>
-        </is>
-      </c>
-      <c r="E29" t="inlineStr">
-        <is>
-          <t>175/65R15</t>
-        </is>
-      </c>
-      <c r="F29" t="inlineStr">
-        <is>
-          <t>Бел-1001</t>
-        </is>
-      </c>
-      <c r="G29" t="inlineStr">
-        <is>
-          <t>сер, легк</t>
-        </is>
-      </c>
-      <c r="H29" t="n">
-        <v>2</v>
-      </c>
-      <c r="I29" s="1" t="n">
-        <v>45005</v>
-      </c>
-      <c r="J29" t="inlineStr">
-        <is>
-          <t>нет данных</t>
-        </is>
-      </c>
-    </row>
-    <row r="30">
-      <c r="A30" t="inlineStr">
-        <is>
-          <t>Бел-145</t>
-        </is>
-      </c>
-      <c r="B30" t="inlineStr">
-        <is>
-          <t>445/65R22.5</t>
-        </is>
-      </c>
-      <c r="C30" t="inlineStr">
-        <is>
-          <t>б/к груз сер</t>
-        </is>
-      </c>
-    </row>
-    <row r="31">
-      <c r="A31" t="inlineStr">
-        <is>
-          <t>Бел-230</t>
-        </is>
-      </c>
-      <c r="B31" t="inlineStr">
-        <is>
-          <t>355/65-15</t>
-        </is>
-      </c>
-      <c r="C31" t="inlineStr">
-        <is>
-          <t>сер</t>
-        </is>
-      </c>
-    </row>
-    <row r="32">
-      <c r="A32" t="inlineStr">
-        <is>
-          <t>Бел-230М</t>
-        </is>
-      </c>
-      <c r="B32" t="inlineStr">
-        <is>
-          <t>355/65-15</t>
-        </is>
-      </c>
-      <c r="C32" t="inlineStr">
-        <is>
-          <t>сер</t>
-        </is>
-      </c>
-    </row>
-    <row r="33">
-      <c r="A33" t="inlineStr">
-        <is>
-          <t>BEL-262</t>
-        </is>
-      </c>
-      <c r="B33" t="inlineStr">
-        <is>
-          <t>205/55R16</t>
-        </is>
-      </c>
-      <c r="C33" t="inlineStr">
-        <is>
-          <t>б/к сер легк</t>
-        </is>
-      </c>
-    </row>
-    <row r="34">
-      <c r="A34" t="inlineStr">
-        <is>
-          <t>BEL-317</t>
-        </is>
-      </c>
-      <c r="B34" t="inlineStr">
-        <is>
-          <t>205/55R16</t>
-        </is>
-      </c>
-      <c r="C34" t="inlineStr">
-        <is>
-          <t>б/к сер легк</t>
-        </is>
-      </c>
-    </row>
-    <row r="35">
-      <c r="A35" t="inlineStr">
-        <is>
-          <t>BEL-317S</t>
-        </is>
-      </c>
-      <c r="B35" t="inlineStr">
-        <is>
-          <t>205/55R16</t>
-        </is>
-      </c>
-      <c r="C35" t="inlineStr">
-        <is>
-          <t>сер ошип</t>
-        </is>
-      </c>
-    </row>
-    <row r="36">
-      <c r="A36" t="inlineStr">
-        <is>
-          <t>BEL-277</t>
-        </is>
-      </c>
-      <c r="B36" t="inlineStr">
-        <is>
-          <t>205/60R16</t>
-        </is>
-      </c>
-      <c r="C36" t="inlineStr">
-        <is>
-          <t>б/к сер легк</t>
-        </is>
-      </c>
-    </row>
-    <row r="37">
-      <c r="A37" t="inlineStr">
-        <is>
-          <t>Бел-103</t>
-        </is>
-      </c>
-      <c r="B37" t="inlineStr">
-        <is>
-          <t>175/70R13</t>
-        </is>
-      </c>
-      <c r="C37" t="inlineStr">
-        <is>
-          <t>б/к сер легк</t>
-        </is>
-      </c>
-    </row>
-    <row r="38">
-      <c r="A38" t="inlineStr">
-        <is>
-          <t>Бел-119</t>
-        </is>
-      </c>
-      <c r="B38" t="inlineStr">
-        <is>
-          <t>195/65R15</t>
-        </is>
-      </c>
-      <c r="C38" t="inlineStr">
-        <is>
-          <t>сер легк</t>
-        </is>
-      </c>
-    </row>
-    <row r="39">
-      <c r="A39" t="inlineStr">
-        <is>
-          <t>Бел-777</t>
-        </is>
-      </c>
-      <c r="B39" t="inlineStr">
-        <is>
-          <t>210/80R16</t>
-        </is>
-      </c>
-      <c r="C39" t="inlineStr">
-        <is>
-          <t>сер легк</t>
-        </is>
-      </c>
-    </row>
-    <row r="40">
-      <c r="A40" t="inlineStr">
-        <is>
-          <t>Бел-1000</t>
-        </is>
-      </c>
-      <c r="B40" t="inlineStr">
-        <is>
-          <t>215/65R16C</t>
-        </is>
-      </c>
-      <c r="C40" t="inlineStr">
-        <is>
-          <t>сер легк</t>
-        </is>
-      </c>
-    </row>
-    <row r="41">
-      <c r="A41" t="inlineStr">
-        <is>
-          <t>Бел-1001</t>
-        </is>
-      </c>
-      <c r="B41" t="inlineStr">
-        <is>
-          <t>175/65R15</t>
-        </is>
-      </c>
-      <c r="C41" t="inlineStr">
         <is>
           <t>сер легк</t>
         </is>

</xml_diff>

<commit_message>
CHEMCOURIER IMPROVEMENTS at 15/10/2023
</commit_message>
<xml_diff>
--- a/src/Tyres.xlsx
+++ b/src/Tyres.xlsx
@@ -502,7 +502,7 @@
         <v>2</v>
       </c>
       <c r="I2" s="1" t="n">
-        <v>45110</v>
+        <v>45138</v>
       </c>
       <c r="J2" t="inlineStr">
         <is>
@@ -545,7 +545,7 @@
         <v>2</v>
       </c>
       <c r="I3" s="1" t="n">
-        <v>45110</v>
+        <v>45138</v>
       </c>
       <c r="J3" t="inlineStr">
         <is>
@@ -588,7 +588,7 @@
         <v>2</v>
       </c>
       <c r="I4" s="1" t="n">
-        <v>45110</v>
+        <v>45138</v>
       </c>
       <c r="J4" t="inlineStr">
         <is>
@@ -631,7 +631,7 @@
         <v>2</v>
       </c>
       <c r="I5" s="1" t="n">
-        <v>45110</v>
+        <v>45138</v>
       </c>
       <c r="J5" t="inlineStr">
         <is>
@@ -674,7 +674,7 @@
         <v>2</v>
       </c>
       <c r="I6" s="1" t="n">
-        <v>45110</v>
+        <v>45138</v>
       </c>
       <c r="J6" t="inlineStr">
         <is>
@@ -717,7 +717,7 @@
         <v>2</v>
       </c>
       <c r="I7" s="1" t="n">
-        <v>45110</v>
+        <v>45138</v>
       </c>
       <c r="J7" t="inlineStr">
         <is>
@@ -760,7 +760,7 @@
         <v>2</v>
       </c>
       <c r="I8" s="1" t="n">
-        <v>45110</v>
+        <v>45138</v>
       </c>
       <c r="J8" t="inlineStr">
         <is>
@@ -803,7 +803,7 @@
         <v>2</v>
       </c>
       <c r="I9" s="1" t="n">
-        <v>45110</v>
+        <v>45138</v>
       </c>
       <c r="J9" t="inlineStr">
         <is>
@@ -846,7 +846,7 @@
         <v>2</v>
       </c>
       <c r="I10" s="1" t="n">
-        <v>45110</v>
+        <v>45138</v>
       </c>
       <c r="J10" t="inlineStr">
         <is>
@@ -889,7 +889,7 @@
         <v>2</v>
       </c>
       <c r="I11" s="1" t="n">
-        <v>45110</v>
+        <v>45138</v>
       </c>
       <c r="J11" t="inlineStr">
         <is>
@@ -932,7 +932,7 @@
         <v>2</v>
       </c>
       <c r="I12" s="1" t="n">
-        <v>45110</v>
+        <v>45138</v>
       </c>
       <c r="J12" t="inlineStr">
         <is>
@@ -975,7 +975,7 @@
         <v>2</v>
       </c>
       <c r="I13" s="1" t="n">
-        <v>45110</v>
+        <v>45138</v>
       </c>
       <c r="J13" t="inlineStr">
         <is>
@@ -1018,7 +1018,7 @@
         <v>2</v>
       </c>
       <c r="I14" s="1" t="n">
-        <v>45110</v>
+        <v>45138</v>
       </c>
       <c r="J14" t="inlineStr">
         <is>
@@ -1061,7 +1061,7 @@
         <v>2</v>
       </c>
       <c r="I15" s="1" t="n">
-        <v>45110</v>
+        <v>45138</v>
       </c>
       <c r="J15" t="inlineStr">
         <is>
@@ -1104,7 +1104,7 @@
         <v>2</v>
       </c>
       <c r="I16" s="1" t="n">
-        <v>45110</v>
+        <v>45138</v>
       </c>
       <c r="J16" t="inlineStr">
         <is>
@@ -1147,7 +1147,7 @@
         <v>2</v>
       </c>
       <c r="I17" s="1" t="n">
-        <v>45110</v>
+        <v>45138</v>
       </c>
       <c r="J17" t="inlineStr">
         <is>
@@ -1190,7 +1190,7 @@
         <v>2</v>
       </c>
       <c r="I18" s="1" t="n">
-        <v>45110</v>
+        <v>45138</v>
       </c>
       <c r="J18" t="inlineStr">
         <is>
@@ -1233,7 +1233,7 @@
         <v>2</v>
       </c>
       <c r="I19" s="1" t="n">
-        <v>45110</v>
+        <v>45138</v>
       </c>
       <c r="J19" t="inlineStr">
         <is>
@@ -1276,7 +1276,7 @@
         <v>2</v>
       </c>
       <c r="I20" s="1" t="n">
-        <v>45110</v>
+        <v>45138</v>
       </c>
       <c r="J20" t="inlineStr">
         <is>
@@ -1319,7 +1319,7 @@
         <v>2</v>
       </c>
       <c r="I21" s="1" t="n">
-        <v>45110</v>
+        <v>45138</v>
       </c>
       <c r="J21" t="inlineStr">
         <is>

</xml_diff>

<commit_message>
chemcurier v.0.9.1 table in excel creation v.1 at 28/10/2023
</commit_message>
<xml_diff>
--- a/src/Tyres.xlsx
+++ b/src/Tyres.xlsx
@@ -17,9 +17,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="yyyy-mm-dd"/>
-  </numFmts>
+  <numFmts count="0"/>
   <fonts count="1">
     <font>
       <name val="Calibri"/>
@@ -49,9 +47,8 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
@@ -417,7 +414,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J22"/>
+  <dimension ref="A1:C23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -436,36 +433,7 @@
           <t xml:space="preserve"> </t>
         </is>
       </c>
-      <c r="E1" t="inlineStr">
-        <is>
-          <t>Tyre Size</t>
-        </is>
-      </c>
-      <c r="F1" t="inlineStr">
-        <is>
-          <t>Model</t>
-        </is>
-      </c>
-      <c r="G1" t="inlineStr">
-        <is>
-          <t>Param</t>
-        </is>
-      </c>
-      <c r="H1" t="inlineStr">
-        <is>
-          <t>Sales value</t>
-        </is>
-      </c>
-      <c r="I1" t="inlineStr">
-        <is>
-          <t>Date_of_sales</t>
-        </is>
-      </c>
-      <c r="J1" t="inlineStr">
-        <is>
-          <t>Contragent</t>
-        </is>
-      </c>
+      <c r="C1" t="inlineStr"/>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
@@ -483,32 +451,6 @@
           <t>42 30 груз сер</t>
         </is>
       </c>
-      <c r="E2" t="inlineStr">
-        <is>
-          <t>35/65-33</t>
-        </is>
-      </c>
-      <c r="F2" t="inlineStr">
-        <is>
-          <t>ФБел-283</t>
-        </is>
-      </c>
-      <c r="G2" t="inlineStr">
-        <is>
-          <t>42, 30, груз, сер</t>
-        </is>
-      </c>
-      <c r="H2" t="n">
-        <v>2</v>
-      </c>
-      <c r="I2" s="1" t="n">
-        <v>45138</v>
-      </c>
-      <c r="J2" t="inlineStr">
-        <is>
-          <t>нет данных</t>
-        </is>
-      </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -526,32 +468,6 @@
           <t>сер легк б/к</t>
         </is>
       </c>
-      <c r="E3" t="inlineStr">
-        <is>
-          <t>205/55R16</t>
-        </is>
-      </c>
-      <c r="F3" t="inlineStr">
-        <is>
-          <t>BEL-262</t>
-        </is>
-      </c>
-      <c r="G3" t="inlineStr">
-        <is>
-          <t>сер, легк, б/к</t>
-        </is>
-      </c>
-      <c r="H3" t="n">
-        <v>2</v>
-      </c>
-      <c r="I3" s="1" t="n">
-        <v>45138</v>
-      </c>
-      <c r="J3" t="inlineStr">
-        <is>
-          <t>нет данных</t>
-        </is>
-      </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
@@ -569,32 +485,6 @@
           <t>сер легк б/к</t>
         </is>
       </c>
-      <c r="E4" t="inlineStr">
-        <is>
-          <t>205/55R16</t>
-        </is>
-      </c>
-      <c r="F4" t="inlineStr">
-        <is>
-          <t>BEL-317</t>
-        </is>
-      </c>
-      <c r="G4" t="inlineStr">
-        <is>
-          <t>сер, легк, б/к</t>
-        </is>
-      </c>
-      <c r="H4" t="n">
-        <v>2</v>
-      </c>
-      <c r="I4" s="1" t="n">
-        <v>45138</v>
-      </c>
-      <c r="J4" t="inlineStr">
-        <is>
-          <t>нет данных</t>
-        </is>
-      </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
@@ -612,32 +502,6 @@
           <t>ошип сер</t>
         </is>
       </c>
-      <c r="E5" t="inlineStr">
-        <is>
-          <t>205/55R16</t>
-        </is>
-      </c>
-      <c r="F5" t="inlineStr">
-        <is>
-          <t>BEL-317S</t>
-        </is>
-      </c>
-      <c r="G5" t="inlineStr">
-        <is>
-          <t>ошип, сер</t>
-        </is>
-      </c>
-      <c r="H5" t="n">
-        <v>2</v>
-      </c>
-      <c r="I5" s="1" t="n">
-        <v>45138</v>
-      </c>
-      <c r="J5" t="inlineStr">
-        <is>
-          <t>нет данных</t>
-        </is>
-      </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
@@ -655,32 +519,6 @@
           <t>сер легк</t>
         </is>
       </c>
-      <c r="E6" t="inlineStr">
-        <is>
-          <t>235/75R15</t>
-        </is>
-      </c>
-      <c r="F6" t="inlineStr">
-        <is>
-          <t>BEL-1001</t>
-        </is>
-      </c>
-      <c r="G6" t="inlineStr">
-        <is>
-          <t>сер, легк</t>
-        </is>
-      </c>
-      <c r="H6" t="n">
-        <v>2</v>
-      </c>
-      <c r="I6" s="1" t="n">
-        <v>45138</v>
-      </c>
-      <c r="J6" t="inlineStr">
-        <is>
-          <t>нет данных</t>
-        </is>
-      </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
@@ -698,32 +536,6 @@
           <t>сер легк</t>
         </is>
       </c>
-      <c r="E7" t="inlineStr">
-        <is>
-          <t>155/65R13</t>
-        </is>
-      </c>
-      <c r="F7" t="inlineStr">
-        <is>
-          <t>BEL-1002</t>
-        </is>
-      </c>
-      <c r="G7" t="inlineStr">
-        <is>
-          <t>сер, легк</t>
-        </is>
-      </c>
-      <c r="H7" t="n">
-        <v>2</v>
-      </c>
-      <c r="I7" s="1" t="n">
-        <v>45138</v>
-      </c>
-      <c r="J7" t="inlineStr">
-        <is>
-          <t>нет данных</t>
-        </is>
-      </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
@@ -741,32 +553,6 @@
           <t>сер легк</t>
         </is>
       </c>
-      <c r="E8" t="inlineStr">
-        <is>
-          <t>205/55R16</t>
-        </is>
-      </c>
-      <c r="F8" t="inlineStr">
-        <is>
-          <t>BEL-1004</t>
-        </is>
-      </c>
-      <c r="G8" t="inlineStr">
-        <is>
-          <t>сер, легк</t>
-        </is>
-      </c>
-      <c r="H8" t="n">
-        <v>2</v>
-      </c>
-      <c r="I8" s="1" t="n">
-        <v>45138</v>
-      </c>
-      <c r="J8" t="inlineStr">
-        <is>
-          <t>нет данных</t>
-        </is>
-      </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
@@ -784,32 +570,6 @@
           <t>сер легк</t>
         </is>
       </c>
-      <c r="E9" t="inlineStr">
-        <is>
-          <t>225/50R17</t>
-        </is>
-      </c>
-      <c r="F9" t="inlineStr">
-        <is>
-          <t>BEL-1005</t>
-        </is>
-      </c>
-      <c r="G9" t="inlineStr">
-        <is>
-          <t>сер, легк</t>
-        </is>
-      </c>
-      <c r="H9" t="n">
-        <v>2</v>
-      </c>
-      <c r="I9" s="1" t="n">
-        <v>45138</v>
-      </c>
-      <c r="J9" t="inlineStr">
-        <is>
-          <t>нет данных</t>
-        </is>
-      </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
@@ -827,32 +587,6 @@
           <t>210B H Type C сер</t>
         </is>
       </c>
-      <c r="E10" t="inlineStr">
-        <is>
-          <t>24.00R35</t>
-        </is>
-      </c>
-      <c r="F10" t="inlineStr">
-        <is>
-          <t>Бел-202</t>
-        </is>
-      </c>
-      <c r="G10" t="inlineStr">
-        <is>
-          <t>210B, H, Type, C, сер</t>
-        </is>
-      </c>
-      <c r="H10" t="n">
-        <v>2</v>
-      </c>
-      <c r="I10" s="1" t="n">
-        <v>45138</v>
-      </c>
-      <c r="J10" t="inlineStr">
-        <is>
-          <t>нет данных</t>
-        </is>
-      </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
@@ -870,32 +604,6 @@
           <t>груз Type LS-2 сер</t>
         </is>
       </c>
-      <c r="E11" t="inlineStr">
-        <is>
-          <t>24.00R35</t>
-        </is>
-      </c>
-      <c r="F11" t="inlineStr">
-        <is>
-          <t>Бел-212</t>
-        </is>
-      </c>
-      <c r="G11" t="inlineStr">
-        <is>
-          <t>груз, Type, LS-2, сер</t>
-        </is>
-      </c>
-      <c r="H11" t="n">
-        <v>2</v>
-      </c>
-      <c r="I11" s="1" t="n">
-        <v>45138</v>
-      </c>
-      <c r="J11" t="inlineStr">
-        <is>
-          <t>нет данных</t>
-        </is>
-      </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
@@ -913,32 +621,6 @@
           <t>202B Type C сер</t>
         </is>
       </c>
-      <c r="E12" t="inlineStr">
-        <is>
-          <t>21.00R35</t>
-        </is>
-      </c>
-      <c r="F12" t="inlineStr">
-        <is>
-          <t>Бел-200</t>
-        </is>
-      </c>
-      <c r="G12" t="inlineStr">
-        <is>
-          <t>202B, Type, C, сер</t>
-        </is>
-      </c>
-      <c r="H12" t="n">
-        <v>2</v>
-      </c>
-      <c r="I12" s="1" t="n">
-        <v>45138</v>
-      </c>
-      <c r="J12" t="inlineStr">
-        <is>
-          <t>нет данных</t>
-        </is>
-      </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
@@ -956,32 +638,6 @@
           <t>202B H Type LS-2 C сер</t>
         </is>
       </c>
-      <c r="E13" t="inlineStr">
-        <is>
-          <t>21.00R35</t>
-        </is>
-      </c>
-      <c r="F13" t="inlineStr">
-        <is>
-          <t>Бел-210</t>
-        </is>
-      </c>
-      <c r="G13" t="inlineStr">
-        <is>
-          <t>202B, H, Type, LS-2, C, сер</t>
-        </is>
-      </c>
-      <c r="H13" t="n">
-        <v>2</v>
-      </c>
-      <c r="I13" s="1" t="n">
-        <v>45138</v>
-      </c>
-      <c r="J13" t="inlineStr">
-        <is>
-          <t>нет данных</t>
-        </is>
-      </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
@@ -999,32 +655,6 @@
           <t>груз сер б/к</t>
         </is>
       </c>
-      <c r="E14" t="inlineStr">
-        <is>
-          <t>14.00R20</t>
-        </is>
-      </c>
-      <c r="F14" t="inlineStr">
-        <is>
-          <t>BEL-248</t>
-        </is>
-      </c>
-      <c r="G14" t="inlineStr">
-        <is>
-          <t>груз, сер, б/к</t>
-        </is>
-      </c>
-      <c r="H14" t="n">
-        <v>2</v>
-      </c>
-      <c r="I14" s="1" t="n">
-        <v>45138</v>
-      </c>
-      <c r="J14" t="inlineStr">
-        <is>
-          <t>нет данных</t>
-        </is>
-      </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
@@ -1042,32 +672,6 @@
           <t>сер легк б/к</t>
         </is>
       </c>
-      <c r="E15" t="inlineStr">
-        <is>
-          <t>175/70R13</t>
-        </is>
-      </c>
-      <c r="F15" t="inlineStr">
-        <is>
-          <t>Бел-103</t>
-        </is>
-      </c>
-      <c r="G15" t="inlineStr">
-        <is>
-          <t>сер, легк, б/к</t>
-        </is>
-      </c>
-      <c r="H15" t="n">
-        <v>2</v>
-      </c>
-      <c r="I15" s="1" t="n">
-        <v>45138</v>
-      </c>
-      <c r="J15" t="inlineStr">
-        <is>
-          <t>нет данных</t>
-        </is>
-      </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
@@ -1085,32 +689,6 @@
           <t>сер легк б/к</t>
         </is>
       </c>
-      <c r="E16" t="inlineStr">
-        <is>
-          <t>175/70R13</t>
-        </is>
-      </c>
-      <c r="F16" t="inlineStr">
-        <is>
-          <t>Бел-100</t>
-        </is>
-      </c>
-      <c r="G16" t="inlineStr">
-        <is>
-          <t>сер, легк, б/к</t>
-        </is>
-      </c>
-      <c r="H16" t="n">
-        <v>2</v>
-      </c>
-      <c r="I16" s="1" t="n">
-        <v>45138</v>
-      </c>
-      <c r="J16" t="inlineStr">
-        <is>
-          <t>нет данных</t>
-        </is>
-      </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
@@ -1128,32 +706,6 @@
           <t>8 сх сер</t>
         </is>
       </c>
-      <c r="E17" t="inlineStr">
-        <is>
-          <t>195/65R15</t>
-        </is>
-      </c>
-      <c r="F17" t="inlineStr">
-        <is>
-          <t>Бел-119</t>
-        </is>
-      </c>
-      <c r="G17" t="inlineStr">
-        <is>
-          <t>сер, легк</t>
-        </is>
-      </c>
-      <c r="H17" t="n">
-        <v>2</v>
-      </c>
-      <c r="I17" s="1" t="n">
-        <v>45138</v>
-      </c>
-      <c r="J17" t="inlineStr">
-        <is>
-          <t>нет данных</t>
-        </is>
-      </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
@@ -1171,32 +723,6 @@
           <t>сер легк</t>
         </is>
       </c>
-      <c r="E18" t="inlineStr">
-        <is>
-          <t>210/80R16</t>
-        </is>
-      </c>
-      <c r="F18" t="inlineStr">
-        <is>
-          <t>Бел-777</t>
-        </is>
-      </c>
-      <c r="G18" t="inlineStr">
-        <is>
-          <t>сер, легк</t>
-        </is>
-      </c>
-      <c r="H18" t="n">
-        <v>2</v>
-      </c>
-      <c r="I18" s="1" t="n">
-        <v>45138</v>
-      </c>
-      <c r="J18" t="inlineStr">
-        <is>
-          <t>нет данных</t>
-        </is>
-      </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
@@ -1214,32 +740,6 @@
           <t>сер легк</t>
         </is>
       </c>
-      <c r="E19" t="inlineStr">
-        <is>
-          <t>215/65R16C</t>
-        </is>
-      </c>
-      <c r="F19" t="inlineStr">
-        <is>
-          <t>Бел-1000</t>
-        </is>
-      </c>
-      <c r="G19" t="inlineStr">
-        <is>
-          <t>сер, легк</t>
-        </is>
-      </c>
-      <c r="H19" t="n">
-        <v>2</v>
-      </c>
-      <c r="I19" s="1" t="n">
-        <v>45138</v>
-      </c>
-      <c r="J19" t="inlineStr">
-        <is>
-          <t>нет данных</t>
-        </is>
-      </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
@@ -1257,32 +757,6 @@
           <t>сер легк</t>
         </is>
       </c>
-      <c r="E20" t="inlineStr">
-        <is>
-          <t>205/55R16</t>
-        </is>
-      </c>
-      <c r="F20" t="inlineStr">
-        <is>
-          <t>Бел-1001</t>
-        </is>
-      </c>
-      <c r="G20" t="inlineStr">
-        <is>
-          <t>сер, легк</t>
-        </is>
-      </c>
-      <c r="H20" t="n">
-        <v>2</v>
-      </c>
-      <c r="I20" s="1" t="n">
-        <v>45138</v>
-      </c>
-      <c r="J20" t="inlineStr">
-        <is>
-          <t>нет данных</t>
-        </is>
-      </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
@@ -1300,32 +774,6 @@
           <t>сер легк</t>
         </is>
       </c>
-      <c r="E21" t="inlineStr">
-        <is>
-          <t>225/50R17</t>
-        </is>
-      </c>
-      <c r="F21" t="inlineStr">
-        <is>
-          <t>Бел-1005</t>
-        </is>
-      </c>
-      <c r="G21" t="inlineStr">
-        <is>
-          <t>сер, легк</t>
-        </is>
-      </c>
-      <c r="H21" t="n">
-        <v>2</v>
-      </c>
-      <c r="I21" s="1" t="n">
-        <v>45138</v>
-      </c>
-      <c r="J21" t="inlineStr">
-        <is>
-          <t>нет данных</t>
-        </is>
-      </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
@@ -1341,6 +789,23 @@
       <c r="C22" t="inlineStr">
         <is>
           <t>сер легк</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>superDuper</t>
+        </is>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>155/65R13</t>
+        </is>
+      </c>
+      <c r="C23" t="inlineStr">
+        <is>
+          <t>легк</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
chemcurier v.0.9.4 v.1.6 with download at 04/11/2023
</commit_message>
<xml_diff>
--- a/src/Tyres.xlsx
+++ b/src/Tyres.xlsx
@@ -17,7 +17,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="0"/>
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="yyyy-mm-dd"/>
+  </numFmts>
   <fonts count="1">
     <font>
       <name val="Calibri"/>
@@ -47,8 +49,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
@@ -414,7 +417,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C23"/>
+  <dimension ref="A1:J23"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -433,7 +436,36 @@
           <t xml:space="preserve"> </t>
         </is>
       </c>
-      <c r="C1" t="inlineStr"/>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>Tyre Size</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>Model</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
+        <is>
+          <t>Param</t>
+        </is>
+      </c>
+      <c r="H1" t="inlineStr">
+        <is>
+          <t>Sales value</t>
+        </is>
+      </c>
+      <c r="I1" t="inlineStr">
+        <is>
+          <t>Date_of_sales</t>
+        </is>
+      </c>
+      <c r="J1" t="inlineStr">
+        <is>
+          <t>Contragent</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
@@ -451,6 +483,32 @@
           <t>42 30 груз сер</t>
         </is>
       </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>35/65-33</t>
+        </is>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>ФБел-283</t>
+        </is>
+      </c>
+      <c r="G2" t="inlineStr">
+        <is>
+          <t>42, 30, груз, сер</t>
+        </is>
+      </c>
+      <c r="H2" t="n">
+        <v>2</v>
+      </c>
+      <c r="I2" s="1" t="n">
+        <v>45138</v>
+      </c>
+      <c r="J2" t="inlineStr">
+        <is>
+          <t>нет данных</t>
+        </is>
+      </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -468,6 +526,32 @@
           <t>сер легк б/к</t>
         </is>
       </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>205/55R16</t>
+        </is>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>BEL-262</t>
+        </is>
+      </c>
+      <c r="G3" t="inlineStr">
+        <is>
+          <t>сер, легк, б/к</t>
+        </is>
+      </c>
+      <c r="H3" t="n">
+        <v>2</v>
+      </c>
+      <c r="I3" s="1" t="n">
+        <v>45138</v>
+      </c>
+      <c r="J3" t="inlineStr">
+        <is>
+          <t>нет данных</t>
+        </is>
+      </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
@@ -485,6 +569,32 @@
           <t>сер легк б/к</t>
         </is>
       </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>205/55R16</t>
+        </is>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>BEL-317</t>
+        </is>
+      </c>
+      <c r="G4" t="inlineStr">
+        <is>
+          <t>сер, легк, б/к</t>
+        </is>
+      </c>
+      <c r="H4" t="n">
+        <v>2</v>
+      </c>
+      <c r="I4" s="1" t="n">
+        <v>45138</v>
+      </c>
+      <c r="J4" t="inlineStr">
+        <is>
+          <t>нет данных</t>
+        </is>
+      </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
@@ -502,6 +612,32 @@
           <t>ошип сер</t>
         </is>
       </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>205/55R16</t>
+        </is>
+      </c>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>BEL-317S</t>
+        </is>
+      </c>
+      <c r="G5" t="inlineStr">
+        <is>
+          <t>ошип, сер</t>
+        </is>
+      </c>
+      <c r="H5" t="n">
+        <v>2</v>
+      </c>
+      <c r="I5" s="1" t="n">
+        <v>45138</v>
+      </c>
+      <c r="J5" t="inlineStr">
+        <is>
+          <t>нет данных</t>
+        </is>
+      </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
@@ -519,6 +655,32 @@
           <t>сер легк</t>
         </is>
       </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>235/75R15</t>
+        </is>
+      </c>
+      <c r="F6" t="inlineStr">
+        <is>
+          <t>BEL-1001</t>
+        </is>
+      </c>
+      <c r="G6" t="inlineStr">
+        <is>
+          <t>сер, легк</t>
+        </is>
+      </c>
+      <c r="H6" t="n">
+        <v>2</v>
+      </c>
+      <c r="I6" s="1" t="n">
+        <v>45138</v>
+      </c>
+      <c r="J6" t="inlineStr">
+        <is>
+          <t>нет данных</t>
+        </is>
+      </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
@@ -536,6 +698,32 @@
           <t>сер легк</t>
         </is>
       </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>155/65R13</t>
+        </is>
+      </c>
+      <c r="F7" t="inlineStr">
+        <is>
+          <t>BEL-1002</t>
+        </is>
+      </c>
+      <c r="G7" t="inlineStr">
+        <is>
+          <t>сер, легк</t>
+        </is>
+      </c>
+      <c r="H7" t="n">
+        <v>2</v>
+      </c>
+      <c r="I7" s="1" t="n">
+        <v>45138</v>
+      </c>
+      <c r="J7" t="inlineStr">
+        <is>
+          <t>нет данных</t>
+        </is>
+      </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
@@ -553,6 +741,32 @@
           <t>сер легк</t>
         </is>
       </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>205/55R16</t>
+        </is>
+      </c>
+      <c r="F8" t="inlineStr">
+        <is>
+          <t>BEL-1004</t>
+        </is>
+      </c>
+      <c r="G8" t="inlineStr">
+        <is>
+          <t>сер, легк</t>
+        </is>
+      </c>
+      <c r="H8" t="n">
+        <v>2</v>
+      </c>
+      <c r="I8" s="1" t="n">
+        <v>45138</v>
+      </c>
+      <c r="J8" t="inlineStr">
+        <is>
+          <t>нет данных</t>
+        </is>
+      </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
@@ -570,6 +784,32 @@
           <t>сер легк</t>
         </is>
       </c>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>225/50R17</t>
+        </is>
+      </c>
+      <c r="F9" t="inlineStr">
+        <is>
+          <t>BEL-1005</t>
+        </is>
+      </c>
+      <c r="G9" t="inlineStr">
+        <is>
+          <t>сер, легк</t>
+        </is>
+      </c>
+      <c r="H9" t="n">
+        <v>2</v>
+      </c>
+      <c r="I9" s="1" t="n">
+        <v>45138</v>
+      </c>
+      <c r="J9" t="inlineStr">
+        <is>
+          <t>нет данных</t>
+        </is>
+      </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
@@ -587,6 +827,32 @@
           <t>210B H Type C сер</t>
         </is>
       </c>
+      <c r="E10" t="inlineStr">
+        <is>
+          <t>24.00R35</t>
+        </is>
+      </c>
+      <c r="F10" t="inlineStr">
+        <is>
+          <t>Бел-202</t>
+        </is>
+      </c>
+      <c r="G10" t="inlineStr">
+        <is>
+          <t>210B, H, Type, C, сер</t>
+        </is>
+      </c>
+      <c r="H10" t="n">
+        <v>2</v>
+      </c>
+      <c r="I10" s="1" t="n">
+        <v>45138</v>
+      </c>
+      <c r="J10" t="inlineStr">
+        <is>
+          <t>нет данных</t>
+        </is>
+      </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
@@ -604,6 +870,32 @@
           <t>груз Type LS-2 сер</t>
         </is>
       </c>
+      <c r="E11" t="inlineStr">
+        <is>
+          <t>24.00R35</t>
+        </is>
+      </c>
+      <c r="F11" t="inlineStr">
+        <is>
+          <t>Бел-212</t>
+        </is>
+      </c>
+      <c r="G11" t="inlineStr">
+        <is>
+          <t>груз, Type, LS-2, сер</t>
+        </is>
+      </c>
+      <c r="H11" t="n">
+        <v>2</v>
+      </c>
+      <c r="I11" s="1" t="n">
+        <v>45138</v>
+      </c>
+      <c r="J11" t="inlineStr">
+        <is>
+          <t>нет данных</t>
+        </is>
+      </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
@@ -621,6 +913,32 @@
           <t>202B Type C сер</t>
         </is>
       </c>
+      <c r="E12" t="inlineStr">
+        <is>
+          <t>21.00R35</t>
+        </is>
+      </c>
+      <c r="F12" t="inlineStr">
+        <is>
+          <t>Бел-200</t>
+        </is>
+      </c>
+      <c r="G12" t="inlineStr">
+        <is>
+          <t>202B, Type, C, сер</t>
+        </is>
+      </c>
+      <c r="H12" t="n">
+        <v>2</v>
+      </c>
+      <c r="I12" s="1" t="n">
+        <v>45138</v>
+      </c>
+      <c r="J12" t="inlineStr">
+        <is>
+          <t>нет данных</t>
+        </is>
+      </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
@@ -638,6 +956,32 @@
           <t>202B H Type LS-2 C сер</t>
         </is>
       </c>
+      <c r="E13" t="inlineStr">
+        <is>
+          <t>21.00R35</t>
+        </is>
+      </c>
+      <c r="F13" t="inlineStr">
+        <is>
+          <t>Бел-210</t>
+        </is>
+      </c>
+      <c r="G13" t="inlineStr">
+        <is>
+          <t>202B, H, Type, LS-2, C, сер</t>
+        </is>
+      </c>
+      <c r="H13" t="n">
+        <v>2</v>
+      </c>
+      <c r="I13" s="1" t="n">
+        <v>45138</v>
+      </c>
+      <c r="J13" t="inlineStr">
+        <is>
+          <t>нет данных</t>
+        </is>
+      </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
@@ -655,6 +999,32 @@
           <t>груз сер б/к</t>
         </is>
       </c>
+      <c r="E14" t="inlineStr">
+        <is>
+          <t>14.00R20</t>
+        </is>
+      </c>
+      <c r="F14" t="inlineStr">
+        <is>
+          <t>BEL-248</t>
+        </is>
+      </c>
+      <c r="G14" t="inlineStr">
+        <is>
+          <t>груз, сер, б/к</t>
+        </is>
+      </c>
+      <c r="H14" t="n">
+        <v>2</v>
+      </c>
+      <c r="I14" s="1" t="n">
+        <v>45138</v>
+      </c>
+      <c r="J14" t="inlineStr">
+        <is>
+          <t>нет данных</t>
+        </is>
+      </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
@@ -672,6 +1042,32 @@
           <t>сер легк б/к</t>
         </is>
       </c>
+      <c r="E15" t="inlineStr">
+        <is>
+          <t>175/70R13</t>
+        </is>
+      </c>
+      <c r="F15" t="inlineStr">
+        <is>
+          <t>Бел-103</t>
+        </is>
+      </c>
+      <c r="G15" t="inlineStr">
+        <is>
+          <t>сер, легк, б/к</t>
+        </is>
+      </c>
+      <c r="H15" t="n">
+        <v>2</v>
+      </c>
+      <c r="I15" s="1" t="n">
+        <v>45138</v>
+      </c>
+      <c r="J15" t="inlineStr">
+        <is>
+          <t>нет данных</t>
+        </is>
+      </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
@@ -689,6 +1085,32 @@
           <t>сер легк б/к</t>
         </is>
       </c>
+      <c r="E16" t="inlineStr">
+        <is>
+          <t>175/70R13</t>
+        </is>
+      </c>
+      <c r="F16" t="inlineStr">
+        <is>
+          <t>Бел-100</t>
+        </is>
+      </c>
+      <c r="G16" t="inlineStr">
+        <is>
+          <t>сер, легк, б/к</t>
+        </is>
+      </c>
+      <c r="H16" t="n">
+        <v>2</v>
+      </c>
+      <c r="I16" s="1" t="n">
+        <v>45138</v>
+      </c>
+      <c r="J16" t="inlineStr">
+        <is>
+          <t>нет данных</t>
+        </is>
+      </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
@@ -706,6 +1128,32 @@
           <t>8 сх сер</t>
         </is>
       </c>
+      <c r="E17" t="inlineStr">
+        <is>
+          <t>195/65R15</t>
+        </is>
+      </c>
+      <c r="F17" t="inlineStr">
+        <is>
+          <t>Бел-119</t>
+        </is>
+      </c>
+      <c r="G17" t="inlineStr">
+        <is>
+          <t>сер, легк</t>
+        </is>
+      </c>
+      <c r="H17" t="n">
+        <v>2</v>
+      </c>
+      <c r="I17" s="1" t="n">
+        <v>45138</v>
+      </c>
+      <c r="J17" t="inlineStr">
+        <is>
+          <t>нет данных</t>
+        </is>
+      </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
@@ -723,6 +1171,32 @@
           <t>сер легк</t>
         </is>
       </c>
+      <c r="E18" t="inlineStr">
+        <is>
+          <t>210/80R16</t>
+        </is>
+      </c>
+      <c r="F18" t="inlineStr">
+        <is>
+          <t>Бел-777</t>
+        </is>
+      </c>
+      <c r="G18" t="inlineStr">
+        <is>
+          <t>сер, легк</t>
+        </is>
+      </c>
+      <c r="H18" t="n">
+        <v>2</v>
+      </c>
+      <c r="I18" s="1" t="n">
+        <v>45138</v>
+      </c>
+      <c r="J18" t="inlineStr">
+        <is>
+          <t>нет данных</t>
+        </is>
+      </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
@@ -740,6 +1214,32 @@
           <t>сер легк</t>
         </is>
       </c>
+      <c r="E19" t="inlineStr">
+        <is>
+          <t>215/65R16C</t>
+        </is>
+      </c>
+      <c r="F19" t="inlineStr">
+        <is>
+          <t>Бел-1000</t>
+        </is>
+      </c>
+      <c r="G19" t="inlineStr">
+        <is>
+          <t>сер, легк</t>
+        </is>
+      </c>
+      <c r="H19" t="n">
+        <v>2</v>
+      </c>
+      <c r="I19" s="1" t="n">
+        <v>45138</v>
+      </c>
+      <c r="J19" t="inlineStr">
+        <is>
+          <t>нет данных</t>
+        </is>
+      </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
@@ -757,6 +1257,32 @@
           <t>сер легк</t>
         </is>
       </c>
+      <c r="E20" t="inlineStr">
+        <is>
+          <t>205/55R16</t>
+        </is>
+      </c>
+      <c r="F20" t="inlineStr">
+        <is>
+          <t>Бел-1001</t>
+        </is>
+      </c>
+      <c r="G20" t="inlineStr">
+        <is>
+          <t>сер, легк</t>
+        </is>
+      </c>
+      <c r="H20" t="n">
+        <v>2</v>
+      </c>
+      <c r="I20" s="1" t="n">
+        <v>45138</v>
+      </c>
+      <c r="J20" t="inlineStr">
+        <is>
+          <t>нет данных</t>
+        </is>
+      </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
@@ -772,6 +1298,32 @@
       <c r="C21" t="inlineStr">
         <is>
           <t>сер легк</t>
+        </is>
+      </c>
+      <c r="E21" t="inlineStr">
+        <is>
+          <t>225/50R17</t>
+        </is>
+      </c>
+      <c r="F21" t="inlineStr">
+        <is>
+          <t>Бел-1005</t>
+        </is>
+      </c>
+      <c r="G21" t="inlineStr">
+        <is>
+          <t>сер, легк</t>
+        </is>
+      </c>
+      <c r="H21" t="n">
+        <v>2</v>
+      </c>
+      <c r="I21" s="1" t="n">
+        <v>45138</v>
+      </c>
+      <c r="J21" t="inlineStr">
+        <is>
+          <t>нет данных</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
after second total system crash recovery at 14/11/2023
</commit_message>
<xml_diff>
--- a/src/Tyres.xlsx
+++ b/src/Tyres.xlsx
@@ -417,7 +417,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J23"/>
+  <dimension ref="A1:J22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -480,7 +480,7 @@
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>42 30 груз сер</t>
+          <t>42 груз сер</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
@@ -495,14 +495,14 @@
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>42, 30, груз, сер</t>
+          <t>42, груз, сер</t>
         </is>
       </c>
       <c r="H2" t="n">
         <v>2</v>
       </c>
       <c r="I2" s="1" t="n">
-        <v>45138</v>
+        <v>45244</v>
       </c>
       <c r="J2" t="inlineStr">
         <is>
@@ -513,39 +513,39 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
+          <t>Бел-122</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>24.00R35</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>груз C сер H Type LS-2</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>205/55R16</t>
+        </is>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
           <t>BEL-262</t>
         </is>
       </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>205/55R16</t>
-        </is>
-      </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>сер легк б/к</t>
-        </is>
-      </c>
-      <c r="E3" t="inlineStr">
-        <is>
-          <t>205/55R16</t>
-        </is>
-      </c>
-      <c r="F3" t="inlineStr">
-        <is>
-          <t>BEL-262</t>
-        </is>
-      </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>сер, легк, б/к</t>
+          <t>б/к, сер, легк</t>
         </is>
       </c>
       <c r="H3" t="n">
         <v>2</v>
       </c>
       <c r="I3" s="1" t="n">
-        <v>45138</v>
+        <v>45244</v>
       </c>
       <c r="J3" t="inlineStr">
         <is>
@@ -556,39 +556,39 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
+          <t>Бел-202</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>24.00R35</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>210B C сер H Type LS-2</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>205/55R16</t>
+        </is>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
           <t>BEL-317</t>
         </is>
       </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>205/55R16</t>
-        </is>
-      </c>
-      <c r="C4" t="inlineStr">
-        <is>
-          <t>сер легк б/к</t>
-        </is>
-      </c>
-      <c r="E4" t="inlineStr">
-        <is>
-          <t>205/55R16</t>
-        </is>
-      </c>
-      <c r="F4" t="inlineStr">
-        <is>
-          <t>BEL-317</t>
-        </is>
-      </c>
       <c r="G4" t="inlineStr">
         <is>
-          <t>сер, легк, б/к</t>
+          <t>б/к, сер, легк</t>
         </is>
       </c>
       <c r="H4" t="n">
         <v>2</v>
       </c>
       <c r="I4" s="1" t="n">
-        <v>45138</v>
+        <v>45244</v>
       </c>
       <c r="J4" t="inlineStr">
         <is>
@@ -599,39 +599,39 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
+          <t>Бел-212</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>24.00R35</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>груз C сер H Type LS-2</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>205/55R16</t>
+        </is>
+      </c>
+      <c r="F5" t="inlineStr">
+        <is>
           <t>BEL-317S</t>
         </is>
       </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>205/55R16</t>
-        </is>
-      </c>
-      <c r="C5" t="inlineStr">
-        <is>
-          <t>ошип сер</t>
-        </is>
-      </c>
-      <c r="E5" t="inlineStr">
-        <is>
-          <t>205/55R16</t>
-        </is>
-      </c>
-      <c r="F5" t="inlineStr">
-        <is>
-          <t>BEL-317S</t>
-        </is>
-      </c>
       <c r="G5" t="inlineStr">
         <is>
-          <t>ошип, сер</t>
+          <t>сер, ошип</t>
         </is>
       </c>
       <c r="H5" t="n">
         <v>2</v>
       </c>
       <c r="I5" s="1" t="n">
-        <v>45138</v>
+        <v>45244</v>
       </c>
       <c r="J5" t="inlineStr">
         <is>
@@ -642,39 +642,39 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>BEL-1001</t>
+          <t>Бел-200</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>235/75R15</t>
+          <t>21.00R35</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>сер легк</t>
+          <t>202B C сер H Type LS-2</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>235/75R15</t>
+          <t>24.00R35</t>
         </is>
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>BEL-1001</t>
+          <t>Бел-202</t>
         </is>
       </c>
       <c r="G6" t="inlineStr">
         <is>
-          <t>сер, легк</t>
+          <t>210B, C, сер, H, Type, LS-2</t>
         </is>
       </c>
       <c r="H6" t="n">
         <v>2</v>
       </c>
       <c r="I6" s="1" t="n">
-        <v>45138</v>
+        <v>45244</v>
       </c>
       <c r="J6" t="inlineStr">
         <is>
@@ -685,39 +685,39 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>BEL-1002</t>
+          <t>Бел-210</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>155/65R13</t>
+          <t>21.00R35</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>сер легк</t>
+          <t>202B C сер H Type LS-2</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>155/65R13</t>
+          <t>24.00R35</t>
         </is>
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>BEL-1002</t>
+          <t>Бел-212</t>
         </is>
       </c>
       <c r="G7" t="inlineStr">
         <is>
-          <t>сер, легк</t>
+          <t>груз, C, сер, H, Type, LS-2</t>
         </is>
       </c>
       <c r="H7" t="n">
         <v>2</v>
       </c>
       <c r="I7" s="1" t="n">
-        <v>45138</v>
+        <v>45244</v>
       </c>
       <c r="J7" t="inlineStr">
         <is>
@@ -728,39 +728,39 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>BEL-1004</t>
+          <t>BEL-248</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>205/55R16</t>
+          <t>14.00R20</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>сер легк</t>
+          <t>б/к груз сер</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>205/55R16</t>
+          <t>21.00R35</t>
         </is>
       </c>
       <c r="F8" t="inlineStr">
         <is>
-          <t>BEL-1004</t>
+          <t>Бел-200</t>
         </is>
       </c>
       <c r="G8" t="inlineStr">
         <is>
-          <t>сер, легк</t>
+          <t>202B, C, сер, H, Type, LS-2</t>
         </is>
       </c>
       <c r="H8" t="n">
         <v>2</v>
       </c>
       <c r="I8" s="1" t="n">
-        <v>45138</v>
+        <v>45244</v>
       </c>
       <c r="J8" t="inlineStr">
         <is>
@@ -771,39 +771,39 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>BEL-1005</t>
+          <t>BEL-288</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>225/50R17</t>
+          <t>12.00R20</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>сер легк</t>
+          <t>груз сер</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>225/50R17</t>
+          <t>21.00R35</t>
         </is>
       </c>
       <c r="F9" t="inlineStr">
         <is>
-          <t>BEL-1005</t>
+          <t>Бел-210</t>
         </is>
       </c>
       <c r="G9" t="inlineStr">
         <is>
-          <t>сер, легк</t>
+          <t>202B, C, сер, H, Type, LS-2</t>
         </is>
       </c>
       <c r="H9" t="n">
         <v>2</v>
       </c>
       <c r="I9" s="1" t="n">
-        <v>45138</v>
+        <v>45244</v>
       </c>
       <c r="J9" t="inlineStr">
         <is>
@@ -814,39 +814,39 @@
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>Бел-202</t>
+          <t>Бел-95</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>24.00R35</t>
+          <t>16.00R20</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>210B H Type C сер</t>
+          <t>173G б/к груз сер</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>24.00R35</t>
+          <t>14.00R20</t>
         </is>
       </c>
       <c r="F10" t="inlineStr">
         <is>
-          <t>Бел-202</t>
+          <t>BEL-248</t>
         </is>
       </c>
       <c r="G10" t="inlineStr">
         <is>
-          <t>210B, H, Type, C, сер</t>
+          <t>б/к, груз, сер</t>
         </is>
       </c>
       <c r="H10" t="n">
         <v>2</v>
       </c>
       <c r="I10" s="1" t="n">
-        <v>45138</v>
+        <v>45244</v>
       </c>
       <c r="J10" t="inlineStr">
         <is>
@@ -857,39 +857,39 @@
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>Бел-212</t>
+          <t>BEL-405</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>24.00R35</t>
+          <t>395/85R20</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>груз Type LS-2 сер</t>
+          <t>168J груз сер</t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>24.00R35</t>
+          <t>175/70R13</t>
         </is>
       </c>
       <c r="F11" t="inlineStr">
         <is>
-          <t>Бел-212</t>
+          <t>Бел-103</t>
         </is>
       </c>
       <c r="G11" t="inlineStr">
         <is>
-          <t>груз, Type, LS-2, сер</t>
+          <t>б/к, сер, легк</t>
         </is>
       </c>
       <c r="H11" t="n">
         <v>2</v>
       </c>
       <c r="I11" s="1" t="n">
-        <v>45138</v>
+        <v>45244</v>
       </c>
       <c r="J11" t="inlineStr">
         <is>
@@ -900,39 +900,39 @@
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>Бел-200</t>
+          <t>Бел-145</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>21.00R35</t>
+          <t>445/65R22.5</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>202B Type C сер</t>
+          <t>б/к груз сер</t>
         </is>
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>21.00R35</t>
+          <t>175/70R13</t>
         </is>
       </c>
       <c r="F12" t="inlineStr">
         <is>
-          <t>Бел-200</t>
+          <t>Бел-100</t>
         </is>
       </c>
       <c r="G12" t="inlineStr">
         <is>
-          <t>202B, Type, C, сер</t>
+          <t>б/к, сер, легк</t>
         </is>
       </c>
       <c r="H12" t="n">
         <v>2</v>
       </c>
       <c r="I12" s="1" t="n">
-        <v>45138</v>
+        <v>45244</v>
       </c>
       <c r="J12" t="inlineStr">
         <is>
@@ -943,39 +943,39 @@
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>Бел-210</t>
+          <t>Бел-230</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>21.00R35</t>
+          <t>355/65-15</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>202B H Type LS-2 C сер</t>
+          <t>сер</t>
         </is>
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>21.00R35</t>
+          <t>195/65R15</t>
         </is>
       </c>
       <c r="F13" t="inlineStr">
         <is>
-          <t>Бел-210</t>
+          <t>Бел-119</t>
         </is>
       </c>
       <c r="G13" t="inlineStr">
         <is>
-          <t>202B, H, Type, LS-2, C, сер</t>
+          <t>сер, легк</t>
         </is>
       </c>
       <c r="H13" t="n">
         <v>2</v>
       </c>
       <c r="I13" s="1" t="n">
-        <v>45138</v>
+        <v>45244</v>
       </c>
       <c r="J13" t="inlineStr">
         <is>
@@ -986,378 +986,153 @@
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>BEL-248</t>
+          <t>Бел-230М</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>14.00R20</t>
+          <t>355/65-15</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>груз сер б/к</t>
-        </is>
-      </c>
-      <c r="E14" t="inlineStr">
-        <is>
-          <t>14.00R20</t>
-        </is>
-      </c>
-      <c r="F14" t="inlineStr">
-        <is>
-          <t>BEL-248</t>
-        </is>
-      </c>
-      <c r="G14" t="inlineStr">
-        <is>
-          <t>груз, сер, б/к</t>
-        </is>
-      </c>
-      <c r="H14" t="n">
-        <v>2</v>
-      </c>
-      <c r="I14" s="1" t="n">
-        <v>45138</v>
-      </c>
-      <c r="J14" t="inlineStr">
-        <is>
-          <t>нет данных</t>
+          <t>сер</t>
         </is>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>Бел-103</t>
+          <t>BEL-262</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>175/70R13</t>
+          <t>205/55R16</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>сер легк б/к</t>
-        </is>
-      </c>
-      <c r="E15" t="inlineStr">
-        <is>
-          <t>175/70R13</t>
-        </is>
-      </c>
-      <c r="F15" t="inlineStr">
-        <is>
-          <t>Бел-103</t>
-        </is>
-      </c>
-      <c r="G15" t="inlineStr">
-        <is>
-          <t>сер, легк, б/к</t>
-        </is>
-      </c>
-      <c r="H15" t="n">
-        <v>2</v>
-      </c>
-      <c r="I15" s="1" t="n">
-        <v>45138</v>
-      </c>
-      <c r="J15" t="inlineStr">
-        <is>
-          <t>нет данных</t>
+          <t>б/к сер легк</t>
         </is>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>Бел-100</t>
+          <t>BEL-317</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>175/70R13</t>
+          <t>205/55R16</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>сер легк б/к</t>
-        </is>
-      </c>
-      <c r="E16" t="inlineStr">
-        <is>
-          <t>175/70R13</t>
-        </is>
-      </c>
-      <c r="F16" t="inlineStr">
-        <is>
-          <t>Бел-100</t>
-        </is>
-      </c>
-      <c r="G16" t="inlineStr">
-        <is>
-          <t>сер, легк, б/к</t>
-        </is>
-      </c>
-      <c r="H16" t="n">
-        <v>2</v>
-      </c>
-      <c r="I16" s="1" t="n">
-        <v>45138</v>
-      </c>
-      <c r="J16" t="inlineStr">
-        <is>
-          <t>нет данных</t>
+          <t>б/к сер легк</t>
         </is>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>Ф-35-1</t>
+          <t>BEL-317S</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>11.2-20</t>
+          <t>205/55R16</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>8 сх сер</t>
-        </is>
-      </c>
-      <c r="E17" t="inlineStr">
-        <is>
-          <t>195/65R15</t>
-        </is>
-      </c>
-      <c r="F17" t="inlineStr">
-        <is>
-          <t>Бел-119</t>
-        </is>
-      </c>
-      <c r="G17" t="inlineStr">
-        <is>
-          <t>сер, легк</t>
-        </is>
-      </c>
-      <c r="H17" t="n">
-        <v>2</v>
-      </c>
-      <c r="I17" s="1" t="n">
-        <v>45138</v>
-      </c>
-      <c r="J17" t="inlineStr">
-        <is>
-          <t>нет данных</t>
+          <t>сер ошип</t>
         </is>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>Бел-119</t>
+          <t>BEL-277</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>195/65R15</t>
+          <t>205/60R16</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>сер легк</t>
-        </is>
-      </c>
-      <c r="E18" t="inlineStr">
-        <is>
-          <t>210/80R16</t>
-        </is>
-      </c>
-      <c r="F18" t="inlineStr">
-        <is>
-          <t>Бел-777</t>
-        </is>
-      </c>
-      <c r="G18" t="inlineStr">
-        <is>
-          <t>сер, легк</t>
-        </is>
-      </c>
-      <c r="H18" t="n">
-        <v>2</v>
-      </c>
-      <c r="I18" s="1" t="n">
-        <v>45138</v>
-      </c>
-      <c r="J18" t="inlineStr">
-        <is>
-          <t>нет данных</t>
+          <t>б/к сер легк</t>
         </is>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>Бел-777</t>
+          <t>Бел-103</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>210/80R16</t>
+          <t>175/70R13</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>сер легк</t>
-        </is>
-      </c>
-      <c r="E19" t="inlineStr">
-        <is>
-          <t>215/65R16C</t>
-        </is>
-      </c>
-      <c r="F19" t="inlineStr">
-        <is>
-          <t>Бел-1000</t>
-        </is>
-      </c>
-      <c r="G19" t="inlineStr">
-        <is>
-          <t>сер, легк</t>
-        </is>
-      </c>
-      <c r="H19" t="n">
-        <v>2</v>
-      </c>
-      <c r="I19" s="1" t="n">
-        <v>45138</v>
-      </c>
-      <c r="J19" t="inlineStr">
-        <is>
-          <t>нет данных</t>
+          <t>б/к сер легк</t>
         </is>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>Бел-1000</t>
+          <t>Бел-100</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>215/65R16C</t>
+          <t>175/70R13</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>сер легк</t>
-        </is>
-      </c>
-      <c r="E20" t="inlineStr">
-        <is>
-          <t>205/55R16</t>
-        </is>
-      </c>
-      <c r="F20" t="inlineStr">
-        <is>
-          <t>Бел-1001</t>
-        </is>
-      </c>
-      <c r="G20" t="inlineStr">
-        <is>
-          <t>сер, легк</t>
-        </is>
-      </c>
-      <c r="H20" t="n">
-        <v>2</v>
-      </c>
-      <c r="I20" s="1" t="n">
-        <v>45138</v>
-      </c>
-      <c r="J20" t="inlineStr">
-        <is>
-          <t>нет данных</t>
+          <t>б/к сер легк</t>
         </is>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>Бел-1001</t>
+          <t>Ф-35-1</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>205/55R16</t>
+          <t>11.2-20</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>сер легк</t>
-        </is>
-      </c>
-      <c r="E21" t="inlineStr">
-        <is>
-          <t>225/50R17</t>
-        </is>
-      </c>
-      <c r="F21" t="inlineStr">
-        <is>
-          <t>Бел-1005</t>
-        </is>
-      </c>
-      <c r="G21" t="inlineStr">
-        <is>
-          <t>сер, легк</t>
-        </is>
-      </c>
-      <c r="H21" t="n">
-        <v>2</v>
-      </c>
-      <c r="I21" s="1" t="n">
-        <v>45138</v>
-      </c>
-      <c r="J21" t="inlineStr">
-        <is>
-          <t>нет данных</t>
+          <t>8 168J сх сер</t>
         </is>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>Бел-1005</t>
+          <t>Бел-119</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>225/50R17</t>
+          <t>195/65R15</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
         <is>
           <t>сер легк</t>
-        </is>
-      </c>
-    </row>
-    <row r="23">
-      <c r="A23" t="inlineStr">
-        <is>
-          <t>superDuper</t>
-        </is>
-      </c>
-      <c r="B23" t="inlineStr">
-        <is>
-          <t>155/65R13</t>
-        </is>
-      </c>
-      <c r="C23" t="inlineStr">
-        <is>
-          <t>легк</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
10.02/2024 - return to host 12
</commit_message>
<xml_diff>
--- a/src/Tyres.xlsx
+++ b/src/Tyres.xlsx
@@ -417,7 +417,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J22"/>
+  <dimension ref="A1:J41"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1341,6 +1341,564 @@
       <c r="C22" t="inlineStr">
         <is>
           <t>легк сер</t>
+        </is>
+      </c>
+      <c r="E22" t="inlineStr">
+        <is>
+          <t>35/65-33</t>
+        </is>
+      </c>
+      <c r="F22" t="inlineStr">
+        <is>
+          <t>ФБел-283</t>
+        </is>
+      </c>
+      <c r="G22" t="inlineStr">
+        <is>
+          <t>42, 30, груз, сер</t>
+        </is>
+      </c>
+      <c r="H22" t="n">
+        <v>2</v>
+      </c>
+      <c r="I22" s="1" t="n">
+        <v>45335</v>
+      </c>
+      <c r="J22" t="inlineStr">
+        <is>
+          <t>нет данных</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="E23" t="inlineStr">
+        <is>
+          <t>205/55R16</t>
+        </is>
+      </c>
+      <c r="F23" t="inlineStr">
+        <is>
+          <t>BEL-262</t>
+        </is>
+      </c>
+      <c r="G23" t="inlineStr">
+        <is>
+          <t>легк, сер, б/к</t>
+        </is>
+      </c>
+      <c r="H23" t="n">
+        <v>2</v>
+      </c>
+      <c r="I23" s="1" t="n">
+        <v>45335</v>
+      </c>
+      <c r="J23" t="inlineStr">
+        <is>
+          <t>нет данных</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="E24" t="inlineStr">
+        <is>
+          <t>205/55R16</t>
+        </is>
+      </c>
+      <c r="F24" t="inlineStr">
+        <is>
+          <t>BEL-317</t>
+        </is>
+      </c>
+      <c r="G24" t="inlineStr">
+        <is>
+          <t>легк, сер, б/к</t>
+        </is>
+      </c>
+      <c r="H24" t="n">
+        <v>2</v>
+      </c>
+      <c r="I24" s="1" t="n">
+        <v>45335</v>
+      </c>
+      <c r="J24" t="inlineStr">
+        <is>
+          <t>нет данных</t>
+        </is>
+      </c>
+    </row>
+    <row r="25">
+      <c r="E25" t="inlineStr">
+        <is>
+          <t>205/55R16</t>
+        </is>
+      </c>
+      <c r="F25" t="inlineStr">
+        <is>
+          <t>BEL-317S</t>
+        </is>
+      </c>
+      <c r="G25" t="inlineStr">
+        <is>
+          <t>сер, ошип</t>
+        </is>
+      </c>
+      <c r="H25" t="n">
+        <v>2</v>
+      </c>
+      <c r="I25" s="1" t="n">
+        <v>45335</v>
+      </c>
+      <c r="J25" t="inlineStr">
+        <is>
+          <t>нет данных</t>
+        </is>
+      </c>
+    </row>
+    <row r="26">
+      <c r="E26" t="inlineStr">
+        <is>
+          <t>235/75R15</t>
+        </is>
+      </c>
+      <c r="F26" t="inlineStr">
+        <is>
+          <t>BEL-1001</t>
+        </is>
+      </c>
+      <c r="G26" t="inlineStr">
+        <is>
+          <t>легк, сер</t>
+        </is>
+      </c>
+      <c r="H26" t="n">
+        <v>2</v>
+      </c>
+      <c r="I26" s="1" t="n">
+        <v>45335</v>
+      </c>
+      <c r="J26" t="inlineStr">
+        <is>
+          <t>нет данных</t>
+        </is>
+      </c>
+    </row>
+    <row r="27">
+      <c r="E27" t="inlineStr">
+        <is>
+          <t>155/65R13</t>
+        </is>
+      </c>
+      <c r="F27" t="inlineStr">
+        <is>
+          <t>BEL-1002</t>
+        </is>
+      </c>
+      <c r="G27" t="inlineStr">
+        <is>
+          <t>легк, сер</t>
+        </is>
+      </c>
+      <c r="H27" t="n">
+        <v>2</v>
+      </c>
+      <c r="I27" s="1" t="n">
+        <v>45335</v>
+      </c>
+      <c r="J27" t="inlineStr">
+        <is>
+          <t>нет данных</t>
+        </is>
+      </c>
+    </row>
+    <row r="28">
+      <c r="E28" t="inlineStr">
+        <is>
+          <t>205/55R16</t>
+        </is>
+      </c>
+      <c r="F28" t="inlineStr">
+        <is>
+          <t>BEL-1004</t>
+        </is>
+      </c>
+      <c r="G28" t="inlineStr">
+        <is>
+          <t>легк, сер</t>
+        </is>
+      </c>
+      <c r="H28" t="n">
+        <v>2</v>
+      </c>
+      <c r="I28" s="1" t="n">
+        <v>45335</v>
+      </c>
+      <c r="J28" t="inlineStr">
+        <is>
+          <t>нет данных</t>
+        </is>
+      </c>
+    </row>
+    <row r="29">
+      <c r="E29" t="inlineStr">
+        <is>
+          <t>225/50R17</t>
+        </is>
+      </c>
+      <c r="F29" t="inlineStr">
+        <is>
+          <t>BEL-1005</t>
+        </is>
+      </c>
+      <c r="G29" t="inlineStr">
+        <is>
+          <t>легк, сер</t>
+        </is>
+      </c>
+      <c r="H29" t="n">
+        <v>2</v>
+      </c>
+      <c r="I29" s="1" t="n">
+        <v>45335</v>
+      </c>
+      <c r="J29" t="inlineStr">
+        <is>
+          <t>нет данных</t>
+        </is>
+      </c>
+    </row>
+    <row r="30">
+      <c r="E30" t="inlineStr">
+        <is>
+          <t>24.00R35</t>
+        </is>
+      </c>
+      <c r="F30" t="inlineStr">
+        <is>
+          <t>Бел-202</t>
+        </is>
+      </c>
+      <c r="G30" t="inlineStr">
+        <is>
+          <t>210B, Type, сер, C, H</t>
+        </is>
+      </c>
+      <c r="H30" t="n">
+        <v>2</v>
+      </c>
+      <c r="I30" s="1" t="n">
+        <v>45335</v>
+      </c>
+      <c r="J30" t="inlineStr">
+        <is>
+          <t>нет данных</t>
+        </is>
+      </c>
+    </row>
+    <row r="31">
+      <c r="E31" t="inlineStr">
+        <is>
+          <t>24.00R35</t>
+        </is>
+      </c>
+      <c r="F31" t="inlineStr">
+        <is>
+          <t>Бел-212</t>
+        </is>
+      </c>
+      <c r="G31" t="inlineStr">
+        <is>
+          <t>груз, Type, сер, LS-2</t>
+        </is>
+      </c>
+      <c r="H31" t="n">
+        <v>2</v>
+      </c>
+      <c r="I31" s="1" t="n">
+        <v>45335</v>
+      </c>
+      <c r="J31" t="inlineStr">
+        <is>
+          <t>нет данных</t>
+        </is>
+      </c>
+    </row>
+    <row r="32">
+      <c r="E32" t="inlineStr">
+        <is>
+          <t>21.00R35</t>
+        </is>
+      </c>
+      <c r="F32" t="inlineStr">
+        <is>
+          <t>Бел-200</t>
+        </is>
+      </c>
+      <c r="G32" t="inlineStr">
+        <is>
+          <t>202B, Type, сер, C</t>
+        </is>
+      </c>
+      <c r="H32" t="n">
+        <v>2</v>
+      </c>
+      <c r="I32" s="1" t="n">
+        <v>45335</v>
+      </c>
+      <c r="J32" t="inlineStr">
+        <is>
+          <t>нет данных</t>
+        </is>
+      </c>
+    </row>
+    <row r="33">
+      <c r="E33" t="inlineStr">
+        <is>
+          <t>21.00R35</t>
+        </is>
+      </c>
+      <c r="F33" t="inlineStr">
+        <is>
+          <t>Бел-210</t>
+        </is>
+      </c>
+      <c r="G33" t="inlineStr">
+        <is>
+          <t>202B, Type, сер, C, H, LS-2</t>
+        </is>
+      </c>
+      <c r="H33" t="n">
+        <v>2</v>
+      </c>
+      <c r="I33" s="1" t="n">
+        <v>45335</v>
+      </c>
+      <c r="J33" t="inlineStr">
+        <is>
+          <t>нет данных</t>
+        </is>
+      </c>
+    </row>
+    <row r="34">
+      <c r="E34" t="inlineStr">
+        <is>
+          <t>14.00R20</t>
+        </is>
+      </c>
+      <c r="F34" t="inlineStr">
+        <is>
+          <t>BEL-248</t>
+        </is>
+      </c>
+      <c r="G34" t="inlineStr">
+        <is>
+          <t>груз, сер, б/к</t>
+        </is>
+      </c>
+      <c r="H34" t="n">
+        <v>2</v>
+      </c>
+      <c r="I34" s="1" t="n">
+        <v>45335</v>
+      </c>
+      <c r="J34" t="inlineStr">
+        <is>
+          <t>нет данных</t>
+        </is>
+      </c>
+    </row>
+    <row r="35">
+      <c r="E35" t="inlineStr">
+        <is>
+          <t>175/70R13</t>
+        </is>
+      </c>
+      <c r="F35" t="inlineStr">
+        <is>
+          <t>Бел-103</t>
+        </is>
+      </c>
+      <c r="G35" t="inlineStr">
+        <is>
+          <t>легк, сер, б/к</t>
+        </is>
+      </c>
+      <c r="H35" t="n">
+        <v>2</v>
+      </c>
+      <c r="I35" s="1" t="n">
+        <v>45335</v>
+      </c>
+      <c r="J35" t="inlineStr">
+        <is>
+          <t>нет данных</t>
+        </is>
+      </c>
+    </row>
+    <row r="36">
+      <c r="E36" t="inlineStr">
+        <is>
+          <t>175/70R13</t>
+        </is>
+      </c>
+      <c r="F36" t="inlineStr">
+        <is>
+          <t>Бел-100</t>
+        </is>
+      </c>
+      <c r="G36" t="inlineStr">
+        <is>
+          <t>легк, сер, б/к</t>
+        </is>
+      </c>
+      <c r="H36" t="n">
+        <v>2</v>
+      </c>
+      <c r="I36" s="1" t="n">
+        <v>45335</v>
+      </c>
+      <c r="J36" t="inlineStr">
+        <is>
+          <t>нет данных</t>
+        </is>
+      </c>
+    </row>
+    <row r="37">
+      <c r="E37" t="inlineStr">
+        <is>
+          <t>195/65R15</t>
+        </is>
+      </c>
+      <c r="F37" t="inlineStr">
+        <is>
+          <t>Бел-119</t>
+        </is>
+      </c>
+      <c r="G37" t="inlineStr">
+        <is>
+          <t>легк, сер</t>
+        </is>
+      </c>
+      <c r="H37" t="n">
+        <v>2</v>
+      </c>
+      <c r="I37" s="1" t="n">
+        <v>45335</v>
+      </c>
+      <c r="J37" t="inlineStr">
+        <is>
+          <t>нет данных</t>
+        </is>
+      </c>
+    </row>
+    <row r="38">
+      <c r="E38" t="inlineStr">
+        <is>
+          <t>210/80R16</t>
+        </is>
+      </c>
+      <c r="F38" t="inlineStr">
+        <is>
+          <t>Бел-777</t>
+        </is>
+      </c>
+      <c r="G38" t="inlineStr">
+        <is>
+          <t>легк, сер</t>
+        </is>
+      </c>
+      <c r="H38" t="n">
+        <v>2</v>
+      </c>
+      <c r="I38" s="1" t="n">
+        <v>45335</v>
+      </c>
+      <c r="J38" t="inlineStr">
+        <is>
+          <t>нет данных</t>
+        </is>
+      </c>
+    </row>
+    <row r="39">
+      <c r="E39" t="inlineStr">
+        <is>
+          <t>215/65R16C</t>
+        </is>
+      </c>
+      <c r="F39" t="inlineStr">
+        <is>
+          <t>Бел-1000</t>
+        </is>
+      </c>
+      <c r="G39" t="inlineStr">
+        <is>
+          <t>легк, сер</t>
+        </is>
+      </c>
+      <c r="H39" t="n">
+        <v>2</v>
+      </c>
+      <c r="I39" s="1" t="n">
+        <v>45335</v>
+      </c>
+      <c r="J39" t="inlineStr">
+        <is>
+          <t>нет данных</t>
+        </is>
+      </c>
+    </row>
+    <row r="40">
+      <c r="E40" t="inlineStr">
+        <is>
+          <t>205/55R16</t>
+        </is>
+      </c>
+      <c r="F40" t="inlineStr">
+        <is>
+          <t>Бел-1001</t>
+        </is>
+      </c>
+      <c r="G40" t="inlineStr">
+        <is>
+          <t>легк, сер</t>
+        </is>
+      </c>
+      <c r="H40" t="n">
+        <v>2</v>
+      </c>
+      <c r="I40" s="1" t="n">
+        <v>45335</v>
+      </c>
+      <c r="J40" t="inlineStr">
+        <is>
+          <t>нет данных</t>
+        </is>
+      </c>
+    </row>
+    <row r="41">
+      <c r="E41" t="inlineStr">
+        <is>
+          <t>225/50R17</t>
+        </is>
+      </c>
+      <c r="F41" t="inlineStr">
+        <is>
+          <t>Бел-1005</t>
+        </is>
+      </c>
+      <c r="G41" t="inlineStr">
+        <is>
+          <t>легк, сер</t>
+        </is>
+      </c>
+      <c r="H41" t="n">
+        <v>2</v>
+      </c>
+      <c r="I41" s="1" t="n">
+        <v>45335</v>
+      </c>
+      <c r="J41" t="inlineStr">
+        <is>
+          <t>нет данных</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
10.02/2024 - return to host 14
</commit_message>
<xml_diff>
--- a/src/Tyres.xlsx
+++ b/src/Tyres.xlsx
@@ -17,7 +17,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="0"/>
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="yyyy-mm-dd"/>
+  </numFmts>
   <fonts count="1">
     <font>
       <name val="Calibri"/>
@@ -47,8 +49,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
@@ -414,7 +417,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C22"/>
+  <dimension ref="A1:J30"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -433,7 +436,36 @@
           <t xml:space="preserve"> </t>
         </is>
       </c>
-      <c r="C1" t="inlineStr"/>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>Tyre Size</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>Model</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
+        <is>
+          <t>Param</t>
+        </is>
+      </c>
+      <c r="H1" t="inlineStr">
+        <is>
+          <t>Sales value</t>
+        </is>
+      </c>
+      <c r="I1" t="inlineStr">
+        <is>
+          <t>Date_of_sales</t>
+        </is>
+      </c>
+      <c r="J1" t="inlineStr">
+        <is>
+          <t>Contragent</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
@@ -448,7 +480,33 @@
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>42 30 сер груз</t>
+          <t>30 42 сер груз</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>35/65-33</t>
+        </is>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>ФБел-283</t>
+        </is>
+      </c>
+      <c r="G2" t="inlineStr">
+        <is>
+          <t>30, 42, сер, груз</t>
+        </is>
+      </c>
+      <c r="H2" t="n">
+        <v>2</v>
+      </c>
+      <c r="I2" s="1" t="n">
+        <v>45340</v>
+      </c>
+      <c r="J2" t="inlineStr">
+        <is>
+          <t>нет данных</t>
         </is>
       </c>
     </row>
@@ -465,7 +523,33 @@
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>легк б/к сер</t>
+          <t>б/к сер легк</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>35/65-33</t>
+        </is>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>ФБел-283</t>
+        </is>
+      </c>
+      <c r="G3" t="inlineStr">
+        <is>
+          <t>30, 42, сер, груз</t>
+        </is>
+      </c>
+      <c r="H3" t="n">
+        <v>2</v>
+      </c>
+      <c r="I3" s="1" t="n">
+        <v>45340</v>
+      </c>
+      <c r="J3" t="inlineStr">
+        <is>
+          <t>нет данных</t>
         </is>
       </c>
     </row>
@@ -482,7 +566,33 @@
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>легк б/к сер</t>
+          <t>б/к сер легк</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>205/55R16</t>
+        </is>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>BEL-262</t>
+        </is>
+      </c>
+      <c r="G4" t="inlineStr">
+        <is>
+          <t>б/к, сер, легк</t>
+        </is>
+      </c>
+      <c r="H4" t="n">
+        <v>2</v>
+      </c>
+      <c r="I4" s="1" t="n">
+        <v>45340</v>
+      </c>
+      <c r="J4" t="inlineStr">
+        <is>
+          <t>нет данных</t>
         </is>
       </c>
     </row>
@@ -502,6 +612,32 @@
           <t>сер ошип</t>
         </is>
       </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>205/55R16</t>
+        </is>
+      </c>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>BEL-317</t>
+        </is>
+      </c>
+      <c r="G5" t="inlineStr">
+        <is>
+          <t>б/к, сер, легк</t>
+        </is>
+      </c>
+      <c r="H5" t="n">
+        <v>2</v>
+      </c>
+      <c r="I5" s="1" t="n">
+        <v>45340</v>
+      </c>
+      <c r="J5" t="inlineStr">
+        <is>
+          <t>нет данных</t>
+        </is>
+      </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
@@ -516,7 +652,33 @@
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>легк сер</t>
+          <t>сер легк</t>
+        </is>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>205/55R16</t>
+        </is>
+      </c>
+      <c r="F6" t="inlineStr">
+        <is>
+          <t>BEL-317S</t>
+        </is>
+      </c>
+      <c r="G6" t="inlineStr">
+        <is>
+          <t>сер, ошип</t>
+        </is>
+      </c>
+      <c r="H6" t="n">
+        <v>2</v>
+      </c>
+      <c r="I6" s="1" t="n">
+        <v>45340</v>
+      </c>
+      <c r="J6" t="inlineStr">
+        <is>
+          <t>нет данных</t>
         </is>
       </c>
     </row>
@@ -533,7 +695,33 @@
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>легк сер</t>
+          <t>сер легк</t>
+        </is>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>235/75R15</t>
+        </is>
+      </c>
+      <c r="F7" t="inlineStr">
+        <is>
+          <t>BEL-1001</t>
+        </is>
+      </c>
+      <c r="G7" t="inlineStr">
+        <is>
+          <t>сер, легк</t>
+        </is>
+      </c>
+      <c r="H7" t="n">
+        <v>2</v>
+      </c>
+      <c r="I7" s="1" t="n">
+        <v>45340</v>
+      </c>
+      <c r="J7" t="inlineStr">
+        <is>
+          <t>нет данных</t>
         </is>
       </c>
     </row>
@@ -550,7 +738,33 @@
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>легк сер</t>
+          <t>сер легк</t>
+        </is>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>155/65R13</t>
+        </is>
+      </c>
+      <c r="F8" t="inlineStr">
+        <is>
+          <t>BEL-1002</t>
+        </is>
+      </c>
+      <c r="G8" t="inlineStr">
+        <is>
+          <t>сер, легк</t>
+        </is>
+      </c>
+      <c r="H8" t="n">
+        <v>2</v>
+      </c>
+      <c r="I8" s="1" t="n">
+        <v>45340</v>
+      </c>
+      <c r="J8" t="inlineStr">
+        <is>
+          <t>нет данных</t>
         </is>
       </c>
     </row>
@@ -567,7 +781,33 @@
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>легк сер</t>
+          <t>сер легк</t>
+        </is>
+      </c>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>205/55R16</t>
+        </is>
+      </c>
+      <c r="F9" t="inlineStr">
+        <is>
+          <t>BEL-1004</t>
+        </is>
+      </c>
+      <c r="G9" t="inlineStr">
+        <is>
+          <t>сер, легк</t>
+        </is>
+      </c>
+      <c r="H9" t="n">
+        <v>2</v>
+      </c>
+      <c r="I9" s="1" t="n">
+        <v>45340</v>
+      </c>
+      <c r="J9" t="inlineStr">
+        <is>
+          <t>нет данных</t>
         </is>
       </c>
     </row>
@@ -584,7 +824,33 @@
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>210B сер C Type H</t>
+          <t>210B C сер H Type</t>
+        </is>
+      </c>
+      <c r="E10" t="inlineStr">
+        <is>
+          <t>225/50R17</t>
+        </is>
+      </c>
+      <c r="F10" t="inlineStr">
+        <is>
+          <t>BEL-1005</t>
+        </is>
+      </c>
+      <c r="G10" t="inlineStr">
+        <is>
+          <t>сер, легк</t>
+        </is>
+      </c>
+      <c r="H10" t="n">
+        <v>2</v>
+      </c>
+      <c r="I10" s="1" t="n">
+        <v>45340</v>
+      </c>
+      <c r="J10" t="inlineStr">
+        <is>
+          <t>нет данных</t>
         </is>
       </c>
     </row>
@@ -601,7 +867,33 @@
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>LS-2 сер груз Type</t>
+          <t>сер груз Type LS-2</t>
+        </is>
+      </c>
+      <c r="E11" t="inlineStr">
+        <is>
+          <t>24.00R35</t>
+        </is>
+      </c>
+      <c r="F11" t="inlineStr">
+        <is>
+          <t>Бел-202</t>
+        </is>
+      </c>
+      <c r="G11" t="inlineStr">
+        <is>
+          <t>210B, C, сер, H, Type</t>
+        </is>
+      </c>
+      <c r="H11" t="n">
+        <v>2</v>
+      </c>
+      <c r="I11" s="1" t="n">
+        <v>45340</v>
+      </c>
+      <c r="J11" t="inlineStr">
+        <is>
+          <t>нет данных</t>
         </is>
       </c>
     </row>
@@ -618,7 +910,33 @@
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>202B сер C Type</t>
+          <t>202B C сер Type</t>
+        </is>
+      </c>
+      <c r="E12" t="inlineStr">
+        <is>
+          <t>24.00R35</t>
+        </is>
+      </c>
+      <c r="F12" t="inlineStr">
+        <is>
+          <t>Бел-202</t>
+        </is>
+      </c>
+      <c r="G12" t="inlineStr">
+        <is>
+          <t>210B, C, сер, H, Type</t>
+        </is>
+      </c>
+      <c r="H12" t="n">
+        <v>2</v>
+      </c>
+      <c r="I12" s="1" t="n">
+        <v>45340</v>
+      </c>
+      <c r="J12" t="inlineStr">
+        <is>
+          <t>нет данных</t>
         </is>
       </c>
     </row>
@@ -635,7 +953,33 @@
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>202B LS-2 сер C Type H</t>
+          <t>202B C сер H Type LS-2</t>
+        </is>
+      </c>
+      <c r="E13" t="inlineStr">
+        <is>
+          <t>24.00R35</t>
+        </is>
+      </c>
+      <c r="F13" t="inlineStr">
+        <is>
+          <t>Бел-212</t>
+        </is>
+      </c>
+      <c r="G13" t="inlineStr">
+        <is>
+          <t>сер, груз, Type, LS-2</t>
+        </is>
+      </c>
+      <c r="H13" t="n">
+        <v>2</v>
+      </c>
+      <c r="I13" s="1" t="n">
+        <v>45340</v>
+      </c>
+      <c r="J13" t="inlineStr">
+        <is>
+          <t>нет данных</t>
         </is>
       </c>
     </row>
@@ -655,6 +999,32 @@
           <t>б/к сер груз</t>
         </is>
       </c>
+      <c r="E14" t="inlineStr">
+        <is>
+          <t>21.00R35</t>
+        </is>
+      </c>
+      <c r="F14" t="inlineStr">
+        <is>
+          <t>Бел-200</t>
+        </is>
+      </c>
+      <c r="G14" t="inlineStr">
+        <is>
+          <t>202B, C, сер, Type</t>
+        </is>
+      </c>
+      <c r="H14" t="n">
+        <v>2</v>
+      </c>
+      <c r="I14" s="1" t="n">
+        <v>45340</v>
+      </c>
+      <c r="J14" t="inlineStr">
+        <is>
+          <t>нет данных</t>
+        </is>
+      </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
@@ -669,7 +1039,33 @@
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>легк б/к сер</t>
+          <t>б/к сер легк</t>
+        </is>
+      </c>
+      <c r="E15" t="inlineStr">
+        <is>
+          <t>21.00R35</t>
+        </is>
+      </c>
+      <c r="F15" t="inlineStr">
+        <is>
+          <t>Бел-210</t>
+        </is>
+      </c>
+      <c r="G15" t="inlineStr">
+        <is>
+          <t>202B, C, сер, H, Type, LS-2</t>
+        </is>
+      </c>
+      <c r="H15" t="n">
+        <v>2</v>
+      </c>
+      <c r="I15" s="1" t="n">
+        <v>45340</v>
+      </c>
+      <c r="J15" t="inlineStr">
+        <is>
+          <t>нет данных</t>
         </is>
       </c>
     </row>
@@ -686,7 +1082,33 @@
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>легк б/к сер</t>
+          <t>б/к сер легк</t>
+        </is>
+      </c>
+      <c r="E16" t="inlineStr">
+        <is>
+          <t>21.00R35</t>
+        </is>
+      </c>
+      <c r="F16" t="inlineStr">
+        <is>
+          <t>Бел-210</t>
+        </is>
+      </c>
+      <c r="G16" t="inlineStr">
+        <is>
+          <t>202B, C, сер, H, Type, LS-2</t>
+        </is>
+      </c>
+      <c r="H16" t="n">
+        <v>2</v>
+      </c>
+      <c r="I16" s="1" t="n">
+        <v>45340</v>
+      </c>
+      <c r="J16" t="inlineStr">
+        <is>
+          <t>нет данных</t>
         </is>
       </c>
     </row>
@@ -706,6 +1128,32 @@
           <t>8 сер сх</t>
         </is>
       </c>
+      <c r="E17" t="inlineStr">
+        <is>
+          <t>21.00R35</t>
+        </is>
+      </c>
+      <c r="F17" t="inlineStr">
+        <is>
+          <t>Бел-210</t>
+        </is>
+      </c>
+      <c r="G17" t="inlineStr">
+        <is>
+          <t>202B, C, сер, H, Type, LS-2</t>
+        </is>
+      </c>
+      <c r="H17" t="n">
+        <v>2</v>
+      </c>
+      <c r="I17" s="1" t="n">
+        <v>45340</v>
+      </c>
+      <c r="J17" t="inlineStr">
+        <is>
+          <t>нет данных</t>
+        </is>
+      </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
@@ -720,7 +1168,33 @@
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>легк сер</t>
+          <t>сер легк</t>
+        </is>
+      </c>
+      <c r="E18" t="inlineStr">
+        <is>
+          <t>14.00R20</t>
+        </is>
+      </c>
+      <c r="F18" t="inlineStr">
+        <is>
+          <t>BEL-248</t>
+        </is>
+      </c>
+      <c r="G18" t="inlineStr">
+        <is>
+          <t>б/к, сер, груз</t>
+        </is>
+      </c>
+      <c r="H18" t="n">
+        <v>2</v>
+      </c>
+      <c r="I18" s="1" t="n">
+        <v>45340</v>
+      </c>
+      <c r="J18" t="inlineStr">
+        <is>
+          <t>нет данных</t>
         </is>
       </c>
     </row>
@@ -737,7 +1211,33 @@
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>легк сер</t>
+          <t>сер легк</t>
+        </is>
+      </c>
+      <c r="E19" t="inlineStr">
+        <is>
+          <t>14.00R20</t>
+        </is>
+      </c>
+      <c r="F19" t="inlineStr">
+        <is>
+          <t>BEL-248</t>
+        </is>
+      </c>
+      <c r="G19" t="inlineStr">
+        <is>
+          <t>б/к, сер, груз</t>
+        </is>
+      </c>
+      <c r="H19" t="n">
+        <v>2</v>
+      </c>
+      <c r="I19" s="1" t="n">
+        <v>45340</v>
+      </c>
+      <c r="J19" t="inlineStr">
+        <is>
+          <t>нет данных</t>
         </is>
       </c>
     </row>
@@ -754,7 +1254,33 @@
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>легк сер</t>
+          <t>сер легк</t>
+        </is>
+      </c>
+      <c r="E20" t="inlineStr">
+        <is>
+          <t>14.00R20</t>
+        </is>
+      </c>
+      <c r="F20" t="inlineStr">
+        <is>
+          <t>BEL-248</t>
+        </is>
+      </c>
+      <c r="G20" t="inlineStr">
+        <is>
+          <t>б/к, сер, груз</t>
+        </is>
+      </c>
+      <c r="H20" t="n">
+        <v>2</v>
+      </c>
+      <c r="I20" s="1" t="n">
+        <v>45340</v>
+      </c>
+      <c r="J20" t="inlineStr">
+        <is>
+          <t>нет данных</t>
         </is>
       </c>
     </row>
@@ -771,7 +1297,33 @@
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>легк сер</t>
+          <t>сер легк</t>
+        </is>
+      </c>
+      <c r="E21" t="inlineStr">
+        <is>
+          <t>14.00R20</t>
+        </is>
+      </c>
+      <c r="F21" t="inlineStr">
+        <is>
+          <t>BEL-248</t>
+        </is>
+      </c>
+      <c r="G21" t="inlineStr">
+        <is>
+          <t>б/к, сер, груз</t>
+        </is>
+      </c>
+      <c r="H21" t="n">
+        <v>2</v>
+      </c>
+      <c r="I21" s="1" t="n">
+        <v>45340</v>
+      </c>
+      <c r="J21" t="inlineStr">
+        <is>
+          <t>нет данных</t>
         </is>
       </c>
     </row>
@@ -788,7 +1340,257 @@
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>легк сер</t>
+          <t>сер легк</t>
+        </is>
+      </c>
+      <c r="E22" t="inlineStr">
+        <is>
+          <t>175/70R13</t>
+        </is>
+      </c>
+      <c r="F22" t="inlineStr">
+        <is>
+          <t>Бел-103</t>
+        </is>
+      </c>
+      <c r="G22" t="inlineStr">
+        <is>
+          <t>б/к, сер, легк</t>
+        </is>
+      </c>
+      <c r="H22" t="n">
+        <v>2</v>
+      </c>
+      <c r="I22" s="1" t="n">
+        <v>45340</v>
+      </c>
+      <c r="J22" t="inlineStr">
+        <is>
+          <t>нет данных</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="E23" t="inlineStr">
+        <is>
+          <t>175/70R13</t>
+        </is>
+      </c>
+      <c r="F23" t="inlineStr">
+        <is>
+          <t>Бел-100</t>
+        </is>
+      </c>
+      <c r="G23" t="inlineStr">
+        <is>
+          <t>б/к, сер, легк</t>
+        </is>
+      </c>
+      <c r="H23" t="n">
+        <v>2</v>
+      </c>
+      <c r="I23" s="1" t="n">
+        <v>45340</v>
+      </c>
+      <c r="J23" t="inlineStr">
+        <is>
+          <t>нет данных</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="E24" t="inlineStr">
+        <is>
+          <t>195/65R15</t>
+        </is>
+      </c>
+      <c r="F24" t="inlineStr">
+        <is>
+          <t>Бел-119</t>
+        </is>
+      </c>
+      <c r="G24" t="inlineStr">
+        <is>
+          <t>сер, легк</t>
+        </is>
+      </c>
+      <c r="H24" t="n">
+        <v>2</v>
+      </c>
+      <c r="I24" s="1" t="n">
+        <v>45340</v>
+      </c>
+      <c r="J24" t="inlineStr">
+        <is>
+          <t>нет данных</t>
+        </is>
+      </c>
+    </row>
+    <row r="25">
+      <c r="E25" t="inlineStr">
+        <is>
+          <t>195/65R15</t>
+        </is>
+      </c>
+      <c r="F25" t="inlineStr">
+        <is>
+          <t>Бел-119</t>
+        </is>
+      </c>
+      <c r="G25" t="inlineStr">
+        <is>
+          <t>сер, легк</t>
+        </is>
+      </c>
+      <c r="H25" t="n">
+        <v>2</v>
+      </c>
+      <c r="I25" s="1" t="n">
+        <v>45340</v>
+      </c>
+      <c r="J25" t="inlineStr">
+        <is>
+          <t>нет данных</t>
+        </is>
+      </c>
+    </row>
+    <row r="26">
+      <c r="E26" t="inlineStr">
+        <is>
+          <t>195/65R15</t>
+        </is>
+      </c>
+      <c r="F26" t="inlineStr">
+        <is>
+          <t>Бел-119</t>
+        </is>
+      </c>
+      <c r="G26" t="inlineStr">
+        <is>
+          <t>сер, легк</t>
+        </is>
+      </c>
+      <c r="H26" t="n">
+        <v>2</v>
+      </c>
+      <c r="I26" s="1" t="n">
+        <v>45340</v>
+      </c>
+      <c r="J26" t="inlineStr">
+        <is>
+          <t>нет данных</t>
+        </is>
+      </c>
+    </row>
+    <row r="27">
+      <c r="E27" t="inlineStr">
+        <is>
+          <t>210/80R16</t>
+        </is>
+      </c>
+      <c r="F27" t="inlineStr">
+        <is>
+          <t>Бел-777</t>
+        </is>
+      </c>
+      <c r="G27" t="inlineStr">
+        <is>
+          <t>сер, легк</t>
+        </is>
+      </c>
+      <c r="H27" t="n">
+        <v>2</v>
+      </c>
+      <c r="I27" s="1" t="n">
+        <v>45340</v>
+      </c>
+      <c r="J27" t="inlineStr">
+        <is>
+          <t>нет данных</t>
+        </is>
+      </c>
+    </row>
+    <row r="28">
+      <c r="E28" t="inlineStr">
+        <is>
+          <t>215/65R16C</t>
+        </is>
+      </c>
+      <c r="F28" t="inlineStr">
+        <is>
+          <t>Бел-1000</t>
+        </is>
+      </c>
+      <c r="G28" t="inlineStr">
+        <is>
+          <t>сер, легк</t>
+        </is>
+      </c>
+      <c r="H28" t="n">
+        <v>2</v>
+      </c>
+      <c r="I28" s="1" t="n">
+        <v>45340</v>
+      </c>
+      <c r="J28" t="inlineStr">
+        <is>
+          <t>нет данных</t>
+        </is>
+      </c>
+    </row>
+    <row r="29">
+      <c r="E29" t="inlineStr">
+        <is>
+          <t>205/55R16</t>
+        </is>
+      </c>
+      <c r="F29" t="inlineStr">
+        <is>
+          <t>Бел-1001</t>
+        </is>
+      </c>
+      <c r="G29" t="inlineStr">
+        <is>
+          <t>сер, легк</t>
+        </is>
+      </c>
+      <c r="H29" t="n">
+        <v>2</v>
+      </c>
+      <c r="I29" s="1" t="n">
+        <v>45340</v>
+      </c>
+      <c r="J29" t="inlineStr">
+        <is>
+          <t>нет данных</t>
+        </is>
+      </c>
+    </row>
+    <row r="30">
+      <c r="E30" t="inlineStr">
+        <is>
+          <t>225/50R17</t>
+        </is>
+      </c>
+      <c r="F30" t="inlineStr">
+        <is>
+          <t>Бел-1005</t>
+        </is>
+      </c>
+      <c r="G30" t="inlineStr">
+        <is>
+          <t>сер, легк</t>
+        </is>
+      </c>
+      <c r="H30" t="n">
+        <v>2</v>
+      </c>
+      <c r="I30" s="1" t="n">
+        <v>45340</v>
+      </c>
+      <c r="J30" t="inlineStr">
+        <is>
+          <t>нет данных</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
10.02/2024 - return to host 17
</commit_message>
<xml_diff>
--- a/src/Tyres.xlsx
+++ b/src/Tyres.xlsx
@@ -480,7 +480,7 @@
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>30 42 сер груз</t>
+          <t>42 30 груз сер</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
@@ -495,7 +495,7 @@
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>30, 42, сер, груз</t>
+          <t>42, 30, груз, сер</t>
         </is>
       </c>
       <c r="H2" t="n">
@@ -523,7 +523,7 @@
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>б/к сер легк</t>
+          <t>легк б/к сер</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
@@ -538,7 +538,7 @@
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>30, 42, сер, груз</t>
+          <t>42, 30, груз, сер</t>
         </is>
       </c>
       <c r="H3" t="n">
@@ -566,7 +566,7 @@
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>б/к сер легк</t>
+          <t>легк б/к сер</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
@@ -581,7 +581,7 @@
       </c>
       <c r="G4" t="inlineStr">
         <is>
-          <t>б/к, сер, легк</t>
+          <t>легк, б/к, сер</t>
         </is>
       </c>
       <c r="H4" t="n">
@@ -609,7 +609,7 @@
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>сер ошип</t>
+          <t>ошип сер</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
@@ -624,7 +624,7 @@
       </c>
       <c r="G5" t="inlineStr">
         <is>
-          <t>б/к, сер, легк</t>
+          <t>легк, б/к, сер</t>
         </is>
       </c>
       <c r="H5" t="n">
@@ -652,7 +652,7 @@
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>сер легк</t>
+          <t>легк сер</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
@@ -667,7 +667,7 @@
       </c>
       <c r="G6" t="inlineStr">
         <is>
-          <t>сер, ошип</t>
+          <t>ошип, сер</t>
         </is>
       </c>
       <c r="H6" t="n">
@@ -695,7 +695,7 @@
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>сер легк</t>
+          <t>легк сер</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
@@ -710,7 +710,7 @@
       </c>
       <c r="G7" t="inlineStr">
         <is>
-          <t>сер, легк</t>
+          <t>легк, сер</t>
         </is>
       </c>
       <c r="H7" t="n">
@@ -738,7 +738,7 @@
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>сер легк</t>
+          <t>легк сер</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
@@ -753,7 +753,7 @@
       </c>
       <c r="G8" t="inlineStr">
         <is>
-          <t>сер, легк</t>
+          <t>легк, сер</t>
         </is>
       </c>
       <c r="H8" t="n">
@@ -781,7 +781,7 @@
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>сер легк</t>
+          <t>легк сер</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
@@ -796,7 +796,7 @@
       </c>
       <c r="G9" t="inlineStr">
         <is>
-          <t>сер, легк</t>
+          <t>легк, сер</t>
         </is>
       </c>
       <c r="H9" t="n">
@@ -824,7 +824,7 @@
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>210B C сер H Type</t>
+          <t>210B Type H C сер</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
@@ -839,7 +839,7 @@
       </c>
       <c r="G10" t="inlineStr">
         <is>
-          <t>сер, легк</t>
+          <t>легк, сер</t>
         </is>
       </c>
       <c r="H10" t="n">
@@ -867,7 +867,7 @@
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>сер груз Type LS-2</t>
+          <t>Type груз сер LS-2</t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
@@ -882,7 +882,7 @@
       </c>
       <c r="G11" t="inlineStr">
         <is>
-          <t>210B, C, сер, H, Type</t>
+          <t>210B, Type, H, C, сер</t>
         </is>
       </c>
       <c r="H11" t="n">
@@ -910,7 +910,7 @@
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>202B C сер Type</t>
+          <t>202B Type C сер</t>
         </is>
       </c>
       <c r="E12" t="inlineStr">
@@ -925,7 +925,7 @@
       </c>
       <c r="G12" t="inlineStr">
         <is>
-          <t>210B, C, сер, H, Type</t>
+          <t>210B, Type, H, C, сер</t>
         </is>
       </c>
       <c r="H12" t="n">
@@ -953,7 +953,7 @@
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>202B C сер H Type LS-2</t>
+          <t>202B Type H C сер LS-2</t>
         </is>
       </c>
       <c r="E13" t="inlineStr">
@@ -968,7 +968,7 @@
       </c>
       <c r="G13" t="inlineStr">
         <is>
-          <t>сер, груз, Type, LS-2</t>
+          <t>Type, груз, сер, LS-2</t>
         </is>
       </c>
       <c r="H13" t="n">
@@ -996,7 +996,7 @@
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>б/к сер груз</t>
+          <t>б/к груз сер</t>
         </is>
       </c>
       <c r="E14" t="inlineStr">
@@ -1011,7 +1011,7 @@
       </c>
       <c r="G14" t="inlineStr">
         <is>
-          <t>202B, C, сер, Type</t>
+          <t>202B, Type, C, сер</t>
         </is>
       </c>
       <c r="H14" t="n">
@@ -1039,7 +1039,7 @@
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>б/к сер легк</t>
+          <t>легк б/к сер</t>
         </is>
       </c>
       <c r="E15" t="inlineStr">
@@ -1054,7 +1054,7 @@
       </c>
       <c r="G15" t="inlineStr">
         <is>
-          <t>202B, C, сер, H, Type, LS-2</t>
+          <t>202B, Type, H, C, сер, LS-2</t>
         </is>
       </c>
       <c r="H15" t="n">
@@ -1082,7 +1082,7 @@
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>б/к сер легк</t>
+          <t>легк б/к сер</t>
         </is>
       </c>
       <c r="E16" t="inlineStr">
@@ -1097,7 +1097,7 @@
       </c>
       <c r="G16" t="inlineStr">
         <is>
-          <t>202B, C, сер, H, Type, LS-2</t>
+          <t>202B, Type, H, C, сер, LS-2</t>
         </is>
       </c>
       <c r="H16" t="n">
@@ -1125,7 +1125,7 @@
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>8 сер сх</t>
+          <t>8 сх сер</t>
         </is>
       </c>
       <c r="E17" t="inlineStr">
@@ -1140,7 +1140,7 @@
       </c>
       <c r="G17" t="inlineStr">
         <is>
-          <t>202B, C, сер, H, Type, LS-2</t>
+          <t>202B, Type, H, C, сер, LS-2</t>
         </is>
       </c>
       <c r="H17" t="n">
@@ -1168,7 +1168,7 @@
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>сер легк</t>
+          <t>легк сер</t>
         </is>
       </c>
       <c r="E18" t="inlineStr">
@@ -1183,7 +1183,7 @@
       </c>
       <c r="G18" t="inlineStr">
         <is>
-          <t>б/к, сер, груз</t>
+          <t>б/к, груз, сер</t>
         </is>
       </c>
       <c r="H18" t="n">
@@ -1211,7 +1211,7 @@
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>сер легк</t>
+          <t>легк сер</t>
         </is>
       </c>
       <c r="E19" t="inlineStr">
@@ -1226,7 +1226,7 @@
       </c>
       <c r="G19" t="inlineStr">
         <is>
-          <t>б/к, сер, груз</t>
+          <t>б/к, груз, сер</t>
         </is>
       </c>
       <c r="H19" t="n">
@@ -1254,7 +1254,7 @@
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>сер легк</t>
+          <t>легк сер</t>
         </is>
       </c>
       <c r="E20" t="inlineStr">
@@ -1269,7 +1269,7 @@
       </c>
       <c r="G20" t="inlineStr">
         <is>
-          <t>б/к, сер, груз</t>
+          <t>б/к, груз, сер</t>
         </is>
       </c>
       <c r="H20" t="n">
@@ -1297,7 +1297,7 @@
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>сер легк</t>
+          <t>легк сер</t>
         </is>
       </c>
       <c r="E21" t="inlineStr">
@@ -1312,7 +1312,7 @@
       </c>
       <c r="G21" t="inlineStr">
         <is>
-          <t>б/к, сер, груз</t>
+          <t>б/к, груз, сер</t>
         </is>
       </c>
       <c r="H21" t="n">
@@ -1340,7 +1340,7 @@
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>сер легк</t>
+          <t>легк сер</t>
         </is>
       </c>
       <c r="E22" t="inlineStr">
@@ -1355,7 +1355,7 @@
       </c>
       <c r="G22" t="inlineStr">
         <is>
-          <t>б/к, сер, легк</t>
+          <t>легк, б/к, сер</t>
         </is>
       </c>
       <c r="H22" t="n">
@@ -1383,7 +1383,7 @@
       </c>
       <c r="G23" t="inlineStr">
         <is>
-          <t>б/к, сер, легк</t>
+          <t>легк, б/к, сер</t>
         </is>
       </c>
       <c r="H23" t="n">
@@ -1411,7 +1411,7 @@
       </c>
       <c r="G24" t="inlineStr">
         <is>
-          <t>сер, легк</t>
+          <t>легк, сер</t>
         </is>
       </c>
       <c r="H24" t="n">
@@ -1439,7 +1439,7 @@
       </c>
       <c r="G25" t="inlineStr">
         <is>
-          <t>сер, легк</t>
+          <t>легк, сер</t>
         </is>
       </c>
       <c r="H25" t="n">
@@ -1467,7 +1467,7 @@
       </c>
       <c r="G26" t="inlineStr">
         <is>
-          <t>сер, легк</t>
+          <t>легк, сер</t>
         </is>
       </c>
       <c r="H26" t="n">
@@ -1495,7 +1495,7 @@
       </c>
       <c r="G27" t="inlineStr">
         <is>
-          <t>сер, легк</t>
+          <t>легк, сер</t>
         </is>
       </c>
       <c r="H27" t="n">
@@ -1523,7 +1523,7 @@
       </c>
       <c r="G28" t="inlineStr">
         <is>
-          <t>сер, легк</t>
+          <t>легк, сер</t>
         </is>
       </c>
       <c r="H28" t="n">
@@ -1551,7 +1551,7 @@
       </c>
       <c r="G29" t="inlineStr">
         <is>
-          <t>сер, легк</t>
+          <t>легк, сер</t>
         </is>
       </c>
       <c r="H29" t="n">
@@ -1579,7 +1579,7 @@
       </c>
       <c r="G30" t="inlineStr">
         <is>
-          <t>сер, легк</t>
+          <t>легк, сер</t>
         </is>
       </c>
       <c r="H30" t="n">

</xml_diff>

<commit_message>
10.02/2024 - return to host 18
</commit_message>
<xml_diff>
--- a/src/Tyres.xlsx
+++ b/src/Tyres.xlsx
@@ -480,7 +480,7 @@
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>42 30 груз сер</t>
+          <t>42 30 сер груз</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
@@ -495,14 +495,14 @@
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>42, 30, груз, сер</t>
+          <t>42, 30, сер, груз</t>
         </is>
       </c>
       <c r="H2" t="n">
         <v>2</v>
       </c>
       <c r="I2" s="1" t="n">
-        <v>45340</v>
+        <v>45341</v>
       </c>
       <c r="J2" t="inlineStr">
         <is>
@@ -523,7 +523,7 @@
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>легк б/к сер</t>
+          <t>сер легк б/к</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
@@ -538,14 +538,14 @@
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>42, 30, груз, сер</t>
+          <t>42, 30, сер, груз</t>
         </is>
       </c>
       <c r="H3" t="n">
         <v>2</v>
       </c>
       <c r="I3" s="1" t="n">
-        <v>45340</v>
+        <v>45341</v>
       </c>
       <c r="J3" t="inlineStr">
         <is>
@@ -566,7 +566,7 @@
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>легк б/к сер</t>
+          <t>сер легк б/к</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
@@ -581,14 +581,14 @@
       </c>
       <c r="G4" t="inlineStr">
         <is>
-          <t>легк, б/к, сер</t>
+          <t>сер, легк, б/к</t>
         </is>
       </c>
       <c r="H4" t="n">
         <v>2</v>
       </c>
       <c r="I4" s="1" t="n">
-        <v>45340</v>
+        <v>45341</v>
       </c>
       <c r="J4" t="inlineStr">
         <is>
@@ -609,7 +609,7 @@
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>ошип сер</t>
+          <t>сер ошип</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
@@ -624,14 +624,14 @@
       </c>
       <c r="G5" t="inlineStr">
         <is>
-          <t>легк, б/к, сер</t>
+          <t>сер, легк, б/к</t>
         </is>
       </c>
       <c r="H5" t="n">
         <v>2</v>
       </c>
       <c r="I5" s="1" t="n">
-        <v>45340</v>
+        <v>45341</v>
       </c>
       <c r="J5" t="inlineStr">
         <is>
@@ -652,7 +652,7 @@
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>легк сер</t>
+          <t>сер легк</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
@@ -667,14 +667,14 @@
       </c>
       <c r="G6" t="inlineStr">
         <is>
-          <t>ошип, сер</t>
+          <t>сер, ошип</t>
         </is>
       </c>
       <c r="H6" t="n">
         <v>2</v>
       </c>
       <c r="I6" s="1" t="n">
-        <v>45340</v>
+        <v>45341</v>
       </c>
       <c r="J6" t="inlineStr">
         <is>
@@ -695,7 +695,7 @@
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>легк сер</t>
+          <t>сер легк</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
@@ -710,14 +710,14 @@
       </c>
       <c r="G7" t="inlineStr">
         <is>
-          <t>легк, сер</t>
+          <t>сер, легк</t>
         </is>
       </c>
       <c r="H7" t="n">
         <v>2</v>
       </c>
       <c r="I7" s="1" t="n">
-        <v>45340</v>
+        <v>45341</v>
       </c>
       <c r="J7" t="inlineStr">
         <is>
@@ -738,7 +738,7 @@
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>легк сер</t>
+          <t>сер легк</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
@@ -753,14 +753,14 @@
       </c>
       <c r="G8" t="inlineStr">
         <is>
-          <t>легк, сер</t>
+          <t>сер, легк</t>
         </is>
       </c>
       <c r="H8" t="n">
         <v>2</v>
       </c>
       <c r="I8" s="1" t="n">
-        <v>45340</v>
+        <v>45341</v>
       </c>
       <c r="J8" t="inlineStr">
         <is>
@@ -781,7 +781,7 @@
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>легк сер</t>
+          <t>сер легк</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
@@ -796,14 +796,14 @@
       </c>
       <c r="G9" t="inlineStr">
         <is>
-          <t>легк, сер</t>
+          <t>сер, легк</t>
         </is>
       </c>
       <c r="H9" t="n">
         <v>2</v>
       </c>
       <c r="I9" s="1" t="n">
-        <v>45340</v>
+        <v>45341</v>
       </c>
       <c r="J9" t="inlineStr">
         <is>
@@ -824,7 +824,7 @@
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>210B Type H C сер</t>
+          <t>210B Type сер H C</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
@@ -839,14 +839,14 @@
       </c>
       <c r="G10" t="inlineStr">
         <is>
-          <t>легк, сер</t>
+          <t>сер, легк</t>
         </is>
       </c>
       <c r="H10" t="n">
         <v>2</v>
       </c>
       <c r="I10" s="1" t="n">
-        <v>45340</v>
+        <v>45341</v>
       </c>
       <c r="J10" t="inlineStr">
         <is>
@@ -867,7 +867,7 @@
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>Type груз сер LS-2</t>
+          <t>Type сер LS-2 груз</t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
@@ -882,14 +882,14 @@
       </c>
       <c r="G11" t="inlineStr">
         <is>
-          <t>210B, Type, H, C, сер</t>
+          <t>210B, Type, сер, H, C</t>
         </is>
       </c>
       <c r="H11" t="n">
         <v>2</v>
       </c>
       <c r="I11" s="1" t="n">
-        <v>45340</v>
+        <v>45341</v>
       </c>
       <c r="J11" t="inlineStr">
         <is>
@@ -910,7 +910,7 @@
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>202B Type C сер</t>
+          <t>202B Type сер C</t>
         </is>
       </c>
       <c r="E12" t="inlineStr">
@@ -925,14 +925,14 @@
       </c>
       <c r="G12" t="inlineStr">
         <is>
-          <t>210B, Type, H, C, сер</t>
+          <t>210B, Type, сер, H, C</t>
         </is>
       </c>
       <c r="H12" t="n">
         <v>2</v>
       </c>
       <c r="I12" s="1" t="n">
-        <v>45340</v>
+        <v>45341</v>
       </c>
       <c r="J12" t="inlineStr">
         <is>
@@ -953,7 +953,7 @@
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>202B Type H C сер LS-2</t>
+          <t>202B Type сер LS-2 H C</t>
         </is>
       </c>
       <c r="E13" t="inlineStr">
@@ -968,14 +968,14 @@
       </c>
       <c r="G13" t="inlineStr">
         <is>
-          <t>Type, груз, сер, LS-2</t>
+          <t>Type, сер, LS-2, груз</t>
         </is>
       </c>
       <c r="H13" t="n">
         <v>2</v>
       </c>
       <c r="I13" s="1" t="n">
-        <v>45340</v>
+        <v>45341</v>
       </c>
       <c r="J13" t="inlineStr">
         <is>
@@ -996,7 +996,7 @@
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>б/к груз сер</t>
+          <t>сер б/к груз</t>
         </is>
       </c>
       <c r="E14" t="inlineStr">
@@ -1011,14 +1011,14 @@
       </c>
       <c r="G14" t="inlineStr">
         <is>
-          <t>202B, Type, C, сер</t>
+          <t>202B, Type, сер, C</t>
         </is>
       </c>
       <c r="H14" t="n">
         <v>2</v>
       </c>
       <c r="I14" s="1" t="n">
-        <v>45340</v>
+        <v>45341</v>
       </c>
       <c r="J14" t="inlineStr">
         <is>
@@ -1039,7 +1039,7 @@
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>легк б/к сер</t>
+          <t>сер легк б/к</t>
         </is>
       </c>
       <c r="E15" t="inlineStr">
@@ -1054,14 +1054,14 @@
       </c>
       <c r="G15" t="inlineStr">
         <is>
-          <t>202B, Type, H, C, сер, LS-2</t>
+          <t>202B, Type, сер, LS-2, H, C</t>
         </is>
       </c>
       <c r="H15" t="n">
         <v>2</v>
       </c>
       <c r="I15" s="1" t="n">
-        <v>45340</v>
+        <v>45341</v>
       </c>
       <c r="J15" t="inlineStr">
         <is>
@@ -1082,7 +1082,7 @@
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>легк б/к сер</t>
+          <t>сер легк б/к</t>
         </is>
       </c>
       <c r="E16" t="inlineStr">
@@ -1097,14 +1097,14 @@
       </c>
       <c r="G16" t="inlineStr">
         <is>
-          <t>202B, Type, H, C, сер, LS-2</t>
+          <t>202B, Type, сер, LS-2, H, C</t>
         </is>
       </c>
       <c r="H16" t="n">
         <v>2</v>
       </c>
       <c r="I16" s="1" t="n">
-        <v>45340</v>
+        <v>45341</v>
       </c>
       <c r="J16" t="inlineStr">
         <is>
@@ -1125,7 +1125,7 @@
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>8 сх сер</t>
+          <t>8 сер сх</t>
         </is>
       </c>
       <c r="E17" t="inlineStr">
@@ -1140,14 +1140,14 @@
       </c>
       <c r="G17" t="inlineStr">
         <is>
-          <t>202B, Type, H, C, сер, LS-2</t>
+          <t>202B, Type, сер, LS-2, H, C</t>
         </is>
       </c>
       <c r="H17" t="n">
         <v>2</v>
       </c>
       <c r="I17" s="1" t="n">
-        <v>45340</v>
+        <v>45341</v>
       </c>
       <c r="J17" t="inlineStr">
         <is>
@@ -1168,7 +1168,7 @@
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>легк сер</t>
+          <t>сер легк</t>
         </is>
       </c>
       <c r="E18" t="inlineStr">
@@ -1183,14 +1183,14 @@
       </c>
       <c r="G18" t="inlineStr">
         <is>
-          <t>б/к, груз, сер</t>
+          <t>сер, б/к, груз</t>
         </is>
       </c>
       <c r="H18" t="n">
         <v>2</v>
       </c>
       <c r="I18" s="1" t="n">
-        <v>45340</v>
+        <v>45341</v>
       </c>
       <c r="J18" t="inlineStr">
         <is>
@@ -1211,7 +1211,7 @@
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>легк сер</t>
+          <t>сер легк</t>
         </is>
       </c>
       <c r="E19" t="inlineStr">
@@ -1226,14 +1226,14 @@
       </c>
       <c r="G19" t="inlineStr">
         <is>
-          <t>б/к, груз, сер</t>
+          <t>сер, б/к, груз</t>
         </is>
       </c>
       <c r="H19" t="n">
         <v>2</v>
       </c>
       <c r="I19" s="1" t="n">
-        <v>45340</v>
+        <v>45341</v>
       </c>
       <c r="J19" t="inlineStr">
         <is>
@@ -1254,7 +1254,7 @@
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>легк сер</t>
+          <t>сер легк</t>
         </is>
       </c>
       <c r="E20" t="inlineStr">
@@ -1269,14 +1269,14 @@
       </c>
       <c r="G20" t="inlineStr">
         <is>
-          <t>б/к, груз, сер</t>
+          <t>сер, б/к, груз</t>
         </is>
       </c>
       <c r="H20" t="n">
         <v>2</v>
       </c>
       <c r="I20" s="1" t="n">
-        <v>45340</v>
+        <v>45341</v>
       </c>
       <c r="J20" t="inlineStr">
         <is>
@@ -1297,7 +1297,7 @@
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>легк сер</t>
+          <t>сер легк</t>
         </is>
       </c>
       <c r="E21" t="inlineStr">
@@ -1312,14 +1312,14 @@
       </c>
       <c r="G21" t="inlineStr">
         <is>
-          <t>б/к, груз, сер</t>
+          <t>сер, б/к, груз</t>
         </is>
       </c>
       <c r="H21" t="n">
         <v>2</v>
       </c>
       <c r="I21" s="1" t="n">
-        <v>45340</v>
+        <v>45341</v>
       </c>
       <c r="J21" t="inlineStr">
         <is>
@@ -1340,7 +1340,7 @@
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>легк сер</t>
+          <t>сер легк</t>
         </is>
       </c>
       <c r="E22" t="inlineStr">
@@ -1355,14 +1355,14 @@
       </c>
       <c r="G22" t="inlineStr">
         <is>
-          <t>легк, б/к, сер</t>
+          <t>сер, легк, б/к</t>
         </is>
       </c>
       <c r="H22" t="n">
         <v>2</v>
       </c>
       <c r="I22" s="1" t="n">
-        <v>45340</v>
+        <v>45341</v>
       </c>
       <c r="J22" t="inlineStr">
         <is>
@@ -1383,14 +1383,14 @@
       </c>
       <c r="G23" t="inlineStr">
         <is>
-          <t>легк, б/к, сер</t>
+          <t>сер, легк, б/к</t>
         </is>
       </c>
       <c r="H23" t="n">
         <v>2</v>
       </c>
       <c r="I23" s="1" t="n">
-        <v>45340</v>
+        <v>45341</v>
       </c>
       <c r="J23" t="inlineStr">
         <is>
@@ -1411,14 +1411,14 @@
       </c>
       <c r="G24" t="inlineStr">
         <is>
-          <t>легк, сер</t>
+          <t>сер, легк</t>
         </is>
       </c>
       <c r="H24" t="n">
         <v>2</v>
       </c>
       <c r="I24" s="1" t="n">
-        <v>45340</v>
+        <v>45341</v>
       </c>
       <c r="J24" t="inlineStr">
         <is>
@@ -1439,14 +1439,14 @@
       </c>
       <c r="G25" t="inlineStr">
         <is>
-          <t>легк, сер</t>
+          <t>сер, легк</t>
         </is>
       </c>
       <c r="H25" t="n">
         <v>2</v>
       </c>
       <c r="I25" s="1" t="n">
-        <v>45340</v>
+        <v>45341</v>
       </c>
       <c r="J25" t="inlineStr">
         <is>
@@ -1467,14 +1467,14 @@
       </c>
       <c r="G26" t="inlineStr">
         <is>
-          <t>легк, сер</t>
+          <t>сер, легк</t>
         </is>
       </c>
       <c r="H26" t="n">
         <v>2</v>
       </c>
       <c r="I26" s="1" t="n">
-        <v>45340</v>
+        <v>45341</v>
       </c>
       <c r="J26" t="inlineStr">
         <is>
@@ -1495,14 +1495,14 @@
       </c>
       <c r="G27" t="inlineStr">
         <is>
-          <t>легк, сер</t>
+          <t>сер, легк</t>
         </is>
       </c>
       <c r="H27" t="n">
         <v>2</v>
       </c>
       <c r="I27" s="1" t="n">
-        <v>45340</v>
+        <v>45341</v>
       </c>
       <c r="J27" t="inlineStr">
         <is>
@@ -1523,14 +1523,14 @@
       </c>
       <c r="G28" t="inlineStr">
         <is>
-          <t>легк, сер</t>
+          <t>сер, легк</t>
         </is>
       </c>
       <c r="H28" t="n">
         <v>2</v>
       </c>
       <c r="I28" s="1" t="n">
-        <v>45340</v>
+        <v>45341</v>
       </c>
       <c r="J28" t="inlineStr">
         <is>
@@ -1551,14 +1551,14 @@
       </c>
       <c r="G29" t="inlineStr">
         <is>
-          <t>легк, сер</t>
+          <t>сер, легк</t>
         </is>
       </c>
       <c r="H29" t="n">
         <v>2</v>
       </c>
       <c r="I29" s="1" t="n">
-        <v>45340</v>
+        <v>45341</v>
       </c>
       <c r="J29" t="inlineStr">
         <is>
@@ -1579,14 +1579,14 @@
       </c>
       <c r="G30" t="inlineStr">
         <is>
-          <t>легк, сер</t>
+          <t>сер, легк</t>
         </is>
       </c>
       <c r="H30" t="n">
         <v>2</v>
       </c>
       <c r="I30" s="1" t="n">
-        <v>45340</v>
+        <v>45341</v>
       </c>
       <c r="J30" t="inlineStr">
         <is>

</xml_diff>

<commit_message>
10.02/2024 - return to host 19
</commit_message>
<xml_diff>
--- a/src/Tyres.xlsx
+++ b/src/Tyres.xlsx
@@ -480,7 +480,7 @@
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>42 30 сер груз</t>
+          <t>42 30 груз сер</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
@@ -495,7 +495,7 @@
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>42, 30, сер, груз</t>
+          <t>42, 30, груз, сер</t>
         </is>
       </c>
       <c r="H2" t="n">
@@ -523,7 +523,7 @@
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>сер легк б/к</t>
+          <t>легк б/к сер</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
@@ -538,7 +538,7 @@
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>42, 30, сер, груз</t>
+          <t>42, 30, груз, сер</t>
         </is>
       </c>
       <c r="H3" t="n">
@@ -566,7 +566,7 @@
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>сер легк б/к</t>
+          <t>легк б/к сер</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
@@ -581,7 +581,7 @@
       </c>
       <c r="G4" t="inlineStr">
         <is>
-          <t>сер, легк, б/к</t>
+          <t>легк, б/к, сер</t>
         </is>
       </c>
       <c r="H4" t="n">
@@ -609,7 +609,7 @@
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>сер ошип</t>
+          <t>ошип сер</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
@@ -624,7 +624,7 @@
       </c>
       <c r="G5" t="inlineStr">
         <is>
-          <t>сер, легк, б/к</t>
+          <t>легк, б/к, сер</t>
         </is>
       </c>
       <c r="H5" t="n">
@@ -652,7 +652,7 @@
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>сер легк</t>
+          <t>легк сер</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
@@ -667,7 +667,7 @@
       </c>
       <c r="G6" t="inlineStr">
         <is>
-          <t>сер, ошип</t>
+          <t>ошип, сер</t>
         </is>
       </c>
       <c r="H6" t="n">
@@ -695,7 +695,7 @@
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>сер легк</t>
+          <t>легк сер</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
@@ -710,7 +710,7 @@
       </c>
       <c r="G7" t="inlineStr">
         <is>
-          <t>сер, легк</t>
+          <t>легк, сер</t>
         </is>
       </c>
       <c r="H7" t="n">
@@ -738,7 +738,7 @@
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>сер легк</t>
+          <t>легк сер</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
@@ -753,7 +753,7 @@
       </c>
       <c r="G8" t="inlineStr">
         <is>
-          <t>сер, легк</t>
+          <t>легк, сер</t>
         </is>
       </c>
       <c r="H8" t="n">
@@ -781,7 +781,7 @@
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>сер легк</t>
+          <t>легк сер</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
@@ -796,7 +796,7 @@
       </c>
       <c r="G9" t="inlineStr">
         <is>
-          <t>сер, легк</t>
+          <t>легк, сер</t>
         </is>
       </c>
       <c r="H9" t="n">
@@ -824,7 +824,7 @@
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>210B Type сер H C</t>
+          <t>210B H Type C сер</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
@@ -839,7 +839,7 @@
       </c>
       <c r="G10" t="inlineStr">
         <is>
-          <t>сер, легк</t>
+          <t>легк, сер</t>
         </is>
       </c>
       <c r="H10" t="n">
@@ -867,7 +867,7 @@
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>Type сер LS-2 груз</t>
+          <t>груз Type LS-2 сер</t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
@@ -882,7 +882,7 @@
       </c>
       <c r="G11" t="inlineStr">
         <is>
-          <t>210B, Type, сер, H, C</t>
+          <t>210B, H, Type, C, сер</t>
         </is>
       </c>
       <c r="H11" t="n">
@@ -910,7 +910,7 @@
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>202B Type сер C</t>
+          <t>202B Type C сер</t>
         </is>
       </c>
       <c r="E12" t="inlineStr">
@@ -925,7 +925,7 @@
       </c>
       <c r="G12" t="inlineStr">
         <is>
-          <t>210B, Type, сер, H, C</t>
+          <t>210B, H, Type, C, сер</t>
         </is>
       </c>
       <c r="H12" t="n">
@@ -953,7 +953,7 @@
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>202B Type сер LS-2 H C</t>
+          <t>202B H Type C LS-2 сер</t>
         </is>
       </c>
       <c r="E13" t="inlineStr">
@@ -968,7 +968,7 @@
       </c>
       <c r="G13" t="inlineStr">
         <is>
-          <t>Type, сер, LS-2, груз</t>
+          <t>груз, Type, LS-2, сер</t>
         </is>
       </c>
       <c r="H13" t="n">
@@ -996,7 +996,7 @@
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>сер б/к груз</t>
+          <t>груз б/к сер</t>
         </is>
       </c>
       <c r="E14" t="inlineStr">
@@ -1011,7 +1011,7 @@
       </c>
       <c r="G14" t="inlineStr">
         <is>
-          <t>202B, Type, сер, C</t>
+          <t>202B, Type, C, сер</t>
         </is>
       </c>
       <c r="H14" t="n">
@@ -1039,7 +1039,7 @@
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>сер легк б/к</t>
+          <t>легк б/к сер</t>
         </is>
       </c>
       <c r="E15" t="inlineStr">
@@ -1054,7 +1054,7 @@
       </c>
       <c r="G15" t="inlineStr">
         <is>
-          <t>202B, Type, сер, LS-2, H, C</t>
+          <t>202B, H, Type, C, LS-2, сер</t>
         </is>
       </c>
       <c r="H15" t="n">
@@ -1082,7 +1082,7 @@
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>сер легк б/к</t>
+          <t>легк б/к сер</t>
         </is>
       </c>
       <c r="E16" t="inlineStr">
@@ -1097,7 +1097,7 @@
       </c>
       <c r="G16" t="inlineStr">
         <is>
-          <t>202B, Type, сер, LS-2, H, C</t>
+          <t>202B, H, Type, C, LS-2, сер</t>
         </is>
       </c>
       <c r="H16" t="n">
@@ -1125,7 +1125,7 @@
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>8 сер сх</t>
+          <t>8 сх сер</t>
         </is>
       </c>
       <c r="E17" t="inlineStr">
@@ -1140,7 +1140,7 @@
       </c>
       <c r="G17" t="inlineStr">
         <is>
-          <t>202B, Type, сер, LS-2, H, C</t>
+          <t>202B, H, Type, C, LS-2, сер</t>
         </is>
       </c>
       <c r="H17" t="n">
@@ -1168,7 +1168,7 @@
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>сер легк</t>
+          <t>легк сер</t>
         </is>
       </c>
       <c r="E18" t="inlineStr">
@@ -1183,7 +1183,7 @@
       </c>
       <c r="G18" t="inlineStr">
         <is>
-          <t>сер, б/к, груз</t>
+          <t>груз, б/к, сер</t>
         </is>
       </c>
       <c r="H18" t="n">
@@ -1211,7 +1211,7 @@
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>сер легк</t>
+          <t>легк сер</t>
         </is>
       </c>
       <c r="E19" t="inlineStr">
@@ -1226,7 +1226,7 @@
       </c>
       <c r="G19" t="inlineStr">
         <is>
-          <t>сер, б/к, груз</t>
+          <t>груз, б/к, сер</t>
         </is>
       </c>
       <c r="H19" t="n">
@@ -1254,7 +1254,7 @@
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>сер легк</t>
+          <t>легк сер</t>
         </is>
       </c>
       <c r="E20" t="inlineStr">
@@ -1269,7 +1269,7 @@
       </c>
       <c r="G20" t="inlineStr">
         <is>
-          <t>сер, б/к, груз</t>
+          <t>груз, б/к, сер</t>
         </is>
       </c>
       <c r="H20" t="n">
@@ -1297,7 +1297,7 @@
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>сер легк</t>
+          <t>легк сер</t>
         </is>
       </c>
       <c r="E21" t="inlineStr">
@@ -1312,7 +1312,7 @@
       </c>
       <c r="G21" t="inlineStr">
         <is>
-          <t>сер, б/к, груз</t>
+          <t>груз, б/к, сер</t>
         </is>
       </c>
       <c r="H21" t="n">
@@ -1340,7 +1340,7 @@
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>сер легк</t>
+          <t>легк сер</t>
         </is>
       </c>
       <c r="E22" t="inlineStr">
@@ -1355,7 +1355,7 @@
       </c>
       <c r="G22" t="inlineStr">
         <is>
-          <t>сер, легк, б/к</t>
+          <t>легк, б/к, сер</t>
         </is>
       </c>
       <c r="H22" t="n">
@@ -1383,7 +1383,7 @@
       </c>
       <c r="G23" t="inlineStr">
         <is>
-          <t>сер, легк, б/к</t>
+          <t>легк, б/к, сер</t>
         </is>
       </c>
       <c r="H23" t="n">
@@ -1411,7 +1411,7 @@
       </c>
       <c r="G24" t="inlineStr">
         <is>
-          <t>сер, легк</t>
+          <t>легк, сер</t>
         </is>
       </c>
       <c r="H24" t="n">
@@ -1439,7 +1439,7 @@
       </c>
       <c r="G25" t="inlineStr">
         <is>
-          <t>сер, легк</t>
+          <t>легк, сер</t>
         </is>
       </c>
       <c r="H25" t="n">
@@ -1467,7 +1467,7 @@
       </c>
       <c r="G26" t="inlineStr">
         <is>
-          <t>сер, легк</t>
+          <t>легк, сер</t>
         </is>
       </c>
       <c r="H26" t="n">
@@ -1495,7 +1495,7 @@
       </c>
       <c r="G27" t="inlineStr">
         <is>
-          <t>сер, легк</t>
+          <t>легк, сер</t>
         </is>
       </c>
       <c r="H27" t="n">
@@ -1523,7 +1523,7 @@
       </c>
       <c r="G28" t="inlineStr">
         <is>
-          <t>сер, легк</t>
+          <t>легк, сер</t>
         </is>
       </c>
       <c r="H28" t="n">
@@ -1551,7 +1551,7 @@
       </c>
       <c r="G29" t="inlineStr">
         <is>
-          <t>сер, легк</t>
+          <t>легк, сер</t>
         </is>
       </c>
       <c r="H29" t="n">
@@ -1579,7 +1579,7 @@
       </c>
       <c r="G30" t="inlineStr">
         <is>
-          <t>сер, легк</t>
+          <t>легк, сер</t>
         </is>
       </c>
       <c r="H30" t="n">

</xml_diff>

<commit_message>
10.02/2024 - return to host 21
</commit_message>
<xml_diff>
--- a/src/Tyres.xlsx
+++ b/src/Tyres.xlsx
@@ -502,7 +502,7 @@
         <v>2</v>
       </c>
       <c r="I2" s="1" t="n">
-        <v>45341</v>
+        <v>45342</v>
       </c>
       <c r="J2" t="inlineStr">
         <is>
@@ -523,7 +523,7 @@
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>легк б/к сер</t>
+          <t>б/к легк сер</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
@@ -545,7 +545,7 @@
         <v>2</v>
       </c>
       <c r="I3" s="1" t="n">
-        <v>45341</v>
+        <v>45342</v>
       </c>
       <c r="J3" t="inlineStr">
         <is>
@@ -566,7 +566,7 @@
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>легк б/к сер</t>
+          <t>б/к легк сер</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
@@ -581,14 +581,14 @@
       </c>
       <c r="G4" t="inlineStr">
         <is>
-          <t>легк, б/к, сер</t>
+          <t>б/к, легк, сер</t>
         </is>
       </c>
       <c r="H4" t="n">
         <v>2</v>
       </c>
       <c r="I4" s="1" t="n">
-        <v>45341</v>
+        <v>45342</v>
       </c>
       <c r="J4" t="inlineStr">
         <is>
@@ -624,14 +624,14 @@
       </c>
       <c r="G5" t="inlineStr">
         <is>
-          <t>легк, б/к, сер</t>
+          <t>б/к, легк, сер</t>
         </is>
       </c>
       <c r="H5" t="n">
         <v>2</v>
       </c>
       <c r="I5" s="1" t="n">
-        <v>45341</v>
+        <v>45342</v>
       </c>
       <c r="J5" t="inlineStr">
         <is>
@@ -674,7 +674,7 @@
         <v>2</v>
       </c>
       <c r="I6" s="1" t="n">
-        <v>45341</v>
+        <v>45342</v>
       </c>
       <c r="J6" t="inlineStr">
         <is>
@@ -717,7 +717,7 @@
         <v>2</v>
       </c>
       <c r="I7" s="1" t="n">
-        <v>45341</v>
+        <v>45342</v>
       </c>
       <c r="J7" t="inlineStr">
         <is>
@@ -760,7 +760,7 @@
         <v>2</v>
       </c>
       <c r="I8" s="1" t="n">
-        <v>45341</v>
+        <v>45342</v>
       </c>
       <c r="J8" t="inlineStr">
         <is>
@@ -803,7 +803,7 @@
         <v>2</v>
       </c>
       <c r="I9" s="1" t="n">
-        <v>45341</v>
+        <v>45342</v>
       </c>
       <c r="J9" t="inlineStr">
         <is>
@@ -846,7 +846,7 @@
         <v>2</v>
       </c>
       <c r="I10" s="1" t="n">
-        <v>45341</v>
+        <v>45342</v>
       </c>
       <c r="J10" t="inlineStr">
         <is>
@@ -867,7 +867,7 @@
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>груз Type LS-2 сер</t>
+          <t>Type LS-2 груз сер</t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
@@ -889,7 +889,7 @@
         <v>2</v>
       </c>
       <c r="I11" s="1" t="n">
-        <v>45341</v>
+        <v>45342</v>
       </c>
       <c r="J11" t="inlineStr">
         <is>
@@ -932,7 +932,7 @@
         <v>2</v>
       </c>
       <c r="I12" s="1" t="n">
-        <v>45341</v>
+        <v>45342</v>
       </c>
       <c r="J12" t="inlineStr">
         <is>
@@ -953,7 +953,7 @@
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>202B H Type C LS-2 сер</t>
+          <t>202B H Type LS-2 C сер</t>
         </is>
       </c>
       <c r="E13" t="inlineStr">
@@ -968,14 +968,14 @@
       </c>
       <c r="G13" t="inlineStr">
         <is>
-          <t>груз, Type, LS-2, сер</t>
+          <t>Type, LS-2, груз, сер</t>
         </is>
       </c>
       <c r="H13" t="n">
         <v>2</v>
       </c>
       <c r="I13" s="1" t="n">
-        <v>45341</v>
+        <v>45342</v>
       </c>
       <c r="J13" t="inlineStr">
         <is>
@@ -996,7 +996,7 @@
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>груз б/к сер</t>
+          <t>б/к груз сер</t>
         </is>
       </c>
       <c r="E14" t="inlineStr">
@@ -1018,7 +1018,7 @@
         <v>2</v>
       </c>
       <c r="I14" s="1" t="n">
-        <v>45341</v>
+        <v>45342</v>
       </c>
       <c r="J14" t="inlineStr">
         <is>
@@ -1039,7 +1039,7 @@
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>легк б/к сер</t>
+          <t>б/к легк сер</t>
         </is>
       </c>
       <c r="E15" t="inlineStr">
@@ -1054,14 +1054,14 @@
       </c>
       <c r="G15" t="inlineStr">
         <is>
-          <t>202B, H, Type, C, LS-2, сер</t>
+          <t>202B, H, Type, LS-2, C, сер</t>
         </is>
       </c>
       <c r="H15" t="n">
         <v>2</v>
       </c>
       <c r="I15" s="1" t="n">
-        <v>45341</v>
+        <v>45342</v>
       </c>
       <c r="J15" t="inlineStr">
         <is>
@@ -1082,7 +1082,7 @@
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>легк б/к сер</t>
+          <t>б/к легк сер</t>
         </is>
       </c>
       <c r="E16" t="inlineStr">
@@ -1097,14 +1097,14 @@
       </c>
       <c r="G16" t="inlineStr">
         <is>
-          <t>202B, H, Type, C, LS-2, сер</t>
+          <t>202B, H, Type, LS-2, C, сер</t>
         </is>
       </c>
       <c r="H16" t="n">
         <v>2</v>
       </c>
       <c r="I16" s="1" t="n">
-        <v>45341</v>
+        <v>45342</v>
       </c>
       <c r="J16" t="inlineStr">
         <is>
@@ -1125,7 +1125,7 @@
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>8 сх сер</t>
+          <t>8 сер сх</t>
         </is>
       </c>
       <c r="E17" t="inlineStr">
@@ -1140,14 +1140,14 @@
       </c>
       <c r="G17" t="inlineStr">
         <is>
-          <t>202B, H, Type, C, LS-2, сер</t>
+          <t>202B, H, Type, LS-2, C, сер</t>
         </is>
       </c>
       <c r="H17" t="n">
         <v>2</v>
       </c>
       <c r="I17" s="1" t="n">
-        <v>45341</v>
+        <v>45342</v>
       </c>
       <c r="J17" t="inlineStr">
         <is>
@@ -1183,14 +1183,14 @@
       </c>
       <c r="G18" t="inlineStr">
         <is>
-          <t>груз, б/к, сер</t>
+          <t>б/к, груз, сер</t>
         </is>
       </c>
       <c r="H18" t="n">
         <v>2</v>
       </c>
       <c r="I18" s="1" t="n">
-        <v>45341</v>
+        <v>45342</v>
       </c>
       <c r="J18" t="inlineStr">
         <is>
@@ -1226,14 +1226,14 @@
       </c>
       <c r="G19" t="inlineStr">
         <is>
-          <t>груз, б/к, сер</t>
+          <t>б/к, груз, сер</t>
         </is>
       </c>
       <c r="H19" t="n">
         <v>2</v>
       </c>
       <c r="I19" s="1" t="n">
-        <v>45341</v>
+        <v>45342</v>
       </c>
       <c r="J19" t="inlineStr">
         <is>
@@ -1269,14 +1269,14 @@
       </c>
       <c r="G20" t="inlineStr">
         <is>
-          <t>груз, б/к, сер</t>
+          <t>б/к, груз, сер</t>
         </is>
       </c>
       <c r="H20" t="n">
         <v>2</v>
       </c>
       <c r="I20" s="1" t="n">
-        <v>45341</v>
+        <v>45342</v>
       </c>
       <c r="J20" t="inlineStr">
         <is>
@@ -1312,14 +1312,14 @@
       </c>
       <c r="G21" t="inlineStr">
         <is>
-          <t>груз, б/к, сер</t>
+          <t>б/к, груз, сер</t>
         </is>
       </c>
       <c r="H21" t="n">
         <v>2</v>
       </c>
       <c r="I21" s="1" t="n">
-        <v>45341</v>
+        <v>45342</v>
       </c>
       <c r="J21" t="inlineStr">
         <is>
@@ -1355,14 +1355,14 @@
       </c>
       <c r="G22" t="inlineStr">
         <is>
-          <t>легк, б/к, сер</t>
+          <t>б/к, легк, сер</t>
         </is>
       </c>
       <c r="H22" t="n">
         <v>2</v>
       </c>
       <c r="I22" s="1" t="n">
-        <v>45341</v>
+        <v>45342</v>
       </c>
       <c r="J22" t="inlineStr">
         <is>
@@ -1383,14 +1383,14 @@
       </c>
       <c r="G23" t="inlineStr">
         <is>
-          <t>легк, б/к, сер</t>
+          <t>б/к, легк, сер</t>
         </is>
       </c>
       <c r="H23" t="n">
         <v>2</v>
       </c>
       <c r="I23" s="1" t="n">
-        <v>45341</v>
+        <v>45342</v>
       </c>
       <c r="J23" t="inlineStr">
         <is>
@@ -1418,7 +1418,7 @@
         <v>2</v>
       </c>
       <c r="I24" s="1" t="n">
-        <v>45341</v>
+        <v>45342</v>
       </c>
       <c r="J24" t="inlineStr">
         <is>
@@ -1446,7 +1446,7 @@
         <v>2</v>
       </c>
       <c r="I25" s="1" t="n">
-        <v>45341</v>
+        <v>45342</v>
       </c>
       <c r="J25" t="inlineStr">
         <is>
@@ -1474,7 +1474,7 @@
         <v>2</v>
       </c>
       <c r="I26" s="1" t="n">
-        <v>45341</v>
+        <v>45342</v>
       </c>
       <c r="J26" t="inlineStr">
         <is>
@@ -1502,7 +1502,7 @@
         <v>2</v>
       </c>
       <c r="I27" s="1" t="n">
-        <v>45341</v>
+        <v>45342</v>
       </c>
       <c r="J27" t="inlineStr">
         <is>
@@ -1530,7 +1530,7 @@
         <v>2</v>
       </c>
       <c r="I28" s="1" t="n">
-        <v>45341</v>
+        <v>45342</v>
       </c>
       <c r="J28" t="inlineStr">
         <is>
@@ -1558,7 +1558,7 @@
         <v>2</v>
       </c>
       <c r="I29" s="1" t="n">
-        <v>45341</v>
+        <v>45342</v>
       </c>
       <c r="J29" t="inlineStr">
         <is>
@@ -1586,7 +1586,7 @@
         <v>2</v>
       </c>
       <c r="I30" s="1" t="n">
-        <v>45341</v>
+        <v>45342</v>
       </c>
       <c r="J30" t="inlineStr">
         <is>

</xml_diff>

<commit_message>
10.02/2024 - return to host 22
</commit_message>
<xml_diff>
--- a/src/Tyres.xlsx
+++ b/src/Tyres.xlsx
@@ -480,7 +480,7 @@
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>42 30 груз сер</t>
+          <t>30 42 сер груз</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
@@ -495,7 +495,7 @@
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>42, 30, груз, сер</t>
+          <t>30, 42, сер, груз</t>
         </is>
       </c>
       <c r="H2" t="n">
@@ -523,7 +523,7 @@
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>б/к легк сер</t>
+          <t>сер легк б/к</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
@@ -538,7 +538,7 @@
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>42, 30, груз, сер</t>
+          <t>30, 42, сер, груз</t>
         </is>
       </c>
       <c r="H3" t="n">
@@ -566,7 +566,7 @@
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>б/к легк сер</t>
+          <t>сер легк б/к</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
@@ -581,7 +581,7 @@
       </c>
       <c r="G4" t="inlineStr">
         <is>
-          <t>б/к, легк, сер</t>
+          <t>сер, легк, б/к</t>
         </is>
       </c>
       <c r="H4" t="n">
@@ -609,7 +609,7 @@
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>ошип сер</t>
+          <t>сер ошип</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
@@ -624,7 +624,7 @@
       </c>
       <c r="G5" t="inlineStr">
         <is>
-          <t>б/к, легк, сер</t>
+          <t>сер, легк, б/к</t>
         </is>
       </c>
       <c r="H5" t="n">
@@ -652,7 +652,7 @@
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>легк сер</t>
+          <t>сер легк</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
@@ -667,7 +667,7 @@
       </c>
       <c r="G6" t="inlineStr">
         <is>
-          <t>ошип, сер</t>
+          <t>сер, ошип</t>
         </is>
       </c>
       <c r="H6" t="n">
@@ -695,7 +695,7 @@
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>легк сер</t>
+          <t>сер легк</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
@@ -710,7 +710,7 @@
       </c>
       <c r="G7" t="inlineStr">
         <is>
-          <t>легк, сер</t>
+          <t>сер, легк</t>
         </is>
       </c>
       <c r="H7" t="n">
@@ -738,7 +738,7 @@
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>легк сер</t>
+          <t>сер легк</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
@@ -753,7 +753,7 @@
       </c>
       <c r="G8" t="inlineStr">
         <is>
-          <t>легк, сер</t>
+          <t>сер, легк</t>
         </is>
       </c>
       <c r="H8" t="n">
@@ -781,7 +781,7 @@
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>легк сер</t>
+          <t>сер легк</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
@@ -796,7 +796,7 @@
       </c>
       <c r="G9" t="inlineStr">
         <is>
-          <t>легк, сер</t>
+          <t>сер, легк</t>
         </is>
       </c>
       <c r="H9" t="n">
@@ -824,7 +824,7 @@
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>210B H Type C сер</t>
+          <t>210B сер Type H C</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
@@ -839,7 +839,7 @@
       </c>
       <c r="G10" t="inlineStr">
         <is>
-          <t>легк, сер</t>
+          <t>сер, легк</t>
         </is>
       </c>
       <c r="H10" t="n">
@@ -867,7 +867,7 @@
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>Type LS-2 груз сер</t>
+          <t>сер груз Type LS-2</t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
@@ -882,7 +882,7 @@
       </c>
       <c r="G11" t="inlineStr">
         <is>
-          <t>210B, H, Type, C, сер</t>
+          <t>210B, сер, Type, H, C</t>
         </is>
       </c>
       <c r="H11" t="n">
@@ -910,7 +910,7 @@
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>202B Type C сер</t>
+          <t>202B сер Type C</t>
         </is>
       </c>
       <c r="E12" t="inlineStr">
@@ -925,7 +925,7 @@
       </c>
       <c r="G12" t="inlineStr">
         <is>
-          <t>210B, H, Type, C, сер</t>
+          <t>210B, сер, Type, H, C</t>
         </is>
       </c>
       <c r="H12" t="n">
@@ -953,7 +953,7 @@
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>202B H Type LS-2 C сер</t>
+          <t>202B сер Type LS-2 H C</t>
         </is>
       </c>
       <c r="E13" t="inlineStr">
@@ -968,7 +968,7 @@
       </c>
       <c r="G13" t="inlineStr">
         <is>
-          <t>Type, LS-2, груз, сер</t>
+          <t>сер, груз, Type, LS-2</t>
         </is>
       </c>
       <c r="H13" t="n">
@@ -996,7 +996,7 @@
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>б/к груз сер</t>
+          <t>сер груз б/к</t>
         </is>
       </c>
       <c r="E14" t="inlineStr">
@@ -1011,7 +1011,7 @@
       </c>
       <c r="G14" t="inlineStr">
         <is>
-          <t>202B, Type, C, сер</t>
+          <t>202B, сер, Type, C</t>
         </is>
       </c>
       <c r="H14" t="n">
@@ -1039,7 +1039,7 @@
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>б/к легк сер</t>
+          <t>сер легк б/к</t>
         </is>
       </c>
       <c r="E15" t="inlineStr">
@@ -1054,7 +1054,7 @@
       </c>
       <c r="G15" t="inlineStr">
         <is>
-          <t>202B, H, Type, LS-2, C, сер</t>
+          <t>202B, сер, Type, LS-2, H, C</t>
         </is>
       </c>
       <c r="H15" t="n">
@@ -1082,7 +1082,7 @@
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>б/к легк сер</t>
+          <t>сер легк б/к</t>
         </is>
       </c>
       <c r="E16" t="inlineStr">
@@ -1097,7 +1097,7 @@
       </c>
       <c r="G16" t="inlineStr">
         <is>
-          <t>202B, H, Type, LS-2, C, сер</t>
+          <t>202B, сер, Type, LS-2, H, C</t>
         </is>
       </c>
       <c r="H16" t="n">
@@ -1140,7 +1140,7 @@
       </c>
       <c r="G17" t="inlineStr">
         <is>
-          <t>202B, H, Type, LS-2, C, сер</t>
+          <t>202B, сер, Type, LS-2, H, C</t>
         </is>
       </c>
       <c r="H17" t="n">
@@ -1168,7 +1168,7 @@
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>легк сер</t>
+          <t>сер легк</t>
         </is>
       </c>
       <c r="E18" t="inlineStr">
@@ -1183,7 +1183,7 @@
       </c>
       <c r="G18" t="inlineStr">
         <is>
-          <t>б/к, груз, сер</t>
+          <t>сер, груз, б/к</t>
         </is>
       </c>
       <c r="H18" t="n">
@@ -1211,7 +1211,7 @@
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>легк сер</t>
+          <t>сер легк</t>
         </is>
       </c>
       <c r="E19" t="inlineStr">
@@ -1226,7 +1226,7 @@
       </c>
       <c r="G19" t="inlineStr">
         <is>
-          <t>б/к, груз, сер</t>
+          <t>сер, груз, б/к</t>
         </is>
       </c>
       <c r="H19" t="n">
@@ -1254,7 +1254,7 @@
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>легк сер</t>
+          <t>сер легк</t>
         </is>
       </c>
       <c r="E20" t="inlineStr">
@@ -1269,7 +1269,7 @@
       </c>
       <c r="G20" t="inlineStr">
         <is>
-          <t>б/к, груз, сер</t>
+          <t>сер, груз, б/к</t>
         </is>
       </c>
       <c r="H20" t="n">
@@ -1297,7 +1297,7 @@
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>легк сер</t>
+          <t>сер легк</t>
         </is>
       </c>
       <c r="E21" t="inlineStr">
@@ -1312,7 +1312,7 @@
       </c>
       <c r="G21" t="inlineStr">
         <is>
-          <t>б/к, груз, сер</t>
+          <t>сер, груз, б/к</t>
         </is>
       </c>
       <c r="H21" t="n">
@@ -1340,7 +1340,7 @@
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>легк сер</t>
+          <t>сер легк</t>
         </is>
       </c>
       <c r="E22" t="inlineStr">
@@ -1355,7 +1355,7 @@
       </c>
       <c r="G22" t="inlineStr">
         <is>
-          <t>б/к, легк, сер</t>
+          <t>сер, легк, б/к</t>
         </is>
       </c>
       <c r="H22" t="n">
@@ -1383,7 +1383,7 @@
       </c>
       <c r="G23" t="inlineStr">
         <is>
-          <t>б/к, легк, сер</t>
+          <t>сер, легк, б/к</t>
         </is>
       </c>
       <c r="H23" t="n">
@@ -1411,7 +1411,7 @@
       </c>
       <c r="G24" t="inlineStr">
         <is>
-          <t>легк, сер</t>
+          <t>сер, легк</t>
         </is>
       </c>
       <c r="H24" t="n">
@@ -1439,7 +1439,7 @@
       </c>
       <c r="G25" t="inlineStr">
         <is>
-          <t>легк, сер</t>
+          <t>сер, легк</t>
         </is>
       </c>
       <c r="H25" t="n">
@@ -1467,7 +1467,7 @@
       </c>
       <c r="G26" t="inlineStr">
         <is>
-          <t>легк, сер</t>
+          <t>сер, легк</t>
         </is>
       </c>
       <c r="H26" t="n">
@@ -1495,7 +1495,7 @@
       </c>
       <c r="G27" t="inlineStr">
         <is>
-          <t>легк, сер</t>
+          <t>сер, легк</t>
         </is>
       </c>
       <c r="H27" t="n">
@@ -1523,7 +1523,7 @@
       </c>
       <c r="G28" t="inlineStr">
         <is>
-          <t>легк, сер</t>
+          <t>сер, легк</t>
         </is>
       </c>
       <c r="H28" t="n">
@@ -1551,7 +1551,7 @@
       </c>
       <c r="G29" t="inlineStr">
         <is>
-          <t>легк, сер</t>
+          <t>сер, легк</t>
         </is>
       </c>
       <c r="H29" t="n">
@@ -1579,7 +1579,7 @@
       </c>
       <c r="G30" t="inlineStr">
         <is>
-          <t>легк, сер</t>
+          <t>сер, легк</t>
         </is>
       </c>
       <c r="H30" t="n">

</xml_diff>

<commit_message>
10.02/2024 - return to host 29
</commit_message>
<xml_diff>
--- a/src/Tyres.xlsx
+++ b/src/Tyres.xlsx
@@ -465,7 +465,7 @@
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>легк б/к сер</t>
+          <t>легк сер б/к</t>
         </is>
       </c>
     </row>
@@ -482,7 +482,7 @@
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>легк б/к сер</t>
+          <t>легк сер б/к</t>
         </is>
       </c>
     </row>
@@ -584,7 +584,7 @@
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>210B C Type сер H</t>
+          <t>210B C H сер Type</t>
         </is>
       </c>
     </row>
@@ -601,7 +601,7 @@
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>Type груз LS-2 сер</t>
+          <t>LS-2 груз сер Type</t>
         </is>
       </c>
     </row>
@@ -618,7 +618,7 @@
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>202B C Type сер</t>
+          <t>202B C сер Type</t>
         </is>
       </c>
     </row>
@@ -635,7 +635,7 @@
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>202B C Type LS-2 сер H</t>
+          <t>202B C LS-2 H сер Type</t>
         </is>
       </c>
     </row>
@@ -652,7 +652,7 @@
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>груз б/к сер</t>
+          <t>груз сер б/к</t>
         </is>
       </c>
     </row>
@@ -669,7 +669,7 @@
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>легк б/к сер</t>
+          <t>легк сер б/к</t>
         </is>
       </c>
     </row>
@@ -686,7 +686,7 @@
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>легк б/к сер</t>
+          <t>легк сер б/к</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
10.02/2024 - return to host 31
</commit_message>
<xml_diff>
--- a/src/Tyres.xlsx
+++ b/src/Tyres.xlsx
@@ -17,7 +17,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="0"/>
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="yyyy-mm-dd"/>
+  </numFmts>
   <fonts count="1">
     <font>
       <name val="Calibri"/>
@@ -47,8 +49,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
@@ -414,7 +417,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C22"/>
+  <dimension ref="A1:J30"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -433,7 +436,36 @@
           <t xml:space="preserve"> </t>
         </is>
       </c>
-      <c r="C1" t="inlineStr"/>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>Tyre Size</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>Model</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
+        <is>
+          <t>Param</t>
+        </is>
+      </c>
+      <c r="H1" t="inlineStr">
+        <is>
+          <t>Sales value</t>
+        </is>
+      </c>
+      <c r="I1" t="inlineStr">
+        <is>
+          <t>Date_of_sales</t>
+        </is>
+      </c>
+      <c r="J1" t="inlineStr">
+        <is>
+          <t>Contragent</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
@@ -448,7 +480,33 @@
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>42 30 груз сер</t>
+          <t>30 42 сер груз</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>35/65-33</t>
+        </is>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>ФБел-283</t>
+        </is>
+      </c>
+      <c r="G2" t="inlineStr">
+        <is>
+          <t>30, 42, сер, груз</t>
+        </is>
+      </c>
+      <c r="H2" t="n">
+        <v>2</v>
+      </c>
+      <c r="I2" s="1" t="n">
+        <v>45348</v>
+      </c>
+      <c r="J2" t="inlineStr">
+        <is>
+          <t>нет данных</t>
         </is>
       </c>
     </row>
@@ -465,7 +523,33 @@
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>легк сер б/к</t>
+          <t>сер б/к легк</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>35/65-33</t>
+        </is>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>ФБел-283</t>
+        </is>
+      </c>
+      <c r="G3" t="inlineStr">
+        <is>
+          <t>30, 42, сер, груз</t>
+        </is>
+      </c>
+      <c r="H3" t="n">
+        <v>2</v>
+      </c>
+      <c r="I3" s="1" t="n">
+        <v>45348</v>
+      </c>
+      <c r="J3" t="inlineStr">
+        <is>
+          <t>нет данных</t>
         </is>
       </c>
     </row>
@@ -482,7 +566,33 @@
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>легк сер б/к</t>
+          <t>сер б/к легк</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>205/55R16</t>
+        </is>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>BEL-262</t>
+        </is>
+      </c>
+      <c r="G4" t="inlineStr">
+        <is>
+          <t>сер, б/к, легк</t>
+        </is>
+      </c>
+      <c r="H4" t="n">
+        <v>2</v>
+      </c>
+      <c r="I4" s="1" t="n">
+        <v>45348</v>
+      </c>
+      <c r="J4" t="inlineStr">
+        <is>
+          <t>нет данных</t>
         </is>
       </c>
     </row>
@@ -502,6 +612,32 @@
           <t>сер ошип</t>
         </is>
       </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>205/55R16</t>
+        </is>
+      </c>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>BEL-317</t>
+        </is>
+      </c>
+      <c r="G5" t="inlineStr">
+        <is>
+          <t>сер, б/к, легк</t>
+        </is>
+      </c>
+      <c r="H5" t="n">
+        <v>2</v>
+      </c>
+      <c r="I5" s="1" t="n">
+        <v>45348</v>
+      </c>
+      <c r="J5" t="inlineStr">
+        <is>
+          <t>нет данных</t>
+        </is>
+      </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
@@ -516,7 +652,33 @@
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>легк сер</t>
+          <t>сер легк</t>
+        </is>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>205/55R16</t>
+        </is>
+      </c>
+      <c r="F6" t="inlineStr">
+        <is>
+          <t>BEL-317S</t>
+        </is>
+      </c>
+      <c r="G6" t="inlineStr">
+        <is>
+          <t>сер, ошип</t>
+        </is>
+      </c>
+      <c r="H6" t="n">
+        <v>2</v>
+      </c>
+      <c r="I6" s="1" t="n">
+        <v>45348</v>
+      </c>
+      <c r="J6" t="inlineStr">
+        <is>
+          <t>нет данных</t>
         </is>
       </c>
     </row>
@@ -533,7 +695,33 @@
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>легк сер</t>
+          <t>сер легк</t>
+        </is>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>235/75R15</t>
+        </is>
+      </c>
+      <c r="F7" t="inlineStr">
+        <is>
+          <t>BEL-1001</t>
+        </is>
+      </c>
+      <c r="G7" t="inlineStr">
+        <is>
+          <t>сер, легк</t>
+        </is>
+      </c>
+      <c r="H7" t="n">
+        <v>2</v>
+      </c>
+      <c r="I7" s="1" t="n">
+        <v>45348</v>
+      </c>
+      <c r="J7" t="inlineStr">
+        <is>
+          <t>нет данных</t>
         </is>
       </c>
     </row>
@@ -550,7 +738,33 @@
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>легк сер</t>
+          <t>сер легк</t>
+        </is>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>155/65R13</t>
+        </is>
+      </c>
+      <c r="F8" t="inlineStr">
+        <is>
+          <t>BEL-1002</t>
+        </is>
+      </c>
+      <c r="G8" t="inlineStr">
+        <is>
+          <t>сер, легк</t>
+        </is>
+      </c>
+      <c r="H8" t="n">
+        <v>2</v>
+      </c>
+      <c r="I8" s="1" t="n">
+        <v>45348</v>
+      </c>
+      <c r="J8" t="inlineStr">
+        <is>
+          <t>нет данных</t>
         </is>
       </c>
     </row>
@@ -567,7 +781,33 @@
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>легк сер</t>
+          <t>сер легк</t>
+        </is>
+      </c>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>205/55R16</t>
+        </is>
+      </c>
+      <c r="F9" t="inlineStr">
+        <is>
+          <t>BEL-1004</t>
+        </is>
+      </c>
+      <c r="G9" t="inlineStr">
+        <is>
+          <t>сер, легк</t>
+        </is>
+      </c>
+      <c r="H9" t="n">
+        <v>2</v>
+      </c>
+      <c r="I9" s="1" t="n">
+        <v>45348</v>
+      </c>
+      <c r="J9" t="inlineStr">
+        <is>
+          <t>нет данных</t>
         </is>
       </c>
     </row>
@@ -584,7 +824,33 @@
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>210B C H сер Type</t>
+          <t>210B сер C H Type</t>
+        </is>
+      </c>
+      <c r="E10" t="inlineStr">
+        <is>
+          <t>225/50R17</t>
+        </is>
+      </c>
+      <c r="F10" t="inlineStr">
+        <is>
+          <t>BEL-1005</t>
+        </is>
+      </c>
+      <c r="G10" t="inlineStr">
+        <is>
+          <t>сер, легк</t>
+        </is>
+      </c>
+      <c r="H10" t="n">
+        <v>2</v>
+      </c>
+      <c r="I10" s="1" t="n">
+        <v>45348</v>
+      </c>
+      <c r="J10" t="inlineStr">
+        <is>
+          <t>нет данных</t>
         </is>
       </c>
     </row>
@@ -601,7 +867,33 @@
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>LS-2 груз сер Type</t>
+          <t>LS-2 сер Type груз</t>
+        </is>
+      </c>
+      <c r="E11" t="inlineStr">
+        <is>
+          <t>24.00R35</t>
+        </is>
+      </c>
+      <c r="F11" t="inlineStr">
+        <is>
+          <t>Бел-202</t>
+        </is>
+      </c>
+      <c r="G11" t="inlineStr">
+        <is>
+          <t>210B, сер, C, H, Type</t>
+        </is>
+      </c>
+      <c r="H11" t="n">
+        <v>2</v>
+      </c>
+      <c r="I11" s="1" t="n">
+        <v>45348</v>
+      </c>
+      <c r="J11" t="inlineStr">
+        <is>
+          <t>нет данных</t>
         </is>
       </c>
     </row>
@@ -618,7 +910,33 @@
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>202B C сер Type</t>
+          <t>202B сер C Type</t>
+        </is>
+      </c>
+      <c r="E12" t="inlineStr">
+        <is>
+          <t>24.00R35</t>
+        </is>
+      </c>
+      <c r="F12" t="inlineStr">
+        <is>
+          <t>Бел-202</t>
+        </is>
+      </c>
+      <c r="G12" t="inlineStr">
+        <is>
+          <t>210B, сер, C, H, Type</t>
+        </is>
+      </c>
+      <c r="H12" t="n">
+        <v>2</v>
+      </c>
+      <c r="I12" s="1" t="n">
+        <v>45348</v>
+      </c>
+      <c r="J12" t="inlineStr">
+        <is>
+          <t>нет данных</t>
         </is>
       </c>
     </row>
@@ -635,7 +953,33 @@
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>202B C LS-2 H сер Type</t>
+          <t>202B LS-2 сер C H Type</t>
+        </is>
+      </c>
+      <c r="E13" t="inlineStr">
+        <is>
+          <t>24.00R35</t>
+        </is>
+      </c>
+      <c r="F13" t="inlineStr">
+        <is>
+          <t>Бел-212</t>
+        </is>
+      </c>
+      <c r="G13" t="inlineStr">
+        <is>
+          <t>LS-2, сер, Type, груз</t>
+        </is>
+      </c>
+      <c r="H13" t="n">
+        <v>2</v>
+      </c>
+      <c r="I13" s="1" t="n">
+        <v>45348</v>
+      </c>
+      <c r="J13" t="inlineStr">
+        <is>
+          <t>нет данных</t>
         </is>
       </c>
     </row>
@@ -652,7 +996,33 @@
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>груз сер б/к</t>
+          <t>сер б/к груз</t>
+        </is>
+      </c>
+      <c r="E14" t="inlineStr">
+        <is>
+          <t>21.00R35</t>
+        </is>
+      </c>
+      <c r="F14" t="inlineStr">
+        <is>
+          <t>Бел-200</t>
+        </is>
+      </c>
+      <c r="G14" t="inlineStr">
+        <is>
+          <t>202B, сер, C, Type</t>
+        </is>
+      </c>
+      <c r="H14" t="n">
+        <v>2</v>
+      </c>
+      <c r="I14" s="1" t="n">
+        <v>45348</v>
+      </c>
+      <c r="J14" t="inlineStr">
+        <is>
+          <t>нет данных</t>
         </is>
       </c>
     </row>
@@ -669,7 +1039,33 @@
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>легк сер б/к</t>
+          <t>сер б/к легк</t>
+        </is>
+      </c>
+      <c r="E15" t="inlineStr">
+        <is>
+          <t>21.00R35</t>
+        </is>
+      </c>
+      <c r="F15" t="inlineStr">
+        <is>
+          <t>Бел-210</t>
+        </is>
+      </c>
+      <c r="G15" t="inlineStr">
+        <is>
+          <t>202B, LS-2, сер, C, H, Type</t>
+        </is>
+      </c>
+      <c r="H15" t="n">
+        <v>2</v>
+      </c>
+      <c r="I15" s="1" t="n">
+        <v>45348</v>
+      </c>
+      <c r="J15" t="inlineStr">
+        <is>
+          <t>нет данных</t>
         </is>
       </c>
     </row>
@@ -686,7 +1082,33 @@
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>легк сер б/к</t>
+          <t>сер б/к легк</t>
+        </is>
+      </c>
+      <c r="E16" t="inlineStr">
+        <is>
+          <t>21.00R35</t>
+        </is>
+      </c>
+      <c r="F16" t="inlineStr">
+        <is>
+          <t>Бел-210</t>
+        </is>
+      </c>
+      <c r="G16" t="inlineStr">
+        <is>
+          <t>202B, LS-2, сер, C, H, Type</t>
+        </is>
+      </c>
+      <c r="H16" t="n">
+        <v>2</v>
+      </c>
+      <c r="I16" s="1" t="n">
+        <v>45348</v>
+      </c>
+      <c r="J16" t="inlineStr">
+        <is>
+          <t>нет данных</t>
         </is>
       </c>
     </row>
@@ -706,6 +1128,32 @@
           <t>8 сер сх</t>
         </is>
       </c>
+      <c r="E17" t="inlineStr">
+        <is>
+          <t>21.00R35</t>
+        </is>
+      </c>
+      <c r="F17" t="inlineStr">
+        <is>
+          <t>Бел-210</t>
+        </is>
+      </c>
+      <c r="G17" t="inlineStr">
+        <is>
+          <t>202B, LS-2, сер, C, H, Type</t>
+        </is>
+      </c>
+      <c r="H17" t="n">
+        <v>2</v>
+      </c>
+      <c r="I17" s="1" t="n">
+        <v>45348</v>
+      </c>
+      <c r="J17" t="inlineStr">
+        <is>
+          <t>нет данных</t>
+        </is>
+      </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
@@ -720,7 +1168,33 @@
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>легк сер</t>
+          <t>сер легк</t>
+        </is>
+      </c>
+      <c r="E18" t="inlineStr">
+        <is>
+          <t>14.00R20</t>
+        </is>
+      </c>
+      <c r="F18" t="inlineStr">
+        <is>
+          <t>BEL-248</t>
+        </is>
+      </c>
+      <c r="G18" t="inlineStr">
+        <is>
+          <t>сер, б/к, груз</t>
+        </is>
+      </c>
+      <c r="H18" t="n">
+        <v>2</v>
+      </c>
+      <c r="I18" s="1" t="n">
+        <v>45348</v>
+      </c>
+      <c r="J18" t="inlineStr">
+        <is>
+          <t>нет данных</t>
         </is>
       </c>
     </row>
@@ -737,7 +1211,33 @@
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>легк сер</t>
+          <t>сер легк</t>
+        </is>
+      </c>
+      <c r="E19" t="inlineStr">
+        <is>
+          <t>14.00R20</t>
+        </is>
+      </c>
+      <c r="F19" t="inlineStr">
+        <is>
+          <t>BEL-248</t>
+        </is>
+      </c>
+      <c r="G19" t="inlineStr">
+        <is>
+          <t>сер, б/к, груз</t>
+        </is>
+      </c>
+      <c r="H19" t="n">
+        <v>2</v>
+      </c>
+      <c r="I19" s="1" t="n">
+        <v>45348</v>
+      </c>
+      <c r="J19" t="inlineStr">
+        <is>
+          <t>нет данных</t>
         </is>
       </c>
     </row>
@@ -754,7 +1254,33 @@
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>легк сер</t>
+          <t>сер легк</t>
+        </is>
+      </c>
+      <c r="E20" t="inlineStr">
+        <is>
+          <t>14.00R20</t>
+        </is>
+      </c>
+      <c r="F20" t="inlineStr">
+        <is>
+          <t>BEL-248</t>
+        </is>
+      </c>
+      <c r="G20" t="inlineStr">
+        <is>
+          <t>сер, б/к, груз</t>
+        </is>
+      </c>
+      <c r="H20" t="n">
+        <v>2</v>
+      </c>
+      <c r="I20" s="1" t="n">
+        <v>45348</v>
+      </c>
+      <c r="J20" t="inlineStr">
+        <is>
+          <t>нет данных</t>
         </is>
       </c>
     </row>
@@ -771,7 +1297,33 @@
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>легк сер</t>
+          <t>сер легк</t>
+        </is>
+      </c>
+      <c r="E21" t="inlineStr">
+        <is>
+          <t>14.00R20</t>
+        </is>
+      </c>
+      <c r="F21" t="inlineStr">
+        <is>
+          <t>BEL-248</t>
+        </is>
+      </c>
+      <c r="G21" t="inlineStr">
+        <is>
+          <t>сер, б/к, груз</t>
+        </is>
+      </c>
+      <c r="H21" t="n">
+        <v>2</v>
+      </c>
+      <c r="I21" s="1" t="n">
+        <v>45348</v>
+      </c>
+      <c r="J21" t="inlineStr">
+        <is>
+          <t>нет данных</t>
         </is>
       </c>
     </row>
@@ -788,7 +1340,257 @@
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>легк сер</t>
+          <t>сер легк</t>
+        </is>
+      </c>
+      <c r="E22" t="inlineStr">
+        <is>
+          <t>175/70R13</t>
+        </is>
+      </c>
+      <c r="F22" t="inlineStr">
+        <is>
+          <t>Бел-103</t>
+        </is>
+      </c>
+      <c r="G22" t="inlineStr">
+        <is>
+          <t>сер, б/к, легк</t>
+        </is>
+      </c>
+      <c r="H22" t="n">
+        <v>2</v>
+      </c>
+      <c r="I22" s="1" t="n">
+        <v>45348</v>
+      </c>
+      <c r="J22" t="inlineStr">
+        <is>
+          <t>нет данных</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="E23" t="inlineStr">
+        <is>
+          <t>175/70R13</t>
+        </is>
+      </c>
+      <c r="F23" t="inlineStr">
+        <is>
+          <t>Бел-100</t>
+        </is>
+      </c>
+      <c r="G23" t="inlineStr">
+        <is>
+          <t>сер, б/к, легк</t>
+        </is>
+      </c>
+      <c r="H23" t="n">
+        <v>2</v>
+      </c>
+      <c r="I23" s="1" t="n">
+        <v>45348</v>
+      </c>
+      <c r="J23" t="inlineStr">
+        <is>
+          <t>нет данных</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="E24" t="inlineStr">
+        <is>
+          <t>195/65R15</t>
+        </is>
+      </c>
+      <c r="F24" t="inlineStr">
+        <is>
+          <t>Бел-119</t>
+        </is>
+      </c>
+      <c r="G24" t="inlineStr">
+        <is>
+          <t>сер, легк</t>
+        </is>
+      </c>
+      <c r="H24" t="n">
+        <v>2</v>
+      </c>
+      <c r="I24" s="1" t="n">
+        <v>45348</v>
+      </c>
+      <c r="J24" t="inlineStr">
+        <is>
+          <t>нет данных</t>
+        </is>
+      </c>
+    </row>
+    <row r="25">
+      <c r="E25" t="inlineStr">
+        <is>
+          <t>195/65R15</t>
+        </is>
+      </c>
+      <c r="F25" t="inlineStr">
+        <is>
+          <t>Бел-119</t>
+        </is>
+      </c>
+      <c r="G25" t="inlineStr">
+        <is>
+          <t>сер, легк</t>
+        </is>
+      </c>
+      <c r="H25" t="n">
+        <v>2</v>
+      </c>
+      <c r="I25" s="1" t="n">
+        <v>45348</v>
+      </c>
+      <c r="J25" t="inlineStr">
+        <is>
+          <t>нет данных</t>
+        </is>
+      </c>
+    </row>
+    <row r="26">
+      <c r="E26" t="inlineStr">
+        <is>
+          <t>195/65R15</t>
+        </is>
+      </c>
+      <c r="F26" t="inlineStr">
+        <is>
+          <t>Бел-119</t>
+        </is>
+      </c>
+      <c r="G26" t="inlineStr">
+        <is>
+          <t>сер, легк</t>
+        </is>
+      </c>
+      <c r="H26" t="n">
+        <v>2</v>
+      </c>
+      <c r="I26" s="1" t="n">
+        <v>45348</v>
+      </c>
+      <c r="J26" t="inlineStr">
+        <is>
+          <t>нет данных</t>
+        </is>
+      </c>
+    </row>
+    <row r="27">
+      <c r="E27" t="inlineStr">
+        <is>
+          <t>210/80R16</t>
+        </is>
+      </c>
+      <c r="F27" t="inlineStr">
+        <is>
+          <t>Бел-777</t>
+        </is>
+      </c>
+      <c r="G27" t="inlineStr">
+        <is>
+          <t>сер, легк</t>
+        </is>
+      </c>
+      <c r="H27" t="n">
+        <v>2</v>
+      </c>
+      <c r="I27" s="1" t="n">
+        <v>45348</v>
+      </c>
+      <c r="J27" t="inlineStr">
+        <is>
+          <t>нет данных</t>
+        </is>
+      </c>
+    </row>
+    <row r="28">
+      <c r="E28" t="inlineStr">
+        <is>
+          <t>215/65R16C</t>
+        </is>
+      </c>
+      <c r="F28" t="inlineStr">
+        <is>
+          <t>Бел-1000</t>
+        </is>
+      </c>
+      <c r="G28" t="inlineStr">
+        <is>
+          <t>сер, легк</t>
+        </is>
+      </c>
+      <c r="H28" t="n">
+        <v>2</v>
+      </c>
+      <c r="I28" s="1" t="n">
+        <v>45348</v>
+      </c>
+      <c r="J28" t="inlineStr">
+        <is>
+          <t>нет данных</t>
+        </is>
+      </c>
+    </row>
+    <row r="29">
+      <c r="E29" t="inlineStr">
+        <is>
+          <t>205/55R16</t>
+        </is>
+      </c>
+      <c r="F29" t="inlineStr">
+        <is>
+          <t>Бел-1001</t>
+        </is>
+      </c>
+      <c r="G29" t="inlineStr">
+        <is>
+          <t>сер, легк</t>
+        </is>
+      </c>
+      <c r="H29" t="n">
+        <v>2</v>
+      </c>
+      <c r="I29" s="1" t="n">
+        <v>45348</v>
+      </c>
+      <c r="J29" t="inlineStr">
+        <is>
+          <t>нет данных</t>
+        </is>
+      </c>
+    </row>
+    <row r="30">
+      <c r="E30" t="inlineStr">
+        <is>
+          <t>225/50R17</t>
+        </is>
+      </c>
+      <c r="F30" t="inlineStr">
+        <is>
+          <t>Бел-1005</t>
+        </is>
+      </c>
+      <c r="G30" t="inlineStr">
+        <is>
+          <t>сер, легк</t>
+        </is>
+      </c>
+      <c r="H30" t="n">
+        <v>2</v>
+      </c>
+      <c r="I30" s="1" t="n">
+        <v>45348</v>
+      </c>
+      <c r="J30" t="inlineStr">
+        <is>
+          <t>нет данных</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
10.02/2024 - return to host 33
</commit_message>
<xml_diff>
--- a/src/Tyres.xlsx
+++ b/src/Tyres.xlsx
@@ -502,7 +502,7 @@
         <v>2</v>
       </c>
       <c r="I2" s="1" t="n">
-        <v>45348</v>
+        <v>45349</v>
       </c>
       <c r="J2" t="inlineStr">
         <is>
@@ -523,7 +523,7 @@
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>сер б/к легк</t>
+          <t>б/к сер легк</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
@@ -545,7 +545,7 @@
         <v>2</v>
       </c>
       <c r="I3" s="1" t="n">
-        <v>45348</v>
+        <v>45349</v>
       </c>
       <c r="J3" t="inlineStr">
         <is>
@@ -566,7 +566,7 @@
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>сер б/к легк</t>
+          <t>б/к сер легк</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
@@ -581,14 +581,14 @@
       </c>
       <c r="G4" t="inlineStr">
         <is>
-          <t>сер, б/к, легк</t>
+          <t>б/к, сер, легк</t>
         </is>
       </c>
       <c r="H4" t="n">
         <v>2</v>
       </c>
       <c r="I4" s="1" t="n">
-        <v>45348</v>
+        <v>45349</v>
       </c>
       <c r="J4" t="inlineStr">
         <is>
@@ -624,14 +624,14 @@
       </c>
       <c r="G5" t="inlineStr">
         <is>
-          <t>сер, б/к, легк</t>
+          <t>б/к, сер, легк</t>
         </is>
       </c>
       <c r="H5" t="n">
         <v>2</v>
       </c>
       <c r="I5" s="1" t="n">
-        <v>45348</v>
+        <v>45349</v>
       </c>
       <c r="J5" t="inlineStr">
         <is>
@@ -674,7 +674,7 @@
         <v>2</v>
       </c>
       <c r="I6" s="1" t="n">
-        <v>45348</v>
+        <v>45349</v>
       </c>
       <c r="J6" t="inlineStr">
         <is>
@@ -717,7 +717,7 @@
         <v>2</v>
       </c>
       <c r="I7" s="1" t="n">
-        <v>45348</v>
+        <v>45349</v>
       </c>
       <c r="J7" t="inlineStr">
         <is>
@@ -760,7 +760,7 @@
         <v>2</v>
       </c>
       <c r="I8" s="1" t="n">
-        <v>45348</v>
+        <v>45349</v>
       </c>
       <c r="J8" t="inlineStr">
         <is>
@@ -803,7 +803,7 @@
         <v>2</v>
       </c>
       <c r="I9" s="1" t="n">
-        <v>45348</v>
+        <v>45349</v>
       </c>
       <c r="J9" t="inlineStr">
         <is>
@@ -824,7 +824,7 @@
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>210B сер C H Type</t>
+          <t>210B сер Type C H</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
@@ -846,7 +846,7 @@
         <v>2</v>
       </c>
       <c r="I10" s="1" t="n">
-        <v>45348</v>
+        <v>45349</v>
       </c>
       <c r="J10" t="inlineStr">
         <is>
@@ -867,7 +867,7 @@
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>LS-2 сер Type груз</t>
+          <t>LS-2 сер груз Type</t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
@@ -882,14 +882,14 @@
       </c>
       <c r="G11" t="inlineStr">
         <is>
-          <t>210B, сер, C, H, Type</t>
+          <t>210B, сер, Type, C, H</t>
         </is>
       </c>
       <c r="H11" t="n">
         <v>2</v>
       </c>
       <c r="I11" s="1" t="n">
-        <v>45348</v>
+        <v>45349</v>
       </c>
       <c r="J11" t="inlineStr">
         <is>
@@ -910,7 +910,7 @@
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>202B сер C Type</t>
+          <t>202B сер Type C</t>
         </is>
       </c>
       <c r="E12" t="inlineStr">
@@ -925,14 +925,14 @@
       </c>
       <c r="G12" t="inlineStr">
         <is>
-          <t>210B, сер, C, H, Type</t>
+          <t>210B, сер, Type, C, H</t>
         </is>
       </c>
       <c r="H12" t="n">
         <v>2</v>
       </c>
       <c r="I12" s="1" t="n">
-        <v>45348</v>
+        <v>45349</v>
       </c>
       <c r="J12" t="inlineStr">
         <is>
@@ -953,7 +953,7 @@
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>202B LS-2 сер C H Type</t>
+          <t>202B LS-2 сер Type C H</t>
         </is>
       </c>
       <c r="E13" t="inlineStr">
@@ -968,14 +968,14 @@
       </c>
       <c r="G13" t="inlineStr">
         <is>
-          <t>LS-2, сер, Type, груз</t>
+          <t>LS-2, сер, груз, Type</t>
         </is>
       </c>
       <c r="H13" t="n">
         <v>2</v>
       </c>
       <c r="I13" s="1" t="n">
-        <v>45348</v>
+        <v>45349</v>
       </c>
       <c r="J13" t="inlineStr">
         <is>
@@ -996,7 +996,7 @@
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>сер б/к груз</t>
+          <t>б/к сер груз</t>
         </is>
       </c>
       <c r="E14" t="inlineStr">
@@ -1011,14 +1011,14 @@
       </c>
       <c r="G14" t="inlineStr">
         <is>
-          <t>202B, сер, C, Type</t>
+          <t>202B, сер, Type, C</t>
         </is>
       </c>
       <c r="H14" t="n">
         <v>2</v>
       </c>
       <c r="I14" s="1" t="n">
-        <v>45348</v>
+        <v>45349</v>
       </c>
       <c r="J14" t="inlineStr">
         <is>
@@ -1039,7 +1039,7 @@
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>сер б/к легк</t>
+          <t>б/к сер легк</t>
         </is>
       </c>
       <c r="E15" t="inlineStr">
@@ -1054,14 +1054,14 @@
       </c>
       <c r="G15" t="inlineStr">
         <is>
-          <t>202B, LS-2, сер, C, H, Type</t>
+          <t>202B, LS-2, сер, Type, C, H</t>
         </is>
       </c>
       <c r="H15" t="n">
         <v>2</v>
       </c>
       <c r="I15" s="1" t="n">
-        <v>45348</v>
+        <v>45349</v>
       </c>
       <c r="J15" t="inlineStr">
         <is>
@@ -1082,7 +1082,7 @@
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>сер б/к легк</t>
+          <t>б/к сер легк</t>
         </is>
       </c>
       <c r="E16" t="inlineStr">
@@ -1097,14 +1097,14 @@
       </c>
       <c r="G16" t="inlineStr">
         <is>
-          <t>202B, LS-2, сер, C, H, Type</t>
+          <t>202B, LS-2, сер, Type, C, H</t>
         </is>
       </c>
       <c r="H16" t="n">
         <v>2</v>
       </c>
       <c r="I16" s="1" t="n">
-        <v>45348</v>
+        <v>45349</v>
       </c>
       <c r="J16" t="inlineStr">
         <is>
@@ -1140,14 +1140,14 @@
       </c>
       <c r="G17" t="inlineStr">
         <is>
-          <t>202B, LS-2, сер, C, H, Type</t>
+          <t>202B, LS-2, сер, Type, C, H</t>
         </is>
       </c>
       <c r="H17" t="n">
         <v>2</v>
       </c>
       <c r="I17" s="1" t="n">
-        <v>45348</v>
+        <v>45349</v>
       </c>
       <c r="J17" t="inlineStr">
         <is>
@@ -1183,14 +1183,14 @@
       </c>
       <c r="G18" t="inlineStr">
         <is>
-          <t>сер, б/к, груз</t>
+          <t>б/к, сер, груз</t>
         </is>
       </c>
       <c r="H18" t="n">
         <v>2</v>
       </c>
       <c r="I18" s="1" t="n">
-        <v>45348</v>
+        <v>45349</v>
       </c>
       <c r="J18" t="inlineStr">
         <is>
@@ -1226,14 +1226,14 @@
       </c>
       <c r="G19" t="inlineStr">
         <is>
-          <t>сер, б/к, груз</t>
+          <t>б/к, сер, груз</t>
         </is>
       </c>
       <c r="H19" t="n">
         <v>2</v>
       </c>
       <c r="I19" s="1" t="n">
-        <v>45348</v>
+        <v>45349</v>
       </c>
       <c r="J19" t="inlineStr">
         <is>
@@ -1269,14 +1269,14 @@
       </c>
       <c r="G20" t="inlineStr">
         <is>
-          <t>сер, б/к, груз</t>
+          <t>б/к, сер, груз</t>
         </is>
       </c>
       <c r="H20" t="n">
         <v>2</v>
       </c>
       <c r="I20" s="1" t="n">
-        <v>45348</v>
+        <v>45349</v>
       </c>
       <c r="J20" t="inlineStr">
         <is>
@@ -1312,14 +1312,14 @@
       </c>
       <c r="G21" t="inlineStr">
         <is>
-          <t>сер, б/к, груз</t>
+          <t>б/к, сер, груз</t>
         </is>
       </c>
       <c r="H21" t="n">
         <v>2</v>
       </c>
       <c r="I21" s="1" t="n">
-        <v>45348</v>
+        <v>45349</v>
       </c>
       <c r="J21" t="inlineStr">
         <is>
@@ -1355,14 +1355,14 @@
       </c>
       <c r="G22" t="inlineStr">
         <is>
-          <t>сер, б/к, легк</t>
+          <t>б/к, сер, легк</t>
         </is>
       </c>
       <c r="H22" t="n">
         <v>2</v>
       </c>
       <c r="I22" s="1" t="n">
-        <v>45348</v>
+        <v>45349</v>
       </c>
       <c r="J22" t="inlineStr">
         <is>
@@ -1383,14 +1383,14 @@
       </c>
       <c r="G23" t="inlineStr">
         <is>
-          <t>сер, б/к, легк</t>
+          <t>б/к, сер, легк</t>
         </is>
       </c>
       <c r="H23" t="n">
         <v>2</v>
       </c>
       <c r="I23" s="1" t="n">
-        <v>45348</v>
+        <v>45349</v>
       </c>
       <c r="J23" t="inlineStr">
         <is>
@@ -1418,7 +1418,7 @@
         <v>2</v>
       </c>
       <c r="I24" s="1" t="n">
-        <v>45348</v>
+        <v>45349</v>
       </c>
       <c r="J24" t="inlineStr">
         <is>
@@ -1446,7 +1446,7 @@
         <v>2</v>
       </c>
       <c r="I25" s="1" t="n">
-        <v>45348</v>
+        <v>45349</v>
       </c>
       <c r="J25" t="inlineStr">
         <is>
@@ -1474,7 +1474,7 @@
         <v>2</v>
       </c>
       <c r="I26" s="1" t="n">
-        <v>45348</v>
+        <v>45349</v>
       </c>
       <c r="J26" t="inlineStr">
         <is>
@@ -1502,7 +1502,7 @@
         <v>2</v>
       </c>
       <c r="I27" s="1" t="n">
-        <v>45348</v>
+        <v>45349</v>
       </c>
       <c r="J27" t="inlineStr">
         <is>
@@ -1530,7 +1530,7 @@
         <v>2</v>
       </c>
       <c r="I28" s="1" t="n">
-        <v>45348</v>
+        <v>45349</v>
       </c>
       <c r="J28" t="inlineStr">
         <is>
@@ -1558,7 +1558,7 @@
         <v>2</v>
       </c>
       <c r="I29" s="1" t="n">
-        <v>45348</v>
+        <v>45349</v>
       </c>
       <c r="J29" t="inlineStr">
         <is>
@@ -1586,7 +1586,7 @@
         <v>2</v>
       </c>
       <c r="I30" s="1" t="n">
-        <v>45348</v>
+        <v>45349</v>
       </c>
       <c r="J30" t="inlineStr">
         <is>

</xml_diff>

<commit_message>
10.02/2024 - return to host 34
</commit_message>
<xml_diff>
--- a/src/Tyres.xlsx
+++ b/src/Tyres.xlsx
@@ -502,7 +502,7 @@
         <v>2</v>
       </c>
       <c r="I2" s="1" t="n">
-        <v>45349</v>
+        <v>45350</v>
       </c>
       <c r="J2" t="inlineStr">
         <is>
@@ -523,7 +523,7 @@
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>б/к сер легк</t>
+          <t>сер легк б/к</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
@@ -545,7 +545,7 @@
         <v>2</v>
       </c>
       <c r="I3" s="1" t="n">
-        <v>45349</v>
+        <v>45350</v>
       </c>
       <c r="J3" t="inlineStr">
         <is>
@@ -566,7 +566,7 @@
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>б/к сер легк</t>
+          <t>сер легк б/к</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
@@ -581,14 +581,14 @@
       </c>
       <c r="G4" t="inlineStr">
         <is>
-          <t>б/к, сер, легк</t>
+          <t>сер, легк, б/к</t>
         </is>
       </c>
       <c r="H4" t="n">
         <v>2</v>
       </c>
       <c r="I4" s="1" t="n">
-        <v>45349</v>
+        <v>45350</v>
       </c>
       <c r="J4" t="inlineStr">
         <is>
@@ -624,14 +624,14 @@
       </c>
       <c r="G5" t="inlineStr">
         <is>
-          <t>б/к, сер, легк</t>
+          <t>сер, легк, б/к</t>
         </is>
       </c>
       <c r="H5" t="n">
         <v>2</v>
       </c>
       <c r="I5" s="1" t="n">
-        <v>45349</v>
+        <v>45350</v>
       </c>
       <c r="J5" t="inlineStr">
         <is>
@@ -674,7 +674,7 @@
         <v>2</v>
       </c>
       <c r="I6" s="1" t="n">
-        <v>45349</v>
+        <v>45350</v>
       </c>
       <c r="J6" t="inlineStr">
         <is>
@@ -717,7 +717,7 @@
         <v>2</v>
       </c>
       <c r="I7" s="1" t="n">
-        <v>45349</v>
+        <v>45350</v>
       </c>
       <c r="J7" t="inlineStr">
         <is>
@@ -760,7 +760,7 @@
         <v>2</v>
       </c>
       <c r="I8" s="1" t="n">
-        <v>45349</v>
+        <v>45350</v>
       </c>
       <c r="J8" t="inlineStr">
         <is>
@@ -803,7 +803,7 @@
         <v>2</v>
       </c>
       <c r="I9" s="1" t="n">
-        <v>45349</v>
+        <v>45350</v>
       </c>
       <c r="J9" t="inlineStr">
         <is>
@@ -824,7 +824,7 @@
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>210B сер Type C H</t>
+          <t>210B H сер C Type</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
@@ -846,7 +846,7 @@
         <v>2</v>
       </c>
       <c r="I10" s="1" t="n">
-        <v>45349</v>
+        <v>45350</v>
       </c>
       <c r="J10" t="inlineStr">
         <is>
@@ -882,14 +882,14 @@
       </c>
       <c r="G11" t="inlineStr">
         <is>
-          <t>210B, сер, Type, C, H</t>
+          <t>210B, H, сер, C, Type</t>
         </is>
       </c>
       <c r="H11" t="n">
         <v>2</v>
       </c>
       <c r="I11" s="1" t="n">
-        <v>45349</v>
+        <v>45350</v>
       </c>
       <c r="J11" t="inlineStr">
         <is>
@@ -910,7 +910,7 @@
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>202B сер Type C</t>
+          <t>202B сер C Type</t>
         </is>
       </c>
       <c r="E12" t="inlineStr">
@@ -925,14 +925,14 @@
       </c>
       <c r="G12" t="inlineStr">
         <is>
-          <t>210B, сер, Type, C, H</t>
+          <t>210B, H, сер, C, Type</t>
         </is>
       </c>
       <c r="H12" t="n">
         <v>2</v>
       </c>
       <c r="I12" s="1" t="n">
-        <v>45349</v>
+        <v>45350</v>
       </c>
       <c r="J12" t="inlineStr">
         <is>
@@ -953,7 +953,7 @@
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>202B LS-2 сер Type C H</t>
+          <t>202B LS-2 H сер C Type</t>
         </is>
       </c>
       <c r="E13" t="inlineStr">
@@ -975,7 +975,7 @@
         <v>2</v>
       </c>
       <c r="I13" s="1" t="n">
-        <v>45349</v>
+        <v>45350</v>
       </c>
       <c r="J13" t="inlineStr">
         <is>
@@ -996,7 +996,7 @@
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>б/к сер груз</t>
+          <t>сер груз б/к</t>
         </is>
       </c>
       <c r="E14" t="inlineStr">
@@ -1011,14 +1011,14 @@
       </c>
       <c r="G14" t="inlineStr">
         <is>
-          <t>202B, сер, Type, C</t>
+          <t>202B, сер, C, Type</t>
         </is>
       </c>
       <c r="H14" t="n">
         <v>2</v>
       </c>
       <c r="I14" s="1" t="n">
-        <v>45349</v>
+        <v>45350</v>
       </c>
       <c r="J14" t="inlineStr">
         <is>
@@ -1039,7 +1039,7 @@
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>б/к сер легк</t>
+          <t>сер легк б/к</t>
         </is>
       </c>
       <c r="E15" t="inlineStr">
@@ -1054,14 +1054,14 @@
       </c>
       <c r="G15" t="inlineStr">
         <is>
-          <t>202B, LS-2, сер, Type, C, H</t>
+          <t>202B, LS-2, H, сер, C, Type</t>
         </is>
       </c>
       <c r="H15" t="n">
         <v>2</v>
       </c>
       <c r="I15" s="1" t="n">
-        <v>45349</v>
+        <v>45350</v>
       </c>
       <c r="J15" t="inlineStr">
         <is>
@@ -1082,7 +1082,7 @@
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>б/к сер легк</t>
+          <t>сер легк б/к</t>
         </is>
       </c>
       <c r="E16" t="inlineStr">
@@ -1097,14 +1097,14 @@
       </c>
       <c r="G16" t="inlineStr">
         <is>
-          <t>202B, LS-2, сер, Type, C, H</t>
+          <t>202B, LS-2, H, сер, C, Type</t>
         </is>
       </c>
       <c r="H16" t="n">
         <v>2</v>
       </c>
       <c r="I16" s="1" t="n">
-        <v>45349</v>
+        <v>45350</v>
       </c>
       <c r="J16" t="inlineStr">
         <is>
@@ -1140,14 +1140,14 @@
       </c>
       <c r="G17" t="inlineStr">
         <is>
-          <t>202B, LS-2, сер, Type, C, H</t>
+          <t>202B, LS-2, H, сер, C, Type</t>
         </is>
       </c>
       <c r="H17" t="n">
         <v>2</v>
       </c>
       <c r="I17" s="1" t="n">
-        <v>45349</v>
+        <v>45350</v>
       </c>
       <c r="J17" t="inlineStr">
         <is>
@@ -1183,14 +1183,14 @@
       </c>
       <c r="G18" t="inlineStr">
         <is>
-          <t>б/к, сер, груз</t>
+          <t>сер, груз, б/к</t>
         </is>
       </c>
       <c r="H18" t="n">
         <v>2</v>
       </c>
       <c r="I18" s="1" t="n">
-        <v>45349</v>
+        <v>45350</v>
       </c>
       <c r="J18" t="inlineStr">
         <is>
@@ -1226,14 +1226,14 @@
       </c>
       <c r="G19" t="inlineStr">
         <is>
-          <t>б/к, сер, груз</t>
+          <t>сер, груз, б/к</t>
         </is>
       </c>
       <c r="H19" t="n">
         <v>2</v>
       </c>
       <c r="I19" s="1" t="n">
-        <v>45349</v>
+        <v>45350</v>
       </c>
       <c r="J19" t="inlineStr">
         <is>
@@ -1269,14 +1269,14 @@
       </c>
       <c r="G20" t="inlineStr">
         <is>
-          <t>б/к, сер, груз</t>
+          <t>сер, груз, б/к</t>
         </is>
       </c>
       <c r="H20" t="n">
         <v>2</v>
       </c>
       <c r="I20" s="1" t="n">
-        <v>45349</v>
+        <v>45350</v>
       </c>
       <c r="J20" t="inlineStr">
         <is>
@@ -1312,14 +1312,14 @@
       </c>
       <c r="G21" t="inlineStr">
         <is>
-          <t>б/к, сер, груз</t>
+          <t>сер, груз, б/к</t>
         </is>
       </c>
       <c r="H21" t="n">
         <v>2</v>
       </c>
       <c r="I21" s="1" t="n">
-        <v>45349</v>
+        <v>45350</v>
       </c>
       <c r="J21" t="inlineStr">
         <is>
@@ -1355,14 +1355,14 @@
       </c>
       <c r="G22" t="inlineStr">
         <is>
-          <t>б/к, сер, легк</t>
+          <t>сер, легк, б/к</t>
         </is>
       </c>
       <c r="H22" t="n">
         <v>2</v>
       </c>
       <c r="I22" s="1" t="n">
-        <v>45349</v>
+        <v>45350</v>
       </c>
       <c r="J22" t="inlineStr">
         <is>
@@ -1383,14 +1383,14 @@
       </c>
       <c r="G23" t="inlineStr">
         <is>
-          <t>б/к, сер, легк</t>
+          <t>сер, легк, б/к</t>
         </is>
       </c>
       <c r="H23" t="n">
         <v>2</v>
       </c>
       <c r="I23" s="1" t="n">
-        <v>45349</v>
+        <v>45350</v>
       </c>
       <c r="J23" t="inlineStr">
         <is>
@@ -1418,7 +1418,7 @@
         <v>2</v>
       </c>
       <c r="I24" s="1" t="n">
-        <v>45349</v>
+        <v>45350</v>
       </c>
       <c r="J24" t="inlineStr">
         <is>
@@ -1446,7 +1446,7 @@
         <v>2</v>
       </c>
       <c r="I25" s="1" t="n">
-        <v>45349</v>
+        <v>45350</v>
       </c>
       <c r="J25" t="inlineStr">
         <is>
@@ -1474,7 +1474,7 @@
         <v>2</v>
       </c>
       <c r="I26" s="1" t="n">
-        <v>45349</v>
+        <v>45350</v>
       </c>
       <c r="J26" t="inlineStr">
         <is>
@@ -1502,7 +1502,7 @@
         <v>2</v>
       </c>
       <c r="I27" s="1" t="n">
-        <v>45349</v>
+        <v>45350</v>
       </c>
       <c r="J27" t="inlineStr">
         <is>
@@ -1530,7 +1530,7 @@
         <v>2</v>
       </c>
       <c r="I28" s="1" t="n">
-        <v>45349</v>
+        <v>45350</v>
       </c>
       <c r="J28" t="inlineStr">
         <is>
@@ -1558,7 +1558,7 @@
         <v>2</v>
       </c>
       <c r="I29" s="1" t="n">
-        <v>45349</v>
+        <v>45350</v>
       </c>
       <c r="J29" t="inlineStr">
         <is>
@@ -1586,7 +1586,7 @@
         <v>2</v>
       </c>
       <c r="I30" s="1" t="n">
-        <v>45349</v>
+        <v>45350</v>
       </c>
       <c r="J30" t="inlineStr">
         <is>

</xml_diff>

<commit_message>
10.02/2024 - return to host 35
</commit_message>
<xml_diff>
--- a/src/Tyres.xlsx
+++ b/src/Tyres.xlsx
@@ -480,7 +480,7 @@
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>30 42 сер груз</t>
+          <t>42 30 сер груз</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
@@ -495,7 +495,7 @@
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>30, 42, сер, груз</t>
+          <t>42, 30, сер, груз</t>
         </is>
       </c>
       <c r="H2" t="n">
@@ -523,7 +523,7 @@
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>сер легк б/к</t>
+          <t>легк б/к сер</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
@@ -538,7 +538,7 @@
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>30, 42, сер, груз</t>
+          <t>42, 30, сер, груз</t>
         </is>
       </c>
       <c r="H3" t="n">
@@ -566,7 +566,7 @@
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>сер легк б/к</t>
+          <t>легк б/к сер</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
@@ -581,7 +581,7 @@
       </c>
       <c r="G4" t="inlineStr">
         <is>
-          <t>сер, легк, б/к</t>
+          <t>легк, б/к, сер</t>
         </is>
       </c>
       <c r="H4" t="n">
@@ -609,7 +609,7 @@
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>сер ошип</t>
+          <t>ошип сер</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
@@ -624,7 +624,7 @@
       </c>
       <c r="G5" t="inlineStr">
         <is>
-          <t>сер, легк, б/к</t>
+          <t>легк, б/к, сер</t>
         </is>
       </c>
       <c r="H5" t="n">
@@ -652,7 +652,7 @@
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>сер легк</t>
+          <t>легк сер</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
@@ -667,7 +667,7 @@
       </c>
       <c r="G6" t="inlineStr">
         <is>
-          <t>сер, ошип</t>
+          <t>ошип, сер</t>
         </is>
       </c>
       <c r="H6" t="n">
@@ -695,7 +695,7 @@
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>сер легк</t>
+          <t>легк сер</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
@@ -710,7 +710,7 @@
       </c>
       <c r="G7" t="inlineStr">
         <is>
-          <t>сер, легк</t>
+          <t>легк, сер</t>
         </is>
       </c>
       <c r="H7" t="n">
@@ -738,7 +738,7 @@
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>сер легк</t>
+          <t>легк сер</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
@@ -753,7 +753,7 @@
       </c>
       <c r="G8" t="inlineStr">
         <is>
-          <t>сер, легк</t>
+          <t>легк, сер</t>
         </is>
       </c>
       <c r="H8" t="n">
@@ -781,7 +781,7 @@
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>сер легк</t>
+          <t>легк сер</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
@@ -796,7 +796,7 @@
       </c>
       <c r="G9" t="inlineStr">
         <is>
-          <t>сер, легк</t>
+          <t>легк, сер</t>
         </is>
       </c>
       <c r="H9" t="n">
@@ -824,7 +824,7 @@
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>210B H сер C Type</t>
+          <t>210B C Type сер H</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
@@ -839,7 +839,7 @@
       </c>
       <c r="G10" t="inlineStr">
         <is>
-          <t>сер, легк</t>
+          <t>легк, сер</t>
         </is>
       </c>
       <c r="H10" t="n">
@@ -867,7 +867,7 @@
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>LS-2 сер груз Type</t>
+          <t>LS-2 Type сер груз</t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
@@ -882,7 +882,7 @@
       </c>
       <c r="G11" t="inlineStr">
         <is>
-          <t>210B, H, сер, C, Type</t>
+          <t>210B, C, Type, сер, H</t>
         </is>
       </c>
       <c r="H11" t="n">
@@ -910,7 +910,7 @@
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>202B сер C Type</t>
+          <t>202B C Type сер</t>
         </is>
       </c>
       <c r="E12" t="inlineStr">
@@ -925,7 +925,7 @@
       </c>
       <c r="G12" t="inlineStr">
         <is>
-          <t>210B, H, сер, C, Type</t>
+          <t>210B, C, Type, сер, H</t>
         </is>
       </c>
       <c r="H12" t="n">
@@ -953,7 +953,7 @@
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>202B LS-2 H сер C Type</t>
+          <t>202B C LS-2 Type сер H</t>
         </is>
       </c>
       <c r="E13" t="inlineStr">
@@ -968,7 +968,7 @@
       </c>
       <c r="G13" t="inlineStr">
         <is>
-          <t>LS-2, сер, груз, Type</t>
+          <t>LS-2, Type, сер, груз</t>
         </is>
       </c>
       <c r="H13" t="n">
@@ -996,7 +996,7 @@
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>сер груз б/к</t>
+          <t>б/к сер груз</t>
         </is>
       </c>
       <c r="E14" t="inlineStr">
@@ -1011,7 +1011,7 @@
       </c>
       <c r="G14" t="inlineStr">
         <is>
-          <t>202B, сер, C, Type</t>
+          <t>202B, C, Type, сер</t>
         </is>
       </c>
       <c r="H14" t="n">
@@ -1039,7 +1039,7 @@
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>сер легк б/к</t>
+          <t>легк б/к сер</t>
         </is>
       </c>
       <c r="E15" t="inlineStr">
@@ -1054,7 +1054,7 @@
       </c>
       <c r="G15" t="inlineStr">
         <is>
-          <t>202B, LS-2, H, сер, C, Type</t>
+          <t>202B, C, LS-2, Type, сер, H</t>
         </is>
       </c>
       <c r="H15" t="n">
@@ -1082,7 +1082,7 @@
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>сер легк б/к</t>
+          <t>легк б/к сер</t>
         </is>
       </c>
       <c r="E16" t="inlineStr">
@@ -1097,7 +1097,7 @@
       </c>
       <c r="G16" t="inlineStr">
         <is>
-          <t>202B, LS-2, H, сер, C, Type</t>
+          <t>202B, C, LS-2, Type, сер, H</t>
         </is>
       </c>
       <c r="H16" t="n">
@@ -1140,7 +1140,7 @@
       </c>
       <c r="G17" t="inlineStr">
         <is>
-          <t>202B, LS-2, H, сер, C, Type</t>
+          <t>202B, C, LS-2, Type, сер, H</t>
         </is>
       </c>
       <c r="H17" t="n">
@@ -1168,7 +1168,7 @@
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>сер легк</t>
+          <t>легк сер</t>
         </is>
       </c>
       <c r="E18" t="inlineStr">
@@ -1183,7 +1183,7 @@
       </c>
       <c r="G18" t="inlineStr">
         <is>
-          <t>сер, груз, б/к</t>
+          <t>б/к, сер, груз</t>
         </is>
       </c>
       <c r="H18" t="n">
@@ -1211,7 +1211,7 @@
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>сер легк</t>
+          <t>легк сер</t>
         </is>
       </c>
       <c r="E19" t="inlineStr">
@@ -1226,7 +1226,7 @@
       </c>
       <c r="G19" t="inlineStr">
         <is>
-          <t>сер, груз, б/к</t>
+          <t>б/к, сер, груз</t>
         </is>
       </c>
       <c r="H19" t="n">
@@ -1254,7 +1254,7 @@
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>сер легк</t>
+          <t>легк сер</t>
         </is>
       </c>
       <c r="E20" t="inlineStr">
@@ -1269,7 +1269,7 @@
       </c>
       <c r="G20" t="inlineStr">
         <is>
-          <t>сер, груз, б/к</t>
+          <t>б/к, сер, груз</t>
         </is>
       </c>
       <c r="H20" t="n">
@@ -1297,7 +1297,7 @@
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>сер легк</t>
+          <t>легк сер</t>
         </is>
       </c>
       <c r="E21" t="inlineStr">
@@ -1312,7 +1312,7 @@
       </c>
       <c r="G21" t="inlineStr">
         <is>
-          <t>сер, груз, б/к</t>
+          <t>б/к, сер, груз</t>
         </is>
       </c>
       <c r="H21" t="n">
@@ -1340,7 +1340,7 @@
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>сер легк</t>
+          <t>легк сер</t>
         </is>
       </c>
       <c r="E22" t="inlineStr">
@@ -1355,7 +1355,7 @@
       </c>
       <c r="G22" t="inlineStr">
         <is>
-          <t>сер, легк, б/к</t>
+          <t>легк, б/к, сер</t>
         </is>
       </c>
       <c r="H22" t="n">
@@ -1383,7 +1383,7 @@
       </c>
       <c r="G23" t="inlineStr">
         <is>
-          <t>сер, легк, б/к</t>
+          <t>легк, б/к, сер</t>
         </is>
       </c>
       <c r="H23" t="n">
@@ -1411,7 +1411,7 @@
       </c>
       <c r="G24" t="inlineStr">
         <is>
-          <t>сер, легк</t>
+          <t>легк, сер</t>
         </is>
       </c>
       <c r="H24" t="n">
@@ -1439,7 +1439,7 @@
       </c>
       <c r="G25" t="inlineStr">
         <is>
-          <t>сер, легк</t>
+          <t>легк, сер</t>
         </is>
       </c>
       <c r="H25" t="n">
@@ -1467,7 +1467,7 @@
       </c>
       <c r="G26" t="inlineStr">
         <is>
-          <t>сер, легк</t>
+          <t>легк, сер</t>
         </is>
       </c>
       <c r="H26" t="n">
@@ -1495,7 +1495,7 @@
       </c>
       <c r="G27" t="inlineStr">
         <is>
-          <t>сер, легк</t>
+          <t>легк, сер</t>
         </is>
       </c>
       <c r="H27" t="n">
@@ -1523,7 +1523,7 @@
       </c>
       <c r="G28" t="inlineStr">
         <is>
-          <t>сер, легк</t>
+          <t>легк, сер</t>
         </is>
       </c>
       <c r="H28" t="n">
@@ -1551,7 +1551,7 @@
       </c>
       <c r="G29" t="inlineStr">
         <is>
-          <t>сер, легк</t>
+          <t>легк, сер</t>
         </is>
       </c>
       <c r="H29" t="n">
@@ -1579,7 +1579,7 @@
       </c>
       <c r="G30" t="inlineStr">
         <is>
-          <t>сер, легк</t>
+          <t>легк, сер</t>
         </is>
       </c>
       <c r="H30" t="n">

</xml_diff>

<commit_message>
10.02/2024 - return to host 37
</commit_message>
<xml_diff>
--- a/src/Tyres.xlsx
+++ b/src/Tyres.xlsx
@@ -480,7 +480,7 @@
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>42 30 сер груз</t>
+          <t>30 42 груз сер</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
@@ -495,14 +495,14 @@
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>42, 30, сер, груз</t>
+          <t>30, 42, груз, сер</t>
         </is>
       </c>
       <c r="H2" t="n">
         <v>2</v>
       </c>
       <c r="I2" s="1" t="n">
-        <v>45350</v>
+        <v>45351</v>
       </c>
       <c r="J2" t="inlineStr">
         <is>
@@ -538,14 +538,14 @@
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>42, 30, сер, груз</t>
+          <t>30, 42, груз, сер</t>
         </is>
       </c>
       <c r="H3" t="n">
         <v>2</v>
       </c>
       <c r="I3" s="1" t="n">
-        <v>45350</v>
+        <v>45351</v>
       </c>
       <c r="J3" t="inlineStr">
         <is>
@@ -588,7 +588,7 @@
         <v>2</v>
       </c>
       <c r="I4" s="1" t="n">
-        <v>45350</v>
+        <v>45351</v>
       </c>
       <c r="J4" t="inlineStr">
         <is>
@@ -631,7 +631,7 @@
         <v>2</v>
       </c>
       <c r="I5" s="1" t="n">
-        <v>45350</v>
+        <v>45351</v>
       </c>
       <c r="J5" t="inlineStr">
         <is>
@@ -674,7 +674,7 @@
         <v>2</v>
       </c>
       <c r="I6" s="1" t="n">
-        <v>45350</v>
+        <v>45351</v>
       </c>
       <c r="J6" t="inlineStr">
         <is>
@@ -717,7 +717,7 @@
         <v>2</v>
       </c>
       <c r="I7" s="1" t="n">
-        <v>45350</v>
+        <v>45351</v>
       </c>
       <c r="J7" t="inlineStr">
         <is>
@@ -760,7 +760,7 @@
         <v>2</v>
       </c>
       <c r="I8" s="1" t="n">
-        <v>45350</v>
+        <v>45351</v>
       </c>
       <c r="J8" t="inlineStr">
         <is>
@@ -803,7 +803,7 @@
         <v>2</v>
       </c>
       <c r="I9" s="1" t="n">
-        <v>45350</v>
+        <v>45351</v>
       </c>
       <c r="J9" t="inlineStr">
         <is>
@@ -846,7 +846,7 @@
         <v>2</v>
       </c>
       <c r="I10" s="1" t="n">
-        <v>45350</v>
+        <v>45351</v>
       </c>
       <c r="J10" t="inlineStr">
         <is>
@@ -867,7 +867,7 @@
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>LS-2 Type сер груз</t>
+          <t>Type груз сер LS-2</t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
@@ -889,7 +889,7 @@
         <v>2</v>
       </c>
       <c r="I11" s="1" t="n">
-        <v>45350</v>
+        <v>45351</v>
       </c>
       <c r="J11" t="inlineStr">
         <is>
@@ -932,7 +932,7 @@
         <v>2</v>
       </c>
       <c r="I12" s="1" t="n">
-        <v>45350</v>
+        <v>45351</v>
       </c>
       <c r="J12" t="inlineStr">
         <is>
@@ -953,7 +953,7 @@
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>202B C LS-2 Type сер H</t>
+          <t>202B C Type сер LS-2 H</t>
         </is>
       </c>
       <c r="E13" t="inlineStr">
@@ -968,14 +968,14 @@
       </c>
       <c r="G13" t="inlineStr">
         <is>
-          <t>LS-2, Type, сер, груз</t>
+          <t>Type, груз, сер, LS-2</t>
         </is>
       </c>
       <c r="H13" t="n">
         <v>2</v>
       </c>
       <c r="I13" s="1" t="n">
-        <v>45350</v>
+        <v>45351</v>
       </c>
       <c r="J13" t="inlineStr">
         <is>
@@ -996,7 +996,7 @@
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>б/к сер груз</t>
+          <t>груз б/к сер</t>
         </is>
       </c>
       <c r="E14" t="inlineStr">
@@ -1018,7 +1018,7 @@
         <v>2</v>
       </c>
       <c r="I14" s="1" t="n">
-        <v>45350</v>
+        <v>45351</v>
       </c>
       <c r="J14" t="inlineStr">
         <is>
@@ -1054,14 +1054,14 @@
       </c>
       <c r="G15" t="inlineStr">
         <is>
-          <t>202B, C, LS-2, Type, сер, H</t>
+          <t>202B, C, Type, сер, LS-2, H</t>
         </is>
       </c>
       <c r="H15" t="n">
         <v>2</v>
       </c>
       <c r="I15" s="1" t="n">
-        <v>45350</v>
+        <v>45351</v>
       </c>
       <c r="J15" t="inlineStr">
         <is>
@@ -1097,14 +1097,14 @@
       </c>
       <c r="G16" t="inlineStr">
         <is>
-          <t>202B, C, LS-2, Type, сер, H</t>
+          <t>202B, C, Type, сер, LS-2, H</t>
         </is>
       </c>
       <c r="H16" t="n">
         <v>2</v>
       </c>
       <c r="I16" s="1" t="n">
-        <v>45350</v>
+        <v>45351</v>
       </c>
       <c r="J16" t="inlineStr">
         <is>
@@ -1125,7 +1125,7 @@
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>8 сер сх</t>
+          <t>8 сх сер</t>
         </is>
       </c>
       <c r="E17" t="inlineStr">
@@ -1140,14 +1140,14 @@
       </c>
       <c r="G17" t="inlineStr">
         <is>
-          <t>202B, C, LS-2, Type, сер, H</t>
+          <t>202B, C, Type, сер, LS-2, H</t>
         </is>
       </c>
       <c r="H17" t="n">
         <v>2</v>
       </c>
       <c r="I17" s="1" t="n">
-        <v>45350</v>
+        <v>45351</v>
       </c>
       <c r="J17" t="inlineStr">
         <is>
@@ -1183,14 +1183,14 @@
       </c>
       <c r="G18" t="inlineStr">
         <is>
-          <t>б/к, сер, груз</t>
+          <t>груз, б/к, сер</t>
         </is>
       </c>
       <c r="H18" t="n">
         <v>2</v>
       </c>
       <c r="I18" s="1" t="n">
-        <v>45350</v>
+        <v>45351</v>
       </c>
       <c r="J18" t="inlineStr">
         <is>
@@ -1226,14 +1226,14 @@
       </c>
       <c r="G19" t="inlineStr">
         <is>
-          <t>б/к, сер, груз</t>
+          <t>груз, б/к, сер</t>
         </is>
       </c>
       <c r="H19" t="n">
         <v>2</v>
       </c>
       <c r="I19" s="1" t="n">
-        <v>45350</v>
+        <v>45351</v>
       </c>
       <c r="J19" t="inlineStr">
         <is>
@@ -1269,14 +1269,14 @@
       </c>
       <c r="G20" t="inlineStr">
         <is>
-          <t>б/к, сер, груз</t>
+          <t>груз, б/к, сер</t>
         </is>
       </c>
       <c r="H20" t="n">
         <v>2</v>
       </c>
       <c r="I20" s="1" t="n">
-        <v>45350</v>
+        <v>45351</v>
       </c>
       <c r="J20" t="inlineStr">
         <is>
@@ -1312,14 +1312,14 @@
       </c>
       <c r="G21" t="inlineStr">
         <is>
-          <t>б/к, сер, груз</t>
+          <t>груз, б/к, сер</t>
         </is>
       </c>
       <c r="H21" t="n">
         <v>2</v>
       </c>
       <c r="I21" s="1" t="n">
-        <v>45350</v>
+        <v>45351</v>
       </c>
       <c r="J21" t="inlineStr">
         <is>
@@ -1362,7 +1362,7 @@
         <v>2</v>
       </c>
       <c r="I22" s="1" t="n">
-        <v>45350</v>
+        <v>45351</v>
       </c>
       <c r="J22" t="inlineStr">
         <is>
@@ -1390,7 +1390,7 @@
         <v>2</v>
       </c>
       <c r="I23" s="1" t="n">
-        <v>45350</v>
+        <v>45351</v>
       </c>
       <c r="J23" t="inlineStr">
         <is>
@@ -1418,7 +1418,7 @@
         <v>2</v>
       </c>
       <c r="I24" s="1" t="n">
-        <v>45350</v>
+        <v>45351</v>
       </c>
       <c r="J24" t="inlineStr">
         <is>
@@ -1446,7 +1446,7 @@
         <v>2</v>
       </c>
       <c r="I25" s="1" t="n">
-        <v>45350</v>
+        <v>45351</v>
       </c>
       <c r="J25" t="inlineStr">
         <is>
@@ -1474,7 +1474,7 @@
         <v>2</v>
       </c>
       <c r="I26" s="1" t="n">
-        <v>45350</v>
+        <v>45351</v>
       </c>
       <c r="J26" t="inlineStr">
         <is>
@@ -1502,7 +1502,7 @@
         <v>2</v>
       </c>
       <c r="I27" s="1" t="n">
-        <v>45350</v>
+        <v>45351</v>
       </c>
       <c r="J27" t="inlineStr">
         <is>
@@ -1530,7 +1530,7 @@
         <v>2</v>
       </c>
       <c r="I28" s="1" t="n">
-        <v>45350</v>
+        <v>45351</v>
       </c>
       <c r="J28" t="inlineStr">
         <is>
@@ -1558,7 +1558,7 @@
         <v>2</v>
       </c>
       <c r="I29" s="1" t="n">
-        <v>45350</v>
+        <v>45351</v>
       </c>
       <c r="J29" t="inlineStr">
         <is>
@@ -1586,7 +1586,7 @@
         <v>2</v>
       </c>
       <c r="I30" s="1" t="n">
-        <v>45350</v>
+        <v>45351</v>
       </c>
       <c r="J30" t="inlineStr">
         <is>

</xml_diff>

<commit_message>
10.02/2024 - return to host 38
</commit_message>
<xml_diff>
--- a/src/Tyres.xlsx
+++ b/src/Tyres.xlsx
@@ -523,7 +523,7 @@
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>легк б/к сер</t>
+          <t>б/к сер легк</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
@@ -566,7 +566,7 @@
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>легк б/к сер</t>
+          <t>б/к сер легк</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
@@ -581,7 +581,7 @@
       </c>
       <c r="G4" t="inlineStr">
         <is>
-          <t>легк, б/к, сер</t>
+          <t>б/к, сер, легк</t>
         </is>
       </c>
       <c r="H4" t="n">
@@ -624,7 +624,7 @@
       </c>
       <c r="G5" t="inlineStr">
         <is>
-          <t>легк, б/к, сер</t>
+          <t>б/к, сер, легк</t>
         </is>
       </c>
       <c r="H5" t="n">
@@ -652,7 +652,7 @@
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>легк сер</t>
+          <t>сер легк</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
@@ -695,7 +695,7 @@
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>легк сер</t>
+          <t>сер легк</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
@@ -710,7 +710,7 @@
       </c>
       <c r="G7" t="inlineStr">
         <is>
-          <t>легк, сер</t>
+          <t>сер, легк</t>
         </is>
       </c>
       <c r="H7" t="n">
@@ -738,7 +738,7 @@
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>легк сер</t>
+          <t>сер легк</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
@@ -753,7 +753,7 @@
       </c>
       <c r="G8" t="inlineStr">
         <is>
-          <t>легк, сер</t>
+          <t>сер, легк</t>
         </is>
       </c>
       <c r="H8" t="n">
@@ -781,7 +781,7 @@
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>легк сер</t>
+          <t>сер легк</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
@@ -796,7 +796,7 @@
       </c>
       <c r="G9" t="inlineStr">
         <is>
-          <t>легк, сер</t>
+          <t>сер, легк</t>
         </is>
       </c>
       <c r="H9" t="n">
@@ -824,7 +824,7 @@
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>210B C Type сер H</t>
+          <t>210B Type сер C H</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
@@ -839,7 +839,7 @@
       </c>
       <c r="G10" t="inlineStr">
         <is>
-          <t>легк, сер</t>
+          <t>сер, легк</t>
         </is>
       </c>
       <c r="H10" t="n">
@@ -882,7 +882,7 @@
       </c>
       <c r="G11" t="inlineStr">
         <is>
-          <t>210B, C, Type, сер, H</t>
+          <t>210B, Type, сер, C, H</t>
         </is>
       </c>
       <c r="H11" t="n">
@@ -910,7 +910,7 @@
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>202B C Type сер</t>
+          <t>202B Type сер C</t>
         </is>
       </c>
       <c r="E12" t="inlineStr">
@@ -925,7 +925,7 @@
       </c>
       <c r="G12" t="inlineStr">
         <is>
-          <t>210B, C, Type, сер, H</t>
+          <t>210B, Type, сер, C, H</t>
         </is>
       </c>
       <c r="H12" t="n">
@@ -953,7 +953,7 @@
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>202B C Type сер LS-2 H</t>
+          <t>202B Type сер C H LS-2</t>
         </is>
       </c>
       <c r="E13" t="inlineStr">
@@ -996,7 +996,7 @@
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>груз б/к сер</t>
+          <t>б/к груз сер</t>
         </is>
       </c>
       <c r="E14" t="inlineStr">
@@ -1011,7 +1011,7 @@
       </c>
       <c r="G14" t="inlineStr">
         <is>
-          <t>202B, C, Type, сер</t>
+          <t>202B, Type, сер, C</t>
         </is>
       </c>
       <c r="H14" t="n">
@@ -1039,7 +1039,7 @@
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>легк б/к сер</t>
+          <t>б/к сер легк</t>
         </is>
       </c>
       <c r="E15" t="inlineStr">
@@ -1054,7 +1054,7 @@
       </c>
       <c r="G15" t="inlineStr">
         <is>
-          <t>202B, C, Type, сер, LS-2, H</t>
+          <t>202B, Type, сер, C, H, LS-2</t>
         </is>
       </c>
       <c r="H15" t="n">
@@ -1082,7 +1082,7 @@
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>легк б/к сер</t>
+          <t>б/к сер легк</t>
         </is>
       </c>
       <c r="E16" t="inlineStr">
@@ -1097,7 +1097,7 @@
       </c>
       <c r="G16" t="inlineStr">
         <is>
-          <t>202B, C, Type, сер, LS-2, H</t>
+          <t>202B, Type, сер, C, H, LS-2</t>
         </is>
       </c>
       <c r="H16" t="n">
@@ -1125,7 +1125,7 @@
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>8 сх сер</t>
+          <t>8 сер сх</t>
         </is>
       </c>
       <c r="E17" t="inlineStr">
@@ -1140,7 +1140,7 @@
       </c>
       <c r="G17" t="inlineStr">
         <is>
-          <t>202B, C, Type, сер, LS-2, H</t>
+          <t>202B, Type, сер, C, H, LS-2</t>
         </is>
       </c>
       <c r="H17" t="n">
@@ -1168,7 +1168,7 @@
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>легк сер</t>
+          <t>сер легк</t>
         </is>
       </c>
       <c r="E18" t="inlineStr">
@@ -1183,7 +1183,7 @@
       </c>
       <c r="G18" t="inlineStr">
         <is>
-          <t>груз, б/к, сер</t>
+          <t>б/к, груз, сер</t>
         </is>
       </c>
       <c r="H18" t="n">
@@ -1211,7 +1211,7 @@
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>легк сер</t>
+          <t>сер легк</t>
         </is>
       </c>
       <c r="E19" t="inlineStr">
@@ -1226,7 +1226,7 @@
       </c>
       <c r="G19" t="inlineStr">
         <is>
-          <t>груз, б/к, сер</t>
+          <t>б/к, груз, сер</t>
         </is>
       </c>
       <c r="H19" t="n">
@@ -1254,7 +1254,7 @@
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>легк сер</t>
+          <t>сер легк</t>
         </is>
       </c>
       <c r="E20" t="inlineStr">
@@ -1269,7 +1269,7 @@
       </c>
       <c r="G20" t="inlineStr">
         <is>
-          <t>груз, б/к, сер</t>
+          <t>б/к, груз, сер</t>
         </is>
       </c>
       <c r="H20" t="n">
@@ -1297,7 +1297,7 @@
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>легк сер</t>
+          <t>сер легк</t>
         </is>
       </c>
       <c r="E21" t="inlineStr">
@@ -1312,7 +1312,7 @@
       </c>
       <c r="G21" t="inlineStr">
         <is>
-          <t>груз, б/к, сер</t>
+          <t>б/к, груз, сер</t>
         </is>
       </c>
       <c r="H21" t="n">
@@ -1340,7 +1340,7 @@
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>легк сер</t>
+          <t>сер легк</t>
         </is>
       </c>
       <c r="E22" t="inlineStr">
@@ -1355,7 +1355,7 @@
       </c>
       <c r="G22" t="inlineStr">
         <is>
-          <t>легк, б/к, сер</t>
+          <t>б/к, сер, легк</t>
         </is>
       </c>
       <c r="H22" t="n">
@@ -1383,7 +1383,7 @@
       </c>
       <c r="G23" t="inlineStr">
         <is>
-          <t>легк, б/к, сер</t>
+          <t>б/к, сер, легк</t>
         </is>
       </c>
       <c r="H23" t="n">
@@ -1411,7 +1411,7 @@
       </c>
       <c r="G24" t="inlineStr">
         <is>
-          <t>легк, сер</t>
+          <t>сер, легк</t>
         </is>
       </c>
       <c r="H24" t="n">
@@ -1439,7 +1439,7 @@
       </c>
       <c r="G25" t="inlineStr">
         <is>
-          <t>легк, сер</t>
+          <t>сер, легк</t>
         </is>
       </c>
       <c r="H25" t="n">
@@ -1467,7 +1467,7 @@
       </c>
       <c r="G26" t="inlineStr">
         <is>
-          <t>легк, сер</t>
+          <t>сер, легк</t>
         </is>
       </c>
       <c r="H26" t="n">
@@ -1495,7 +1495,7 @@
       </c>
       <c r="G27" t="inlineStr">
         <is>
-          <t>легк, сер</t>
+          <t>сер, легк</t>
         </is>
       </c>
       <c r="H27" t="n">
@@ -1523,7 +1523,7 @@
       </c>
       <c r="G28" t="inlineStr">
         <is>
-          <t>легк, сер</t>
+          <t>сер, легк</t>
         </is>
       </c>
       <c r="H28" t="n">
@@ -1551,7 +1551,7 @@
       </c>
       <c r="G29" t="inlineStr">
         <is>
-          <t>легк, сер</t>
+          <t>сер, легк</t>
         </is>
       </c>
       <c r="H29" t="n">
@@ -1579,7 +1579,7 @@
       </c>
       <c r="G30" t="inlineStr">
         <is>
-          <t>легк, сер</t>
+          <t>сер, легк</t>
         </is>
       </c>
       <c r="H30" t="n">

</xml_diff>

<commit_message>
10.02/2024 - return to host 41
</commit_message>
<xml_diff>
--- a/src/Tyres.xlsx
+++ b/src/Tyres.xlsx
@@ -480,7 +480,7 @@
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>30 42 груз сер</t>
+          <t>42 30 груз сер</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
@@ -495,7 +495,7 @@
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>30, 42, груз, сер</t>
+          <t>42, 30, груз, сер</t>
         </is>
       </c>
       <c r="H2" t="n">
@@ -523,7 +523,7 @@
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>б/к сер легк</t>
+          <t>б/к легк сер</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
@@ -538,7 +538,7 @@
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>30, 42, груз, сер</t>
+          <t>42, 30, груз, сер</t>
         </is>
       </c>
       <c r="H3" t="n">
@@ -566,7 +566,7 @@
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>б/к сер легк</t>
+          <t>б/к легк сер</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
@@ -581,7 +581,7 @@
       </c>
       <c r="G4" t="inlineStr">
         <is>
-          <t>б/к, сер, легк</t>
+          <t>б/к, легк, сер</t>
         </is>
       </c>
       <c r="H4" t="n">
@@ -624,7 +624,7 @@
       </c>
       <c r="G5" t="inlineStr">
         <is>
-          <t>б/к, сер, легк</t>
+          <t>б/к, легк, сер</t>
         </is>
       </c>
       <c r="H5" t="n">
@@ -652,7 +652,7 @@
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>сер легк</t>
+          <t>легк сер</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
@@ -695,7 +695,7 @@
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>сер легк</t>
+          <t>легк сер</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
@@ -710,7 +710,7 @@
       </c>
       <c r="G7" t="inlineStr">
         <is>
-          <t>сер, легк</t>
+          <t>легк, сер</t>
         </is>
       </c>
       <c r="H7" t="n">
@@ -738,7 +738,7 @@
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>сер легк</t>
+          <t>легк сер</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
@@ -753,7 +753,7 @@
       </c>
       <c r="G8" t="inlineStr">
         <is>
-          <t>сер, легк</t>
+          <t>легк, сер</t>
         </is>
       </c>
       <c r="H8" t="n">
@@ -781,7 +781,7 @@
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>сер легк</t>
+          <t>легк сер</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
@@ -796,7 +796,7 @@
       </c>
       <c r="G9" t="inlineStr">
         <is>
-          <t>сер, легк</t>
+          <t>легк, сер</t>
         </is>
       </c>
       <c r="H9" t="n">
@@ -824,7 +824,7 @@
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>210B Type сер C H</t>
+          <t>210B C H Type сер</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
@@ -839,7 +839,7 @@
       </c>
       <c r="G10" t="inlineStr">
         <is>
-          <t>сер, легк</t>
+          <t>легк, сер</t>
         </is>
       </c>
       <c r="H10" t="n">
@@ -867,7 +867,7 @@
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>Type груз сер LS-2</t>
+          <t>груз LS-2 Type сер</t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
@@ -882,7 +882,7 @@
       </c>
       <c r="G11" t="inlineStr">
         <is>
-          <t>210B, Type, сер, C, H</t>
+          <t>210B, C, H, Type, сер</t>
         </is>
       </c>
       <c r="H11" t="n">
@@ -910,7 +910,7 @@
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>202B Type сер C</t>
+          <t>202B C Type сер</t>
         </is>
       </c>
       <c r="E12" t="inlineStr">
@@ -925,7 +925,7 @@
       </c>
       <c r="G12" t="inlineStr">
         <is>
-          <t>210B, Type, сер, C, H</t>
+          <t>210B, C, H, Type, сер</t>
         </is>
       </c>
       <c r="H12" t="n">
@@ -953,7 +953,7 @@
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>202B Type сер C H LS-2</t>
+          <t>202B C LS-2 H Type сер</t>
         </is>
       </c>
       <c r="E13" t="inlineStr">
@@ -968,7 +968,7 @@
       </c>
       <c r="G13" t="inlineStr">
         <is>
-          <t>Type, груз, сер, LS-2</t>
+          <t>груз, LS-2, Type, сер</t>
         </is>
       </c>
       <c r="H13" t="n">
@@ -996,7 +996,7 @@
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>б/к груз сер</t>
+          <t>груз б/к сер</t>
         </is>
       </c>
       <c r="E14" t="inlineStr">
@@ -1011,7 +1011,7 @@
       </c>
       <c r="G14" t="inlineStr">
         <is>
-          <t>202B, Type, сер, C</t>
+          <t>202B, C, Type, сер</t>
         </is>
       </c>
       <c r="H14" t="n">
@@ -1039,7 +1039,7 @@
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>б/к сер легк</t>
+          <t>б/к легк сер</t>
         </is>
       </c>
       <c r="E15" t="inlineStr">
@@ -1054,7 +1054,7 @@
       </c>
       <c r="G15" t="inlineStr">
         <is>
-          <t>202B, Type, сер, C, H, LS-2</t>
+          <t>202B, C, LS-2, H, Type, сер</t>
         </is>
       </c>
       <c r="H15" t="n">
@@ -1082,7 +1082,7 @@
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>б/к сер легк</t>
+          <t>б/к легк сер</t>
         </is>
       </c>
       <c r="E16" t="inlineStr">
@@ -1097,7 +1097,7 @@
       </c>
       <c r="G16" t="inlineStr">
         <is>
-          <t>202B, Type, сер, C, H, LS-2</t>
+          <t>202B, C, LS-2, H, Type, сер</t>
         </is>
       </c>
       <c r="H16" t="n">
@@ -1125,7 +1125,7 @@
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>8 сер сх</t>
+          <t>8 сх сер</t>
         </is>
       </c>
       <c r="E17" t="inlineStr">
@@ -1140,7 +1140,7 @@
       </c>
       <c r="G17" t="inlineStr">
         <is>
-          <t>202B, Type, сер, C, H, LS-2</t>
+          <t>202B, C, LS-2, H, Type, сер</t>
         </is>
       </c>
       <c r="H17" t="n">
@@ -1168,7 +1168,7 @@
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>сер легк</t>
+          <t>легк сер</t>
         </is>
       </c>
       <c r="E18" t="inlineStr">
@@ -1183,7 +1183,7 @@
       </c>
       <c r="G18" t="inlineStr">
         <is>
-          <t>б/к, груз, сер</t>
+          <t>груз, б/к, сер</t>
         </is>
       </c>
       <c r="H18" t="n">
@@ -1211,7 +1211,7 @@
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>сер легк</t>
+          <t>легк сер</t>
         </is>
       </c>
       <c r="E19" t="inlineStr">
@@ -1226,7 +1226,7 @@
       </c>
       <c r="G19" t="inlineStr">
         <is>
-          <t>б/к, груз, сер</t>
+          <t>груз, б/к, сер</t>
         </is>
       </c>
       <c r="H19" t="n">
@@ -1254,7 +1254,7 @@
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>сер легк</t>
+          <t>легк сер</t>
         </is>
       </c>
       <c r="E20" t="inlineStr">
@@ -1269,7 +1269,7 @@
       </c>
       <c r="G20" t="inlineStr">
         <is>
-          <t>б/к, груз, сер</t>
+          <t>груз, б/к, сер</t>
         </is>
       </c>
       <c r="H20" t="n">
@@ -1297,7 +1297,7 @@
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>сер легк</t>
+          <t>легк сер</t>
         </is>
       </c>
       <c r="E21" t="inlineStr">
@@ -1312,7 +1312,7 @@
       </c>
       <c r="G21" t="inlineStr">
         <is>
-          <t>б/к, груз, сер</t>
+          <t>груз, б/к, сер</t>
         </is>
       </c>
       <c r="H21" t="n">
@@ -1340,7 +1340,7 @@
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>сер легк</t>
+          <t>легк сер</t>
         </is>
       </c>
       <c r="E22" t="inlineStr">
@@ -1355,7 +1355,7 @@
       </c>
       <c r="G22" t="inlineStr">
         <is>
-          <t>б/к, сер, легк</t>
+          <t>б/к, легк, сер</t>
         </is>
       </c>
       <c r="H22" t="n">
@@ -1383,7 +1383,7 @@
       </c>
       <c r="G23" t="inlineStr">
         <is>
-          <t>б/к, сер, легк</t>
+          <t>б/к, легк, сер</t>
         </is>
       </c>
       <c r="H23" t="n">
@@ -1411,7 +1411,7 @@
       </c>
       <c r="G24" t="inlineStr">
         <is>
-          <t>сер, легк</t>
+          <t>легк, сер</t>
         </is>
       </c>
       <c r="H24" t="n">
@@ -1439,7 +1439,7 @@
       </c>
       <c r="G25" t="inlineStr">
         <is>
-          <t>сер, легк</t>
+          <t>легк, сер</t>
         </is>
       </c>
       <c r="H25" t="n">
@@ -1467,7 +1467,7 @@
       </c>
       <c r="G26" t="inlineStr">
         <is>
-          <t>сер, легк</t>
+          <t>легк, сер</t>
         </is>
       </c>
       <c r="H26" t="n">
@@ -1495,7 +1495,7 @@
       </c>
       <c r="G27" t="inlineStr">
         <is>
-          <t>сер, легк</t>
+          <t>легк, сер</t>
         </is>
       </c>
       <c r="H27" t="n">
@@ -1523,7 +1523,7 @@
       </c>
       <c r="G28" t="inlineStr">
         <is>
-          <t>сер, легк</t>
+          <t>легк, сер</t>
         </is>
       </c>
       <c r="H28" t="n">
@@ -1551,7 +1551,7 @@
       </c>
       <c r="G29" t="inlineStr">
         <is>
-          <t>сер, легк</t>
+          <t>легк, сер</t>
         </is>
       </c>
       <c r="H29" t="n">
@@ -1579,7 +1579,7 @@
       </c>
       <c r="G30" t="inlineStr">
         <is>
-          <t>сер, легк</t>
+          <t>легк, сер</t>
         </is>
       </c>
       <c r="H30" t="n">

</xml_diff>

<commit_message>
10.02/2024 - return to host 93
</commit_message>
<xml_diff>
--- a/src/Tyres.xlsx
+++ b/src/Tyres.xlsx
@@ -417,7 +417,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J30"/>
+  <dimension ref="A1:J34"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -470,39 +470,39 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>ФБел-283</t>
+          <t>BEL-262</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>35/65-33</t>
+          <t>205/55R16</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>42 30 груз сер</t>
+          <t>легк сер б/к</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>35/65-33</t>
+          <t>205/55R16</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>ФБел-283</t>
+          <t>BEL-262</t>
         </is>
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>42, 30, груз, сер</t>
+          <t>легк, сер, б/к</t>
         </is>
       </c>
       <c r="H2" t="n">
         <v>2</v>
       </c>
       <c r="I2" s="1" t="n">
-        <v>45351</v>
+        <v>45371</v>
       </c>
       <c r="J2" t="inlineStr">
         <is>
@@ -513,7 +513,7 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>BEL-262</t>
+          <t>BEL-317</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
@@ -523,29 +523,29 @@
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>б/к легк сер</t>
+          <t>легк сер б/к</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>35/65-33</t>
+          <t>205/55R16</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>ФБел-283</t>
+          <t>BEL-317</t>
         </is>
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>42, 30, груз, сер</t>
+          <t>легк, сер, б/к</t>
         </is>
       </c>
       <c r="H3" t="n">
         <v>2</v>
       </c>
       <c r="I3" s="1" t="n">
-        <v>45351</v>
+        <v>45371</v>
       </c>
       <c r="J3" t="inlineStr">
         <is>
@@ -556,7 +556,7 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>BEL-317</t>
+          <t>BEL-317S</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
@@ -566,7 +566,7 @@
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>б/к легк сер</t>
+          <t>сер ошип</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
@@ -576,19 +576,19 @@
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>BEL-262</t>
+          <t>BEL-317S</t>
         </is>
       </c>
       <c r="G4" t="inlineStr">
         <is>
-          <t>б/к, легк, сер</t>
+          <t>сер, ошип</t>
         </is>
       </c>
       <c r="H4" t="n">
         <v>2</v>
       </c>
       <c r="I4" s="1" t="n">
-        <v>45351</v>
+        <v>45371</v>
       </c>
       <c r="J4" t="inlineStr">
         <is>
@@ -599,39 +599,39 @@
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>BEL-317S</t>
+          <t>BEL-1001</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>205/55R16</t>
+          <t>235/75R15</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>ошип сер</t>
+          <t>легк сер</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>205/55R16</t>
+          <t>235/75R15</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>BEL-317</t>
+          <t>BEL-1001</t>
         </is>
       </c>
       <c r="G5" t="inlineStr">
         <is>
-          <t>б/к, легк, сер</t>
+          <t>легк, сер</t>
         </is>
       </c>
       <c r="H5" t="n">
         <v>2</v>
       </c>
       <c r="I5" s="1" t="n">
-        <v>45351</v>
+        <v>45371</v>
       </c>
       <c r="J5" t="inlineStr">
         <is>
@@ -642,12 +642,12 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>BEL-1001</t>
+          <t>BEL-1002</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>235/75R15</t>
+          <t>155/65R13</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
@@ -657,24 +657,24 @@
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>205/55R16</t>
+          <t>155/65R13</t>
         </is>
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>BEL-317S</t>
+          <t>BEL-1002</t>
         </is>
       </c>
       <c r="G6" t="inlineStr">
         <is>
-          <t>ошип, сер</t>
+          <t>легк, сер</t>
         </is>
       </c>
       <c r="H6" t="n">
         <v>2</v>
       </c>
       <c r="I6" s="1" t="n">
-        <v>45351</v>
+        <v>45371</v>
       </c>
       <c r="J6" t="inlineStr">
         <is>
@@ -685,12 +685,12 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>BEL-1002</t>
+          <t>BEL-1004</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>155/65R13</t>
+          <t>205/55R16</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
@@ -700,12 +700,12 @@
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>235/75R15</t>
+          <t>205/55R16</t>
         </is>
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>BEL-1001</t>
+          <t>BEL-1004</t>
         </is>
       </c>
       <c r="G7" t="inlineStr">
@@ -717,7 +717,7 @@
         <v>2</v>
       </c>
       <c r="I7" s="1" t="n">
-        <v>45351</v>
+        <v>45371</v>
       </c>
       <c r="J7" t="inlineStr">
         <is>
@@ -728,29 +728,29 @@
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
+          <t>BEL-1005</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>225/50R17</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>легк сер</t>
+        </is>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>205/55R16</t>
+        </is>
+      </c>
+      <c r="F8" t="inlineStr">
+        <is>
           <t>BEL-1004</t>
         </is>
       </c>
-      <c r="B8" t="inlineStr">
-        <is>
-          <t>205/55R16</t>
-        </is>
-      </c>
-      <c r="C8" t="inlineStr">
-        <is>
-          <t>легк сер</t>
-        </is>
-      </c>
-      <c r="E8" t="inlineStr">
-        <is>
-          <t>155/65R13</t>
-        </is>
-      </c>
-      <c r="F8" t="inlineStr">
-        <is>
-          <t>BEL-1002</t>
-        </is>
-      </c>
       <c r="G8" t="inlineStr">
         <is>
           <t>легк, сер</t>
@@ -760,7 +760,7 @@
         <v>2</v>
       </c>
       <c r="I8" s="1" t="n">
-        <v>45351</v>
+        <v>45371</v>
       </c>
       <c r="J8" t="inlineStr">
         <is>
@@ -771,29 +771,29 @@
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
+          <t>Бел-202</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>24.00R35</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>210B Type H сер</t>
+        </is>
+      </c>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>225/50R17</t>
+        </is>
+      </c>
+      <c r="F9" t="inlineStr">
+        <is>
           <t>BEL-1005</t>
         </is>
       </c>
-      <c r="B9" t="inlineStr">
-        <is>
-          <t>225/50R17</t>
-        </is>
-      </c>
-      <c r="C9" t="inlineStr">
-        <is>
-          <t>легк сер</t>
-        </is>
-      </c>
-      <c r="E9" t="inlineStr">
-        <is>
-          <t>205/55R16</t>
-        </is>
-      </c>
-      <c r="F9" t="inlineStr">
-        <is>
-          <t>BEL-1004</t>
-        </is>
-      </c>
       <c r="G9" t="inlineStr">
         <is>
           <t>легк, сер</t>
@@ -803,7 +803,7 @@
         <v>2</v>
       </c>
       <c r="I9" s="1" t="n">
-        <v>45351</v>
+        <v>45371</v>
       </c>
       <c r="J9" t="inlineStr">
         <is>
@@ -814,39 +814,39 @@
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
+          <t>BEL-248</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>14.00R20</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>груз сер б/к</t>
+        </is>
+      </c>
+      <c r="E10" t="inlineStr">
+        <is>
+          <t>24.00R35</t>
+        </is>
+      </c>
+      <c r="F10" t="inlineStr">
+        <is>
           <t>Бел-202</t>
         </is>
       </c>
-      <c r="B10" t="inlineStr">
-        <is>
-          <t>24.00R35</t>
-        </is>
-      </c>
-      <c r="C10" t="inlineStr">
-        <is>
-          <t>210B C H Type сер</t>
-        </is>
-      </c>
-      <c r="E10" t="inlineStr">
-        <is>
-          <t>225/50R17</t>
-        </is>
-      </c>
-      <c r="F10" t="inlineStr">
-        <is>
-          <t>BEL-1005</t>
-        </is>
-      </c>
       <c r="G10" t="inlineStr">
         <is>
-          <t>легк, сер</t>
+          <t>210B, Type, H, сер</t>
         </is>
       </c>
       <c r="H10" t="n">
         <v>2</v>
       </c>
       <c r="I10" s="1" t="n">
-        <v>45351</v>
+        <v>45371</v>
       </c>
       <c r="J10" t="inlineStr">
         <is>
@@ -857,39 +857,39 @@
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>Бел-212</t>
+          <t>Бел-103</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>24.00R35</t>
+          <t>175/70R13</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>груз LS-2 Type сер</t>
+          <t>легк сер б/к</t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>24.00R35</t>
+          <t>14.00R20</t>
         </is>
       </c>
       <c r="F11" t="inlineStr">
         <is>
-          <t>Бел-202</t>
+          <t>BEL-248</t>
         </is>
       </c>
       <c r="G11" t="inlineStr">
         <is>
-          <t>210B, C, H, Type, сер</t>
+          <t>груз, сер, б/к</t>
         </is>
       </c>
       <c r="H11" t="n">
         <v>2</v>
       </c>
       <c r="I11" s="1" t="n">
-        <v>45351</v>
+        <v>45371</v>
       </c>
       <c r="J11" t="inlineStr">
         <is>
@@ -900,39 +900,39 @@
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>Бел-200</t>
+          <t>Бел-100</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>21.00R35</t>
+          <t>175/70R13</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>202B C Type сер</t>
+          <t>легк сер б/к</t>
         </is>
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>24.00R35</t>
+          <t>14.00R20</t>
         </is>
       </c>
       <c r="F12" t="inlineStr">
         <is>
-          <t>Бел-202</t>
+          <t>BEL-248</t>
         </is>
       </c>
       <c r="G12" t="inlineStr">
         <is>
-          <t>210B, C, H, Type, сер</t>
+          <t>груз, сер, б/к</t>
         </is>
       </c>
       <c r="H12" t="n">
         <v>2</v>
       </c>
       <c r="I12" s="1" t="n">
-        <v>45351</v>
+        <v>45371</v>
       </c>
       <c r="J12" t="inlineStr">
         <is>
@@ -943,39 +943,39 @@
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>Бел-210</t>
+          <t>Ф-35-1</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>21.00R35</t>
+          <t>11.2-20</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>202B C LS-2 H Type сер</t>
+          <t>8 сх сер</t>
         </is>
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>24.00R35</t>
+          <t>14.00R20</t>
         </is>
       </c>
       <c r="F13" t="inlineStr">
         <is>
-          <t>Бел-212</t>
+          <t>BEL-248</t>
         </is>
       </c>
       <c r="G13" t="inlineStr">
         <is>
-          <t>груз, LS-2, Type, сер</t>
+          <t>груз, сер, б/к</t>
         </is>
       </c>
       <c r="H13" t="n">
         <v>2</v>
       </c>
       <c r="I13" s="1" t="n">
-        <v>45351</v>
+        <v>45371</v>
       </c>
       <c r="J13" t="inlineStr">
         <is>
@@ -986,39 +986,39 @@
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
+          <t>Бел-119</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>195/65R15</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>легк сер</t>
+        </is>
+      </c>
+      <c r="E14" t="inlineStr">
+        <is>
+          <t>14.00R20</t>
+        </is>
+      </c>
+      <c r="F14" t="inlineStr">
+        <is>
           <t>BEL-248</t>
         </is>
       </c>
-      <c r="B14" t="inlineStr">
-        <is>
-          <t>14.00R20</t>
-        </is>
-      </c>
-      <c r="C14" t="inlineStr">
-        <is>
-          <t>груз б/к сер</t>
-        </is>
-      </c>
-      <c r="E14" t="inlineStr">
-        <is>
-          <t>21.00R35</t>
-        </is>
-      </c>
-      <c r="F14" t="inlineStr">
-        <is>
-          <t>Бел-200</t>
-        </is>
-      </c>
       <c r="G14" t="inlineStr">
         <is>
-          <t>202B, C, Type, сер</t>
+          <t>груз, сер, б/к</t>
         </is>
       </c>
       <c r="H14" t="n">
         <v>2</v>
       </c>
       <c r="I14" s="1" t="n">
-        <v>45351</v>
+        <v>45371</v>
       </c>
       <c r="J14" t="inlineStr">
         <is>
@@ -1029,39 +1029,39 @@
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
+          <t>Бел-1149</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>195/65R15</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>легк сер</t>
+        </is>
+      </c>
+      <c r="E15" t="inlineStr">
+        <is>
+          <t>175/70R13</t>
+        </is>
+      </c>
+      <c r="F15" t="inlineStr">
+        <is>
           <t>Бел-103</t>
         </is>
       </c>
-      <c r="B15" t="inlineStr">
-        <is>
-          <t>175/70R13</t>
-        </is>
-      </c>
-      <c r="C15" t="inlineStr">
-        <is>
-          <t>б/к легк сер</t>
-        </is>
-      </c>
-      <c r="E15" t="inlineStr">
-        <is>
-          <t>21.00R35</t>
-        </is>
-      </c>
-      <c r="F15" t="inlineStr">
-        <is>
-          <t>Бел-210</t>
-        </is>
-      </c>
       <c r="G15" t="inlineStr">
         <is>
-          <t>202B, C, LS-2, H, Type, сер</t>
+          <t>легк, сер, б/к</t>
         </is>
       </c>
       <c r="H15" t="n">
         <v>2</v>
       </c>
       <c r="I15" s="1" t="n">
-        <v>45351</v>
+        <v>45371</v>
       </c>
       <c r="J15" t="inlineStr">
         <is>
@@ -1072,39 +1072,39 @@
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
+          <t>Бел-777</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>210/80R16</t>
+        </is>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>легк сер</t>
+        </is>
+      </c>
+      <c r="E16" t="inlineStr">
+        <is>
+          <t>175/70R13</t>
+        </is>
+      </c>
+      <c r="F16" t="inlineStr">
+        <is>
           <t>Бел-100</t>
         </is>
       </c>
-      <c r="B16" t="inlineStr">
-        <is>
-          <t>175/70R13</t>
-        </is>
-      </c>
-      <c r="C16" t="inlineStr">
-        <is>
-          <t>б/к легк сер</t>
-        </is>
-      </c>
-      <c r="E16" t="inlineStr">
-        <is>
-          <t>21.00R35</t>
-        </is>
-      </c>
-      <c r="F16" t="inlineStr">
-        <is>
-          <t>Бел-210</t>
-        </is>
-      </c>
       <c r="G16" t="inlineStr">
         <is>
-          <t>202B, C, LS-2, H, Type, сер</t>
+          <t>легк, сер, б/к</t>
         </is>
       </c>
       <c r="H16" t="n">
         <v>2</v>
       </c>
       <c r="I16" s="1" t="n">
-        <v>45351</v>
+        <v>45371</v>
       </c>
       <c r="J16" t="inlineStr">
         <is>
@@ -1115,39 +1115,39 @@
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>Ф-35-1</t>
+          <t>Бел-1000</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>11.2-20</t>
+          <t>215/65R16C</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>8 сх сер</t>
+          <t>легк сер</t>
         </is>
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>21.00R35</t>
+          <t>195/65R15</t>
         </is>
       </c>
       <c r="F17" t="inlineStr">
         <is>
-          <t>Бел-210</t>
+          <t>Бел-119</t>
         </is>
       </c>
       <c r="G17" t="inlineStr">
         <is>
-          <t>202B, C, LS-2, H, Type, сер</t>
+          <t>легк, сер</t>
         </is>
       </c>
       <c r="H17" t="n">
         <v>2</v>
       </c>
       <c r="I17" s="1" t="n">
-        <v>45351</v>
+        <v>45371</v>
       </c>
       <c r="J17" t="inlineStr">
         <is>
@@ -1158,39 +1158,39 @@
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
+          <t>Бел-1001</t>
+        </is>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>205/55R16</t>
+        </is>
+      </c>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>легк сер</t>
+        </is>
+      </c>
+      <c r="E18" t="inlineStr">
+        <is>
+          <t>195/65R15</t>
+        </is>
+      </c>
+      <c r="F18" t="inlineStr">
+        <is>
           <t>Бел-119</t>
         </is>
       </c>
-      <c r="B18" t="inlineStr">
-        <is>
-          <t>195/65R15</t>
-        </is>
-      </c>
-      <c r="C18" t="inlineStr">
-        <is>
-          <t>легк сер</t>
-        </is>
-      </c>
-      <c r="E18" t="inlineStr">
-        <is>
-          <t>14.00R20</t>
-        </is>
-      </c>
-      <c r="F18" t="inlineStr">
-        <is>
-          <t>BEL-248</t>
-        </is>
-      </c>
       <c r="G18" t="inlineStr">
         <is>
-          <t>груз, б/к, сер</t>
+          <t>легк, сер</t>
         </is>
       </c>
       <c r="H18" t="n">
         <v>2</v>
       </c>
       <c r="I18" s="1" t="n">
-        <v>45351</v>
+        <v>45371</v>
       </c>
       <c r="J18" t="inlineStr">
         <is>
@@ -1201,12 +1201,12 @@
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>Бел-777</t>
+          <t>Бел-1005</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>210/80R16</t>
+          <t>225/50R17</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
@@ -1216,24 +1216,24 @@
       </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t>14.00R20</t>
+          <t>195/65R15</t>
         </is>
       </c>
       <c r="F19" t="inlineStr">
         <is>
-          <t>BEL-248</t>
+          <t>Бел-119</t>
         </is>
       </c>
       <c r="G19" t="inlineStr">
         <is>
-          <t>груз, б/к, сер</t>
+          <t>легк, сер</t>
         </is>
       </c>
       <c r="H19" t="n">
         <v>2</v>
       </c>
       <c r="I19" s="1" t="n">
-        <v>45351</v>
+        <v>45371</v>
       </c>
       <c r="J19" t="inlineStr">
         <is>
@@ -1244,39 +1244,39 @@
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>Бел-1000</t>
+          <t>BEL-734</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>215/65R16C</t>
+          <t>205/70R14</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>легк сер</t>
+          <t>легк сер б/к</t>
         </is>
       </c>
       <c r="E20" t="inlineStr">
         <is>
-          <t>14.00R20</t>
+          <t>195/65R15</t>
         </is>
       </c>
       <c r="F20" t="inlineStr">
         <is>
-          <t>BEL-248</t>
+          <t>Бел-1149</t>
         </is>
       </c>
       <c r="G20" t="inlineStr">
         <is>
-          <t>груз, б/к, сер</t>
+          <t>легк, сер</t>
         </is>
       </c>
       <c r="H20" t="n">
         <v>2</v>
       </c>
       <c r="I20" s="1" t="n">
-        <v>45351</v>
+        <v>45371</v>
       </c>
       <c r="J20" t="inlineStr">
         <is>
@@ -1287,39 +1287,39 @@
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>Бел-1001</t>
+          <t>BEL-261</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>205/55R16</t>
+          <t>195/65R15</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>легк сер</t>
+          <t>легк сер б/к</t>
         </is>
       </c>
       <c r="E21" t="inlineStr">
         <is>
-          <t>14.00R20</t>
+          <t>210/80R16</t>
         </is>
       </c>
       <c r="F21" t="inlineStr">
         <is>
-          <t>BEL-248</t>
+          <t>Бел-777</t>
         </is>
       </c>
       <c r="G21" t="inlineStr">
         <is>
-          <t>груз, б/к, сер</t>
+          <t>легк, сер</t>
         </is>
       </c>
       <c r="H21" t="n">
         <v>2</v>
       </c>
       <c r="I21" s="1" t="n">
-        <v>45351</v>
+        <v>45371</v>
       </c>
       <c r="J21" t="inlineStr">
         <is>
@@ -1330,123 +1330,168 @@
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
+          <t>BEL-337</t>
+        </is>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>195/65R15</t>
+        </is>
+      </c>
+      <c r="C22" t="inlineStr">
+        <is>
+          <t>легк сер б/к</t>
+        </is>
+      </c>
+      <c r="E22" t="inlineStr">
+        <is>
+          <t>215/65R16C</t>
+        </is>
+      </c>
+      <c r="F22" t="inlineStr">
+        <is>
+          <t>Бел-1000</t>
+        </is>
+      </c>
+      <c r="G22" t="inlineStr">
+        <is>
+          <t>легк, сер</t>
+        </is>
+      </c>
+      <c r="H22" t="n">
+        <v>2</v>
+      </c>
+      <c r="I22" s="1" t="n">
+        <v>45371</v>
+      </c>
+      <c r="J22" t="inlineStr">
+        <is>
+          <t>нет данных</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>BEL-337S</t>
+        </is>
+      </c>
+      <c r="B23" t="inlineStr">
+        <is>
+          <t>195/65R15</t>
+        </is>
+      </c>
+      <c r="C23" t="inlineStr">
+        <is>
+          <t>сер ошип</t>
+        </is>
+      </c>
+      <c r="E23" t="inlineStr">
+        <is>
+          <t>205/55R16</t>
+        </is>
+      </c>
+      <c r="F23" t="inlineStr">
+        <is>
+          <t>Бел-1001</t>
+        </is>
+      </c>
+      <c r="G23" t="inlineStr">
+        <is>
+          <t>легк, сер</t>
+        </is>
+      </c>
+      <c r="H23" t="n">
+        <v>2</v>
+      </c>
+      <c r="I23" s="1" t="n">
+        <v>45371</v>
+      </c>
+      <c r="J23" t="inlineStr">
+        <is>
+          <t>нет данных</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="inlineStr">
+        <is>
+          <t>BEL-705</t>
+        </is>
+      </c>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>195/65R15</t>
+        </is>
+      </c>
+      <c r="C24" t="inlineStr">
+        <is>
+          <t>легк сер б/к</t>
+        </is>
+      </c>
+      <c r="E24" t="inlineStr">
+        <is>
+          <t>225/50R17</t>
+        </is>
+      </c>
+      <c r="F24" t="inlineStr">
+        <is>
           <t>Бел-1005</t>
         </is>
       </c>
-      <c r="B22" t="inlineStr">
-        <is>
-          <t>225/50R17</t>
-        </is>
-      </c>
-      <c r="C22" t="inlineStr">
+      <c r="G24" t="inlineStr">
+        <is>
+          <t>легк, сер</t>
+        </is>
+      </c>
+      <c r="H24" t="n">
+        <v>2</v>
+      </c>
+      <c r="I24" s="1" t="n">
+        <v>45371</v>
+      </c>
+      <c r="J24" t="inlineStr">
+        <is>
+          <t>нет данных</t>
+        </is>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="inlineStr">
+        <is>
+          <t>Бел-188</t>
+        </is>
+      </c>
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>175/70R13</t>
+        </is>
+      </c>
+      <c r="C25" t="inlineStr">
         <is>
           <t>легк сер</t>
         </is>
       </c>
-      <c r="E22" t="inlineStr">
-        <is>
-          <t>175/70R13</t>
-        </is>
-      </c>
-      <c r="F22" t="inlineStr">
-        <is>
-          <t>Бел-103</t>
-        </is>
-      </c>
-      <c r="G22" t="inlineStr">
-        <is>
-          <t>б/к, легк, сер</t>
-        </is>
-      </c>
-      <c r="H22" t="n">
-        <v>2</v>
-      </c>
-      <c r="I22" s="1" t="n">
-        <v>45351</v>
-      </c>
-      <c r="J22" t="inlineStr">
-        <is>
-          <t>нет данных</t>
-        </is>
-      </c>
-    </row>
-    <row r="23">
-      <c r="E23" t="inlineStr">
-        <is>
-          <t>175/70R13</t>
-        </is>
-      </c>
-      <c r="F23" t="inlineStr">
-        <is>
-          <t>Бел-100</t>
-        </is>
-      </c>
-      <c r="G23" t="inlineStr">
-        <is>
-          <t>б/к, легк, сер</t>
-        </is>
-      </c>
-      <c r="H23" t="n">
-        <v>2</v>
-      </c>
-      <c r="I23" s="1" t="n">
-        <v>45351</v>
-      </c>
-      <c r="J23" t="inlineStr">
-        <is>
-          <t>нет данных</t>
-        </is>
-      </c>
-    </row>
-    <row r="24">
-      <c r="E24" t="inlineStr">
-        <is>
-          <t>195/65R15</t>
-        </is>
-      </c>
-      <c r="F24" t="inlineStr">
-        <is>
-          <t>Бел-119</t>
-        </is>
-      </c>
-      <c r="G24" t="inlineStr">
-        <is>
-          <t>легк, сер</t>
-        </is>
-      </c>
-      <c r="H24" t="n">
-        <v>2</v>
-      </c>
-      <c r="I24" s="1" t="n">
-        <v>45351</v>
-      </c>
-      <c r="J24" t="inlineStr">
-        <is>
-          <t>нет данных</t>
-        </is>
-      </c>
-    </row>
-    <row r="25">
       <c r="E25" t="inlineStr">
         <is>
-          <t>195/65R15</t>
+          <t>205/70R14</t>
         </is>
       </c>
       <c r="F25" t="inlineStr">
         <is>
-          <t>Бел-119</t>
+          <t>BEL-734</t>
         </is>
       </c>
       <c r="G25" t="inlineStr">
         <is>
-          <t>легк, сер</t>
+          <t>легк, сер, б/к</t>
         </is>
       </c>
       <c r="H25" t="n">
         <v>2</v>
       </c>
       <c r="I25" s="1" t="n">
-        <v>45351</v>
+        <v>45371</v>
       </c>
       <c r="J25" t="inlineStr">
         <is>
@@ -1462,19 +1507,19 @@
       </c>
       <c r="F26" t="inlineStr">
         <is>
-          <t>Бел-119</t>
+          <t>BEL-261</t>
         </is>
       </c>
       <c r="G26" t="inlineStr">
         <is>
-          <t>легк, сер</t>
+          <t>легк, сер, б/к</t>
         </is>
       </c>
       <c r="H26" t="n">
         <v>2</v>
       </c>
       <c r="I26" s="1" t="n">
-        <v>45351</v>
+        <v>45371</v>
       </c>
       <c r="J26" t="inlineStr">
         <is>
@@ -1485,24 +1530,24 @@
     <row r="27">
       <c r="E27" t="inlineStr">
         <is>
-          <t>210/80R16</t>
+          <t>195/65R15</t>
         </is>
       </c>
       <c r="F27" t="inlineStr">
         <is>
-          <t>Бел-777</t>
+          <t>BEL-337</t>
         </is>
       </c>
       <c r="G27" t="inlineStr">
         <is>
-          <t>легк, сер</t>
+          <t>легк, сер, б/к</t>
         </is>
       </c>
       <c r="H27" t="n">
         <v>2</v>
       </c>
       <c r="I27" s="1" t="n">
-        <v>45351</v>
+        <v>45371</v>
       </c>
       <c r="J27" t="inlineStr">
         <is>
@@ -1513,24 +1558,24 @@
     <row r="28">
       <c r="E28" t="inlineStr">
         <is>
-          <t>215/65R16C</t>
+          <t>195/65R15</t>
         </is>
       </c>
       <c r="F28" t="inlineStr">
         <is>
-          <t>Бел-1000</t>
+          <t>BEL-337S</t>
         </is>
       </c>
       <c r="G28" t="inlineStr">
         <is>
-          <t>легк, сер</t>
+          <t>сер, ошип</t>
         </is>
       </c>
       <c r="H28" t="n">
         <v>2</v>
       </c>
       <c r="I28" s="1" t="n">
-        <v>45351</v>
+        <v>45371</v>
       </c>
       <c r="J28" t="inlineStr">
         <is>
@@ -1541,24 +1586,24 @@
     <row r="29">
       <c r="E29" t="inlineStr">
         <is>
-          <t>205/55R16</t>
+          <t>195/65R15</t>
         </is>
       </c>
       <c r="F29" t="inlineStr">
         <is>
-          <t>Бел-1001</t>
+          <t>BEL-705</t>
         </is>
       </c>
       <c r="G29" t="inlineStr">
         <is>
-          <t>легк, сер</t>
+          <t>легк, сер, б/к</t>
         </is>
       </c>
       <c r="H29" t="n">
         <v>2</v>
       </c>
       <c r="I29" s="1" t="n">
-        <v>45351</v>
+        <v>45371</v>
       </c>
       <c r="J29" t="inlineStr">
         <is>
@@ -1569,26 +1614,138 @@
     <row r="30">
       <c r="E30" t="inlineStr">
         <is>
-          <t>225/50R17</t>
+          <t>205/55R16</t>
         </is>
       </c>
       <c r="F30" t="inlineStr">
         <is>
-          <t>Бел-1005</t>
+          <t>BEL-262</t>
         </is>
       </c>
       <c r="G30" t="inlineStr">
         <is>
+          <t>легк, сер, б/к</t>
+        </is>
+      </c>
+      <c r="H30" t="n">
+        <v>2</v>
+      </c>
+      <c r="I30" s="1" t="n">
+        <v>45371</v>
+      </c>
+      <c r="J30" t="inlineStr">
+        <is>
+          <t>нет данных</t>
+        </is>
+      </c>
+    </row>
+    <row r="31">
+      <c r="E31" t="inlineStr">
+        <is>
+          <t>205/55R16</t>
+        </is>
+      </c>
+      <c r="F31" t="inlineStr">
+        <is>
+          <t>BEL-317</t>
+        </is>
+      </c>
+      <c r="G31" t="inlineStr">
+        <is>
+          <t>легк, сер, б/к</t>
+        </is>
+      </c>
+      <c r="H31" t="n">
+        <v>2</v>
+      </c>
+      <c r="I31" s="1" t="n">
+        <v>45371</v>
+      </c>
+      <c r="J31" t="inlineStr">
+        <is>
+          <t>нет данных</t>
+        </is>
+      </c>
+    </row>
+    <row r="32">
+      <c r="E32" t="inlineStr">
+        <is>
+          <t>175/70R13</t>
+        </is>
+      </c>
+      <c r="F32" t="inlineStr">
+        <is>
+          <t>Бел-103</t>
+        </is>
+      </c>
+      <c r="G32" t="inlineStr">
+        <is>
+          <t>легк, сер, б/к</t>
+        </is>
+      </c>
+      <c r="H32" t="n">
+        <v>2</v>
+      </c>
+      <c r="I32" s="1" t="n">
+        <v>45371</v>
+      </c>
+      <c r="J32" t="inlineStr">
+        <is>
+          <t>нет данных</t>
+        </is>
+      </c>
+    </row>
+    <row r="33">
+      <c r="E33" t="inlineStr">
+        <is>
+          <t>175/70R13</t>
+        </is>
+      </c>
+      <c r="F33" t="inlineStr">
+        <is>
+          <t>Бел-100</t>
+        </is>
+      </c>
+      <c r="G33" t="inlineStr">
+        <is>
+          <t>легк, сер, б/к</t>
+        </is>
+      </c>
+      <c r="H33" t="n">
+        <v>2</v>
+      </c>
+      <c r="I33" s="1" t="n">
+        <v>45371</v>
+      </c>
+      <c r="J33" t="inlineStr">
+        <is>
+          <t>нет данных</t>
+        </is>
+      </c>
+    </row>
+    <row r="34">
+      <c r="E34" t="inlineStr">
+        <is>
+          <t>175/70R13</t>
+        </is>
+      </c>
+      <c r="F34" t="inlineStr">
+        <is>
+          <t>Бел-188</t>
+        </is>
+      </c>
+      <c r="G34" t="inlineStr">
+        <is>
           <t>легк, сер</t>
         </is>
       </c>
-      <c r="H30" t="n">
-        <v>2</v>
-      </c>
-      <c r="I30" s="1" t="n">
-        <v>45351</v>
-      </c>
-      <c r="J30" t="inlineStr">
+      <c r="H34" t="n">
+        <v>2</v>
+      </c>
+      <c r="I34" s="1" t="n">
+        <v>45371</v>
+      </c>
+      <c r="J34" t="inlineStr">
         <is>
           <t>нет данных</t>
         </is>

</xml_diff>

<commit_message>
10.02/2024 - return to host 97.98
</commit_message>
<xml_diff>
--- a/src/Tyres.xlsx
+++ b/src/Tyres.xlsx
@@ -480,7 +480,7 @@
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>легк сер б/к</t>
+          <t>сер легк б/к</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
@@ -495,14 +495,14 @@
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>легк, сер, б/к</t>
+          <t>сер, легк, б/к</t>
         </is>
       </c>
       <c r="H2" t="n">
         <v>2</v>
       </c>
       <c r="I2" s="1" t="n">
-        <v>45371</v>
+        <v>45417</v>
       </c>
       <c r="J2" t="inlineStr">
         <is>
@@ -523,7 +523,7 @@
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>легк сер б/к</t>
+          <t>сер легк б/к</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
@@ -538,14 +538,14 @@
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>легк, сер, б/к</t>
+          <t>сер, легк, б/к</t>
         </is>
       </c>
       <c r="H3" t="n">
         <v>2</v>
       </c>
       <c r="I3" s="1" t="n">
-        <v>45371</v>
+        <v>45417</v>
       </c>
       <c r="J3" t="inlineStr">
         <is>
@@ -588,7 +588,7 @@
         <v>2</v>
       </c>
       <c r="I4" s="1" t="n">
-        <v>45371</v>
+        <v>45417</v>
       </c>
       <c r="J4" t="inlineStr">
         <is>
@@ -609,7 +609,7 @@
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>легк сер</t>
+          <t>сер легк</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
@@ -624,14 +624,14 @@
       </c>
       <c r="G5" t="inlineStr">
         <is>
-          <t>легк, сер</t>
+          <t>сер, легк</t>
         </is>
       </c>
       <c r="H5" t="n">
         <v>2</v>
       </c>
       <c r="I5" s="1" t="n">
-        <v>45371</v>
+        <v>45417</v>
       </c>
       <c r="J5" t="inlineStr">
         <is>
@@ -652,7 +652,7 @@
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>легк сер</t>
+          <t>сер легк</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
@@ -667,14 +667,14 @@
       </c>
       <c r="G6" t="inlineStr">
         <is>
-          <t>легк, сер</t>
+          <t>сер, легк</t>
         </is>
       </c>
       <c r="H6" t="n">
         <v>2</v>
       </c>
       <c r="I6" s="1" t="n">
-        <v>45371</v>
+        <v>45417</v>
       </c>
       <c r="J6" t="inlineStr">
         <is>
@@ -695,7 +695,7 @@
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>легк сер</t>
+          <t>сер легк</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
@@ -710,14 +710,14 @@
       </c>
       <c r="G7" t="inlineStr">
         <is>
-          <t>легк, сер</t>
+          <t>сер, легк</t>
         </is>
       </c>
       <c r="H7" t="n">
         <v>2</v>
       </c>
       <c r="I7" s="1" t="n">
-        <v>45371</v>
+        <v>45417</v>
       </c>
       <c r="J7" t="inlineStr">
         <is>
@@ -738,7 +738,7 @@
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>легк сер</t>
+          <t>сер легк</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
@@ -753,14 +753,14 @@
       </c>
       <c r="G8" t="inlineStr">
         <is>
-          <t>легк, сер</t>
+          <t>сер, легк</t>
         </is>
       </c>
       <c r="H8" t="n">
         <v>2</v>
       </c>
       <c r="I8" s="1" t="n">
-        <v>45371</v>
+        <v>45417</v>
       </c>
       <c r="J8" t="inlineStr">
         <is>
@@ -781,7 +781,7 @@
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>210B Type H сер</t>
+          <t>210B сер Type H</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
@@ -796,14 +796,14 @@
       </c>
       <c r="G9" t="inlineStr">
         <is>
-          <t>легк, сер</t>
+          <t>сер, легк</t>
         </is>
       </c>
       <c r="H9" t="n">
         <v>2</v>
       </c>
       <c r="I9" s="1" t="n">
-        <v>45371</v>
+        <v>45417</v>
       </c>
       <c r="J9" t="inlineStr">
         <is>
@@ -824,7 +824,7 @@
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>груз сер б/к</t>
+          <t>сер б/к груз</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
@@ -839,14 +839,14 @@
       </c>
       <c r="G10" t="inlineStr">
         <is>
-          <t>210B, Type, H, сер</t>
+          <t>210B, сер, Type, H</t>
         </is>
       </c>
       <c r="H10" t="n">
         <v>2</v>
       </c>
       <c r="I10" s="1" t="n">
-        <v>45371</v>
+        <v>45417</v>
       </c>
       <c r="J10" t="inlineStr">
         <is>
@@ -867,7 +867,7 @@
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>легк сер б/к</t>
+          <t>сер легк б/к</t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
@@ -882,14 +882,14 @@
       </c>
       <c r="G11" t="inlineStr">
         <is>
-          <t>груз, сер, б/к</t>
+          <t>сер, б/к, груз</t>
         </is>
       </c>
       <c r="H11" t="n">
         <v>2</v>
       </c>
       <c r="I11" s="1" t="n">
-        <v>45371</v>
+        <v>45417</v>
       </c>
       <c r="J11" t="inlineStr">
         <is>
@@ -910,7 +910,7 @@
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>легк сер б/к</t>
+          <t>сер легк б/к</t>
         </is>
       </c>
       <c r="E12" t="inlineStr">
@@ -925,14 +925,14 @@
       </c>
       <c r="G12" t="inlineStr">
         <is>
-          <t>груз, сер, б/к</t>
+          <t>сер, б/к, груз</t>
         </is>
       </c>
       <c r="H12" t="n">
         <v>2</v>
       </c>
       <c r="I12" s="1" t="n">
-        <v>45371</v>
+        <v>45417</v>
       </c>
       <c r="J12" t="inlineStr">
         <is>
@@ -953,7 +953,7 @@
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>8 сх сер</t>
+          <t>8 сер сх</t>
         </is>
       </c>
       <c r="E13" t="inlineStr">
@@ -968,14 +968,14 @@
       </c>
       <c r="G13" t="inlineStr">
         <is>
-          <t>груз, сер, б/к</t>
+          <t>сер, б/к, груз</t>
         </is>
       </c>
       <c r="H13" t="n">
         <v>2</v>
       </c>
       <c r="I13" s="1" t="n">
-        <v>45371</v>
+        <v>45417</v>
       </c>
       <c r="J13" t="inlineStr">
         <is>
@@ -996,7 +996,7 @@
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>легк сер</t>
+          <t>сер легк</t>
         </is>
       </c>
       <c r="E14" t="inlineStr">
@@ -1011,14 +1011,14 @@
       </c>
       <c r="G14" t="inlineStr">
         <is>
-          <t>груз, сер, б/к</t>
+          <t>сер, б/к, груз</t>
         </is>
       </c>
       <c r="H14" t="n">
         <v>2</v>
       </c>
       <c r="I14" s="1" t="n">
-        <v>45371</v>
+        <v>45417</v>
       </c>
       <c r="J14" t="inlineStr">
         <is>
@@ -1039,7 +1039,7 @@
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>легк сер</t>
+          <t>сер легк</t>
         </is>
       </c>
       <c r="E15" t="inlineStr">
@@ -1054,14 +1054,14 @@
       </c>
       <c r="G15" t="inlineStr">
         <is>
-          <t>легк, сер, б/к</t>
+          <t>сер, легк, б/к</t>
         </is>
       </c>
       <c r="H15" t="n">
         <v>2</v>
       </c>
       <c r="I15" s="1" t="n">
-        <v>45371</v>
+        <v>45417</v>
       </c>
       <c r="J15" t="inlineStr">
         <is>
@@ -1082,7 +1082,7 @@
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>легк сер</t>
+          <t>сер легк</t>
         </is>
       </c>
       <c r="E16" t="inlineStr">
@@ -1097,14 +1097,14 @@
       </c>
       <c r="G16" t="inlineStr">
         <is>
-          <t>легк, сер, б/к</t>
+          <t>сер, легк, б/к</t>
         </is>
       </c>
       <c r="H16" t="n">
         <v>2</v>
       </c>
       <c r="I16" s="1" t="n">
-        <v>45371</v>
+        <v>45417</v>
       </c>
       <c r="J16" t="inlineStr">
         <is>
@@ -1125,7 +1125,7 @@
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>легк сер</t>
+          <t>сер легк</t>
         </is>
       </c>
       <c r="E17" t="inlineStr">
@@ -1140,14 +1140,14 @@
       </c>
       <c r="G17" t="inlineStr">
         <is>
-          <t>легк, сер</t>
+          <t>сер, легк</t>
         </is>
       </c>
       <c r="H17" t="n">
         <v>2</v>
       </c>
       <c r="I17" s="1" t="n">
-        <v>45371</v>
+        <v>45417</v>
       </c>
       <c r="J17" t="inlineStr">
         <is>
@@ -1168,7 +1168,7 @@
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>легк сер</t>
+          <t>сер легк</t>
         </is>
       </c>
       <c r="E18" t="inlineStr">
@@ -1183,14 +1183,14 @@
       </c>
       <c r="G18" t="inlineStr">
         <is>
-          <t>легк, сер</t>
+          <t>сер, легк</t>
         </is>
       </c>
       <c r="H18" t="n">
         <v>2</v>
       </c>
       <c r="I18" s="1" t="n">
-        <v>45371</v>
+        <v>45417</v>
       </c>
       <c r="J18" t="inlineStr">
         <is>
@@ -1211,7 +1211,7 @@
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>легк сер</t>
+          <t>сер легк</t>
         </is>
       </c>
       <c r="E19" t="inlineStr">
@@ -1226,14 +1226,14 @@
       </c>
       <c r="G19" t="inlineStr">
         <is>
-          <t>легк, сер</t>
+          <t>сер, легк</t>
         </is>
       </c>
       <c r="H19" t="n">
         <v>2</v>
       </c>
       <c r="I19" s="1" t="n">
-        <v>45371</v>
+        <v>45417</v>
       </c>
       <c r="J19" t="inlineStr">
         <is>
@@ -1254,7 +1254,7 @@
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>легк сер б/к</t>
+          <t>сер легк б/к</t>
         </is>
       </c>
       <c r="E20" t="inlineStr">
@@ -1269,14 +1269,14 @@
       </c>
       <c r="G20" t="inlineStr">
         <is>
-          <t>легк, сер</t>
+          <t>сер, легк</t>
         </is>
       </c>
       <c r="H20" t="n">
         <v>2</v>
       </c>
       <c r="I20" s="1" t="n">
-        <v>45371</v>
+        <v>45417</v>
       </c>
       <c r="J20" t="inlineStr">
         <is>
@@ -1297,7 +1297,7 @@
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>легк сер б/к</t>
+          <t>сер легк б/к</t>
         </is>
       </c>
       <c r="E21" t="inlineStr">
@@ -1312,14 +1312,14 @@
       </c>
       <c r="G21" t="inlineStr">
         <is>
-          <t>легк, сер</t>
+          <t>сер, легк</t>
         </is>
       </c>
       <c r="H21" t="n">
         <v>2</v>
       </c>
       <c r="I21" s="1" t="n">
-        <v>45371</v>
+        <v>45417</v>
       </c>
       <c r="J21" t="inlineStr">
         <is>
@@ -1340,7 +1340,7 @@
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>легк сер б/к</t>
+          <t>сер легк б/к</t>
         </is>
       </c>
       <c r="E22" t="inlineStr">
@@ -1355,14 +1355,14 @@
       </c>
       <c r="G22" t="inlineStr">
         <is>
-          <t>легк, сер</t>
+          <t>сер, легк</t>
         </is>
       </c>
       <c r="H22" t="n">
         <v>2</v>
       </c>
       <c r="I22" s="1" t="n">
-        <v>45371</v>
+        <v>45417</v>
       </c>
       <c r="J22" t="inlineStr">
         <is>
@@ -1398,14 +1398,14 @@
       </c>
       <c r="G23" t="inlineStr">
         <is>
-          <t>легк, сер</t>
+          <t>сер, легк</t>
         </is>
       </c>
       <c r="H23" t="n">
         <v>2</v>
       </c>
       <c r="I23" s="1" t="n">
-        <v>45371</v>
+        <v>45417</v>
       </c>
       <c r="J23" t="inlineStr">
         <is>
@@ -1426,7 +1426,7 @@
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>легк сер б/к</t>
+          <t>сер легк б/к</t>
         </is>
       </c>
       <c r="E24" t="inlineStr">
@@ -1441,14 +1441,14 @@
       </c>
       <c r="G24" t="inlineStr">
         <is>
-          <t>легк, сер</t>
+          <t>сер, легк</t>
         </is>
       </c>
       <c r="H24" t="n">
         <v>2</v>
       </c>
       <c r="I24" s="1" t="n">
-        <v>45371</v>
+        <v>45417</v>
       </c>
       <c r="J24" t="inlineStr">
         <is>
@@ -1469,7 +1469,7 @@
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>легк сер</t>
+          <t>сер легк</t>
         </is>
       </c>
       <c r="E25" t="inlineStr">
@@ -1484,14 +1484,14 @@
       </c>
       <c r="G25" t="inlineStr">
         <is>
-          <t>легк, сер, б/к</t>
+          <t>сер, легк, б/к</t>
         </is>
       </c>
       <c r="H25" t="n">
         <v>2</v>
       </c>
       <c r="I25" s="1" t="n">
-        <v>45371</v>
+        <v>45417</v>
       </c>
       <c r="J25" t="inlineStr">
         <is>
@@ -1512,14 +1512,14 @@
       </c>
       <c r="G26" t="inlineStr">
         <is>
-          <t>легк, сер, б/к</t>
+          <t>сер, легк, б/к</t>
         </is>
       </c>
       <c r="H26" t="n">
         <v>2</v>
       </c>
       <c r="I26" s="1" t="n">
-        <v>45371</v>
+        <v>45417</v>
       </c>
       <c r="J26" t="inlineStr">
         <is>
@@ -1540,14 +1540,14 @@
       </c>
       <c r="G27" t="inlineStr">
         <is>
-          <t>легк, сер, б/к</t>
+          <t>сер, легк, б/к</t>
         </is>
       </c>
       <c r="H27" t="n">
         <v>2</v>
       </c>
       <c r="I27" s="1" t="n">
-        <v>45371</v>
+        <v>45417</v>
       </c>
       <c r="J27" t="inlineStr">
         <is>
@@ -1575,7 +1575,7 @@
         <v>2</v>
       </c>
       <c r="I28" s="1" t="n">
-        <v>45371</v>
+        <v>45417</v>
       </c>
       <c r="J28" t="inlineStr">
         <is>
@@ -1596,14 +1596,14 @@
       </c>
       <c r="G29" t="inlineStr">
         <is>
-          <t>легк, сер, б/к</t>
+          <t>сер, легк, б/к</t>
         </is>
       </c>
       <c r="H29" t="n">
         <v>2</v>
       </c>
       <c r="I29" s="1" t="n">
-        <v>45371</v>
+        <v>45417</v>
       </c>
       <c r="J29" t="inlineStr">
         <is>
@@ -1624,14 +1624,14 @@
       </c>
       <c r="G30" t="inlineStr">
         <is>
-          <t>легк, сер, б/к</t>
+          <t>сер, легк, б/к</t>
         </is>
       </c>
       <c r="H30" t="n">
         <v>2</v>
       </c>
       <c r="I30" s="1" t="n">
-        <v>45371</v>
+        <v>45417</v>
       </c>
       <c r="J30" t="inlineStr">
         <is>
@@ -1652,14 +1652,14 @@
       </c>
       <c r="G31" t="inlineStr">
         <is>
-          <t>легк, сер, б/к</t>
+          <t>сер, легк, б/к</t>
         </is>
       </c>
       <c r="H31" t="n">
         <v>2</v>
       </c>
       <c r="I31" s="1" t="n">
-        <v>45371</v>
+        <v>45417</v>
       </c>
       <c r="J31" t="inlineStr">
         <is>
@@ -1680,14 +1680,14 @@
       </c>
       <c r="G32" t="inlineStr">
         <is>
-          <t>легк, сер, б/к</t>
+          <t>сер, легк, б/к</t>
         </is>
       </c>
       <c r="H32" t="n">
         <v>2</v>
       </c>
       <c r="I32" s="1" t="n">
-        <v>45371</v>
+        <v>45417</v>
       </c>
       <c r="J32" t="inlineStr">
         <is>
@@ -1708,14 +1708,14 @@
       </c>
       <c r="G33" t="inlineStr">
         <is>
-          <t>легк, сер, б/к</t>
+          <t>сер, легк, б/к</t>
         </is>
       </c>
       <c r="H33" t="n">
         <v>2</v>
       </c>
       <c r="I33" s="1" t="n">
-        <v>45371</v>
+        <v>45417</v>
       </c>
       <c r="J33" t="inlineStr">
         <is>
@@ -1736,14 +1736,14 @@
       </c>
       <c r="G34" t="inlineStr">
         <is>
-          <t>легк, сер</t>
+          <t>сер, легк</t>
         </is>
       </c>
       <c r="H34" t="n">
         <v>2</v>
       </c>
       <c r="I34" s="1" t="n">
-        <v>45371</v>
+        <v>45417</v>
       </c>
       <c r="J34" t="inlineStr">
         <is>

</xml_diff>